<commit_message>
GDE-6688 Fx Rates EU Configuration for Dataset
</commit_message>
<xml_diff>
--- a/DataSet/Integration_DataSet/TL/TL_Data_Set_AU.xlsx
+++ b/DataSet/Integration_DataSet/TL/TL_Data_Set_AU.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\Integration_DataSet\TL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B1CDC2B-32FE-43D6-A311-A6BFFB8E204A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05D60997-DB15-4187-884F-5DC225A6CAE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BaseRate_Fields" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1434" uniqueCount="1119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1436" uniqueCount="1120">
   <si>
     <t>rowid</t>
   </si>
@@ -2021,9 +2021,6 @@
   </si>
   <si>
     <t>\DataSet\TL_DataSet\FxRates_GSFile\TL_FX_08_Files\</t>
-  </si>
-  <si>
-    <t>\DataSet\TL_DataSet\FxRates_GSFile\TL_FX_01_Files\</t>
   </si>
   <si>
     <t>\DataSet\TL_DataSet\FxRates_GSFile\TL_FX_02_Files\</t>
@@ -3437,6 +3434,12 @@
   </si>
   <si>
     <t>\DataSet\Integration_DataSet\TL\BaseRates_GSFile\AU\TL_BASE_01_Files\</t>
+  </si>
+  <si>
+    <t>\DataSet\Integration_DataSet\TL\FXRates_GSFile\</t>
+  </si>
+  <si>
+    <t>\DataSet\Integration_DataSet\TL\FXRates_GSFile\AU\TL_FX_01_Files\</t>
   </si>
 </sst>
 </file>
@@ -4389,8 +4392,8 @@
   </sheetPr>
   <dimension ref="A1:N42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4419,7 +4422,7 @@
         <v>17</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>1</v>
@@ -4452,7 +4455,7 @@
         <v>155</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -4463,10 +4466,10 @@
         <v>11</v>
       </c>
       <c r="C2" s="9" t="s">
+        <v>1116</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>1117</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>1118</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>94</v>
@@ -4481,7 +4484,7 @@
         <v>18</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>21</v>
@@ -4571,7 +4574,7 @@
         <v>136</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -4661,10 +4664,10 @@
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="9" t="s">
+        <v>915</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>916</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>917</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>59</v>
@@ -4676,7 +4679,7 @@
         <v>61</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="J7" s="5" t="s">
         <v>62</v>
@@ -4688,7 +4691,7 @@
         <v>139</v>
       </c>
       <c r="M7" s="5" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -4700,10 +4703,10 @@
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="9" t="s">
+        <v>917</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>918</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>919</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>66</v>
@@ -4715,7 +4718,7 @@
         <v>68</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="J8" s="5" t="s">
         <v>69</v>
@@ -4724,10 +4727,10 @@
         <v>70</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -4739,10 +4742,10 @@
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="9" t="s">
+        <v>919</v>
+      </c>
+      <c r="E9" s="5" t="s">
         <v>920</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>921</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>98</v>
@@ -4754,7 +4757,7 @@
         <v>100</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="J9" s="5" t="s">
         <v>101</v>
@@ -4763,10 +4766,10 @@
         <v>102</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="M9" s="5" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -4778,7 +4781,7 @@
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="9" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>105</v>
@@ -4793,7 +4796,7 @@
         <v>108</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="J10" s="5" t="s">
         <v>109</v>
@@ -4802,10 +4805,10 @@
         <v>110</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="M10" s="5" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -5047,38 +5050,38 @@
         <v>333</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="9" t="s">
+        <v>922</v>
+      </c>
+      <c r="E17" s="5" t="s">
         <v>923</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="F17" s="5" t="s">
         <v>924</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="G17" s="5" t="s">
         <v>925</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="H17" s="5" t="s">
         <v>926</v>
       </c>
-      <c r="H17" s="5" t="s">
+      <c r="I17" s="9" t="s">
+        <v>922</v>
+      </c>
+      <c r="J17" s="5" t="s">
         <v>927</v>
       </c>
-      <c r="I17" s="9" t="s">
-        <v>923</v>
-      </c>
-      <c r="J17" s="5" t="s">
+      <c r="K17" s="5" t="s">
         <v>928</v>
       </c>
-      <c r="K17" s="5" t="s">
+      <c r="L17" s="5" t="s">
         <v>929</v>
       </c>
-      <c r="L17" s="5" t="s">
+      <c r="M17" s="5" t="s">
         <v>930</v>
-      </c>
-      <c r="M17" s="5" t="s">
-        <v>931</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -5086,38 +5089,38 @@
         <v>343</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="9" t="s">
+        <v>1077</v>
+      </c>
+      <c r="E18" s="5" t="s">
         <v>1078</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="F18" s="5" t="s">
         <v>1079</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="G18" s="5" t="s">
         <v>1080</v>
       </c>
-      <c r="G18" s="5" t="s">
+      <c r="H18" s="5" t="s">
         <v>1081</v>
       </c>
-      <c r="H18" s="5" t="s">
+      <c r="I18" s="9" t="s">
+        <v>1077</v>
+      </c>
+      <c r="J18" s="5" t="s">
         <v>1082</v>
       </c>
-      <c r="I18" s="9" t="s">
-        <v>1078</v>
-      </c>
-      <c r="J18" s="5" t="s">
+      <c r="K18" s="5" t="s">
         <v>1083</v>
       </c>
-      <c r="K18" s="5" t="s">
+      <c r="L18" s="5" t="s">
         <v>1084</v>
       </c>
-      <c r="L18" s="5" t="s">
+      <c r="M18" s="5" t="s">
         <v>1085</v>
-      </c>
-      <c r="M18" s="5" t="s">
-        <v>1086</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -5125,38 +5128,38 @@
         <v>353</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="9" t="s">
+        <v>1018</v>
+      </c>
+      <c r="E19" s="5" t="s">
         <v>1019</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="F19" s="5" t="s">
         <v>1020</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="G19" s="5" t="s">
         <v>1021</v>
       </c>
-      <c r="G19" s="5" t="s">
+      <c r="H19" s="5" t="s">
         <v>1022</v>
       </c>
-      <c r="H19" s="5" t="s">
+      <c r="I19" s="9" t="s">
+        <v>1018</v>
+      </c>
+      <c r="J19" s="5" t="s">
         <v>1023</v>
       </c>
-      <c r="I19" s="9" t="s">
-        <v>1019</v>
-      </c>
-      <c r="J19" s="5" t="s">
+      <c r="K19" s="5" t="s">
         <v>1024</v>
       </c>
-      <c r="K19" s="5" t="s">
+      <c r="L19" s="5" t="s">
         <v>1025</v>
       </c>
-      <c r="L19" s="5" t="s">
+      <c r="M19" s="5" t="s">
         <v>1026</v>
-      </c>
-      <c r="M19" s="5" t="s">
-        <v>1027</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
@@ -5398,38 +5401,38 @@
         <v>448</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="9" t="s">
+        <v>701</v>
+      </c>
+      <c r="E26" s="6" t="s">
         <v>702</v>
       </c>
-      <c r="E26" s="6" t="s">
+      <c r="F26" s="5" t="s">
         <v>703</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="G26" s="5" t="s">
         <v>704</v>
       </c>
-      <c r="G26" s="5" t="s">
+      <c r="H26" s="5" t="s">
         <v>705</v>
       </c>
-      <c r="H26" s="5" t="s">
+      <c r="I26" s="9" t="s">
+        <v>701</v>
+      </c>
+      <c r="J26" s="5" t="s">
         <v>706</v>
       </c>
-      <c r="I26" s="9" t="s">
-        <v>702</v>
-      </c>
-      <c r="J26" s="5" t="s">
+      <c r="K26" s="5" t="s">
         <v>707</v>
       </c>
-      <c r="K26" s="5" t="s">
+      <c r="L26" s="5" t="s">
         <v>708</v>
       </c>
-      <c r="L26" s="5" t="s">
+      <c r="M26" s="5" t="s">
         <v>709</v>
-      </c>
-      <c r="M26" s="5" t="s">
-        <v>710</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
@@ -5437,38 +5440,38 @@
         <v>458</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="9" t="s">
+        <v>1087</v>
+      </c>
+      <c r="E27" s="5" t="s">
         <v>1088</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="F27" s="5" t="s">
         <v>1089</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="G27" s="5" t="s">
         <v>1090</v>
       </c>
-      <c r="G27" s="5" t="s">
+      <c r="H27" s="5" t="s">
         <v>1091</v>
       </c>
-      <c r="H27" s="5" t="s">
+      <c r="I27" s="9" t="s">
+        <v>1087</v>
+      </c>
+      <c r="J27" s="5" t="s">
         <v>1092</v>
       </c>
-      <c r="I27" s="9" t="s">
-        <v>1088</v>
-      </c>
-      <c r="J27" s="5" t="s">
+      <c r="K27" s="5" t="s">
         <v>1093</v>
       </c>
-      <c r="K27" s="5" t="s">
+      <c r="L27" s="5" t="s">
         <v>1094</v>
       </c>
-      <c r="L27" s="5" t="s">
+      <c r="M27" s="5" t="s">
         <v>1095</v>
-      </c>
-      <c r="M27" s="5" t="s">
-        <v>1096</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
@@ -5476,38 +5479,38 @@
         <v>468</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="9" t="s">
+        <v>673</v>
+      </c>
+      <c r="E28" s="6" t="s">
         <v>674</v>
       </c>
-      <c r="E28" s="6" t="s">
+      <c r="F28" s="5" t="s">
         <v>675</v>
       </c>
-      <c r="F28" s="5" t="s">
+      <c r="G28" s="5" t="s">
         <v>676</v>
       </c>
-      <c r="G28" s="5" t="s">
+      <c r="H28" s="5" t="s">
         <v>677</v>
       </c>
-      <c r="H28" s="5" t="s">
+      <c r="I28" s="9" t="s">
+        <v>673</v>
+      </c>
+      <c r="J28" s="5" t="s">
         <v>678</v>
       </c>
-      <c r="I28" s="9" t="s">
-        <v>674</v>
-      </c>
-      <c r="J28" s="5" t="s">
+      <c r="K28" s="5" t="s">
         <v>679</v>
       </c>
-      <c r="K28" s="5" t="s">
+      <c r="L28" s="5" t="s">
         <v>680</v>
       </c>
-      <c r="L28" s="5" t="s">
+      <c r="M28" s="5" t="s">
         <v>681</v>
-      </c>
-      <c r="M28" s="5" t="s">
-        <v>682</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
@@ -5515,38 +5518,38 @@
         <v>593</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="9" t="s">
+        <v>683</v>
+      </c>
+      <c r="E29" s="6" t="s">
         <v>684</v>
       </c>
-      <c r="E29" s="6" t="s">
+      <c r="F29" s="5" t="s">
         <v>685</v>
       </c>
-      <c r="F29" s="5" t="s">
+      <c r="G29" s="5" t="s">
         <v>686</v>
       </c>
-      <c r="G29" s="5" t="s">
+      <c r="H29" s="5" t="s">
         <v>687</v>
       </c>
-      <c r="H29" s="5" t="s">
+      <c r="I29" s="9" t="s">
+        <v>683</v>
+      </c>
+      <c r="J29" s="5" t="s">
         <v>688</v>
       </c>
-      <c r="I29" s="9" t="s">
-        <v>684</v>
-      </c>
-      <c r="J29" s="5" t="s">
+      <c r="K29" s="5" t="s">
         <v>689</v>
       </c>
-      <c r="K29" s="5" t="s">
+      <c r="L29" s="5" t="s">
         <v>690</v>
       </c>
-      <c r="L29" s="5" t="s">
+      <c r="M29" s="5" t="s">
         <v>691</v>
-      </c>
-      <c r="M29" s="5" t="s">
-        <v>692</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
@@ -5554,77 +5557,77 @@
         <v>611</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="9" t="s">
+        <v>719</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>733</v>
+      </c>
+      <c r="F30" s="5" t="s">
         <v>720</v>
       </c>
-      <c r="E30" s="6" t="s">
+      <c r="G30" s="5" t="s">
+        <v>721</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>722</v>
+      </c>
+      <c r="I30" s="9" t="s">
+        <v>719</v>
+      </c>
+      <c r="J30" s="5" t="s">
+        <v>723</v>
+      </c>
+      <c r="K30" s="5" t="s">
+        <v>724</v>
+      </c>
+      <c r="L30" s="5" t="s">
         <v>734</v>
       </c>
-      <c r="F30" s="5" t="s">
-        <v>721</v>
-      </c>
-      <c r="G30" s="5" t="s">
-        <v>722</v>
-      </c>
-      <c r="H30" s="5" t="s">
-        <v>723</v>
-      </c>
-      <c r="I30" s="9" t="s">
-        <v>720</v>
-      </c>
-      <c r="J30" s="5" t="s">
-        <v>724</v>
-      </c>
-      <c r="K30" s="5" t="s">
+      <c r="M30" s="5" t="s">
         <v>725</v>
-      </c>
-      <c r="L30" s="5" t="s">
-        <v>735</v>
-      </c>
-      <c r="M30" s="5" t="s">
-        <v>726</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="9" t="s">
+        <v>719</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>731</v>
+      </c>
+      <c r="F31" s="5" t="s">
         <v>720</v>
       </c>
-      <c r="E31" s="6" t="s">
-        <v>732</v>
-      </c>
-      <c r="F31" s="5" t="s">
+      <c r="G31" s="5" t="s">
         <v>721</v>
       </c>
-      <c r="G31" s="5" t="s">
+      <c r="H31" s="5" t="s">
         <v>722</v>
       </c>
-      <c r="H31" s="5" t="s">
+      <c r="I31" s="9" t="s">
+        <v>719</v>
+      </c>
+      <c r="J31" s="5" t="s">
         <v>723</v>
       </c>
-      <c r="I31" s="9" t="s">
-        <v>720</v>
-      </c>
-      <c r="J31" s="5" t="s">
+      <c r="K31" s="5" t="s">
         <v>724</v>
       </c>
-      <c r="K31" s="5" t="s">
+      <c r="L31" s="5" t="s">
+        <v>735</v>
+      </c>
+      <c r="M31" s="5" t="s">
         <v>725</v>
-      </c>
-      <c r="L31" s="5" t="s">
-        <v>736</v>
-      </c>
-      <c r="M31" s="5" t="s">
-        <v>726</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
@@ -5632,38 +5635,38 @@
         <v>620</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="9" t="s">
+        <v>932</v>
+      </c>
+      <c r="E32" s="6" t="s">
         <v>933</v>
       </c>
-      <c r="E32" s="6" t="s">
+      <c r="F32" s="5" t="s">
         <v>934</v>
       </c>
-      <c r="F32" s="5" t="s">
+      <c r="G32" s="5" t="s">
         <v>935</v>
       </c>
-      <c r="G32" s="5" t="s">
+      <c r="H32" s="5" t="s">
         <v>936</v>
       </c>
-      <c r="H32" s="5" t="s">
+      <c r="I32" s="9" t="s">
+        <v>932</v>
+      </c>
+      <c r="J32" s="5" t="s">
         <v>937</v>
       </c>
-      <c r="I32" s="9" t="s">
-        <v>933</v>
-      </c>
-      <c r="J32" s="5" t="s">
+      <c r="K32" s="5" t="s">
         <v>938</v>
       </c>
-      <c r="K32" s="5" t="s">
+      <c r="L32" s="5" t="s">
         <v>939</v>
       </c>
-      <c r="L32" s="5" t="s">
+      <c r="M32" s="5" t="s">
         <v>940</v>
-      </c>
-      <c r="M32" s="5" t="s">
-        <v>941</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
@@ -5671,38 +5674,38 @@
         <v>629</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="9" t="s">
+        <v>942</v>
+      </c>
+      <c r="E33" s="6" t="s">
         <v>943</v>
       </c>
-      <c r="E33" s="6" t="s">
+      <c r="F33" s="5" t="s">
         <v>944</v>
       </c>
-      <c r="F33" s="5" t="s">
+      <c r="G33" s="5" t="s">
         <v>945</v>
       </c>
-      <c r="G33" s="5" t="s">
+      <c r="H33" s="5" t="s">
         <v>946</v>
       </c>
-      <c r="H33" s="5" t="s">
+      <c r="I33" s="9" t="s">
+        <v>942</v>
+      </c>
+      <c r="J33" s="5" t="s">
         <v>947</v>
       </c>
-      <c r="I33" s="9" t="s">
-        <v>943</v>
-      </c>
-      <c r="J33" s="5" t="s">
+      <c r="K33" s="5" t="s">
         <v>948</v>
       </c>
-      <c r="K33" s="5" t="s">
+      <c r="L33" s="5" t="s">
         <v>949</v>
       </c>
-      <c r="L33" s="5" t="s">
+      <c r="M33" s="5" t="s">
         <v>950</v>
-      </c>
-      <c r="M33" s="5" t="s">
-        <v>951</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
@@ -5710,38 +5713,38 @@
         <v>547</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="9" t="s">
+        <v>952</v>
+      </c>
+      <c r="E34" s="6" t="s">
         <v>953</v>
       </c>
-      <c r="E34" s="6" t="s">
+      <c r="F34" s="5" t="s">
         <v>954</v>
       </c>
-      <c r="F34" s="5" t="s">
+      <c r="G34" s="5" t="s">
         <v>955</v>
       </c>
-      <c r="G34" s="5" t="s">
+      <c r="H34" s="5" t="s">
         <v>956</v>
       </c>
-      <c r="H34" s="5" t="s">
+      <c r="I34" s="9" t="s">
+        <v>952</v>
+      </c>
+      <c r="J34" s="5" t="s">
         <v>957</v>
       </c>
-      <c r="I34" s="9" t="s">
-        <v>953</v>
-      </c>
-      <c r="J34" s="5" t="s">
+      <c r="K34" s="5" t="s">
         <v>958</v>
       </c>
-      <c r="K34" s="5" t="s">
+      <c r="L34" s="5" t="s">
         <v>959</v>
       </c>
-      <c r="L34" s="5" t="s">
+      <c r="M34" s="5" t="s">
         <v>960</v>
-      </c>
-      <c r="M34" s="5" t="s">
-        <v>961</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
@@ -5749,315 +5752,315 @@
         <v>556</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="C35" s="5"/>
       <c r="D35" s="9" t="s">
+        <v>962</v>
+      </c>
+      <c r="E35" s="6" t="s">
         <v>963</v>
       </c>
-      <c r="E35" s="6" t="s">
+      <c r="F35" s="5" t="s">
         <v>964</v>
       </c>
-      <c r="F35" s="5" t="s">
+      <c r="G35" s="5" t="s">
         <v>965</v>
       </c>
-      <c r="G35" s="5" t="s">
+      <c r="H35" s="5" t="s">
         <v>966</v>
       </c>
-      <c r="H35" s="5" t="s">
+      <c r="I35" s="9" t="s">
+        <v>962</v>
+      </c>
+      <c r="J35" s="5" t="s">
         <v>967</v>
       </c>
-      <c r="I35" s="9" t="s">
-        <v>963</v>
-      </c>
-      <c r="J35" s="5" t="s">
+      <c r="K35" s="5" t="s">
         <v>968</v>
       </c>
-      <c r="K35" s="5" t="s">
+      <c r="L35" s="5" t="s">
         <v>969</v>
       </c>
-      <c r="L35" s="5" t="s">
+      <c r="M35" s="5" t="s">
         <v>970</v>
-      </c>
-      <c r="M35" s="5" t="s">
-        <v>971</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
+        <v>971</v>
+      </c>
+      <c r="B36" s="5" t="s">
         <v>972</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>973</v>
       </c>
       <c r="C36" s="5"/>
       <c r="D36" s="9" t="s">
+        <v>973</v>
+      </c>
+      <c r="E36" s="6" t="s">
         <v>974</v>
       </c>
-      <c r="E36" s="6" t="s">
+      <c r="F36" s="5" t="s">
         <v>975</v>
       </c>
-      <c r="F36" s="5" t="s">
+      <c r="G36" s="5" t="s">
         <v>976</v>
       </c>
-      <c r="G36" s="5" t="s">
+      <c r="H36" s="5" t="s">
         <v>977</v>
       </c>
-      <c r="H36" s="5" t="s">
+      <c r="I36" s="9" t="s">
+        <v>973</v>
+      </c>
+      <c r="J36" s="5" t="s">
         <v>978</v>
       </c>
-      <c r="I36" s="9" t="s">
-        <v>974</v>
-      </c>
-      <c r="J36" s="5" t="s">
+      <c r="K36" s="5" t="s">
         <v>979</v>
       </c>
-      <c r="K36" s="5" t="s">
+      <c r="L36" s="5" t="s">
         <v>980</v>
       </c>
-      <c r="L36" s="5" t="s">
+      <c r="M36" s="5" t="s">
         <v>981</v>
-      </c>
-      <c r="M36" s="5" t="s">
-        <v>982</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
+        <v>1096</v>
+      </c>
+      <c r="B37" s="5" t="s">
         <v>1097</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>1098</v>
       </c>
       <c r="C37" s="5"/>
       <c r="D37" s="9" t="s">
+        <v>1098</v>
+      </c>
+      <c r="E37" s="5" t="s">
         <v>1099</v>
       </c>
-      <c r="E37" s="5" t="s">
+      <c r="F37" s="5" t="s">
         <v>1100</v>
       </c>
-      <c r="F37" s="5" t="s">
+      <c r="G37" s="5" t="s">
         <v>1101</v>
       </c>
-      <c r="G37" s="5" t="s">
+      <c r="H37" s="5" t="s">
         <v>1102</v>
       </c>
-      <c r="H37" s="5" t="s">
+      <c r="I37" s="9" t="s">
+        <v>1098</v>
+      </c>
+      <c r="J37" s="5" t="s">
         <v>1103</v>
       </c>
-      <c r="I37" s="9" t="s">
-        <v>1099</v>
-      </c>
-      <c r="J37" s="5" t="s">
+      <c r="K37" s="5" t="s">
         <v>1104</v>
       </c>
-      <c r="K37" s="5" t="s">
+      <c r="L37" s="5" t="s">
         <v>1105</v>
       </c>
-      <c r="L37" s="5" t="s">
+      <c r="M37" s="5" t="s">
         <v>1106</v>
-      </c>
-      <c r="M37" s="5" t="s">
-        <v>1107</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
+        <v>736</v>
+      </c>
+      <c r="B38" s="5" t="s">
         <v>737</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>738</v>
       </c>
       <c r="C38" s="5"/>
       <c r="D38" s="9" t="s">
+        <v>738</v>
+      </c>
+      <c r="E38" s="6" t="s">
         <v>739</v>
       </c>
-      <c r="E38" s="6" t="s">
+      <c r="F38" s="5" t="s">
         <v>740</v>
       </c>
-      <c r="F38" s="5" t="s">
+      <c r="G38" s="5" t="s">
         <v>741</v>
       </c>
-      <c r="G38" s="5" t="s">
+      <c r="H38" s="5" t="s">
         <v>742</v>
       </c>
-      <c r="H38" s="5" t="s">
+      <c r="I38" s="9" t="s">
+        <v>738</v>
+      </c>
+      <c r="J38" s="5" t="s">
         <v>743</v>
       </c>
-      <c r="I38" s="9" t="s">
-        <v>739</v>
-      </c>
-      <c r="J38" s="5" t="s">
+      <c r="K38" s="5" t="s">
         <v>744</v>
       </c>
-      <c r="K38" s="5" t="s">
+      <c r="L38" s="5" t="s">
         <v>745</v>
       </c>
-      <c r="L38" s="5" t="s">
+      <c r="M38" s="5" t="s">
         <v>746</v>
-      </c>
-      <c r="M38" s="5" t="s">
-        <v>747</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
+        <v>769</v>
+      </c>
+      <c r="B39" s="5" t="s">
         <v>770</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>771</v>
       </c>
       <c r="C39" s="5"/>
       <c r="D39" s="9" t="s">
+        <v>771</v>
+      </c>
+      <c r="E39" s="6" t="s">
         <v>772</v>
       </c>
-      <c r="E39" s="6" t="s">
+      <c r="F39" s="5" t="s">
         <v>773</v>
       </c>
-      <c r="F39" s="5" t="s">
+      <c r="G39" s="5" t="s">
         <v>774</v>
       </c>
-      <c r="G39" s="5" t="s">
+      <c r="H39" s="5" t="s">
         <v>775</v>
       </c>
-      <c r="H39" s="5" t="s">
+      <c r="I39" s="9" t="s">
+        <v>771</v>
+      </c>
+      <c r="J39" s="5" t="s">
         <v>776</v>
       </c>
-      <c r="I39" s="9" t="s">
-        <v>772</v>
-      </c>
-      <c r="J39" s="5" t="s">
+      <c r="K39" s="5" t="s">
         <v>777</v>
       </c>
-      <c r="K39" s="5" t="s">
+      <c r="L39" s="5" t="s">
         <v>778</v>
       </c>
-      <c r="L39" s="5" t="s">
+      <c r="M39" s="5" t="s">
         <v>779</v>
       </c>
-      <c r="M39" s="5" t="s">
-        <v>780</v>
-      </c>
       <c r="N39" s="5" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
+        <v>782</v>
+      </c>
+      <c r="B40" s="5" t="s">
         <v>783</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>784</v>
       </c>
       <c r="C40" s="5"/>
       <c r="D40" s="9" t="s">
+        <v>784</v>
+      </c>
+      <c r="E40" s="6" t="s">
         <v>785</v>
       </c>
-      <c r="E40" s="6" t="s">
+      <c r="F40" s="5" t="s">
         <v>786</v>
       </c>
-      <c r="F40" s="5" t="s">
+      <c r="G40" s="5" t="s">
         <v>787</v>
       </c>
-      <c r="G40" s="5" t="s">
+      <c r="H40" s="5" t="s">
         <v>788</v>
       </c>
-      <c r="H40" s="5" t="s">
+      <c r="I40" s="9" t="s">
+        <v>784</v>
+      </c>
+      <c r="J40" s="5" t="s">
         <v>789</v>
       </c>
-      <c r="I40" s="9" t="s">
-        <v>785</v>
-      </c>
-      <c r="J40" s="5" t="s">
+      <c r="K40" s="5" t="s">
         <v>790</v>
       </c>
-      <c r="K40" s="5" t="s">
+      <c r="L40" s="5" t="s">
         <v>791</v>
       </c>
-      <c r="L40" s="5" t="s">
+      <c r="M40" s="5" t="s">
         <v>792</v>
-      </c>
-      <c r="M40" s="5" t="s">
-        <v>793</v>
       </c>
       <c r="N40" s="5"/>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="11" t="s">
+        <v>747</v>
+      </c>
+      <c r="B41" s="5" t="s">
         <v>748</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>749</v>
       </c>
       <c r="C41" s="5"/>
       <c r="D41" s="9" t="s">
+        <v>749</v>
+      </c>
+      <c r="E41" s="6" t="s">
         <v>750</v>
       </c>
-      <c r="E41" s="6" t="s">
+      <c r="F41" s="5" t="s">
         <v>751</v>
       </c>
-      <c r="F41" s="5" t="s">
+      <c r="G41" s="5" t="s">
         <v>752</v>
       </c>
-      <c r="G41" s="5" t="s">
+      <c r="H41" s="5" t="s">
         <v>753</v>
       </c>
-      <c r="H41" s="5" t="s">
+      <c r="I41" s="9" t="s">
+        <v>749</v>
+      </c>
+      <c r="J41" s="5" t="s">
         <v>754</v>
       </c>
-      <c r="I41" s="9" t="s">
-        <v>750</v>
-      </c>
-      <c r="J41" s="5" t="s">
+      <c r="K41" s="5" t="s">
         <v>755</v>
       </c>
-      <c r="K41" s="5" t="s">
+      <c r="L41" s="5" t="s">
         <v>756</v>
       </c>
-      <c r="L41" s="5" t="s">
+      <c r="M41" s="5" t="s">
         <v>757</v>
-      </c>
-      <c r="M41" s="5" t="s">
-        <v>758</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
+        <v>758</v>
+      </c>
+      <c r="B42" s="5" t="s">
         <v>759</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>760</v>
       </c>
       <c r="C42" s="5"/>
       <c r="D42" s="9" t="s">
+        <v>760</v>
+      </c>
+      <c r="E42" s="6" t="s">
         <v>761</v>
       </c>
-      <c r="E42" s="6" t="s">
+      <c r="F42" s="5" t="s">
         <v>762</v>
       </c>
-      <c r="F42" s="5" t="s">
+      <c r="G42" s="5" t="s">
         <v>763</v>
       </c>
-      <c r="G42" s="5" t="s">
+      <c r="H42" s="5" t="s">
         <v>764</v>
       </c>
-      <c r="H42" s="5" t="s">
+      <c r="I42" s="9" t="s">
+        <v>760</v>
+      </c>
+      <c r="J42" s="5" t="s">
         <v>765</v>
       </c>
-      <c r="I42" s="9" t="s">
-        <v>761</v>
-      </c>
-      <c r="J42" s="5" t="s">
+      <c r="K42" s="5" t="s">
         <v>766</v>
       </c>
-      <c r="K42" s="5" t="s">
+      <c r="L42" s="5" t="s">
         <v>767</v>
       </c>
-      <c r="L42" s="5" t="s">
+      <c r="M42" s="5" t="s">
         <v>768</v>
-      </c>
-      <c r="M42" s="5" t="s">
-        <v>769</v>
       </c>
     </row>
   </sheetData>
@@ -6135,31 +6138,32 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="FXRates_Fields"/>
-  <dimension ref="A1:O36"/>
+  <dimension ref="A1:P36"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="43.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="34.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="40.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="40.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="66.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="61.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="45.85546875" customWidth="1"/>
+    <col min="11" max="11" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -6167,46 +6171,49 @@
         <v>17</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>1115</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="O1" s="4" t="s">
-        <v>1108</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="P1" s="4" t="s">
+        <v>1107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -6214,1555 +6221,1593 @@
         <v>44</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="D2" s="5" t="s">
+        <v>1118</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>1119</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="H2" s="9" t="s">
-        <v>666</v>
-      </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="9" t="s">
+        <v>1119</v>
+      </c>
+      <c r="J2" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="K2" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="L2" s="5" t="s">
         <v>241</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="M2" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="N2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="O2" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>22</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="5"/>
+      <c r="D3" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="E3" s="5" t="s">
         <v>244</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="F3" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="G3" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="H3" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="H3" s="9" t="s">
-        <v>667</v>
-      </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="J3" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="K3" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="L3" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="M3" s="5" t="s">
         <v>246</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="N3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="5" t="s">
+      <c r="O3" s="5" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>36</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="5"/>
+      <c r="D4" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="E4" s="5" t="s">
         <v>247</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="F4" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="G4" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="H4" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="H4" s="9" t="s">
-        <v>668</v>
-      </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="9" t="s">
+        <v>667</v>
+      </c>
+      <c r="J4" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="K4" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="L4" s="5" t="s">
         <v>248</v>
       </c>
-      <c r="L4" s="5" t="s">
+      <c r="M4" s="5" t="s">
         <v>249</v>
       </c>
-      <c r="M4" s="5" t="s">
+      <c r="N4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N4" s="5" t="s">
+      <c r="O4" s="5" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>43</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="5"/>
+      <c r="D5" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="E5" s="5" t="s">
         <v>250</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="F5" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="G5" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="H5" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="H5" s="9" t="s">
-        <v>669</v>
-      </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="9" t="s">
+        <v>668</v>
+      </c>
+      <c r="J5" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="K5" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="L5" s="5" t="s">
         <v>251</v>
       </c>
-      <c r="L5" s="5" t="s">
+      <c r="M5" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="M5" s="5" t="s">
+      <c r="N5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N5" s="5" t="s">
+      <c r="O5" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>49</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="5"/>
+      <c r="D6" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="E6" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="F6" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="G6" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="H6" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="H6" s="9" t="s">
-        <v>670</v>
-      </c>
-      <c r="I6" s="5" t="s">
+      <c r="I6" s="9" t="s">
+        <v>669</v>
+      </c>
+      <c r="J6" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="J6" s="5" t="s">
+      <c r="K6" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="K6" s="5" t="s">
+      <c r="L6" s="5" t="s">
         <v>254</v>
       </c>
-      <c r="L6" s="5" t="s">
+      <c r="M6" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="M6" s="5" t="s">
+      <c r="N6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N6" s="5" t="s">
+      <c r="O6" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>57</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="5"/>
+      <c r="D7" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="E7" s="5" t="s">
         <v>256</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="F7" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="G7" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="H7" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="H7" s="9" t="s">
-        <v>671</v>
-      </c>
-      <c r="I7" s="5" t="s">
+      <c r="I7" s="9" t="s">
+        <v>670</v>
+      </c>
+      <c r="J7" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="J7" s="5" t="s">
+      <c r="K7" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="K7" s="5" t="s">
+      <c r="L7" s="5" t="s">
         <v>257</v>
       </c>
-      <c r="L7" s="5" t="s">
+      <c r="M7" s="5" t="s">
         <v>258</v>
       </c>
-      <c r="M7" s="5" t="s">
+      <c r="N7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N7" s="5" t="s">
+      <c r="O7" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>64</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>259</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="5"/>
+      <c r="D8" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>1013</v>
-      </c>
       <c r="E8" s="5" t="s">
+        <v>1012</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>260</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="G8" s="5" t="s">
         <v>261</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="H8" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="H8" s="9" t="s">
-        <v>672</v>
-      </c>
-      <c r="I8" s="5" t="s">
+      <c r="I8" s="9" t="s">
+        <v>671</v>
+      </c>
+      <c r="J8" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="J8" s="5" t="s">
+      <c r="K8" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="K8" s="5" t="s">
+      <c r="L8" s="5" t="s">
         <v>265</v>
       </c>
-      <c r="L8" s="5" t="s">
+      <c r="M8" s="5" t="s">
         <v>266</v>
       </c>
-      <c r="M8" s="5" t="s">
+      <c r="N8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N8" s="5" t="s">
+      <c r="O8" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>96</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>267</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="5"/>
+      <c r="D9" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="D9" s="12" t="s">
-        <v>1014</v>
-      </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="12" t="s">
+        <v>1013</v>
+      </c>
+      <c r="F9" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="G9" s="5" t="s">
         <v>269</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="H9" s="5" t="s">
         <v>270</v>
       </c>
-      <c r="H9" s="9" t="s">
+      <c r="I9" s="9" t="s">
         <v>665</v>
       </c>
-      <c r="I9" s="5" t="s">
+      <c r="J9" s="5" t="s">
         <v>271</v>
       </c>
-      <c r="J9" s="5" t="s">
+      <c r="K9" s="5" t="s">
         <v>272</v>
       </c>
-      <c r="K9" s="5" t="s">
+      <c r="L9" s="5" t="s">
         <v>273</v>
       </c>
-      <c r="L9" s="5" t="s">
+      <c r="M9" s="5" t="s">
         <v>274</v>
       </c>
-      <c r="M9" s="5" t="s">
+      <c r="N9" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N9" s="5" t="s">
+      <c r="O9" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>103</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>275</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="5"/>
+      <c r="D10" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>1015</v>
-      </c>
       <c r="E10" s="5" t="s">
+        <v>1014</v>
+      </c>
+      <c r="F10" s="5" t="s">
         <v>276</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="G10" s="5" t="s">
         <v>277</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="H10" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="H10" s="9" t="s">
+      <c r="I10" s="9" t="s">
         <v>664</v>
       </c>
-      <c r="I10" s="5" t="s">
+      <c r="J10" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J10" s="5" t="s">
+      <c r="K10" s="5" t="s">
         <v>280</v>
       </c>
-      <c r="K10" s="5" t="s">
+      <c r="L10" s="5" t="s">
         <v>281</v>
       </c>
-      <c r="L10" s="5" t="s">
+      <c r="M10" s="5" t="s">
         <v>282</v>
       </c>
-      <c r="M10" s="5" t="s">
+      <c r="N10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N10" s="5" t="s">
+      <c r="O10" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>111</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>283</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="5"/>
+      <c r="D11" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>1016</v>
-      </c>
       <c r="E11" s="5" t="s">
+        <v>1015</v>
+      </c>
+      <c r="F11" s="5" t="s">
         <v>284</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="G11" s="5" t="s">
         <v>285</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="H11" s="5" t="s">
         <v>286</v>
       </c>
-      <c r="H11" s="9" t="s">
+      <c r="I11" s="9" t="s">
         <v>655</v>
       </c>
-      <c r="I11" s="5" t="s">
+      <c r="J11" s="5" t="s">
         <v>287</v>
       </c>
-      <c r="J11" s="5" t="s">
+      <c r="K11" s="5" t="s">
         <v>288</v>
       </c>
-      <c r="K11" s="5" t="s">
+      <c r="L11" s="5" t="s">
         <v>289</v>
       </c>
-      <c r="L11" s="5" t="s">
+      <c r="M11" s="5" t="s">
         <v>290</v>
       </c>
-      <c r="M11" s="5" t="s">
+      <c r="N11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N11" s="5" t="s">
+      <c r="O11" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>113</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>291</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="5"/>
+      <c r="D12" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>1113</v>
-      </c>
       <c r="E12" s="5" t="s">
+        <v>1112</v>
+      </c>
+      <c r="F12" s="5" t="s">
         <v>292</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="G12" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="H12" s="5" t="s">
         <v>294</v>
       </c>
-      <c r="H12" s="9" t="s">
+      <c r="I12" s="9" t="s">
         <v>656</v>
       </c>
-      <c r="I12" s="5" t="s">
+      <c r="J12" s="5" t="s">
         <v>295</v>
       </c>
-      <c r="J12" s="5" t="s">
+      <c r="K12" s="5" t="s">
         <v>296</v>
       </c>
-      <c r="K12" s="5" t="s">
+      <c r="L12" s="5" t="s">
         <v>297</v>
       </c>
-      <c r="L12" s="5" t="s">
+      <c r="M12" s="5" t="s">
         <v>298</v>
       </c>
-      <c r="M12" s="5" t="s">
+      <c r="N12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N12" s="5" t="s">
+      <c r="O12" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>115</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>299</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="5"/>
+      <c r="D13" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>1114</v>
-      </c>
       <c r="E13" s="5" t="s">
+        <v>1113</v>
+      </c>
+      <c r="F13" s="5" t="s">
         <v>300</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="G13" s="5" t="s">
         <v>301</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="H13" s="5" t="s">
         <v>302</v>
       </c>
-      <c r="H13" s="9" t="s">
+      <c r="I13" s="9" t="s">
         <v>657</v>
       </c>
-      <c r="I13" s="5" t="s">
+      <c r="J13" s="5" t="s">
         <v>303</v>
       </c>
-      <c r="J13" s="5" t="s">
+      <c r="K13" s="5" t="s">
         <v>304</v>
       </c>
-      <c r="K13" s="5" t="s">
+      <c r="L13" s="5" t="s">
         <v>305</v>
       </c>
-      <c r="L13" s="5" t="s">
+      <c r="M13" s="5" t="s">
         <v>306</v>
       </c>
-      <c r="M13" s="5" t="s">
+      <c r="N13" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N13" s="5" t="s">
+      <c r="O13" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>117</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>307</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="5"/>
+      <c r="D14" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="D14" s="5" t="s">
-        <v>1115</v>
-      </c>
       <c r="E14" s="5" t="s">
+        <v>1114</v>
+      </c>
+      <c r="F14" s="5" t="s">
         <v>308</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="G14" s="5" t="s">
         <v>309</v>
       </c>
-      <c r="G14" s="5" t="s">
+      <c r="H14" s="5" t="s">
         <v>310</v>
       </c>
-      <c r="H14" s="9" t="s">
+      <c r="I14" s="9" t="s">
         <v>658</v>
       </c>
-      <c r="I14" s="5" t="s">
+      <c r="J14" s="5" t="s">
         <v>311</v>
       </c>
-      <c r="J14" s="5" t="s">
+      <c r="K14" s="5" t="s">
         <v>312</v>
       </c>
-      <c r="K14" s="5" t="s">
+      <c r="L14" s="5" t="s">
         <v>313</v>
       </c>
-      <c r="L14" s="5" t="s">
+      <c r="M14" s="5" t="s">
         <v>314</v>
       </c>
-      <c r="M14" s="5" t="s">
+      <c r="N14" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N14" s="5" t="s">
+      <c r="O14" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>119</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>315</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="5"/>
+      <c r="D15" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="E15" s="5" t="s">
         <v>316</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="F15" s="5" t="s">
         <v>317</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="G15" s="5" t="s">
         <v>318</v>
       </c>
-      <c r="G15" s="5" t="s">
+      <c r="H15" s="5" t="s">
         <v>319</v>
       </c>
-      <c r="H15" s="9" t="s">
+      <c r="I15" s="9" t="s">
         <v>659</v>
       </c>
-      <c r="I15" s="5" t="s">
+      <c r="J15" s="5" t="s">
         <v>320</v>
       </c>
-      <c r="J15" s="5" t="s">
+      <c r="K15" s="5" t="s">
         <v>321</v>
       </c>
-      <c r="K15" s="5" t="s">
+      <c r="L15" s="5" t="s">
         <v>322</v>
       </c>
-      <c r="L15" s="5" t="s">
+      <c r="M15" s="5" t="s">
         <v>323</v>
       </c>
-      <c r="M15" s="5" t="s">
+      <c r="N15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N15" s="5" t="s">
+      <c r="O15" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>146</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>324</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="5"/>
+      <c r="D16" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="E16" s="5" t="s">
         <v>325</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="F16" s="5" t="s">
         <v>326</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="G16" s="5" t="s">
         <v>327</v>
       </c>
-      <c r="G16" s="5" t="s">
+      <c r="H16" s="5" t="s">
         <v>328</v>
       </c>
-      <c r="H16" s="9" t="s">
+      <c r="I16" s="9" t="s">
         <v>660</v>
       </c>
-      <c r="I16" s="5" t="s">
+      <c r="J16" s="5" t="s">
         <v>329</v>
       </c>
-      <c r="J16" s="5" t="s">
+      <c r="K16" s="5" t="s">
         <v>330</v>
       </c>
-      <c r="K16" s="5" t="s">
+      <c r="L16" s="5" t="s">
         <v>331</v>
       </c>
-      <c r="L16" s="5" t="s">
+      <c r="M16" s="5" t="s">
         <v>332</v>
       </c>
-      <c r="M16" s="5" t="s">
+      <c r="N16" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N16" s="5" t="s">
+      <c r="O16" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>333</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>334</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="5"/>
+      <c r="D17" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="E17" s="5" t="s">
         <v>335</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="F17" s="5" t="s">
         <v>336</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="G17" s="5" t="s">
         <v>337</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="H17" s="5" t="s">
         <v>338</v>
       </c>
-      <c r="H17" s="9" t="s">
+      <c r="I17" s="9" t="s">
         <v>661</v>
       </c>
-      <c r="I17" s="5" t="s">
+      <c r="J17" s="5" t="s">
         <v>339</v>
       </c>
-      <c r="J17" s="5" t="s">
+      <c r="K17" s="5" t="s">
         <v>340</v>
       </c>
-      <c r="K17" s="5" t="s">
+      <c r="L17" s="5" t="s">
         <v>341</v>
       </c>
-      <c r="L17" s="5" t="s">
+      <c r="M17" s="5" t="s">
         <v>342</v>
       </c>
-      <c r="M17" s="5" t="s">
+      <c r="N17" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N17" s="5" t="s">
+      <c r="O17" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>343</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>344</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="5"/>
+      <c r="D18" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="E18" s="5" t="s">
         <v>345</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="F18" s="5" t="s">
         <v>346</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="G18" s="5" t="s">
         <v>347</v>
       </c>
-      <c r="G18" s="5" t="s">
+      <c r="H18" s="5" t="s">
         <v>348</v>
       </c>
-      <c r="H18" s="9" t="s">
+      <c r="I18" s="9" t="s">
         <v>662</v>
       </c>
-      <c r="I18" s="5" t="s">
+      <c r="J18" s="5" t="s">
         <v>349</v>
       </c>
-      <c r="J18" s="5" t="s">
+      <c r="K18" s="5" t="s">
         <v>350</v>
       </c>
-      <c r="K18" s="5" t="s">
+      <c r="L18" s="5" t="s">
         <v>351</v>
       </c>
-      <c r="L18" s="5" t="s">
+      <c r="M18" s="5" t="s">
         <v>352</v>
       </c>
-      <c r="M18" s="5" t="s">
+      <c r="N18" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N18" s="5" t="s">
+      <c r="O18" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>353</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>354</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="5"/>
+      <c r="D19" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="E19" s="5" t="s">
         <v>355</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="F19" s="5" t="s">
         <v>356</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="G19" s="5" t="s">
         <v>357</v>
       </c>
-      <c r="G19" s="5" t="s">
+      <c r="H19" s="5" t="s">
         <v>358</v>
       </c>
-      <c r="H19" s="9" t="s">
+      <c r="I19" s="9" t="s">
         <v>663</v>
       </c>
-      <c r="I19" s="5" t="s">
+      <c r="J19" s="5" t="s">
         <v>359</v>
       </c>
-      <c r="J19" s="5" t="s">
+      <c r="K19" s="5" t="s">
         <v>360</v>
       </c>
-      <c r="K19" s="5" t="s">
+      <c r="L19" s="5" t="s">
         <v>361</v>
       </c>
-      <c r="L19" s="5" t="s">
+      <c r="M19" s="5" t="s">
         <v>362</v>
       </c>
-      <c r="M19" s="5" t="s">
+      <c r="N19" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N19" s="5" t="s">
+      <c r="O19" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>169</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>363</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="5"/>
+      <c r="D20" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="E20" s="5" t="s">
         <v>364</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="F20" s="5" t="s">
         <v>365</v>
       </c>
-      <c r="F20" s="5" t="s">
+      <c r="G20" s="5" t="s">
         <v>366</v>
       </c>
-      <c r="G20" s="5" t="s">
+      <c r="H20" s="5" t="s">
         <v>367</v>
       </c>
-      <c r="H20" s="9" t="s">
+      <c r="I20" s="9" t="s">
         <v>654</v>
       </c>
-      <c r="I20" s="5" t="s">
+      <c r="J20" s="5" t="s">
         <v>368</v>
       </c>
-      <c r="J20" s="5" t="s">
+      <c r="K20" s="5" t="s">
         <v>369</v>
       </c>
-      <c r="K20" s="5" t="s">
+      <c r="L20" s="5" t="s">
         <v>370</v>
       </c>
-      <c r="L20" s="5" t="s">
+      <c r="M20" s="5" t="s">
         <v>371</v>
       </c>
-      <c r="M20" s="5" t="s">
+      <c r="N20" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N20" s="5" t="s">
+      <c r="O20" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="O20" s="5" t="s">
-        <v>1109</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="P20" s="5" t="s">
+        <v>1108</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>210</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>372</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="5"/>
+      <c r="D21" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="E21" s="5" t="s">
         <v>373</v>
       </c>
-      <c r="E21" s="5" t="s">
+      <c r="F21" s="5" t="s">
         <v>374</v>
       </c>
-      <c r="F21" s="5" t="s">
+      <c r="G21" s="5" t="s">
         <v>375</v>
       </c>
-      <c r="G21" s="5" t="s">
+      <c r="H21" s="5" t="s">
         <v>376</v>
       </c>
-      <c r="H21" s="9" t="s">
+      <c r="I21" s="9" t="s">
         <v>645</v>
       </c>
-      <c r="I21" s="5" t="s">
+      <c r="J21" s="5" t="s">
         <v>377</v>
       </c>
-      <c r="J21" s="5" t="s">
+      <c r="K21" s="5" t="s">
         <v>378</v>
       </c>
-      <c r="K21" s="5" t="s">
+      <c r="L21" s="5" t="s">
         <v>379</v>
       </c>
-      <c r="L21" s="5" t="s">
+      <c r="M21" s="5" t="s">
         <v>380</v>
       </c>
-      <c r="M21" s="5" t="s">
+      <c r="N21" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N21" s="5" t="s">
+      <c r="O21" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>230</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>381</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="5"/>
+      <c r="D22" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="E22" s="5" t="s">
         <v>382</v>
       </c>
-      <c r="E22" s="5" t="s">
+      <c r="F22" s="5" t="s">
         <v>383</v>
       </c>
-      <c r="F22" s="5" t="s">
+      <c r="G22" s="5" t="s">
         <v>384</v>
       </c>
-      <c r="G22" s="5" t="s">
+      <c r="H22" s="5" t="s">
         <v>385</v>
       </c>
-      <c r="H22" s="9" t="s">
+      <c r="I22" s="9" t="s">
         <v>646</v>
       </c>
-      <c r="I22" s="5" t="s">
+      <c r="J22" s="5" t="s">
         <v>386</v>
       </c>
-      <c r="J22" s="5" t="s">
+      <c r="K22" s="5" t="s">
         <v>387</v>
       </c>
-      <c r="K22" s="5" t="s">
+      <c r="L22" s="5" t="s">
         <v>388</v>
       </c>
-      <c r="L22" s="5" t="s">
+      <c r="M22" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="M22" s="5" t="s">
+      <c r="N22" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N22" s="5" t="s">
+      <c r="O22" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>232</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>390</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="C23" s="5"/>
+      <c r="D23" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="E23" s="5" t="s">
         <v>391</v>
       </c>
-      <c r="E23" s="5" t="s">
+      <c r="F23" s="5" t="s">
         <v>392</v>
       </c>
-      <c r="F23" s="5" t="s">
+      <c r="G23" s="5" t="s">
         <v>393</v>
       </c>
-      <c r="G23" s="5" t="s">
+      <c r="H23" s="5" t="s">
         <v>394</v>
       </c>
-      <c r="H23" s="9" t="s">
+      <c r="I23" s="9" t="s">
         <v>647</v>
       </c>
-      <c r="I23" s="5" t="s">
+      <c r="J23" s="5" t="s">
         <v>395</v>
       </c>
-      <c r="J23" s="5" t="s">
+      <c r="K23" s="5" t="s">
         <v>396</v>
       </c>
-      <c r="K23" s="5" t="s">
+      <c r="L23" s="5" t="s">
         <v>397</v>
       </c>
-      <c r="L23" s="5" t="s">
+      <c r="M23" s="5" t="s">
         <v>398</v>
       </c>
-      <c r="M23" s="5" t="s">
+      <c r="N23" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N23" s="5" t="s">
+      <c r="O23" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>399</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>400</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="C24" s="5"/>
+      <c r="D24" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="E24" s="5" t="s">
         <v>401</v>
       </c>
-      <c r="E24" s="5" t="s">
+      <c r="F24" s="5" t="s">
         <v>402</v>
       </c>
-      <c r="F24" s="5" t="s">
+      <c r="G24" s="5" t="s">
         <v>403</v>
       </c>
-      <c r="G24" s="5" t="s">
+      <c r="H24" s="5" t="s">
         <v>404</v>
       </c>
-      <c r="H24" s="9" t="s">
+      <c r="I24" s="9" t="s">
         <v>648</v>
       </c>
-      <c r="I24" s="5" t="s">
+      <c r="J24" s="5" t="s">
         <v>405</v>
       </c>
-      <c r="J24" s="5" t="s">
+      <c r="K24" s="5" t="s">
         <v>406</v>
       </c>
-      <c r="K24" s="5" t="s">
+      <c r="L24" s="5" t="s">
         <v>407</v>
       </c>
-      <c r="L24" s="5" t="s">
+      <c r="M24" s="5" t="s">
         <v>408</v>
       </c>
-      <c r="M24" s="5" t="s">
+      <c r="N24" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N24" s="5" t="s">
+      <c r="O24" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>409</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>410</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="C25" s="5"/>
+      <c r="D25" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="E25" s="5" t="s">
         <v>411</v>
       </c>
-      <c r="E25" s="5" t="s">
+      <c r="F25" s="5" t="s">
         <v>412</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="G25" s="5" t="s">
         <v>413</v>
       </c>
-      <c r="G25" s="5" t="s">
+      <c r="H25" s="5" t="s">
         <v>414</v>
       </c>
-      <c r="H25" s="9" t="s">
+      <c r="I25" s="9" t="s">
         <v>649</v>
       </c>
-      <c r="I25" s="5" t="s">
+      <c r="J25" s="5" t="s">
         <v>415</v>
       </c>
-      <c r="J25" s="5" t="s">
+      <c r="K25" s="5" t="s">
         <v>416</v>
       </c>
-      <c r="K25" s="5" t="s">
+      <c r="L25" s="5" t="s">
         <v>417</v>
       </c>
-      <c r="L25" s="5" t="s">
+      <c r="M25" s="5" t="s">
         <v>418</v>
       </c>
-      <c r="M25" s="5" t="s">
+      <c r="N25" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N25" s="5" t="s">
+      <c r="O25" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>419</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>420</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="C26" s="5"/>
+      <c r="D26" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="E26" s="5" t="s">
         <v>478</v>
       </c>
-      <c r="E26" s="5" t="s">
+      <c r="F26" s="5" t="s">
         <v>421</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="G26" s="5" t="s">
         <v>422</v>
       </c>
-      <c r="G26" s="5" t="s">
+      <c r="H26" s="5" t="s">
         <v>423</v>
       </c>
-      <c r="H26" s="9" t="s">
+      <c r="I26" s="9" t="s">
         <v>650</v>
       </c>
-      <c r="I26" s="5" t="s">
+      <c r="J26" s="5" t="s">
         <v>424</v>
       </c>
-      <c r="J26" s="5" t="s">
+      <c r="K26" s="5" t="s">
         <v>425</v>
       </c>
-      <c r="K26" s="5" t="s">
+      <c r="L26" s="5" t="s">
         <v>426</v>
       </c>
-      <c r="L26" s="5" t="s">
+      <c r="M26" s="5" t="s">
         <v>427</v>
       </c>
-      <c r="M26" s="5" t="s">
+      <c r="N26" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N26" s="5" t="s">
+      <c r="O26" s="5" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>428</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>429</v>
       </c>
-      <c r="C27" s="9" t="s">
+      <c r="C27" s="5"/>
+      <c r="D27" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="E27" s="5" t="s">
         <v>430</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="F27" s="5" t="s">
         <v>431</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="G27" s="5" t="s">
         <v>432</v>
       </c>
-      <c r="G27" s="5" t="s">
+      <c r="H27" s="5" t="s">
         <v>433</v>
       </c>
-      <c r="H27" s="9" t="s">
+      <c r="I27" s="9" t="s">
         <v>651</v>
       </c>
-      <c r="I27" s="5" t="s">
+      <c r="J27" s="5" t="s">
         <v>434</v>
       </c>
-      <c r="J27" s="5" t="s">
+      <c r="K27" s="5" t="s">
         <v>435</v>
       </c>
-      <c r="K27" s="5" t="s">
+      <c r="L27" s="5" t="s">
         <v>436</v>
       </c>
-      <c r="L27" s="5" t="s">
+      <c r="M27" s="5" t="s">
         <v>437</v>
       </c>
-      <c r="M27" s="5" t="s">
+      <c r="N27" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N27" s="5" t="s">
+      <c r="O27" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>438</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>439</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="C28" s="5"/>
+      <c r="D28" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="E28" s="5" t="s">
         <v>440</v>
       </c>
-      <c r="E28" s="5" t="s">
+      <c r="F28" s="5" t="s">
         <v>441</v>
       </c>
-      <c r="F28" s="5" t="s">
+      <c r="G28" s="5" t="s">
         <v>442</v>
       </c>
-      <c r="G28" s="5" t="s">
+      <c r="H28" s="5" t="s">
         <v>443</v>
       </c>
-      <c r="H28" s="9" t="s">
+      <c r="I28" s="9" t="s">
         <v>652</v>
       </c>
-      <c r="I28" s="5" t="s">
+      <c r="J28" s="5" t="s">
         <v>444</v>
       </c>
-      <c r="J28" s="5" t="s">
+      <c r="K28" s="5" t="s">
         <v>445</v>
       </c>
-      <c r="K28" s="5" t="s">
+      <c r="L28" s="5" t="s">
         <v>446</v>
       </c>
-      <c r="L28" s="5" t="s">
+      <c r="M28" s="5" t="s">
         <v>447</v>
       </c>
-      <c r="M28" s="5" t="s">
+      <c r="N28" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N28" s="5" t="s">
+      <c r="O28" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>448</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>449</v>
       </c>
-      <c r="C29" s="9" t="s">
+      <c r="C29" s="5"/>
+      <c r="D29" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="E29" s="5" t="s">
         <v>450</v>
       </c>
-      <c r="E29" s="5" t="s">
+      <c r="F29" s="5" t="s">
         <v>451</v>
       </c>
-      <c r="F29" s="5" t="s">
+      <c r="G29" s="5" t="s">
         <v>452</v>
       </c>
-      <c r="G29" s="5" t="s">
+      <c r="H29" s="5" t="s">
         <v>453</v>
       </c>
-      <c r="H29" s="9" t="s">
+      <c r="I29" s="9" t="s">
         <v>653</v>
       </c>
-      <c r="I29" s="5" t="s">
+      <c r="J29" s="5" t="s">
         <v>454</v>
       </c>
-      <c r="J29" s="5" t="s">
+      <c r="K29" s="5" t="s">
         <v>455</v>
       </c>
-      <c r="K29" s="5" t="s">
+      <c r="L29" s="5" t="s">
         <v>456</v>
       </c>
-      <c r="L29" s="5" t="s">
+      <c r="M29" s="5" t="s">
         <v>457</v>
       </c>
-      <c r="M29" s="5" t="s">
+      <c r="N29" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N29" s="5" t="s">
+      <c r="O29" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>458</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>459</v>
       </c>
-      <c r="C30" s="9" t="s">
+      <c r="C30" s="5"/>
+      <c r="D30" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="E30" s="5" t="s">
         <v>460</v>
       </c>
-      <c r="E30" s="5" t="s">
+      <c r="F30" s="5" t="s">
         <v>461</v>
       </c>
-      <c r="F30" s="5" t="s">
+      <c r="G30" s="5" t="s">
         <v>462</v>
       </c>
-      <c r="G30" s="5" t="s">
+      <c r="H30" s="5" t="s">
         <v>463</v>
       </c>
-      <c r="H30" s="9" t="s">
+      <c r="I30" s="9" t="s">
         <v>644</v>
       </c>
-      <c r="I30" s="5" t="s">
+      <c r="J30" s="5" t="s">
         <v>464</v>
       </c>
-      <c r="J30" s="5" t="s">
+      <c r="K30" s="5" t="s">
         <v>465</v>
       </c>
-      <c r="K30" s="5" t="s">
+      <c r="L30" s="5" t="s">
         <v>466</v>
       </c>
-      <c r="L30" s="5" t="s">
+      <c r="M30" s="5" t="s">
         <v>467</v>
       </c>
-      <c r="M30" s="5" t="s">
+      <c r="N30" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N30" s="5" t="s">
+      <c r="O30" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>468</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>469</v>
       </c>
-      <c r="C31" s="9" t="s">
+      <c r="C31" s="5"/>
+      <c r="D31" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="E31" s="5" t="s">
         <v>470</v>
       </c>
-      <c r="E31" s="5" t="s">
+      <c r="F31" s="5" t="s">
         <v>471</v>
       </c>
-      <c r="F31" s="5" t="s">
+      <c r="G31" s="5" t="s">
         <v>472</v>
       </c>
-      <c r="G31" s="5" t="s">
+      <c r="H31" s="5" t="s">
         <v>473</v>
       </c>
-      <c r="H31" s="9" t="s">
+      <c r="I31" s="9" t="s">
         <v>643</v>
       </c>
-      <c r="I31" s="5" t="s">
+      <c r="J31" s="5" t="s">
         <v>474</v>
       </c>
-      <c r="J31" s="5" t="s">
+      <c r="K31" s="5" t="s">
         <v>475</v>
       </c>
-      <c r="K31" s="5" t="s">
+      <c r="L31" s="5" t="s">
         <v>476</v>
       </c>
-      <c r="L31" s="5" t="s">
+      <c r="M31" s="5" t="s">
         <v>477</v>
       </c>
-      <c r="M31" s="5" t="s">
+      <c r="N31" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N31" s="5" t="s">
+      <c r="O31" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>593</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>594</v>
       </c>
-      <c r="C32" s="9" t="s">
+      <c r="C32" s="5"/>
+      <c r="D32" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="D32" s="5" t="s">
-        <v>727</v>
-      </c>
       <c r="E32" s="5" t="s">
+        <v>726</v>
+      </c>
+      <c r="F32" s="5" t="s">
         <v>595</v>
       </c>
-      <c r="F32" s="5" t="s">
+      <c r="G32" s="5" t="s">
         <v>596</v>
       </c>
-      <c r="G32" s="5" t="s">
+      <c r="H32" s="5" t="s">
         <v>597</v>
       </c>
-      <c r="H32" s="9" t="s">
+      <c r="I32" s="9" t="s">
         <v>642</v>
       </c>
-      <c r="I32" s="5" t="s">
+      <c r="J32" s="5" t="s">
         <v>598</v>
       </c>
-      <c r="J32" s="5" t="s">
+      <c r="K32" s="5" t="s">
         <v>599</v>
       </c>
-      <c r="K32" s="5" t="s">
+      <c r="L32" s="5" t="s">
         <v>600</v>
       </c>
-      <c r="L32" s="5" t="s">
+      <c r="M32" s="5" t="s">
         <v>601</v>
       </c>
-      <c r="M32" s="5" t="s">
+      <c r="N32" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N32" s="5" t="s">
+      <c r="O32" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
         <v>602</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>603</v>
       </c>
-      <c r="C33" s="9" t="s">
+      <c r="C33" s="5"/>
+      <c r="D33" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="D33" s="5" t="s">
-        <v>728</v>
-      </c>
       <c r="E33" s="5" t="s">
+        <v>727</v>
+      </c>
+      <c r="F33" s="5" t="s">
         <v>604</v>
       </c>
-      <c r="F33" s="5" t="s">
+      <c r="G33" s="5" t="s">
         <v>605</v>
       </c>
-      <c r="G33" s="5" t="s">
+      <c r="H33" s="5" t="s">
         <v>606</v>
       </c>
-      <c r="H33" s="9" t="s">
+      <c r="I33" s="9" t="s">
         <v>641</v>
       </c>
-      <c r="I33" s="5" t="s">
+      <c r="J33" s="5" t="s">
         <v>607</v>
       </c>
-      <c r="J33" s="5" t="s">
+      <c r="K33" s="5" t="s">
         <v>608</v>
       </c>
-      <c r="K33" s="5" t="s">
+      <c r="L33" s="5" t="s">
         <v>609</v>
       </c>
-      <c r="L33" s="5" t="s">
+      <c r="M33" s="5" t="s">
         <v>610</v>
       </c>
-      <c r="M33" s="5" t="s">
+      <c r="N33" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N33" s="5" t="s">
+      <c r="O33" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>611</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>612</v>
       </c>
-      <c r="C34" s="9" t="s">
+      <c r="C34" s="5"/>
+      <c r="D34" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="D34" s="5" t="s">
-        <v>729</v>
-      </c>
       <c r="E34" s="5" t="s">
+        <v>728</v>
+      </c>
+      <c r="F34" s="5" t="s">
         <v>613</v>
       </c>
-      <c r="F34" s="5" t="s">
+      <c r="G34" s="5" t="s">
         <v>614</v>
       </c>
-      <c r="G34" s="5" t="s">
+      <c r="H34" s="5" t="s">
         <v>615</v>
       </c>
-      <c r="H34" s="9" t="s">
+      <c r="I34" s="9" t="s">
         <v>640</v>
       </c>
-      <c r="I34" s="5" t="s">
+      <c r="J34" s="5" t="s">
         <v>616</v>
       </c>
-      <c r="J34" s="5" t="s">
+      <c r="K34" s="5" t="s">
         <v>617</v>
       </c>
-      <c r="K34" s="5" t="s">
+      <c r="L34" s="5" t="s">
         <v>618</v>
       </c>
-      <c r="L34" s="5" t="s">
+      <c r="M34" s="5" t="s">
         <v>619</v>
       </c>
-      <c r="M34" s="5" t="s">
+      <c r="N34" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N34" s="5" t="s">
+      <c r="O34" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>620</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>621</v>
       </c>
-      <c r="C35" s="9" t="s">
+      <c r="C35" s="5"/>
+      <c r="D35" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="D35" s="5" t="s">
-        <v>730</v>
-      </c>
       <c r="E35" s="5" t="s">
+        <v>729</v>
+      </c>
+      <c r="F35" s="5" t="s">
         <v>622</v>
       </c>
-      <c r="F35" s="5" t="s">
+      <c r="G35" s="5" t="s">
         <v>623</v>
       </c>
-      <c r="G35" s="5" t="s">
+      <c r="H35" s="5" t="s">
         <v>624</v>
       </c>
-      <c r="H35" s="9" t="s">
+      <c r="I35" s="9" t="s">
         <v>639</v>
       </c>
-      <c r="I35" s="5" t="s">
+      <c r="J35" s="5" t="s">
         <v>625</v>
       </c>
-      <c r="J35" s="5" t="s">
+      <c r="K35" s="5" t="s">
         <v>626</v>
       </c>
-      <c r="K35" s="5" t="s">
+      <c r="L35" s="5" t="s">
         <v>627</v>
       </c>
-      <c r="L35" s="5" t="s">
+      <c r="M35" s="5" t="s">
         <v>628</v>
       </c>
-      <c r="M35" s="5" t="s">
+      <c r="N35" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N35" s="5" t="s">
+      <c r="O35" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
         <v>629</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>630</v>
       </c>
-      <c r="C36" s="9" t="s">
+      <c r="C36" s="5"/>
+      <c r="D36" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="D36" s="5" t="s">
-        <v>731</v>
-      </c>
       <c r="E36" s="5" t="s">
+        <v>730</v>
+      </c>
+      <c r="F36" s="5" t="s">
         <v>631</v>
       </c>
-      <c r="F36" s="5" t="s">
+      <c r="G36" s="5" t="s">
         <v>632</v>
       </c>
-      <c r="G36" s="5" t="s">
+      <c r="H36" s="5" t="s">
         <v>633</v>
       </c>
-      <c r="H36" s="9" t="s">
+      <c r="I36" s="9" t="s">
         <v>638</v>
       </c>
-      <c r="I36" s="5" t="s">
+      <c r="J36" s="5" t="s">
         <v>634</v>
       </c>
-      <c r="J36" s="5" t="s">
+      <c r="K36" s="5" t="s">
         <v>635</v>
       </c>
-      <c r="K36" s="5" t="s">
+      <c r="L36" s="5" t="s">
         <v>636</v>
       </c>
-      <c r="L36" s="5" t="s">
+      <c r="M36" s="5" t="s">
         <v>637</v>
       </c>
-      <c r="M36" s="5" t="s">
+      <c r="N36" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N36" s="5" t="s">
+      <c r="O36" s="5" t="s">
         <v>243</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="\\DataSet\\TL_DataSet\\FxRates_GSFile\\" xr:uid="{94121ADA-ADA1-40BE-A021-98D4F05A3E44}"/>
-    <hyperlink ref="C3:C7" r:id="rId2" display="\\DataSet\\TL_DataSet\\FxRates_GSFile\\" xr:uid="{1C2361F4-1B13-456E-9BA3-E3D8B7F812A7}"/>
-    <hyperlink ref="C8:C22" r:id="rId3" display="\\DataSet\\TL_DataSet\\FxRates_GSFile\\" xr:uid="{30D6AB87-ED81-4A29-A8BC-F1B921F77AB7}"/>
-    <hyperlink ref="H8:H22" r:id="rId4" display="\\DataSet\\TL_DataSet\\FxRates_GSFile\\" xr:uid="{6E3D10A6-4C88-4334-881C-8676178CABF0}"/>
-    <hyperlink ref="C23:C31" r:id="rId5" display="\\DataSet\\TL_DataSet\\FxRates_GSFile\\" xr:uid="{6B3504B3-9870-47D0-8E2F-5CAB415D1405}"/>
-    <hyperlink ref="H23:H31" r:id="rId6" display="\\DataSet\\TL_DataSet\\FxRates_GSFile\\" xr:uid="{57CD682C-3C14-436B-ADDE-9A80258650CD}"/>
-    <hyperlink ref="C32:C34" r:id="rId7" display="\\DataSet\\TL_DataSet\\FxRates_GSFile\\" xr:uid="{202A1715-BE83-4EB7-A90F-52978138A4F3}"/>
-    <hyperlink ref="C35:C36" r:id="rId8" display="\\DataSet\\TL_DataSet\\FxRates_GSFile\\" xr:uid="{9840F825-8637-4C41-AA65-6AF3ECBC53D3}"/>
-    <hyperlink ref="H35:H36" r:id="rId9" display="\\DataSet\\TL_DataSet\\FxRates_GSFile\\" xr:uid="{E6DF1C66-E06C-4508-BF64-80E6763D6FB9}"/>
-    <hyperlink ref="H32:H34" r:id="rId10" display="\\DataSet\\TL_DataSet\\FxRates_GSFile\\" xr:uid="{5D520F54-CC93-417A-ADE8-C492B5E5E28A}"/>
-    <hyperlink ref="H21:H29" r:id="rId11" display="\\DataSet\\TL_DataSet\\FxRates_GSFile\\" xr:uid="{47A9315B-DFC8-4430-A45E-9D03C065A594}"/>
-    <hyperlink ref="H2:H8" r:id="rId12" display="\\DataSet\\TL_DataSet\\FxRates_GSFile\\" xr:uid="{21BBCC78-8612-4F9C-A722-A37062C86D04}"/>
+    <hyperlink ref="D3:D7" r:id="rId1" display="\\DataSet\\TL_DataSet\\FxRates_GSFile\\" xr:uid="{1C2361F4-1B13-456E-9BA3-E3D8B7F812A7}"/>
+    <hyperlink ref="D8:D22" r:id="rId2" display="\\DataSet\\TL_DataSet\\FxRates_GSFile\\" xr:uid="{30D6AB87-ED81-4A29-A8BC-F1B921F77AB7}"/>
+    <hyperlink ref="I8:I22" r:id="rId3" display="\\DataSet\\TL_DataSet\\FxRates_GSFile\\" xr:uid="{6E3D10A6-4C88-4334-881C-8676178CABF0}"/>
+    <hyperlink ref="D23:D31" r:id="rId4" display="\\DataSet\\TL_DataSet\\FxRates_GSFile\\" xr:uid="{6B3504B3-9870-47D0-8E2F-5CAB415D1405}"/>
+    <hyperlink ref="I23:I31" r:id="rId5" display="\\DataSet\\TL_DataSet\\FxRates_GSFile\\" xr:uid="{57CD682C-3C14-436B-ADDE-9A80258650CD}"/>
+    <hyperlink ref="D32:D34" r:id="rId6" display="\\DataSet\\TL_DataSet\\FxRates_GSFile\\" xr:uid="{202A1715-BE83-4EB7-A90F-52978138A4F3}"/>
+    <hyperlink ref="D35:D36" r:id="rId7" display="\\DataSet\\TL_DataSet\\FxRates_GSFile\\" xr:uid="{9840F825-8637-4C41-AA65-6AF3ECBC53D3}"/>
+    <hyperlink ref="I35:I36" r:id="rId8" display="\\DataSet\\TL_DataSet\\FxRates_GSFile\\" xr:uid="{E6DF1C66-E06C-4508-BF64-80E6763D6FB9}"/>
+    <hyperlink ref="I32:I34" r:id="rId9" display="\\DataSet\\TL_DataSet\\FxRates_GSFile\\" xr:uid="{5D520F54-CC93-417A-ADE8-C492B5E5E28A}"/>
+    <hyperlink ref="I21:I29" r:id="rId10" display="\\DataSet\\TL_DataSet\\FxRates_GSFile\\" xr:uid="{47A9315B-DFC8-4430-A45E-9D03C065A594}"/>
+    <hyperlink ref="C2" r:id="rId11" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{DC17FF84-1D37-4112-BF5D-BCB4C73CD0FB}"/>
+    <hyperlink ref="D2" r:id="rId12" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{7887B602-EE56-45AE-936D-8A968AF005AA}"/>
+    <hyperlink ref="I2" r:id="rId13" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{883636BB-DB43-4D2E-AC6F-B249FF19C9EB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7847,7 +7892,7 @@
         <v>480</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>143</v>
@@ -7885,7 +7930,7 @@
         <v>482</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>483</v>
@@ -7897,7 +7942,7 @@
         <v>485</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="I3" s="9" t="s">
         <v>482</v>
@@ -7920,40 +7965,40 @@
         <v>36</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>875</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>876</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="D4" s="6" t="s">
+        <v>884</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>877</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>885</v>
-      </c>
-      <c r="E4" s="5" t="s">
+      <c r="F4" s="5" t="s">
         <v>878</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="G4" s="5" t="s">
         <v>879</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="H4" s="5" t="s">
         <v>880</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="I4" s="9" t="s">
+        <v>876</v>
+      </c>
+      <c r="J4" s="5" t="s">
         <v>881</v>
       </c>
-      <c r="I4" s="9" t="s">
-        <v>877</v>
-      </c>
-      <c r="J4" s="5" t="s">
+      <c r="K4" s="5" t="s">
         <v>882</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="L4" s="5" t="s">
         <v>883</v>
       </c>
-      <c r="L4" s="5" t="s">
-        <v>884</v>
-      </c>
       <c r="M4" s="5" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -7961,40 +8006,40 @@
         <v>43</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>885</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>886</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="D5" s="6" t="s">
+        <v>894</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>887</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>895</v>
-      </c>
-      <c r="E5" s="5" t="s">
+      <c r="F5" s="5" t="s">
         <v>888</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="G5" s="5" t="s">
         <v>889</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="H5" s="5" t="s">
         <v>890</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="I5" s="9" t="s">
+        <v>886</v>
+      </c>
+      <c r="J5" s="5" t="s">
         <v>891</v>
       </c>
-      <c r="I5" s="9" t="s">
-        <v>887</v>
-      </c>
-      <c r="J5" s="5" t="s">
+      <c r="K5" s="5" t="s">
         <v>892</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="L5" s="5" t="s">
         <v>893</v>
       </c>
-      <c r="L5" s="5" t="s">
-        <v>894</v>
-      </c>
       <c r="M5" s="5" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -8002,40 +8047,40 @@
         <v>64</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>822</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>823</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="D6" s="6" t="s">
         <v>824</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="E6" s="5" t="s">
         <v>825</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="F6" s="5" t="s">
         <v>826</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="G6" s="5" t="s">
         <v>827</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="H6" s="5" t="s">
         <v>828</v>
       </c>
-      <c r="H6" s="5" t="s">
-        <v>829</v>
-      </c>
       <c r="I6" s="9" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="J6" s="5" t="s">
+        <v>831</v>
+      </c>
+      <c r="K6" s="5" t="s">
         <v>832</v>
       </c>
-      <c r="K6" s="5" t="s">
+      <c r="L6" s="5" t="s">
         <v>833</v>
       </c>
-      <c r="L6" s="5" t="s">
-        <v>834</v>
-      </c>
       <c r="M6" s="5" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -8043,40 +8088,40 @@
         <v>96</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>803</v>
+      </c>
+      <c r="C7" s="9" t="s">
         <v>804</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="D7" s="6" t="s">
+        <v>810</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>805</v>
       </c>
-      <c r="D7" s="6" t="s">
-        <v>811</v>
-      </c>
-      <c r="E7" s="5" t="s">
+      <c r="F7" s="5" t="s">
         <v>806</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="G7" s="5" t="s">
         <v>807</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="H7" s="5" t="s">
+        <v>829</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>804</v>
+      </c>
+      <c r="J7" s="5" t="s">
         <v>808</v>
       </c>
-      <c r="H7" s="5" t="s">
-        <v>830</v>
-      </c>
-      <c r="I7" s="9" t="s">
-        <v>805</v>
-      </c>
-      <c r="J7" s="5" t="s">
+      <c r="K7" s="5" t="s">
         <v>809</v>
-      </c>
-      <c r="K7" s="5" t="s">
-        <v>810</v>
       </c>
       <c r="L7" s="5" t="s">
         <v>488</v>
       </c>
       <c r="M7" s="5" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -8084,40 +8129,40 @@
         <v>103</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>811</v>
+      </c>
+      <c r="C8" s="9" t="s">
         <v>812</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="D8" s="6" t="s">
+        <v>820</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>813</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>821</v>
-      </c>
-      <c r="E8" s="5" t="s">
+      <c r="F8" s="5" t="s">
         <v>814</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="G8" s="5" t="s">
         <v>815</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="H8" s="5" t="s">
+        <v>830</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>812</v>
+      </c>
+      <c r="J8" s="5" t="s">
         <v>816</v>
       </c>
-      <c r="H8" s="5" t="s">
-        <v>831</v>
-      </c>
-      <c r="I8" s="9" t="s">
-        <v>813</v>
-      </c>
-      <c r="J8" s="5" t="s">
+      <c r="K8" s="5" t="s">
         <v>817</v>
-      </c>
-      <c r="K8" s="5" t="s">
-        <v>818</v>
       </c>
       <c r="L8" s="5" t="s">
         <v>488</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -8125,40 +8170,40 @@
         <v>111</v>
       </c>
       <c r="B9" s="5" t="s">
+        <v>835</v>
+      </c>
+      <c r="C9" s="9" t="s">
         <v>836</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="D9" s="6" t="s">
         <v>837</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="E9" s="5" t="s">
         <v>838</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="F9" s="5" t="s">
         <v>839</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="G9" s="5" t="s">
         <v>840</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="H9" s="5" t="s">
         <v>841</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="I9" s="9" t="s">
+        <v>836</v>
+      </c>
+      <c r="J9" s="5" t="s">
         <v>842</v>
       </c>
-      <c r="I9" s="9" t="s">
-        <v>837</v>
-      </c>
-      <c r="J9" s="5" t="s">
+      <c r="K9" s="5" t="s">
         <v>843</v>
       </c>
-      <c r="K9" s="5" t="s">
+      <c r="L9" s="5" t="s">
         <v>844</v>
       </c>
-      <c r="L9" s="5" t="s">
-        <v>845</v>
-      </c>
       <c r="M9" s="5" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -8172,7 +8217,7 @@
         <v>490</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>491</v>
@@ -8184,7 +8229,7 @@
         <v>493</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="I10" s="9" t="s">
         <v>490</v>
@@ -8207,40 +8252,40 @@
         <v>115</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>1027</v>
+      </c>
+      <c r="C11" s="9" t="s">
         <v>1028</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="D11" s="6" t="s">
         <v>1029</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="E11" s="5" t="s">
         <v>1030</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="F11" s="5" t="s">
         <v>1031</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="G11" s="5" t="s">
         <v>1032</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="H11" s="5" t="s">
         <v>1033</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="I11" s="9" t="s">
+        <v>1028</v>
+      </c>
+      <c r="J11" s="5" t="s">
         <v>1034</v>
       </c>
-      <c r="I11" s="9" t="s">
-        <v>1029</v>
-      </c>
-      <c r="J11" s="5" t="s">
+      <c r="K11" s="5" t="s">
         <v>1035</v>
       </c>
-      <c r="K11" s="5" t="s">
+      <c r="L11" s="5" t="s">
         <v>1036</v>
       </c>
-      <c r="L11" s="5" t="s">
-        <v>1037</v>
-      </c>
       <c r="M11" s="5" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -8248,40 +8293,40 @@
         <v>117</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>1037</v>
+      </c>
+      <c r="C12" s="9" t="s">
         <v>1038</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="D12" s="6" t="s">
         <v>1039</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="E12" s="5" t="s">
         <v>1040</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="F12" s="5" t="s">
         <v>1041</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="G12" s="5" t="s">
         <v>1042</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="H12" s="5" t="s">
         <v>1043</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="I12" s="9" t="s">
+        <v>1038</v>
+      </c>
+      <c r="J12" s="5" t="s">
         <v>1044</v>
       </c>
-      <c r="I12" s="9" t="s">
-        <v>1039</v>
-      </c>
-      <c r="J12" s="5" t="s">
+      <c r="K12" s="5" t="s">
         <v>1045</v>
       </c>
-      <c r="K12" s="5" t="s">
+      <c r="L12" s="5" t="s">
         <v>1046</v>
       </c>
-      <c r="L12" s="5" t="s">
-        <v>1047</v>
-      </c>
       <c r="M12" s="5" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -8289,40 +8334,40 @@
         <v>119</v>
       </c>
       <c r="B13" s="5" t="s">
+        <v>905</v>
+      </c>
+      <c r="C13" s="9" t="s">
         <v>906</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="D13" s="6" t="s">
         <v>907</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="E13" s="5" t="s">
         <v>908</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="F13" s="5" t="s">
         <v>909</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="G13" s="5" t="s">
         <v>910</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="H13" s="5" t="s">
         <v>911</v>
       </c>
-      <c r="H13" s="5" t="s">
+      <c r="I13" s="9" t="s">
+        <v>906</v>
+      </c>
+      <c r="J13" s="5" t="s">
         <v>912</v>
       </c>
-      <c r="I13" s="9" t="s">
-        <v>907</v>
-      </c>
-      <c r="J13" s="5" t="s">
+      <c r="K13" s="5" t="s">
         <v>913</v>
       </c>
-      <c r="K13" s="5" t="s">
+      <c r="L13" s="5" t="s">
         <v>914</v>
       </c>
-      <c r="L13" s="5" t="s">
-        <v>915</v>
-      </c>
       <c r="M13" s="5" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -8336,7 +8381,7 @@
         <v>498</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>499</v>
@@ -8375,7 +8420,7 @@
         <v>507</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>508</v>
@@ -8414,7 +8459,7 @@
         <v>507</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>516</v>
@@ -8453,7 +8498,7 @@
         <v>523</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>524</v>
@@ -8494,7 +8539,7 @@
         <v>532</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>533</v>
@@ -8533,7 +8578,7 @@
         <v>540</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>541</v>
@@ -8566,38 +8611,38 @@
         <v>210</v>
       </c>
       <c r="B20" s="5" t="s">
+        <v>692</v>
+      </c>
+      <c r="C20" s="9" t="s">
         <v>693</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="D20" s="6" t="s">
+        <v>800</v>
+      </c>
+      <c r="E20" s="5" t="s">
         <v>694</v>
       </c>
-      <c r="D20" s="6" t="s">
-        <v>801</v>
-      </c>
-      <c r="E20" s="5" t="s">
+      <c r="F20" s="5" t="s">
         <v>695</v>
       </c>
-      <c r="F20" s="5" t="s">
+      <c r="G20" s="5" t="s">
         <v>696</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>697</v>
       </c>
       <c r="H20" s="5"/>
       <c r="I20" s="9" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="J20" s="5" t="s">
+        <v>697</v>
+      </c>
+      <c r="K20" s="5" t="s">
         <v>698</v>
       </c>
-      <c r="K20" s="5" t="s">
+      <c r="L20" s="5" t="s">
         <v>699</v>
       </c>
-      <c r="L20" s="5" t="s">
-        <v>700</v>
-      </c>
       <c r="M20" s="5" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -8611,7 +8656,7 @@
         <v>586</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>587</v>
@@ -8644,40 +8689,40 @@
         <v>419</v>
       </c>
       <c r="B22" s="5" t="s">
+        <v>1067</v>
+      </c>
+      <c r="C22" s="9" t="s">
         <v>1068</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="D22" s="6" t="s">
+        <v>1109</v>
+      </c>
+      <c r="E22" s="5" t="s">
         <v>1069</v>
       </c>
-      <c r="D22" s="6" t="s">
-        <v>1110</v>
-      </c>
-      <c r="E22" s="5" t="s">
+      <c r="F22" s="5" t="s">
         <v>1070</v>
       </c>
-      <c r="F22" s="5" t="s">
+      <c r="G22" s="5" t="s">
         <v>1071</v>
       </c>
-      <c r="G22" s="5" t="s">
+      <c r="H22" s="5" t="s">
         <v>1072</v>
       </c>
-      <c r="H22" s="5" t="s">
+      <c r="I22" s="9" t="s">
+        <v>1068</v>
+      </c>
+      <c r="J22" s="5" t="s">
         <v>1073</v>
       </c>
-      <c r="I22" s="9" t="s">
-        <v>1069</v>
-      </c>
-      <c r="J22" s="5" t="s">
+      <c r="K22" s="5" t="s">
         <v>1074</v>
       </c>
-      <c r="K22" s="5" t="s">
+      <c r="L22" s="5" t="s">
         <v>1075</v>
       </c>
-      <c r="L22" s="5" t="s">
-        <v>1076</v>
-      </c>
       <c r="M22" s="5" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -8685,40 +8730,40 @@
         <v>428</v>
       </c>
       <c r="B23" s="5" t="s">
+        <v>846</v>
+      </c>
+      <c r="C23" s="9" t="s">
         <v>847</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="D23" s="6" t="s">
+        <v>1110</v>
+      </c>
+      <c r="E23" s="5" t="s">
         <v>848</v>
       </c>
-      <c r="D23" s="6" t="s">
-        <v>1111</v>
-      </c>
-      <c r="E23" s="5" t="s">
+      <c r="F23" s="5" t="s">
         <v>849</v>
       </c>
-      <c r="F23" s="5" t="s">
+      <c r="G23" s="5" t="s">
         <v>850</v>
       </c>
-      <c r="G23" s="5" t="s">
+      <c r="H23" s="5" t="s">
         <v>851</v>
       </c>
-      <c r="H23" s="5" t="s">
+      <c r="I23" s="9" t="s">
+        <v>847</v>
+      </c>
+      <c r="J23" s="5" t="s">
         <v>852</v>
       </c>
-      <c r="I23" s="9" t="s">
-        <v>848</v>
-      </c>
-      <c r="J23" s="5" t="s">
+      <c r="K23" s="5" t="s">
         <v>853</v>
       </c>
-      <c r="K23" s="5" t="s">
+      <c r="L23" s="5" t="s">
         <v>854</v>
       </c>
-      <c r="L23" s="5" t="s">
-        <v>855</v>
-      </c>
       <c r="M23" s="5" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -8726,40 +8771,40 @@
         <v>438</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="C24" s="9" t="s">
+        <v>857</v>
+      </c>
+      <c r="D24" s="6" t="s">
         <v>858</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="E24" s="5" t="s">
         <v>859</v>
       </c>
-      <c r="E24" s="5" t="s">
+      <c r="F24" s="5" t="s">
         <v>860</v>
       </c>
-      <c r="F24" s="5" t="s">
+      <c r="G24" s="5" t="s">
         <v>861</v>
       </c>
-      <c r="G24" s="5" t="s">
+      <c r="H24" s="5" t="s">
         <v>862</v>
       </c>
-      <c r="H24" s="5" t="s">
+      <c r="I24" s="9" t="s">
+        <v>857</v>
+      </c>
+      <c r="J24" s="5" t="s">
         <v>863</v>
       </c>
-      <c r="I24" s="9" t="s">
-        <v>858</v>
-      </c>
-      <c r="J24" s="5" t="s">
+      <c r="K24" s="5" t="s">
         <v>864</v>
       </c>
-      <c r="K24" s="5" t="s">
+      <c r="L24" s="5" t="s">
         <v>865</v>
       </c>
-      <c r="L24" s="5" t="s">
-        <v>866</v>
-      </c>
       <c r="M24" s="5" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -8767,40 +8812,40 @@
         <v>448</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="C25" s="9" t="s">
+        <v>866</v>
+      </c>
+      <c r="D25" s="6" t="s">
         <v>867</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="E25" s="5" t="s">
         <v>868</v>
       </c>
-      <c r="E25" s="5" t="s">
+      <c r="F25" s="5" t="s">
         <v>869</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="G25" s="5" t="s">
         <v>870</v>
       </c>
-      <c r="G25" s="5" t="s">
+      <c r="H25" s="5" t="s">
         <v>871</v>
       </c>
-      <c r="H25" s="5" t="s">
+      <c r="I25" s="9" t="s">
+        <v>866</v>
+      </c>
+      <c r="J25" s="5" t="s">
         <v>872</v>
       </c>
-      <c r="I25" s="9" t="s">
-        <v>867</v>
-      </c>
-      <c r="J25" s="5" t="s">
+      <c r="K25" s="5" t="s">
         <v>873</v>
       </c>
-      <c r="K25" s="5" t="s">
+      <c r="L25" s="5" t="s">
         <v>874</v>
       </c>
-      <c r="L25" s="5" t="s">
-        <v>875</v>
-      </c>
       <c r="M25" s="5" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -8808,40 +8853,40 @@
         <v>458</v>
       </c>
       <c r="B26" s="5" t="s">
+        <v>982</v>
+      </c>
+      <c r="C26" s="9" t="s">
         <v>983</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="D26" s="6" t="s">
         <v>984</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="E26" s="5" t="s">
         <v>985</v>
       </c>
-      <c r="E26" s="5" t="s">
+      <c r="F26" s="5" t="s">
         <v>986</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="G26" s="5" t="s">
         <v>987</v>
       </c>
-      <c r="G26" s="5" t="s">
+      <c r="H26" s="5" t="s">
         <v>988</v>
       </c>
-      <c r="H26" s="5" t="s">
+      <c r="I26" s="9" t="s">
+        <v>983</v>
+      </c>
+      <c r="J26" s="5" t="s">
         <v>989</v>
       </c>
-      <c r="I26" s="9" t="s">
-        <v>984</v>
-      </c>
-      <c r="J26" s="5" t="s">
+      <c r="K26" s="5" t="s">
         <v>990</v>
       </c>
-      <c r="K26" s="5" t="s">
+      <c r="L26" s="5" t="s">
         <v>991</v>
       </c>
-      <c r="L26" s="5" t="s">
-        <v>992</v>
-      </c>
       <c r="M26" s="5" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -8849,40 +8894,40 @@
         <v>468</v>
       </c>
       <c r="B27" s="5" t="s">
+        <v>992</v>
+      </c>
+      <c r="C27" s="9" t="s">
         <v>993</v>
       </c>
-      <c r="C27" s="9" t="s">
+      <c r="D27" s="6" t="s">
         <v>994</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="E27" s="5" t="s">
         <v>995</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="F27" s="5" t="s">
         <v>996</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="G27" s="5" t="s">
         <v>997</v>
       </c>
-      <c r="G27" s="5" t="s">
+      <c r="H27" s="5" t="s">
         <v>998</v>
       </c>
-      <c r="H27" s="5" t="s">
+      <c r="I27" s="9" t="s">
+        <v>993</v>
+      </c>
+      <c r="J27" s="5" t="s">
         <v>999</v>
       </c>
-      <c r="I27" s="9" t="s">
-        <v>994</v>
-      </c>
-      <c r="J27" s="5" t="s">
+      <c r="K27" s="5" t="s">
         <v>1000</v>
       </c>
-      <c r="K27" s="5" t="s">
+      <c r="L27" s="5" t="s">
         <v>1001</v>
       </c>
-      <c r="L27" s="5" t="s">
-        <v>1002</v>
-      </c>
       <c r="M27" s="5" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -8890,40 +8935,40 @@
         <v>593</v>
       </c>
       <c r="B28" s="5" t="s">
+        <v>1002</v>
+      </c>
+      <c r="C28" s="9" t="s">
         <v>1003</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="D28" s="6" t="s">
         <v>1004</v>
       </c>
-      <c r="D28" s="6" t="s">
+      <c r="E28" s="5" t="s">
         <v>1005</v>
       </c>
-      <c r="E28" s="5" t="s">
+      <c r="F28" s="5" t="s">
         <v>1006</v>
       </c>
-      <c r="F28" s="5" t="s">
+      <c r="G28" s="5" t="s">
         <v>1007</v>
       </c>
-      <c r="G28" s="5" t="s">
+      <c r="H28" s="5" t="s">
         <v>1008</v>
       </c>
-      <c r="H28" s="5" t="s">
+      <c r="I28" s="9" t="s">
+        <v>1003</v>
+      </c>
+      <c r="J28" s="5" t="s">
         <v>1009</v>
       </c>
-      <c r="I28" s="9" t="s">
-        <v>1004</v>
-      </c>
-      <c r="J28" s="5" t="s">
+      <c r="K28" s="5" t="s">
         <v>1010</v>
       </c>
-      <c r="K28" s="5" t="s">
+      <c r="L28" s="5" t="s">
         <v>1011</v>
       </c>
-      <c r="L28" s="5" t="s">
-        <v>1012</v>
-      </c>
       <c r="M28" s="5" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -8931,40 +8976,40 @@
         <v>602</v>
       </c>
       <c r="B29" s="5" t="s">
+        <v>1047</v>
+      </c>
+      <c r="C29" s="9" t="s">
         <v>1048</v>
       </c>
-      <c r="C29" s="9" t="s">
+      <c r="D29" s="6" t="s">
         <v>1049</v>
       </c>
-      <c r="D29" s="6" t="s">
+      <c r="E29" s="5" t="s">
         <v>1050</v>
       </c>
-      <c r="E29" s="5" t="s">
+      <c r="F29" s="5" t="s">
         <v>1051</v>
       </c>
-      <c r="F29" s="5" t="s">
+      <c r="G29" s="5" t="s">
         <v>1052</v>
       </c>
-      <c r="G29" s="5" t="s">
+      <c r="H29" s="5" t="s">
         <v>1053</v>
       </c>
-      <c r="H29" s="5" t="s">
+      <c r="I29" s="9" t="s">
+        <v>1048</v>
+      </c>
+      <c r="J29" s="5" t="s">
         <v>1054</v>
       </c>
-      <c r="I29" s="9" t="s">
-        <v>1049</v>
-      </c>
-      <c r="J29" s="5" t="s">
+      <c r="K29" s="5" t="s">
         <v>1055</v>
       </c>
-      <c r="K29" s="5" t="s">
+      <c r="L29" s="5" t="s">
         <v>1056</v>
       </c>
-      <c r="L29" s="5" t="s">
-        <v>1057</v>
-      </c>
       <c r="M29" s="5" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -8972,40 +9017,40 @@
         <v>611</v>
       </c>
       <c r="B30" s="5" t="s">
+        <v>1057</v>
+      </c>
+      <c r="C30" s="9" t="s">
         <v>1058</v>
       </c>
-      <c r="C30" s="9" t="s">
+      <c r="D30" s="6" t="s">
         <v>1059</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="E30" s="5" t="s">
         <v>1060</v>
       </c>
-      <c r="E30" s="5" t="s">
+      <c r="F30" s="5" t="s">
         <v>1061</v>
       </c>
-      <c r="F30" s="5" t="s">
+      <c r="G30" s="5" t="s">
         <v>1062</v>
       </c>
-      <c r="G30" s="5" t="s">
+      <c r="H30" s="5" t="s">
         <v>1063</v>
       </c>
-      <c r="H30" s="5" t="s">
+      <c r="I30" s="9" t="s">
+        <v>1058</v>
+      </c>
+      <c r="J30" s="5" t="s">
         <v>1064</v>
       </c>
-      <c r="I30" s="9" t="s">
-        <v>1059</v>
-      </c>
-      <c r="J30" s="5" t="s">
+      <c r="K30" s="5" t="s">
         <v>1065</v>
       </c>
-      <c r="K30" s="5" t="s">
+      <c r="L30" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="L30" s="5" t="s">
-        <v>1067</v>
-      </c>
       <c r="M30" s="5" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -9013,40 +9058,40 @@
         <v>629</v>
       </c>
       <c r="B31" s="5" t="s">
+        <v>895</v>
+      </c>
+      <c r="C31" s="9" t="s">
         <v>896</v>
       </c>
-      <c r="C31" s="9" t="s">
+      <c r="D31" s="6" t="s">
+        <v>904</v>
+      </c>
+      <c r="E31" s="5" t="s">
         <v>897</v>
       </c>
-      <c r="D31" s="6" t="s">
-        <v>905</v>
-      </c>
-      <c r="E31" s="5" t="s">
+      <c r="F31" s="5" t="s">
         <v>898</v>
       </c>
-      <c r="F31" s="5" t="s">
+      <c r="G31" s="5" t="s">
         <v>899</v>
       </c>
-      <c r="G31" s="5" t="s">
+      <c r="H31" s="5" t="s">
         <v>900</v>
       </c>
-      <c r="H31" s="5" t="s">
+      <c r="I31" s="9" t="s">
+        <v>896</v>
+      </c>
+      <c r="J31" s="5" t="s">
         <v>901</v>
       </c>
-      <c r="I31" s="9" t="s">
-        <v>897</v>
-      </c>
-      <c r="J31" s="5" t="s">
+      <c r="K31" s="5" t="s">
         <v>902</v>
       </c>
-      <c r="K31" s="5" t="s">
+      <c r="L31" s="5" t="s">
         <v>903</v>
       </c>
-      <c r="L31" s="5" t="s">
-        <v>904</v>
-      </c>
       <c r="M31" s="5" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -9060,7 +9105,7 @@
         <v>549</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="E32" s="5" t="s">
         <v>550</v>
@@ -9099,7 +9144,7 @@
         <v>558</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="E33" s="5" t="s">
         <v>559</v>

</xml_diff>

<commit_message>
GDE-7302 - data set and script fixes
Updated TL_CAL_01_files with valid Codes
Updated the path for InputFilePath and OutputFilePath on TL_Data_Set_AU
Updated variable source name on global variables
Updated Calendar properties with correct path
Fixed script to scroll to view first before double clicking on TextJMS
results
</commit_message>
<xml_diff>
--- a/DataSet/Integration_DataSet/TL/TL_Data_Set_AU.xlsx
+++ b/DataSet/Integration_DataSet/TL/TL_Data_Set_AU.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\Integration_DataSet\TL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05D60997-DB15-4187-884F-5DC225A6CAE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{683D4D1F-A3F6-449D-AEEC-F5486E129DE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34800" yWindow="5505" windowWidth="18435" windowHeight="9105" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BaseRate_Fields" sheetId="1" r:id="rId1"/>
@@ -1463,9 +1463,6 @@
   </si>
   <si>
     <t>Expected_CustomCBAPush_Response</t>
-  </si>
-  <si>
-    <t>\DataSet\TL_DataSet\Calendar_GSFile\TL_CAL_01_Files\</t>
   </si>
   <si>
     <t>TL_CAL_02</t>
@@ -3415,9 +3412,6 @@
     <t>Holidays_Banks_20190126_1.xls,Holidays_Banks_20190126_2.xls,Holidays_Banks_20190126_1.csv,Holidays_Banks_20190126_2.csv,Holidays_Misc_20190126.xls</t>
   </si>
   <si>
-    <t>Holidays_Banks_20200101_1.xlsx,Holidays_Banks_20200101_2.xlsx,Holidays_Banks_20200101_1.csv,Holidays_Banks_20200101_2.csv,Holidays_Misc_20200101.xlsx</t>
-  </si>
-  <si>
     <t>FINASTRA_CCB_FX_NY_FX11.txt</t>
   </si>
   <si>
@@ -3440,6 +3434,12 @@
   </si>
   <si>
     <t>\DataSet\Integration_DataSet\TL\FXRates_GSFile\AU\TL_FX_01_Files\</t>
+  </si>
+  <si>
+    <t>\DataSet\Integration_DataSet\TL\Calendar_GSFile\TL_CAL_01_Files\</t>
+  </si>
+  <si>
+    <t>Holidays_Banks_20200123_1.xlsx,Holidays_Banks_20200123_2.xlsx,Holidays_Banks_20200123_1.csv,Holidays_Banks_20200123_2.csv,Holidays_Misc_20200123.xlsx</t>
   </si>
 </sst>
 </file>
@@ -4422,7 +4422,7 @@
         <v>17</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>1115</v>
+        <v>1113</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>1</v>
@@ -4455,7 +4455,7 @@
         <v>155</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -4466,10 +4466,10 @@
         <v>11</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>1116</v>
+        <v>1114</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>1117</v>
+        <v>1115</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>94</v>
@@ -4484,7 +4484,7 @@
         <v>18</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>1117</v>
+        <v>1115</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>21</v>
@@ -4574,7 +4574,7 @@
         <v>136</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -4664,10 +4664,10 @@
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="9" t="s">
+        <v>914</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>915</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>916</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>59</v>
@@ -4679,7 +4679,7 @@
         <v>61</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="J7" s="5" t="s">
         <v>62</v>
@@ -4691,7 +4691,7 @@
         <v>139</v>
       </c>
       <c r="M7" s="5" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -4703,10 +4703,10 @@
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="9" t="s">
+        <v>916</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>917</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>918</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>66</v>
@@ -4718,7 +4718,7 @@
         <v>68</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="J8" s="5" t="s">
         <v>69</v>
@@ -4727,10 +4727,10 @@
         <v>70</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -4742,10 +4742,10 @@
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="9" t="s">
+        <v>918</v>
+      </c>
+      <c r="E9" s="5" t="s">
         <v>919</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>920</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>98</v>
@@ -4757,7 +4757,7 @@
         <v>100</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="J9" s="5" t="s">
         <v>101</v>
@@ -4766,10 +4766,10 @@
         <v>102</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="M9" s="5" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -4781,7 +4781,7 @@
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="9" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>105</v>
@@ -4796,7 +4796,7 @@
         <v>108</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="J10" s="5" t="s">
         <v>109</v>
@@ -4805,10 +4805,10 @@
         <v>110</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="M10" s="5" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -5050,38 +5050,38 @@
         <v>333</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="9" t="s">
+        <v>921</v>
+      </c>
+      <c r="E17" s="5" t="s">
         <v>922</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="F17" s="5" t="s">
         <v>923</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="G17" s="5" t="s">
         <v>924</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="H17" s="5" t="s">
         <v>925</v>
       </c>
-      <c r="H17" s="5" t="s">
+      <c r="I17" s="9" t="s">
+        <v>921</v>
+      </c>
+      <c r="J17" s="5" t="s">
         <v>926</v>
       </c>
-      <c r="I17" s="9" t="s">
-        <v>922</v>
-      </c>
-      <c r="J17" s="5" t="s">
+      <c r="K17" s="5" t="s">
         <v>927</v>
       </c>
-      <c r="K17" s="5" t="s">
+      <c r="L17" s="5" t="s">
         <v>928</v>
       </c>
-      <c r="L17" s="5" t="s">
+      <c r="M17" s="5" t="s">
         <v>929</v>
-      </c>
-      <c r="M17" s="5" t="s">
-        <v>930</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -5089,38 +5089,38 @@
         <v>343</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="9" t="s">
+        <v>1076</v>
+      </c>
+      <c r="E18" s="5" t="s">
         <v>1077</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="F18" s="5" t="s">
         <v>1078</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="G18" s="5" t="s">
         <v>1079</v>
       </c>
-      <c r="G18" s="5" t="s">
+      <c r="H18" s="5" t="s">
         <v>1080</v>
       </c>
-      <c r="H18" s="5" t="s">
+      <c r="I18" s="9" t="s">
+        <v>1076</v>
+      </c>
+      <c r="J18" s="5" t="s">
         <v>1081</v>
       </c>
-      <c r="I18" s="9" t="s">
-        <v>1077</v>
-      </c>
-      <c r="J18" s="5" t="s">
+      <c r="K18" s="5" t="s">
         <v>1082</v>
       </c>
-      <c r="K18" s="5" t="s">
+      <c r="L18" s="5" t="s">
         <v>1083</v>
       </c>
-      <c r="L18" s="5" t="s">
+      <c r="M18" s="5" t="s">
         <v>1084</v>
-      </c>
-      <c r="M18" s="5" t="s">
-        <v>1085</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -5128,38 +5128,38 @@
         <v>353</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="9" t="s">
+        <v>1017</v>
+      </c>
+      <c r="E19" s="5" t="s">
         <v>1018</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="F19" s="5" t="s">
         <v>1019</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="G19" s="5" t="s">
         <v>1020</v>
       </c>
-      <c r="G19" s="5" t="s">
+      <c r="H19" s="5" t="s">
         <v>1021</v>
       </c>
-      <c r="H19" s="5" t="s">
+      <c r="I19" s="9" t="s">
+        <v>1017</v>
+      </c>
+      <c r="J19" s="5" t="s">
         <v>1022</v>
       </c>
-      <c r="I19" s="9" t="s">
-        <v>1018</v>
-      </c>
-      <c r="J19" s="5" t="s">
+      <c r="K19" s="5" t="s">
         <v>1023</v>
       </c>
-      <c r="K19" s="5" t="s">
+      <c r="L19" s="5" t="s">
         <v>1024</v>
       </c>
-      <c r="L19" s="5" t="s">
+      <c r="M19" s="5" t="s">
         <v>1025</v>
-      </c>
-      <c r="M19" s="5" t="s">
-        <v>1026</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
@@ -5323,38 +5323,38 @@
         <v>428</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="9" t="s">
+        <v>565</v>
+      </c>
+      <c r="E24" s="6" t="s">
         <v>566</v>
       </c>
-      <c r="E24" s="6" t="s">
+      <c r="F24" s="5" t="s">
         <v>567</v>
       </c>
-      <c r="F24" s="5" t="s">
+      <c r="G24" s="5" t="s">
         <v>568</v>
       </c>
-      <c r="G24" s="5" t="s">
+      <c r="H24" s="5" t="s">
         <v>569</v>
       </c>
-      <c r="H24" s="5" t="s">
+      <c r="I24" s="9" t="s">
+        <v>565</v>
+      </c>
+      <c r="J24" s="5" t="s">
         <v>570</v>
       </c>
-      <c r="I24" s="9" t="s">
-        <v>566</v>
-      </c>
-      <c r="J24" s="5" t="s">
+      <c r="K24" s="5" t="s">
         <v>571</v>
       </c>
-      <c r="K24" s="5" t="s">
+      <c r="L24" s="5" t="s">
         <v>572</v>
       </c>
-      <c r="L24" s="5" t="s">
+      <c r="M24" s="5" t="s">
         <v>573</v>
-      </c>
-      <c r="M24" s="5" t="s">
-        <v>574</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -5362,38 +5362,38 @@
         <v>438</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="9" t="s">
+        <v>574</v>
+      </c>
+      <c r="E25" s="6" t="s">
         <v>575</v>
       </c>
-      <c r="E25" s="6" t="s">
+      <c r="F25" s="5" t="s">
         <v>576</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="G25" s="5" t="s">
         <v>577</v>
       </c>
-      <c r="G25" s="5" t="s">
+      <c r="H25" s="5" t="s">
         <v>578</v>
       </c>
-      <c r="H25" s="5" t="s">
+      <c r="I25" s="9" t="s">
+        <v>574</v>
+      </c>
+      <c r="J25" s="5" t="s">
         <v>579</v>
       </c>
-      <c r="I25" s="9" t="s">
-        <v>575</v>
-      </c>
-      <c r="J25" s="5" t="s">
+      <c r="K25" s="5" t="s">
         <v>580</v>
       </c>
-      <c r="K25" s="5" t="s">
+      <c r="L25" s="5" t="s">
         <v>581</v>
       </c>
-      <c r="L25" s="5" t="s">
+      <c r="M25" s="5" t="s">
         <v>582</v>
-      </c>
-      <c r="M25" s="5" t="s">
-        <v>583</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -5401,38 +5401,38 @@
         <v>448</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="9" t="s">
+        <v>700</v>
+      </c>
+      <c r="E26" s="6" t="s">
         <v>701</v>
       </c>
-      <c r="E26" s="6" t="s">
+      <c r="F26" s="5" t="s">
         <v>702</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="G26" s="5" t="s">
         <v>703</v>
       </c>
-      <c r="G26" s="5" t="s">
+      <c r="H26" s="5" t="s">
         <v>704</v>
       </c>
-      <c r="H26" s="5" t="s">
+      <c r="I26" s="9" t="s">
+        <v>700</v>
+      </c>
+      <c r="J26" s="5" t="s">
         <v>705</v>
       </c>
-      <c r="I26" s="9" t="s">
-        <v>701</v>
-      </c>
-      <c r="J26" s="5" t="s">
+      <c r="K26" s="5" t="s">
         <v>706</v>
       </c>
-      <c r="K26" s="5" t="s">
+      <c r="L26" s="5" t="s">
         <v>707</v>
       </c>
-      <c r="L26" s="5" t="s">
+      <c r="M26" s="5" t="s">
         <v>708</v>
-      </c>
-      <c r="M26" s="5" t="s">
-        <v>709</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
@@ -5440,38 +5440,38 @@
         <v>458</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="9" t="s">
+        <v>1086</v>
+      </c>
+      <c r="E27" s="5" t="s">
         <v>1087</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="F27" s="5" t="s">
         <v>1088</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="G27" s="5" t="s">
         <v>1089</v>
       </c>
-      <c r="G27" s="5" t="s">
+      <c r="H27" s="5" t="s">
         <v>1090</v>
       </c>
-      <c r="H27" s="5" t="s">
+      <c r="I27" s="9" t="s">
+        <v>1086</v>
+      </c>
+      <c r="J27" s="5" t="s">
         <v>1091</v>
       </c>
-      <c r="I27" s="9" t="s">
-        <v>1087</v>
-      </c>
-      <c r="J27" s="5" t="s">
+      <c r="K27" s="5" t="s">
         <v>1092</v>
       </c>
-      <c r="K27" s="5" t="s">
+      <c r="L27" s="5" t="s">
         <v>1093</v>
       </c>
-      <c r="L27" s="5" t="s">
+      <c r="M27" s="5" t="s">
         <v>1094</v>
-      </c>
-      <c r="M27" s="5" t="s">
-        <v>1095</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
@@ -5479,588 +5479,588 @@
         <v>468</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="9" t="s">
+        <v>672</v>
+      </c>
+      <c r="E28" s="6" t="s">
         <v>673</v>
       </c>
-      <c r="E28" s="6" t="s">
+      <c r="F28" s="5" t="s">
         <v>674</v>
       </c>
-      <c r="F28" s="5" t="s">
+      <c r="G28" s="5" t="s">
         <v>675</v>
       </c>
-      <c r="G28" s="5" t="s">
+      <c r="H28" s="5" t="s">
         <v>676</v>
       </c>
-      <c r="H28" s="5" t="s">
+      <c r="I28" s="9" t="s">
+        <v>672</v>
+      </c>
+      <c r="J28" s="5" t="s">
         <v>677</v>
       </c>
-      <c r="I28" s="9" t="s">
-        <v>673</v>
-      </c>
-      <c r="J28" s="5" t="s">
+      <c r="K28" s="5" t="s">
         <v>678</v>
       </c>
-      <c r="K28" s="5" t="s">
+      <c r="L28" s="5" t="s">
         <v>679</v>
       </c>
-      <c r="L28" s="5" t="s">
+      <c r="M28" s="5" t="s">
         <v>680</v>
-      </c>
-      <c r="M28" s="5" t="s">
-        <v>681</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="9" t="s">
+        <v>682</v>
+      </c>
+      <c r="E29" s="6" t="s">
         <v>683</v>
       </c>
-      <c r="E29" s="6" t="s">
+      <c r="F29" s="5" t="s">
         <v>684</v>
       </c>
-      <c r="F29" s="5" t="s">
+      <c r="G29" s="5" t="s">
         <v>685</v>
       </c>
-      <c r="G29" s="5" t="s">
+      <c r="H29" s="5" t="s">
         <v>686</v>
       </c>
-      <c r="H29" s="5" t="s">
+      <c r="I29" s="9" t="s">
+        <v>682</v>
+      </c>
+      <c r="J29" s="5" t="s">
         <v>687</v>
       </c>
-      <c r="I29" s="9" t="s">
-        <v>683</v>
-      </c>
-      <c r="J29" s="5" t="s">
+      <c r="K29" s="5" t="s">
         <v>688</v>
       </c>
-      <c r="K29" s="5" t="s">
+      <c r="L29" s="5" t="s">
         <v>689</v>
       </c>
-      <c r="L29" s="5" t="s">
+      <c r="M29" s="5" t="s">
         <v>690</v>
-      </c>
-      <c r="M29" s="5" t="s">
-        <v>691</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="9" t="s">
+        <v>718</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>732</v>
+      </c>
+      <c r="F30" s="5" t="s">
         <v>719</v>
       </c>
-      <c r="E30" s="6" t="s">
+      <c r="G30" s="5" t="s">
+        <v>720</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>721</v>
+      </c>
+      <c r="I30" s="9" t="s">
+        <v>718</v>
+      </c>
+      <c r="J30" s="5" t="s">
+        <v>722</v>
+      </c>
+      <c r="K30" s="5" t="s">
+        <v>723</v>
+      </c>
+      <c r="L30" s="5" t="s">
         <v>733</v>
       </c>
-      <c r="F30" s="5" t="s">
-        <v>720</v>
-      </c>
-      <c r="G30" s="5" t="s">
-        <v>721</v>
-      </c>
-      <c r="H30" s="5" t="s">
-        <v>722</v>
-      </c>
-      <c r="I30" s="9" t="s">
-        <v>719</v>
-      </c>
-      <c r="J30" s="5" t="s">
-        <v>723</v>
-      </c>
-      <c r="K30" s="5" t="s">
+      <c r="M30" s="5" t="s">
         <v>724</v>
-      </c>
-      <c r="L30" s="5" t="s">
-        <v>734</v>
-      </c>
-      <c r="M30" s="5" t="s">
-        <v>725</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="9" t="s">
+        <v>718</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>730</v>
+      </c>
+      <c r="F31" s="5" t="s">
         <v>719</v>
       </c>
-      <c r="E31" s="6" t="s">
-        <v>731</v>
-      </c>
-      <c r="F31" s="5" t="s">
+      <c r="G31" s="5" t="s">
         <v>720</v>
       </c>
-      <c r="G31" s="5" t="s">
+      <c r="H31" s="5" t="s">
         <v>721</v>
       </c>
-      <c r="H31" s="5" t="s">
+      <c r="I31" s="9" t="s">
+        <v>718</v>
+      </c>
+      <c r="J31" s="5" t="s">
         <v>722</v>
       </c>
-      <c r="I31" s="9" t="s">
-        <v>719</v>
-      </c>
-      <c r="J31" s="5" t="s">
+      <c r="K31" s="5" t="s">
         <v>723</v>
       </c>
-      <c r="K31" s="5" t="s">
+      <c r="L31" s="5" t="s">
+        <v>734</v>
+      </c>
+      <c r="M31" s="5" t="s">
         <v>724</v>
-      </c>
-      <c r="L31" s="5" t="s">
-        <v>735</v>
-      </c>
-      <c r="M31" s="5" t="s">
-        <v>725</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="9" t="s">
+        <v>931</v>
+      </c>
+      <c r="E32" s="6" t="s">
         <v>932</v>
       </c>
-      <c r="E32" s="6" t="s">
+      <c r="F32" s="5" t="s">
         <v>933</v>
       </c>
-      <c r="F32" s="5" t="s">
+      <c r="G32" s="5" t="s">
         <v>934</v>
       </c>
-      <c r="G32" s="5" t="s">
+      <c r="H32" s="5" t="s">
         <v>935</v>
       </c>
-      <c r="H32" s="5" t="s">
+      <c r="I32" s="9" t="s">
+        <v>931</v>
+      </c>
+      <c r="J32" s="5" t="s">
         <v>936</v>
       </c>
-      <c r="I32" s="9" t="s">
-        <v>932</v>
-      </c>
-      <c r="J32" s="5" t="s">
+      <c r="K32" s="5" t="s">
         <v>937</v>
       </c>
-      <c r="K32" s="5" t="s">
+      <c r="L32" s="5" t="s">
         <v>938</v>
       </c>
-      <c r="L32" s="5" t="s">
+      <c r="M32" s="5" t="s">
         <v>939</v>
-      </c>
-      <c r="M32" s="5" t="s">
-        <v>940</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="9" t="s">
+        <v>941</v>
+      </c>
+      <c r="E33" s="6" t="s">
         <v>942</v>
       </c>
-      <c r="E33" s="6" t="s">
+      <c r="F33" s="5" t="s">
         <v>943</v>
       </c>
-      <c r="F33" s="5" t="s">
+      <c r="G33" s="5" t="s">
         <v>944</v>
       </c>
-      <c r="G33" s="5" t="s">
+      <c r="H33" s="5" t="s">
         <v>945</v>
       </c>
-      <c r="H33" s="5" t="s">
+      <c r="I33" s="9" t="s">
+        <v>941</v>
+      </c>
+      <c r="J33" s="5" t="s">
         <v>946</v>
       </c>
-      <c r="I33" s="9" t="s">
-        <v>942</v>
-      </c>
-      <c r="J33" s="5" t="s">
+      <c r="K33" s="5" t="s">
         <v>947</v>
       </c>
-      <c r="K33" s="5" t="s">
+      <c r="L33" s="5" t="s">
         <v>948</v>
       </c>
-      <c r="L33" s="5" t="s">
+      <c r="M33" s="5" t="s">
         <v>949</v>
-      </c>
-      <c r="M33" s="5" t="s">
-        <v>950</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="9" t="s">
+        <v>951</v>
+      </c>
+      <c r="E34" s="6" t="s">
         <v>952</v>
       </c>
-      <c r="E34" s="6" t="s">
+      <c r="F34" s="5" t="s">
         <v>953</v>
       </c>
-      <c r="F34" s="5" t="s">
+      <c r="G34" s="5" t="s">
         <v>954</v>
       </c>
-      <c r="G34" s="5" t="s">
+      <c r="H34" s="5" t="s">
         <v>955</v>
       </c>
-      <c r="H34" s="5" t="s">
+      <c r="I34" s="9" t="s">
+        <v>951</v>
+      </c>
+      <c r="J34" s="5" t="s">
         <v>956</v>
       </c>
-      <c r="I34" s="9" t="s">
-        <v>952</v>
-      </c>
-      <c r="J34" s="5" t="s">
+      <c r="K34" s="5" t="s">
         <v>957</v>
       </c>
-      <c r="K34" s="5" t="s">
+      <c r="L34" s="5" t="s">
         <v>958</v>
       </c>
-      <c r="L34" s="5" t="s">
+      <c r="M34" s="5" t="s">
         <v>959</v>
-      </c>
-      <c r="M34" s="5" t="s">
-        <v>960</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="C35" s="5"/>
       <c r="D35" s="9" t="s">
+        <v>961</v>
+      </c>
+      <c r="E35" s="6" t="s">
         <v>962</v>
       </c>
-      <c r="E35" s="6" t="s">
+      <c r="F35" s="5" t="s">
         <v>963</v>
       </c>
-      <c r="F35" s="5" t="s">
+      <c r="G35" s="5" t="s">
         <v>964</v>
       </c>
-      <c r="G35" s="5" t="s">
+      <c r="H35" s="5" t="s">
         <v>965</v>
       </c>
-      <c r="H35" s="5" t="s">
+      <c r="I35" s="9" t="s">
+        <v>961</v>
+      </c>
+      <c r="J35" s="5" t="s">
         <v>966</v>
       </c>
-      <c r="I35" s="9" t="s">
-        <v>962</v>
-      </c>
-      <c r="J35" s="5" t="s">
+      <c r="K35" s="5" t="s">
         <v>967</v>
       </c>
-      <c r="K35" s="5" t="s">
+      <c r="L35" s="5" t="s">
         <v>968</v>
       </c>
-      <c r="L35" s="5" t="s">
+      <c r="M35" s="5" t="s">
         <v>969</v>
-      </c>
-      <c r="M35" s="5" t="s">
-        <v>970</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
+        <v>970</v>
+      </c>
+      <c r="B36" s="5" t="s">
         <v>971</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>972</v>
       </c>
       <c r="C36" s="5"/>
       <c r="D36" s="9" t="s">
+        <v>972</v>
+      </c>
+      <c r="E36" s="6" t="s">
         <v>973</v>
       </c>
-      <c r="E36" s="6" t="s">
+      <c r="F36" s="5" t="s">
         <v>974</v>
       </c>
-      <c r="F36" s="5" t="s">
+      <c r="G36" s="5" t="s">
         <v>975</v>
       </c>
-      <c r="G36" s="5" t="s">
+      <c r="H36" s="5" t="s">
         <v>976</v>
       </c>
-      <c r="H36" s="5" t="s">
+      <c r="I36" s="9" t="s">
+        <v>972</v>
+      </c>
+      <c r="J36" s="5" t="s">
         <v>977</v>
       </c>
-      <c r="I36" s="9" t="s">
-        <v>973</v>
-      </c>
-      <c r="J36" s="5" t="s">
+      <c r="K36" s="5" t="s">
         <v>978</v>
       </c>
-      <c r="K36" s="5" t="s">
+      <c r="L36" s="5" t="s">
         <v>979</v>
       </c>
-      <c r="L36" s="5" t="s">
+      <c r="M36" s="5" t="s">
         <v>980</v>
-      </c>
-      <c r="M36" s="5" t="s">
-        <v>981</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
+        <v>1095</v>
+      </c>
+      <c r="B37" s="5" t="s">
         <v>1096</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>1097</v>
       </c>
       <c r="C37" s="5"/>
       <c r="D37" s="9" t="s">
+        <v>1097</v>
+      </c>
+      <c r="E37" s="5" t="s">
         <v>1098</v>
       </c>
-      <c r="E37" s="5" t="s">
+      <c r="F37" s="5" t="s">
         <v>1099</v>
       </c>
-      <c r="F37" s="5" t="s">
+      <c r="G37" s="5" t="s">
         <v>1100</v>
       </c>
-      <c r="G37" s="5" t="s">
+      <c r="H37" s="5" t="s">
         <v>1101</v>
       </c>
-      <c r="H37" s="5" t="s">
+      <c r="I37" s="9" t="s">
+        <v>1097</v>
+      </c>
+      <c r="J37" s="5" t="s">
         <v>1102</v>
       </c>
-      <c r="I37" s="9" t="s">
-        <v>1098</v>
-      </c>
-      <c r="J37" s="5" t="s">
+      <c r="K37" s="5" t="s">
         <v>1103</v>
       </c>
-      <c r="K37" s="5" t="s">
+      <c r="L37" s="5" t="s">
         <v>1104</v>
       </c>
-      <c r="L37" s="5" t="s">
+      <c r="M37" s="5" t="s">
         <v>1105</v>
-      </c>
-      <c r="M37" s="5" t="s">
-        <v>1106</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
+        <v>735</v>
+      </c>
+      <c r="B38" s="5" t="s">
         <v>736</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>737</v>
       </c>
       <c r="C38" s="5"/>
       <c r="D38" s="9" t="s">
+        <v>737</v>
+      </c>
+      <c r="E38" s="6" t="s">
         <v>738</v>
       </c>
-      <c r="E38" s="6" t="s">
+      <c r="F38" s="5" t="s">
         <v>739</v>
       </c>
-      <c r="F38" s="5" t="s">
+      <c r="G38" s="5" t="s">
         <v>740</v>
       </c>
-      <c r="G38" s="5" t="s">
+      <c r="H38" s="5" t="s">
         <v>741</v>
       </c>
-      <c r="H38" s="5" t="s">
+      <c r="I38" s="9" t="s">
+        <v>737</v>
+      </c>
+      <c r="J38" s="5" t="s">
         <v>742</v>
       </c>
-      <c r="I38" s="9" t="s">
-        <v>738</v>
-      </c>
-      <c r="J38" s="5" t="s">
+      <c r="K38" s="5" t="s">
         <v>743</v>
       </c>
-      <c r="K38" s="5" t="s">
+      <c r="L38" s="5" t="s">
         <v>744</v>
       </c>
-      <c r="L38" s="5" t="s">
+      <c r="M38" s="5" t="s">
         <v>745</v>
-      </c>
-      <c r="M38" s="5" t="s">
-        <v>746</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
+        <v>768</v>
+      </c>
+      <c r="B39" s="5" t="s">
         <v>769</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>770</v>
       </c>
       <c r="C39" s="5"/>
       <c r="D39" s="9" t="s">
+        <v>770</v>
+      </c>
+      <c r="E39" s="6" t="s">
         <v>771</v>
       </c>
-      <c r="E39" s="6" t="s">
+      <c r="F39" s="5" t="s">
         <v>772</v>
       </c>
-      <c r="F39" s="5" t="s">
+      <c r="G39" s="5" t="s">
         <v>773</v>
       </c>
-      <c r="G39" s="5" t="s">
+      <c r="H39" s="5" t="s">
         <v>774</v>
       </c>
-      <c r="H39" s="5" t="s">
+      <c r="I39" s="9" t="s">
+        <v>770</v>
+      </c>
+      <c r="J39" s="5" t="s">
         <v>775</v>
       </c>
-      <c r="I39" s="9" t="s">
-        <v>771</v>
-      </c>
-      <c r="J39" s="5" t="s">
+      <c r="K39" s="5" t="s">
         <v>776</v>
       </c>
-      <c r="K39" s="5" t="s">
+      <c r="L39" s="5" t="s">
         <v>777</v>
       </c>
-      <c r="L39" s="5" t="s">
+      <c r="M39" s="5" t="s">
         <v>778</v>
       </c>
-      <c r="M39" s="5" t="s">
-        <v>779</v>
-      </c>
       <c r="N39" s="5" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
+        <v>781</v>
+      </c>
+      <c r="B40" s="5" t="s">
         <v>782</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>783</v>
       </c>
       <c r="C40" s="5"/>
       <c r="D40" s="9" t="s">
+        <v>783</v>
+      </c>
+      <c r="E40" s="6" t="s">
         <v>784</v>
       </c>
-      <c r="E40" s="6" t="s">
+      <c r="F40" s="5" t="s">
         <v>785</v>
       </c>
-      <c r="F40" s="5" t="s">
+      <c r="G40" s="5" t="s">
         <v>786</v>
       </c>
-      <c r="G40" s="5" t="s">
+      <c r="H40" s="5" t="s">
         <v>787</v>
       </c>
-      <c r="H40" s="5" t="s">
+      <c r="I40" s="9" t="s">
+        <v>783</v>
+      </c>
+      <c r="J40" s="5" t="s">
         <v>788</v>
       </c>
-      <c r="I40" s="9" t="s">
-        <v>784</v>
-      </c>
-      <c r="J40" s="5" t="s">
+      <c r="K40" s="5" t="s">
         <v>789</v>
       </c>
-      <c r="K40" s="5" t="s">
+      <c r="L40" s="5" t="s">
         <v>790</v>
       </c>
-      <c r="L40" s="5" t="s">
+      <c r="M40" s="5" t="s">
         <v>791</v>
-      </c>
-      <c r="M40" s="5" t="s">
-        <v>792</v>
       </c>
       <c r="N40" s="5"/>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="11" t="s">
+        <v>746</v>
+      </c>
+      <c r="B41" s="5" t="s">
         <v>747</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>748</v>
       </c>
       <c r="C41" s="5"/>
       <c r="D41" s="9" t="s">
+        <v>748</v>
+      </c>
+      <c r="E41" s="6" t="s">
         <v>749</v>
       </c>
-      <c r="E41" s="6" t="s">
+      <c r="F41" s="5" t="s">
         <v>750</v>
       </c>
-      <c r="F41" s="5" t="s">
+      <c r="G41" s="5" t="s">
         <v>751</v>
       </c>
-      <c r="G41" s="5" t="s">
+      <c r="H41" s="5" t="s">
         <v>752</v>
       </c>
-      <c r="H41" s="5" t="s">
+      <c r="I41" s="9" t="s">
+        <v>748</v>
+      </c>
+      <c r="J41" s="5" t="s">
         <v>753</v>
       </c>
-      <c r="I41" s="9" t="s">
-        <v>749</v>
-      </c>
-      <c r="J41" s="5" t="s">
+      <c r="K41" s="5" t="s">
         <v>754</v>
       </c>
-      <c r="K41" s="5" t="s">
+      <c r="L41" s="5" t="s">
         <v>755</v>
       </c>
-      <c r="L41" s="5" t="s">
+      <c r="M41" s="5" t="s">
         <v>756</v>
-      </c>
-      <c r="M41" s="5" t="s">
-        <v>757</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
+        <v>757</v>
+      </c>
+      <c r="B42" s="5" t="s">
         <v>758</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>759</v>
       </c>
       <c r="C42" s="5"/>
       <c r="D42" s="9" t="s">
+        <v>759</v>
+      </c>
+      <c r="E42" s="6" t="s">
         <v>760</v>
       </c>
-      <c r="E42" s="6" t="s">
+      <c r="F42" s="5" t="s">
         <v>761</v>
       </c>
-      <c r="F42" s="5" t="s">
+      <c r="G42" s="5" t="s">
         <v>762</v>
       </c>
-      <c r="G42" s="5" t="s">
+      <c r="H42" s="5" t="s">
         <v>763</v>
       </c>
-      <c r="H42" s="5" t="s">
+      <c r="I42" s="9" t="s">
+        <v>759</v>
+      </c>
+      <c r="J42" s="5" t="s">
         <v>764</v>
       </c>
-      <c r="I42" s="9" t="s">
-        <v>760</v>
-      </c>
-      <c r="J42" s="5" t="s">
+      <c r="K42" s="5" t="s">
         <v>765</v>
       </c>
-      <c r="K42" s="5" t="s">
+      <c r="L42" s="5" t="s">
         <v>766</v>
       </c>
-      <c r="L42" s="5" t="s">
+      <c r="M42" s="5" t="s">
         <v>767</v>
-      </c>
-      <c r="M42" s="5" t="s">
-        <v>768</v>
       </c>
     </row>
   </sheetData>
@@ -6140,7 +6140,7 @@
   <sheetPr codeName="FXRates_Fields"/>
   <dimension ref="A1:P36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -6171,7 +6171,7 @@
         <v>17</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>1115</v>
+        <v>1113</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>1</v>
@@ -6210,7 +6210,7 @@
         <v>121</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="15" x14ac:dyDescent="0.25">
@@ -6221,10 +6221,10 @@
         <v>44</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>1118</v>
+        <v>1116</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>1119</v>
+        <v>1117</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>132</v>
@@ -6239,7 +6239,7 @@
         <v>48</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>1119</v>
+        <v>1117</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>129</v>
@@ -6284,7 +6284,7 @@
         <v>74</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="J3" s="5" t="s">
         <v>75</v>
@@ -6329,7 +6329,7 @@
         <v>85</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="J4" s="5" t="s">
         <v>81</v>
@@ -6374,7 +6374,7 @@
         <v>86</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="J5" s="5" t="s">
         <v>82</v>
@@ -6419,7 +6419,7 @@
         <v>91</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="J6" s="5" t="s">
         <v>92</v>
@@ -6464,7 +6464,7 @@
         <v>126</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="J7" s="5" t="s">
         <v>127</v>
@@ -6497,7 +6497,7 @@
         <v>130</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>260</v>
@@ -6509,7 +6509,7 @@
         <v>262</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="J8" s="5" t="s">
         <v>263</v>
@@ -6542,7 +6542,7 @@
         <v>130</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>268</v>
@@ -6554,7 +6554,7 @@
         <v>270</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="J9" s="5" t="s">
         <v>271</v>
@@ -6587,7 +6587,7 @@
         <v>130</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>276</v>
@@ -6599,7 +6599,7 @@
         <v>278</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="J10" s="5" t="s">
         <v>279</v>
@@ -6632,7 +6632,7 @@
         <v>130</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>284</v>
@@ -6644,7 +6644,7 @@
         <v>286</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="J11" s="5" t="s">
         <v>287</v>
@@ -6677,7 +6677,7 @@
         <v>130</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>1112</v>
+        <v>1110</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>292</v>
@@ -6689,7 +6689,7 @@
         <v>294</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="J12" s="5" t="s">
         <v>295</v>
@@ -6722,7 +6722,7 @@
         <v>130</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>1113</v>
+        <v>1111</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>300</v>
@@ -6734,7 +6734,7 @@
         <v>302</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="J13" s="5" t="s">
         <v>303</v>
@@ -6767,7 +6767,7 @@
         <v>130</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>1114</v>
+        <v>1112</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>308</v>
@@ -6779,7 +6779,7 @@
         <v>310</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="J14" s="5" t="s">
         <v>311</v>
@@ -6824,7 +6824,7 @@
         <v>319</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="J15" s="5" t="s">
         <v>320</v>
@@ -6869,7 +6869,7 @@
         <v>328</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="J16" s="5" t="s">
         <v>329</v>
@@ -6914,7 +6914,7 @@
         <v>338</v>
       </c>
       <c r="I17" s="9" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="J17" s="5" t="s">
         <v>339</v>
@@ -6959,7 +6959,7 @@
         <v>348</v>
       </c>
       <c r="I18" s="9" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="J18" s="5" t="s">
         <v>349</v>
@@ -7004,7 +7004,7 @@
         <v>358</v>
       </c>
       <c r="I19" s="9" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="J19" s="5" t="s">
         <v>359</v>
@@ -7049,7 +7049,7 @@
         <v>367</v>
       </c>
       <c r="I20" s="9" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="J20" s="5" t="s">
         <v>368</v>
@@ -7070,7 +7070,7 @@
         <v>243</v>
       </c>
       <c r="P20" s="5" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="15" x14ac:dyDescent="0.25">
@@ -7097,7 +7097,7 @@
         <v>376</v>
       </c>
       <c r="I21" s="9" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="J21" s="5" t="s">
         <v>377</v>
@@ -7142,7 +7142,7 @@
         <v>385</v>
       </c>
       <c r="I22" s="9" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="J22" s="5" t="s">
         <v>386</v>
@@ -7187,7 +7187,7 @@
         <v>394</v>
       </c>
       <c r="I23" s="9" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="J23" s="5" t="s">
         <v>395</v>
@@ -7232,7 +7232,7 @@
         <v>404</v>
       </c>
       <c r="I24" s="9" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="J24" s="5" t="s">
         <v>405</v>
@@ -7277,7 +7277,7 @@
         <v>414</v>
       </c>
       <c r="I25" s="9" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="J25" s="5" t="s">
         <v>415</v>
@@ -7322,7 +7322,7 @@
         <v>423</v>
       </c>
       <c r="I26" s="9" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="J26" s="5" t="s">
         <v>424</v>
@@ -7367,7 +7367,7 @@
         <v>433</v>
       </c>
       <c r="I27" s="9" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="J27" s="5" t="s">
         <v>434</v>
@@ -7412,7 +7412,7 @@
         <v>443</v>
       </c>
       <c r="I28" s="9" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="J28" s="5" t="s">
         <v>444</v>
@@ -7457,7 +7457,7 @@
         <v>453</v>
       </c>
       <c r="I29" s="9" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="J29" s="5" t="s">
         <v>454</v>
@@ -7502,7 +7502,7 @@
         <v>463</v>
       </c>
       <c r="I30" s="9" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="J30" s="5" t="s">
         <v>464</v>
@@ -7547,7 +7547,7 @@
         <v>473</v>
       </c>
       <c r="I31" s="9" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="J31" s="5" t="s">
         <v>474</v>
@@ -7570,41 +7570,41 @@
     </row>
     <row r="32" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
+        <v>592</v>
+      </c>
+      <c r="B32" s="5" t="s">
         <v>593</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>594</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="9" t="s">
         <v>130</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="F32" s="5" t="s">
+        <v>594</v>
+      </c>
+      <c r="G32" s="5" t="s">
         <v>595</v>
       </c>
-      <c r="G32" s="5" t="s">
+      <c r="H32" s="5" t="s">
         <v>596</v>
       </c>
-      <c r="H32" s="5" t="s">
+      <c r="I32" s="9" t="s">
+        <v>641</v>
+      </c>
+      <c r="J32" s="5" t="s">
         <v>597</v>
       </c>
-      <c r="I32" s="9" t="s">
-        <v>642</v>
-      </c>
-      <c r="J32" s="5" t="s">
+      <c r="K32" s="5" t="s">
         <v>598</v>
       </c>
-      <c r="K32" s="5" t="s">
+      <c r="L32" s="5" t="s">
         <v>599</v>
       </c>
-      <c r="L32" s="5" t="s">
+      <c r="M32" s="5" t="s">
         <v>600</v>
-      </c>
-      <c r="M32" s="5" t="s">
-        <v>601</v>
       </c>
       <c r="N32" s="5" t="s">
         <v>12</v>
@@ -7615,41 +7615,41 @@
     </row>
     <row r="33" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
+        <v>601</v>
+      </c>
+      <c r="B33" s="5" t="s">
         <v>602</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>603</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="9" t="s">
         <v>130</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="F33" s="5" t="s">
+        <v>603</v>
+      </c>
+      <c r="G33" s="5" t="s">
         <v>604</v>
       </c>
-      <c r="G33" s="5" t="s">
+      <c r="H33" s="5" t="s">
         <v>605</v>
       </c>
-      <c r="H33" s="5" t="s">
+      <c r="I33" s="9" t="s">
+        <v>640</v>
+      </c>
+      <c r="J33" s="5" t="s">
         <v>606</v>
       </c>
-      <c r="I33" s="9" t="s">
-        <v>641</v>
-      </c>
-      <c r="J33" s="5" t="s">
+      <c r="K33" s="5" t="s">
         <v>607</v>
       </c>
-      <c r="K33" s="5" t="s">
+      <c r="L33" s="5" t="s">
         <v>608</v>
       </c>
-      <c r="L33" s="5" t="s">
+      <c r="M33" s="5" t="s">
         <v>609</v>
-      </c>
-      <c r="M33" s="5" t="s">
-        <v>610</v>
       </c>
       <c r="N33" s="5" t="s">
         <v>12</v>
@@ -7660,41 +7660,41 @@
     </row>
     <row r="34" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
+        <v>610</v>
+      </c>
+      <c r="B34" s="5" t="s">
         <v>611</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>612</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="9" t="s">
         <v>130</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="F34" s="5" t="s">
+        <v>612</v>
+      </c>
+      <c r="G34" s="5" t="s">
         <v>613</v>
       </c>
-      <c r="G34" s="5" t="s">
+      <c r="H34" s="5" t="s">
         <v>614</v>
       </c>
-      <c r="H34" s="5" t="s">
+      <c r="I34" s="9" t="s">
+        <v>639</v>
+      </c>
+      <c r="J34" s="5" t="s">
         <v>615</v>
       </c>
-      <c r="I34" s="9" t="s">
-        <v>640</v>
-      </c>
-      <c r="J34" s="5" t="s">
+      <c r="K34" s="5" t="s">
         <v>616</v>
       </c>
-      <c r="K34" s="5" t="s">
+      <c r="L34" s="5" t="s">
         <v>617</v>
       </c>
-      <c r="L34" s="5" t="s">
+      <c r="M34" s="5" t="s">
         <v>618</v>
-      </c>
-      <c r="M34" s="5" t="s">
-        <v>619</v>
       </c>
       <c r="N34" s="5" t="s">
         <v>12</v>
@@ -7705,41 +7705,41 @@
     </row>
     <row r="35" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
+        <v>619</v>
+      </c>
+      <c r="B35" s="5" t="s">
         <v>620</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>621</v>
       </c>
       <c r="C35" s="5"/>
       <c r="D35" s="9" t="s">
         <v>130</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="F35" s="5" t="s">
+        <v>621</v>
+      </c>
+      <c r="G35" s="5" t="s">
         <v>622</v>
       </c>
-      <c r="G35" s="5" t="s">
+      <c r="H35" s="5" t="s">
         <v>623</v>
       </c>
-      <c r="H35" s="5" t="s">
+      <c r="I35" s="9" t="s">
+        <v>638</v>
+      </c>
+      <c r="J35" s="5" t="s">
         <v>624</v>
       </c>
-      <c r="I35" s="9" t="s">
-        <v>639</v>
-      </c>
-      <c r="J35" s="5" t="s">
+      <c r="K35" s="5" t="s">
         <v>625</v>
       </c>
-      <c r="K35" s="5" t="s">
+      <c r="L35" s="5" t="s">
         <v>626</v>
       </c>
-      <c r="L35" s="5" t="s">
+      <c r="M35" s="5" t="s">
         <v>627</v>
-      </c>
-      <c r="M35" s="5" t="s">
-        <v>628</v>
       </c>
       <c r="N35" s="5" t="s">
         <v>12</v>
@@ -7750,41 +7750,41 @@
     </row>
     <row r="36" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
+        <v>628</v>
+      </c>
+      <c r="B36" s="5" t="s">
         <v>629</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>630</v>
       </c>
       <c r="C36" s="5"/>
       <c r="D36" s="9" t="s">
         <v>130</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="F36" s="5" t="s">
+        <v>630</v>
+      </c>
+      <c r="G36" s="5" t="s">
         <v>631</v>
       </c>
-      <c r="G36" s="5" t="s">
+      <c r="H36" s="5" t="s">
         <v>632</v>
       </c>
-      <c r="H36" s="5" t="s">
+      <c r="I36" s="9" t="s">
+        <v>637</v>
+      </c>
+      <c r="J36" s="5" t="s">
         <v>633</v>
       </c>
-      <c r="I36" s="9" t="s">
-        <v>638</v>
-      </c>
-      <c r="J36" s="5" t="s">
+      <c r="K36" s="5" t="s">
         <v>634</v>
       </c>
-      <c r="K36" s="5" t="s">
+      <c r="L36" s="5" t="s">
         <v>635</v>
       </c>
-      <c r="L36" s="5" t="s">
+      <c r="M36" s="5" t="s">
         <v>636</v>
-      </c>
-      <c r="M36" s="5" t="s">
-        <v>637</v>
       </c>
       <c r="N36" s="5" t="s">
         <v>12</v>
@@ -7820,23 +7820,24 @@
   </sheetPr>
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="53.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="67.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="94" style="1" customWidth="1"/>
     <col min="5" max="5" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="33.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="42.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="36.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="33.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="75.7109375" style="1" customWidth="1"/>
     <col min="10" max="10" width="37.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="40" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="40" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="60.28515625" customWidth="1"/>
     <col min="13" max="13" width="45" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -7881,7 +7882,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -7889,10 +7890,10 @@
         <v>140</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>480</v>
+        <v>1118</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>143</v>
@@ -7904,7 +7905,7 @@
         <v>145</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>480</v>
+        <v>1118</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>166</v>
@@ -7919,1279 +7920,1279 @@
         <v>168</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>480</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>481</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="D3" s="6" t="s">
+        <v>833</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>482</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>834</v>
-      </c>
-      <c r="E3" s="5" t="s">
+      <c r="F3" s="5" t="s">
         <v>483</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="G3" s="5" t="s">
         <v>484</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="H3" s="5" t="s">
+        <v>820</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>481</v>
+      </c>
+      <c r="J3" s="5" t="s">
         <v>485</v>
       </c>
-      <c r="H3" s="5" t="s">
-        <v>821</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>482</v>
-      </c>
-      <c r="J3" s="5" t="s">
+      <c r="K3" s="5" t="s">
         <v>486</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="L3" s="5" t="s">
         <v>487</v>
       </c>
-      <c r="L3" s="5" t="s">
-        <v>488</v>
-      </c>
       <c r="M3" s="5" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>36</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>874</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>875</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="D4" s="6" t="s">
+        <v>883</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>876</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>884</v>
-      </c>
-      <c r="E4" s="5" t="s">
+      <c r="F4" s="5" t="s">
         <v>877</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="G4" s="5" t="s">
         <v>878</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="H4" s="5" t="s">
         <v>879</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="I4" s="9" t="s">
+        <v>875</v>
+      </c>
+      <c r="J4" s="5" t="s">
         <v>880</v>
       </c>
-      <c r="I4" s="9" t="s">
-        <v>876</v>
-      </c>
-      <c r="J4" s="5" t="s">
+      <c r="K4" s="5" t="s">
         <v>881</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="L4" s="5" t="s">
         <v>882</v>
       </c>
-      <c r="L4" s="5" t="s">
-        <v>883</v>
-      </c>
       <c r="M4" s="5" t="s">
-        <v>883</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>43</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>884</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>885</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="D5" s="6" t="s">
+        <v>893</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>886</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>894</v>
-      </c>
-      <c r="E5" s="5" t="s">
+      <c r="F5" s="5" t="s">
         <v>887</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="G5" s="5" t="s">
         <v>888</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="H5" s="5" t="s">
         <v>889</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="I5" s="9" t="s">
+        <v>885</v>
+      </c>
+      <c r="J5" s="5" t="s">
         <v>890</v>
       </c>
-      <c r="I5" s="9" t="s">
-        <v>886</v>
-      </c>
-      <c r="J5" s="5" t="s">
+      <c r="K5" s="5" t="s">
         <v>891</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="L5" s="5" t="s">
         <v>892</v>
       </c>
-      <c r="L5" s="5" t="s">
-        <v>893</v>
-      </c>
       <c r="M5" s="5" t="s">
-        <v>893</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>64</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>821</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>822</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="D6" s="6" t="s">
         <v>823</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="E6" s="5" t="s">
         <v>824</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="F6" s="5" t="s">
         <v>825</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="G6" s="5" t="s">
         <v>826</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="H6" s="5" t="s">
         <v>827</v>
       </c>
-      <c r="H6" s="5" t="s">
-        <v>828</v>
-      </c>
       <c r="I6" s="9" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="J6" s="5" t="s">
+        <v>830</v>
+      </c>
+      <c r="K6" s="5" t="s">
         <v>831</v>
       </c>
-      <c r="K6" s="5" t="s">
+      <c r="L6" s="5" t="s">
         <v>832</v>
       </c>
-      <c r="L6" s="5" t="s">
-        <v>833</v>
-      </c>
       <c r="M6" s="5" t="s">
-        <v>833</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>96</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>802</v>
+      </c>
+      <c r="C7" s="9" t="s">
         <v>803</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="D7" s="6" t="s">
+        <v>809</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>804</v>
       </c>
-      <c r="D7" s="6" t="s">
-        <v>810</v>
-      </c>
-      <c r="E7" s="5" t="s">
+      <c r="F7" s="5" t="s">
         <v>805</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="G7" s="5" t="s">
         <v>806</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="H7" s="5" t="s">
+        <v>828</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>803</v>
+      </c>
+      <c r="J7" s="5" t="s">
         <v>807</v>
       </c>
-      <c r="H7" s="5" t="s">
-        <v>829</v>
-      </c>
-      <c r="I7" s="9" t="s">
-        <v>804</v>
-      </c>
-      <c r="J7" s="5" t="s">
+      <c r="K7" s="5" t="s">
         <v>808</v>
       </c>
-      <c r="K7" s="5" t="s">
-        <v>809</v>
-      </c>
       <c r="L7" s="5" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="M7" s="5" t="s">
-        <v>819</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>103</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>810</v>
+      </c>
+      <c r="C8" s="9" t="s">
         <v>811</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="D8" s="6" t="s">
+        <v>819</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>812</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>820</v>
-      </c>
-      <c r="E8" s="5" t="s">
+      <c r="F8" s="5" t="s">
         <v>813</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="G8" s="5" t="s">
         <v>814</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="H8" s="5" t="s">
+        <v>829</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>811</v>
+      </c>
+      <c r="J8" s="5" t="s">
         <v>815</v>
       </c>
-      <c r="H8" s="5" t="s">
-        <v>830</v>
-      </c>
-      <c r="I8" s="9" t="s">
-        <v>812</v>
-      </c>
-      <c r="J8" s="5" t="s">
+      <c r="K8" s="5" t="s">
         <v>816</v>
       </c>
-      <c r="K8" s="5" t="s">
+      <c r="L8" s="5" t="s">
+        <v>487</v>
+      </c>
+      <c r="M8" s="5" t="s">
         <v>817</v>
       </c>
-      <c r="L8" s="5" t="s">
-        <v>488</v>
-      </c>
-      <c r="M8" s="5" t="s">
-        <v>818</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>111</v>
       </c>
       <c r="B9" s="5" t="s">
+        <v>834</v>
+      </c>
+      <c r="C9" s="9" t="s">
         <v>835</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="D9" s="6" t="s">
         <v>836</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="E9" s="5" t="s">
         <v>837</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="F9" s="5" t="s">
         <v>838</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="G9" s="5" t="s">
         <v>839</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="H9" s="5" t="s">
         <v>840</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="I9" s="9" t="s">
+        <v>835</v>
+      </c>
+      <c r="J9" s="5" t="s">
         <v>841</v>
       </c>
-      <c r="I9" s="9" t="s">
-        <v>836</v>
-      </c>
-      <c r="J9" s="5" t="s">
+      <c r="K9" s="5" t="s">
         <v>842</v>
       </c>
-      <c r="K9" s="5" t="s">
+      <c r="L9" s="5" t="s">
         <v>843</v>
       </c>
-      <c r="L9" s="5" t="s">
-        <v>844</v>
-      </c>
       <c r="M9" s="5" t="s">
-        <v>844</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>113</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>488</v>
+      </c>
+      <c r="C10" s="9" t="s">
         <v>489</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="D10" s="6" t="s">
+        <v>792</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>490</v>
       </c>
-      <c r="D10" s="6" t="s">
-        <v>793</v>
-      </c>
-      <c r="E10" s="5" t="s">
+      <c r="F10" s="5" t="s">
         <v>491</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="G10" s="5" t="s">
         <v>492</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="H10" s="5" t="s">
+        <v>844</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>489</v>
+      </c>
+      <c r="J10" s="5" t="s">
         <v>493</v>
       </c>
-      <c r="H10" s="5" t="s">
-        <v>845</v>
-      </c>
-      <c r="I10" s="9" t="s">
-        <v>490</v>
-      </c>
-      <c r="J10" s="5" t="s">
+      <c r="K10" s="5" t="s">
         <v>494</v>
       </c>
-      <c r="K10" s="5" t="s">
+      <c r="L10" s="5" t="s">
         <v>495</v>
       </c>
-      <c r="L10" s="5" t="s">
-        <v>496</v>
-      </c>
       <c r="M10" s="5" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>115</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>1026</v>
+      </c>
+      <c r="C11" s="9" t="s">
         <v>1027</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="D11" s="6" t="s">
         <v>1028</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="E11" s="5" t="s">
         <v>1029</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="F11" s="5" t="s">
         <v>1030</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="G11" s="5" t="s">
         <v>1031</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="H11" s="5" t="s">
         <v>1032</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="I11" s="9" t="s">
+        <v>1027</v>
+      </c>
+      <c r="J11" s="5" t="s">
         <v>1033</v>
       </c>
-      <c r="I11" s="9" t="s">
-        <v>1028</v>
-      </c>
-      <c r="J11" s="5" t="s">
+      <c r="K11" s="5" t="s">
         <v>1034</v>
       </c>
-      <c r="K11" s="5" t="s">
+      <c r="L11" s="5" t="s">
         <v>1035</v>
       </c>
-      <c r="L11" s="5" t="s">
-        <v>1036</v>
-      </c>
       <c r="M11" s="5" t="s">
-        <v>1036</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>117</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>1036</v>
+      </c>
+      <c r="C12" s="9" t="s">
         <v>1037</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="D12" s="6" t="s">
         <v>1038</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="E12" s="5" t="s">
         <v>1039</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="F12" s="5" t="s">
         <v>1040</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="G12" s="5" t="s">
         <v>1041</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="H12" s="5" t="s">
         <v>1042</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="I12" s="9" t="s">
+        <v>1037</v>
+      </c>
+      <c r="J12" s="5" t="s">
         <v>1043</v>
       </c>
-      <c r="I12" s="9" t="s">
-        <v>1038</v>
-      </c>
-      <c r="J12" s="5" t="s">
+      <c r="K12" s="5" t="s">
         <v>1044</v>
       </c>
-      <c r="K12" s="5" t="s">
+      <c r="L12" s="5" t="s">
         <v>1045</v>
       </c>
-      <c r="L12" s="5" t="s">
-        <v>1046</v>
-      </c>
       <c r="M12" s="5" t="s">
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>119</v>
       </c>
       <c r="B13" s="5" t="s">
+        <v>904</v>
+      </c>
+      <c r="C13" s="9" t="s">
         <v>905</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="D13" s="6" t="s">
         <v>906</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="E13" s="5" t="s">
         <v>907</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="F13" s="5" t="s">
         <v>908</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="G13" s="5" t="s">
         <v>909</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="H13" s="5" t="s">
         <v>910</v>
       </c>
-      <c r="H13" s="5" t="s">
+      <c r="I13" s="9" t="s">
+        <v>905</v>
+      </c>
+      <c r="J13" s="5" t="s">
         <v>911</v>
       </c>
-      <c r="I13" s="9" t="s">
-        <v>906</v>
-      </c>
-      <c r="J13" s="5" t="s">
+      <c r="K13" s="5" t="s">
         <v>912</v>
       </c>
-      <c r="K13" s="5" t="s">
+      <c r="L13" s="5" t="s">
         <v>913</v>
       </c>
-      <c r="L13" s="5" t="s">
-        <v>914</v>
-      </c>
       <c r="M13" s="5" t="s">
-        <v>914</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>146</v>
       </c>
       <c r="B14" s="5" t="s">
+        <v>496</v>
+      </c>
+      <c r="C14" s="9" t="s">
         <v>497</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="D14" s="6" t="s">
+        <v>793</v>
+      </c>
+      <c r="E14" s="5" t="s">
         <v>498</v>
       </c>
-      <c r="D14" s="6" t="s">
-        <v>794</v>
-      </c>
-      <c r="E14" s="5" t="s">
+      <c r="F14" s="5" t="s">
         <v>499</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="G14" s="5" t="s">
         <v>500</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>501</v>
       </c>
       <c r="H14" s="5"/>
       <c r="I14" s="9" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="J14" s="5" t="s">
+        <v>501</v>
+      </c>
+      <c r="K14" s="5" t="s">
         <v>502</v>
       </c>
-      <c r="K14" s="5" t="s">
+      <c r="L14" s="5" t="s">
         <v>503</v>
       </c>
-      <c r="L14" s="5" t="s">
+      <c r="M14" s="5" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
         <v>504</v>
       </c>
-      <c r="M14" s="5" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+      <c r="B15" s="5" t="s">
         <v>505</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="C15" s="9" t="s">
         <v>506</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="D15" s="6" t="s">
+        <v>794</v>
+      </c>
+      <c r="E15" s="5" t="s">
         <v>507</v>
       </c>
-      <c r="D15" s="6" t="s">
-        <v>795</v>
-      </c>
-      <c r="E15" s="5" t="s">
+      <c r="F15" s="5" t="s">
         <v>508</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="G15" s="5" t="s">
         <v>509</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>510</v>
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="9" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="J15" s="5" t="s">
+        <v>510</v>
+      </c>
+      <c r="K15" s="5" t="s">
         <v>511</v>
       </c>
-      <c r="K15" s="5" t="s">
+      <c r="L15" s="5" t="s">
         <v>512</v>
       </c>
-      <c r="L15" s="5" t="s">
+      <c r="M15" s="5" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
         <v>513</v>
       </c>
-      <c r="M15" s="5" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+      <c r="B16" s="5" t="s">
         <v>514</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="C16" s="9" t="s">
+        <v>506</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>795</v>
+      </c>
+      <c r="E16" s="5" t="s">
         <v>515</v>
       </c>
-      <c r="C16" s="9" t="s">
-        <v>507</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>796</v>
-      </c>
-      <c r="E16" s="5" t="s">
+      <c r="F16" s="5" t="s">
         <v>516</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="G16" s="5" t="s">
         <v>517</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>518</v>
       </c>
       <c r="H16" s="5"/>
       <c r="I16" s="9" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="J16" s="5" t="s">
+        <v>518</v>
+      </c>
+      <c r="K16" s="5" t="s">
         <v>519</v>
       </c>
-      <c r="K16" s="5" t="s">
+      <c r="L16" s="5" t="s">
         <v>520</v>
       </c>
-      <c r="L16" s="5" t="s">
-        <v>521</v>
-      </c>
       <c r="M16" s="5" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>17</v>
       </c>
       <c r="B17" s="5" t="s">
+        <v>521</v>
+      </c>
+      <c r="C17" s="9" t="s">
         <v>522</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="D17" s="6" t="s">
+        <v>796</v>
+      </c>
+      <c r="E17" s="5" t="s">
         <v>523</v>
       </c>
-      <c r="D17" s="6" t="s">
-        <v>797</v>
-      </c>
-      <c r="E17" s="5" t="s">
+      <c r="F17" s="5" t="s">
         <v>524</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="G17" s="5" t="s">
         <v>525</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="H17" s="5" t="s">
         <v>526</v>
       </c>
-      <c r="H17" s="5" t="s">
+      <c r="I17" s="9" t="s">
+        <v>522</v>
+      </c>
+      <c r="J17" s="5" t="s">
         <v>527</v>
       </c>
-      <c r="I17" s="9" t="s">
-        <v>523</v>
-      </c>
-      <c r="J17" s="5" t="s">
+      <c r="K17" s="5" t="s">
         <v>528</v>
       </c>
-      <c r="K17" s="5" t="s">
+      <c r="L17" s="5" t="s">
         <v>529</v>
       </c>
-      <c r="L17" s="5" t="s">
-        <v>530</v>
-      </c>
       <c r="M17" s="5" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>18</v>
       </c>
       <c r="B18" s="5" t="s">
+        <v>530</v>
+      </c>
+      <c r="C18" s="9" t="s">
         <v>531</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="D18" s="6" t="s">
+        <v>797</v>
+      </c>
+      <c r="E18" s="5" t="s">
         <v>532</v>
       </c>
-      <c r="D18" s="6" t="s">
-        <v>798</v>
-      </c>
-      <c r="E18" s="5" t="s">
+      <c r="F18" s="5" t="s">
         <v>533</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="G18" s="5" t="s">
         <v>534</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>535</v>
       </c>
       <c r="H18" s="5"/>
       <c r="I18" s="9" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="J18" s="5" t="s">
+        <v>535</v>
+      </c>
+      <c r="K18" s="5" t="s">
         <v>536</v>
       </c>
-      <c r="K18" s="5" t="s">
+      <c r="L18" s="5" t="s">
         <v>537</v>
       </c>
-      <c r="L18" s="5" t="s">
-        <v>538</v>
-      </c>
       <c r="M18" s="5" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>19</v>
       </c>
       <c r="B19" s="5" t="s">
+        <v>538</v>
+      </c>
+      <c r="C19" s="9" t="s">
         <v>539</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="D19" s="6" t="s">
+        <v>798</v>
+      </c>
+      <c r="E19" s="5" t="s">
         <v>540</v>
       </c>
-      <c r="D19" s="6" t="s">
-        <v>799</v>
-      </c>
-      <c r="E19" s="5" t="s">
+      <c r="F19" s="5" t="s">
         <v>541</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="G19" s="5" t="s">
         <v>542</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>543</v>
       </c>
       <c r="H19" s="5"/>
       <c r="I19" s="9" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="J19" s="5" t="s">
+        <v>543</v>
+      </c>
+      <c r="K19" s="5" t="s">
         <v>544</v>
       </c>
-      <c r="K19" s="5" t="s">
+      <c r="L19" s="5" t="s">
         <v>545</v>
       </c>
-      <c r="L19" s="5" t="s">
-        <v>546</v>
-      </c>
       <c r="M19" s="5" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>210</v>
       </c>
       <c r="B20" s="5" t="s">
+        <v>691</v>
+      </c>
+      <c r="C20" s="9" t="s">
         <v>692</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="D20" s="6" t="s">
+        <v>799</v>
+      </c>
+      <c r="E20" s="5" t="s">
         <v>693</v>
       </c>
-      <c r="D20" s="6" t="s">
-        <v>800</v>
-      </c>
-      <c r="E20" s="5" t="s">
+      <c r="F20" s="5" t="s">
         <v>694</v>
       </c>
-      <c r="F20" s="5" t="s">
+      <c r="G20" s="5" t="s">
         <v>695</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>696</v>
       </c>
       <c r="H20" s="5"/>
       <c r="I20" s="9" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="J20" s="5" t="s">
+        <v>696</v>
+      </c>
+      <c r="K20" s="5" t="s">
         <v>697</v>
       </c>
-      <c r="K20" s="5" t="s">
+      <c r="L20" s="5" t="s">
         <v>698</v>
       </c>
-      <c r="L20" s="5" t="s">
-        <v>699</v>
-      </c>
       <c r="M20" s="5" t="s">
-        <v>699</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>230</v>
       </c>
       <c r="B21" s="5" t="s">
+        <v>584</v>
+      </c>
+      <c r="C21" s="9" t="s">
         <v>585</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="D21" s="6" t="s">
+        <v>799</v>
+      </c>
+      <c r="E21" s="5" t="s">
         <v>586</v>
       </c>
-      <c r="D21" s="6" t="s">
-        <v>800</v>
-      </c>
-      <c r="E21" s="5" t="s">
+      <c r="F21" s="5" t="s">
         <v>587</v>
       </c>
-      <c r="F21" s="5" t="s">
+      <c r="G21" s="5" t="s">
         <v>588</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>589</v>
       </c>
       <c r="H21" s="5"/>
       <c r="I21" s="9" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="J21" s="5" t="s">
+        <v>589</v>
+      </c>
+      <c r="K21" s="5" t="s">
         <v>590</v>
       </c>
-      <c r="K21" s="5" t="s">
+      <c r="L21" s="5" t="s">
         <v>591</v>
       </c>
-      <c r="L21" s="5" t="s">
-        <v>592</v>
-      </c>
       <c r="M21" s="5" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>419</v>
       </c>
       <c r="B22" s="5" t="s">
+        <v>1066</v>
+      </c>
+      <c r="C22" s="9" t="s">
         <v>1067</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="D22" s="6" t="s">
+        <v>1108</v>
+      </c>
+      <c r="E22" s="5" t="s">
         <v>1068</v>
       </c>
-      <c r="D22" s="6" t="s">
-        <v>1109</v>
-      </c>
-      <c r="E22" s="5" t="s">
+      <c r="F22" s="5" t="s">
         <v>1069</v>
       </c>
-      <c r="F22" s="5" t="s">
+      <c r="G22" s="5" t="s">
         <v>1070</v>
       </c>
-      <c r="G22" s="5" t="s">
+      <c r="H22" s="5" t="s">
         <v>1071</v>
       </c>
-      <c r="H22" s="5" t="s">
+      <c r="I22" s="9" t="s">
+        <v>1067</v>
+      </c>
+      <c r="J22" s="5" t="s">
         <v>1072</v>
       </c>
-      <c r="I22" s="9" t="s">
-        <v>1068</v>
-      </c>
-      <c r="J22" s="5" t="s">
+      <c r="K22" s="5" t="s">
         <v>1073</v>
       </c>
-      <c r="K22" s="5" t="s">
+      <c r="L22" s="5" t="s">
         <v>1074</v>
       </c>
-      <c r="L22" s="5" t="s">
-        <v>1075</v>
-      </c>
       <c r="M22" s="5" t="s">
-        <v>1075</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>1074</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>428</v>
       </c>
       <c r="B23" s="5" t="s">
+        <v>845</v>
+      </c>
+      <c r="C23" s="9" t="s">
         <v>846</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="D23" s="6" t="s">
+        <v>1109</v>
+      </c>
+      <c r="E23" s="5" t="s">
         <v>847</v>
       </c>
-      <c r="D23" s="6" t="s">
-        <v>1110</v>
-      </c>
-      <c r="E23" s="5" t="s">
+      <c r="F23" s="5" t="s">
         <v>848</v>
       </c>
-      <c r="F23" s="5" t="s">
+      <c r="G23" s="5" t="s">
         <v>849</v>
       </c>
-      <c r="G23" s="5" t="s">
+      <c r="H23" s="5" t="s">
         <v>850</v>
       </c>
-      <c r="H23" s="5" t="s">
+      <c r="I23" s="9" t="s">
+        <v>846</v>
+      </c>
+      <c r="J23" s="5" t="s">
         <v>851</v>
       </c>
-      <c r="I23" s="9" t="s">
-        <v>847</v>
-      </c>
-      <c r="J23" s="5" t="s">
+      <c r="K23" s="5" t="s">
         <v>852</v>
       </c>
-      <c r="K23" s="5" t="s">
+      <c r="L23" s="5" t="s">
         <v>853</v>
       </c>
-      <c r="L23" s="5" t="s">
-        <v>854</v>
-      </c>
       <c r="M23" s="5" t="s">
-        <v>854</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>438</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="C24" s="9" t="s">
+        <v>856</v>
+      </c>
+      <c r="D24" s="6" t="s">
         <v>857</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="E24" s="5" t="s">
         <v>858</v>
       </c>
-      <c r="E24" s="5" t="s">
+      <c r="F24" s="5" t="s">
         <v>859</v>
       </c>
-      <c r="F24" s="5" t="s">
+      <c r="G24" s="5" t="s">
         <v>860</v>
       </c>
-      <c r="G24" s="5" t="s">
+      <c r="H24" s="5" t="s">
         <v>861</v>
       </c>
-      <c r="H24" s="5" t="s">
+      <c r="I24" s="9" t="s">
+        <v>856</v>
+      </c>
+      <c r="J24" s="5" t="s">
         <v>862</v>
       </c>
-      <c r="I24" s="9" t="s">
-        <v>857</v>
-      </c>
-      <c r="J24" s="5" t="s">
+      <c r="K24" s="5" t="s">
         <v>863</v>
       </c>
-      <c r="K24" s="5" t="s">
+      <c r="L24" s="5" t="s">
         <v>864</v>
       </c>
-      <c r="L24" s="5" t="s">
-        <v>865</v>
-      </c>
       <c r="M24" s="5" t="s">
-        <v>865</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>448</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="C25" s="9" t="s">
+        <v>865</v>
+      </c>
+      <c r="D25" s="6" t="s">
         <v>866</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="E25" s="5" t="s">
         <v>867</v>
       </c>
-      <c r="E25" s="5" t="s">
+      <c r="F25" s="5" t="s">
         <v>868</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="G25" s="5" t="s">
         <v>869</v>
       </c>
-      <c r="G25" s="5" t="s">
+      <c r="H25" s="5" t="s">
         <v>870</v>
       </c>
-      <c r="H25" s="5" t="s">
+      <c r="I25" s="9" t="s">
+        <v>865</v>
+      </c>
+      <c r="J25" s="5" t="s">
         <v>871</v>
       </c>
-      <c r="I25" s="9" t="s">
-        <v>866</v>
-      </c>
-      <c r="J25" s="5" t="s">
+      <c r="K25" s="5" t="s">
         <v>872</v>
       </c>
-      <c r="K25" s="5" t="s">
+      <c r="L25" s="5" t="s">
         <v>873</v>
       </c>
-      <c r="L25" s="5" t="s">
-        <v>874</v>
-      </c>
       <c r="M25" s="5" t="s">
-        <v>874</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>458</v>
       </c>
       <c r="B26" s="5" t="s">
+        <v>981</v>
+      </c>
+      <c r="C26" s="9" t="s">
         <v>982</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="D26" s="6" t="s">
         <v>983</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="E26" s="5" t="s">
         <v>984</v>
       </c>
-      <c r="E26" s="5" t="s">
+      <c r="F26" s="5" t="s">
         <v>985</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="G26" s="5" t="s">
         <v>986</v>
       </c>
-      <c r="G26" s="5" t="s">
+      <c r="H26" s="5" t="s">
         <v>987</v>
       </c>
-      <c r="H26" s="5" t="s">
+      <c r="I26" s="9" t="s">
+        <v>982</v>
+      </c>
+      <c r="J26" s="5" t="s">
         <v>988</v>
       </c>
-      <c r="I26" s="9" t="s">
-        <v>983</v>
-      </c>
-      <c r="J26" s="5" t="s">
+      <c r="K26" s="5" t="s">
         <v>989</v>
       </c>
-      <c r="K26" s="5" t="s">
+      <c r="L26" s="5" t="s">
         <v>990</v>
       </c>
-      <c r="L26" s="5" t="s">
-        <v>991</v>
-      </c>
       <c r="M26" s="5" t="s">
-        <v>991</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>468</v>
       </c>
       <c r="B27" s="5" t="s">
+        <v>991</v>
+      </c>
+      <c r="C27" s="9" t="s">
         <v>992</v>
       </c>
-      <c r="C27" s="9" t="s">
+      <c r="D27" s="6" t="s">
         <v>993</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="E27" s="5" t="s">
         <v>994</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="F27" s="5" t="s">
         <v>995</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="G27" s="5" t="s">
         <v>996</v>
       </c>
-      <c r="G27" s="5" t="s">
+      <c r="H27" s="5" t="s">
         <v>997</v>
       </c>
-      <c r="H27" s="5" t="s">
+      <c r="I27" s="9" t="s">
+        <v>992</v>
+      </c>
+      <c r="J27" s="5" t="s">
         <v>998</v>
       </c>
-      <c r="I27" s="9" t="s">
-        <v>993</v>
-      </c>
-      <c r="J27" s="5" t="s">
+      <c r="K27" s="5" t="s">
         <v>999</v>
       </c>
-      <c r="K27" s="5" t="s">
+      <c r="L27" s="5" t="s">
         <v>1000</v>
       </c>
-      <c r="L27" s="5" t="s">
+      <c r="M27" s="5" t="s">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>592</v>
+      </c>
+      <c r="B28" s="5" t="s">
         <v>1001</v>
       </c>
-      <c r="M27" s="5" t="s">
-        <v>1001</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
-        <v>593</v>
-      </c>
-      <c r="B28" s="5" t="s">
+      <c r="C28" s="9" t="s">
         <v>1002</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="D28" s="6" t="s">
         <v>1003</v>
       </c>
-      <c r="D28" s="6" t="s">
+      <c r="E28" s="5" t="s">
         <v>1004</v>
       </c>
-      <c r="E28" s="5" t="s">
+      <c r="F28" s="5" t="s">
         <v>1005</v>
       </c>
-      <c r="F28" s="5" t="s">
+      <c r="G28" s="5" t="s">
         <v>1006</v>
       </c>
-      <c r="G28" s="5" t="s">
+      <c r="H28" s="5" t="s">
         <v>1007</v>
       </c>
-      <c r="H28" s="5" t="s">
+      <c r="I28" s="9" t="s">
+        <v>1002</v>
+      </c>
+      <c r="J28" s="5" t="s">
         <v>1008</v>
       </c>
-      <c r="I28" s="9" t="s">
-        <v>1003</v>
-      </c>
-      <c r="J28" s="5" t="s">
+      <c r="K28" s="5" t="s">
         <v>1009</v>
       </c>
-      <c r="K28" s="5" t="s">
+      <c r="L28" s="5" t="s">
         <v>1010</v>
       </c>
-      <c r="L28" s="5" t="s">
-        <v>1011</v>
-      </c>
       <c r="M28" s="5" t="s">
-        <v>1011</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="B29" s="5" t="s">
+        <v>1046</v>
+      </c>
+      <c r="C29" s="9" t="s">
         <v>1047</v>
       </c>
-      <c r="C29" s="9" t="s">
+      <c r="D29" s="6" t="s">
         <v>1048</v>
       </c>
-      <c r="D29" s="6" t="s">
+      <c r="E29" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="E29" s="5" t="s">
+      <c r="F29" s="5" t="s">
         <v>1050</v>
       </c>
-      <c r="F29" s="5" t="s">
+      <c r="G29" s="5" t="s">
         <v>1051</v>
       </c>
-      <c r="G29" s="5" t="s">
+      <c r="H29" s="5" t="s">
         <v>1052</v>
       </c>
-      <c r="H29" s="5" t="s">
+      <c r="I29" s="9" t="s">
+        <v>1047</v>
+      </c>
+      <c r="J29" s="5" t="s">
         <v>1053</v>
       </c>
-      <c r="I29" s="9" t="s">
-        <v>1048</v>
-      </c>
-      <c r="J29" s="5" t="s">
+      <c r="K29" s="5" t="s">
         <v>1054</v>
       </c>
-      <c r="K29" s="5" t="s">
+      <c r="L29" s="5" t="s">
         <v>1055</v>
       </c>
-      <c r="L29" s="5" t="s">
+      <c r="M29" s="5" t="s">
+        <v>1055</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>610</v>
+      </c>
+      <c r="B30" s="5" t="s">
         <v>1056</v>
       </c>
-      <c r="M29" s="5" t="s">
-        <v>1056</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
-        <v>611</v>
-      </c>
-      <c r="B30" s="5" t="s">
+      <c r="C30" s="9" t="s">
         <v>1057</v>
       </c>
-      <c r="C30" s="9" t="s">
+      <c r="D30" s="6" t="s">
         <v>1058</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="E30" s="5" t="s">
         <v>1059</v>
       </c>
-      <c r="E30" s="5" t="s">
+      <c r="F30" s="5" t="s">
         <v>1060</v>
       </c>
-      <c r="F30" s="5" t="s">
+      <c r="G30" s="5" t="s">
         <v>1061</v>
       </c>
-      <c r="G30" s="5" t="s">
+      <c r="H30" s="5" t="s">
         <v>1062</v>
       </c>
-      <c r="H30" s="5" t="s">
+      <c r="I30" s="9" t="s">
+        <v>1057</v>
+      </c>
+      <c r="J30" s="5" t="s">
         <v>1063</v>
       </c>
-      <c r="I30" s="9" t="s">
-        <v>1058</v>
-      </c>
-      <c r="J30" s="5" t="s">
+      <c r="K30" s="5" t="s">
         <v>1064</v>
       </c>
-      <c r="K30" s="5" t="s">
+      <c r="L30" s="5" t="s">
         <v>1065</v>
       </c>
-      <c r="L30" s="5" t="s">
-        <v>1066</v>
-      </c>
       <c r="M30" s="5" t="s">
-        <v>1066</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="B31" s="5" t="s">
+        <v>894</v>
+      </c>
+      <c r="C31" s="9" t="s">
         <v>895</v>
       </c>
-      <c r="C31" s="9" t="s">
+      <c r="D31" s="6" t="s">
+        <v>903</v>
+      </c>
+      <c r="E31" s="5" t="s">
         <v>896</v>
       </c>
-      <c r="D31" s="6" t="s">
-        <v>904</v>
-      </c>
-      <c r="E31" s="5" t="s">
+      <c r="F31" s="5" t="s">
         <v>897</v>
       </c>
-      <c r="F31" s="5" t="s">
+      <c r="G31" s="5" t="s">
         <v>898</v>
       </c>
-      <c r="G31" s="5" t="s">
+      <c r="H31" s="5" t="s">
         <v>899</v>
       </c>
-      <c r="H31" s="5" t="s">
+      <c r="I31" s="9" t="s">
+        <v>895</v>
+      </c>
+      <c r="J31" s="5" t="s">
         <v>900</v>
       </c>
-      <c r="I31" s="9" t="s">
-        <v>896</v>
-      </c>
-      <c r="J31" s="5" t="s">
+      <c r="K31" s="5" t="s">
         <v>901</v>
       </c>
-      <c r="K31" s="5" t="s">
+      <c r="L31" s="5" t="s">
         <v>902</v>
       </c>
-      <c r="L31" s="5" t="s">
-        <v>903</v>
-      </c>
       <c r="M31" s="5" t="s">
-        <v>903</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
+        <v>546</v>
+      </c>
+      <c r="B32" s="5" t="s">
         <v>547</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="C32" s="9" t="s">
         <v>548</v>
       </c>
-      <c r="C32" s="9" t="s">
+      <c r="D32" s="6" t="s">
+        <v>800</v>
+      </c>
+      <c r="E32" s="5" t="s">
         <v>549</v>
       </c>
-      <c r="D32" s="6" t="s">
-        <v>801</v>
-      </c>
-      <c r="E32" s="5" t="s">
+      <c r="F32" s="5" t="s">
         <v>550</v>
       </c>
-      <c r="F32" s="5" t="s">
+      <c r="G32" s="5" t="s">
         <v>551</v>
-      </c>
-      <c r="G32" s="5" t="s">
-        <v>552</v>
       </c>
       <c r="H32" s="5"/>
       <c r="I32" s="9" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="J32" s="5" t="s">
+        <v>552</v>
+      </c>
+      <c r="K32" s="5" t="s">
         <v>553</v>
       </c>
-      <c r="K32" s="5" t="s">
+      <c r="L32" s="5" t="s">
         <v>554</v>
       </c>
-      <c r="L32" s="5" t="s">
+      <c r="M32" s="5" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
         <v>555</v>
       </c>
-      <c r="M32" s="5" t="s">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
+      <c r="B33" s="5" t="s">
         <v>556</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="C33" s="9" t="s">
         <v>557</v>
       </c>
-      <c r="C33" s="9" t="s">
+      <c r="D33" s="6" t="s">
+        <v>801</v>
+      </c>
+      <c r="E33" s="5" t="s">
         <v>558</v>
       </c>
-      <c r="D33" s="6" t="s">
-        <v>802</v>
-      </c>
-      <c r="E33" s="5" t="s">
+      <c r="F33" s="5" t="s">
         <v>559</v>
       </c>
-      <c r="F33" s="5" t="s">
+      <c r="G33" s="5" t="s">
         <v>560</v>
-      </c>
-      <c r="G33" s="5" t="s">
-        <v>561</v>
       </c>
       <c r="H33" s="5"/>
       <c r="I33" s="9" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="J33" s="5" t="s">
+        <v>561</v>
+      </c>
+      <c r="K33" s="5" t="s">
         <v>562</v>
       </c>
-      <c r="K33" s="5" t="s">
+      <c r="L33" s="5" t="s">
         <v>563</v>
       </c>
-      <c r="L33" s="5" t="s">
-        <v>564</v>
-      </c>
       <c r="M33" s="5" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{74E20924-6280-4075-B5D0-D312227048CF}"/>
-    <hyperlink ref="I2" r:id="rId2" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{18762434-D983-4BB3-8AD8-05A439AF0886}"/>
-    <hyperlink ref="C26" r:id="rId3" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{47554786-550A-41E9-AF83-B6969AD357DC}"/>
-    <hyperlink ref="I26" r:id="rId4" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{E1BBE2F9-8E32-4E4D-AEFE-43FA02765A58}"/>
-    <hyperlink ref="C27" r:id="rId5" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{993DD2A2-B832-44A7-AA80-CCC5C19C765A}"/>
-    <hyperlink ref="I27" r:id="rId6" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{AD4E0AC8-D9A9-4391-B80D-4FDD236094A9}"/>
-    <hyperlink ref="C30" r:id="rId7" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{889F9053-9FF6-4D5A-B636-90737961BD78}"/>
-    <hyperlink ref="I30" r:id="rId8" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{52F1A0B0-B3EF-4196-9723-AF1D81794325}"/>
-    <hyperlink ref="C28" r:id="rId9" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{9E97B247-4F12-47FB-B824-A9C8EE015367}"/>
-    <hyperlink ref="I28" r:id="rId10" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{1EDA50B5-1DDE-4ABB-9353-B3AF32C0D269}"/>
-    <hyperlink ref="C29" r:id="rId11" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{5BC5C9C8-3CD1-4A40-8170-1D0AC81580C7}"/>
-    <hyperlink ref="I29" r:id="rId12" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{42A3303C-BA7A-49DE-8323-C772CFCF1F43}"/>
-    <hyperlink ref="C11" r:id="rId13" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{96AC723F-D956-4FC1-9FA1-B481C6608FA1}"/>
-    <hyperlink ref="I11" r:id="rId14" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{7CECBDA1-EDB5-4EA3-8CAB-FF77BAF10FF0}"/>
-    <hyperlink ref="C12" r:id="rId15" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{2DF60C4B-F0D0-4E92-BC3C-029858EE6E91}"/>
-    <hyperlink ref="I12" r:id="rId16" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{F3BDE6DD-1CE6-44F7-85A8-71859FDB93DA}"/>
-    <hyperlink ref="C22" r:id="rId17" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{5CE45785-443D-4B93-94C8-46519383162E}"/>
-    <hyperlink ref="I22" r:id="rId18" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{C768F8CA-C09C-46D8-8EFF-8D6D4DFE5A02}"/>
+    <hyperlink ref="C26" r:id="rId1" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{47554786-550A-41E9-AF83-B6969AD357DC}"/>
+    <hyperlink ref="I26" r:id="rId2" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{E1BBE2F9-8E32-4E4D-AEFE-43FA02765A58}"/>
+    <hyperlink ref="C27" r:id="rId3" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{993DD2A2-B832-44A7-AA80-CCC5C19C765A}"/>
+    <hyperlink ref="I27" r:id="rId4" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{AD4E0AC8-D9A9-4391-B80D-4FDD236094A9}"/>
+    <hyperlink ref="C30" r:id="rId5" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{889F9053-9FF6-4D5A-B636-90737961BD78}"/>
+    <hyperlink ref="I30" r:id="rId6" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{52F1A0B0-B3EF-4196-9723-AF1D81794325}"/>
+    <hyperlink ref="C28" r:id="rId7" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{9E97B247-4F12-47FB-B824-A9C8EE015367}"/>
+    <hyperlink ref="I28" r:id="rId8" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{1EDA50B5-1DDE-4ABB-9353-B3AF32C0D269}"/>
+    <hyperlink ref="C29" r:id="rId9" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{5BC5C9C8-3CD1-4A40-8170-1D0AC81580C7}"/>
+    <hyperlink ref="I29" r:id="rId10" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{42A3303C-BA7A-49DE-8323-C772CFCF1F43}"/>
+    <hyperlink ref="C11" r:id="rId11" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{96AC723F-D956-4FC1-9FA1-B481C6608FA1}"/>
+    <hyperlink ref="I11" r:id="rId12" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{7CECBDA1-EDB5-4EA3-8CAB-FF77BAF10FF0}"/>
+    <hyperlink ref="C12" r:id="rId13" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{2DF60C4B-F0D0-4E92-BC3C-029858EE6E91}"/>
+    <hyperlink ref="I12" r:id="rId14" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{F3BDE6DD-1CE6-44F7-85A8-71859FDB93DA}"/>
+    <hyperlink ref="C22" r:id="rId15" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{5CE45785-443D-4B93-94C8-46519383162E}"/>
+    <hyperlink ref="I22" r:id="rId16" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{C768F8CA-C09C-46D8-8EFF-8D6D4DFE5A02}"/>
+    <hyperlink ref="C2" r:id="rId17" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{06F53D74-C7A6-4A0D-8D9C-4D7B09C907DB}"/>
+    <hyperlink ref="I2" r:id="rId18" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{CB2C38DA-1BB9-46E6-B59C-F655A3FBE838}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.3" right="0.3" top="0.61" bottom="0.37" header="0.1" footer="0.1"/>

</xml_diff>

<commit_message>
GDE-7303 data set fixes for TL_CAL_08
Updated the path for InputFilePath and OutputFilePath on TL_Data_Set_AU
Added TL_CAL_08 folder path and files for running
</commit_message>
<xml_diff>
--- a/DataSet/Integration_DataSet/TL/TL_Data_Set_AU.xlsx
+++ b/DataSet/Integration_DataSet/TL/TL_Data_Set_AU.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\Integration_DataSet\TL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{683D4D1F-A3F6-449D-AEEC-F5486E129DE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29B2C55D-4AA6-4AA8-B6F4-5E3A6CAD87F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34800" yWindow="5505" windowWidth="18435" windowHeight="9105" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BaseRate_Fields" sheetId="1" r:id="rId1"/>
@@ -2434,9 +2434,6 @@
     <t>TL_CAL_08</t>
   </si>
   <si>
-    <t>\DataSet\TL_DataSet\Calendar_GSFile\TL_CAL_08_Files\</t>
-  </si>
-  <si>
     <t>INPUTJSON_TL_CAL08</t>
   </si>
   <si>
@@ -2450,9 +2447,6 @@
   </si>
   <si>
     <t>Actual_wsFinalLIQDestination_TL_CAL08</t>
-  </si>
-  <si>
-    <t>Holidays_Banks_20180108_1.xlsx,Holidays_Banks_20180108_2.xlsx,Holidays_Banks_20180108_1.csv,Holidays_Banks_20180108_2.csv,Holidays_Misc_20180108.xlsx</t>
   </si>
   <si>
     <t>TL_CAL_09</t>
@@ -3440,6 +3434,12 @@
   </si>
   <si>
     <t>Holidays_Banks_20200123_1.xlsx,Holidays_Banks_20200123_2.xlsx,Holidays_Banks_20200123_1.csv,Holidays_Banks_20200123_2.csv,Holidays_Misc_20200123.xlsx</t>
+  </si>
+  <si>
+    <t>\DataSet\Integration_DataSet\TL\Calendar_GSFile\TL_CAL_08_Files\</t>
+  </si>
+  <si>
+    <t>Holidays_Banks_20200127_1.xlsx,Holidays_Banks_20200127_2.xlsx,Holidays_Banks_20200127_1.csv,Holidays_Banks_20200127_2.csv,Holidays_Misc_20200127.xlsx</t>
   </si>
 </sst>
 </file>
@@ -4396,25 +4396,25 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="65.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="53.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="21.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="41.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="65.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="33.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="38.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="44.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="41.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="65.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="53.44140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="21.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="41.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="65.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="33.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="38.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="44.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="41.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="34.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4422,7 +4422,7 @@
         <v>17</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>1113</v>
+        <v>1111</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>1</v>
@@ -4458,7 +4458,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -4466,10 +4466,10 @@
         <v>11</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>1114</v>
+        <v>1112</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>1115</v>
+        <v>1113</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>94</v>
@@ -4484,7 +4484,7 @@
         <v>18</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>1115</v>
+        <v>1113</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>21</v>
@@ -4499,7 +4499,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>22</v>
       </c>
@@ -4538,7 +4538,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>36</v>
       </c>
@@ -4577,7 +4577,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>43</v>
       </c>
@@ -4616,7 +4616,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>49</v>
       </c>
@@ -4655,7 +4655,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>57</v>
       </c>
@@ -4664,10 +4664,10 @@
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="9" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>59</v>
@@ -4679,7 +4679,7 @@
         <v>61</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="J7" s="5" t="s">
         <v>62</v>
@@ -4694,7 +4694,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>64</v>
       </c>
@@ -4703,10 +4703,10 @@
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="9" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>66</v>
@@ -4718,7 +4718,7 @@
         <v>68</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="J8" s="5" t="s">
         <v>69</v>
@@ -4733,7 +4733,7 @@
         <v>713</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>96</v>
       </c>
@@ -4742,10 +4742,10 @@
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="9" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>98</v>
@@ -4757,7 +4757,7 @@
         <v>100</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="J9" s="5" t="s">
         <v>101</v>
@@ -4772,7 +4772,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>103</v>
       </c>
@@ -4781,7 +4781,7 @@
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="9" t="s">
-        <v>1015</v>
+        <v>1013</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>105</v>
@@ -4796,7 +4796,7 @@
         <v>108</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>1015</v>
+        <v>1013</v>
       </c>
       <c r="J10" s="5" t="s">
         <v>109</v>
@@ -4811,7 +4811,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>111</v>
       </c>
@@ -4850,7 +4850,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>113</v>
       </c>
@@ -4889,7 +4889,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>115</v>
       </c>
@@ -4928,7 +4928,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>117</v>
       </c>
@@ -4967,7 +4967,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>119</v>
       </c>
@@ -5006,7 +5006,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>146</v>
       </c>
@@ -5045,124 +5045,124 @@
         <v>185</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>333</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="9" t="s">
+        <v>919</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>920</v>
+      </c>
+      <c r="F17" s="5" t="s">
         <v>921</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="G17" s="5" t="s">
         <v>922</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="H17" s="5" t="s">
         <v>923</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="I17" s="9" t="s">
+        <v>919</v>
+      </c>
+      <c r="J17" s="5" t="s">
         <v>924</v>
       </c>
-      <c r="H17" s="5" t="s">
+      <c r="K17" s="5" t="s">
         <v>925</v>
       </c>
-      <c r="I17" s="9" t="s">
-        <v>921</v>
-      </c>
-      <c r="J17" s="5" t="s">
+      <c r="L17" s="5" t="s">
         <v>926</v>
       </c>
-      <c r="K17" s="5" t="s">
+      <c r="M17" s="5" t="s">
         <v>927</v>
       </c>
-      <c r="L17" s="5" t="s">
-        <v>928</v>
-      </c>
-      <c r="M17" s="5" t="s">
-        <v>929</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>343</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="9" t="s">
+        <v>1074</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>1075</v>
+      </c>
+      <c r="F18" s="5" t="s">
         <v>1076</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="G18" s="5" t="s">
         <v>1077</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="H18" s="5" t="s">
         <v>1078</v>
       </c>
-      <c r="G18" s="5" t="s">
+      <c r="I18" s="9" t="s">
+        <v>1074</v>
+      </c>
+      <c r="J18" s="5" t="s">
         <v>1079</v>
       </c>
-      <c r="H18" s="5" t="s">
+      <c r="K18" s="5" t="s">
         <v>1080</v>
       </c>
-      <c r="I18" s="9" t="s">
-        <v>1076</v>
-      </c>
-      <c r="J18" s="5" t="s">
+      <c r="L18" s="5" t="s">
         <v>1081</v>
       </c>
-      <c r="K18" s="5" t="s">
+      <c r="M18" s="5" t="s">
         <v>1082</v>
       </c>
-      <c r="L18" s="5" t="s">
-        <v>1083</v>
-      </c>
-      <c r="M18" s="5" t="s">
-        <v>1084</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>353</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>1016</v>
+        <v>1014</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="9" t="s">
+        <v>1015</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>1016</v>
+      </c>
+      <c r="F19" s="5" t="s">
         <v>1017</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="G19" s="5" t="s">
         <v>1018</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="H19" s="5" t="s">
         <v>1019</v>
       </c>
-      <c r="G19" s="5" t="s">
+      <c r="I19" s="9" t="s">
+        <v>1015</v>
+      </c>
+      <c r="J19" s="5" t="s">
         <v>1020</v>
       </c>
-      <c r="H19" s="5" t="s">
+      <c r="K19" s="5" t="s">
         <v>1021</v>
       </c>
-      <c r="I19" s="9" t="s">
-        <v>1017</v>
-      </c>
-      <c r="J19" s="5" t="s">
+      <c r="L19" s="5" t="s">
         <v>1022</v>
       </c>
-      <c r="K19" s="5" t="s">
+      <c r="M19" s="5" t="s">
         <v>1023</v>
       </c>
-      <c r="L19" s="5" t="s">
-        <v>1024</v>
-      </c>
-      <c r="M19" s="5" t="s">
-        <v>1025</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>169</v>
       </c>
@@ -5201,7 +5201,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>210</v>
       </c>
@@ -5240,7 +5240,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>230</v>
       </c>
@@ -5279,7 +5279,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>232</v>
       </c>
@@ -5318,7 +5318,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
         <v>428</v>
       </c>
@@ -5357,7 +5357,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
         <v>438</v>
       </c>
@@ -5396,7 +5396,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
         <v>448</v>
       </c>
@@ -5435,46 +5435,46 @@
         <v>708</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>458</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>1085</v>
+        <v>1083</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="9" t="s">
+        <v>1084</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>1085</v>
+      </c>
+      <c r="F27" s="5" t="s">
         <v>1086</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="G27" s="5" t="s">
         <v>1087</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="H27" s="5" t="s">
         <v>1088</v>
       </c>
-      <c r="G27" s="5" t="s">
+      <c r="I27" s="9" t="s">
+        <v>1084</v>
+      </c>
+      <c r="J27" s="5" t="s">
         <v>1089</v>
       </c>
-      <c r="H27" s="5" t="s">
+      <c r="K27" s="5" t="s">
         <v>1090</v>
       </c>
-      <c r="I27" s="9" t="s">
-        <v>1086</v>
-      </c>
-      <c r="J27" s="5" t="s">
+      <c r="L27" s="5" t="s">
         <v>1091</v>
       </c>
-      <c r="K27" s="5" t="s">
+      <c r="M27" s="5" t="s">
         <v>1092</v>
       </c>
-      <c r="L27" s="5" t="s">
-        <v>1093</v>
-      </c>
-      <c r="M27" s="5" t="s">
-        <v>1094</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="11" t="s">
         <v>468</v>
       </c>
@@ -5513,7 +5513,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="11" t="s">
         <v>592</v>
       </c>
@@ -5552,7 +5552,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
         <v>610</v>
       </c>
@@ -5591,7 +5591,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="11" t="s">
         <v>731</v>
       </c>
@@ -5630,241 +5630,241 @@
         <v>724</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
         <v>619</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="9" t="s">
+        <v>929</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>930</v>
+      </c>
+      <c r="F32" s="5" t="s">
         <v>931</v>
       </c>
-      <c r="E32" s="6" t="s">
+      <c r="G32" s="5" t="s">
         <v>932</v>
       </c>
-      <c r="F32" s="5" t="s">
+      <c r="H32" s="5" t="s">
         <v>933</v>
       </c>
-      <c r="G32" s="5" t="s">
+      <c r="I32" s="9" t="s">
+        <v>929</v>
+      </c>
+      <c r="J32" s="5" t="s">
         <v>934</v>
       </c>
-      <c r="H32" s="5" t="s">
+      <c r="K32" s="5" t="s">
         <v>935</v>
       </c>
-      <c r="I32" s="9" t="s">
-        <v>931</v>
-      </c>
-      <c r="J32" s="5" t="s">
+      <c r="L32" s="5" t="s">
         <v>936</v>
       </c>
-      <c r="K32" s="5" t="s">
+      <c r="M32" s="5" t="s">
         <v>937</v>
       </c>
-      <c r="L32" s="5" t="s">
-        <v>938</v>
-      </c>
-      <c r="M32" s="5" t="s">
-        <v>939</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" s="11" t="s">
         <v>628</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>940</v>
+        <v>938</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="9" t="s">
+        <v>939</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>940</v>
+      </c>
+      <c r="F33" s="5" t="s">
         <v>941</v>
       </c>
-      <c r="E33" s="6" t="s">
+      <c r="G33" s="5" t="s">
         <v>942</v>
       </c>
-      <c r="F33" s="5" t="s">
+      <c r="H33" s="5" t="s">
         <v>943</v>
       </c>
-      <c r="G33" s="5" t="s">
+      <c r="I33" s="9" t="s">
+        <v>939</v>
+      </c>
+      <c r="J33" s="5" t="s">
         <v>944</v>
       </c>
-      <c r="H33" s="5" t="s">
+      <c r="K33" s="5" t="s">
         <v>945</v>
       </c>
-      <c r="I33" s="9" t="s">
-        <v>941</v>
-      </c>
-      <c r="J33" s="5" t="s">
+      <c r="L33" s="5" t="s">
         <v>946</v>
       </c>
-      <c r="K33" s="5" t="s">
+      <c r="M33" s="5" t="s">
         <v>947</v>
       </c>
-      <c r="L33" s="5" t="s">
-        <v>948</v>
-      </c>
-      <c r="M33" s="5" t="s">
-        <v>949</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" s="11" t="s">
         <v>546</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>950</v>
+        <v>948</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="9" t="s">
+        <v>949</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>950</v>
+      </c>
+      <c r="F34" s="5" t="s">
         <v>951</v>
       </c>
-      <c r="E34" s="6" t="s">
+      <c r="G34" s="5" t="s">
         <v>952</v>
       </c>
-      <c r="F34" s="5" t="s">
+      <c r="H34" s="5" t="s">
         <v>953</v>
       </c>
-      <c r="G34" s="5" t="s">
+      <c r="I34" s="9" t="s">
+        <v>949</v>
+      </c>
+      <c r="J34" s="5" t="s">
         <v>954</v>
       </c>
-      <c r="H34" s="5" t="s">
+      <c r="K34" s="5" t="s">
         <v>955</v>
       </c>
-      <c r="I34" s="9" t="s">
-        <v>951</v>
-      </c>
-      <c r="J34" s="5" t="s">
+      <c r="L34" s="5" t="s">
         <v>956</v>
       </c>
-      <c r="K34" s="5" t="s">
+      <c r="M34" s="5" t="s">
         <v>957</v>
       </c>
-      <c r="L34" s="5" t="s">
-        <v>958</v>
-      </c>
-      <c r="M34" s="5" t="s">
-        <v>959</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" s="11" t="s">
         <v>555</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
       <c r="C35" s="5"/>
       <c r="D35" s="9" t="s">
+        <v>959</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>960</v>
+      </c>
+      <c r="F35" s="5" t="s">
         <v>961</v>
       </c>
-      <c r="E35" s="6" t="s">
+      <c r="G35" s="5" t="s">
         <v>962</v>
       </c>
-      <c r="F35" s="5" t="s">
+      <c r="H35" s="5" t="s">
         <v>963</v>
       </c>
-      <c r="G35" s="5" t="s">
+      <c r="I35" s="9" t="s">
+        <v>959</v>
+      </c>
+      <c r="J35" s="5" t="s">
         <v>964</v>
       </c>
-      <c r="H35" s="5" t="s">
+      <c r="K35" s="5" t="s">
         <v>965</v>
       </c>
-      <c r="I35" s="9" t="s">
-        <v>961</v>
-      </c>
-      <c r="J35" s="5" t="s">
+      <c r="L35" s="5" t="s">
         <v>966</v>
       </c>
-      <c r="K35" s="5" t="s">
+      <c r="M35" s="5" t="s">
         <v>967</v>
       </c>
-      <c r="L35" s="5" t="s">
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A36" s="11" t="s">
         <v>968</v>
       </c>
-      <c r="M35" s="5" t="s">
+      <c r="B36" s="5" t="s">
         <v>969</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36" s="11" t="s">
-        <v>970</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>971</v>
       </c>
       <c r="C36" s="5"/>
       <c r="D36" s="9" t="s">
+        <v>970</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>971</v>
+      </c>
+      <c r="F36" s="5" t="s">
         <v>972</v>
       </c>
-      <c r="E36" s="6" t="s">
+      <c r="G36" s="5" t="s">
         <v>973</v>
       </c>
-      <c r="F36" s="5" t="s">
+      <c r="H36" s="5" t="s">
         <v>974</v>
       </c>
-      <c r="G36" s="5" t="s">
+      <c r="I36" s="9" t="s">
+        <v>970</v>
+      </c>
+      <c r="J36" s="5" t="s">
         <v>975</v>
       </c>
-      <c r="H36" s="5" t="s">
+      <c r="K36" s="5" t="s">
         <v>976</v>
       </c>
-      <c r="I36" s="9" t="s">
-        <v>972</v>
-      </c>
-      <c r="J36" s="5" t="s">
+      <c r="L36" s="5" t="s">
         <v>977</v>
       </c>
-      <c r="K36" s="5" t="s">
+      <c r="M36" s="5" t="s">
         <v>978</v>
       </c>
-      <c r="L36" s="5" t="s">
-        <v>979</v>
-      </c>
-      <c r="M36" s="5" t="s">
-        <v>980</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
-        <v>1095</v>
+        <v>1093</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>1096</v>
+        <v>1094</v>
       </c>
       <c r="C37" s="5"/>
       <c r="D37" s="9" t="s">
+        <v>1095</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>1096</v>
+      </c>
+      <c r="F37" s="5" t="s">
         <v>1097</v>
       </c>
-      <c r="E37" s="5" t="s">
+      <c r="G37" s="5" t="s">
         <v>1098</v>
       </c>
-      <c r="F37" s="5" t="s">
+      <c r="H37" s="5" t="s">
         <v>1099</v>
       </c>
-      <c r="G37" s="5" t="s">
+      <c r="I37" s="9" t="s">
+        <v>1095</v>
+      </c>
+      <c r="J37" s="5" t="s">
         <v>1100</v>
       </c>
-      <c r="H37" s="5" t="s">
+      <c r="K37" s="5" t="s">
         <v>1101</v>
       </c>
-      <c r="I37" s="9" t="s">
-        <v>1097</v>
-      </c>
-      <c r="J37" s="5" t="s">
+      <c r="L37" s="5" t="s">
         <v>1102</v>
       </c>
-      <c r="K37" s="5" t="s">
+      <c r="M37" s="5" t="s">
         <v>1103</v>
       </c>
-      <c r="L37" s="5" t="s">
-        <v>1104</v>
-      </c>
-      <c r="M37" s="5" t="s">
-        <v>1105</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A38" s="11" t="s">
         <v>735</v>
       </c>
@@ -5903,7 +5903,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A39" s="11" t="s">
         <v>768</v>
       </c>
@@ -5945,7 +5945,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A40" s="11" t="s">
         <v>781</v>
       </c>
@@ -5985,7 +5985,7 @@
       </c>
       <c r="N40" s="5"/>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A41" s="11" t="s">
         <v>746</v>
       </c>
@@ -6024,7 +6024,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A42" s="11" t="s">
         <v>757</v>
       </c>
@@ -6144,26 +6144,26 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="66.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="44.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="43.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="61.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="45.85546875" customWidth="1"/>
-    <col min="11" max="11" width="40.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="40.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="66.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="43.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="61.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="45.88671875" customWidth="1"/>
+    <col min="11" max="11" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="40.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -6171,7 +6171,7 @@
         <v>17</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>1113</v>
+        <v>1111</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>1</v>
@@ -6210,10 +6210,10 @@
         <v>121</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>1106</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+        <v>1104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -6221,10 +6221,10 @@
         <v>44</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>1116</v>
+        <v>1114</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>1117</v>
+        <v>1115</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>132</v>
@@ -6239,7 +6239,7 @@
         <v>48</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>1117</v>
+        <v>1115</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>129</v>
@@ -6260,7 +6260,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>22</v>
       </c>
@@ -6305,7 +6305,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>36</v>
       </c>
@@ -6350,7 +6350,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>43</v>
       </c>
@@ -6395,7 +6395,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>49</v>
       </c>
@@ -6440,7 +6440,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>57</v>
       </c>
@@ -6485,7 +6485,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>64</v>
       </c>
@@ -6497,7 +6497,7 @@
         <v>130</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>1011</v>
+        <v>1009</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>260</v>
@@ -6530,7 +6530,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>96</v>
       </c>
@@ -6542,7 +6542,7 @@
         <v>130</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>268</v>
@@ -6575,7 +6575,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>103</v>
       </c>
@@ -6587,7 +6587,7 @@
         <v>130</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>1013</v>
+        <v>1011</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>276</v>
@@ -6620,7 +6620,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>111</v>
       </c>
@@ -6632,7 +6632,7 @@
         <v>130</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>1014</v>
+        <v>1012</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>284</v>
@@ -6665,7 +6665,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>113</v>
       </c>
@@ -6677,7 +6677,7 @@
         <v>130</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>1110</v>
+        <v>1108</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>292</v>
@@ -6710,7 +6710,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>115</v>
       </c>
@@ -6722,7 +6722,7 @@
         <v>130</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>1111</v>
+        <v>1109</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>300</v>
@@ -6755,7 +6755,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>117</v>
       </c>
@@ -6767,7 +6767,7 @@
         <v>130</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>1112</v>
+        <v>1110</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>308</v>
@@ -6800,7 +6800,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>119</v>
       </c>
@@ -6845,7 +6845,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
         <v>146</v>
       </c>
@@ -6890,7 +6890,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>333</v>
       </c>
@@ -6935,7 +6935,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>343</v>
       </c>
@@ -6980,7 +6980,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>353</v>
       </c>
@@ -7025,7 +7025,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>169</v>
       </c>
@@ -7070,10 +7070,10 @@
         <v>243</v>
       </c>
       <c r="P20" s="5" t="s">
-        <v>1107</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+        <v>1105</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>210</v>
       </c>
@@ -7118,7 +7118,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
         <v>230</v>
       </c>
@@ -7163,7 +7163,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
         <v>232</v>
       </c>
@@ -7208,7 +7208,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
         <v>399</v>
       </c>
@@ -7253,7 +7253,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
         <v>409</v>
       </c>
@@ -7298,7 +7298,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="26" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
         <v>419</v>
       </c>
@@ -7343,7 +7343,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="27" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
         <v>428</v>
       </c>
@@ -7388,7 +7388,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
         <v>438</v>
       </c>
@@ -7433,7 +7433,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
         <v>448</v>
       </c>
@@ -7478,7 +7478,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
         <v>458</v>
       </c>
@@ -7523,7 +7523,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="31" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
         <v>468</v>
       </c>
@@ -7568,7 +7568,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="32" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
         <v>592</v>
       </c>
@@ -7613,7 +7613,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
         <v>601</v>
       </c>
@@ -7658,7 +7658,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
         <v>610</v>
       </c>
@@ -7703,7 +7703,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
         <v>619</v>
       </c>
@@ -7748,7 +7748,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
         <v>628</v>
       </c>
@@ -7821,27 +7821,27 @@
   <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="67.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="67.88671875" style="1" customWidth="1"/>
     <col min="4" max="4" width="94" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="42.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="36.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="75.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="37.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="42.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="36.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="75.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="37.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="40" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="60.28515625" customWidth="1"/>
+    <col min="12" max="12" width="60.33203125" customWidth="1"/>
     <col min="13" max="13" width="45" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -7882,7 +7882,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -7890,10 +7890,10 @@
         <v>140</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>1118</v>
+        <v>1116</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>1119</v>
+        <v>1117</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>143</v>
@@ -7905,7 +7905,7 @@
         <v>145</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>1118</v>
+        <v>1116</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>166</v>
@@ -7920,7 +7920,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>22</v>
       </c>
@@ -7931,7 +7931,7 @@
         <v>481</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>482</v>
@@ -7943,7 +7943,7 @@
         <v>484</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="I3" s="9" t="s">
         <v>481</v>
@@ -7961,130 +7961,130 @@
         <v>487</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>36</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>872</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>873</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>881</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>874</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="F4" s="5" t="s">
         <v>875</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>883</v>
-      </c>
-      <c r="E4" s="5" t="s">
+      <c r="G4" s="5" t="s">
         <v>876</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="H4" s="5" t="s">
         <v>877</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="I4" s="9" t="s">
+        <v>873</v>
+      </c>
+      <c r="J4" s="5" t="s">
         <v>878</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="K4" s="5" t="s">
         <v>879</v>
       </c>
-      <c r="I4" s="9" t="s">
-        <v>875</v>
-      </c>
-      <c r="J4" s="5" t="s">
+      <c r="L4" s="5" t="s">
         <v>880</v>
       </c>
-      <c r="K4" s="5" t="s">
-        <v>881</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>882</v>
-      </c>
       <c r="M4" s="5" t="s">
-        <v>882</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>43</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>882</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>883</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>891</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>884</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="F5" s="5" t="s">
         <v>885</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>893</v>
-      </c>
-      <c r="E5" s="5" t="s">
+      <c r="G5" s="5" t="s">
         <v>886</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="H5" s="5" t="s">
         <v>887</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="I5" s="9" t="s">
+        <v>883</v>
+      </c>
+      <c r="J5" s="5" t="s">
         <v>888</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="K5" s="5" t="s">
         <v>889</v>
       </c>
-      <c r="I5" s="9" t="s">
-        <v>885</v>
-      </c>
-      <c r="J5" s="5" t="s">
+      <c r="L5" s="5" t="s">
         <v>890</v>
       </c>
-      <c r="K5" s="5" t="s">
-        <v>891</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>892</v>
-      </c>
       <c r="M5" s="5" t="s">
-        <v>892</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>64</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>819</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>820</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>821</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="E6" s="5" t="s">
         <v>822</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="F6" s="5" t="s">
         <v>823</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="G6" s="5" t="s">
         <v>824</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="H6" s="5" t="s">
         <v>825</v>
       </c>
-      <c r="G6" s="5" t="s">
-        <v>826</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>827</v>
-      </c>
       <c r="I6" s="9" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="J6" s="5" t="s">
+        <v>828</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>829</v>
+      </c>
+      <c r="L6" s="5" t="s">
         <v>830</v>
       </c>
-      <c r="K6" s="5" t="s">
-        <v>831</v>
-      </c>
-      <c r="L6" s="5" t="s">
-        <v>832</v>
-      </c>
       <c r="M6" s="5" t="s">
-        <v>832</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>96</v>
       </c>
@@ -8092,122 +8092,122 @@
         <v>802</v>
       </c>
       <c r="C7" s="9" t="s">
+        <v>1118</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>1119</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>803</v>
       </c>
-      <c r="D7" s="6" t="s">
-        <v>809</v>
-      </c>
-      <c r="E7" s="5" t="s">
+      <c r="F7" s="5" t="s">
         <v>804</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="G7" s="5" t="s">
         <v>805</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="H7" s="5" t="s">
+        <v>826</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>1118</v>
+      </c>
+      <c r="J7" s="5" t="s">
         <v>806</v>
       </c>
-      <c r="H7" s="5" t="s">
-        <v>828</v>
-      </c>
-      <c r="I7" s="9" t="s">
-        <v>803</v>
-      </c>
-      <c r="J7" s="5" t="s">
+      <c r="K7" s="5" t="s">
         <v>807</v>
-      </c>
-      <c r="K7" s="5" t="s">
-        <v>808</v>
       </c>
       <c r="L7" s="5" t="s">
         <v>487</v>
       </c>
       <c r="M7" s="5" t="s">
-        <v>818</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>103</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>808</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>809</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>817</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>810</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="F8" s="5" t="s">
         <v>811</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>819</v>
-      </c>
-      <c r="E8" s="5" t="s">
+      <c r="G8" s="5" t="s">
         <v>812</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="H8" s="5" t="s">
+        <v>827</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>809</v>
+      </c>
+      <c r="J8" s="5" t="s">
         <v>813</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="K8" s="5" t="s">
         <v>814</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>829</v>
-      </c>
-      <c r="I8" s="9" t="s">
-        <v>811</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>815</v>
-      </c>
-      <c r="K8" s="5" t="s">
-        <v>816</v>
       </c>
       <c r="L8" s="5" t="s">
         <v>487</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>817</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>111</v>
       </c>
       <c r="B9" s="5" t="s">
+        <v>832</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>833</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>834</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="E9" s="5" t="s">
         <v>835</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="F9" s="5" t="s">
         <v>836</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="G9" s="5" t="s">
         <v>837</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="H9" s="5" t="s">
         <v>838</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="I9" s="9" t="s">
+        <v>833</v>
+      </c>
+      <c r="J9" s="5" t="s">
         <v>839</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="K9" s="5" t="s">
         <v>840</v>
       </c>
-      <c r="I9" s="9" t="s">
-        <v>835</v>
-      </c>
-      <c r="J9" s="5" t="s">
+      <c r="L9" s="5" t="s">
         <v>841</v>
       </c>
-      <c r="K9" s="5" t="s">
-        <v>842</v>
-      </c>
-      <c r="L9" s="5" t="s">
-        <v>843</v>
-      </c>
       <c r="M9" s="5" t="s">
-        <v>843</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>113</v>
       </c>
@@ -8230,7 +8230,7 @@
         <v>492</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="I10" s="9" t="s">
         <v>489</v>
@@ -8248,130 +8248,130 @@
         <v>495</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>115</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>1024</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>1025</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>1026</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="E11" s="5" t="s">
         <v>1027</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="F11" s="5" t="s">
         <v>1028</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="G11" s="5" t="s">
         <v>1029</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="H11" s="5" t="s">
         <v>1030</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="I11" s="9" t="s">
+        <v>1025</v>
+      </c>
+      <c r="J11" s="5" t="s">
         <v>1031</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="K11" s="5" t="s">
         <v>1032</v>
       </c>
-      <c r="I11" s="9" t="s">
-        <v>1027</v>
-      </c>
-      <c r="J11" s="5" t="s">
+      <c r="L11" s="5" t="s">
         <v>1033</v>
       </c>
-      <c r="K11" s="5" t="s">
-        <v>1034</v>
-      </c>
-      <c r="L11" s="5" t="s">
-        <v>1035</v>
-      </c>
       <c r="M11" s="5" t="s">
-        <v>1035</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>1033</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>117</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>1034</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>1035</v>
+      </c>
+      <c r="D12" s="6" t="s">
         <v>1036</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="E12" s="5" t="s">
         <v>1037</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="F12" s="5" t="s">
         <v>1038</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="G12" s="5" t="s">
         <v>1039</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="H12" s="5" t="s">
         <v>1040</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="I12" s="9" t="s">
+        <v>1035</v>
+      </c>
+      <c r="J12" s="5" t="s">
         <v>1041</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="K12" s="5" t="s">
         <v>1042</v>
       </c>
-      <c r="I12" s="9" t="s">
-        <v>1037</v>
-      </c>
-      <c r="J12" s="5" t="s">
+      <c r="L12" s="5" t="s">
         <v>1043</v>
       </c>
-      <c r="K12" s="5" t="s">
-        <v>1044</v>
-      </c>
-      <c r="L12" s="5" t="s">
-        <v>1045</v>
-      </c>
       <c r="M12" s="5" t="s">
-        <v>1045</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>1043</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>119</v>
       </c>
       <c r="B13" s="5" t="s">
+        <v>902</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>903</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>904</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="E13" s="5" t="s">
         <v>905</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="F13" s="5" t="s">
         <v>906</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="G13" s="5" t="s">
         <v>907</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="H13" s="5" t="s">
         <v>908</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="I13" s="9" t="s">
+        <v>903</v>
+      </c>
+      <c r="J13" s="5" t="s">
         <v>909</v>
       </c>
-      <c r="H13" s="5" t="s">
+      <c r="K13" s="5" t="s">
         <v>910</v>
       </c>
-      <c r="I13" s="9" t="s">
-        <v>905</v>
-      </c>
-      <c r="J13" s="5" t="s">
+      <c r="L13" s="5" t="s">
         <v>911</v>
       </c>
-      <c r="K13" s="5" t="s">
-        <v>912</v>
-      </c>
-      <c r="L13" s="5" t="s">
-        <v>913</v>
-      </c>
       <c r="M13" s="5" t="s">
-        <v>913</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>146</v>
       </c>
@@ -8410,7 +8410,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>504</v>
       </c>
@@ -8449,7 +8449,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>513</v>
       </c>
@@ -8488,7 +8488,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>17</v>
       </c>
@@ -8529,7 +8529,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <v>18</v>
       </c>
@@ -8568,7 +8568,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
         <v>19</v>
       </c>
@@ -8607,7 +8607,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>210</v>
       </c>
@@ -8646,7 +8646,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>230</v>
       </c>
@@ -8685,417 +8685,417 @@
         <v>591</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>419</v>
       </c>
       <c r="B22" s="5" t="s">
+        <v>1064</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>1065</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>1106</v>
+      </c>
+      <c r="E22" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="F22" s="5" t="s">
         <v>1067</v>
       </c>
-      <c r="D22" s="6" t="s">
-        <v>1108</v>
-      </c>
-      <c r="E22" s="5" t="s">
+      <c r="G22" s="5" t="s">
         <v>1068</v>
       </c>
-      <c r="F22" s="5" t="s">
+      <c r="H22" s="5" t="s">
         <v>1069</v>
       </c>
-      <c r="G22" s="5" t="s">
+      <c r="I22" s="9" t="s">
+        <v>1065</v>
+      </c>
+      <c r="J22" s="5" t="s">
         <v>1070</v>
       </c>
-      <c r="H22" s="5" t="s">
+      <c r="K22" s="5" t="s">
         <v>1071</v>
       </c>
-      <c r="I22" s="9" t="s">
-        <v>1067</v>
-      </c>
-      <c r="J22" s="5" t="s">
+      <c r="L22" s="5" t="s">
         <v>1072</v>
       </c>
-      <c r="K22" s="5" t="s">
-        <v>1073</v>
-      </c>
-      <c r="L22" s="5" t="s">
-        <v>1074</v>
-      </c>
       <c r="M22" s="5" t="s">
-        <v>1074</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>428</v>
       </c>
       <c r="B23" s="5" t="s">
+        <v>843</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>844</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>1107</v>
+      </c>
+      <c r="E23" s="5" t="s">
         <v>845</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="F23" s="5" t="s">
         <v>846</v>
       </c>
-      <c r="D23" s="6" t="s">
-        <v>1109</v>
-      </c>
-      <c r="E23" s="5" t="s">
+      <c r="G23" s="5" t="s">
         <v>847</v>
       </c>
-      <c r="F23" s="5" t="s">
+      <c r="H23" s="5" t="s">
         <v>848</v>
       </c>
-      <c r="G23" s="5" t="s">
+      <c r="I23" s="9" t="s">
+        <v>844</v>
+      </c>
+      <c r="J23" s="5" t="s">
         <v>849</v>
       </c>
-      <c r="H23" s="5" t="s">
+      <c r="K23" s="5" t="s">
         <v>850</v>
       </c>
-      <c r="I23" s="9" t="s">
-        <v>846</v>
-      </c>
-      <c r="J23" s="5" t="s">
+      <c r="L23" s="5" t="s">
         <v>851</v>
       </c>
-      <c r="K23" s="5" t="s">
-        <v>852</v>
-      </c>
-      <c r="L23" s="5" t="s">
-        <v>853</v>
-      </c>
       <c r="M23" s="5" t="s">
-        <v>853</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>438</v>
       </c>
       <c r="B24" s="5" t="s">
+        <v>852</v>
+      </c>
+      <c r="C24" s="9" t="s">
         <v>854</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="D24" s="6" t="s">
+        <v>855</v>
+      </c>
+      <c r="E24" s="5" t="s">
         <v>856</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="F24" s="5" t="s">
         <v>857</v>
       </c>
-      <c r="E24" s="5" t="s">
+      <c r="G24" s="5" t="s">
         <v>858</v>
       </c>
-      <c r="F24" s="5" t="s">
+      <c r="H24" s="5" t="s">
         <v>859</v>
       </c>
-      <c r="G24" s="5" t="s">
+      <c r="I24" s="9" t="s">
+        <v>854</v>
+      </c>
+      <c r="J24" s="5" t="s">
         <v>860</v>
       </c>
-      <c r="H24" s="5" t="s">
+      <c r="K24" s="5" t="s">
         <v>861</v>
       </c>
-      <c r="I24" s="9" t="s">
-        <v>856</v>
-      </c>
-      <c r="J24" s="5" t="s">
+      <c r="L24" s="5" t="s">
         <v>862</v>
       </c>
-      <c r="K24" s="5" t="s">
-        <v>863</v>
-      </c>
-      <c r="L24" s="5" t="s">
-        <v>864</v>
-      </c>
       <c r="M24" s="5" t="s">
-        <v>864</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>448</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
       <c r="C25" s="9" t="s">
+        <v>863</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>864</v>
+      </c>
+      <c r="E25" s="5" t="s">
         <v>865</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="F25" s="5" t="s">
         <v>866</v>
       </c>
-      <c r="E25" s="5" t="s">
+      <c r="G25" s="5" t="s">
         <v>867</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="H25" s="5" t="s">
         <v>868</v>
       </c>
-      <c r="G25" s="5" t="s">
+      <c r="I25" s="9" t="s">
+        <v>863</v>
+      </c>
+      <c r="J25" s="5" t="s">
         <v>869</v>
       </c>
-      <c r="H25" s="5" t="s">
+      <c r="K25" s="5" t="s">
         <v>870</v>
       </c>
-      <c r="I25" s="9" t="s">
-        <v>865</v>
-      </c>
-      <c r="J25" s="5" t="s">
+      <c r="L25" s="5" t="s">
         <v>871</v>
       </c>
-      <c r="K25" s="5" t="s">
-        <v>872</v>
-      </c>
-      <c r="L25" s="5" t="s">
-        <v>873</v>
-      </c>
       <c r="M25" s="5" t="s">
-        <v>873</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>458</v>
       </c>
       <c r="B26" s="5" t="s">
+        <v>979</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>980</v>
+      </c>
+      <c r="D26" s="6" t="s">
         <v>981</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="E26" s="5" t="s">
         <v>982</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="F26" s="5" t="s">
         <v>983</v>
       </c>
-      <c r="E26" s="5" t="s">
+      <c r="G26" s="5" t="s">
         <v>984</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="H26" s="5" t="s">
         <v>985</v>
       </c>
-      <c r="G26" s="5" t="s">
+      <c r="I26" s="9" t="s">
+        <v>980</v>
+      </c>
+      <c r="J26" s="5" t="s">
         <v>986</v>
       </c>
-      <c r="H26" s="5" t="s">
+      <c r="K26" s="5" t="s">
         <v>987</v>
       </c>
-      <c r="I26" s="9" t="s">
-        <v>982</v>
-      </c>
-      <c r="J26" s="5" t="s">
+      <c r="L26" s="5" t="s">
         <v>988</v>
       </c>
-      <c r="K26" s="5" t="s">
-        <v>989</v>
-      </c>
-      <c r="L26" s="5" t="s">
-        <v>990</v>
-      </c>
       <c r="M26" s="5" t="s">
-        <v>990</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>468</v>
       </c>
       <c r="B27" s="5" t="s">
+        <v>989</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>990</v>
+      </c>
+      <c r="D27" s="6" t="s">
         <v>991</v>
       </c>
-      <c r="C27" s="9" t="s">
+      <c r="E27" s="5" t="s">
         <v>992</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="F27" s="5" t="s">
         <v>993</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="G27" s="5" t="s">
         <v>994</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="H27" s="5" t="s">
         <v>995</v>
       </c>
-      <c r="G27" s="5" t="s">
+      <c r="I27" s="9" t="s">
+        <v>990</v>
+      </c>
+      <c r="J27" s="5" t="s">
         <v>996</v>
       </c>
-      <c r="H27" s="5" t="s">
+      <c r="K27" s="5" t="s">
         <v>997</v>
       </c>
-      <c r="I27" s="9" t="s">
-        <v>992</v>
-      </c>
-      <c r="J27" s="5" t="s">
+      <c r="L27" s="5" t="s">
         <v>998</v>
       </c>
-      <c r="K27" s="5" t="s">
-        <v>999</v>
-      </c>
-      <c r="L27" s="5" t="s">
-        <v>1000</v>
-      </c>
       <c r="M27" s="5" t="s">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>998</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>592</v>
       </c>
       <c r="B28" s="5" t="s">
+        <v>999</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>1000</v>
+      </c>
+      <c r="D28" s="6" t="s">
         <v>1001</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="E28" s="5" t="s">
         <v>1002</v>
       </c>
-      <c r="D28" s="6" t="s">
+      <c r="F28" s="5" t="s">
         <v>1003</v>
       </c>
-      <c r="E28" s="5" t="s">
+      <c r="G28" s="5" t="s">
         <v>1004</v>
       </c>
-      <c r="F28" s="5" t="s">
+      <c r="H28" s="5" t="s">
         <v>1005</v>
       </c>
-      <c r="G28" s="5" t="s">
+      <c r="I28" s="9" t="s">
+        <v>1000</v>
+      </c>
+      <c r="J28" s="5" t="s">
         <v>1006</v>
       </c>
-      <c r="H28" s="5" t="s">
+      <c r="K28" s="5" t="s">
         <v>1007</v>
       </c>
-      <c r="I28" s="9" t="s">
-        <v>1002</v>
-      </c>
-      <c r="J28" s="5" t="s">
+      <c r="L28" s="5" t="s">
         <v>1008</v>
       </c>
-      <c r="K28" s="5" t="s">
-        <v>1009</v>
-      </c>
-      <c r="L28" s="5" t="s">
-        <v>1010</v>
-      </c>
       <c r="M28" s="5" t="s">
-        <v>1010</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>601</v>
       </c>
       <c r="B29" s="5" t="s">
+        <v>1044</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>1045</v>
+      </c>
+      <c r="D29" s="6" t="s">
         <v>1046</v>
       </c>
-      <c r="C29" s="9" t="s">
+      <c r="E29" s="5" t="s">
         <v>1047</v>
       </c>
-      <c r="D29" s="6" t="s">
+      <c r="F29" s="5" t="s">
         <v>1048</v>
       </c>
-      <c r="E29" s="5" t="s">
+      <c r="G29" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="F29" s="5" t="s">
+      <c r="H29" s="5" t="s">
         <v>1050</v>
       </c>
-      <c r="G29" s="5" t="s">
+      <c r="I29" s="9" t="s">
+        <v>1045</v>
+      </c>
+      <c r="J29" s="5" t="s">
         <v>1051</v>
       </c>
-      <c r="H29" s="5" t="s">
+      <c r="K29" s="5" t="s">
         <v>1052</v>
       </c>
-      <c r="I29" s="9" t="s">
-        <v>1047</v>
-      </c>
-      <c r="J29" s="5" t="s">
+      <c r="L29" s="5" t="s">
         <v>1053</v>
       </c>
-      <c r="K29" s="5" t="s">
-        <v>1054</v>
-      </c>
-      <c r="L29" s="5" t="s">
-        <v>1055</v>
-      </c>
       <c r="M29" s="5" t="s">
-        <v>1055</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>1053</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>610</v>
       </c>
       <c r="B30" s="5" t="s">
+        <v>1054</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>1055</v>
+      </c>
+      <c r="D30" s="6" t="s">
         <v>1056</v>
       </c>
-      <c r="C30" s="9" t="s">
+      <c r="E30" s="5" t="s">
         <v>1057</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="F30" s="5" t="s">
         <v>1058</v>
       </c>
-      <c r="E30" s="5" t="s">
+      <c r="G30" s="5" t="s">
         <v>1059</v>
       </c>
-      <c r="F30" s="5" t="s">
+      <c r="H30" s="5" t="s">
         <v>1060</v>
       </c>
-      <c r="G30" s="5" t="s">
+      <c r="I30" s="9" t="s">
+        <v>1055</v>
+      </c>
+      <c r="J30" s="5" t="s">
         <v>1061</v>
       </c>
-      <c r="H30" s="5" t="s">
+      <c r="K30" s="5" t="s">
         <v>1062</v>
       </c>
-      <c r="I30" s="9" t="s">
-        <v>1057</v>
-      </c>
-      <c r="J30" s="5" t="s">
+      <c r="L30" s="5" t="s">
         <v>1063</v>
       </c>
-      <c r="K30" s="5" t="s">
-        <v>1064</v>
-      </c>
-      <c r="L30" s="5" t="s">
-        <v>1065</v>
-      </c>
       <c r="M30" s="5" t="s">
-        <v>1065</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>628</v>
       </c>
       <c r="B31" s="5" t="s">
+        <v>892</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>893</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>901</v>
+      </c>
+      <c r="E31" s="5" t="s">
         <v>894</v>
       </c>
-      <c r="C31" s="9" t="s">
+      <c r="F31" s="5" t="s">
         <v>895</v>
       </c>
-      <c r="D31" s="6" t="s">
-        <v>903</v>
-      </c>
-      <c r="E31" s="5" t="s">
+      <c r="G31" s="5" t="s">
         <v>896</v>
       </c>
-      <c r="F31" s="5" t="s">
+      <c r="H31" s="5" t="s">
         <v>897</v>
       </c>
-      <c r="G31" s="5" t="s">
+      <c r="I31" s="9" t="s">
+        <v>893</v>
+      </c>
+      <c r="J31" s="5" t="s">
         <v>898</v>
       </c>
-      <c r="H31" s="5" t="s">
+      <c r="K31" s="5" t="s">
         <v>899</v>
       </c>
-      <c r="I31" s="9" t="s">
-        <v>895</v>
-      </c>
-      <c r="J31" s="5" t="s">
+      <c r="L31" s="5" t="s">
         <v>900</v>
       </c>
-      <c r="K31" s="5" t="s">
-        <v>901</v>
-      </c>
-      <c r="L31" s="5" t="s">
-        <v>902</v>
-      </c>
       <c r="M31" s="5" t="s">
-        <v>902</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>546</v>
       </c>
@@ -9134,7 +9134,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>555</v>
       </c>
@@ -9213,9 +9213,9 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -9223,7 +9223,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
GDE-7303 additional changes on data set file for TL_CAL_08
</commit_message>
<xml_diff>
--- a/DataSet/Integration_DataSet/TL/TL_Data_Set_AU.xlsx
+++ b/DataSet/Integration_DataSet/TL/TL_Data_Set_AU.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\Integration_DataSet\TL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29B2C55D-4AA6-4AA8-B6F4-5E3A6CAD87F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5B28F4F-D2C3-4256-8996-AE695C404F9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BaseRate_Fields" sheetId="1" r:id="rId1"/>
@@ -7821,7 +7821,7 @@
   <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8119,7 +8119,7 @@
         <v>807</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>487</v>
+        <v>816</v>
       </c>
       <c r="M7" s="5" t="s">
         <v>816</v>

</xml_diff>

<commit_message>
GDE-7202 intial fixex for TLBASE02
</commit_message>
<xml_diff>
--- a/DataSet/Integration_DataSet/TL/TL_Data_Set_AU.xlsx
+++ b/DataSet/Integration_DataSet/TL/TL_Data_Set_AU.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\Integration_DataSet\TL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05D60997-DB15-4187-884F-5DC225A6CAE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F0DC872-5E37-47C4-B392-F36C51B47BFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BaseRate_Fields" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1436" uniqueCount="1120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1477" uniqueCount="1121">
   <si>
     <t>rowid</t>
   </si>
@@ -2942,9 +2942,6 @@
   </si>
   <si>
     <t>TL_BASE_38</t>
-  </si>
-  <si>
-    <t>\DataSet\TL_DataSet\BaseRates_GSFile\TL_BASE_38_Files\</t>
   </si>
   <si>
     <t>FINASTRA_CCB_BASERATE_SY_GROUP99_BASE38.csv</t>
@@ -3440,6 +3437,12 @@
   </si>
   <si>
     <t>\DataSet\Integration_DataSet\TL\FXRates_GSFile\AU\TL_FX_01_Files\</t>
+  </si>
+  <si>
+    <t>\DataSet\Integration_DataSet\TL\BaseRates_GSFile\AU\TL_BASE_02_Files\</t>
+  </si>
+  <si>
+    <t>\DataSet\Integration_DataSet\TL\BaseRates_GSFile\AU\TL_BASE_38_Files\</t>
   </si>
 </sst>
 </file>
@@ -4392,8 +4395,8 @@
   </sheetPr>
   <dimension ref="A1:N42"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4422,7 +4425,7 @@
         <v>17</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>1</v>
@@ -4466,10 +4469,10 @@
         <v>11</v>
       </c>
       <c r="C2" s="9" t="s">
+        <v>1115</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>1116</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>1117</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>94</v>
@@ -4484,7 +4487,7 @@
         <v>18</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>21</v>
@@ -4506,9 +4509,11 @@
       <c r="B3" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="5"/>
+      <c r="C3" s="9" t="s">
+        <v>1115</v>
+      </c>
       <c r="D3" s="9" t="s">
-        <v>131</v>
+        <v>1119</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>95</v>
@@ -4523,7 +4528,7 @@
         <v>25</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>131</v>
+        <v>1119</v>
       </c>
       <c r="J3" s="5" t="s">
         <v>26</v>
@@ -4545,7 +4550,9 @@
       <c r="B4" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="5"/>
+      <c r="C4" s="9" t="s">
+        <v>1115</v>
+      </c>
       <c r="D4" s="9" t="s">
         <v>131</v>
       </c>
@@ -4584,7 +4591,9 @@
       <c r="B5" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="5"/>
+      <c r="C5" s="9" t="s">
+        <v>1115</v>
+      </c>
       <c r="D5" s="9" t="s">
         <v>131</v>
       </c>
@@ -4623,7 +4632,9 @@
       <c r="B6" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C6" s="5"/>
+      <c r="C6" s="9" t="s">
+        <v>1115</v>
+      </c>
       <c r="D6" s="9" t="s">
         <v>131</v>
       </c>
@@ -4662,7 +4673,9 @@
       <c r="B7" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C7" s="5"/>
+      <c r="C7" s="9" t="s">
+        <v>1115</v>
+      </c>
       <c r="D7" s="9" t="s">
         <v>915</v>
       </c>
@@ -4701,7 +4714,9 @@
       <c r="B8" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C8" s="5"/>
+      <c r="C8" s="9" t="s">
+        <v>1115</v>
+      </c>
       <c r="D8" s="9" t="s">
         <v>917</v>
       </c>
@@ -4740,7 +4755,9 @@
       <c r="B9" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="C9" s="5"/>
+      <c r="C9" s="9" t="s">
+        <v>1115</v>
+      </c>
       <c r="D9" s="9" t="s">
         <v>919</v>
       </c>
@@ -4779,9 +4796,11 @@
       <c r="B10" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="C10" s="5"/>
+      <c r="C10" s="9" t="s">
+        <v>1115</v>
+      </c>
       <c r="D10" s="9" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>105</v>
@@ -4796,7 +4815,7 @@
         <v>108</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="J10" s="5" t="s">
         <v>109</v>
@@ -4818,7 +4837,9 @@
       <c r="B11" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="C11" s="5"/>
+      <c r="C11" s="9" t="s">
+        <v>1115</v>
+      </c>
       <c r="D11" s="9" t="s">
         <v>131</v>
       </c>
@@ -4857,7 +4878,9 @@
       <c r="B12" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="C12" s="5"/>
+      <c r="C12" s="9" t="s">
+        <v>1115</v>
+      </c>
       <c r="D12" s="9" t="s">
         <v>131</v>
       </c>
@@ -4896,7 +4919,9 @@
       <c r="B13" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="C13" s="5"/>
+      <c r="C13" s="9" t="s">
+        <v>1115</v>
+      </c>
       <c r="D13" s="9" t="s">
         <v>131</v>
       </c>
@@ -4935,7 +4960,9 @@
       <c r="B14" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="C14" s="5"/>
+      <c r="C14" s="9" t="s">
+        <v>1115</v>
+      </c>
       <c r="D14" s="9" t="s">
         <v>131</v>
       </c>
@@ -4974,7 +5001,9 @@
       <c r="B15" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="C15" s="5"/>
+      <c r="C15" s="9" t="s">
+        <v>1115</v>
+      </c>
       <c r="D15" s="9" t="s">
         <v>131</v>
       </c>
@@ -5013,7 +5042,9 @@
       <c r="B16" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="C16" s="5"/>
+      <c r="C16" s="9" t="s">
+        <v>1115</v>
+      </c>
       <c r="D16" s="9" t="s">
         <v>131</v>
       </c>
@@ -5052,7 +5083,9 @@
       <c r="B17" s="5" t="s">
         <v>921</v>
       </c>
-      <c r="C17" s="5"/>
+      <c r="C17" s="9" t="s">
+        <v>1115</v>
+      </c>
       <c r="D17" s="9" t="s">
         <v>922</v>
       </c>
@@ -5089,38 +5122,40 @@
         <v>343</v>
       </c>
       <c r="B18" s="5" t="s">
+        <v>1075</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>1115</v>
+      </c>
+      <c r="D18" s="9" t="s">
         <v>1076</v>
       </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="9" t="s">
+      <c r="E18" s="5" t="s">
         <v>1077</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="F18" s="5" t="s">
         <v>1078</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="G18" s="5" t="s">
         <v>1079</v>
       </c>
-      <c r="G18" s="5" t="s">
+      <c r="H18" s="5" t="s">
         <v>1080</v>
       </c>
-      <c r="H18" s="5" t="s">
+      <c r="I18" s="9" t="s">
+        <v>1076</v>
+      </c>
+      <c r="J18" s="5" t="s">
         <v>1081</v>
       </c>
-      <c r="I18" s="9" t="s">
-        <v>1077</v>
-      </c>
-      <c r="J18" s="5" t="s">
+      <c r="K18" s="5" t="s">
         <v>1082</v>
       </c>
-      <c r="K18" s="5" t="s">
+      <c r="L18" s="5" t="s">
         <v>1083</v>
       </c>
-      <c r="L18" s="5" t="s">
+      <c r="M18" s="5" t="s">
         <v>1084</v>
-      </c>
-      <c r="M18" s="5" t="s">
-        <v>1085</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -5128,38 +5163,40 @@
         <v>353</v>
       </c>
       <c r="B19" s="5" t="s">
+        <v>1016</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>1115</v>
+      </c>
+      <c r="D19" s="9" t="s">
         <v>1017</v>
       </c>
-      <c r="C19" s="5"/>
-      <c r="D19" s="9" t="s">
+      <c r="E19" s="5" t="s">
         <v>1018</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="F19" s="5" t="s">
         <v>1019</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="G19" s="5" t="s">
         <v>1020</v>
       </c>
-      <c r="G19" s="5" t="s">
+      <c r="H19" s="5" t="s">
         <v>1021</v>
       </c>
-      <c r="H19" s="5" t="s">
+      <c r="I19" s="9" t="s">
+        <v>1017</v>
+      </c>
+      <c r="J19" s="5" t="s">
         <v>1022</v>
       </c>
-      <c r="I19" s="9" t="s">
-        <v>1018</v>
-      </c>
-      <c r="J19" s="5" t="s">
+      <c r="K19" s="5" t="s">
         <v>1023</v>
       </c>
-      <c r="K19" s="5" t="s">
+      <c r="L19" s="5" t="s">
         <v>1024</v>
       </c>
-      <c r="L19" s="5" t="s">
+      <c r="M19" s="5" t="s">
         <v>1025</v>
-      </c>
-      <c r="M19" s="5" t="s">
-        <v>1026</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
@@ -5169,7 +5206,9 @@
       <c r="B20" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="C20" s="5"/>
+      <c r="C20" s="9" t="s">
+        <v>1115</v>
+      </c>
       <c r="D20" s="9" t="s">
         <v>131</v>
       </c>
@@ -5208,7 +5247,9 @@
       <c r="B21" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="C21" s="5"/>
+      <c r="C21" s="9" t="s">
+        <v>1115</v>
+      </c>
       <c r="D21" s="9" t="s">
         <v>131</v>
       </c>
@@ -5247,7 +5288,9 @@
       <c r="B22" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="C22" s="5"/>
+      <c r="C22" s="9" t="s">
+        <v>1115</v>
+      </c>
       <c r="D22" s="9" t="s">
         <v>131</v>
       </c>
@@ -5286,7 +5329,9 @@
       <c r="B23" s="5" t="s">
         <v>231</v>
       </c>
-      <c r="C23" s="5"/>
+      <c r="C23" s="9" t="s">
+        <v>1115</v>
+      </c>
       <c r="D23" s="9" t="s">
         <v>131</v>
       </c>
@@ -5325,7 +5370,9 @@
       <c r="B24" s="5" t="s">
         <v>565</v>
       </c>
-      <c r="C24" s="5"/>
+      <c r="C24" s="9" t="s">
+        <v>1115</v>
+      </c>
       <c r="D24" s="9" t="s">
         <v>566</v>
       </c>
@@ -5364,7 +5411,9 @@
       <c r="B25" s="5" t="s">
         <v>584</v>
       </c>
-      <c r="C25" s="5"/>
+      <c r="C25" s="9" t="s">
+        <v>1115</v>
+      </c>
       <c r="D25" s="9" t="s">
         <v>575</v>
       </c>
@@ -5403,7 +5452,9 @@
       <c r="B26" s="5" t="s">
         <v>700</v>
       </c>
-      <c r="C26" s="5"/>
+      <c r="C26" s="9" t="s">
+        <v>1115</v>
+      </c>
       <c r="D26" s="9" t="s">
         <v>701</v>
       </c>
@@ -5440,38 +5491,40 @@
         <v>458</v>
       </c>
       <c r="B27" s="5" t="s">
+        <v>1085</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>1115</v>
+      </c>
+      <c r="D27" s="9" t="s">
         <v>1086</v>
       </c>
-      <c r="C27" s="5"/>
-      <c r="D27" s="9" t="s">
+      <c r="E27" s="5" t="s">
         <v>1087</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="F27" s="5" t="s">
         <v>1088</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="G27" s="5" t="s">
         <v>1089</v>
       </c>
-      <c r="G27" s="5" t="s">
+      <c r="H27" s="5" t="s">
         <v>1090</v>
       </c>
-      <c r="H27" s="5" t="s">
+      <c r="I27" s="9" t="s">
+        <v>1086</v>
+      </c>
+      <c r="J27" s="5" t="s">
         <v>1091</v>
       </c>
-      <c r="I27" s="9" t="s">
-        <v>1087</v>
-      </c>
-      <c r="J27" s="5" t="s">
+      <c r="K27" s="5" t="s">
         <v>1092</v>
       </c>
-      <c r="K27" s="5" t="s">
+      <c r="L27" s="5" t="s">
         <v>1093</v>
       </c>
-      <c r="L27" s="5" t="s">
+      <c r="M27" s="5" t="s">
         <v>1094</v>
-      </c>
-      <c r="M27" s="5" t="s">
-        <v>1095</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
@@ -5481,7 +5534,9 @@
       <c r="B28" s="5" t="s">
         <v>672</v>
       </c>
-      <c r="C28" s="5"/>
+      <c r="C28" s="9" t="s">
+        <v>1115</v>
+      </c>
       <c r="D28" s="9" t="s">
         <v>673</v>
       </c>
@@ -5520,7 +5575,9 @@
       <c r="B29" s="5" t="s">
         <v>682</v>
       </c>
-      <c r="C29" s="5"/>
+      <c r="C29" s="9" t="s">
+        <v>1115</v>
+      </c>
       <c r="D29" s="9" t="s">
         <v>683</v>
       </c>
@@ -5559,7 +5616,9 @@
       <c r="B30" s="5" t="s">
         <v>718</v>
       </c>
-      <c r="C30" s="5"/>
+      <c r="C30" s="9" t="s">
+        <v>1115</v>
+      </c>
       <c r="D30" s="9" t="s">
         <v>719</v>
       </c>
@@ -5598,7 +5657,9 @@
       <c r="B31" s="5" t="s">
         <v>718</v>
       </c>
-      <c r="C31" s="5"/>
+      <c r="C31" s="9" t="s">
+        <v>1115</v>
+      </c>
       <c r="D31" s="9" t="s">
         <v>719</v>
       </c>
@@ -5637,7 +5698,9 @@
       <c r="B32" s="5" t="s">
         <v>931</v>
       </c>
-      <c r="C32" s="5"/>
+      <c r="C32" s="9" t="s">
+        <v>1115</v>
+      </c>
       <c r="D32" s="9" t="s">
         <v>932</v>
       </c>
@@ -5676,7 +5739,9 @@
       <c r="B33" s="5" t="s">
         <v>941</v>
       </c>
-      <c r="C33" s="5"/>
+      <c r="C33" s="9" t="s">
+        <v>1115</v>
+      </c>
       <c r="D33" s="9" t="s">
         <v>942</v>
       </c>
@@ -5715,7 +5780,9 @@
       <c r="B34" s="5" t="s">
         <v>951</v>
       </c>
-      <c r="C34" s="5"/>
+      <c r="C34" s="9" t="s">
+        <v>1115</v>
+      </c>
       <c r="D34" s="9" t="s">
         <v>952</v>
       </c>
@@ -5754,7 +5821,9 @@
       <c r="B35" s="5" t="s">
         <v>961</v>
       </c>
-      <c r="C35" s="5"/>
+      <c r="C35" s="9" t="s">
+        <v>1115</v>
+      </c>
       <c r="D35" s="9" t="s">
         <v>962</v>
       </c>
@@ -5793,75 +5862,79 @@
       <c r="B36" s="5" t="s">
         <v>972</v>
       </c>
-      <c r="C36" s="5"/>
+      <c r="C36" s="9" t="s">
+        <v>1115</v>
+      </c>
       <c r="D36" s="9" t="s">
+        <v>1120</v>
+      </c>
+      <c r="E36" s="6" t="s">
         <v>973</v>
       </c>
-      <c r="E36" s="6" t="s">
+      <c r="F36" s="5" t="s">
         <v>974</v>
       </c>
-      <c r="F36" s="5" t="s">
+      <c r="G36" s="5" t="s">
         <v>975</v>
       </c>
-      <c r="G36" s="5" t="s">
+      <c r="H36" s="5" t="s">
         <v>976</v>
       </c>
-      <c r="H36" s="5" t="s">
+      <c r="I36" s="9" t="s">
+        <v>1120</v>
+      </c>
+      <c r="J36" s="5" t="s">
         <v>977</v>
       </c>
-      <c r="I36" s="9" t="s">
-        <v>973</v>
-      </c>
-      <c r="J36" s="5" t="s">
+      <c r="K36" s="5" t="s">
         <v>978</v>
       </c>
-      <c r="K36" s="5" t="s">
+      <c r="L36" s="5" t="s">
         <v>979</v>
       </c>
-      <c r="L36" s="5" t="s">
+      <c r="M36" s="5" t="s">
         <v>980</v>
-      </c>
-      <c r="M36" s="5" t="s">
-        <v>981</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
+        <v>1095</v>
+      </c>
+      <c r="B37" s="5" t="s">
         <v>1096</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="C37" s="9" t="s">
+        <v>1115</v>
+      </c>
+      <c r="D37" s="9" t="s">
         <v>1097</v>
       </c>
-      <c r="C37" s="5"/>
-      <c r="D37" s="9" t="s">
+      <c r="E37" s="5" t="s">
         <v>1098</v>
       </c>
-      <c r="E37" s="5" t="s">
+      <c r="F37" s="5" t="s">
         <v>1099</v>
       </c>
-      <c r="F37" s="5" t="s">
+      <c r="G37" s="5" t="s">
         <v>1100</v>
       </c>
-      <c r="G37" s="5" t="s">
+      <c r="H37" s="5" t="s">
         <v>1101</v>
       </c>
-      <c r="H37" s="5" t="s">
+      <c r="I37" s="9" t="s">
+        <v>1097</v>
+      </c>
+      <c r="J37" s="5" t="s">
         <v>1102</v>
       </c>
-      <c r="I37" s="9" t="s">
-        <v>1098</v>
-      </c>
-      <c r="J37" s="5" t="s">
+      <c r="K37" s="5" t="s">
         <v>1103</v>
       </c>
-      <c r="K37" s="5" t="s">
+      <c r="L37" s="5" t="s">
         <v>1104</v>
       </c>
-      <c r="L37" s="5" t="s">
+      <c r="M37" s="5" t="s">
         <v>1105</v>
-      </c>
-      <c r="M37" s="5" t="s">
-        <v>1106</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
@@ -5871,7 +5944,9 @@
       <c r="B38" s="5" t="s">
         <v>737</v>
       </c>
-      <c r="C38" s="5"/>
+      <c r="C38" s="9" t="s">
+        <v>1115</v>
+      </c>
       <c r="D38" s="9" t="s">
         <v>738</v>
       </c>
@@ -5910,7 +5985,9 @@
       <c r="B39" s="5" t="s">
         <v>770</v>
       </c>
-      <c r="C39" s="5"/>
+      <c r="C39" s="9" t="s">
+        <v>1115</v>
+      </c>
       <c r="D39" s="9" t="s">
         <v>771</v>
       </c>
@@ -5952,7 +6029,9 @@
       <c r="B40" s="5" t="s">
         <v>783</v>
       </c>
-      <c r="C40" s="5"/>
+      <c r="C40" s="9" t="s">
+        <v>1115</v>
+      </c>
       <c r="D40" s="9" t="s">
         <v>784</v>
       </c>
@@ -5992,7 +6071,9 @@
       <c r="B41" s="5" t="s">
         <v>748</v>
       </c>
-      <c r="C41" s="5"/>
+      <c r="C41" s="9" t="s">
+        <v>1115</v>
+      </c>
       <c r="D41" s="9" t="s">
         <v>749</v>
       </c>
@@ -6031,7 +6112,9 @@
       <c r="B42" s="5" t="s">
         <v>759</v>
       </c>
-      <c r="C42" s="5"/>
+      <c r="C42" s="9" t="s">
+        <v>1115</v>
+      </c>
       <c r="D42" s="9" t="s">
         <v>760</v>
       </c>
@@ -6066,64 +6149,66 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{E222DBE2-AD55-4081-ACB5-91B6B0A7094E}"/>
-    <hyperlink ref="I3:I15" r:id="rId2" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{F2409101-F4DA-42F3-988A-9AF7922C773A}"/>
-    <hyperlink ref="D3:D15" r:id="rId3" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{32233F94-4832-4BCF-B2E9-DB216977EE67}"/>
-    <hyperlink ref="I16" r:id="rId4" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{DD6A71EB-82F8-4555-8BC1-E21692C0A9D8}"/>
-    <hyperlink ref="D16" r:id="rId5" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{1E6673C8-05B2-49CF-B15C-C05DC68EE09D}"/>
-    <hyperlink ref="I20" r:id="rId6" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{A21C788D-B886-45D3-A70B-8E4542A7BEF5}"/>
-    <hyperlink ref="D20" r:id="rId7" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{7F46C1BA-5DA7-4D92-A42B-C71BD9EA5745}"/>
-    <hyperlink ref="I21" r:id="rId8" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{E4218A2A-B2B6-44CA-94BB-7A216E566E81}"/>
-    <hyperlink ref="D21" r:id="rId9" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{8251AD55-A7DC-4CEB-B6AF-0BE1AFAD6F71}"/>
-    <hyperlink ref="I22" r:id="rId10" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{0DF9F788-8479-4507-AA61-D8F974D9BCB1}"/>
-    <hyperlink ref="D22" r:id="rId11" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{E1F54B31-1206-4B59-AF75-E8CAD04ECBEA}"/>
-    <hyperlink ref="I23" r:id="rId12" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{A7FB320A-5F86-449D-B547-764AD24BFF52}"/>
-    <hyperlink ref="D23" r:id="rId13" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{35740293-7EEE-49C4-80E5-A96C12A3D4BF}"/>
-    <hyperlink ref="I24" r:id="rId14" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{ACFC6A23-91D4-4C43-B643-1AF4E4DA6B6E}"/>
-    <hyperlink ref="D24" r:id="rId15" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{6223798A-153D-4A66-B8CF-301B174D7DB7}"/>
-    <hyperlink ref="I25" r:id="rId16" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{C04E7C11-1F4B-4B75-A866-C4EDB113FB99}"/>
-    <hyperlink ref="D25" r:id="rId17" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{52BD4B3C-911C-45B5-BBAC-7F8DE8BA150E}"/>
-    <hyperlink ref="D28" r:id="rId18" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{EF9BF8AE-77D8-47B1-925C-CFA5D3D1EDDA}"/>
-    <hyperlink ref="D29" r:id="rId19" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{4B664857-B6CF-46D6-873E-1A5585372303}"/>
-    <hyperlink ref="D26" r:id="rId20" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{CDF2C16F-5921-4E5D-A819-FAC3430367A5}"/>
-    <hyperlink ref="I26" r:id="rId21" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{9379B31E-411A-4D47-A347-E83BA0B617EC}"/>
-    <hyperlink ref="I28" r:id="rId22" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{D7475230-43D3-45C7-9DC9-F493EEE99A1C}"/>
-    <hyperlink ref="I29" r:id="rId23" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{2FE7045F-9240-4E97-A3F9-0B3AADD49370}"/>
-    <hyperlink ref="D30" r:id="rId24" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{E4F81E86-9E57-41D5-9A8B-9DA9C6AC75AB}"/>
-    <hyperlink ref="I30" r:id="rId25" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{AAC6D86A-E2BF-4C02-8787-80191BED54BB}"/>
-    <hyperlink ref="D31" r:id="rId26" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{3563E6B9-C77F-4D9F-97CB-4C245E6CC18C}"/>
-    <hyperlink ref="I31" r:id="rId27" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{EC84FA26-4C99-44AF-9B40-B034738A6757}"/>
-    <hyperlink ref="D41" r:id="rId28" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{87382ADA-8A97-45BA-B8C1-A4D301E200B8}"/>
-    <hyperlink ref="I41" r:id="rId29" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{98073778-1519-4CAA-B79F-18D0CF454C9F}"/>
-    <hyperlink ref="D42" r:id="rId30" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{301000FF-65A0-4601-875E-D69C8BE4B4C5}"/>
-    <hyperlink ref="I42" r:id="rId31" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{B0802975-66A5-423A-834B-AEB1BEB43ACC}"/>
-    <hyperlink ref="D39" r:id="rId32" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{44C44DF0-B4EF-45CC-9D42-B5EC4D9B05A7}"/>
-    <hyperlink ref="I39" r:id="rId33" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{D2B94F32-58AC-4013-B620-07D1AF9FAFCA}"/>
-    <hyperlink ref="D40" r:id="rId34" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{F6E39756-3427-4341-83CB-95AFE7B66C86}"/>
-    <hyperlink ref="I40" r:id="rId35" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{33D1D3C7-54B1-4640-A26B-17C5DBC752B3}"/>
-    <hyperlink ref="D17" r:id="rId36" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{2D5A03EB-6379-4450-9AC9-26DCE06D1A0A}"/>
-    <hyperlink ref="I17" r:id="rId37" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{3C8671ED-2DD6-46FE-BD17-2A7F170D378E}"/>
-    <hyperlink ref="D32" r:id="rId38" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{3650E5BA-817D-4640-B16F-D558CCA9ABB3}"/>
-    <hyperlink ref="I32" r:id="rId39" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{C206FA82-ADFE-4AF1-BE12-1473CECEC67E}"/>
-    <hyperlink ref="I38" r:id="rId40" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{017369F0-A74E-412E-9826-F2E85D5CDCF3}"/>
-    <hyperlink ref="D38" r:id="rId41" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{0D3B1B11-E8BA-4A4A-8612-65A84A715DDB}"/>
-    <hyperlink ref="D33" r:id="rId42" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{86E45C2A-35FB-4862-81B2-32EBEBC4419D}"/>
-    <hyperlink ref="I33" r:id="rId43" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{FC10F196-4ACE-40AA-8B19-C4F3F6EBEAD2}"/>
-    <hyperlink ref="D34" r:id="rId44" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{8A18D22D-FFE3-4A25-8680-1D575513ACF9}"/>
-    <hyperlink ref="I34" r:id="rId45" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{2D2A1FFD-A1CF-4898-89AC-366D631A4AE9}"/>
-    <hyperlink ref="D35" r:id="rId46" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{17087BD1-D3E5-4AA0-932F-EF6585B39DAD}"/>
-    <hyperlink ref="I35" r:id="rId47" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{C2EE35C7-B69C-4CFE-A9C7-8147CC81F993}"/>
-    <hyperlink ref="D36" r:id="rId48" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{148BD777-7D4F-4D9C-BE58-657825E990DC}"/>
-    <hyperlink ref="I36" r:id="rId49" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{E8A6541D-C266-4297-BE02-9DB617BCE6E9}"/>
-    <hyperlink ref="D19" r:id="rId50" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{6E642722-BFB2-445A-9B7B-53C0A272604A}"/>
-    <hyperlink ref="I19" r:id="rId51" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{0C1BBEBF-D848-4240-A469-BF25D2FF4893}"/>
-    <hyperlink ref="D18" r:id="rId52" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{B37D5DAB-9BBF-4734-A8F3-C544C4DA476C}"/>
-    <hyperlink ref="I18" r:id="rId53" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{527EEE72-0B11-40B4-96A9-24D97A6864B7}"/>
-    <hyperlink ref="D27" r:id="rId54" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{CD10DEA0-475B-4977-B943-77B7CACFA7CC}"/>
-    <hyperlink ref="I27" r:id="rId55" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{748072CF-65E5-4932-9033-FEA7A8832219}"/>
-    <hyperlink ref="D37" r:id="rId56" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{2016704E-36EB-49AB-A36D-01EEB9E33415}"/>
-    <hyperlink ref="I37" r:id="rId57" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{111E8F37-E507-4086-A947-F3F427867099}"/>
-    <hyperlink ref="C2" r:id="rId58" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{D0DABB52-96E5-41AF-9FAC-9921DADC3D95}"/>
-    <hyperlink ref="I2" r:id="rId59" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{432E7AC4-2F08-431B-AE35-E60F0B5F2AC0}"/>
+    <hyperlink ref="I16" r:id="rId2" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{DD6A71EB-82F8-4555-8BC1-E21692C0A9D8}"/>
+    <hyperlink ref="D16" r:id="rId3" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{1E6673C8-05B2-49CF-B15C-C05DC68EE09D}"/>
+    <hyperlink ref="I20" r:id="rId4" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{A21C788D-B886-45D3-A70B-8E4542A7BEF5}"/>
+    <hyperlink ref="D20" r:id="rId5" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{7F46C1BA-5DA7-4D92-A42B-C71BD9EA5745}"/>
+    <hyperlink ref="I21" r:id="rId6" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{E4218A2A-B2B6-44CA-94BB-7A216E566E81}"/>
+    <hyperlink ref="D21" r:id="rId7" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{8251AD55-A7DC-4CEB-B6AF-0BE1AFAD6F71}"/>
+    <hyperlink ref="I22" r:id="rId8" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{0DF9F788-8479-4507-AA61-D8F974D9BCB1}"/>
+    <hyperlink ref="D22" r:id="rId9" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{E1F54B31-1206-4B59-AF75-E8CAD04ECBEA}"/>
+    <hyperlink ref="I23" r:id="rId10" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{A7FB320A-5F86-449D-B547-764AD24BFF52}"/>
+    <hyperlink ref="D23" r:id="rId11" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{35740293-7EEE-49C4-80E5-A96C12A3D4BF}"/>
+    <hyperlink ref="I24" r:id="rId12" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{ACFC6A23-91D4-4C43-B643-1AF4E4DA6B6E}"/>
+    <hyperlink ref="D24" r:id="rId13" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{6223798A-153D-4A66-B8CF-301B174D7DB7}"/>
+    <hyperlink ref="I25" r:id="rId14" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{C04E7C11-1F4B-4B75-A866-C4EDB113FB99}"/>
+    <hyperlink ref="D25" r:id="rId15" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{52BD4B3C-911C-45B5-BBAC-7F8DE8BA150E}"/>
+    <hyperlink ref="D28" r:id="rId16" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{EF9BF8AE-77D8-47B1-925C-CFA5D3D1EDDA}"/>
+    <hyperlink ref="D29" r:id="rId17" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{4B664857-B6CF-46D6-873E-1A5585372303}"/>
+    <hyperlink ref="D26" r:id="rId18" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{CDF2C16F-5921-4E5D-A819-FAC3430367A5}"/>
+    <hyperlink ref="I26" r:id="rId19" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{9379B31E-411A-4D47-A347-E83BA0B617EC}"/>
+    <hyperlink ref="I28" r:id="rId20" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{D7475230-43D3-45C7-9DC9-F493EEE99A1C}"/>
+    <hyperlink ref="I29" r:id="rId21" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{2FE7045F-9240-4E97-A3F9-0B3AADD49370}"/>
+    <hyperlink ref="D30" r:id="rId22" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{E4F81E86-9E57-41D5-9A8B-9DA9C6AC75AB}"/>
+    <hyperlink ref="I30" r:id="rId23" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{AAC6D86A-E2BF-4C02-8787-80191BED54BB}"/>
+    <hyperlink ref="D31" r:id="rId24" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{3563E6B9-C77F-4D9F-97CB-4C245E6CC18C}"/>
+    <hyperlink ref="I31" r:id="rId25" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{EC84FA26-4C99-44AF-9B40-B034738A6757}"/>
+    <hyperlink ref="D41" r:id="rId26" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{87382ADA-8A97-45BA-B8C1-A4D301E200B8}"/>
+    <hyperlink ref="I41" r:id="rId27" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{98073778-1519-4CAA-B79F-18D0CF454C9F}"/>
+    <hyperlink ref="D42" r:id="rId28" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{301000FF-65A0-4601-875E-D69C8BE4B4C5}"/>
+    <hyperlink ref="I42" r:id="rId29" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{B0802975-66A5-423A-834B-AEB1BEB43ACC}"/>
+    <hyperlink ref="D39" r:id="rId30" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{44C44DF0-B4EF-45CC-9D42-B5EC4D9B05A7}"/>
+    <hyperlink ref="I39" r:id="rId31" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{D2B94F32-58AC-4013-B620-07D1AF9FAFCA}"/>
+    <hyperlink ref="D40" r:id="rId32" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{F6E39756-3427-4341-83CB-95AFE7B66C86}"/>
+    <hyperlink ref="I40" r:id="rId33" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{33D1D3C7-54B1-4640-A26B-17C5DBC752B3}"/>
+    <hyperlink ref="D17" r:id="rId34" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{2D5A03EB-6379-4450-9AC9-26DCE06D1A0A}"/>
+    <hyperlink ref="I17" r:id="rId35" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{3C8671ED-2DD6-46FE-BD17-2A7F170D378E}"/>
+    <hyperlink ref="D32" r:id="rId36" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{3650E5BA-817D-4640-B16F-D558CCA9ABB3}"/>
+    <hyperlink ref="I32" r:id="rId37" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{C206FA82-ADFE-4AF1-BE12-1473CECEC67E}"/>
+    <hyperlink ref="I38" r:id="rId38" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{017369F0-A74E-412E-9826-F2E85D5CDCF3}"/>
+    <hyperlink ref="D38" r:id="rId39" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{0D3B1B11-E8BA-4A4A-8612-65A84A715DDB}"/>
+    <hyperlink ref="D33" r:id="rId40" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{86E45C2A-35FB-4862-81B2-32EBEBC4419D}"/>
+    <hyperlink ref="I33" r:id="rId41" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{FC10F196-4ACE-40AA-8B19-C4F3F6EBEAD2}"/>
+    <hyperlink ref="D34" r:id="rId42" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{8A18D22D-FFE3-4A25-8680-1D575513ACF9}"/>
+    <hyperlink ref="I34" r:id="rId43" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{2D2A1FFD-A1CF-4898-89AC-366D631A4AE9}"/>
+    <hyperlink ref="D35" r:id="rId44" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{17087BD1-D3E5-4AA0-932F-EF6585B39DAD}"/>
+    <hyperlink ref="I35" r:id="rId45" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{C2EE35C7-B69C-4CFE-A9C7-8147CC81F993}"/>
+    <hyperlink ref="D19" r:id="rId46" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{6E642722-BFB2-445A-9B7B-53C0A272604A}"/>
+    <hyperlink ref="I19" r:id="rId47" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{0C1BBEBF-D848-4240-A469-BF25D2FF4893}"/>
+    <hyperlink ref="D18" r:id="rId48" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{B37D5DAB-9BBF-4734-A8F3-C544C4DA476C}"/>
+    <hyperlink ref="I18" r:id="rId49" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{527EEE72-0B11-40B4-96A9-24D97A6864B7}"/>
+    <hyperlink ref="D27" r:id="rId50" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{CD10DEA0-475B-4977-B943-77B7CACFA7CC}"/>
+    <hyperlink ref="I27" r:id="rId51" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{748072CF-65E5-4932-9033-FEA7A8832219}"/>
+    <hyperlink ref="D37" r:id="rId52" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{2016704E-36EB-49AB-A36D-01EEB9E33415}"/>
+    <hyperlink ref="I37" r:id="rId53" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{111E8F37-E507-4086-A947-F3F427867099}"/>
+    <hyperlink ref="C2" r:id="rId54" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{D0DABB52-96E5-41AF-9FAC-9921DADC3D95}"/>
+    <hyperlink ref="I2" r:id="rId55" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{432E7AC4-2F08-431B-AE35-E60F0B5F2AC0}"/>
+    <hyperlink ref="C3" r:id="rId56" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{2F191E07-BEF7-450A-BA0C-578BEE86F6B4}"/>
+    <hyperlink ref="D3" r:id="rId57" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{4AE14356-97F7-4452-BD29-39FF296CFE6A}"/>
+    <hyperlink ref="I3" r:id="rId58" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{67C679D5-D34E-43F6-BBCC-092330D9F932}"/>
+    <hyperlink ref="D36" r:id="rId59" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{D580A5C7-8B14-47F7-8147-066E2F0B18F9}"/>
+    <hyperlink ref="I36" r:id="rId60" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{831F29D8-7436-407F-980E-6F4C938C8C72}"/>
+    <hyperlink ref="C4:C42" r:id="rId61" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{2E8C67A0-F9B8-4D78-B193-735D950464FA}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.3" right="0.3" top="0.61" bottom="0.37" header="0.1" footer="0.1"/>
@@ -6140,8 +6225,8 @@
   <sheetPr codeName="FXRates_Fields"/>
   <dimension ref="A1:P36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6171,7 +6256,7 @@
         <v>17</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>1</v>
@@ -6210,7 +6295,7 @@
         <v>121</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="15" x14ac:dyDescent="0.25">
@@ -6221,10 +6306,10 @@
         <v>44</v>
       </c>
       <c r="C2" s="9" t="s">
+        <v>1117</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>1118</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>1119</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>132</v>
@@ -6239,7 +6324,7 @@
         <v>48</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>129</v>
@@ -6267,7 +6352,9 @@
       <c r="B3" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C3" s="5"/>
+      <c r="C3" s="9" t="s">
+        <v>1117</v>
+      </c>
       <c r="D3" s="9" t="s">
         <v>130</v>
       </c>
@@ -6497,7 +6584,7 @@
         <v>130</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>260</v>
@@ -6542,7 +6629,7 @@
         <v>130</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>268</v>
@@ -6587,7 +6674,7 @@
         <v>130</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>276</v>
@@ -6632,7 +6719,7 @@
         <v>130</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>284</v>
@@ -6677,7 +6764,7 @@
         <v>130</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>292</v>
@@ -6722,7 +6809,7 @@
         <v>130</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>300</v>
@@ -6767,7 +6854,7 @@
         <v>130</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>308</v>
@@ -7070,7 +7157,7 @@
         <v>243</v>
       </c>
       <c r="P20" s="5" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="15" x14ac:dyDescent="0.25">
@@ -7795,19 +7882,20 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D3:D7" r:id="rId1" display="\\DataSet\\TL_DataSet\\FxRates_GSFile\\" xr:uid="{1C2361F4-1B13-456E-9BA3-E3D8B7F812A7}"/>
-    <hyperlink ref="D8:D22" r:id="rId2" display="\\DataSet\\TL_DataSet\\FxRates_GSFile\\" xr:uid="{30D6AB87-ED81-4A29-A8BC-F1B921F77AB7}"/>
-    <hyperlink ref="I8:I22" r:id="rId3" display="\\DataSet\\TL_DataSet\\FxRates_GSFile\\" xr:uid="{6E3D10A6-4C88-4334-881C-8676178CABF0}"/>
-    <hyperlink ref="D23:D31" r:id="rId4" display="\\DataSet\\TL_DataSet\\FxRates_GSFile\\" xr:uid="{6B3504B3-9870-47D0-8E2F-5CAB415D1405}"/>
-    <hyperlink ref="I23:I31" r:id="rId5" display="\\DataSet\\TL_DataSet\\FxRates_GSFile\\" xr:uid="{57CD682C-3C14-436B-ADDE-9A80258650CD}"/>
-    <hyperlink ref="D32:D34" r:id="rId6" display="\\DataSet\\TL_DataSet\\FxRates_GSFile\\" xr:uid="{202A1715-BE83-4EB7-A90F-52978138A4F3}"/>
-    <hyperlink ref="D35:D36" r:id="rId7" display="\\DataSet\\TL_DataSet\\FxRates_GSFile\\" xr:uid="{9840F825-8637-4C41-AA65-6AF3ECBC53D3}"/>
-    <hyperlink ref="I35:I36" r:id="rId8" display="\\DataSet\\TL_DataSet\\FxRates_GSFile\\" xr:uid="{E6DF1C66-E06C-4508-BF64-80E6763D6FB9}"/>
-    <hyperlink ref="I32:I34" r:id="rId9" display="\\DataSet\\TL_DataSet\\FxRates_GSFile\\" xr:uid="{5D520F54-CC93-417A-ADE8-C492B5E5E28A}"/>
-    <hyperlink ref="I21:I29" r:id="rId10" display="\\DataSet\\TL_DataSet\\FxRates_GSFile\\" xr:uid="{47A9315B-DFC8-4430-A45E-9D03C065A594}"/>
-    <hyperlink ref="C2" r:id="rId11" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{DC17FF84-1D37-4112-BF5D-BCB4C73CD0FB}"/>
-    <hyperlink ref="D2" r:id="rId12" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{7887B602-EE56-45AE-936D-8A968AF005AA}"/>
-    <hyperlink ref="I2" r:id="rId13" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{883636BB-DB43-4D2E-AC6F-B249FF19C9EB}"/>
+    <hyperlink ref="D8:D22" r:id="rId1" display="\\DataSet\\TL_DataSet\\FxRates_GSFile\\" xr:uid="{30D6AB87-ED81-4A29-A8BC-F1B921F77AB7}"/>
+    <hyperlink ref="I8:I22" r:id="rId2" display="\\DataSet\\TL_DataSet\\FxRates_GSFile\\" xr:uid="{6E3D10A6-4C88-4334-881C-8676178CABF0}"/>
+    <hyperlink ref="D23:D31" r:id="rId3" display="\\DataSet\\TL_DataSet\\FxRates_GSFile\\" xr:uid="{6B3504B3-9870-47D0-8E2F-5CAB415D1405}"/>
+    <hyperlink ref="I23:I31" r:id="rId4" display="\\DataSet\\TL_DataSet\\FxRates_GSFile\\" xr:uid="{57CD682C-3C14-436B-ADDE-9A80258650CD}"/>
+    <hyperlink ref="D32:D34" r:id="rId5" display="\\DataSet\\TL_DataSet\\FxRates_GSFile\\" xr:uid="{202A1715-BE83-4EB7-A90F-52978138A4F3}"/>
+    <hyperlink ref="D35:D36" r:id="rId6" display="\\DataSet\\TL_DataSet\\FxRates_GSFile\\" xr:uid="{9840F825-8637-4C41-AA65-6AF3ECBC53D3}"/>
+    <hyperlink ref="I35:I36" r:id="rId7" display="\\DataSet\\TL_DataSet\\FxRates_GSFile\\" xr:uid="{E6DF1C66-E06C-4508-BF64-80E6763D6FB9}"/>
+    <hyperlink ref="I32:I34" r:id="rId8" display="\\DataSet\\TL_DataSet\\FxRates_GSFile\\" xr:uid="{5D520F54-CC93-417A-ADE8-C492B5E5E28A}"/>
+    <hyperlink ref="I21:I29" r:id="rId9" display="\\DataSet\\TL_DataSet\\FxRates_GSFile\\" xr:uid="{47A9315B-DFC8-4430-A45E-9D03C065A594}"/>
+    <hyperlink ref="C2" r:id="rId10" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{DC17FF84-1D37-4112-BF5D-BCB4C73CD0FB}"/>
+    <hyperlink ref="D2" r:id="rId11" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{7887B602-EE56-45AE-936D-8A968AF005AA}"/>
+    <hyperlink ref="I2" r:id="rId12" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{883636BB-DB43-4D2E-AC6F-B249FF19C9EB}"/>
+    <hyperlink ref="C3" r:id="rId13" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{52EFE070-5816-4737-AB21-85096BEC8477}"/>
+    <hyperlink ref="D3:D7" r:id="rId14" display="\\DataSet\\TL_DataSet\\FxRates_GSFile\\" xr:uid="{1C2361F4-1B13-456E-9BA3-E3D8B7F812A7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7892,7 +7980,7 @@
         <v>480</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>143</v>
@@ -8252,40 +8340,40 @@
         <v>115</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>1026</v>
+      </c>
+      <c r="C11" s="9" t="s">
         <v>1027</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="D11" s="6" t="s">
         <v>1028</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="E11" s="5" t="s">
         <v>1029</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="F11" s="5" t="s">
         <v>1030</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="G11" s="5" t="s">
         <v>1031</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="H11" s="5" t="s">
         <v>1032</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="I11" s="9" t="s">
+        <v>1027</v>
+      </c>
+      <c r="J11" s="5" t="s">
         <v>1033</v>
       </c>
-      <c r="I11" s="9" t="s">
-        <v>1028</v>
-      </c>
-      <c r="J11" s="5" t="s">
+      <c r="K11" s="5" t="s">
         <v>1034</v>
       </c>
-      <c r="K11" s="5" t="s">
+      <c r="L11" s="5" t="s">
         <v>1035</v>
       </c>
-      <c r="L11" s="5" t="s">
-        <v>1036</v>
-      </c>
       <c r="M11" s="5" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -8293,40 +8381,40 @@
         <v>117</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>1036</v>
+      </c>
+      <c r="C12" s="9" t="s">
         <v>1037</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="D12" s="6" t="s">
         <v>1038</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="E12" s="5" t="s">
         <v>1039</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="F12" s="5" t="s">
         <v>1040</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="G12" s="5" t="s">
         <v>1041</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="H12" s="5" t="s">
         <v>1042</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="I12" s="9" t="s">
+        <v>1037</v>
+      </c>
+      <c r="J12" s="5" t="s">
         <v>1043</v>
       </c>
-      <c r="I12" s="9" t="s">
-        <v>1038</v>
-      </c>
-      <c r="J12" s="5" t="s">
+      <c r="K12" s="5" t="s">
         <v>1044</v>
       </c>
-      <c r="K12" s="5" t="s">
+      <c r="L12" s="5" t="s">
         <v>1045</v>
       </c>
-      <c r="L12" s="5" t="s">
-        <v>1046</v>
-      </c>
       <c r="M12" s="5" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -8689,40 +8777,40 @@
         <v>419</v>
       </c>
       <c r="B22" s="5" t="s">
+        <v>1066</v>
+      </c>
+      <c r="C22" s="9" t="s">
         <v>1067</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="D22" s="6" t="s">
+        <v>1108</v>
+      </c>
+      <c r="E22" s="5" t="s">
         <v>1068</v>
       </c>
-      <c r="D22" s="6" t="s">
-        <v>1109</v>
-      </c>
-      <c r="E22" s="5" t="s">
+      <c r="F22" s="5" t="s">
         <v>1069</v>
       </c>
-      <c r="F22" s="5" t="s">
+      <c r="G22" s="5" t="s">
         <v>1070</v>
       </c>
-      <c r="G22" s="5" t="s">
+      <c r="H22" s="5" t="s">
         <v>1071</v>
       </c>
-      <c r="H22" s="5" t="s">
+      <c r="I22" s="9" t="s">
+        <v>1067</v>
+      </c>
+      <c r="J22" s="5" t="s">
         <v>1072</v>
       </c>
-      <c r="I22" s="9" t="s">
-        <v>1068</v>
-      </c>
-      <c r="J22" s="5" t="s">
+      <c r="K22" s="5" t="s">
         <v>1073</v>
       </c>
-      <c r="K22" s="5" t="s">
+      <c r="L22" s="5" t="s">
         <v>1074</v>
       </c>
-      <c r="L22" s="5" t="s">
-        <v>1075</v>
-      </c>
       <c r="M22" s="5" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -8736,7 +8824,7 @@
         <v>847</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>848</v>
@@ -8853,40 +8941,40 @@
         <v>458</v>
       </c>
       <c r="B26" s="5" t="s">
+        <v>981</v>
+      </c>
+      <c r="C26" s="9" t="s">
         <v>982</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="D26" s="6" t="s">
         <v>983</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="E26" s="5" t="s">
         <v>984</v>
       </c>
-      <c r="E26" s="5" t="s">
+      <c r="F26" s="5" t="s">
         <v>985</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="G26" s="5" t="s">
         <v>986</v>
       </c>
-      <c r="G26" s="5" t="s">
+      <c r="H26" s="5" t="s">
         <v>987</v>
       </c>
-      <c r="H26" s="5" t="s">
+      <c r="I26" s="9" t="s">
+        <v>982</v>
+      </c>
+      <c r="J26" s="5" t="s">
         <v>988</v>
       </c>
-      <c r="I26" s="9" t="s">
-        <v>983</v>
-      </c>
-      <c r="J26" s="5" t="s">
+      <c r="K26" s="5" t="s">
         <v>989</v>
       </c>
-      <c r="K26" s="5" t="s">
+      <c r="L26" s="5" t="s">
         <v>990</v>
       </c>
-      <c r="L26" s="5" t="s">
-        <v>991</v>
-      </c>
       <c r="M26" s="5" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -8894,40 +8982,40 @@
         <v>468</v>
       </c>
       <c r="B27" s="5" t="s">
+        <v>991</v>
+      </c>
+      <c r="C27" s="9" t="s">
         <v>992</v>
       </c>
-      <c r="C27" s="9" t="s">
+      <c r="D27" s="6" t="s">
         <v>993</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="E27" s="5" t="s">
         <v>994</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="F27" s="5" t="s">
         <v>995</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="G27" s="5" t="s">
         <v>996</v>
       </c>
-      <c r="G27" s="5" t="s">
+      <c r="H27" s="5" t="s">
         <v>997</v>
       </c>
-      <c r="H27" s="5" t="s">
+      <c r="I27" s="9" t="s">
+        <v>992</v>
+      </c>
+      <c r="J27" s="5" t="s">
         <v>998</v>
       </c>
-      <c r="I27" s="9" t="s">
-        <v>993</v>
-      </c>
-      <c r="J27" s="5" t="s">
+      <c r="K27" s="5" t="s">
         <v>999</v>
       </c>
-      <c r="K27" s="5" t="s">
+      <c r="L27" s="5" t="s">
         <v>1000</v>
       </c>
-      <c r="L27" s="5" t="s">
-        <v>1001</v>
-      </c>
       <c r="M27" s="5" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -8935,40 +9023,40 @@
         <v>593</v>
       </c>
       <c r="B28" s="5" t="s">
+        <v>1001</v>
+      </c>
+      <c r="C28" s="9" t="s">
         <v>1002</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="D28" s="6" t="s">
         <v>1003</v>
       </c>
-      <c r="D28" s="6" t="s">
+      <c r="E28" s="5" t="s">
         <v>1004</v>
       </c>
-      <c r="E28" s="5" t="s">
+      <c r="F28" s="5" t="s">
         <v>1005</v>
       </c>
-      <c r="F28" s="5" t="s">
+      <c r="G28" s="5" t="s">
         <v>1006</v>
       </c>
-      <c r="G28" s="5" t="s">
+      <c r="H28" s="5" t="s">
         <v>1007</v>
       </c>
-      <c r="H28" s="5" t="s">
+      <c r="I28" s="9" t="s">
+        <v>1002</v>
+      </c>
+      <c r="J28" s="5" t="s">
         <v>1008</v>
       </c>
-      <c r="I28" s="9" t="s">
-        <v>1003</v>
-      </c>
-      <c r="J28" s="5" t="s">
+      <c r="K28" s="5" t="s">
         <v>1009</v>
       </c>
-      <c r="K28" s="5" t="s">
+      <c r="L28" s="5" t="s">
         <v>1010</v>
       </c>
-      <c r="L28" s="5" t="s">
-        <v>1011</v>
-      </c>
       <c r="M28" s="5" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -8976,40 +9064,40 @@
         <v>602</v>
       </c>
       <c r="B29" s="5" t="s">
+        <v>1046</v>
+      </c>
+      <c r="C29" s="9" t="s">
         <v>1047</v>
       </c>
-      <c r="C29" s="9" t="s">
+      <c r="D29" s="6" t="s">
         <v>1048</v>
       </c>
-      <c r="D29" s="6" t="s">
+      <c r="E29" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="E29" s="5" t="s">
+      <c r="F29" s="5" t="s">
         <v>1050</v>
       </c>
-      <c r="F29" s="5" t="s">
+      <c r="G29" s="5" t="s">
         <v>1051</v>
       </c>
-      <c r="G29" s="5" t="s">
+      <c r="H29" s="5" t="s">
         <v>1052</v>
       </c>
-      <c r="H29" s="5" t="s">
+      <c r="I29" s="9" t="s">
+        <v>1047</v>
+      </c>
+      <c r="J29" s="5" t="s">
         <v>1053</v>
       </c>
-      <c r="I29" s="9" t="s">
-        <v>1048</v>
-      </c>
-      <c r="J29" s="5" t="s">
+      <c r="K29" s="5" t="s">
         <v>1054</v>
       </c>
-      <c r="K29" s="5" t="s">
+      <c r="L29" s="5" t="s">
         <v>1055</v>
       </c>
-      <c r="L29" s="5" t="s">
-        <v>1056</v>
-      </c>
       <c r="M29" s="5" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -9017,40 +9105,40 @@
         <v>611</v>
       </c>
       <c r="B30" s="5" t="s">
+        <v>1056</v>
+      </c>
+      <c r="C30" s="9" t="s">
         <v>1057</v>
       </c>
-      <c r="C30" s="9" t="s">
+      <c r="D30" s="6" t="s">
         <v>1058</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="E30" s="5" t="s">
         <v>1059</v>
       </c>
-      <c r="E30" s="5" t="s">
+      <c r="F30" s="5" t="s">
         <v>1060</v>
       </c>
-      <c r="F30" s="5" t="s">
+      <c r="G30" s="5" t="s">
         <v>1061</v>
       </c>
-      <c r="G30" s="5" t="s">
+      <c r="H30" s="5" t="s">
         <v>1062</v>
       </c>
-      <c r="H30" s="5" t="s">
+      <c r="I30" s="9" t="s">
+        <v>1057</v>
+      </c>
+      <c r="J30" s="5" t="s">
         <v>1063</v>
       </c>
-      <c r="I30" s="9" t="s">
-        <v>1058</v>
-      </c>
-      <c r="J30" s="5" t="s">
+      <c r="K30" s="5" t="s">
         <v>1064</v>
       </c>
-      <c r="K30" s="5" t="s">
+      <c r="L30" s="5" t="s">
         <v>1065</v>
       </c>
-      <c r="L30" s="5" t="s">
-        <v>1066</v>
-      </c>
       <c r="M30" s="5" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="45" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
GDE-7246 initial fixes for TLBASE38
</commit_message>
<xml_diff>
--- a/DataSet/Integration_DataSet/TL/TL_Data_Set_AU.xlsx
+++ b/DataSet/Integration_DataSet/TL/TL_Data_Set_AU.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\Integration_DataSet\TL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5B28F4F-D2C3-4256-8996-AE695C404F9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB0EF48A-0C31-4197-96E2-E7460A81507F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BaseRate_Fields" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1436" uniqueCount="1120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1437" uniqueCount="1120">
   <si>
     <t>rowid</t>
   </si>
@@ -2933,9 +2933,6 @@
   </si>
   <si>
     <t>TL_BASE_38</t>
-  </si>
-  <si>
-    <t>\DataSet\TL_DataSet\BaseRates_GSFile\TL_BASE_38_Files\</t>
   </si>
   <si>
     <t>FINASTRA_CCB_BASERATE_SY_GROUP99_BASE38.csv</t>
@@ -3440,6 +3437,9 @@
   </si>
   <si>
     <t>Holidays_Banks_20200127_1.xlsx,Holidays_Banks_20200127_2.xlsx,Holidays_Banks_20200127_1.csv,Holidays_Banks_20200127_2.csv,Holidays_Misc_20200127.xlsx</t>
+  </si>
+  <si>
+    <t>\DataSet\Integration_DataSet\TL\BaseRates_GSFile\AU\TL_BASE_38_Files\</t>
   </si>
 </sst>
 </file>
@@ -4392,29 +4392,29 @@
   </sheetPr>
   <dimension ref="A1:N42"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="65.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="53.44140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="21.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="41.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="65.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="33.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="38.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="44.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="41.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="65.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="53.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="41.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="65.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="33.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="38.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="44.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="41.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="34.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4422,7 +4422,7 @@
         <v>17</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>1</v>
@@ -4458,7 +4458,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -4466,10 +4466,10 @@
         <v>11</v>
       </c>
       <c r="C2" s="9" t="s">
+        <v>1111</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>1112</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>1113</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>94</v>
@@ -4484,7 +4484,7 @@
         <v>18</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>21</v>
@@ -4499,7 +4499,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>22</v>
       </c>
@@ -4538,7 +4538,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>36</v>
       </c>
@@ -4577,7 +4577,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>43</v>
       </c>
@@ -4616,7 +4616,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>49</v>
       </c>
@@ -4655,7 +4655,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>57</v>
       </c>
@@ -4694,7 +4694,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>64</v>
       </c>
@@ -4733,7 +4733,7 @@
         <v>713</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>96</v>
       </c>
@@ -4772,7 +4772,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>103</v>
       </c>
@@ -4781,7 +4781,7 @@
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="9" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>105</v>
@@ -4796,7 +4796,7 @@
         <v>108</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="J10" s="5" t="s">
         <v>109</v>
@@ -4811,7 +4811,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>111</v>
       </c>
@@ -4850,7 +4850,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>113</v>
       </c>
@@ -4889,7 +4889,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>115</v>
       </c>
@@ -4928,7 +4928,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>117</v>
       </c>
@@ -4967,7 +4967,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>119</v>
       </c>
@@ -5006,7 +5006,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>146</v>
       </c>
@@ -5045,7 +5045,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>333</v>
       </c>
@@ -5084,85 +5084,85 @@
         <v>927</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>343</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="9" t="s">
+        <v>1073</v>
+      </c>
+      <c r="E18" s="5" t="s">
         <v>1074</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="F18" s="5" t="s">
         <v>1075</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="G18" s="5" t="s">
         <v>1076</v>
       </c>
-      <c r="G18" s="5" t="s">
+      <c r="H18" s="5" t="s">
         <v>1077</v>
       </c>
-      <c r="H18" s="5" t="s">
+      <c r="I18" s="9" t="s">
+        <v>1073</v>
+      </c>
+      <c r="J18" s="5" t="s">
         <v>1078</v>
       </c>
-      <c r="I18" s="9" t="s">
-        <v>1074</v>
-      </c>
-      <c r="J18" s="5" t="s">
+      <c r="K18" s="5" t="s">
         <v>1079</v>
       </c>
-      <c r="K18" s="5" t="s">
+      <c r="L18" s="5" t="s">
         <v>1080</v>
       </c>
-      <c r="L18" s="5" t="s">
+      <c r="M18" s="5" t="s">
         <v>1081</v>
       </c>
-      <c r="M18" s="5" t="s">
-        <v>1082</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>353</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="9" t="s">
+        <v>1014</v>
+      </c>
+      <c r="E19" s="5" t="s">
         <v>1015</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="F19" s="5" t="s">
         <v>1016</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="G19" s="5" t="s">
         <v>1017</v>
       </c>
-      <c r="G19" s="5" t="s">
+      <c r="H19" s="5" t="s">
         <v>1018</v>
       </c>
-      <c r="H19" s="5" t="s">
+      <c r="I19" s="9" t="s">
+        <v>1014</v>
+      </c>
+      <c r="J19" s="5" t="s">
         <v>1019</v>
       </c>
-      <c r="I19" s="9" t="s">
-        <v>1015</v>
-      </c>
-      <c r="J19" s="5" t="s">
+      <c r="K19" s="5" t="s">
         <v>1020</v>
       </c>
-      <c r="K19" s="5" t="s">
+      <c r="L19" s="5" t="s">
         <v>1021</v>
       </c>
-      <c r="L19" s="5" t="s">
+      <c r="M19" s="5" t="s">
         <v>1022</v>
       </c>
-      <c r="M19" s="5" t="s">
-        <v>1023</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>169</v>
       </c>
@@ -5201,7 +5201,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>210</v>
       </c>
@@ -5240,7 +5240,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>230</v>
       </c>
@@ -5279,7 +5279,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>232</v>
       </c>
@@ -5318,7 +5318,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
         <v>428</v>
       </c>
@@ -5357,7 +5357,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>438</v>
       </c>
@@ -5396,7 +5396,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
         <v>448</v>
       </c>
@@ -5435,46 +5435,46 @@
         <v>708</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>458</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="9" t="s">
+        <v>1083</v>
+      </c>
+      <c r="E27" s="5" t="s">
         <v>1084</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="F27" s="5" t="s">
         <v>1085</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="G27" s="5" t="s">
         <v>1086</v>
       </c>
-      <c r="G27" s="5" t="s">
+      <c r="H27" s="5" t="s">
         <v>1087</v>
       </c>
-      <c r="H27" s="5" t="s">
+      <c r="I27" s="9" t="s">
+        <v>1083</v>
+      </c>
+      <c r="J27" s="5" t="s">
         <v>1088</v>
       </c>
-      <c r="I27" s="9" t="s">
-        <v>1084</v>
-      </c>
-      <c r="J27" s="5" t="s">
+      <c r="K27" s="5" t="s">
         <v>1089</v>
       </c>
-      <c r="K27" s="5" t="s">
+      <c r="L27" s="5" t="s">
         <v>1090</v>
       </c>
-      <c r="L27" s="5" t="s">
+      <c r="M27" s="5" t="s">
         <v>1091</v>
       </c>
-      <c r="M27" s="5" t="s">
-        <v>1092</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
         <v>468</v>
       </c>
@@ -5513,7 +5513,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
         <v>592</v>
       </c>
@@ -5552,7 +5552,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
         <v>610</v>
       </c>
@@ -5591,7 +5591,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
         <v>731</v>
       </c>
@@ -5630,7 +5630,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>619</v>
       </c>
@@ -5669,7 +5669,7 @@
         <v>937</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
         <v>628</v>
       </c>
@@ -5708,7 +5708,7 @@
         <v>947</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
         <v>546</v>
       </c>
@@ -5747,7 +5747,7 @@
         <v>957</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
         <v>555</v>
       </c>
@@ -5786,85 +5786,87 @@
         <v>967</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
         <v>968</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>969</v>
       </c>
-      <c r="C36" s="5"/>
+      <c r="C36" s="9" t="s">
+        <v>1111</v>
+      </c>
       <c r="D36" s="9" t="s">
+        <v>1119</v>
+      </c>
+      <c r="E36" s="6" t="s">
         <v>970</v>
       </c>
-      <c r="E36" s="6" t="s">
+      <c r="F36" s="5" t="s">
         <v>971</v>
       </c>
-      <c r="F36" s="5" t="s">
+      <c r="G36" s="5" t="s">
         <v>972</v>
       </c>
-      <c r="G36" s="5" t="s">
+      <c r="H36" s="5" t="s">
         <v>973</v>
       </c>
-      <c r="H36" s="5" t="s">
+      <c r="I36" s="9" t="s">
+        <v>1119</v>
+      </c>
+      <c r="J36" s="5" t="s">
         <v>974</v>
       </c>
-      <c r="I36" s="9" t="s">
-        <v>970</v>
-      </c>
-      <c r="J36" s="5" t="s">
+      <c r="K36" s="5" t="s">
         <v>975</v>
       </c>
-      <c r="K36" s="5" t="s">
+      <c r="L36" s="5" t="s">
         <v>976</v>
       </c>
-      <c r="L36" s="5" t="s">
+      <c r="M36" s="5" t="s">
         <v>977</v>
       </c>
-      <c r="M36" s="5" t="s">
-        <v>978</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
+        <v>1092</v>
+      </c>
+      <c r="B37" s="5" t="s">
         <v>1093</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>1094</v>
       </c>
       <c r="C37" s="5"/>
       <c r="D37" s="9" t="s">
+        <v>1094</v>
+      </c>
+      <c r="E37" s="5" t="s">
         <v>1095</v>
       </c>
-      <c r="E37" s="5" t="s">
+      <c r="F37" s="5" t="s">
         <v>1096</v>
       </c>
-      <c r="F37" s="5" t="s">
+      <c r="G37" s="5" t="s">
         <v>1097</v>
       </c>
-      <c r="G37" s="5" t="s">
+      <c r="H37" s="5" t="s">
         <v>1098</v>
       </c>
-      <c r="H37" s="5" t="s">
+      <c r="I37" s="9" t="s">
+        <v>1094</v>
+      </c>
+      <c r="J37" s="5" t="s">
         <v>1099</v>
       </c>
-      <c r="I37" s="9" t="s">
-        <v>1095</v>
-      </c>
-      <c r="J37" s="5" t="s">
+      <c r="K37" s="5" t="s">
         <v>1100</v>
       </c>
-      <c r="K37" s="5" t="s">
+      <c r="L37" s="5" t="s">
         <v>1101</v>
       </c>
-      <c r="L37" s="5" t="s">
+      <c r="M37" s="5" t="s">
         <v>1102</v>
       </c>
-      <c r="M37" s="5" t="s">
-        <v>1103</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
         <v>735</v>
       </c>
@@ -5903,7 +5905,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
         <v>768</v>
       </c>
@@ -5945,7 +5947,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
         <v>781</v>
       </c>
@@ -5985,7 +5987,7 @@
       </c>
       <c r="N40" s="5"/>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="11" t="s">
         <v>746</v>
       </c>
@@ -6024,7 +6026,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
         <v>757</v>
       </c>
@@ -6112,18 +6114,19 @@
     <hyperlink ref="I34" r:id="rId45" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{2D2A1FFD-A1CF-4898-89AC-366D631A4AE9}"/>
     <hyperlink ref="D35" r:id="rId46" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{17087BD1-D3E5-4AA0-932F-EF6585B39DAD}"/>
     <hyperlink ref="I35" r:id="rId47" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{C2EE35C7-B69C-4CFE-A9C7-8147CC81F993}"/>
-    <hyperlink ref="D36" r:id="rId48" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{148BD777-7D4F-4D9C-BE58-657825E990DC}"/>
-    <hyperlink ref="I36" r:id="rId49" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{E8A6541D-C266-4297-BE02-9DB617BCE6E9}"/>
-    <hyperlink ref="D19" r:id="rId50" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{6E642722-BFB2-445A-9B7B-53C0A272604A}"/>
-    <hyperlink ref="I19" r:id="rId51" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{0C1BBEBF-D848-4240-A469-BF25D2FF4893}"/>
-    <hyperlink ref="D18" r:id="rId52" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{B37D5DAB-9BBF-4734-A8F3-C544C4DA476C}"/>
-    <hyperlink ref="I18" r:id="rId53" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{527EEE72-0B11-40B4-96A9-24D97A6864B7}"/>
-    <hyperlink ref="D27" r:id="rId54" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{CD10DEA0-475B-4977-B943-77B7CACFA7CC}"/>
-    <hyperlink ref="I27" r:id="rId55" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{748072CF-65E5-4932-9033-FEA7A8832219}"/>
-    <hyperlink ref="D37" r:id="rId56" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{2016704E-36EB-49AB-A36D-01EEB9E33415}"/>
-    <hyperlink ref="I37" r:id="rId57" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{111E8F37-E507-4086-A947-F3F427867099}"/>
-    <hyperlink ref="C2" r:id="rId58" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{D0DABB52-96E5-41AF-9FAC-9921DADC3D95}"/>
-    <hyperlink ref="I2" r:id="rId59" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{432E7AC4-2F08-431B-AE35-E60F0B5F2AC0}"/>
+    <hyperlink ref="D19" r:id="rId48" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{6E642722-BFB2-445A-9B7B-53C0A272604A}"/>
+    <hyperlink ref="I19" r:id="rId49" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{0C1BBEBF-D848-4240-A469-BF25D2FF4893}"/>
+    <hyperlink ref="D18" r:id="rId50" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{B37D5DAB-9BBF-4734-A8F3-C544C4DA476C}"/>
+    <hyperlink ref="I18" r:id="rId51" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{527EEE72-0B11-40B4-96A9-24D97A6864B7}"/>
+    <hyperlink ref="D27" r:id="rId52" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{CD10DEA0-475B-4977-B943-77B7CACFA7CC}"/>
+    <hyperlink ref="I27" r:id="rId53" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{748072CF-65E5-4932-9033-FEA7A8832219}"/>
+    <hyperlink ref="D37" r:id="rId54" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{2016704E-36EB-49AB-A36D-01EEB9E33415}"/>
+    <hyperlink ref="I37" r:id="rId55" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{111E8F37-E507-4086-A947-F3F427867099}"/>
+    <hyperlink ref="C2" r:id="rId56" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{D0DABB52-96E5-41AF-9FAC-9921DADC3D95}"/>
+    <hyperlink ref="I2" r:id="rId57" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{432E7AC4-2F08-431B-AE35-E60F0B5F2AC0}"/>
+    <hyperlink ref="C36" r:id="rId58" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{622B310B-FA93-4EF4-AD71-A576AE0B94DD}"/>
+    <hyperlink ref="D36" r:id="rId59" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{EAF866E3-EEA3-45C8-9534-A65564C4AB32}"/>
+    <hyperlink ref="I36" r:id="rId60" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{73FA6ECE-F042-4D99-8A8C-B55F2E410A3E}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.3" right="0.3" top="0.61" bottom="0.37" header="0.1" footer="0.1"/>
@@ -6144,26 +6147,26 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="66.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="44.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="43.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="61.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="45.88671875" customWidth="1"/>
-    <col min="11" max="11" width="40.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="40.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="66.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="61.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="45.85546875" customWidth="1"/>
+    <col min="11" max="11" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -6171,7 +6174,7 @@
         <v>17</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>1</v>
@@ -6210,10 +6213,10 @@
         <v>121</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>1104</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+        <v>1103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -6221,10 +6224,10 @@
         <v>44</v>
       </c>
       <c r="C2" s="9" t="s">
+        <v>1113</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>1114</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>1115</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>132</v>
@@ -6239,7 +6242,7 @@
         <v>48</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>129</v>
@@ -6260,7 +6263,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>22</v>
       </c>
@@ -6305,7 +6308,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>36</v>
       </c>
@@ -6350,7 +6353,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>43</v>
       </c>
@@ -6395,7 +6398,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>49</v>
       </c>
@@ -6440,7 +6443,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>57</v>
       </c>
@@ -6485,7 +6488,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>64</v>
       </c>
@@ -6497,7 +6500,7 @@
         <v>130</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>260</v>
@@ -6530,7 +6533,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>96</v>
       </c>
@@ -6542,7 +6545,7 @@
         <v>130</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>268</v>
@@ -6575,7 +6578,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>103</v>
       </c>
@@ -6587,7 +6590,7 @@
         <v>130</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>276</v>
@@ -6620,7 +6623,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>111</v>
       </c>
@@ -6632,7 +6635,7 @@
         <v>130</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>284</v>
@@ -6665,7 +6668,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>113</v>
       </c>
@@ -6677,7 +6680,7 @@
         <v>130</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>292</v>
@@ -6710,7 +6713,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>115</v>
       </c>
@@ -6722,7 +6725,7 @@
         <v>130</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>300</v>
@@ -6755,7 +6758,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>117</v>
       </c>
@@ -6767,7 +6770,7 @@
         <v>130</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>308</v>
@@ -6800,7 +6803,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>119</v>
       </c>
@@ -6845,7 +6848,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>146</v>
       </c>
@@ -6890,7 +6893,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>333</v>
       </c>
@@ -6935,7 +6938,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>343</v>
       </c>
@@ -6980,7 +6983,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>353</v>
       </c>
@@ -7025,7 +7028,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>169</v>
       </c>
@@ -7070,10 +7073,10 @@
         <v>243</v>
       </c>
       <c r="P20" s="5" t="s">
-        <v>1105</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+        <v>1104</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>210</v>
       </c>
@@ -7118,7 +7121,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>230</v>
       </c>
@@ -7163,7 +7166,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>232</v>
       </c>
@@ -7208,7 +7211,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>399</v>
       </c>
@@ -7253,7 +7256,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>409</v>
       </c>
@@ -7298,7 +7301,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="26" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>419</v>
       </c>
@@ -7343,7 +7346,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="27" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>428</v>
       </c>
@@ -7388,7 +7391,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>438</v>
       </c>
@@ -7433,7 +7436,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>448</v>
       </c>
@@ -7478,7 +7481,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>458</v>
       </c>
@@ -7523,7 +7526,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="31" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>468</v>
       </c>
@@ -7568,7 +7571,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="32" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>592</v>
       </c>
@@ -7613,7 +7616,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
         <v>601</v>
       </c>
@@ -7658,7 +7661,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>610</v>
       </c>
@@ -7703,7 +7706,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>619</v>
       </c>
@@ -7748,7 +7751,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
         <v>628</v>
       </c>
@@ -7820,28 +7823,28 @@
   </sheetPr>
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="67.88671875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="67.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="94" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="42.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="36.33203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="75.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="37.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="42.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="36.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="75.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="37.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="40" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="60.33203125" customWidth="1"/>
+    <col min="12" max="12" width="60.28515625" customWidth="1"/>
     <col min="13" max="13" width="45" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -7882,7 +7885,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -7890,10 +7893,10 @@
         <v>140</v>
       </c>
       <c r="C2" s="9" t="s">
+        <v>1115</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>1116</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>1117</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>143</v>
@@ -7905,7 +7908,7 @@
         <v>145</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>166</v>
@@ -7920,7 +7923,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>22</v>
       </c>
@@ -7961,7 +7964,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>36</v>
       </c>
@@ -8002,7 +8005,7 @@
         <v>880</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>43</v>
       </c>
@@ -8043,7 +8046,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>64</v>
       </c>
@@ -8084,7 +8087,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>96</v>
       </c>
@@ -8092,10 +8095,10 @@
         <v>802</v>
       </c>
       <c r="C7" s="9" t="s">
+        <v>1117</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>1118</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>1119</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>803</v>
@@ -8110,7 +8113,7 @@
         <v>826</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="J7" s="5" t="s">
         <v>806</v>
@@ -8125,7 +8128,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>103</v>
       </c>
@@ -8166,7 +8169,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>111</v>
       </c>
@@ -8207,7 +8210,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>113</v>
       </c>
@@ -8248,89 +8251,89 @@
         <v>495</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>115</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>1023</v>
+      </c>
+      <c r="C11" s="9" t="s">
         <v>1024</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="D11" s="6" t="s">
         <v>1025</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="E11" s="5" t="s">
         <v>1026</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="F11" s="5" t="s">
         <v>1027</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="G11" s="5" t="s">
         <v>1028</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="H11" s="5" t="s">
         <v>1029</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="I11" s="9" t="s">
+        <v>1024</v>
+      </c>
+      <c r="J11" s="5" t="s">
         <v>1030</v>
       </c>
-      <c r="I11" s="9" t="s">
-        <v>1025</v>
-      </c>
-      <c r="J11" s="5" t="s">
+      <c r="K11" s="5" t="s">
         <v>1031</v>
       </c>
-      <c r="K11" s="5" t="s">
+      <c r="L11" s="5" t="s">
         <v>1032</v>
       </c>
-      <c r="L11" s="5" t="s">
-        <v>1033</v>
-      </c>
       <c r="M11" s="5" t="s">
-        <v>1033</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>1032</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>117</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>1033</v>
+      </c>
+      <c r="C12" s="9" t="s">
         <v>1034</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="D12" s="6" t="s">
         <v>1035</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="E12" s="5" t="s">
         <v>1036</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="F12" s="5" t="s">
         <v>1037</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="G12" s="5" t="s">
         <v>1038</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="H12" s="5" t="s">
         <v>1039</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="I12" s="9" t="s">
+        <v>1034</v>
+      </c>
+      <c r="J12" s="5" t="s">
         <v>1040</v>
       </c>
-      <c r="I12" s="9" t="s">
-        <v>1035</v>
-      </c>
-      <c r="J12" s="5" t="s">
+      <c r="K12" s="5" t="s">
         <v>1041</v>
       </c>
-      <c r="K12" s="5" t="s">
+      <c r="L12" s="5" t="s">
         <v>1042</v>
       </c>
-      <c r="L12" s="5" t="s">
-        <v>1043</v>
-      </c>
       <c r="M12" s="5" t="s">
-        <v>1043</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>119</v>
       </c>
@@ -8371,7 +8374,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>146</v>
       </c>
@@ -8410,7 +8413,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>504</v>
       </c>
@@ -8449,7 +8452,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>513</v>
       </c>
@@ -8488,7 +8491,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>17</v>
       </c>
@@ -8529,7 +8532,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>18</v>
       </c>
@@ -8568,7 +8571,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>19</v>
       </c>
@@ -8607,7 +8610,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>210</v>
       </c>
@@ -8646,7 +8649,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>230</v>
       </c>
@@ -8685,48 +8688,48 @@
         <v>591</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>419</v>
       </c>
       <c r="B22" s="5" t="s">
+        <v>1063</v>
+      </c>
+      <c r="C22" s="9" t="s">
         <v>1064</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="D22" s="6" t="s">
+        <v>1105</v>
+      </c>
+      <c r="E22" s="5" t="s">
         <v>1065</v>
       </c>
-      <c r="D22" s="6" t="s">
-        <v>1106</v>
-      </c>
-      <c r="E22" s="5" t="s">
+      <c r="F22" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="F22" s="5" t="s">
+      <c r="G22" s="5" t="s">
         <v>1067</v>
       </c>
-      <c r="G22" s="5" t="s">
+      <c r="H22" s="5" t="s">
         <v>1068</v>
       </c>
-      <c r="H22" s="5" t="s">
+      <c r="I22" s="9" t="s">
+        <v>1064</v>
+      </c>
+      <c r="J22" s="5" t="s">
         <v>1069</v>
       </c>
-      <c r="I22" s="9" t="s">
-        <v>1065</v>
-      </c>
-      <c r="J22" s="5" t="s">
+      <c r="K22" s="5" t="s">
         <v>1070</v>
       </c>
-      <c r="K22" s="5" t="s">
+      <c r="L22" s="5" t="s">
         <v>1071</v>
       </c>
-      <c r="L22" s="5" t="s">
-        <v>1072</v>
-      </c>
       <c r="M22" s="5" t="s">
-        <v>1072</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>1071</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>428</v>
       </c>
@@ -8737,7 +8740,7 @@
         <v>844</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>845</v>
@@ -8767,7 +8770,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>438</v>
       </c>
@@ -8808,7 +8811,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>448</v>
       </c>
@@ -8849,212 +8852,212 @@
         <v>871</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>458</v>
       </c>
       <c r="B26" s="5" t="s">
+        <v>978</v>
+      </c>
+      <c r="C26" s="9" t="s">
         <v>979</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="D26" s="6" t="s">
         <v>980</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="E26" s="5" t="s">
         <v>981</v>
       </c>
-      <c r="E26" s="5" t="s">
+      <c r="F26" s="5" t="s">
         <v>982</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="G26" s="5" t="s">
         <v>983</v>
       </c>
-      <c r="G26" s="5" t="s">
+      <c r="H26" s="5" t="s">
         <v>984</v>
       </c>
-      <c r="H26" s="5" t="s">
+      <c r="I26" s="9" t="s">
+        <v>979</v>
+      </c>
+      <c r="J26" s="5" t="s">
         <v>985</v>
       </c>
-      <c r="I26" s="9" t="s">
-        <v>980</v>
-      </c>
-      <c r="J26" s="5" t="s">
+      <c r="K26" s="5" t="s">
         <v>986</v>
       </c>
-      <c r="K26" s="5" t="s">
+      <c r="L26" s="5" t="s">
         <v>987</v>
       </c>
-      <c r="L26" s="5" t="s">
-        <v>988</v>
-      </c>
       <c r="M26" s="5" t="s">
-        <v>988</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>987</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>468</v>
       </c>
       <c r="B27" s="5" t="s">
+        <v>988</v>
+      </c>
+      <c r="C27" s="9" t="s">
         <v>989</v>
       </c>
-      <c r="C27" s="9" t="s">
+      <c r="D27" s="6" t="s">
         <v>990</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="E27" s="5" t="s">
         <v>991</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="F27" s="5" t="s">
         <v>992</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="G27" s="5" t="s">
         <v>993</v>
       </c>
-      <c r="G27" s="5" t="s">
+      <c r="H27" s="5" t="s">
         <v>994</v>
       </c>
-      <c r="H27" s="5" t="s">
+      <c r="I27" s="9" t="s">
+        <v>989</v>
+      </c>
+      <c r="J27" s="5" t="s">
         <v>995</v>
       </c>
-      <c r="I27" s="9" t="s">
-        <v>990</v>
-      </c>
-      <c r="J27" s="5" t="s">
+      <c r="K27" s="5" t="s">
         <v>996</v>
       </c>
-      <c r="K27" s="5" t="s">
+      <c r="L27" s="5" t="s">
         <v>997</v>
       </c>
-      <c r="L27" s="5" t="s">
-        <v>998</v>
-      </c>
       <c r="M27" s="5" t="s">
-        <v>998</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>592</v>
       </c>
       <c r="B28" s="5" t="s">
+        <v>998</v>
+      </c>
+      <c r="C28" s="9" t="s">
         <v>999</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="D28" s="6" t="s">
         <v>1000</v>
       </c>
-      <c r="D28" s="6" t="s">
+      <c r="E28" s="5" t="s">
         <v>1001</v>
       </c>
-      <c r="E28" s="5" t="s">
+      <c r="F28" s="5" t="s">
         <v>1002</v>
       </c>
-      <c r="F28" s="5" t="s">
+      <c r="G28" s="5" t="s">
         <v>1003</v>
       </c>
-      <c r="G28" s="5" t="s">
+      <c r="H28" s="5" t="s">
         <v>1004</v>
       </c>
-      <c r="H28" s="5" t="s">
+      <c r="I28" s="9" t="s">
+        <v>999</v>
+      </c>
+      <c r="J28" s="5" t="s">
         <v>1005</v>
       </c>
-      <c r="I28" s="9" t="s">
-        <v>1000</v>
-      </c>
-      <c r="J28" s="5" t="s">
+      <c r="K28" s="5" t="s">
         <v>1006</v>
       </c>
-      <c r="K28" s="5" t="s">
+      <c r="L28" s="5" t="s">
         <v>1007</v>
       </c>
-      <c r="L28" s="5" t="s">
-        <v>1008</v>
-      </c>
       <c r="M28" s="5" t="s">
-        <v>1008</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>601</v>
       </c>
       <c r="B29" s="5" t="s">
+        <v>1043</v>
+      </c>
+      <c r="C29" s="9" t="s">
         <v>1044</v>
       </c>
-      <c r="C29" s="9" t="s">
+      <c r="D29" s="6" t="s">
         <v>1045</v>
       </c>
-      <c r="D29" s="6" t="s">
+      <c r="E29" s="5" t="s">
         <v>1046</v>
       </c>
-      <c r="E29" s="5" t="s">
+      <c r="F29" s="5" t="s">
         <v>1047</v>
       </c>
-      <c r="F29" s="5" t="s">
+      <c r="G29" s="5" t="s">
         <v>1048</v>
       </c>
-      <c r="G29" s="5" t="s">
+      <c r="H29" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H29" s="5" t="s">
+      <c r="I29" s="9" t="s">
+        <v>1044</v>
+      </c>
+      <c r="J29" s="5" t="s">
         <v>1050</v>
       </c>
-      <c r="I29" s="9" t="s">
-        <v>1045</v>
-      </c>
-      <c r="J29" s="5" t="s">
+      <c r="K29" s="5" t="s">
         <v>1051</v>
       </c>
-      <c r="K29" s="5" t="s">
+      <c r="L29" s="5" t="s">
         <v>1052</v>
       </c>
-      <c r="L29" s="5" t="s">
-        <v>1053</v>
-      </c>
       <c r="M29" s="5" t="s">
-        <v>1053</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>610</v>
       </c>
       <c r="B30" s="5" t="s">
+        <v>1053</v>
+      </c>
+      <c r="C30" s="9" t="s">
         <v>1054</v>
       </c>
-      <c r="C30" s="9" t="s">
+      <c r="D30" s="6" t="s">
         <v>1055</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="E30" s="5" t="s">
         <v>1056</v>
       </c>
-      <c r="E30" s="5" t="s">
+      <c r="F30" s="5" t="s">
         <v>1057</v>
       </c>
-      <c r="F30" s="5" t="s">
+      <c r="G30" s="5" t="s">
         <v>1058</v>
       </c>
-      <c r="G30" s="5" t="s">
+      <c r="H30" s="5" t="s">
         <v>1059</v>
       </c>
-      <c r="H30" s="5" t="s">
+      <c r="I30" s="9" t="s">
+        <v>1054</v>
+      </c>
+      <c r="J30" s="5" t="s">
         <v>1060</v>
       </c>
-      <c r="I30" s="9" t="s">
-        <v>1055</v>
-      </c>
-      <c r="J30" s="5" t="s">
+      <c r="K30" s="5" t="s">
         <v>1061</v>
       </c>
-      <c r="K30" s="5" t="s">
+      <c r="L30" s="5" t="s">
         <v>1062</v>
       </c>
-      <c r="L30" s="5" t="s">
-        <v>1063</v>
-      </c>
       <c r="M30" s="5" t="s">
-        <v>1063</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>1062</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>628</v>
       </c>
@@ -9095,7 +9098,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>546</v>
       </c>
@@ -9134,7 +9137,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>555</v>
       </c>
@@ -9213,9 +9216,9 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -9223,7 +9226,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
GDE-7307 TL_CAL_15 data and script fixes
Updated the path for InputFilePath and OutputFilePath on TL_Data_Set_AU
for TL_CAL_15
Added TL_CAL_15 folder path and added files to be used for running
Added scroll into view on Navigate Splitter through Instance Name
</commit_message>
<xml_diff>
--- a/DataSet/Integration_DataSet/TL/TL_Data_Set_AU.xlsx
+++ b/DataSet/Integration_DataSet/TL/TL_Data_Set_AU.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\Integration_DataSet\TL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02CF265A-B02D-4244-90F0-34AEB526C42E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F2B0D17-E6AD-452D-86F4-6FDFF8853547}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1510,9 +1510,6 @@
     <t>TL_CAL_15</t>
   </si>
   <si>
-    <t>\DataSet\TL_DataSet\Calendar_GSFile\TL_CAL_15_Files\</t>
-  </si>
-  <si>
     <t>INPUTJSON_TL_CAL15</t>
   </si>
   <si>
@@ -2360,9 +2357,6 @@
   </si>
   <si>
     <t>Actual_ResponseMechanism_TL_BASE_42</t>
-  </si>
-  <si>
-    <t>Holidays_Banks_20190115_1.csv,Holidays_Banks_20190115_1.xlsx,Holidays_Banks_20190115_2.csv,Holidays_Banks_20190115_2.xlsx,Holidays_Misc_20190115.xlsx</t>
   </si>
   <si>
     <t>Holidays_Banks_20190116_1.csv,Holidays_Banks_20190116_1.xlsx,Holidays_Banks_20190116_2.csv,Holidays_Banks_20190116_2.xlsx,Holidays_Misc_20190116.xlsx</t>
@@ -3479,6 +3473,12 @@
   </si>
   <si>
     <t>Holidays_Banks_20200226_1.csv,Holidays_Banks_20200226_1.xlsx,Holidays_Banks_20200226_2.csv,Holidays_Banks_20200226_2.xlsx,Holidays_Misc_20200226.xlsx</t>
+  </si>
+  <si>
+    <t>\DataSet\Integration_DataSet\TL\Calendar_GSFile\TL_CAL_15_Files\</t>
+  </si>
+  <si>
+    <t>Holidays_Banks_20200302_1.csv,Holidays_Banks_20200302_1.xlsx,Holidays_Banks_20200302_2.csv,Holidays_Banks_20200302_2.xlsx,Holidays_Misc_20200302.xlsx</t>
   </si>
 </sst>
 </file>
@@ -4461,7 +4461,7 @@
         <v>17</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>1083</v>
+        <v>1081</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>1</v>
@@ -4494,7 +4494,7 @@
         <v>154</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
@@ -4505,10 +4505,10 @@
         <v>11</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>1085</v>
+        <v>1083</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>94</v>
@@ -4523,7 +4523,7 @@
         <v>18</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>1085</v>
+        <v>1083</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>21</v>
@@ -4546,10 +4546,10 @@
         <v>23</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>1094</v>
+        <v>1092</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>95</v>
@@ -4564,7 +4564,7 @@
         <v>25</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>1094</v>
+        <v>1092</v>
       </c>
       <c r="J3" s="5" t="s">
         <v>26</v>
@@ -4587,10 +4587,10 @@
         <v>30</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>1095</v>
+        <v>1093</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>140</v>
@@ -4605,7 +4605,7 @@
         <v>33</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>1095</v>
+        <v>1093</v>
       </c>
       <c r="J4" s="5" t="s">
         <v>34</v>
@@ -4617,7 +4617,7 @@
         <v>135</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
@@ -4628,10 +4628,10 @@
         <v>37</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>1096</v>
+        <v>1094</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>153</v>
@@ -4646,7 +4646,7 @@
         <v>40</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>1096</v>
+        <v>1094</v>
       </c>
       <c r="J5" s="5" t="s">
         <v>41</v>
@@ -4669,10 +4669,10 @@
         <v>50</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>1097</v>
+        <v>1095</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>51</v>
@@ -4687,7 +4687,7 @@
         <v>54</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>1097</v>
+        <v>1095</v>
       </c>
       <c r="J6" s="5" t="s">
         <v>55</v>
@@ -4710,13 +4710,13 @@
         <v>58</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>1098</v>
+        <v>1096</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>59</v>
@@ -4728,7 +4728,7 @@
         <v>61</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>1098</v>
+        <v>1096</v>
       </c>
       <c r="J7" s="5" t="s">
         <v>62</v>
@@ -4740,7 +4740,7 @@
         <v>138</v>
       </c>
       <c r="M7" s="5" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
@@ -4751,13 +4751,13 @@
         <v>65</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>1099</v>
+        <v>1097</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>66</v>
@@ -4769,7 +4769,7 @@
         <v>68</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>1099</v>
+        <v>1097</v>
       </c>
       <c r="J8" s="5" t="s">
         <v>69</v>
@@ -4778,10 +4778,10 @@
         <v>70</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
@@ -4792,13 +4792,13 @@
         <v>97</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>1100</v>
+        <v>1098</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>98</v>
@@ -4810,7 +4810,7 @@
         <v>100</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>1100</v>
+        <v>1098</v>
       </c>
       <c r="J9" s="5" t="s">
         <v>101</v>
@@ -4819,10 +4819,10 @@
         <v>102</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="M9" s="5" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
@@ -4833,10 +4833,10 @@
         <v>104</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>1101</v>
+        <v>1099</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>105</v>
@@ -4851,7 +4851,7 @@
         <v>108</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>1101</v>
+        <v>1099</v>
       </c>
       <c r="J10" s="5" t="s">
         <v>109</v>
@@ -4860,10 +4860,10 @@
         <v>110</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="M10" s="5" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
@@ -4874,10 +4874,10 @@
         <v>156</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>1102</v>
+        <v>1100</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>112</v>
@@ -4892,7 +4892,7 @@
         <v>159</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>1102</v>
+        <v>1100</v>
       </c>
       <c r="J11" s="5" t="s">
         <v>160</v>
@@ -4915,10 +4915,10 @@
         <v>169</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>114</v>
@@ -4933,7 +4933,7 @@
         <v>191</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="J12" s="5" t="s">
         <v>196</v>
@@ -4956,10 +4956,10 @@
         <v>170</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>1105</v>
+        <v>1103</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>116</v>
@@ -4974,7 +4974,7 @@
         <v>192</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>1105</v>
+        <v>1103</v>
       </c>
       <c r="J13" s="5" t="s">
         <v>197</v>
@@ -4997,10 +4997,10 @@
         <v>171</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>1106</v>
+        <v>1104</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>118</v>
@@ -5015,7 +5015,7 @@
         <v>193</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>1106</v>
+        <v>1104</v>
       </c>
       <c r="J14" s="5" t="s">
         <v>198</v>
@@ -5038,10 +5038,10 @@
         <v>172</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>1107</v>
+        <v>1105</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>120</v>
@@ -5056,7 +5056,7 @@
         <v>194</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>1107</v>
+        <v>1105</v>
       </c>
       <c r="J15" s="5" t="s">
         <v>199</v>
@@ -5079,10 +5079,10 @@
         <v>173</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>1108</v>
+        <v>1106</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>152</v>
@@ -5097,7 +5097,7 @@
         <v>148</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>1108</v>
+        <v>1106</v>
       </c>
       <c r="J16" s="5" t="s">
         <v>149</v>
@@ -5117,40 +5117,40 @@
         <v>332</v>
       </c>
       <c r="B17" s="5" t="s">
+        <v>899</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>1082</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>1107</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>900</v>
+      </c>
+      <c r="F17" s="5" t="s">
         <v>901</v>
       </c>
-      <c r="C17" s="9" t="s">
-        <v>1084</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>1109</v>
-      </c>
-      <c r="E17" s="5" t="s">
+      <c r="G17" s="5" t="s">
         <v>902</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="H17" s="5" t="s">
         <v>903</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="I17" s="9" t="s">
+        <v>1107</v>
+      </c>
+      <c r="J17" s="5" t="s">
         <v>904</v>
       </c>
-      <c r="H17" s="5" t="s">
+      <c r="K17" s="5" t="s">
         <v>905</v>
       </c>
-      <c r="I17" s="9" t="s">
-        <v>1109</v>
-      </c>
-      <c r="J17" s="5" t="s">
+      <c r="L17" s="5" t="s">
         <v>906</v>
       </c>
-      <c r="K17" s="5" t="s">
+      <c r="M17" s="5" t="s">
         <v>907</v>
-      </c>
-      <c r="L17" s="5" t="s">
-        <v>908</v>
-      </c>
-      <c r="M17" s="5" t="s">
-        <v>909</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
@@ -5158,40 +5158,40 @@
         <v>342</v>
       </c>
       <c r="B18" s="5" t="s">
+        <v>1046</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>1082</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>1108</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>1047</v>
+      </c>
+      <c r="F18" s="5" t="s">
         <v>1048</v>
       </c>
-      <c r="C18" s="9" t="s">
-        <v>1084</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>1110</v>
-      </c>
-      <c r="E18" s="5" t="s">
+      <c r="G18" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="H18" s="5" t="s">
         <v>1050</v>
       </c>
-      <c r="G18" s="5" t="s">
+      <c r="I18" s="9" t="s">
+        <v>1108</v>
+      </c>
+      <c r="J18" s="5" t="s">
         <v>1051</v>
       </c>
-      <c r="H18" s="5" t="s">
+      <c r="K18" s="5" t="s">
         <v>1052</v>
       </c>
-      <c r="I18" s="9" t="s">
-        <v>1110</v>
-      </c>
-      <c r="J18" s="5" t="s">
+      <c r="L18" s="5" t="s">
         <v>1053</v>
       </c>
-      <c r="K18" s="5" t="s">
+      <c r="M18" s="5" t="s">
         <v>1054</v>
-      </c>
-      <c r="L18" s="5" t="s">
-        <v>1055</v>
-      </c>
-      <c r="M18" s="5" t="s">
-        <v>1056</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
@@ -5199,40 +5199,40 @@
         <v>352</v>
       </c>
       <c r="B19" s="5" t="s">
+        <v>988</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>1082</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>1109</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>989</v>
+      </c>
+      <c r="F19" s="5" t="s">
         <v>990</v>
       </c>
-      <c r="C19" s="9" t="s">
-        <v>1084</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>1111</v>
-      </c>
-      <c r="E19" s="5" t="s">
+      <c r="G19" s="5" t="s">
         <v>991</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="H19" s="5" t="s">
         <v>992</v>
       </c>
-      <c r="G19" s="5" t="s">
+      <c r="I19" s="9" t="s">
+        <v>1109</v>
+      </c>
+      <c r="J19" s="5" t="s">
         <v>993</v>
       </c>
-      <c r="H19" s="5" t="s">
+      <c r="K19" s="5" t="s">
         <v>994</v>
       </c>
-      <c r="I19" s="9" t="s">
-        <v>1111</v>
-      </c>
-      <c r="J19" s="5" t="s">
+      <c r="L19" s="5" t="s">
         <v>995</v>
       </c>
-      <c r="K19" s="5" t="s">
+      <c r="M19" s="5" t="s">
         <v>996</v>
-      </c>
-      <c r="L19" s="5" t="s">
-        <v>997</v>
-      </c>
-      <c r="M19" s="5" t="s">
-        <v>998</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
@@ -5243,10 +5243,10 @@
         <v>174</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>1112</v>
+        <v>1110</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>206</v>
@@ -5261,7 +5261,7 @@
         <v>195</v>
       </c>
       <c r="I20" s="9" t="s">
-        <v>1112</v>
+        <v>1110</v>
       </c>
       <c r="J20" s="5" t="s">
         <v>200</v>
@@ -5284,10 +5284,10 @@
         <v>219</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>1113</v>
+        <v>1111</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>210</v>
@@ -5302,7 +5302,7 @@
         <v>214</v>
       </c>
       <c r="I21" s="9" t="s">
-        <v>1113</v>
+        <v>1111</v>
       </c>
       <c r="J21" s="5" t="s">
         <v>215</v>
@@ -5325,10 +5325,10 @@
         <v>220</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>1103</v>
+        <v>1101</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>221</v>
@@ -5343,7 +5343,7 @@
         <v>224</v>
       </c>
       <c r="I22" s="9" t="s">
-        <v>1103</v>
+        <v>1101</v>
       </c>
       <c r="J22" s="5" t="s">
         <v>225</v>
@@ -5366,10 +5366,10 @@
         <v>230</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>1114</v>
+        <v>1112</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>239</v>
@@ -5384,7 +5384,7 @@
         <v>234</v>
       </c>
       <c r="I23" s="9" t="s">
-        <v>1114</v>
+        <v>1112</v>
       </c>
       <c r="J23" s="5" t="s">
         <v>235</v>
@@ -5404,40 +5404,40 @@
         <v>427</v>
       </c>
       <c r="B24" s="5" t="s">
+        <v>561</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>1082</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>1113</v>
+      </c>
+      <c r="E24" s="6" t="s">
         <v>562</v>
       </c>
-      <c r="C24" s="9" t="s">
-        <v>1084</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>1115</v>
-      </c>
-      <c r="E24" s="6" t="s">
+      <c r="F24" s="5" t="s">
         <v>563</v>
       </c>
-      <c r="F24" s="5" t="s">
+      <c r="G24" s="5" t="s">
         <v>564</v>
       </c>
-      <c r="G24" s="5" t="s">
+      <c r="H24" s="5" t="s">
         <v>565</v>
       </c>
-      <c r="H24" s="5" t="s">
+      <c r="I24" s="9" t="s">
+        <v>1113</v>
+      </c>
+      <c r="J24" s="5" t="s">
         <v>566</v>
       </c>
-      <c r="I24" s="9" t="s">
-        <v>1115</v>
-      </c>
-      <c r="J24" s="5" t="s">
+      <c r="K24" s="5" t="s">
         <v>567</v>
       </c>
-      <c r="K24" s="5" t="s">
+      <c r="L24" s="5" t="s">
         <v>568</v>
       </c>
-      <c r="L24" s="5" t="s">
+      <c r="M24" s="5" t="s">
         <v>569</v>
-      </c>
-      <c r="M24" s="5" t="s">
-        <v>570</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
@@ -5445,40 +5445,40 @@
         <v>437</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>1116</v>
+        <v>1114</v>
       </c>
       <c r="E25" s="6" t="s">
+        <v>570</v>
+      </c>
+      <c r="F25" s="5" t="s">
         <v>571</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="G25" s="5" t="s">
         <v>572</v>
       </c>
-      <c r="G25" s="5" t="s">
+      <c r="H25" s="5" t="s">
         <v>573</v>
       </c>
-      <c r="H25" s="5" t="s">
+      <c r="I25" s="9" t="s">
+        <v>1114</v>
+      </c>
+      <c r="J25" s="5" t="s">
         <v>574</v>
       </c>
-      <c r="I25" s="9" t="s">
-        <v>1116</v>
-      </c>
-      <c r="J25" s="5" t="s">
+      <c r="K25" s="5" t="s">
         <v>575</v>
       </c>
-      <c r="K25" s="5" t="s">
+      <c r="L25" s="5" t="s">
         <v>576</v>
       </c>
-      <c r="L25" s="5" t="s">
+      <c r="M25" s="5" t="s">
         <v>577</v>
-      </c>
-      <c r="M25" s="5" t="s">
-        <v>578</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -5486,40 +5486,40 @@
         <v>447</v>
       </c>
       <c r="B26" s="5" t="s">
+        <v>692</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>1082</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>1115</v>
+      </c>
+      <c r="E26" s="6" t="s">
         <v>693</v>
       </c>
-      <c r="C26" s="9" t="s">
-        <v>1084</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>1117</v>
-      </c>
-      <c r="E26" s="6" t="s">
+      <c r="F26" s="5" t="s">
         <v>694</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="G26" s="5" t="s">
         <v>695</v>
       </c>
-      <c r="G26" s="5" t="s">
+      <c r="H26" s="5" t="s">
         <v>696</v>
       </c>
-      <c r="H26" s="5" t="s">
+      <c r="I26" s="9" t="s">
+        <v>1115</v>
+      </c>
+      <c r="J26" s="5" t="s">
         <v>697</v>
       </c>
-      <c r="I26" s="9" t="s">
-        <v>1117</v>
-      </c>
-      <c r="J26" s="5" t="s">
+      <c r="K26" s="5" t="s">
         <v>698</v>
       </c>
-      <c r="K26" s="5" t="s">
+      <c r="L26" s="5" t="s">
         <v>699</v>
       </c>
-      <c r="L26" s="5" t="s">
+      <c r="M26" s="5" t="s">
         <v>700</v>
-      </c>
-      <c r="M26" s="5" t="s">
-        <v>701</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
@@ -5527,40 +5527,40 @@
         <v>457</v>
       </c>
       <c r="B27" s="5" t="s">
+        <v>1055</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>1082</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>1091</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>1056</v>
+      </c>
+      <c r="F27" s="5" t="s">
         <v>1057</v>
       </c>
-      <c r="C27" s="9" t="s">
-        <v>1084</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>1093</v>
-      </c>
-      <c r="E27" s="5" t="s">
+      <c r="G27" s="5" t="s">
         <v>1058</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="H27" s="5" t="s">
         <v>1059</v>
       </c>
-      <c r="G27" s="5" t="s">
+      <c r="I27" s="9" t="s">
+        <v>1091</v>
+      </c>
+      <c r="J27" s="5" t="s">
         <v>1060</v>
       </c>
-      <c r="H27" s="5" t="s">
+      <c r="K27" s="5" t="s">
         <v>1061</v>
       </c>
-      <c r="I27" s="9" t="s">
-        <v>1093</v>
-      </c>
-      <c r="J27" s="5" t="s">
+      <c r="L27" s="5" t="s">
         <v>1062</v>
       </c>
-      <c r="K27" s="5" t="s">
+      <c r="M27" s="5" t="s">
         <v>1063</v>
-      </c>
-      <c r="L27" s="5" t="s">
-        <v>1064</v>
-      </c>
-      <c r="M27" s="5" t="s">
-        <v>1065</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
@@ -5568,618 +5568,618 @@
         <v>467</v>
       </c>
       <c r="B28" s="5" t="s">
+        <v>666</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>1082</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>1116</v>
+      </c>
+      <c r="E28" s="6" t="s">
         <v>667</v>
       </c>
-      <c r="C28" s="9" t="s">
-        <v>1084</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>1118</v>
-      </c>
-      <c r="E28" s="6" t="s">
+      <c r="F28" s="5" t="s">
         <v>668</v>
       </c>
-      <c r="F28" s="5" t="s">
+      <c r="G28" s="5" t="s">
         <v>669</v>
       </c>
-      <c r="G28" s="5" t="s">
+      <c r="H28" s="5" t="s">
         <v>670</v>
       </c>
-      <c r="H28" s="5" t="s">
+      <c r="I28" s="9" t="s">
+        <v>1116</v>
+      </c>
+      <c r="J28" s="5" t="s">
         <v>671</v>
       </c>
-      <c r="I28" s="9" t="s">
-        <v>1118</v>
-      </c>
-      <c r="J28" s="5" t="s">
+      <c r="K28" s="5" t="s">
         <v>672</v>
       </c>
-      <c r="K28" s="5" t="s">
+      <c r="L28" s="5" t="s">
         <v>673</v>
       </c>
-      <c r="L28" s="5" t="s">
+      <c r="M28" s="5" t="s">
         <v>674</v>
-      </c>
-      <c r="M28" s="5" t="s">
-        <v>675</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="11" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="B29" s="5" t="s">
+        <v>675</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>1082</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>1117</v>
+      </c>
+      <c r="E29" s="6" t="s">
         <v>676</v>
       </c>
-      <c r="C29" s="9" t="s">
-        <v>1084</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>1119</v>
-      </c>
-      <c r="E29" s="6" t="s">
+      <c r="F29" s="5" t="s">
         <v>677</v>
       </c>
-      <c r="F29" s="5" t="s">
+      <c r="G29" s="5" t="s">
         <v>678</v>
       </c>
-      <c r="G29" s="5" t="s">
+      <c r="H29" s="5" t="s">
         <v>679</v>
       </c>
-      <c r="H29" s="5" t="s">
+      <c r="I29" s="9" t="s">
+        <v>1117</v>
+      </c>
+      <c r="J29" s="5" t="s">
         <v>680</v>
       </c>
-      <c r="I29" s="9" t="s">
-        <v>1119</v>
-      </c>
-      <c r="J29" s="5" t="s">
+      <c r="K29" s="5" t="s">
         <v>681</v>
       </c>
-      <c r="K29" s="5" t="s">
+      <c r="L29" s="5" t="s">
         <v>682</v>
       </c>
-      <c r="L29" s="5" t="s">
+      <c r="M29" s="5" t="s">
         <v>683</v>
-      </c>
-      <c r="M29" s="5" t="s">
-        <v>684</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B30" s="5" t="s">
+        <v>709</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>1082</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>1118</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>723</v>
+      </c>
+      <c r="F30" s="5" t="s">
         <v>710</v>
       </c>
-      <c r="C30" s="9" t="s">
-        <v>1084</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>1120</v>
-      </c>
-      <c r="E30" s="6" t="s">
+      <c r="G30" s="5" t="s">
+        <v>711</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>712</v>
+      </c>
+      <c r="I30" s="9" t="s">
+        <v>1118</v>
+      </c>
+      <c r="J30" s="5" t="s">
+        <v>713</v>
+      </c>
+      <c r="K30" s="5" t="s">
+        <v>714</v>
+      </c>
+      <c r="L30" s="5" t="s">
         <v>724</v>
       </c>
-      <c r="F30" s="5" t="s">
-        <v>711</v>
-      </c>
-      <c r="G30" s="5" t="s">
-        <v>712</v>
-      </c>
-      <c r="H30" s="5" t="s">
-        <v>713</v>
-      </c>
-      <c r="I30" s="9" t="s">
-        <v>1120</v>
-      </c>
-      <c r="J30" s="5" t="s">
-        <v>714</v>
-      </c>
-      <c r="K30" s="5" t="s">
+      <c r="M30" s="5" t="s">
         <v>715</v>
-      </c>
-      <c r="L30" s="5" t="s">
-        <v>725</v>
-      </c>
-      <c r="M30" s="5" t="s">
-        <v>716</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="11" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="B31" s="5" t="s">
+        <v>709</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>1082</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>1118</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>721</v>
+      </c>
+      <c r="F31" s="5" t="s">
         <v>710</v>
       </c>
-      <c r="C31" s="9" t="s">
-        <v>1084</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>1120</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>722</v>
-      </c>
-      <c r="F31" s="5" t="s">
+      <c r="G31" s="5" t="s">
         <v>711</v>
       </c>
-      <c r="G31" s="5" t="s">
+      <c r="H31" s="5" t="s">
         <v>712</v>
       </c>
-      <c r="H31" s="5" t="s">
+      <c r="I31" s="9" t="s">
+        <v>1118</v>
+      </c>
+      <c r="J31" s="5" t="s">
         <v>713</v>
       </c>
-      <c r="I31" s="9" t="s">
-        <v>1120</v>
-      </c>
-      <c r="J31" s="5" t="s">
+      <c r="K31" s="5" t="s">
         <v>714</v>
       </c>
-      <c r="K31" s="5" t="s">
+      <c r="L31" s="5" t="s">
+        <v>725</v>
+      </c>
+      <c r="M31" s="5" t="s">
         <v>715</v>
-      </c>
-      <c r="L31" s="5" t="s">
-        <v>726</v>
-      </c>
-      <c r="M31" s="5" t="s">
-        <v>716</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B32" s="5" t="s">
+        <v>908</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>1082</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>1119</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>909</v>
+      </c>
+      <c r="F32" s="5" t="s">
         <v>910</v>
       </c>
-      <c r="C32" s="9" t="s">
-        <v>1084</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>1121</v>
-      </c>
-      <c r="E32" s="6" t="s">
+      <c r="G32" s="5" t="s">
         <v>911</v>
       </c>
-      <c r="F32" s="5" t="s">
+      <c r="H32" s="5" t="s">
         <v>912</v>
       </c>
-      <c r="G32" s="5" t="s">
+      <c r="I32" s="9" t="s">
+        <v>1119</v>
+      </c>
+      <c r="J32" s="5" t="s">
         <v>913</v>
       </c>
-      <c r="H32" s="5" t="s">
+      <c r="K32" s="5" t="s">
         <v>914</v>
       </c>
-      <c r="I32" s="9" t="s">
-        <v>1121</v>
-      </c>
-      <c r="J32" s="5" t="s">
+      <c r="L32" s="5" t="s">
         <v>915</v>
       </c>
-      <c r="K32" s="5" t="s">
+      <c r="M32" s="5" t="s">
         <v>916</v>
-      </c>
-      <c r="L32" s="5" t="s">
-        <v>917</v>
-      </c>
-      <c r="M32" s="5" t="s">
-        <v>918</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" s="11" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B33" s="5" t="s">
+        <v>917</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>1082</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>1120</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>918</v>
+      </c>
+      <c r="F33" s="5" t="s">
         <v>919</v>
       </c>
-      <c r="C33" s="9" t="s">
-        <v>1084</v>
-      </c>
-      <c r="D33" s="9" t="s">
-        <v>1122</v>
-      </c>
-      <c r="E33" s="6" t="s">
+      <c r="G33" s="5" t="s">
         <v>920</v>
       </c>
-      <c r="F33" s="5" t="s">
+      <c r="H33" s="5" t="s">
         <v>921</v>
       </c>
-      <c r="G33" s="5" t="s">
+      <c r="I33" s="9" t="s">
+        <v>1120</v>
+      </c>
+      <c r="J33" s="5" t="s">
         <v>922</v>
       </c>
-      <c r="H33" s="5" t="s">
+      <c r="K33" s="5" t="s">
         <v>923</v>
       </c>
-      <c r="I33" s="9" t="s">
-        <v>1122</v>
-      </c>
-      <c r="J33" s="5" t="s">
+      <c r="L33" s="5" t="s">
         <v>924</v>
       </c>
-      <c r="K33" s="5" t="s">
+      <c r="M33" s="5" t="s">
         <v>925</v>
-      </c>
-      <c r="L33" s="5" t="s">
-        <v>926</v>
-      </c>
-      <c r="M33" s="5" t="s">
-        <v>927</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" s="11" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B34" s="5" t="s">
+        <v>926</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>1082</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>1121</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>927</v>
+      </c>
+      <c r="F34" s="5" t="s">
         <v>928</v>
       </c>
-      <c r="C34" s="9" t="s">
-        <v>1084</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>1123</v>
-      </c>
-      <c r="E34" s="6" t="s">
+      <c r="G34" s="5" t="s">
         <v>929</v>
       </c>
-      <c r="F34" s="5" t="s">
+      <c r="H34" s="5" t="s">
         <v>930</v>
       </c>
-      <c r="G34" s="5" t="s">
+      <c r="I34" s="9" t="s">
+        <v>1121</v>
+      </c>
+      <c r="J34" s="5" t="s">
         <v>931</v>
       </c>
-      <c r="H34" s="5" t="s">
+      <c r="K34" s="5" t="s">
         <v>932</v>
       </c>
-      <c r="I34" s="9" t="s">
-        <v>1123</v>
-      </c>
-      <c r="J34" s="5" t="s">
+      <c r="L34" s="5" t="s">
         <v>933</v>
       </c>
-      <c r="K34" s="5" t="s">
+      <c r="M34" s="5" t="s">
         <v>934</v>
-      </c>
-      <c r="L34" s="5" t="s">
-        <v>935</v>
-      </c>
-      <c r="M34" s="5" t="s">
-        <v>936</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" s="11" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B35" s="5" t="s">
+        <v>935</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>1082</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>1122</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>936</v>
+      </c>
+      <c r="F35" s="5" t="s">
         <v>937</v>
       </c>
-      <c r="C35" s="9" t="s">
-        <v>1084</v>
-      </c>
-      <c r="D35" s="9" t="s">
-        <v>1124</v>
-      </c>
-      <c r="E35" s="6" t="s">
+      <c r="G35" s="5" t="s">
         <v>938</v>
       </c>
-      <c r="F35" s="5" t="s">
+      <c r="H35" s="5" t="s">
         <v>939</v>
       </c>
-      <c r="G35" s="5" t="s">
+      <c r="I35" s="9" t="s">
+        <v>1122</v>
+      </c>
+      <c r="J35" s="5" t="s">
         <v>940</v>
       </c>
-      <c r="H35" s="5" t="s">
+      <c r="K35" s="5" t="s">
         <v>941</v>
       </c>
-      <c r="I35" s="9" t="s">
-        <v>1124</v>
-      </c>
-      <c r="J35" s="5" t="s">
+      <c r="L35" s="5" t="s">
         <v>942</v>
       </c>
-      <c r="K35" s="5" t="s">
+      <c r="M35" s="5" t="s">
         <v>943</v>
-      </c>
-      <c r="L35" s="5" t="s">
-        <v>944</v>
-      </c>
-      <c r="M35" s="5" t="s">
-        <v>945</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36" s="11" t="s">
+        <v>944</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>945</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>1082</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>1090</v>
+      </c>
+      <c r="E36" s="6" t="s">
         <v>946</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="F36" s="5" t="s">
         <v>947</v>
       </c>
-      <c r="C36" s="9" t="s">
-        <v>1084</v>
-      </c>
-      <c r="D36" s="9" t="s">
-        <v>1092</v>
-      </c>
-      <c r="E36" s="6" t="s">
+      <c r="G36" s="5" t="s">
         <v>948</v>
       </c>
-      <c r="F36" s="5" t="s">
+      <c r="H36" s="5" t="s">
         <v>949</v>
       </c>
-      <c r="G36" s="5" t="s">
+      <c r="I36" s="9" t="s">
+        <v>1090</v>
+      </c>
+      <c r="J36" s="5" t="s">
         <v>950</v>
       </c>
-      <c r="H36" s="5" t="s">
+      <c r="K36" s="5" t="s">
         <v>951</v>
       </c>
-      <c r="I36" s="9" t="s">
-        <v>1092</v>
-      </c>
-      <c r="J36" s="5" t="s">
+      <c r="L36" s="5" t="s">
         <v>952</v>
       </c>
-      <c r="K36" s="5" t="s">
+      <c r="M36" s="5" t="s">
         <v>953</v>
-      </c>
-      <c r="L36" s="5" t="s">
-        <v>954</v>
-      </c>
-      <c r="M36" s="5" t="s">
-        <v>955</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>1065</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>1082</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>1123</v>
+      </c>
+      <c r="E37" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="F37" s="5" t="s">
         <v>1067</v>
       </c>
-      <c r="C37" s="9" t="s">
-        <v>1084</v>
-      </c>
-      <c r="D37" s="9" t="s">
-        <v>1125</v>
-      </c>
-      <c r="E37" s="5" t="s">
+      <c r="G37" s="5" t="s">
         <v>1068</v>
       </c>
-      <c r="F37" s="5" t="s">
+      <c r="H37" s="5" t="s">
         <v>1069</v>
       </c>
-      <c r="G37" s="5" t="s">
+      <c r="I37" s="9" t="s">
+        <v>1123</v>
+      </c>
+      <c r="J37" s="5" t="s">
         <v>1070</v>
       </c>
-      <c r="H37" s="5" t="s">
+      <c r="K37" s="5" t="s">
         <v>1071</v>
       </c>
-      <c r="I37" s="9" t="s">
-        <v>1125</v>
-      </c>
-      <c r="J37" s="5" t="s">
+      <c r="L37" s="5" t="s">
         <v>1072</v>
       </c>
-      <c r="K37" s="5" t="s">
+      <c r="M37" s="5" t="s">
         <v>1073</v>
-      </c>
-      <c r="L37" s="5" t="s">
-        <v>1074</v>
-      </c>
-      <c r="M37" s="5" t="s">
-        <v>1075</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A38" s="11" t="s">
+        <v>726</v>
+      </c>
+      <c r="B38" s="5" t="s">
         <v>727</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="C38" s="9" t="s">
+        <v>1082</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>1124</v>
+      </c>
+      <c r="E38" s="6" t="s">
         <v>728</v>
       </c>
-      <c r="C38" s="9" t="s">
-        <v>1084</v>
-      </c>
-      <c r="D38" s="9" t="s">
-        <v>1126</v>
-      </c>
-      <c r="E38" s="6" t="s">
+      <c r="F38" s="5" t="s">
         <v>729</v>
       </c>
-      <c r="F38" s="5" t="s">
+      <c r="G38" s="5" t="s">
         <v>730</v>
       </c>
-      <c r="G38" s="5" t="s">
+      <c r="H38" s="5" t="s">
         <v>731</v>
       </c>
-      <c r="H38" s="5" t="s">
+      <c r="I38" s="9" t="s">
+        <v>1124</v>
+      </c>
+      <c r="J38" s="5" t="s">
         <v>732</v>
       </c>
-      <c r="I38" s="9" t="s">
-        <v>1126</v>
-      </c>
-      <c r="J38" s="5" t="s">
+      <c r="K38" s="5" t="s">
         <v>733</v>
       </c>
-      <c r="K38" s="5" t="s">
+      <c r="L38" s="5" t="s">
         <v>734</v>
       </c>
-      <c r="L38" s="5" t="s">
+      <c r="M38" s="5" t="s">
         <v>735</v>
-      </c>
-      <c r="M38" s="5" t="s">
-        <v>736</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A39" s="11" t="s">
+        <v>756</v>
+      </c>
+      <c r="B39" s="5" t="s">
         <v>757</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="C39" s="9" t="s">
+        <v>1082</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>1125</v>
+      </c>
+      <c r="E39" s="6" t="s">
         <v>758</v>
       </c>
-      <c r="C39" s="9" t="s">
-        <v>1084</v>
-      </c>
-      <c r="D39" s="9" t="s">
-        <v>1127</v>
-      </c>
-      <c r="E39" s="6" t="s">
+      <c r="F39" s="5" t="s">
         <v>759</v>
       </c>
-      <c r="F39" s="5" t="s">
+      <c r="G39" s="5" t="s">
         <v>760</v>
       </c>
-      <c r="G39" s="5" t="s">
+      <c r="H39" s="5" t="s">
         <v>761</v>
       </c>
-      <c r="H39" s="5" t="s">
+      <c r="I39" s="9" t="s">
+        <v>1125</v>
+      </c>
+      <c r="J39" s="5" t="s">
         <v>762</v>
       </c>
-      <c r="I39" s="9" t="s">
-        <v>1127</v>
-      </c>
-      <c r="J39" s="5" t="s">
+      <c r="K39" s="5" t="s">
         <v>763</v>
       </c>
-      <c r="K39" s="5" t="s">
+      <c r="L39" s="5" t="s">
         <v>764</v>
       </c>
-      <c r="L39" s="5" t="s">
+      <c r="M39" s="5" t="s">
         <v>765</v>
       </c>
-      <c r="M39" s="5" t="s">
-        <v>766</v>
-      </c>
       <c r="N39" s="5" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A40" s="11" t="s">
+        <v>768</v>
+      </c>
+      <c r="B40" s="5" t="s">
         <v>769</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="C40" s="9" t="s">
+        <v>1082</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>1126</v>
+      </c>
+      <c r="E40" s="6" t="s">
         <v>770</v>
       </c>
-      <c r="C40" s="9" t="s">
-        <v>1084</v>
-      </c>
-      <c r="D40" s="9" t="s">
-        <v>1128</v>
-      </c>
-      <c r="E40" s="6" t="s">
+      <c r="F40" s="5" t="s">
         <v>771</v>
       </c>
-      <c r="F40" s="5" t="s">
+      <c r="G40" s="5" t="s">
         <v>772</v>
       </c>
-      <c r="G40" s="5" t="s">
+      <c r="H40" s="5" t="s">
         <v>773</v>
       </c>
-      <c r="H40" s="5" t="s">
+      <c r="I40" s="9" t="s">
+        <v>1126</v>
+      </c>
+      <c r="J40" s="5" t="s">
         <v>774</v>
       </c>
-      <c r="I40" s="9" t="s">
-        <v>1128</v>
-      </c>
-      <c r="J40" s="5" t="s">
+      <c r="K40" s="5" t="s">
         <v>775</v>
       </c>
-      <c r="K40" s="5" t="s">
+      <c r="L40" s="5" t="s">
         <v>776</v>
       </c>
-      <c r="L40" s="5" t="s">
+      <c r="M40" s="5" t="s">
         <v>777</v>
-      </c>
-      <c r="M40" s="5" t="s">
-        <v>778</v>
       </c>
       <c r="N40" s="5"/>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A41" s="11" t="s">
+        <v>736</v>
+      </c>
+      <c r="B41" s="5" t="s">
         <v>737</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="C41" s="9" t="s">
+        <v>1082</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>1127</v>
+      </c>
+      <c r="E41" s="6" t="s">
         <v>738</v>
       </c>
-      <c r="C41" s="9" t="s">
-        <v>1084</v>
-      </c>
-      <c r="D41" s="9" t="s">
-        <v>1129</v>
-      </c>
-      <c r="E41" s="6" t="s">
+      <c r="F41" s="5" t="s">
         <v>739</v>
       </c>
-      <c r="F41" s="5" t="s">
+      <c r="G41" s="5" t="s">
         <v>740</v>
       </c>
-      <c r="G41" s="5" t="s">
+      <c r="H41" s="5" t="s">
         <v>741</v>
       </c>
-      <c r="H41" s="5" t="s">
+      <c r="I41" s="9" t="s">
+        <v>1127</v>
+      </c>
+      <c r="J41" s="5" t="s">
         <v>742</v>
       </c>
-      <c r="I41" s="9" t="s">
-        <v>1129</v>
-      </c>
-      <c r="J41" s="5" t="s">
+      <c r="K41" s="5" t="s">
         <v>743</v>
       </c>
-      <c r="K41" s="5" t="s">
+      <c r="L41" s="5" t="s">
         <v>744</v>
       </c>
-      <c r="L41" s="5" t="s">
+      <c r="M41" s="5" t="s">
         <v>745</v>
-      </c>
-      <c r="M41" s="5" t="s">
-        <v>746</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A42" s="11" t="s">
+        <v>746</v>
+      </c>
+      <c r="B42" s="5" t="s">
         <v>747</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="C42" s="9" t="s">
+        <v>1082</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>1128</v>
+      </c>
+      <c r="E42" s="6" t="s">
         <v>748</v>
       </c>
-      <c r="C42" s="9" t="s">
-        <v>1084</v>
-      </c>
-      <c r="D42" s="9" t="s">
-        <v>1130</v>
-      </c>
-      <c r="E42" s="6" t="s">
+      <c r="F42" s="5" t="s">
         <v>749</v>
       </c>
-      <c r="F42" s="5" t="s">
+      <c r="G42" s="5" t="s">
         <v>750</v>
       </c>
-      <c r="G42" s="5" t="s">
+      <c r="H42" s="5" t="s">
         <v>751</v>
       </c>
-      <c r="H42" s="5" t="s">
+      <c r="I42" s="9" t="s">
+        <v>1128</v>
+      </c>
+      <c r="J42" s="5" t="s">
         <v>752</v>
       </c>
-      <c r="I42" s="9" t="s">
-        <v>1130</v>
-      </c>
-      <c r="J42" s="5" t="s">
+      <c r="K42" s="5" t="s">
         <v>753</v>
       </c>
-      <c r="K42" s="5" t="s">
+      <c r="L42" s="5" t="s">
         <v>754</v>
       </c>
-      <c r="L42" s="5" t="s">
+      <c r="M42" s="5" t="s">
         <v>755</v>
-      </c>
-      <c r="M42" s="5" t="s">
-        <v>756</v>
       </c>
     </row>
   </sheetData>
@@ -6249,7 +6249,7 @@
         <v>17</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>1083</v>
+        <v>1081</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>1</v>
@@ -6288,7 +6288,7 @@
         <v>121</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>1076</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
@@ -6299,10 +6299,10 @@
         <v>44</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>1086</v>
+        <v>1084</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>1087</v>
+        <v>1085</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>131</v>
@@ -6317,7 +6317,7 @@
         <v>48</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>1087</v>
+        <v>1085</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>129</v>
@@ -6362,7 +6362,7 @@
         <v>74</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="J3" s="5" t="s">
         <v>75</v>
@@ -6407,7 +6407,7 @@
         <v>85</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="J4" s="5" t="s">
         <v>81</v>
@@ -6452,7 +6452,7 @@
         <v>86</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="J5" s="5" t="s">
         <v>82</v>
@@ -6497,7 +6497,7 @@
         <v>91</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="J6" s="5" t="s">
         <v>92</v>
@@ -6542,7 +6542,7 @@
         <v>126</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="J7" s="5" t="s">
         <v>127</v>
@@ -6575,7 +6575,7 @@
         <v>130</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>259</v>
@@ -6587,7 +6587,7 @@
         <v>261</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="J8" s="5" t="s">
         <v>262</v>
@@ -6620,7 +6620,7 @@
         <v>130</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>267</v>
@@ -6632,7 +6632,7 @@
         <v>269</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="J9" s="5" t="s">
         <v>270</v>
@@ -6665,7 +6665,7 @@
         <v>130</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>275</v>
@@ -6677,7 +6677,7 @@
         <v>277</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="J10" s="5" t="s">
         <v>278</v>
@@ -6710,7 +6710,7 @@
         <v>130</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>283</v>
@@ -6722,7 +6722,7 @@
         <v>285</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="J11" s="5" t="s">
         <v>286</v>
@@ -6755,7 +6755,7 @@
         <v>130</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>1080</v>
+        <v>1078</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>291</v>
@@ -6767,7 +6767,7 @@
         <v>293</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="J12" s="5" t="s">
         <v>294</v>
@@ -6800,7 +6800,7 @@
         <v>130</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>1081</v>
+        <v>1079</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>299</v>
@@ -6812,7 +6812,7 @@
         <v>301</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="J13" s="5" t="s">
         <v>302</v>
@@ -6845,7 +6845,7 @@
         <v>130</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>1082</v>
+        <v>1080</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>307</v>
@@ -6857,7 +6857,7 @@
         <v>309</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="J14" s="5" t="s">
         <v>310</v>
@@ -6902,7 +6902,7 @@
         <v>318</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="J15" s="5" t="s">
         <v>319</v>
@@ -6947,7 +6947,7 @@
         <v>327</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="J16" s="5" t="s">
         <v>328</v>
@@ -6992,7 +6992,7 @@
         <v>337</v>
       </c>
       <c r="I17" s="9" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="J17" s="5" t="s">
         <v>338</v>
@@ -7037,7 +7037,7 @@
         <v>347</v>
       </c>
       <c r="I18" s="9" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="J18" s="5" t="s">
         <v>348</v>
@@ -7082,7 +7082,7 @@
         <v>357</v>
       </c>
       <c r="I19" s="9" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="J19" s="5" t="s">
         <v>358</v>
@@ -7127,7 +7127,7 @@
         <v>366</v>
       </c>
       <c r="I20" s="9" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="J20" s="5" t="s">
         <v>367</v>
@@ -7148,7 +7148,7 @@
         <v>242</v>
       </c>
       <c r="P20" s="5" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
@@ -7175,7 +7175,7 @@
         <v>375</v>
       </c>
       <c r="I21" s="9" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="J21" s="5" t="s">
         <v>376</v>
@@ -7220,7 +7220,7 @@
         <v>384</v>
       </c>
       <c r="I22" s="9" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="J22" s="5" t="s">
         <v>385</v>
@@ -7265,7 +7265,7 @@
         <v>393</v>
       </c>
       <c r="I23" s="9" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="J23" s="5" t="s">
         <v>394</v>
@@ -7310,7 +7310,7 @@
         <v>403</v>
       </c>
       <c r="I24" s="9" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="J24" s="5" t="s">
         <v>404</v>
@@ -7355,7 +7355,7 @@
         <v>413</v>
       </c>
       <c r="I25" s="9" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="J25" s="5" t="s">
         <v>414</v>
@@ -7400,7 +7400,7 @@
         <v>422</v>
       </c>
       <c r="I26" s="9" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="J26" s="5" t="s">
         <v>423</v>
@@ -7445,7 +7445,7 @@
         <v>432</v>
       </c>
       <c r="I27" s="9" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="J27" s="5" t="s">
         <v>433</v>
@@ -7490,7 +7490,7 @@
         <v>442</v>
       </c>
       <c r="I28" s="9" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="J28" s="5" t="s">
         <v>443</v>
@@ -7535,7 +7535,7 @@
         <v>452</v>
       </c>
       <c r="I29" s="9" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="J29" s="5" t="s">
         <v>453</v>
@@ -7580,7 +7580,7 @@
         <v>462</v>
       </c>
       <c r="I30" s="9" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="J30" s="5" t="s">
         <v>463</v>
@@ -7625,7 +7625,7 @@
         <v>472</v>
       </c>
       <c r="I31" s="9" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="J31" s="5" t="s">
         <v>473</v>
@@ -7648,41 +7648,41 @@
     </row>
     <row r="32" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
+        <v>587</v>
+      </c>
+      <c r="B32" s="5" t="s">
         <v>588</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>589</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="9" t="s">
         <v>130</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="F32" s="5" t="s">
+        <v>589</v>
+      </c>
+      <c r="G32" s="5" t="s">
         <v>590</v>
       </c>
-      <c r="G32" s="5" t="s">
+      <c r="H32" s="5" t="s">
         <v>591</v>
       </c>
-      <c r="H32" s="5" t="s">
+      <c r="I32" s="9" t="s">
+        <v>636</v>
+      </c>
+      <c r="J32" s="5" t="s">
         <v>592</v>
       </c>
-      <c r="I32" s="9" t="s">
-        <v>637</v>
-      </c>
-      <c r="J32" s="5" t="s">
+      <c r="K32" s="5" t="s">
         <v>593</v>
       </c>
-      <c r="K32" s="5" t="s">
+      <c r="L32" s="5" t="s">
         <v>594</v>
       </c>
-      <c r="L32" s="5" t="s">
+      <c r="M32" s="5" t="s">
         <v>595</v>
-      </c>
-      <c r="M32" s="5" t="s">
-        <v>596</v>
       </c>
       <c r="N32" s="5" t="s">
         <v>12</v>
@@ -7693,41 +7693,41 @@
     </row>
     <row r="33" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
+        <v>596</v>
+      </c>
+      <c r="B33" s="5" t="s">
         <v>597</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>598</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="9" t="s">
         <v>130</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="F33" s="5" t="s">
+        <v>598</v>
+      </c>
+      <c r="G33" s="5" t="s">
         <v>599</v>
       </c>
-      <c r="G33" s="5" t="s">
+      <c r="H33" s="5" t="s">
         <v>600</v>
       </c>
-      <c r="H33" s="5" t="s">
+      <c r="I33" s="9" t="s">
+        <v>635</v>
+      </c>
+      <c r="J33" s="5" t="s">
         <v>601</v>
       </c>
-      <c r="I33" s="9" t="s">
-        <v>636</v>
-      </c>
-      <c r="J33" s="5" t="s">
+      <c r="K33" s="5" t="s">
         <v>602</v>
       </c>
-      <c r="K33" s="5" t="s">
+      <c r="L33" s="5" t="s">
         <v>603</v>
       </c>
-      <c r="L33" s="5" t="s">
+      <c r="M33" s="5" t="s">
         <v>604</v>
-      </c>
-      <c r="M33" s="5" t="s">
-        <v>605</v>
       </c>
       <c r="N33" s="5" t="s">
         <v>12</v>
@@ -7738,41 +7738,41 @@
     </row>
     <row r="34" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
+        <v>605</v>
+      </c>
+      <c r="B34" s="5" t="s">
         <v>606</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>607</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="9" t="s">
         <v>130</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="F34" s="5" t="s">
+        <v>607</v>
+      </c>
+      <c r="G34" s="5" t="s">
         <v>608</v>
       </c>
-      <c r="G34" s="5" t="s">
+      <c r="H34" s="5" t="s">
         <v>609</v>
       </c>
-      <c r="H34" s="5" t="s">
+      <c r="I34" s="9" t="s">
+        <v>634</v>
+      </c>
+      <c r="J34" s="5" t="s">
         <v>610</v>
       </c>
-      <c r="I34" s="9" t="s">
-        <v>635</v>
-      </c>
-      <c r="J34" s="5" t="s">
+      <c r="K34" s="5" t="s">
         <v>611</v>
       </c>
-      <c r="K34" s="5" t="s">
+      <c r="L34" s="5" t="s">
         <v>612</v>
       </c>
-      <c r="L34" s="5" t="s">
+      <c r="M34" s="5" t="s">
         <v>613</v>
-      </c>
-      <c r="M34" s="5" t="s">
-        <v>614</v>
       </c>
       <c r="N34" s="5" t="s">
         <v>12</v>
@@ -7783,41 +7783,41 @@
     </row>
     <row r="35" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
+        <v>614</v>
+      </c>
+      <c r="B35" s="5" t="s">
         <v>615</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>616</v>
       </c>
       <c r="C35" s="5"/>
       <c r="D35" s="9" t="s">
         <v>130</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="F35" s="5" t="s">
+        <v>616</v>
+      </c>
+      <c r="G35" s="5" t="s">
         <v>617</v>
       </c>
-      <c r="G35" s="5" t="s">
+      <c r="H35" s="5" t="s">
         <v>618</v>
       </c>
-      <c r="H35" s="5" t="s">
+      <c r="I35" s="9" t="s">
+        <v>633</v>
+      </c>
+      <c r="J35" s="5" t="s">
         <v>619</v>
       </c>
-      <c r="I35" s="9" t="s">
-        <v>634</v>
-      </c>
-      <c r="J35" s="5" t="s">
+      <c r="K35" s="5" t="s">
         <v>620</v>
       </c>
-      <c r="K35" s="5" t="s">
+      <c r="L35" s="5" t="s">
         <v>621</v>
       </c>
-      <c r="L35" s="5" t="s">
+      <c r="M35" s="5" t="s">
         <v>622</v>
-      </c>
-      <c r="M35" s="5" t="s">
-        <v>623</v>
       </c>
       <c r="N35" s="5" t="s">
         <v>12</v>
@@ -7828,41 +7828,41 @@
     </row>
     <row r="36" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
+        <v>623</v>
+      </c>
+      <c r="B36" s="5" t="s">
         <v>624</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>625</v>
       </c>
       <c r="C36" s="5"/>
       <c r="D36" s="9" t="s">
         <v>130</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="F36" s="5" t="s">
+        <v>625</v>
+      </c>
+      <c r="G36" s="5" t="s">
         <v>626</v>
       </c>
-      <c r="G36" s="5" t="s">
+      <c r="H36" s="5" t="s">
         <v>627</v>
       </c>
-      <c r="H36" s="5" t="s">
+      <c r="I36" s="9" t="s">
+        <v>632</v>
+      </c>
+      <c r="J36" s="5" t="s">
         <v>628</v>
       </c>
-      <c r="I36" s="9" t="s">
-        <v>633</v>
-      </c>
-      <c r="J36" s="5" t="s">
+      <c r="K36" s="5" t="s">
         <v>629</v>
       </c>
-      <c r="K36" s="5" t="s">
+      <c r="L36" s="5" t="s">
         <v>630</v>
       </c>
-      <c r="L36" s="5" t="s">
+      <c r="M36" s="5" t="s">
         <v>631</v>
-      </c>
-      <c r="M36" s="5" t="s">
-        <v>632</v>
       </c>
       <c r="N36" s="5" t="s">
         <v>12</v>
@@ -7899,7 +7899,7 @@
   <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7968,10 +7968,10 @@
         <v>139</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>1088</v>
+        <v>1086</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>1089</v>
+        <v>1087</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>142</v>
@@ -7983,7 +7983,7 @@
         <v>144</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>1088</v>
+        <v>1086</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>165</v>
@@ -8009,7 +8009,7 @@
         <v>480</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>481</v>
@@ -8021,7 +8021,7 @@
         <v>483</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="I3" s="9" t="s">
         <v>480</v>
@@ -8044,40 +8044,40 @@
         <v>36</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>856</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>857</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>865</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>858</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="F4" s="5" t="s">
         <v>859</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>867</v>
-      </c>
-      <c r="E4" s="5" t="s">
+      <c r="G4" s="5" t="s">
         <v>860</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="H4" s="5" t="s">
         <v>861</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="I4" s="9" t="s">
+        <v>857</v>
+      </c>
+      <c r="J4" s="5" t="s">
         <v>862</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="K4" s="5" t="s">
         <v>863</v>
       </c>
-      <c r="I4" s="9" t="s">
-        <v>859</v>
-      </c>
-      <c r="J4" s="5" t="s">
+      <c r="L4" s="5" t="s">
         <v>864</v>
       </c>
-      <c r="K4" s="5" t="s">
-        <v>865</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>866</v>
-      </c>
       <c r="M4" s="5" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8085,40 +8085,40 @@
         <v>43</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>866</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>867</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>875</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>868</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="F5" s="5" t="s">
         <v>869</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>877</v>
-      </c>
-      <c r="E5" s="5" t="s">
+      <c r="G5" s="5" t="s">
         <v>870</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="H5" s="5" t="s">
         <v>871</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="I5" s="9" t="s">
+        <v>867</v>
+      </c>
+      <c r="J5" s="5" t="s">
         <v>872</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="K5" s="5" t="s">
         <v>873</v>
       </c>
-      <c r="I5" s="9" t="s">
-        <v>869</v>
-      </c>
-      <c r="J5" s="5" t="s">
+      <c r="L5" s="5" t="s">
         <v>874</v>
       </c>
-      <c r="K5" s="5" t="s">
-        <v>875</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>876</v>
-      </c>
       <c r="M5" s="5" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8126,40 +8126,40 @@
         <v>64</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>803</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>804</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>805</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="E6" s="5" t="s">
         <v>806</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="F6" s="5" t="s">
         <v>807</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="G6" s="5" t="s">
         <v>808</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="H6" s="5" t="s">
         <v>809</v>
       </c>
-      <c r="G6" s="5" t="s">
-        <v>810</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>811</v>
-      </c>
       <c r="I6" s="9" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="J6" s="5" t="s">
+        <v>812</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>813</v>
+      </c>
+      <c r="L6" s="5" t="s">
         <v>814</v>
       </c>
-      <c r="K6" s="5" t="s">
-        <v>815</v>
-      </c>
-      <c r="L6" s="5" t="s">
-        <v>816</v>
-      </c>
       <c r="M6" s="5" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8167,40 +8167,40 @@
         <v>96</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>786</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>1088</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>1089</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>787</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>788</v>
       </c>
-      <c r="C7" s="9" t="s">
-        <v>1090</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>1091</v>
-      </c>
-      <c r="E7" s="5" t="s">
+      <c r="G7" s="5" t="s">
         <v>789</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="H7" s="5" t="s">
+        <v>810</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>1088</v>
+      </c>
+      <c r="J7" s="5" t="s">
         <v>790</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="K7" s="5" t="s">
         <v>791</v>
       </c>
-      <c r="H7" s="5" t="s">
-        <v>812</v>
-      </c>
-      <c r="I7" s="9" t="s">
-        <v>1090</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>792</v>
-      </c>
-      <c r="K7" s="5" t="s">
-        <v>793</v>
-      </c>
       <c r="L7" s="5" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="M7" s="5" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8208,40 +8208,40 @@
         <v>103</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>792</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>793</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>801</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>794</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="F8" s="5" t="s">
         <v>795</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>803</v>
-      </c>
-      <c r="E8" s="5" t="s">
+      <c r="G8" s="5" t="s">
         <v>796</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="H8" s="5" t="s">
+        <v>811</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>793</v>
+      </c>
+      <c r="J8" s="5" t="s">
         <v>797</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="K8" s="5" t="s">
         <v>798</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>813</v>
-      </c>
-      <c r="I8" s="9" t="s">
-        <v>795</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>799</v>
-      </c>
-      <c r="K8" s="5" t="s">
-        <v>800</v>
       </c>
       <c r="L8" s="5" t="s">
         <v>486</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8249,40 +8249,40 @@
         <v>111</v>
       </c>
       <c r="B9" s="5" t="s">
+        <v>816</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>817</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>818</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="E9" s="5" t="s">
         <v>819</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="F9" s="5" t="s">
         <v>820</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="G9" s="5" t="s">
         <v>821</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="H9" s="5" t="s">
         <v>822</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="I9" s="9" t="s">
+        <v>817</v>
+      </c>
+      <c r="J9" s="5" t="s">
         <v>823</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="K9" s="5" t="s">
         <v>824</v>
       </c>
-      <c r="I9" s="9" t="s">
-        <v>819</v>
-      </c>
-      <c r="J9" s="5" t="s">
+      <c r="L9" s="5" t="s">
         <v>825</v>
       </c>
-      <c r="K9" s="5" t="s">
-        <v>826</v>
-      </c>
-      <c r="L9" s="5" t="s">
-        <v>827</v>
-      </c>
       <c r="M9" s="5" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8293,10 +8293,10 @@
         <v>487</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>1131</v>
+        <v>1129</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>1132</v>
+        <v>1130</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>488</v>
@@ -8308,10 +8308,10 @@
         <v>490</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>1131</v>
+        <v>1129</v>
       </c>
       <c r="J10" s="5" t="s">
         <v>491</v>
@@ -8331,40 +8331,40 @@
         <v>115</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>997</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>998</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>999</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="E11" s="5" t="s">
         <v>1000</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="F11" s="5" t="s">
         <v>1001</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="G11" s="5" t="s">
         <v>1002</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="H11" s="5" t="s">
         <v>1003</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="I11" s="9" t="s">
+        <v>998</v>
+      </c>
+      <c r="J11" s="5" t="s">
         <v>1004</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="K11" s="5" t="s">
         <v>1005</v>
       </c>
-      <c r="I11" s="9" t="s">
-        <v>1000</v>
-      </c>
-      <c r="J11" s="5" t="s">
+      <c r="L11" s="5" t="s">
         <v>1006</v>
       </c>
-      <c r="K11" s="5" t="s">
-        <v>1007</v>
-      </c>
-      <c r="L11" s="5" t="s">
-        <v>1008</v>
-      </c>
       <c r="M11" s="5" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8372,40 +8372,40 @@
         <v>117</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>1007</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>1008</v>
+      </c>
+      <c r="D12" s="6" t="s">
         <v>1009</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="E12" s="5" t="s">
         <v>1010</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="F12" s="5" t="s">
         <v>1011</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="G12" s="5" t="s">
         <v>1012</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="H12" s="5" t="s">
         <v>1013</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="I12" s="9" t="s">
+        <v>1008</v>
+      </c>
+      <c r="J12" s="5" t="s">
         <v>1014</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="K12" s="5" t="s">
         <v>1015</v>
       </c>
-      <c r="I12" s="9" t="s">
-        <v>1010</v>
-      </c>
-      <c r="J12" s="5" t="s">
+      <c r="L12" s="5" t="s">
         <v>1016</v>
       </c>
-      <c r="K12" s="5" t="s">
-        <v>1017</v>
-      </c>
-      <c r="L12" s="5" t="s">
-        <v>1018</v>
-      </c>
       <c r="M12" s="5" t="s">
-        <v>1018</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8413,40 +8413,40 @@
         <v>119</v>
       </c>
       <c r="B13" s="5" t="s">
+        <v>886</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>887</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>888</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="E13" s="5" t="s">
         <v>889</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="F13" s="5" t="s">
         <v>890</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="G13" s="5" t="s">
         <v>891</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="H13" s="5" t="s">
         <v>892</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="I13" s="9" t="s">
+        <v>887</v>
+      </c>
+      <c r="J13" s="5" t="s">
         <v>893</v>
       </c>
-      <c r="H13" s="5" t="s">
+      <c r="K13" s="5" t="s">
         <v>894</v>
       </c>
-      <c r="I13" s="9" t="s">
-        <v>889</v>
-      </c>
-      <c r="J13" s="5" t="s">
+      <c r="L13" s="5" t="s">
         <v>895</v>
       </c>
-      <c r="K13" s="5" t="s">
-        <v>896</v>
-      </c>
-      <c r="L13" s="5" t="s">
-        <v>897</v>
-      </c>
       <c r="M13" s="5" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8457,113 +8457,113 @@
         <v>494</v>
       </c>
       <c r="C14" s="9" t="s">
+        <v>1131</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>1132</v>
+      </c>
+      <c r="E14" s="5" t="s">
         <v>495</v>
       </c>
-      <c r="D14" s="6" t="s">
-        <v>779</v>
-      </c>
-      <c r="E14" s="5" t="s">
+      <c r="F14" s="5" t="s">
         <v>496</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="G14" s="5" t="s">
         <v>497</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>498</v>
       </c>
       <c r="H14" s="5"/>
       <c r="I14" s="9" t="s">
-        <v>495</v>
+        <v>1131</v>
       </c>
       <c r="J14" s="5" t="s">
+        <v>498</v>
+      </c>
+      <c r="K14" s="5" t="s">
         <v>499</v>
       </c>
-      <c r="K14" s="5" t="s">
+      <c r="L14" s="5" t="s">
         <v>500</v>
       </c>
-      <c r="L14" s="5" t="s">
-        <v>501</v>
-      </c>
       <c r="M14" s="5" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
+        <v>501</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>502</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="C15" s="9" t="s">
         <v>503</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="D15" s="6" t="s">
+        <v>778</v>
+      </c>
+      <c r="E15" s="5" t="s">
         <v>504</v>
       </c>
-      <c r="D15" s="6" t="s">
-        <v>780</v>
-      </c>
-      <c r="E15" s="5" t="s">
+      <c r="F15" s="5" t="s">
         <v>505</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="G15" s="5" t="s">
         <v>506</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>507</v>
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="9" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="J15" s="5" t="s">
+        <v>507</v>
+      </c>
+      <c r="K15" s="5" t="s">
         <v>508</v>
       </c>
-      <c r="K15" s="5" t="s">
+      <c r="L15" s="5" t="s">
         <v>509</v>
       </c>
-      <c r="L15" s="5" t="s">
-        <v>510</v>
-      </c>
       <c r="M15" s="5" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
+        <v>510</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>511</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="C16" s="9" t="s">
+        <v>503</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>779</v>
+      </c>
+      <c r="E16" s="5" t="s">
         <v>512</v>
       </c>
-      <c r="C16" s="9" t="s">
-        <v>504</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>781</v>
-      </c>
-      <c r="E16" s="5" t="s">
+      <c r="F16" s="5" t="s">
         <v>513</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="G16" s="5" t="s">
         <v>514</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>515</v>
       </c>
       <c r="H16" s="5"/>
       <c r="I16" s="9" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="J16" s="5" t="s">
+        <v>515</v>
+      </c>
+      <c r="K16" s="5" t="s">
         <v>516</v>
       </c>
-      <c r="K16" s="5" t="s">
+      <c r="L16" s="5" t="s">
         <v>517</v>
       </c>
-      <c r="L16" s="5" t="s">
-        <v>518</v>
-      </c>
       <c r="M16" s="5" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8571,40 +8571,40 @@
         <v>17</v>
       </c>
       <c r="B17" s="5" t="s">
+        <v>518</v>
+      </c>
+      <c r="C17" s="9" t="s">
         <v>519</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="D17" s="6" t="s">
+        <v>780</v>
+      </c>
+      <c r="E17" s="5" t="s">
         <v>520</v>
       </c>
-      <c r="D17" s="6" t="s">
-        <v>782</v>
-      </c>
-      <c r="E17" s="5" t="s">
+      <c r="F17" s="5" t="s">
         <v>521</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="G17" s="5" t="s">
         <v>522</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="H17" s="5" t="s">
         <v>523</v>
       </c>
-      <c r="H17" s="5" t="s">
+      <c r="I17" s="9" t="s">
+        <v>519</v>
+      </c>
+      <c r="J17" s="5" t="s">
         <v>524</v>
       </c>
-      <c r="I17" s="9" t="s">
-        <v>520</v>
-      </c>
-      <c r="J17" s="5" t="s">
+      <c r="K17" s="5" t="s">
         <v>525</v>
       </c>
-      <c r="K17" s="5" t="s">
+      <c r="L17" s="5" t="s">
         <v>526</v>
       </c>
-      <c r="L17" s="5" t="s">
-        <v>527</v>
-      </c>
       <c r="M17" s="5" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8612,38 +8612,38 @@
         <v>18</v>
       </c>
       <c r="B18" s="5" t="s">
+        <v>527</v>
+      </c>
+      <c r="C18" s="9" t="s">
         <v>528</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="D18" s="6" t="s">
+        <v>781</v>
+      </c>
+      <c r="E18" s="5" t="s">
         <v>529</v>
       </c>
-      <c r="D18" s="6" t="s">
-        <v>783</v>
-      </c>
-      <c r="E18" s="5" t="s">
+      <c r="F18" s="5" t="s">
         <v>530</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="G18" s="5" t="s">
         <v>531</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>532</v>
       </c>
       <c r="H18" s="5"/>
       <c r="I18" s="9" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="J18" s="5" t="s">
+        <v>532</v>
+      </c>
+      <c r="K18" s="5" t="s">
         <v>533</v>
       </c>
-      <c r="K18" s="5" t="s">
+      <c r="L18" s="5" t="s">
         <v>534</v>
       </c>
-      <c r="L18" s="5" t="s">
-        <v>535</v>
-      </c>
       <c r="M18" s="5" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8651,38 +8651,38 @@
         <v>19</v>
       </c>
       <c r="B19" s="5" t="s">
+        <v>535</v>
+      </c>
+      <c r="C19" s="9" t="s">
         <v>536</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="D19" s="6" t="s">
+        <v>782</v>
+      </c>
+      <c r="E19" s="5" t="s">
         <v>537</v>
       </c>
-      <c r="D19" s="6" t="s">
-        <v>784</v>
-      </c>
-      <c r="E19" s="5" t="s">
+      <c r="F19" s="5" t="s">
         <v>538</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="G19" s="5" t="s">
         <v>539</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>540</v>
       </c>
       <c r="H19" s="5"/>
       <c r="I19" s="9" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="J19" s="5" t="s">
+        <v>540</v>
+      </c>
+      <c r="K19" s="5" t="s">
         <v>541</v>
       </c>
-      <c r="K19" s="5" t="s">
+      <c r="L19" s="5" t="s">
         <v>542</v>
       </c>
-      <c r="L19" s="5" t="s">
-        <v>543</v>
-      </c>
       <c r="M19" s="5" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8690,38 +8690,38 @@
         <v>209</v>
       </c>
       <c r="B20" s="5" t="s">
+        <v>684</v>
+      </c>
+      <c r="C20" s="9" t="s">
         <v>685</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="D20" s="6" t="s">
+        <v>783</v>
+      </c>
+      <c r="E20" s="5" t="s">
         <v>686</v>
       </c>
-      <c r="D20" s="6" t="s">
-        <v>785</v>
-      </c>
-      <c r="E20" s="5" t="s">
+      <c r="F20" s="5" t="s">
         <v>687</v>
       </c>
-      <c r="F20" s="5" t="s">
+      <c r="G20" s="5" t="s">
         <v>688</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>689</v>
       </c>
       <c r="H20" s="5"/>
       <c r="I20" s="9" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="J20" s="5" t="s">
+        <v>689</v>
+      </c>
+      <c r="K20" s="5" t="s">
         <v>690</v>
       </c>
-      <c r="K20" s="5" t="s">
+      <c r="L20" s="5" t="s">
         <v>691</v>
       </c>
-      <c r="L20" s="5" t="s">
-        <v>692</v>
-      </c>
       <c r="M20" s="5" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8729,38 +8729,38 @@
         <v>229</v>
       </c>
       <c r="B21" s="5" t="s">
+        <v>579</v>
+      </c>
+      <c r="C21" s="9" t="s">
         <v>580</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="D21" s="6" t="s">
+        <v>783</v>
+      </c>
+      <c r="E21" s="5" t="s">
         <v>581</v>
       </c>
-      <c r="D21" s="6" t="s">
-        <v>785</v>
-      </c>
-      <c r="E21" s="5" t="s">
+      <c r="F21" s="5" t="s">
         <v>582</v>
       </c>
-      <c r="F21" s="5" t="s">
+      <c r="G21" s="5" t="s">
         <v>583</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>584</v>
       </c>
       <c r="H21" s="5"/>
       <c r="I21" s="9" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="J21" s="5" t="s">
+        <v>584</v>
+      </c>
+      <c r="K21" s="5" t="s">
         <v>585</v>
       </c>
-      <c r="K21" s="5" t="s">
+      <c r="L21" s="5" t="s">
         <v>586</v>
       </c>
-      <c r="L21" s="5" t="s">
-        <v>587</v>
-      </c>
       <c r="M21" s="5" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8768,40 +8768,40 @@
         <v>418</v>
       </c>
       <c r="B22" s="5" t="s">
+        <v>1037</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>1038</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>1076</v>
+      </c>
+      <c r="E22" s="5" t="s">
         <v>1039</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="F22" s="5" t="s">
         <v>1040</v>
       </c>
-      <c r="D22" s="6" t="s">
-        <v>1078</v>
-      </c>
-      <c r="E22" s="5" t="s">
+      <c r="G22" s="5" t="s">
         <v>1041</v>
       </c>
-      <c r="F22" s="5" t="s">
+      <c r="H22" s="5" t="s">
         <v>1042</v>
       </c>
-      <c r="G22" s="5" t="s">
+      <c r="I22" s="9" t="s">
+        <v>1038</v>
+      </c>
+      <c r="J22" s="5" t="s">
         <v>1043</v>
       </c>
-      <c r="H22" s="5" t="s">
+      <c r="K22" s="5" t="s">
         <v>1044</v>
       </c>
-      <c r="I22" s="9" t="s">
-        <v>1040</v>
-      </c>
-      <c r="J22" s="5" t="s">
+      <c r="L22" s="5" t="s">
         <v>1045</v>
       </c>
-      <c r="K22" s="5" t="s">
-        <v>1046</v>
-      </c>
-      <c r="L22" s="5" t="s">
-        <v>1047</v>
-      </c>
       <c r="M22" s="5" t="s">
-        <v>1047</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8809,40 +8809,40 @@
         <v>427</v>
       </c>
       <c r="B23" s="5" t="s">
+        <v>827</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>828</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>1077</v>
+      </c>
+      <c r="E23" s="5" t="s">
         <v>829</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="F23" s="5" t="s">
         <v>830</v>
       </c>
-      <c r="D23" s="6" t="s">
-        <v>1079</v>
-      </c>
-      <c r="E23" s="5" t="s">
+      <c r="G23" s="5" t="s">
         <v>831</v>
       </c>
-      <c r="F23" s="5" t="s">
+      <c r="H23" s="5" t="s">
         <v>832</v>
       </c>
-      <c r="G23" s="5" t="s">
+      <c r="I23" s="9" t="s">
+        <v>828</v>
+      </c>
+      <c r="J23" s="5" t="s">
         <v>833</v>
       </c>
-      <c r="H23" s="5" t="s">
+      <c r="K23" s="5" t="s">
         <v>834</v>
       </c>
-      <c r="I23" s="9" t="s">
-        <v>830</v>
-      </c>
-      <c r="J23" s="5" t="s">
+      <c r="L23" s="5" t="s">
         <v>835</v>
       </c>
-      <c r="K23" s="5" t="s">
-        <v>836</v>
-      </c>
-      <c r="L23" s="5" t="s">
-        <v>837</v>
-      </c>
       <c r="M23" s="5" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8850,40 +8850,40 @@
         <v>437</v>
       </c>
       <c r="B24" s="5" t="s">
+        <v>836</v>
+      </c>
+      <c r="C24" s="9" t="s">
         <v>838</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="D24" s="6" t="s">
+        <v>839</v>
+      </c>
+      <c r="E24" s="5" t="s">
         <v>840</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="F24" s="5" t="s">
         <v>841</v>
       </c>
-      <c r="E24" s="5" t="s">
+      <c r="G24" s="5" t="s">
         <v>842</v>
       </c>
-      <c r="F24" s="5" t="s">
+      <c r="H24" s="5" t="s">
         <v>843</v>
       </c>
-      <c r="G24" s="5" t="s">
+      <c r="I24" s="9" t="s">
+        <v>838</v>
+      </c>
+      <c r="J24" s="5" t="s">
         <v>844</v>
       </c>
-      <c r="H24" s="5" t="s">
+      <c r="K24" s="5" t="s">
         <v>845</v>
       </c>
-      <c r="I24" s="9" t="s">
-        <v>840</v>
-      </c>
-      <c r="J24" s="5" t="s">
+      <c r="L24" s="5" t="s">
         <v>846</v>
       </c>
-      <c r="K24" s="5" t="s">
-        <v>847</v>
-      </c>
-      <c r="L24" s="5" t="s">
-        <v>848</v>
-      </c>
       <c r="M24" s="5" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8891,40 +8891,40 @@
         <v>447</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
       <c r="C25" s="9" t="s">
+        <v>847</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>848</v>
+      </c>
+      <c r="E25" s="5" t="s">
         <v>849</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="F25" s="5" t="s">
         <v>850</v>
       </c>
-      <c r="E25" s="5" t="s">
+      <c r="G25" s="5" t="s">
         <v>851</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="H25" s="5" t="s">
         <v>852</v>
       </c>
-      <c r="G25" s="5" t="s">
+      <c r="I25" s="9" t="s">
+        <v>847</v>
+      </c>
+      <c r="J25" s="5" t="s">
         <v>853</v>
       </c>
-      <c r="H25" s="5" t="s">
+      <c r="K25" s="5" t="s">
         <v>854</v>
       </c>
-      <c r="I25" s="9" t="s">
-        <v>849</v>
-      </c>
-      <c r="J25" s="5" t="s">
+      <c r="L25" s="5" t="s">
         <v>855</v>
       </c>
-      <c r="K25" s="5" t="s">
-        <v>856</v>
-      </c>
-      <c r="L25" s="5" t="s">
-        <v>857</v>
-      </c>
       <c r="M25" s="5" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8932,40 +8932,40 @@
         <v>457</v>
       </c>
       <c r="B26" s="5" t="s">
+        <v>954</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>955</v>
+      </c>
+      <c r="D26" s="6" t="s">
         <v>956</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="E26" s="5" t="s">
         <v>957</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="F26" s="5" t="s">
         <v>958</v>
       </c>
-      <c r="E26" s="5" t="s">
+      <c r="G26" s="5" t="s">
         <v>959</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="H26" s="5" t="s">
         <v>960</v>
       </c>
-      <c r="G26" s="5" t="s">
+      <c r="I26" s="9" t="s">
+        <v>955</v>
+      </c>
+      <c r="J26" s="5" t="s">
         <v>961</v>
       </c>
-      <c r="H26" s="5" t="s">
+      <c r="K26" s="5" t="s">
         <v>962</v>
       </c>
-      <c r="I26" s="9" t="s">
-        <v>957</v>
-      </c>
-      <c r="J26" s="5" t="s">
+      <c r="L26" s="5" t="s">
         <v>963</v>
       </c>
-      <c r="K26" s="5" t="s">
-        <v>964</v>
-      </c>
-      <c r="L26" s="5" t="s">
-        <v>965</v>
-      </c>
       <c r="M26" s="5" t="s">
-        <v>965</v>
+        <v>963</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8973,282 +8973,282 @@
         <v>467</v>
       </c>
       <c r="B27" s="5" t="s">
+        <v>964</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>965</v>
+      </c>
+      <c r="D27" s="6" t="s">
         <v>966</v>
       </c>
-      <c r="C27" s="9" t="s">
+      <c r="E27" s="5" t="s">
         <v>967</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="F27" s="5" t="s">
         <v>968</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="G27" s="5" t="s">
         <v>969</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="H27" s="5" t="s">
         <v>970</v>
       </c>
-      <c r="G27" s="5" t="s">
+      <c r="I27" s="9" t="s">
+        <v>965</v>
+      </c>
+      <c r="J27" s="5" t="s">
         <v>971</v>
       </c>
-      <c r="H27" s="5" t="s">
+      <c r="K27" s="5" t="s">
         <v>972</v>
       </c>
-      <c r="I27" s="9" t="s">
-        <v>967</v>
-      </c>
-      <c r="J27" s="5" t="s">
+      <c r="L27" s="5" t="s">
         <v>973</v>
       </c>
-      <c r="K27" s="5" t="s">
-        <v>974</v>
-      </c>
-      <c r="L27" s="5" t="s">
-        <v>975</v>
-      </c>
       <c r="M27" s="5" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="B28" s="5" t="s">
+        <v>974</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>975</v>
+      </c>
+      <c r="D28" s="6" t="s">
         <v>976</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="E28" s="5" t="s">
         <v>977</v>
       </c>
-      <c r="D28" s="6" t="s">
+      <c r="F28" s="5" t="s">
         <v>978</v>
       </c>
-      <c r="E28" s="5" t="s">
+      <c r="G28" s="5" t="s">
         <v>979</v>
       </c>
-      <c r="F28" s="5" t="s">
+      <c r="H28" s="5" t="s">
         <v>980</v>
       </c>
-      <c r="G28" s="5" t="s">
+      <c r="I28" s="9" t="s">
+        <v>975</v>
+      </c>
+      <c r="J28" s="5" t="s">
         <v>981</v>
       </c>
-      <c r="H28" s="5" t="s">
+      <c r="K28" s="5" t="s">
         <v>982</v>
       </c>
-      <c r="I28" s="9" t="s">
-        <v>977</v>
-      </c>
-      <c r="J28" s="5" t="s">
+      <c r="L28" s="5" t="s">
         <v>983</v>
       </c>
-      <c r="K28" s="5" t="s">
-        <v>984</v>
-      </c>
-      <c r="L28" s="5" t="s">
-        <v>985</v>
-      </c>
       <c r="M28" s="5" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B29" s="5" t="s">
+        <v>1017</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>1018</v>
+      </c>
+      <c r="D29" s="6" t="s">
         <v>1019</v>
       </c>
-      <c r="C29" s="9" t="s">
+      <c r="E29" s="5" t="s">
         <v>1020</v>
       </c>
-      <c r="D29" s="6" t="s">
+      <c r="F29" s="5" t="s">
         <v>1021</v>
       </c>
-      <c r="E29" s="5" t="s">
+      <c r="G29" s="5" t="s">
         <v>1022</v>
       </c>
-      <c r="F29" s="5" t="s">
+      <c r="H29" s="5" t="s">
         <v>1023</v>
       </c>
-      <c r="G29" s="5" t="s">
+      <c r="I29" s="9" t="s">
+        <v>1018</v>
+      </c>
+      <c r="J29" s="5" t="s">
         <v>1024</v>
       </c>
-      <c r="H29" s="5" t="s">
+      <c r="K29" s="5" t="s">
         <v>1025</v>
       </c>
-      <c r="I29" s="9" t="s">
-        <v>1020</v>
-      </c>
-      <c r="J29" s="5" t="s">
+      <c r="L29" s="5" t="s">
         <v>1026</v>
       </c>
-      <c r="K29" s="5" t="s">
-        <v>1027</v>
-      </c>
-      <c r="L29" s="5" t="s">
-        <v>1028</v>
-      </c>
       <c r="M29" s="5" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B30" s="5" t="s">
+        <v>1027</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>1028</v>
+      </c>
+      <c r="D30" s="6" t="s">
         <v>1029</v>
       </c>
-      <c r="C30" s="9" t="s">
+      <c r="E30" s="5" t="s">
         <v>1030</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="F30" s="5" t="s">
         <v>1031</v>
       </c>
-      <c r="E30" s="5" t="s">
+      <c r="G30" s="5" t="s">
         <v>1032</v>
       </c>
-      <c r="F30" s="5" t="s">
+      <c r="H30" s="5" t="s">
         <v>1033</v>
       </c>
-      <c r="G30" s="5" t="s">
+      <c r="I30" s="9" t="s">
+        <v>1028</v>
+      </c>
+      <c r="J30" s="5" t="s">
         <v>1034</v>
       </c>
-      <c r="H30" s="5" t="s">
+      <c r="K30" s="5" t="s">
         <v>1035</v>
       </c>
-      <c r="I30" s="9" t="s">
-        <v>1030</v>
-      </c>
-      <c r="J30" s="5" t="s">
+      <c r="L30" s="5" t="s">
         <v>1036</v>
       </c>
-      <c r="K30" s="5" t="s">
-        <v>1037</v>
-      </c>
-      <c r="L30" s="5" t="s">
-        <v>1038</v>
-      </c>
       <c r="M30" s="5" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B31" s="5" t="s">
+        <v>876</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>877</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>885</v>
+      </c>
+      <c r="E31" s="5" t="s">
         <v>878</v>
       </c>
-      <c r="C31" s="9" t="s">
+      <c r="F31" s="5" t="s">
         <v>879</v>
       </c>
-      <c r="D31" s="6" t="s">
-        <v>887</v>
-      </c>
-      <c r="E31" s="5" t="s">
+      <c r="G31" s="5" t="s">
         <v>880</v>
       </c>
-      <c r="F31" s="5" t="s">
+      <c r="H31" s="5" t="s">
         <v>881</v>
       </c>
-      <c r="G31" s="5" t="s">
+      <c r="I31" s="9" t="s">
+        <v>877</v>
+      </c>
+      <c r="J31" s="5" t="s">
         <v>882</v>
       </c>
-      <c r="H31" s="5" t="s">
+      <c r="K31" s="5" t="s">
         <v>883</v>
       </c>
-      <c r="I31" s="9" t="s">
-        <v>879</v>
-      </c>
-      <c r="J31" s="5" t="s">
+      <c r="L31" s="5" t="s">
         <v>884</v>
       </c>
-      <c r="K31" s="5" t="s">
-        <v>885</v>
-      </c>
-      <c r="L31" s="5" t="s">
-        <v>886</v>
-      </c>
       <c r="M31" s="5" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
+        <v>543</v>
+      </c>
+      <c r="B32" s="5" t="s">
         <v>544</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="C32" s="9" t="s">
         <v>545</v>
       </c>
-      <c r="C32" s="9" t="s">
+      <c r="D32" s="6" t="s">
+        <v>784</v>
+      </c>
+      <c r="E32" s="5" t="s">
         <v>546</v>
       </c>
-      <c r="D32" s="6" t="s">
-        <v>786</v>
-      </c>
-      <c r="E32" s="5" t="s">
+      <c r="F32" s="5" t="s">
         <v>547</v>
       </c>
-      <c r="F32" s="5" t="s">
+      <c r="G32" s="5" t="s">
         <v>548</v>
-      </c>
-      <c r="G32" s="5" t="s">
-        <v>549</v>
       </c>
       <c r="H32" s="5"/>
       <c r="I32" s="9" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="J32" s="5" t="s">
+        <v>549</v>
+      </c>
+      <c r="K32" s="5" t="s">
         <v>550</v>
       </c>
-      <c r="K32" s="5" t="s">
+      <c r="L32" s="5" t="s">
         <v>551</v>
       </c>
-      <c r="L32" s="5" t="s">
-        <v>552</v>
-      </c>
       <c r="M32" s="5" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
+        <v>552</v>
+      </c>
+      <c r="B33" s="5" t="s">
         <v>553</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="C33" s="9" t="s">
         <v>554</v>
       </c>
-      <c r="C33" s="9" t="s">
+      <c r="D33" s="6" t="s">
+        <v>785</v>
+      </c>
+      <c r="E33" s="5" t="s">
         <v>555</v>
       </c>
-      <c r="D33" s="6" t="s">
-        <v>787</v>
-      </c>
-      <c r="E33" s="5" t="s">
+      <c r="F33" s="5" t="s">
         <v>556</v>
       </c>
-      <c r="F33" s="5" t="s">
+      <c r="G33" s="5" t="s">
         <v>557</v>
-      </c>
-      <c r="G33" s="5" t="s">
-        <v>558</v>
       </c>
       <c r="H33" s="5"/>
       <c r="I33" s="9" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="J33" s="5" t="s">
+        <v>558</v>
+      </c>
+      <c r="K33" s="5" t="s">
         <v>559</v>
       </c>
-      <c r="K33" s="5" t="s">
+      <c r="L33" s="5" t="s">
         <v>560</v>
       </c>
-      <c r="L33" s="5" t="s">
-        <v>561</v>
-      </c>
       <c r="M33" s="5" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GDE-7309 Added data and script fix for TL_CAL_17
</commit_message>
<xml_diff>
--- a/DataSet/Integration_DataSet/TL/TL_Data_Set_AU.xlsx
+++ b/DataSet/Integration_DataSet/TL/TL_Data_Set_AU.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\Integration_DataSet\TL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB4AE0D-52C3-479E-9B19-57EE295E35F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D26727AD-ADCF-4954-BACB-5647926167AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30465" yWindow="5400" windowWidth="25890" windowHeight="10200" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BaseRate_Fields" sheetId="1" r:id="rId1"/>
@@ -1579,9 +1579,6 @@
     <t>TL_CAL_17</t>
   </si>
   <si>
-    <t>\DataSet\TL_DataSet\Calendar_GSFile\TL_CAL_17_Files\</t>
-  </si>
-  <si>
     <t>INPUTJSON_TL_CAL17</t>
   </si>
   <si>
@@ -2354,9 +2351,6 @@
   </si>
   <si>
     <t>Actual_ResponseMechanism_TL_BASE_42</t>
-  </si>
-  <si>
-    <t>Holidays_Banks_20190117_1.csv,Holidays_Banks_20190117_1.xlsx,Holidays_Banks_20190117_2.csv,Holidays_Banks_20190117_2.xlsx,Holidays_Misc_20190117.xlsx</t>
   </si>
   <si>
     <t>Holidays_Banks_20190118_1.csv,Holidays_Banks_20190118_1.xlsx,Holidays_Banks_20190118_2.csv,Holidays_Banks_20190118_2.xlsx,Holidays_Misc_20190118.xlsx</t>
@@ -3479,6 +3473,12 @@
   </si>
   <si>
     <t>Holidays_Banks_20200311_1.csv,Holidays_Banks_20200311_1.xlsx,Holidays_Banks_20200311_2.csv,Holidays_Banks_20200311_2.xlsx,Holidays_Misc_20200311.xlsx</t>
+  </si>
+  <si>
+    <t>\DataSet\Integration_DataSet\TL\Calendar_GSFile\TL_CAL_17_Files\</t>
+  </si>
+  <si>
+    <t>Holidays_Banks_20200517_1.csv,Holidays_Banks_20200517_1.xlsx,Holidays_Banks_20200517_2.csv,Holidays_Banks_20200517_2.xlsx,Holidays_Misc_20200517.xlsx</t>
   </si>
 </sst>
 </file>
@@ -4461,7 +4461,7 @@
         <v>17</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>1076</v>
+        <v>1074</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>1</v>
@@ -4494,7 +4494,7 @@
         <v>154</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
@@ -4505,10 +4505,10 @@
         <v>11</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>1078</v>
+        <v>1076</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>94</v>
@@ -4523,7 +4523,7 @@
         <v>18</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>1078</v>
+        <v>1076</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>21</v>
@@ -4546,10 +4546,10 @@
         <v>23</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>1087</v>
+        <v>1085</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>95</v>
@@ -4564,7 +4564,7 @@
         <v>25</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>1087</v>
+        <v>1085</v>
       </c>
       <c r="J3" s="5" t="s">
         <v>26</v>
@@ -4587,10 +4587,10 @@
         <v>30</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>1088</v>
+        <v>1086</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>140</v>
@@ -4605,7 +4605,7 @@
         <v>33</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>1088</v>
+        <v>1086</v>
       </c>
       <c r="J4" s="5" t="s">
         <v>34</v>
@@ -4617,7 +4617,7 @@
         <v>135</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
@@ -4628,10 +4628,10 @@
         <v>37</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>1089</v>
+        <v>1087</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>153</v>
@@ -4646,7 +4646,7 @@
         <v>40</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>1089</v>
+        <v>1087</v>
       </c>
       <c r="J5" s="5" t="s">
         <v>41</v>
@@ -4669,10 +4669,10 @@
         <v>50</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>1090</v>
+        <v>1088</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>51</v>
@@ -4687,7 +4687,7 @@
         <v>54</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>1090</v>
+        <v>1088</v>
       </c>
       <c r="J6" s="5" t="s">
         <v>55</v>
@@ -4710,13 +4710,13 @@
         <v>58</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>1091</v>
+        <v>1089</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>59</v>
@@ -4728,7 +4728,7 @@
         <v>61</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>1091</v>
+        <v>1089</v>
       </c>
       <c r="J7" s="5" t="s">
         <v>62</v>
@@ -4740,7 +4740,7 @@
         <v>138</v>
       </c>
       <c r="M7" s="5" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
@@ -4751,13 +4751,13 @@
         <v>65</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>1092</v>
+        <v>1090</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>66</v>
@@ -4769,7 +4769,7 @@
         <v>68</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>1092</v>
+        <v>1090</v>
       </c>
       <c r="J8" s="5" t="s">
         <v>69</v>
@@ -4778,10 +4778,10 @@
         <v>70</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
@@ -4792,13 +4792,13 @@
         <v>97</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>1093</v>
+        <v>1091</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>98</v>
@@ -4810,7 +4810,7 @@
         <v>100</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>1093</v>
+        <v>1091</v>
       </c>
       <c r="J9" s="5" t="s">
         <v>101</v>
@@ -4819,10 +4819,10 @@
         <v>102</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="M9" s="5" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
@@ -4833,10 +4833,10 @@
         <v>104</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>1094</v>
+        <v>1092</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>105</v>
@@ -4851,7 +4851,7 @@
         <v>108</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>1094</v>
+        <v>1092</v>
       </c>
       <c r="J10" s="5" t="s">
         <v>109</v>
@@ -4860,10 +4860,10 @@
         <v>110</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="M10" s="5" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
@@ -4874,10 +4874,10 @@
         <v>156</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>1095</v>
+        <v>1093</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>112</v>
@@ -4892,7 +4892,7 @@
         <v>159</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>1095</v>
+        <v>1093</v>
       </c>
       <c r="J11" s="5" t="s">
         <v>160</v>
@@ -4915,10 +4915,10 @@
         <v>169</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>1097</v>
+        <v>1095</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>114</v>
@@ -4933,7 +4933,7 @@
         <v>191</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>1097</v>
+        <v>1095</v>
       </c>
       <c r="J12" s="5" t="s">
         <v>196</v>
@@ -4956,10 +4956,10 @@
         <v>170</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>1098</v>
+        <v>1096</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>116</v>
@@ -4974,7 +4974,7 @@
         <v>192</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>1098</v>
+        <v>1096</v>
       </c>
       <c r="J13" s="5" t="s">
         <v>197</v>
@@ -4997,10 +4997,10 @@
         <v>171</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>1099</v>
+        <v>1097</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>118</v>
@@ -5015,7 +5015,7 @@
         <v>193</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>1099</v>
+        <v>1097</v>
       </c>
       <c r="J14" s="5" t="s">
         <v>198</v>
@@ -5038,10 +5038,10 @@
         <v>172</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>1100</v>
+        <v>1098</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>120</v>
@@ -5056,7 +5056,7 @@
         <v>194</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>1100</v>
+        <v>1098</v>
       </c>
       <c r="J15" s="5" t="s">
         <v>199</v>
@@ -5079,10 +5079,10 @@
         <v>173</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>1101</v>
+        <v>1099</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>152</v>
@@ -5097,7 +5097,7 @@
         <v>148</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>1101</v>
+        <v>1099</v>
       </c>
       <c r="J16" s="5" t="s">
         <v>149</v>
@@ -5117,40 +5117,40 @@
         <v>332</v>
       </c>
       <c r="B17" s="5" t="s">
+        <v>892</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>1075</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>1100</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>893</v>
+      </c>
+      <c r="F17" s="5" t="s">
         <v>894</v>
       </c>
-      <c r="C17" s="9" t="s">
-        <v>1077</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>1102</v>
-      </c>
-      <c r="E17" s="5" t="s">
+      <c r="G17" s="5" t="s">
         <v>895</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="H17" s="5" t="s">
         <v>896</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="I17" s="9" t="s">
+        <v>1100</v>
+      </c>
+      <c r="J17" s="5" t="s">
         <v>897</v>
       </c>
-      <c r="H17" s="5" t="s">
+      <c r="K17" s="5" t="s">
         <v>898</v>
       </c>
-      <c r="I17" s="9" t="s">
-        <v>1102</v>
-      </c>
-      <c r="J17" s="5" t="s">
+      <c r="L17" s="5" t="s">
         <v>899</v>
       </c>
-      <c r="K17" s="5" t="s">
+      <c r="M17" s="5" t="s">
         <v>900</v>
-      </c>
-      <c r="L17" s="5" t="s">
-        <v>901</v>
-      </c>
-      <c r="M17" s="5" t="s">
-        <v>902</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
@@ -5158,40 +5158,40 @@
         <v>342</v>
       </c>
       <c r="B18" s="5" t="s">
+        <v>1039</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>1075</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>1101</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>1040</v>
+      </c>
+      <c r="F18" s="5" t="s">
         <v>1041</v>
       </c>
-      <c r="C18" s="9" t="s">
-        <v>1077</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>1103</v>
-      </c>
-      <c r="E18" s="5" t="s">
+      <c r="G18" s="5" t="s">
         <v>1042</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="H18" s="5" t="s">
         <v>1043</v>
       </c>
-      <c r="G18" s="5" t="s">
+      <c r="I18" s="9" t="s">
+        <v>1101</v>
+      </c>
+      <c r="J18" s="5" t="s">
         <v>1044</v>
       </c>
-      <c r="H18" s="5" t="s">
+      <c r="K18" s="5" t="s">
         <v>1045</v>
       </c>
-      <c r="I18" s="9" t="s">
-        <v>1103</v>
-      </c>
-      <c r="J18" s="5" t="s">
+      <c r="L18" s="5" t="s">
         <v>1046</v>
       </c>
-      <c r="K18" s="5" t="s">
+      <c r="M18" s="5" t="s">
         <v>1047</v>
-      </c>
-      <c r="L18" s="5" t="s">
-        <v>1048</v>
-      </c>
-      <c r="M18" s="5" t="s">
-        <v>1049</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
@@ -5199,40 +5199,40 @@
         <v>352</v>
       </c>
       <c r="B19" s="5" t="s">
+        <v>981</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>1075</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>1102</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>982</v>
+      </c>
+      <c r="F19" s="5" t="s">
         <v>983</v>
       </c>
-      <c r="C19" s="9" t="s">
-        <v>1077</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>1104</v>
-      </c>
-      <c r="E19" s="5" t="s">
+      <c r="G19" s="5" t="s">
         <v>984</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="H19" s="5" t="s">
         <v>985</v>
       </c>
-      <c r="G19" s="5" t="s">
+      <c r="I19" s="9" t="s">
+        <v>1102</v>
+      </c>
+      <c r="J19" s="5" t="s">
         <v>986</v>
       </c>
-      <c r="H19" s="5" t="s">
+      <c r="K19" s="5" t="s">
         <v>987</v>
       </c>
-      <c r="I19" s="9" t="s">
-        <v>1104</v>
-      </c>
-      <c r="J19" s="5" t="s">
+      <c r="L19" s="5" t="s">
         <v>988</v>
       </c>
-      <c r="K19" s="5" t="s">
+      <c r="M19" s="5" t="s">
         <v>989</v>
-      </c>
-      <c r="L19" s="5" t="s">
-        <v>990</v>
-      </c>
-      <c r="M19" s="5" t="s">
-        <v>991</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
@@ -5243,10 +5243,10 @@
         <v>174</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>1105</v>
+        <v>1103</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>206</v>
@@ -5261,7 +5261,7 @@
         <v>195</v>
       </c>
       <c r="I20" s="9" t="s">
-        <v>1105</v>
+        <v>1103</v>
       </c>
       <c r="J20" s="5" t="s">
         <v>200</v>
@@ -5284,10 +5284,10 @@
         <v>219</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>1106</v>
+        <v>1104</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>210</v>
@@ -5302,7 +5302,7 @@
         <v>214</v>
       </c>
       <c r="I21" s="9" t="s">
-        <v>1106</v>
+        <v>1104</v>
       </c>
       <c r="J21" s="5" t="s">
         <v>215</v>
@@ -5325,10 +5325,10 @@
         <v>220</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>1096</v>
+        <v>1094</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>221</v>
@@ -5343,7 +5343,7 @@
         <v>224</v>
       </c>
       <c r="I22" s="9" t="s">
-        <v>1096</v>
+        <v>1094</v>
       </c>
       <c r="J22" s="5" t="s">
         <v>225</v>
@@ -5366,10 +5366,10 @@
         <v>230</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>1107</v>
+        <v>1105</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>239</v>
@@ -5384,7 +5384,7 @@
         <v>234</v>
       </c>
       <c r="I23" s="9" t="s">
-        <v>1107</v>
+        <v>1105</v>
       </c>
       <c r="J23" s="5" t="s">
         <v>235</v>
@@ -5404,40 +5404,40 @@
         <v>427</v>
       </c>
       <c r="B24" s="5" t="s">
+        <v>559</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>1075</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>1106</v>
+      </c>
+      <c r="E24" s="6" t="s">
         <v>560</v>
       </c>
-      <c r="C24" s="9" t="s">
-        <v>1077</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>1108</v>
-      </c>
-      <c r="E24" s="6" t="s">
+      <c r="F24" s="5" t="s">
         <v>561</v>
       </c>
-      <c r="F24" s="5" t="s">
+      <c r="G24" s="5" t="s">
         <v>562</v>
       </c>
-      <c r="G24" s="5" t="s">
+      <c r="H24" s="5" t="s">
         <v>563</v>
       </c>
-      <c r="H24" s="5" t="s">
+      <c r="I24" s="9" t="s">
+        <v>1106</v>
+      </c>
+      <c r="J24" s="5" t="s">
         <v>564</v>
       </c>
-      <c r="I24" s="9" t="s">
-        <v>1108</v>
-      </c>
-      <c r="J24" s="5" t="s">
+      <c r="K24" s="5" t="s">
         <v>565</v>
       </c>
-      <c r="K24" s="5" t="s">
+      <c r="L24" s="5" t="s">
         <v>566</v>
       </c>
-      <c r="L24" s="5" t="s">
+      <c r="M24" s="5" t="s">
         <v>567</v>
-      </c>
-      <c r="M24" s="5" t="s">
-        <v>568</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
@@ -5445,40 +5445,40 @@
         <v>437</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>1109</v>
+        <v>1107</v>
       </c>
       <c r="E25" s="6" t="s">
+        <v>568</v>
+      </c>
+      <c r="F25" s="5" t="s">
         <v>569</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="G25" s="5" t="s">
         <v>570</v>
       </c>
-      <c r="G25" s="5" t="s">
+      <c r="H25" s="5" t="s">
         <v>571</v>
       </c>
-      <c r="H25" s="5" t="s">
+      <c r="I25" s="9" t="s">
+        <v>1107</v>
+      </c>
+      <c r="J25" s="5" t="s">
         <v>572</v>
       </c>
-      <c r="I25" s="9" t="s">
-        <v>1109</v>
-      </c>
-      <c r="J25" s="5" t="s">
+      <c r="K25" s="5" t="s">
         <v>573</v>
       </c>
-      <c r="K25" s="5" t="s">
+      <c r="L25" s="5" t="s">
         <v>574</v>
       </c>
-      <c r="L25" s="5" t="s">
+      <c r="M25" s="5" t="s">
         <v>575</v>
-      </c>
-      <c r="M25" s="5" t="s">
-        <v>576</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -5486,40 +5486,40 @@
         <v>447</v>
       </c>
       <c r="B26" s="5" t="s">
+        <v>690</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>1075</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>1108</v>
+      </c>
+      <c r="E26" s="6" t="s">
         <v>691</v>
       </c>
-      <c r="C26" s="9" t="s">
-        <v>1077</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>1110</v>
-      </c>
-      <c r="E26" s="6" t="s">
+      <c r="F26" s="5" t="s">
         <v>692</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="G26" s="5" t="s">
         <v>693</v>
       </c>
-      <c r="G26" s="5" t="s">
+      <c r="H26" s="5" t="s">
         <v>694</v>
       </c>
-      <c r="H26" s="5" t="s">
+      <c r="I26" s="9" t="s">
+        <v>1108</v>
+      </c>
+      <c r="J26" s="5" t="s">
         <v>695</v>
       </c>
-      <c r="I26" s="9" t="s">
-        <v>1110</v>
-      </c>
-      <c r="J26" s="5" t="s">
+      <c r="K26" s="5" t="s">
         <v>696</v>
       </c>
-      <c r="K26" s="5" t="s">
+      <c r="L26" s="5" t="s">
         <v>697</v>
       </c>
-      <c r="L26" s="5" t="s">
+      <c r="M26" s="5" t="s">
         <v>698</v>
-      </c>
-      <c r="M26" s="5" t="s">
-        <v>699</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
@@ -5527,40 +5527,40 @@
         <v>457</v>
       </c>
       <c r="B27" s="5" t="s">
+        <v>1048</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>1075</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>1084</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>1049</v>
+      </c>
+      <c r="F27" s="5" t="s">
         <v>1050</v>
       </c>
-      <c r="C27" s="9" t="s">
-        <v>1077</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>1086</v>
-      </c>
-      <c r="E27" s="5" t="s">
+      <c r="G27" s="5" t="s">
         <v>1051</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="H27" s="5" t="s">
         <v>1052</v>
       </c>
-      <c r="G27" s="5" t="s">
+      <c r="I27" s="9" t="s">
+        <v>1084</v>
+      </c>
+      <c r="J27" s="5" t="s">
         <v>1053</v>
       </c>
-      <c r="H27" s="5" t="s">
+      <c r="K27" s="5" t="s">
         <v>1054</v>
       </c>
-      <c r="I27" s="9" t="s">
-        <v>1086</v>
-      </c>
-      <c r="J27" s="5" t="s">
+      <c r="L27" s="5" t="s">
         <v>1055</v>
       </c>
-      <c r="K27" s="5" t="s">
+      <c r="M27" s="5" t="s">
         <v>1056</v>
-      </c>
-      <c r="L27" s="5" t="s">
-        <v>1057</v>
-      </c>
-      <c r="M27" s="5" t="s">
-        <v>1058</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
@@ -5568,618 +5568,618 @@
         <v>467</v>
       </c>
       <c r="B28" s="5" t="s">
+        <v>664</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>1075</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>1109</v>
+      </c>
+      <c r="E28" s="6" t="s">
         <v>665</v>
       </c>
-      <c r="C28" s="9" t="s">
-        <v>1077</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>1111</v>
-      </c>
-      <c r="E28" s="6" t="s">
+      <c r="F28" s="5" t="s">
         <v>666</v>
       </c>
-      <c r="F28" s="5" t="s">
+      <c r="G28" s="5" t="s">
         <v>667</v>
       </c>
-      <c r="G28" s="5" t="s">
+      <c r="H28" s="5" t="s">
         <v>668</v>
       </c>
-      <c r="H28" s="5" t="s">
+      <c r="I28" s="9" t="s">
+        <v>1109</v>
+      </c>
+      <c r="J28" s="5" t="s">
         <v>669</v>
       </c>
-      <c r="I28" s="9" t="s">
-        <v>1111</v>
-      </c>
-      <c r="J28" s="5" t="s">
+      <c r="K28" s="5" t="s">
         <v>670</v>
       </c>
-      <c r="K28" s="5" t="s">
+      <c r="L28" s="5" t="s">
         <v>671</v>
       </c>
-      <c r="L28" s="5" t="s">
+      <c r="M28" s="5" t="s">
         <v>672</v>
-      </c>
-      <c r="M28" s="5" t="s">
-        <v>673</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="11" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B29" s="5" t="s">
+        <v>673</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>1075</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>1110</v>
+      </c>
+      <c r="E29" s="6" t="s">
         <v>674</v>
       </c>
-      <c r="C29" s="9" t="s">
-        <v>1077</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>1112</v>
-      </c>
-      <c r="E29" s="6" t="s">
+      <c r="F29" s="5" t="s">
         <v>675</v>
       </c>
-      <c r="F29" s="5" t="s">
+      <c r="G29" s="5" t="s">
         <v>676</v>
       </c>
-      <c r="G29" s="5" t="s">
+      <c r="H29" s="5" t="s">
         <v>677</v>
       </c>
-      <c r="H29" s="5" t="s">
+      <c r="I29" s="9" t="s">
+        <v>1110</v>
+      </c>
+      <c r="J29" s="5" t="s">
         <v>678</v>
       </c>
-      <c r="I29" s="9" t="s">
-        <v>1112</v>
-      </c>
-      <c r="J29" s="5" t="s">
+      <c r="K29" s="5" t="s">
         <v>679</v>
       </c>
-      <c r="K29" s="5" t="s">
+      <c r="L29" s="5" t="s">
         <v>680</v>
       </c>
-      <c r="L29" s="5" t="s">
+      <c r="M29" s="5" t="s">
         <v>681</v>
-      </c>
-      <c r="M29" s="5" t="s">
-        <v>682</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B30" s="5" t="s">
+        <v>707</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>1075</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>1111</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>721</v>
+      </c>
+      <c r="F30" s="5" t="s">
         <v>708</v>
       </c>
-      <c r="C30" s="9" t="s">
-        <v>1077</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>1113</v>
-      </c>
-      <c r="E30" s="6" t="s">
+      <c r="G30" s="5" t="s">
+        <v>709</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>710</v>
+      </c>
+      <c r="I30" s="9" t="s">
+        <v>1111</v>
+      </c>
+      <c r="J30" s="5" t="s">
+        <v>711</v>
+      </c>
+      <c r="K30" s="5" t="s">
+        <v>712</v>
+      </c>
+      <c r="L30" s="5" t="s">
         <v>722</v>
       </c>
-      <c r="F30" s="5" t="s">
-        <v>709</v>
-      </c>
-      <c r="G30" s="5" t="s">
-        <v>710</v>
-      </c>
-      <c r="H30" s="5" t="s">
-        <v>711</v>
-      </c>
-      <c r="I30" s="9" t="s">
-        <v>1113</v>
-      </c>
-      <c r="J30" s="5" t="s">
-        <v>712</v>
-      </c>
-      <c r="K30" s="5" t="s">
+      <c r="M30" s="5" t="s">
         <v>713</v>
-      </c>
-      <c r="L30" s="5" t="s">
-        <v>723</v>
-      </c>
-      <c r="M30" s="5" t="s">
-        <v>714</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="11" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="B31" s="5" t="s">
+        <v>707</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>1075</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>1111</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>719</v>
+      </c>
+      <c r="F31" s="5" t="s">
         <v>708</v>
       </c>
-      <c r="C31" s="9" t="s">
-        <v>1077</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>1113</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>720</v>
-      </c>
-      <c r="F31" s="5" t="s">
+      <c r="G31" s="5" t="s">
         <v>709</v>
       </c>
-      <c r="G31" s="5" t="s">
+      <c r="H31" s="5" t="s">
         <v>710</v>
       </c>
-      <c r="H31" s="5" t="s">
+      <c r="I31" s="9" t="s">
+        <v>1111</v>
+      </c>
+      <c r="J31" s="5" t="s">
         <v>711</v>
       </c>
-      <c r="I31" s="9" t="s">
-        <v>1113</v>
-      </c>
-      <c r="J31" s="5" t="s">
+      <c r="K31" s="5" t="s">
         <v>712</v>
       </c>
-      <c r="K31" s="5" t="s">
+      <c r="L31" s="5" t="s">
+        <v>723</v>
+      </c>
+      <c r="M31" s="5" t="s">
         <v>713</v>
-      </c>
-      <c r="L31" s="5" t="s">
-        <v>724</v>
-      </c>
-      <c r="M31" s="5" t="s">
-        <v>714</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B32" s="5" t="s">
+        <v>901</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>1075</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>1112</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>902</v>
+      </c>
+      <c r="F32" s="5" t="s">
         <v>903</v>
       </c>
-      <c r="C32" s="9" t="s">
-        <v>1077</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>1114</v>
-      </c>
-      <c r="E32" s="6" t="s">
+      <c r="G32" s="5" t="s">
         <v>904</v>
       </c>
-      <c r="F32" s="5" t="s">
+      <c r="H32" s="5" t="s">
         <v>905</v>
       </c>
-      <c r="G32" s="5" t="s">
+      <c r="I32" s="9" t="s">
+        <v>1112</v>
+      </c>
+      <c r="J32" s="5" t="s">
         <v>906</v>
       </c>
-      <c r="H32" s="5" t="s">
+      <c r="K32" s="5" t="s">
         <v>907</v>
       </c>
-      <c r="I32" s="9" t="s">
-        <v>1114</v>
-      </c>
-      <c r="J32" s="5" t="s">
+      <c r="L32" s="5" t="s">
         <v>908</v>
       </c>
-      <c r="K32" s="5" t="s">
+      <c r="M32" s="5" t="s">
         <v>909</v>
-      </c>
-      <c r="L32" s="5" t="s">
-        <v>910</v>
-      </c>
-      <c r="M32" s="5" t="s">
-        <v>911</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" s="11" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B33" s="5" t="s">
+        <v>910</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>1075</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>1113</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>911</v>
+      </c>
+      <c r="F33" s="5" t="s">
         <v>912</v>
       </c>
-      <c r="C33" s="9" t="s">
-        <v>1077</v>
-      </c>
-      <c r="D33" s="9" t="s">
-        <v>1115</v>
-      </c>
-      <c r="E33" s="6" t="s">
+      <c r="G33" s="5" t="s">
         <v>913</v>
       </c>
-      <c r="F33" s="5" t="s">
+      <c r="H33" s="5" t="s">
         <v>914</v>
       </c>
-      <c r="G33" s="5" t="s">
+      <c r="I33" s="9" t="s">
+        <v>1113</v>
+      </c>
+      <c r="J33" s="5" t="s">
         <v>915</v>
       </c>
-      <c r="H33" s="5" t="s">
+      <c r="K33" s="5" t="s">
         <v>916</v>
       </c>
-      <c r="I33" s="9" t="s">
-        <v>1115</v>
-      </c>
-      <c r="J33" s="5" t="s">
+      <c r="L33" s="5" t="s">
         <v>917</v>
       </c>
-      <c r="K33" s="5" t="s">
+      <c r="M33" s="5" t="s">
         <v>918</v>
-      </c>
-      <c r="L33" s="5" t="s">
-        <v>919</v>
-      </c>
-      <c r="M33" s="5" t="s">
-        <v>920</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" s="11" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B34" s="5" t="s">
+        <v>919</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>1075</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>1114</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>920</v>
+      </c>
+      <c r="F34" s="5" t="s">
         <v>921</v>
       </c>
-      <c r="C34" s="9" t="s">
-        <v>1077</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>1116</v>
-      </c>
-      <c r="E34" s="6" t="s">
+      <c r="G34" s="5" t="s">
         <v>922</v>
       </c>
-      <c r="F34" s="5" t="s">
+      <c r="H34" s="5" t="s">
         <v>923</v>
       </c>
-      <c r="G34" s="5" t="s">
+      <c r="I34" s="9" t="s">
+        <v>1114</v>
+      </c>
+      <c r="J34" s="5" t="s">
         <v>924</v>
       </c>
-      <c r="H34" s="5" t="s">
+      <c r="K34" s="5" t="s">
         <v>925</v>
       </c>
-      <c r="I34" s="9" t="s">
-        <v>1116</v>
-      </c>
-      <c r="J34" s="5" t="s">
+      <c r="L34" s="5" t="s">
         <v>926</v>
       </c>
-      <c r="K34" s="5" t="s">
+      <c r="M34" s="5" t="s">
         <v>927</v>
-      </c>
-      <c r="L34" s="5" t="s">
-        <v>928</v>
-      </c>
-      <c r="M34" s="5" t="s">
-        <v>929</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" s="11" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B35" s="5" t="s">
+        <v>928</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>1075</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>1115</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>929</v>
+      </c>
+      <c r="F35" s="5" t="s">
         <v>930</v>
       </c>
-      <c r="C35" s="9" t="s">
-        <v>1077</v>
-      </c>
-      <c r="D35" s="9" t="s">
-        <v>1117</v>
-      </c>
-      <c r="E35" s="6" t="s">
+      <c r="G35" s="5" t="s">
         <v>931</v>
       </c>
-      <c r="F35" s="5" t="s">
+      <c r="H35" s="5" t="s">
         <v>932</v>
       </c>
-      <c r="G35" s="5" t="s">
+      <c r="I35" s="9" t="s">
+        <v>1115</v>
+      </c>
+      <c r="J35" s="5" t="s">
         <v>933</v>
       </c>
-      <c r="H35" s="5" t="s">
+      <c r="K35" s="5" t="s">
         <v>934</v>
       </c>
-      <c r="I35" s="9" t="s">
-        <v>1117</v>
-      </c>
-      <c r="J35" s="5" t="s">
+      <c r="L35" s="5" t="s">
         <v>935</v>
       </c>
-      <c r="K35" s="5" t="s">
+      <c r="M35" s="5" t="s">
         <v>936</v>
-      </c>
-      <c r="L35" s="5" t="s">
-        <v>937</v>
-      </c>
-      <c r="M35" s="5" t="s">
-        <v>938</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36" s="11" t="s">
+        <v>937</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>938</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>1075</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>1083</v>
+      </c>
+      <c r="E36" s="6" t="s">
         <v>939</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="F36" s="5" t="s">
         <v>940</v>
       </c>
-      <c r="C36" s="9" t="s">
-        <v>1077</v>
-      </c>
-      <c r="D36" s="9" t="s">
-        <v>1085</v>
-      </c>
-      <c r="E36" s="6" t="s">
+      <c r="G36" s="5" t="s">
         <v>941</v>
       </c>
-      <c r="F36" s="5" t="s">
+      <c r="H36" s="5" t="s">
         <v>942</v>
       </c>
-      <c r="G36" s="5" t="s">
+      <c r="I36" s="9" t="s">
+        <v>1083</v>
+      </c>
+      <c r="J36" s="5" t="s">
         <v>943</v>
       </c>
-      <c r="H36" s="5" t="s">
+      <c r="K36" s="5" t="s">
         <v>944</v>
       </c>
-      <c r="I36" s="9" t="s">
-        <v>1085</v>
-      </c>
-      <c r="J36" s="5" t="s">
+      <c r="L36" s="5" t="s">
         <v>945</v>
       </c>
-      <c r="K36" s="5" t="s">
+      <c r="M36" s="5" t="s">
         <v>946</v>
-      </c>
-      <c r="L36" s="5" t="s">
-        <v>947</v>
-      </c>
-      <c r="M36" s="5" t="s">
-        <v>948</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
+        <v>1057</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>1058</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>1075</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>1116</v>
+      </c>
+      <c r="E37" s="5" t="s">
         <v>1059</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="F37" s="5" t="s">
         <v>1060</v>
       </c>
-      <c r="C37" s="9" t="s">
-        <v>1077</v>
-      </c>
-      <c r="D37" s="9" t="s">
-        <v>1118</v>
-      </c>
-      <c r="E37" s="5" t="s">
+      <c r="G37" s="5" t="s">
         <v>1061</v>
       </c>
-      <c r="F37" s="5" t="s">
+      <c r="H37" s="5" t="s">
         <v>1062</v>
       </c>
-      <c r="G37" s="5" t="s">
+      <c r="I37" s="9" t="s">
+        <v>1116</v>
+      </c>
+      <c r="J37" s="5" t="s">
         <v>1063</v>
       </c>
-      <c r="H37" s="5" t="s">
+      <c r="K37" s="5" t="s">
         <v>1064</v>
       </c>
-      <c r="I37" s="9" t="s">
-        <v>1118</v>
-      </c>
-      <c r="J37" s="5" t="s">
+      <c r="L37" s="5" t="s">
         <v>1065</v>
       </c>
-      <c r="K37" s="5" t="s">
+      <c r="M37" s="5" t="s">
         <v>1066</v>
-      </c>
-      <c r="L37" s="5" t="s">
-        <v>1067</v>
-      </c>
-      <c r="M37" s="5" t="s">
-        <v>1068</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A38" s="11" t="s">
+        <v>724</v>
+      </c>
+      <c r="B38" s="5" t="s">
         <v>725</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="C38" s="9" t="s">
+        <v>1075</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>1117</v>
+      </c>
+      <c r="E38" s="6" t="s">
         <v>726</v>
       </c>
-      <c r="C38" s="9" t="s">
-        <v>1077</v>
-      </c>
-      <c r="D38" s="9" t="s">
-        <v>1119</v>
-      </c>
-      <c r="E38" s="6" t="s">
+      <c r="F38" s="5" t="s">
         <v>727</v>
       </c>
-      <c r="F38" s="5" t="s">
+      <c r="G38" s="5" t="s">
         <v>728</v>
       </c>
-      <c r="G38" s="5" t="s">
+      <c r="H38" s="5" t="s">
         <v>729</v>
       </c>
-      <c r="H38" s="5" t="s">
+      <c r="I38" s="9" t="s">
+        <v>1117</v>
+      </c>
+      <c r="J38" s="5" t="s">
         <v>730</v>
       </c>
-      <c r="I38" s="9" t="s">
-        <v>1119</v>
-      </c>
-      <c r="J38" s="5" t="s">
+      <c r="K38" s="5" t="s">
         <v>731</v>
       </c>
-      <c r="K38" s="5" t="s">
+      <c r="L38" s="5" t="s">
         <v>732</v>
       </c>
-      <c r="L38" s="5" t="s">
+      <c r="M38" s="5" t="s">
         <v>733</v>
-      </c>
-      <c r="M38" s="5" t="s">
-        <v>734</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A39" s="11" t="s">
+        <v>754</v>
+      </c>
+      <c r="B39" s="5" t="s">
         <v>755</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="C39" s="9" t="s">
+        <v>1075</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>1118</v>
+      </c>
+      <c r="E39" s="6" t="s">
         <v>756</v>
       </c>
-      <c r="C39" s="9" t="s">
-        <v>1077</v>
-      </c>
-      <c r="D39" s="9" t="s">
-        <v>1120</v>
-      </c>
-      <c r="E39" s="6" t="s">
+      <c r="F39" s="5" t="s">
         <v>757</v>
       </c>
-      <c r="F39" s="5" t="s">
+      <c r="G39" s="5" t="s">
         <v>758</v>
       </c>
-      <c r="G39" s="5" t="s">
+      <c r="H39" s="5" t="s">
         <v>759</v>
       </c>
-      <c r="H39" s="5" t="s">
+      <c r="I39" s="9" t="s">
+        <v>1118</v>
+      </c>
+      <c r="J39" s="5" t="s">
         <v>760</v>
       </c>
-      <c r="I39" s="9" t="s">
-        <v>1120</v>
-      </c>
-      <c r="J39" s="5" t="s">
+      <c r="K39" s="5" t="s">
         <v>761</v>
       </c>
-      <c r="K39" s="5" t="s">
+      <c r="L39" s="5" t="s">
         <v>762</v>
       </c>
-      <c r="L39" s="5" t="s">
+      <c r="M39" s="5" t="s">
         <v>763</v>
       </c>
-      <c r="M39" s="5" t="s">
-        <v>764</v>
-      </c>
       <c r="N39" s="5" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A40" s="11" t="s">
+        <v>766</v>
+      </c>
+      <c r="B40" s="5" t="s">
         <v>767</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="C40" s="9" t="s">
+        <v>1075</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>1119</v>
+      </c>
+      <c r="E40" s="6" t="s">
         <v>768</v>
       </c>
-      <c r="C40" s="9" t="s">
-        <v>1077</v>
-      </c>
-      <c r="D40" s="9" t="s">
-        <v>1121</v>
-      </c>
-      <c r="E40" s="6" t="s">
+      <c r="F40" s="5" t="s">
         <v>769</v>
       </c>
-      <c r="F40" s="5" t="s">
+      <c r="G40" s="5" t="s">
         <v>770</v>
       </c>
-      <c r="G40" s="5" t="s">
+      <c r="H40" s="5" t="s">
         <v>771</v>
       </c>
-      <c r="H40" s="5" t="s">
+      <c r="I40" s="9" t="s">
+        <v>1119</v>
+      </c>
+      <c r="J40" s="5" t="s">
         <v>772</v>
       </c>
-      <c r="I40" s="9" t="s">
-        <v>1121</v>
-      </c>
-      <c r="J40" s="5" t="s">
+      <c r="K40" s="5" t="s">
         <v>773</v>
       </c>
-      <c r="K40" s="5" t="s">
+      <c r="L40" s="5" t="s">
         <v>774</v>
       </c>
-      <c r="L40" s="5" t="s">
+      <c r="M40" s="5" t="s">
         <v>775</v>
-      </c>
-      <c r="M40" s="5" t="s">
-        <v>776</v>
       </c>
       <c r="N40" s="5"/>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A41" s="11" t="s">
+        <v>734</v>
+      </c>
+      <c r="B41" s="5" t="s">
         <v>735</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="C41" s="9" t="s">
+        <v>1075</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>1120</v>
+      </c>
+      <c r="E41" s="6" t="s">
         <v>736</v>
       </c>
-      <c r="C41" s="9" t="s">
-        <v>1077</v>
-      </c>
-      <c r="D41" s="9" t="s">
-        <v>1122</v>
-      </c>
-      <c r="E41" s="6" t="s">
+      <c r="F41" s="5" t="s">
         <v>737</v>
       </c>
-      <c r="F41" s="5" t="s">
+      <c r="G41" s="5" t="s">
         <v>738</v>
       </c>
-      <c r="G41" s="5" t="s">
+      <c r="H41" s="5" t="s">
         <v>739</v>
       </c>
-      <c r="H41" s="5" t="s">
+      <c r="I41" s="9" t="s">
+        <v>1120</v>
+      </c>
+      <c r="J41" s="5" t="s">
         <v>740</v>
       </c>
-      <c r="I41" s="9" t="s">
-        <v>1122</v>
-      </c>
-      <c r="J41" s="5" t="s">
+      <c r="K41" s="5" t="s">
         <v>741</v>
       </c>
-      <c r="K41" s="5" t="s">
+      <c r="L41" s="5" t="s">
         <v>742</v>
       </c>
-      <c r="L41" s="5" t="s">
+      <c r="M41" s="5" t="s">
         <v>743</v>
-      </c>
-      <c r="M41" s="5" t="s">
-        <v>744</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A42" s="11" t="s">
+        <v>744</v>
+      </c>
+      <c r="B42" s="5" t="s">
         <v>745</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="C42" s="9" t="s">
+        <v>1075</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>1121</v>
+      </c>
+      <c r="E42" s="6" t="s">
         <v>746</v>
       </c>
-      <c r="C42" s="9" t="s">
-        <v>1077</v>
-      </c>
-      <c r="D42" s="9" t="s">
-        <v>1123</v>
-      </c>
-      <c r="E42" s="6" t="s">
+      <c r="F42" s="5" t="s">
         <v>747</v>
       </c>
-      <c r="F42" s="5" t="s">
+      <c r="G42" s="5" t="s">
         <v>748</v>
       </c>
-      <c r="G42" s="5" t="s">
+      <c r="H42" s="5" t="s">
         <v>749</v>
       </c>
-      <c r="H42" s="5" t="s">
+      <c r="I42" s="9" t="s">
+        <v>1121</v>
+      </c>
+      <c r="J42" s="5" t="s">
         <v>750</v>
       </c>
-      <c r="I42" s="9" t="s">
-        <v>1123</v>
-      </c>
-      <c r="J42" s="5" t="s">
+      <c r="K42" s="5" t="s">
         <v>751</v>
       </c>
-      <c r="K42" s="5" t="s">
+      <c r="L42" s="5" t="s">
         <v>752</v>
       </c>
-      <c r="L42" s="5" t="s">
+      <c r="M42" s="5" t="s">
         <v>753</v>
-      </c>
-      <c r="M42" s="5" t="s">
-        <v>754</v>
       </c>
     </row>
   </sheetData>
@@ -6249,7 +6249,7 @@
         <v>17</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>1076</v>
+        <v>1074</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>1</v>
@@ -6288,7 +6288,7 @@
         <v>121</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>1069</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
@@ -6299,10 +6299,10 @@
         <v>44</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>1079</v>
+        <v>1077</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>1080</v>
+        <v>1078</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>131</v>
@@ -6317,7 +6317,7 @@
         <v>48</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>1080</v>
+        <v>1078</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>129</v>
@@ -6362,7 +6362,7 @@
         <v>74</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="J3" s="5" t="s">
         <v>75</v>
@@ -6407,7 +6407,7 @@
         <v>85</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="J4" s="5" t="s">
         <v>81</v>
@@ -6452,7 +6452,7 @@
         <v>86</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="J5" s="5" t="s">
         <v>82</v>
@@ -6497,7 +6497,7 @@
         <v>91</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="J6" s="5" t="s">
         <v>92</v>
@@ -6542,7 +6542,7 @@
         <v>126</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="J7" s="5" t="s">
         <v>127</v>
@@ -6575,7 +6575,7 @@
         <v>130</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>259</v>
@@ -6587,7 +6587,7 @@
         <v>261</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="J8" s="5" t="s">
         <v>262</v>
@@ -6620,7 +6620,7 @@
         <v>130</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>980</v>
+        <v>978</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>267</v>
@@ -6632,7 +6632,7 @@
         <v>269</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="J9" s="5" t="s">
         <v>270</v>
@@ -6665,7 +6665,7 @@
         <v>130</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>275</v>
@@ -6677,7 +6677,7 @@
         <v>277</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="J10" s="5" t="s">
         <v>278</v>
@@ -6710,7 +6710,7 @@
         <v>130</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>283</v>
@@ -6722,7 +6722,7 @@
         <v>285</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="J11" s="5" t="s">
         <v>286</v>
@@ -6755,7 +6755,7 @@
         <v>130</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>291</v>
@@ -6767,7 +6767,7 @@
         <v>293</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="J12" s="5" t="s">
         <v>294</v>
@@ -6800,7 +6800,7 @@
         <v>130</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>299</v>
@@ -6812,7 +6812,7 @@
         <v>301</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="J13" s="5" t="s">
         <v>302</v>
@@ -6845,7 +6845,7 @@
         <v>130</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>307</v>
@@ -6857,7 +6857,7 @@
         <v>309</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="J14" s="5" t="s">
         <v>310</v>
@@ -6902,7 +6902,7 @@
         <v>318</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="J15" s="5" t="s">
         <v>319</v>
@@ -6947,7 +6947,7 @@
         <v>327</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="J16" s="5" t="s">
         <v>328</v>
@@ -6992,7 +6992,7 @@
         <v>337</v>
       </c>
       <c r="I17" s="9" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="J17" s="5" t="s">
         <v>338</v>
@@ -7037,7 +7037,7 @@
         <v>347</v>
       </c>
       <c r="I18" s="9" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="J18" s="5" t="s">
         <v>348</v>
@@ -7082,7 +7082,7 @@
         <v>357</v>
       </c>
       <c r="I19" s="9" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="J19" s="5" t="s">
         <v>358</v>
@@ -7127,7 +7127,7 @@
         <v>366</v>
       </c>
       <c r="I20" s="9" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="J20" s="5" t="s">
         <v>367</v>
@@ -7148,7 +7148,7 @@
         <v>242</v>
       </c>
       <c r="P20" s="5" t="s">
-        <v>1070</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
@@ -7175,7 +7175,7 @@
         <v>375</v>
       </c>
       <c r="I21" s="9" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="J21" s="5" t="s">
         <v>376</v>
@@ -7220,7 +7220,7 @@
         <v>384</v>
       </c>
       <c r="I22" s="9" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="J22" s="5" t="s">
         <v>385</v>
@@ -7265,7 +7265,7 @@
         <v>393</v>
       </c>
       <c r="I23" s="9" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="J23" s="5" t="s">
         <v>394</v>
@@ -7310,7 +7310,7 @@
         <v>403</v>
       </c>
       <c r="I24" s="9" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="J24" s="5" t="s">
         <v>404</v>
@@ -7355,7 +7355,7 @@
         <v>413</v>
       </c>
       <c r="I25" s="9" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="J25" s="5" t="s">
         <v>414</v>
@@ -7400,7 +7400,7 @@
         <v>422</v>
       </c>
       <c r="I26" s="9" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="J26" s="5" t="s">
         <v>423</v>
@@ -7445,7 +7445,7 @@
         <v>432</v>
       </c>
       <c r="I27" s="9" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="J27" s="5" t="s">
         <v>433</v>
@@ -7490,7 +7490,7 @@
         <v>442</v>
       </c>
       <c r="I28" s="9" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="J28" s="5" t="s">
         <v>443</v>
@@ -7535,7 +7535,7 @@
         <v>452</v>
       </c>
       <c r="I29" s="9" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="J29" s="5" t="s">
         <v>453</v>
@@ -7580,7 +7580,7 @@
         <v>462</v>
       </c>
       <c r="I30" s="9" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="J30" s="5" t="s">
         <v>463</v>
@@ -7625,7 +7625,7 @@
         <v>472</v>
       </c>
       <c r="I31" s="9" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="J31" s="5" t="s">
         <v>473</v>
@@ -7648,41 +7648,41 @@
     </row>
     <row r="32" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
+        <v>585</v>
+      </c>
+      <c r="B32" s="5" t="s">
         <v>586</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>587</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="9" t="s">
         <v>130</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="F32" s="5" t="s">
+        <v>587</v>
+      </c>
+      <c r="G32" s="5" t="s">
         <v>588</v>
       </c>
-      <c r="G32" s="5" t="s">
+      <c r="H32" s="5" t="s">
         <v>589</v>
       </c>
-      <c r="H32" s="5" t="s">
+      <c r="I32" s="9" t="s">
+        <v>634</v>
+      </c>
+      <c r="J32" s="5" t="s">
         <v>590</v>
       </c>
-      <c r="I32" s="9" t="s">
-        <v>635</v>
-      </c>
-      <c r="J32" s="5" t="s">
+      <c r="K32" s="5" t="s">
         <v>591</v>
       </c>
-      <c r="K32" s="5" t="s">
+      <c r="L32" s="5" t="s">
         <v>592</v>
       </c>
-      <c r="L32" s="5" t="s">
+      <c r="M32" s="5" t="s">
         <v>593</v>
-      </c>
-      <c r="M32" s="5" t="s">
-        <v>594</v>
       </c>
       <c r="N32" s="5" t="s">
         <v>12</v>
@@ -7693,41 +7693,41 @@
     </row>
     <row r="33" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
+        <v>594</v>
+      </c>
+      <c r="B33" s="5" t="s">
         <v>595</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>596</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="9" t="s">
         <v>130</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="F33" s="5" t="s">
+        <v>596</v>
+      </c>
+      <c r="G33" s="5" t="s">
         <v>597</v>
       </c>
-      <c r="G33" s="5" t="s">
+      <c r="H33" s="5" t="s">
         <v>598</v>
       </c>
-      <c r="H33" s="5" t="s">
+      <c r="I33" s="9" t="s">
+        <v>633</v>
+      </c>
+      <c r="J33" s="5" t="s">
         <v>599</v>
       </c>
-      <c r="I33" s="9" t="s">
-        <v>634</v>
-      </c>
-      <c r="J33" s="5" t="s">
+      <c r="K33" s="5" t="s">
         <v>600</v>
       </c>
-      <c r="K33" s="5" t="s">
+      <c r="L33" s="5" t="s">
         <v>601</v>
       </c>
-      <c r="L33" s="5" t="s">
+      <c r="M33" s="5" t="s">
         <v>602</v>
-      </c>
-      <c r="M33" s="5" t="s">
-        <v>603</v>
       </c>
       <c r="N33" s="5" t="s">
         <v>12</v>
@@ -7738,41 +7738,41 @@
     </row>
     <row r="34" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
+        <v>603</v>
+      </c>
+      <c r="B34" s="5" t="s">
         <v>604</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>605</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="9" t="s">
         <v>130</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="F34" s="5" t="s">
+        <v>605</v>
+      </c>
+      <c r="G34" s="5" t="s">
         <v>606</v>
       </c>
-      <c r="G34" s="5" t="s">
+      <c r="H34" s="5" t="s">
         <v>607</v>
       </c>
-      <c r="H34" s="5" t="s">
+      <c r="I34" s="9" t="s">
+        <v>632</v>
+      </c>
+      <c r="J34" s="5" t="s">
         <v>608</v>
       </c>
-      <c r="I34" s="9" t="s">
-        <v>633</v>
-      </c>
-      <c r="J34" s="5" t="s">
+      <c r="K34" s="5" t="s">
         <v>609</v>
       </c>
-      <c r="K34" s="5" t="s">
+      <c r="L34" s="5" t="s">
         <v>610</v>
       </c>
-      <c r="L34" s="5" t="s">
+      <c r="M34" s="5" t="s">
         <v>611</v>
-      </c>
-      <c r="M34" s="5" t="s">
-        <v>612</v>
       </c>
       <c r="N34" s="5" t="s">
         <v>12</v>
@@ -7783,41 +7783,41 @@
     </row>
     <row r="35" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
+        <v>612</v>
+      </c>
+      <c r="B35" s="5" t="s">
         <v>613</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>614</v>
       </c>
       <c r="C35" s="5"/>
       <c r="D35" s="9" t="s">
         <v>130</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="F35" s="5" t="s">
+        <v>614</v>
+      </c>
+      <c r="G35" s="5" t="s">
         <v>615</v>
       </c>
-      <c r="G35" s="5" t="s">
+      <c r="H35" s="5" t="s">
         <v>616</v>
       </c>
-      <c r="H35" s="5" t="s">
+      <c r="I35" s="9" t="s">
+        <v>631</v>
+      </c>
+      <c r="J35" s="5" t="s">
         <v>617</v>
       </c>
-      <c r="I35" s="9" t="s">
-        <v>632</v>
-      </c>
-      <c r="J35" s="5" t="s">
+      <c r="K35" s="5" t="s">
         <v>618</v>
       </c>
-      <c r="K35" s="5" t="s">
+      <c r="L35" s="5" t="s">
         <v>619</v>
       </c>
-      <c r="L35" s="5" t="s">
+      <c r="M35" s="5" t="s">
         <v>620</v>
-      </c>
-      <c r="M35" s="5" t="s">
-        <v>621</v>
       </c>
       <c r="N35" s="5" t="s">
         <v>12</v>
@@ -7828,41 +7828,41 @@
     </row>
     <row r="36" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
+        <v>621</v>
+      </c>
+      <c r="B36" s="5" t="s">
         <v>622</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>623</v>
       </c>
       <c r="C36" s="5"/>
       <c r="D36" s="9" t="s">
         <v>130</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="F36" s="5" t="s">
+        <v>623</v>
+      </c>
+      <c r="G36" s="5" t="s">
         <v>624</v>
       </c>
-      <c r="G36" s="5" t="s">
+      <c r="H36" s="5" t="s">
         <v>625</v>
       </c>
-      <c r="H36" s="5" t="s">
+      <c r="I36" s="9" t="s">
+        <v>630</v>
+      </c>
+      <c r="J36" s="5" t="s">
         <v>626</v>
       </c>
-      <c r="I36" s="9" t="s">
-        <v>631</v>
-      </c>
-      <c r="J36" s="5" t="s">
+      <c r="K36" s="5" t="s">
         <v>627</v>
       </c>
-      <c r="K36" s="5" t="s">
+      <c r="L36" s="5" t="s">
         <v>628</v>
       </c>
-      <c r="L36" s="5" t="s">
+      <c r="M36" s="5" t="s">
         <v>629</v>
-      </c>
-      <c r="M36" s="5" t="s">
-        <v>630</v>
       </c>
       <c r="N36" s="5" t="s">
         <v>12</v>
@@ -7898,8 +7898,8 @@
   </sheetPr>
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7968,10 +7968,10 @@
         <v>139</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>1081</v>
+        <v>1079</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>1082</v>
+        <v>1080</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>142</v>
@@ -7983,7 +7983,7 @@
         <v>144</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>1081</v>
+        <v>1079</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>165</v>
@@ -8009,7 +8009,7 @@
         <v>480</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>481</v>
@@ -8021,7 +8021,7 @@
         <v>483</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="I3" s="9" t="s">
         <v>480</v>
@@ -8044,40 +8044,40 @@
         <v>36</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>849</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>850</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>858</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>851</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="F4" s="5" t="s">
         <v>852</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>860</v>
-      </c>
-      <c r="E4" s="5" t="s">
+      <c r="G4" s="5" t="s">
         <v>853</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="H4" s="5" t="s">
         <v>854</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="I4" s="9" t="s">
+        <v>850</v>
+      </c>
+      <c r="J4" s="5" t="s">
         <v>855</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="K4" s="5" t="s">
         <v>856</v>
       </c>
-      <c r="I4" s="9" t="s">
-        <v>852</v>
-      </c>
-      <c r="J4" s="5" t="s">
+      <c r="L4" s="5" t="s">
         <v>857</v>
       </c>
-      <c r="K4" s="5" t="s">
-        <v>858</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>859</v>
-      </c>
       <c r="M4" s="5" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8085,40 +8085,40 @@
         <v>43</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>859</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>860</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>868</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>861</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="F5" s="5" t="s">
         <v>862</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>870</v>
-      </c>
-      <c r="E5" s="5" t="s">
+      <c r="G5" s="5" t="s">
         <v>863</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="H5" s="5" t="s">
         <v>864</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="I5" s="9" t="s">
+        <v>860</v>
+      </c>
+      <c r="J5" s="5" t="s">
         <v>865</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="K5" s="5" t="s">
         <v>866</v>
       </c>
-      <c r="I5" s="9" t="s">
-        <v>862</v>
-      </c>
-      <c r="J5" s="5" t="s">
+      <c r="L5" s="5" t="s">
         <v>867</v>
       </c>
-      <c r="K5" s="5" t="s">
-        <v>868</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>869</v>
-      </c>
       <c r="M5" s="5" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8126,40 +8126,40 @@
         <v>64</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>796</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>797</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>798</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="E6" s="5" t="s">
         <v>799</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="F6" s="5" t="s">
         <v>800</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="G6" s="5" t="s">
         <v>801</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="H6" s="5" t="s">
         <v>802</v>
       </c>
-      <c r="G6" s="5" t="s">
-        <v>803</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>804</v>
-      </c>
       <c r="I6" s="9" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="J6" s="5" t="s">
+        <v>805</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>806</v>
+      </c>
+      <c r="L6" s="5" t="s">
         <v>807</v>
       </c>
-      <c r="K6" s="5" t="s">
-        <v>808</v>
-      </c>
-      <c r="L6" s="5" t="s">
-        <v>809</v>
-      </c>
       <c r="M6" s="5" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8167,40 +8167,40 @@
         <v>96</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>781</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>1081</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>1082</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>782</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>783</v>
       </c>
-      <c r="C7" s="9" t="s">
-        <v>1083</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>1084</v>
-      </c>
-      <c r="E7" s="5" t="s">
+      <c r="G7" s="5" t="s">
         <v>784</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="H7" s="5" t="s">
+        <v>803</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>1081</v>
+      </c>
+      <c r="J7" s="5" t="s">
         <v>785</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="K7" s="5" t="s">
         <v>786</v>
       </c>
-      <c r="H7" s="5" t="s">
-        <v>805</v>
-      </c>
-      <c r="I7" s="9" t="s">
-        <v>1083</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>787</v>
-      </c>
-      <c r="K7" s="5" t="s">
-        <v>788</v>
-      </c>
       <c r="L7" s="5" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="M7" s="5" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8208,40 +8208,40 @@
         <v>103</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>787</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>1126</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>1127</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>789</v>
       </c>
-      <c r="C8" s="9" t="s">
-        <v>1128</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>1129</v>
-      </c>
-      <c r="E8" s="5" t="s">
+      <c r="G8" s="5" t="s">
         <v>790</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="H8" s="5" t="s">
+        <v>804</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>1126</v>
+      </c>
+      <c r="J8" s="5" t="s">
         <v>791</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="K8" s="5" t="s">
         <v>792</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>806</v>
-      </c>
-      <c r="I8" s="9" t="s">
-        <v>1128</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>793</v>
-      </c>
-      <c r="K8" s="5" t="s">
-        <v>794</v>
       </c>
       <c r="L8" s="5" t="s">
         <v>486</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8249,40 +8249,40 @@
         <v>111</v>
       </c>
       <c r="B9" s="5" t="s">
+        <v>809</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>810</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>811</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="E9" s="5" t="s">
         <v>812</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="F9" s="5" t="s">
         <v>813</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="G9" s="5" t="s">
         <v>814</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="H9" s="5" t="s">
         <v>815</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="I9" s="9" t="s">
+        <v>810</v>
+      </c>
+      <c r="J9" s="5" t="s">
         <v>816</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="K9" s="5" t="s">
         <v>817</v>
       </c>
-      <c r="I9" s="9" t="s">
-        <v>812</v>
-      </c>
-      <c r="J9" s="5" t="s">
+      <c r="L9" s="5" t="s">
         <v>818</v>
       </c>
-      <c r="K9" s="5" t="s">
-        <v>819</v>
-      </c>
-      <c r="L9" s="5" t="s">
-        <v>820</v>
-      </c>
       <c r="M9" s="5" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8293,10 +8293,10 @@
         <v>487</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>1124</v>
+        <v>1122</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>1125</v>
+        <v>1123</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>488</v>
@@ -8308,10 +8308,10 @@
         <v>490</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>1124</v>
+        <v>1122</v>
       </c>
       <c r="J10" s="5" t="s">
         <v>491</v>
@@ -8331,40 +8331,40 @@
         <v>115</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>990</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>991</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>992</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="E11" s="5" t="s">
         <v>993</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="F11" s="5" t="s">
         <v>994</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="G11" s="5" t="s">
         <v>995</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="H11" s="5" t="s">
         <v>996</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="I11" s="9" t="s">
+        <v>991</v>
+      </c>
+      <c r="J11" s="5" t="s">
         <v>997</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="K11" s="5" t="s">
         <v>998</v>
       </c>
-      <c r="I11" s="9" t="s">
-        <v>993</v>
-      </c>
-      <c r="J11" s="5" t="s">
+      <c r="L11" s="5" t="s">
         <v>999</v>
       </c>
-      <c r="K11" s="5" t="s">
-        <v>1000</v>
-      </c>
-      <c r="L11" s="5" t="s">
-        <v>1001</v>
-      </c>
       <c r="M11" s="5" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8372,40 +8372,40 @@
         <v>117</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>1000</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>1001</v>
+      </c>
+      <c r="D12" s="6" t="s">
         <v>1002</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="E12" s="5" t="s">
         <v>1003</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="F12" s="5" t="s">
         <v>1004</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="G12" s="5" t="s">
         <v>1005</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="H12" s="5" t="s">
         <v>1006</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="I12" s="9" t="s">
+        <v>1001</v>
+      </c>
+      <c r="J12" s="5" t="s">
         <v>1007</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="K12" s="5" t="s">
         <v>1008</v>
       </c>
-      <c r="I12" s="9" t="s">
-        <v>1003</v>
-      </c>
-      <c r="J12" s="5" t="s">
+      <c r="L12" s="5" t="s">
         <v>1009</v>
       </c>
-      <c r="K12" s="5" t="s">
-        <v>1010</v>
-      </c>
-      <c r="L12" s="5" t="s">
-        <v>1011</v>
-      </c>
       <c r="M12" s="5" t="s">
-        <v>1011</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8413,40 +8413,40 @@
         <v>119</v>
       </c>
       <c r="B13" s="5" t="s">
+        <v>879</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>880</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>881</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="E13" s="5" t="s">
         <v>882</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="F13" s="5" t="s">
         <v>883</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="G13" s="5" t="s">
         <v>884</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="H13" s="5" t="s">
         <v>885</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="I13" s="9" t="s">
+        <v>880</v>
+      </c>
+      <c r="J13" s="5" t="s">
         <v>886</v>
       </c>
-      <c r="H13" s="5" t="s">
+      <c r="K13" s="5" t="s">
         <v>887</v>
       </c>
-      <c r="I13" s="9" t="s">
-        <v>882</v>
-      </c>
-      <c r="J13" s="5" t="s">
+      <c r="L13" s="5" t="s">
         <v>888</v>
       </c>
-      <c r="K13" s="5" t="s">
-        <v>889</v>
-      </c>
-      <c r="L13" s="5" t="s">
-        <v>890</v>
-      </c>
       <c r="M13" s="5" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8457,10 +8457,10 @@
         <v>494</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>1126</v>
+        <v>1124</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>1127</v>
+        <v>1125</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>495</v>
@@ -8473,7 +8473,7 @@
       </c>
       <c r="H14" s="5"/>
       <c r="I14" s="9" t="s">
-        <v>1126</v>
+        <v>1124</v>
       </c>
       <c r="J14" s="5" t="s">
         <v>498</v>
@@ -8496,10 +8496,10 @@
         <v>502</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>1130</v>
+        <v>1128</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>1131</v>
+        <v>1129</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>503</v>
@@ -8512,7 +8512,7 @@
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="9" t="s">
-        <v>1130</v>
+        <v>1128</v>
       </c>
       <c r="J15" s="5" t="s">
         <v>506</v>
@@ -8535,10 +8535,10 @@
         <v>510</v>
       </c>
       <c r="C16" s="9" t="s">
+        <v>1128</v>
+      </c>
+      <c r="D16" s="6" t="s">
         <v>1130</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>1132</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>511</v>
@@ -8551,7 +8551,7 @@
       </c>
       <c r="H16" s="5"/>
       <c r="I16" s="9" t="s">
-        <v>1130</v>
+        <v>1128</v>
       </c>
       <c r="J16" s="5" t="s">
         <v>514</v>
@@ -8574,37 +8574,37 @@
         <v>517</v>
       </c>
       <c r="C17" s="9" t="s">
+        <v>1131</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>1132</v>
+      </c>
+      <c r="E17" s="5" t="s">
         <v>518</v>
       </c>
-      <c r="D17" s="6" t="s">
-        <v>777</v>
-      </c>
-      <c r="E17" s="5" t="s">
+      <c r="F17" s="5" t="s">
         <v>519</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="G17" s="5" t="s">
         <v>520</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="H17" s="5" t="s">
         <v>521</v>
       </c>
-      <c r="H17" s="5" t="s">
+      <c r="I17" s="9" t="s">
+        <v>1131</v>
+      </c>
+      <c r="J17" s="5" t="s">
         <v>522</v>
       </c>
-      <c r="I17" s="9" t="s">
-        <v>518</v>
-      </c>
-      <c r="J17" s="5" t="s">
+      <c r="K17" s="5" t="s">
         <v>523</v>
       </c>
-      <c r="K17" s="5" t="s">
+      <c r="L17" s="5" t="s">
         <v>524</v>
       </c>
-      <c r="L17" s="5" t="s">
-        <v>525</v>
-      </c>
       <c r="M17" s="5" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8612,38 +8612,38 @@
         <v>18</v>
       </c>
       <c r="B18" s="5" t="s">
+        <v>525</v>
+      </c>
+      <c r="C18" s="9" t="s">
         <v>526</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="D18" s="6" t="s">
+        <v>776</v>
+      </c>
+      <c r="E18" s="5" t="s">
         <v>527</v>
       </c>
-      <c r="D18" s="6" t="s">
-        <v>778</v>
-      </c>
-      <c r="E18" s="5" t="s">
+      <c r="F18" s="5" t="s">
         <v>528</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="G18" s="5" t="s">
         <v>529</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>530</v>
       </c>
       <c r="H18" s="5"/>
       <c r="I18" s="9" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="J18" s="5" t="s">
+        <v>530</v>
+      </c>
+      <c r="K18" s="5" t="s">
         <v>531</v>
       </c>
-      <c r="K18" s="5" t="s">
+      <c r="L18" s="5" t="s">
         <v>532</v>
       </c>
-      <c r="L18" s="5" t="s">
-        <v>533</v>
-      </c>
       <c r="M18" s="5" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8651,38 +8651,38 @@
         <v>19</v>
       </c>
       <c r="B19" s="5" t="s">
+        <v>533</v>
+      </c>
+      <c r="C19" s="9" t="s">
         <v>534</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="D19" s="6" t="s">
+        <v>777</v>
+      </c>
+      <c r="E19" s="5" t="s">
         <v>535</v>
       </c>
-      <c r="D19" s="6" t="s">
-        <v>779</v>
-      </c>
-      <c r="E19" s="5" t="s">
+      <c r="F19" s="5" t="s">
         <v>536</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="G19" s="5" t="s">
         <v>537</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>538</v>
       </c>
       <c r="H19" s="5"/>
       <c r="I19" s="9" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="J19" s="5" t="s">
+        <v>538</v>
+      </c>
+      <c r="K19" s="5" t="s">
         <v>539</v>
       </c>
-      <c r="K19" s="5" t="s">
+      <c r="L19" s="5" t="s">
         <v>540</v>
       </c>
-      <c r="L19" s="5" t="s">
-        <v>541</v>
-      </c>
       <c r="M19" s="5" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8690,38 +8690,38 @@
         <v>209</v>
       </c>
       <c r="B20" s="5" t="s">
+        <v>682</v>
+      </c>
+      <c r="C20" s="9" t="s">
         <v>683</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="D20" s="6" t="s">
+        <v>778</v>
+      </c>
+      <c r="E20" s="5" t="s">
         <v>684</v>
       </c>
-      <c r="D20" s="6" t="s">
-        <v>780</v>
-      </c>
-      <c r="E20" s="5" t="s">
+      <c r="F20" s="5" t="s">
         <v>685</v>
       </c>
-      <c r="F20" s="5" t="s">
+      <c r="G20" s="5" t="s">
         <v>686</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>687</v>
       </c>
       <c r="H20" s="5"/>
       <c r="I20" s="9" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="J20" s="5" t="s">
+        <v>687</v>
+      </c>
+      <c r="K20" s="5" t="s">
         <v>688</v>
       </c>
-      <c r="K20" s="5" t="s">
+      <c r="L20" s="5" t="s">
         <v>689</v>
       </c>
-      <c r="L20" s="5" t="s">
-        <v>690</v>
-      </c>
       <c r="M20" s="5" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8729,38 +8729,38 @@
         <v>229</v>
       </c>
       <c r="B21" s="5" t="s">
+        <v>577</v>
+      </c>
+      <c r="C21" s="9" t="s">
         <v>578</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="D21" s="6" t="s">
+        <v>778</v>
+      </c>
+      <c r="E21" s="5" t="s">
         <v>579</v>
       </c>
-      <c r="D21" s="6" t="s">
-        <v>780</v>
-      </c>
-      <c r="E21" s="5" t="s">
+      <c r="F21" s="5" t="s">
         <v>580</v>
       </c>
-      <c r="F21" s="5" t="s">
+      <c r="G21" s="5" t="s">
         <v>581</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>582</v>
       </c>
       <c r="H21" s="5"/>
       <c r="I21" s="9" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="J21" s="5" t="s">
+        <v>582</v>
+      </c>
+      <c r="K21" s="5" t="s">
         <v>583</v>
       </c>
-      <c r="K21" s="5" t="s">
+      <c r="L21" s="5" t="s">
         <v>584</v>
       </c>
-      <c r="L21" s="5" t="s">
-        <v>585</v>
-      </c>
       <c r="M21" s="5" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8768,40 +8768,40 @@
         <v>418</v>
       </c>
       <c r="B22" s="5" t="s">
+        <v>1030</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>1031</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>1069</v>
+      </c>
+      <c r="E22" s="5" t="s">
         <v>1032</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="F22" s="5" t="s">
         <v>1033</v>
       </c>
-      <c r="D22" s="6" t="s">
-        <v>1071</v>
-      </c>
-      <c r="E22" s="5" t="s">
+      <c r="G22" s="5" t="s">
         <v>1034</v>
       </c>
-      <c r="F22" s="5" t="s">
+      <c r="H22" s="5" t="s">
         <v>1035</v>
       </c>
-      <c r="G22" s="5" t="s">
+      <c r="I22" s="9" t="s">
+        <v>1031</v>
+      </c>
+      <c r="J22" s="5" t="s">
         <v>1036</v>
       </c>
-      <c r="H22" s="5" t="s">
+      <c r="K22" s="5" t="s">
         <v>1037</v>
       </c>
-      <c r="I22" s="9" t="s">
-        <v>1033</v>
-      </c>
-      <c r="J22" s="5" t="s">
+      <c r="L22" s="5" t="s">
         <v>1038</v>
       </c>
-      <c r="K22" s="5" t="s">
-        <v>1039</v>
-      </c>
-      <c r="L22" s="5" t="s">
-        <v>1040</v>
-      </c>
       <c r="M22" s="5" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8809,40 +8809,40 @@
         <v>427</v>
       </c>
       <c r="B23" s="5" t="s">
+        <v>820</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>821</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>1070</v>
+      </c>
+      <c r="E23" s="5" t="s">
         <v>822</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="F23" s="5" t="s">
         <v>823</v>
       </c>
-      <c r="D23" s="6" t="s">
-        <v>1072</v>
-      </c>
-      <c r="E23" s="5" t="s">
+      <c r="G23" s="5" t="s">
         <v>824</v>
       </c>
-      <c r="F23" s="5" t="s">
+      <c r="H23" s="5" t="s">
         <v>825</v>
       </c>
-      <c r="G23" s="5" t="s">
+      <c r="I23" s="9" t="s">
+        <v>821</v>
+      </c>
+      <c r="J23" s="5" t="s">
         <v>826</v>
       </c>
-      <c r="H23" s="5" t="s">
+      <c r="K23" s="5" t="s">
         <v>827</v>
       </c>
-      <c r="I23" s="9" t="s">
-        <v>823</v>
-      </c>
-      <c r="J23" s="5" t="s">
+      <c r="L23" s="5" t="s">
         <v>828</v>
       </c>
-      <c r="K23" s="5" t="s">
-        <v>829</v>
-      </c>
-      <c r="L23" s="5" t="s">
-        <v>830</v>
-      </c>
       <c r="M23" s="5" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8850,40 +8850,40 @@
         <v>437</v>
       </c>
       <c r="B24" s="5" t="s">
+        <v>829</v>
+      </c>
+      <c r="C24" s="9" t="s">
         <v>831</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="D24" s="6" t="s">
+        <v>832</v>
+      </c>
+      <c r="E24" s="5" t="s">
         <v>833</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="F24" s="5" t="s">
         <v>834</v>
       </c>
-      <c r="E24" s="5" t="s">
+      <c r="G24" s="5" t="s">
         <v>835</v>
       </c>
-      <c r="F24" s="5" t="s">
+      <c r="H24" s="5" t="s">
         <v>836</v>
       </c>
-      <c r="G24" s="5" t="s">
+      <c r="I24" s="9" t="s">
+        <v>831</v>
+      </c>
+      <c r="J24" s="5" t="s">
         <v>837</v>
       </c>
-      <c r="H24" s="5" t="s">
+      <c r="K24" s="5" t="s">
         <v>838</v>
       </c>
-      <c r="I24" s="9" t="s">
-        <v>833</v>
-      </c>
-      <c r="J24" s="5" t="s">
+      <c r="L24" s="5" t="s">
         <v>839</v>
       </c>
-      <c r="K24" s="5" t="s">
-        <v>840</v>
-      </c>
-      <c r="L24" s="5" t="s">
-        <v>841</v>
-      </c>
       <c r="M24" s="5" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8891,40 +8891,40 @@
         <v>447</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="C25" s="9" t="s">
+        <v>840</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>841</v>
+      </c>
+      <c r="E25" s="5" t="s">
         <v>842</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="F25" s="5" t="s">
         <v>843</v>
       </c>
-      <c r="E25" s="5" t="s">
+      <c r="G25" s="5" t="s">
         <v>844</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="H25" s="5" t="s">
         <v>845</v>
       </c>
-      <c r="G25" s="5" t="s">
+      <c r="I25" s="9" t="s">
+        <v>840</v>
+      </c>
+      <c r="J25" s="5" t="s">
         <v>846</v>
       </c>
-      <c r="H25" s="5" t="s">
+      <c r="K25" s="5" t="s">
         <v>847</v>
       </c>
-      <c r="I25" s="9" t="s">
-        <v>842</v>
-      </c>
-      <c r="J25" s="5" t="s">
+      <c r="L25" s="5" t="s">
         <v>848</v>
       </c>
-      <c r="K25" s="5" t="s">
-        <v>849</v>
-      </c>
-      <c r="L25" s="5" t="s">
-        <v>850</v>
-      </c>
       <c r="M25" s="5" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8932,40 +8932,40 @@
         <v>457</v>
       </c>
       <c r="B26" s="5" t="s">
+        <v>947</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>948</v>
+      </c>
+      <c r="D26" s="6" t="s">
         <v>949</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="E26" s="5" t="s">
         <v>950</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="F26" s="5" t="s">
         <v>951</v>
       </c>
-      <c r="E26" s="5" t="s">
+      <c r="G26" s="5" t="s">
         <v>952</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="H26" s="5" t="s">
         <v>953</v>
       </c>
-      <c r="G26" s="5" t="s">
+      <c r="I26" s="9" t="s">
+        <v>948</v>
+      </c>
+      <c r="J26" s="5" t="s">
         <v>954</v>
       </c>
-      <c r="H26" s="5" t="s">
+      <c r="K26" s="5" t="s">
         <v>955</v>
       </c>
-      <c r="I26" s="9" t="s">
-        <v>950</v>
-      </c>
-      <c r="J26" s="5" t="s">
+      <c r="L26" s="5" t="s">
         <v>956</v>
       </c>
-      <c r="K26" s="5" t="s">
-        <v>957</v>
-      </c>
-      <c r="L26" s="5" t="s">
-        <v>958</v>
-      </c>
       <c r="M26" s="5" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8973,282 +8973,282 @@
         <v>467</v>
       </c>
       <c r="B27" s="5" t="s">
+        <v>957</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>958</v>
+      </c>
+      <c r="D27" s="6" t="s">
         <v>959</v>
       </c>
-      <c r="C27" s="9" t="s">
+      <c r="E27" s="5" t="s">
         <v>960</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="F27" s="5" t="s">
         <v>961</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="G27" s="5" t="s">
         <v>962</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="H27" s="5" t="s">
         <v>963</v>
       </c>
-      <c r="G27" s="5" t="s">
+      <c r="I27" s="9" t="s">
+        <v>958</v>
+      </c>
+      <c r="J27" s="5" t="s">
         <v>964</v>
       </c>
-      <c r="H27" s="5" t="s">
+      <c r="K27" s="5" t="s">
         <v>965</v>
       </c>
-      <c r="I27" s="9" t="s">
-        <v>960</v>
-      </c>
-      <c r="J27" s="5" t="s">
+      <c r="L27" s="5" t="s">
         <v>966</v>
       </c>
-      <c r="K27" s="5" t="s">
-        <v>967</v>
-      </c>
-      <c r="L27" s="5" t="s">
-        <v>968</v>
-      </c>
       <c r="M27" s="5" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B28" s="5" t="s">
+        <v>967</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>968</v>
+      </c>
+      <c r="D28" s="6" t="s">
         <v>969</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="E28" s="5" t="s">
         <v>970</v>
       </c>
-      <c r="D28" s="6" t="s">
+      <c r="F28" s="5" t="s">
         <v>971</v>
       </c>
-      <c r="E28" s="5" t="s">
+      <c r="G28" s="5" t="s">
         <v>972</v>
       </c>
-      <c r="F28" s="5" t="s">
+      <c r="H28" s="5" t="s">
         <v>973</v>
       </c>
-      <c r="G28" s="5" t="s">
+      <c r="I28" s="9" t="s">
+        <v>968</v>
+      </c>
+      <c r="J28" s="5" t="s">
         <v>974</v>
       </c>
-      <c r="H28" s="5" t="s">
+      <c r="K28" s="5" t="s">
         <v>975</v>
       </c>
-      <c r="I28" s="9" t="s">
-        <v>970</v>
-      </c>
-      <c r="J28" s="5" t="s">
+      <c r="L28" s="5" t="s">
         <v>976</v>
       </c>
-      <c r="K28" s="5" t="s">
-        <v>977</v>
-      </c>
-      <c r="L28" s="5" t="s">
-        <v>978</v>
-      </c>
       <c r="M28" s="5" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B29" s="5" t="s">
+        <v>1010</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>1011</v>
+      </c>
+      <c r="D29" s="6" t="s">
         <v>1012</v>
       </c>
-      <c r="C29" s="9" t="s">
+      <c r="E29" s="5" t="s">
         <v>1013</v>
       </c>
-      <c r="D29" s="6" t="s">
+      <c r="F29" s="5" t="s">
         <v>1014</v>
       </c>
-      <c r="E29" s="5" t="s">
+      <c r="G29" s="5" t="s">
         <v>1015</v>
       </c>
-      <c r="F29" s="5" t="s">
+      <c r="H29" s="5" t="s">
         <v>1016</v>
       </c>
-      <c r="G29" s="5" t="s">
+      <c r="I29" s="9" t="s">
+        <v>1011</v>
+      </c>
+      <c r="J29" s="5" t="s">
         <v>1017</v>
       </c>
-      <c r="H29" s="5" t="s">
+      <c r="K29" s="5" t="s">
         <v>1018</v>
       </c>
-      <c r="I29" s="9" t="s">
-        <v>1013</v>
-      </c>
-      <c r="J29" s="5" t="s">
+      <c r="L29" s="5" t="s">
         <v>1019</v>
       </c>
-      <c r="K29" s="5" t="s">
-        <v>1020</v>
-      </c>
-      <c r="L29" s="5" t="s">
-        <v>1021</v>
-      </c>
       <c r="M29" s="5" t="s">
-        <v>1021</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B30" s="5" t="s">
+        <v>1020</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>1021</v>
+      </c>
+      <c r="D30" s="6" t="s">
         <v>1022</v>
       </c>
-      <c r="C30" s="9" t="s">
+      <c r="E30" s="5" t="s">
         <v>1023</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="F30" s="5" t="s">
         <v>1024</v>
       </c>
-      <c r="E30" s="5" t="s">
+      <c r="G30" s="5" t="s">
         <v>1025</v>
       </c>
-      <c r="F30" s="5" t="s">
+      <c r="H30" s="5" t="s">
         <v>1026</v>
       </c>
-      <c r="G30" s="5" t="s">
+      <c r="I30" s="9" t="s">
+        <v>1021</v>
+      </c>
+      <c r="J30" s="5" t="s">
         <v>1027</v>
       </c>
-      <c r="H30" s="5" t="s">
+      <c r="K30" s="5" t="s">
         <v>1028</v>
       </c>
-      <c r="I30" s="9" t="s">
-        <v>1023</v>
-      </c>
-      <c r="J30" s="5" t="s">
+      <c r="L30" s="5" t="s">
         <v>1029</v>
       </c>
-      <c r="K30" s="5" t="s">
-        <v>1030</v>
-      </c>
-      <c r="L30" s="5" t="s">
-        <v>1031</v>
-      </c>
       <c r="M30" s="5" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B31" s="5" t="s">
+        <v>869</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>870</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>878</v>
+      </c>
+      <c r="E31" s="5" t="s">
         <v>871</v>
       </c>
-      <c r="C31" s="9" t="s">
+      <c r="F31" s="5" t="s">
         <v>872</v>
       </c>
-      <c r="D31" s="6" t="s">
-        <v>880</v>
-      </c>
-      <c r="E31" s="5" t="s">
+      <c r="G31" s="5" t="s">
         <v>873</v>
       </c>
-      <c r="F31" s="5" t="s">
+      <c r="H31" s="5" t="s">
         <v>874</v>
       </c>
-      <c r="G31" s="5" t="s">
+      <c r="I31" s="9" t="s">
+        <v>870</v>
+      </c>
+      <c r="J31" s="5" t="s">
         <v>875</v>
       </c>
-      <c r="H31" s="5" t="s">
+      <c r="K31" s="5" t="s">
         <v>876</v>
       </c>
-      <c r="I31" s="9" t="s">
-        <v>872</v>
-      </c>
-      <c r="J31" s="5" t="s">
+      <c r="L31" s="5" t="s">
         <v>877</v>
       </c>
-      <c r="K31" s="5" t="s">
-        <v>878</v>
-      </c>
-      <c r="L31" s="5" t="s">
-        <v>879</v>
-      </c>
       <c r="M31" s="5" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
+        <v>541</v>
+      </c>
+      <c r="B32" s="5" t="s">
         <v>542</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="C32" s="9" t="s">
         <v>543</v>
       </c>
-      <c r="C32" s="9" t="s">
+      <c r="D32" s="6" t="s">
+        <v>779</v>
+      </c>
+      <c r="E32" s="5" t="s">
         <v>544</v>
       </c>
-      <c r="D32" s="6" t="s">
-        <v>781</v>
-      </c>
-      <c r="E32" s="5" t="s">
+      <c r="F32" s="5" t="s">
         <v>545</v>
       </c>
-      <c r="F32" s="5" t="s">
+      <c r="G32" s="5" t="s">
         <v>546</v>
-      </c>
-      <c r="G32" s="5" t="s">
-        <v>547</v>
       </c>
       <c r="H32" s="5"/>
       <c r="I32" s="9" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="J32" s="5" t="s">
+        <v>547</v>
+      </c>
+      <c r="K32" s="5" t="s">
         <v>548</v>
       </c>
-      <c r="K32" s="5" t="s">
+      <c r="L32" s="5" t="s">
         <v>549</v>
       </c>
-      <c r="L32" s="5" t="s">
-        <v>550</v>
-      </c>
       <c r="M32" s="5" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
+        <v>550</v>
+      </c>
+      <c r="B33" s="5" t="s">
         <v>551</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="C33" s="9" t="s">
         <v>552</v>
       </c>
-      <c r="C33" s="9" t="s">
+      <c r="D33" s="6" t="s">
+        <v>780</v>
+      </c>
+      <c r="E33" s="5" t="s">
         <v>553</v>
       </c>
-      <c r="D33" s="6" t="s">
-        <v>782</v>
-      </c>
-      <c r="E33" s="5" t="s">
+      <c r="F33" s="5" t="s">
         <v>554</v>
       </c>
-      <c r="F33" s="5" t="s">
+      <c r="G33" s="5" t="s">
         <v>555</v>
-      </c>
-      <c r="G33" s="5" t="s">
-        <v>556</v>
       </c>
       <c r="H33" s="5"/>
       <c r="I33" s="9" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="J33" s="5" t="s">
+        <v>556</v>
+      </c>
+      <c r="K33" s="5" t="s">
         <v>557</v>
       </c>
-      <c r="K33" s="5" t="s">
+      <c r="L33" s="5" t="s">
         <v>558</v>
       </c>
-      <c r="L33" s="5" t="s">
-        <v>559</v>
-      </c>
       <c r="M33" s="5" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GDE-7310 Data set and Files for TL_CAL_18
</commit_message>
<xml_diff>
--- a/DataSet/Integration_DataSet/TL/TL_Data_Set_AU.xlsx
+++ b/DataSet/Integration_DataSet/TL/TL_Data_Set_AU.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\Integration_DataSet\TL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D26727AD-ADCF-4954-BACB-5647926167AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0F2A5CB-3FD4-4B4F-83E5-FAF943C54997}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BaseRate_Fields" sheetId="1" r:id="rId1"/>
@@ -1465,9 +1465,6 @@
     <t>TL_CAL_02</t>
   </si>
   <si>
-    <t>\DataSet\TL_DataSet\Calendar_GSFile\TL_CAL_02_Files\</t>
-  </si>
-  <si>
     <t>INPUTJSON_TL_CAL02</t>
   </si>
   <si>
@@ -1603,9 +1600,6 @@
     <t>TL_CAL_18</t>
   </si>
   <si>
-    <t>\DataSet\TL_DataSet\Calendar_GSFile\TL_CAL_18_Files\</t>
-  </si>
-  <si>
     <t>INPUTJSON_TL_CAL18</t>
   </si>
   <si>
@@ -1627,9 +1621,6 @@
     <t>TL_CAL_19</t>
   </si>
   <si>
-    <t>\DataSet\TL_DataSet\Calendar_GSFile\TL_CAL_19_Files\</t>
-  </si>
-  <si>
     <t>INPUTJSON_TL_CAL19</t>
   </si>
   <si>
@@ -1654,9 +1645,6 @@
     <t>TL_CAL_36</t>
   </si>
   <si>
-    <t>\DataSet\TL_DataSet\Calendar_GSFile\TL_CAL_36_Files\</t>
-  </si>
-  <si>
     <t>INPUTJSON_TL_CAL36</t>
   </si>
   <si>
@@ -1681,9 +1669,6 @@
     <t>TL_CAL_37</t>
   </si>
   <si>
-    <t>\DataSet\TL_DataSet\Calendar_GSFile\TL_CAL_37_Files\</t>
-  </si>
-  <si>
     <t>INPUTJSON_TL_CAL37</t>
   </si>
   <si>
@@ -1759,9 +1744,6 @@
     <t>TL_CAL_21</t>
   </si>
   <si>
-    <t>\DataSet\TL_DataSet\Calendar_GSFile\TL_CAL_21_Files\</t>
-  </si>
-  <si>
     <t>INPUTJSON_TL_CAL21</t>
   </si>
   <si>
@@ -2074,9 +2056,6 @@
     <t>TL_CAL_20</t>
   </si>
   <si>
-    <t>\DataSet\TL_DataSet\Calendar_GSFile\TL_CAL_20_Files\</t>
-  </si>
-  <si>
     <t>INPUTJSON_TL_CAL20</t>
   </si>
   <si>
@@ -2353,9 +2332,6 @@
     <t>Actual_ResponseMechanism_TL_BASE_42</t>
   </si>
   <si>
-    <t>Holidays_Banks_20190118_1.csv,Holidays_Banks_20190118_1.xlsx,Holidays_Banks_20190118_2.csv,Holidays_Banks_20190118_2.xlsx,Holidays_Misc_20190118.xlsx</t>
-  </si>
-  <si>
     <t>Holidays_Banks_20190119_1.csv,Holidays_Banks_20190119_1.xlsx,Holidays_Banks_20190119_2.csv,Holidays_Banks_20190119_2.xlsx,Holidays_Misc_20190119.xlsx</t>
   </si>
   <si>
@@ -2416,9 +2392,6 @@
     <t>TL_CAL_07</t>
   </si>
   <si>
-    <t>\DataSet\TL_DataSet\Calendar_GSFile\TL_CAL_07_Files\</t>
-  </si>
-  <si>
     <t>Holidays_Banks_20180107_1.xlsx,Holidays_Banks_20180107_2.xlsx,Holidays_Banks_20180107_1.csv,Holidays_Banks_20180107_2.csv,Holidays_Misc_20180107.xlsx</t>
   </si>
   <si>
@@ -2455,9 +2428,6 @@
     <t>TL_CAL_10</t>
   </si>
   <si>
-    <t>\DataSet\TL_DataSet\Calendar_GSFile\TL_CAL_10_Files\</t>
-  </si>
-  <si>
     <t>Holidays_Banks_20180110_1.xlsx,Holidays_Banks_20180110_2.xlsx,Holidays_Banks_20180110_1.csv,Holidays_Banks_20180110_2.csv,Holidays_Misc_20180110.xlsx</t>
   </si>
   <si>
@@ -2488,9 +2458,6 @@
     <t>TL_CAL_26</t>
   </si>
   <si>
-    <t>\DataSet\TL_DataSet\Calendar_GSFile\TL_CAL_26_Files\</t>
-  </si>
-  <si>
     <t>INPUTJSON_TL_CAL26</t>
   </si>
   <si>
@@ -2518,9 +2485,6 @@
     <t>TL_CAL_28</t>
   </si>
   <si>
-    <t>\DataSet\TL_DataSet\Calendar_GSFile\TL_CAL_27_Files\</t>
-  </si>
-  <si>
     <t>Holidays_Banks_20190127_1.xls,Holidays_Banks_20190127_2.xls,Holidays_Banks_20190127_1.csv,Holidays_Banks_20190127_2.csv,Holidays_Misc_20190127.xls</t>
   </si>
   <si>
@@ -2545,9 +2509,6 @@
     <t>Actual_CustomCBAPush_Response_TL_CAL_27</t>
   </si>
   <si>
-    <t>\DataSet\TL_DataSet\Calendar_GSFile\TL_CAL_28_Files\</t>
-  </si>
-  <si>
     <t>Holidays_Banks_20190128_1.xls,Holidays_Banks_20190128_2.xls,Holidays_Banks_20190128_1.csv,Holidays_Banks_20190128_2.csv,Holidays_Misc_20190128.xls</t>
   </si>
   <si>
@@ -2575,9 +2536,6 @@
     <t>TL_CAL_03</t>
   </si>
   <si>
-    <t>\DataSet\TL_DataSet\Calendar_GSFile\TL_CAL_03_Files\</t>
-  </si>
-  <si>
     <t>INPUTJSON_TL_CAL03</t>
   </si>
   <si>
@@ -2605,9 +2563,6 @@
     <t>TL_CAL_04</t>
   </si>
   <si>
-    <t>\DataSet\TL_DataSet\Calendar_GSFile\TL_CAL_04_Files\</t>
-  </si>
-  <si>
     <t>INPUTJSON_TL_CAL04</t>
   </si>
   <si>
@@ -2635,9 +2590,6 @@
     <t>TL_CAL_35</t>
   </si>
   <si>
-    <t>\DataSet\TL_DataSet\Calendar_GSFile\TL_CAL_35_Files\</t>
-  </si>
-  <si>
     <t>INPUTJSON_TL_CAL35</t>
   </si>
   <si>
@@ -2665,9 +2617,6 @@
     <t>TL_CAL_14</t>
   </si>
   <si>
-    <t>\DataSet\TL_DataSet\Calendar_GSFile\TL_CAL_14_Files\</t>
-  </si>
-  <si>
     <t>Holidays_Banks_20190114_1.xlsx,Holidays_Banks_20190114_2.xlsx,Holidays_Banks_20190114_1.csv,Holidays_Banks_20190114_2.csv,Holidays_Misc_20190114.xlsx</t>
   </si>
   <si>
@@ -2869,9 +2818,6 @@
     <t>TL_CAL_29</t>
   </si>
   <si>
-    <t>\DataSet\TL_DataSet\Calendar_GSFile\TL_CAL_29_Files\</t>
-  </si>
-  <si>
     <t>Holidays_Banks_20190129_1.xls,Holidays_Banks_20190129_2.xls,Holidays_Banks_20190129_1.csv,Holidays_Banks_20190129_2.csv,Holidays_Misc_20190129.xls</t>
   </si>
   <si>
@@ -2899,9 +2845,6 @@
     <t>TL_CAL_30</t>
   </si>
   <si>
-    <t>\DataSet\TL_DataSet\Calendar_GSFile\TL_CAL_30_Files\</t>
-  </si>
-  <si>
     <t>Holidays_Banks_20190130_1.xls,Holidays_Banks_20190130_2.xls,Holidays_Banks_20190130_1.csv,Holidays_Banks_20190130_2.csv,Holidays_Misc_20190130.xls</t>
   </si>
   <si>
@@ -2927,9 +2870,6 @@
   </si>
   <si>
     <t>TL_CAL_31</t>
-  </si>
-  <si>
-    <t>\DataSet\TL_DataSet\Calendar_GSFile\TL_CAL_31_Files\</t>
   </si>
   <si>
     <t>Holidays_Banks_20190131_1.xls,Holidays_Banks_20190131_2.xls,Holidays_Banks_20190131_1.csv,Holidays_Banks_20190131_2.csv,Holidays_Misc_20190131.xls</t>
@@ -3055,9 +2995,6 @@
     <t>TL_CAL_12</t>
   </si>
   <si>
-    <t>\DataSet\TL_DataSet\Calendar_GSFile\TL_CAL_12_Files\</t>
-  </si>
-  <si>
     <t>Holidays_Banks_20190112_1.xls,Holidays_Banks_20190112_2.xls,Holidays_Banks_20200112_1.csv,Holidays_Banks_20200112_2.csv,Holidays_Misc_20190112.xls</t>
   </si>
   <si>
@@ -3085,9 +3022,6 @@
     <t>TL_CAL_13</t>
   </si>
   <si>
-    <t>\DataSet\TL_DataSet\Calendar_GSFile\TL_CAL_13_Files\</t>
-  </si>
-  <si>
     <t>Holidays_Banks_20190113_1.xls,Holidays_Banks_20190113_2.xls,Holidays_Banks_20200113_1.csv,Holidays_Banks_20200113_2.csv,Holidays_Misc_20190113.xls</t>
   </si>
   <si>
@@ -3115,9 +3049,6 @@
     <t>TL_CAL_32</t>
   </si>
   <si>
-    <t>\DataSet\TL_DataSet\Calendar_GSFile\TL_CAL_32_Files\</t>
-  </si>
-  <si>
     <t>Holidays_Banks_20190132_1.xls,Holidays_Banks_20190132_2.xls,Holidays_Banks_20200132_1.csv,Holidays_Banks_20200132_2.csv,Holidays_Misc_20190132.xls</t>
   </si>
   <si>
@@ -3145,9 +3076,6 @@
     <t>TL_CAL_33</t>
   </si>
   <si>
-    <t>\DataSet\TL_DataSet\Calendar_GSFile\TL_CAL_33_Files\</t>
-  </si>
-  <si>
     <t>Holidays_Banks_20190133_1.xls,Holidays_Banks_20190133_2.xls,Holidays_Banks_20200133_1.csv,Holidays_Banks_20200133_2.csv,Holidays_Misc_20190133.xls</t>
   </si>
   <si>
@@ -3175,9 +3103,6 @@
     <t>TL_CAL_25</t>
   </si>
   <si>
-    <t>\DataSet\TL_DataSet\Calendar_GSFile\TL_CAL_25_Files\</t>
-  </si>
-  <si>
     <t>INPUTJSON_TL_CAL25</t>
   </si>
   <si>
@@ -3289,9 +3214,6 @@
     <t>fxRate.log</t>
   </si>
   <si>
-    <t>Holidays_Banks_20190125_2.xlsx,Holidays_Banks_20200125_1.csv,Holidays_Banks_20200125_2.csv,Holidays_Misc_20190125.xlsx</t>
-  </si>
-  <si>
     <t>Holidays_Banks_20190126_1.xls,Holidays_Banks_20190126_2.xls,Holidays_Banks_20190126_1.csv,Holidays_Banks_20190126_2.csv,Holidays_Misc_20190126.xls</t>
   </si>
   <si>
@@ -3479,6 +3401,84 @@
   </si>
   <si>
     <t>Holidays_Banks_20200517_1.csv,Holidays_Banks_20200517_1.xlsx,Holidays_Banks_20200517_2.csv,Holidays_Banks_20200517_2.xlsx,Holidays_Misc_20200517.xlsx</t>
+  </si>
+  <si>
+    <t>\DataSet\Integration_DataSet\TL\Calendar_GSFile\TL_CAL_18_Files\</t>
+  </si>
+  <si>
+    <t>\DataSet\Integration_DataSet\TL\Calendar_GSFile\TL_CAL_19_Files\</t>
+  </si>
+  <si>
+    <t>\DataSet\Integration_DataSet\TL\Calendar_GSFile\TL_CAL_20_Files\</t>
+  </si>
+  <si>
+    <t>\DataSet\Integration_DataSet\TL\Calendar_GSFile\TL_CAL_02_Files\</t>
+  </si>
+  <si>
+    <t>\DataSet\Integration_DataSet\TL\Calendar_GSFile\TL_CAL_03_Files\</t>
+  </si>
+  <si>
+    <t>\DataSet\Integration_DataSet\TL\Calendar_GSFile\TL_CAL_04_Files\</t>
+  </si>
+  <si>
+    <t>\DataSet\Integration_DataSet\TL\Calendar_GSFile\TL_CAL_07_Files\</t>
+  </si>
+  <si>
+    <t>\DataSet\Integration_DataSet\TL\Calendar_GSFile\TL_CAL_10_Files\</t>
+  </si>
+  <si>
+    <t>\DataSet\Integration_DataSet\TL\Calendar_GSFile\TL_CAL_12_Files\</t>
+  </si>
+  <si>
+    <t>\DataSet\Integration_DataSet\TL\Calendar_GSFile\TL_CAL_13_Files\</t>
+  </si>
+  <si>
+    <t>\DataSet\Integration_DataSet\TL\Calendar_GSFile\TL_CAL_14_Files\</t>
+  </si>
+  <si>
+    <t>\DataSet\Integration_DataSet\TL\Calendar_GSFile\TL_CAL_21_Files\</t>
+  </si>
+  <si>
+    <t>\DataSet\Integration_DataSet\TL\Calendar_GSFile\TL_CAL_25_Files\</t>
+  </si>
+  <si>
+    <t>\DataSet\Integration_DataSet\TL\Calendar_GSFile\TL_CAL_26_Files\</t>
+  </si>
+  <si>
+    <t>\DataSet\Integration_DataSet\TL\Calendar_GSFile\TL_CAL_27_Files\</t>
+  </si>
+  <si>
+    <t>\DataSet\Integration_DataSet\TL\Calendar_GSFile\TL_CAL_28_Files\</t>
+  </si>
+  <si>
+    <t>\DataSet\Integration_DataSet\TL\Calendar_GSFile\TL_CAL_29_Files\</t>
+  </si>
+  <si>
+    <t>\DataSet\Integration_DataSet\TL\Calendar_GSFile\TL_CAL_30_Files\</t>
+  </si>
+  <si>
+    <t>\DataSet\Integration_DataSet\TL\Calendar_GSFile\TL_CAL_31_Files\</t>
+  </si>
+  <si>
+    <t>\DataSet\Integration_DataSet\TL\Calendar_GSFile\TL_CAL_32_Files\</t>
+  </si>
+  <si>
+    <t>\DataSet\Integration_DataSet\TL\Calendar_GSFile\TL_CAL_33_Files\</t>
+  </si>
+  <si>
+    <t>\DataSet\Integration_DataSet\TL\Calendar_GSFile\TL_CAL_35_Files\</t>
+  </si>
+  <si>
+    <t>\DataSet\Integration_DataSet\TL\Calendar_GSFile\TL_CAL_36_Files\</t>
+  </si>
+  <si>
+    <t>\DataSet\Integration_DataSet\TL\Calendar_GSFile\TL_CAL_37_Files\</t>
+  </si>
+  <si>
+    <t>Holidays_Banks_20200318_1.csv,Holidays_Banks_20200318_1.xlsx,Holidays_Banks_20200318_2.csv,Holidays_Banks_20200318_2.xlsx,Holidays_Misc_20200318.xlsx</t>
+  </si>
+  <si>
+    <t>Holidays_Banks_20190125_2.xls,Holidays_Banks_20200125_1.csv,Holidays_Banks_20200125_2.csv,Holidays_Misc_20190125.xls</t>
   </si>
 </sst>
 </file>
@@ -4461,7 +4461,7 @@
         <v>17</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>1074</v>
+        <v>1048</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>1</v>
@@ -4494,7 +4494,7 @@
         <v>154</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>764</v>
+        <v>757</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
@@ -4505,10 +4505,10 @@
         <v>11</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>1075</v>
+        <v>1049</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>1076</v>
+        <v>1050</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>94</v>
@@ -4523,7 +4523,7 @@
         <v>18</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>1076</v>
+        <v>1050</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>21</v>
@@ -4546,10 +4546,10 @@
         <v>23</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>1075</v>
+        <v>1049</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>1085</v>
+        <v>1059</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>95</v>
@@ -4564,7 +4564,7 @@
         <v>25</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>1085</v>
+        <v>1059</v>
       </c>
       <c r="J3" s="5" t="s">
         <v>26</v>
@@ -4587,10 +4587,10 @@
         <v>30</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>1075</v>
+        <v>1049</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>1086</v>
+        <v>1060</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>140</v>
@@ -4605,7 +4605,7 @@
         <v>33</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>1086</v>
+        <v>1060</v>
       </c>
       <c r="J4" s="5" t="s">
         <v>34</v>
@@ -4617,7 +4617,7 @@
         <v>135</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>706</v>
+        <v>699</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
@@ -4628,10 +4628,10 @@
         <v>37</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>1075</v>
+        <v>1049</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>1087</v>
+        <v>1061</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>153</v>
@@ -4646,7 +4646,7 @@
         <v>40</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>1087</v>
+        <v>1061</v>
       </c>
       <c r="J5" s="5" t="s">
         <v>41</v>
@@ -4669,10 +4669,10 @@
         <v>50</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>1075</v>
+        <v>1049</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>1088</v>
+        <v>1062</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>51</v>
@@ -4687,7 +4687,7 @@
         <v>54</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>1088</v>
+        <v>1062</v>
       </c>
       <c r="J6" s="5" t="s">
         <v>55</v>
@@ -4710,13 +4710,13 @@
         <v>58</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>1075</v>
+        <v>1049</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>1089</v>
+        <v>1063</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>889</v>
+        <v>872</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>59</v>
@@ -4728,7 +4728,7 @@
         <v>61</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>1089</v>
+        <v>1063</v>
       </c>
       <c r="J7" s="5" t="s">
         <v>62</v>
@@ -4740,7 +4740,7 @@
         <v>138</v>
       </c>
       <c r="M7" s="5" t="s">
-        <v>702</v>
+        <v>695</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
@@ -4751,13 +4751,13 @@
         <v>65</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>1075</v>
+        <v>1049</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>1090</v>
+        <v>1064</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>890</v>
+        <v>873</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>66</v>
@@ -4769,7 +4769,7 @@
         <v>68</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>1090</v>
+        <v>1064</v>
       </c>
       <c r="J8" s="5" t="s">
         <v>69</v>
@@ -4778,10 +4778,10 @@
         <v>70</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>699</v>
+        <v>692</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>703</v>
+        <v>696</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
@@ -4792,13 +4792,13 @@
         <v>97</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>1075</v>
+        <v>1049</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>1091</v>
+        <v>1065</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>891</v>
+        <v>874</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>98</v>
@@ -4810,7 +4810,7 @@
         <v>100</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>1091</v>
+        <v>1065</v>
       </c>
       <c r="J9" s="5" t="s">
         <v>101</v>
@@ -4819,10 +4819,10 @@
         <v>102</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>700</v>
+        <v>693</v>
       </c>
       <c r="M9" s="5" t="s">
-        <v>704</v>
+        <v>697</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
@@ -4833,10 +4833,10 @@
         <v>104</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>1075</v>
+        <v>1049</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>1092</v>
+        <v>1066</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>105</v>
@@ -4851,7 +4851,7 @@
         <v>108</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>1092</v>
+        <v>1066</v>
       </c>
       <c r="J10" s="5" t="s">
         <v>109</v>
@@ -4860,10 +4860,10 @@
         <v>110</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>701</v>
+        <v>694</v>
       </c>
       <c r="M10" s="5" t="s">
-        <v>705</v>
+        <v>698</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
@@ -4874,10 +4874,10 @@
         <v>156</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>1075</v>
+        <v>1049</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>1093</v>
+        <v>1067</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>112</v>
@@ -4892,7 +4892,7 @@
         <v>159</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>1093</v>
+        <v>1067</v>
       </c>
       <c r="J11" s="5" t="s">
         <v>160</v>
@@ -4915,10 +4915,10 @@
         <v>169</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>1075</v>
+        <v>1049</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>1095</v>
+        <v>1069</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>114</v>
@@ -4933,7 +4933,7 @@
         <v>191</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>1095</v>
+        <v>1069</v>
       </c>
       <c r="J12" s="5" t="s">
         <v>196</v>
@@ -4956,10 +4956,10 @@
         <v>170</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>1075</v>
+        <v>1049</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>1096</v>
+        <v>1070</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>116</v>
@@ -4974,7 +4974,7 @@
         <v>192</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>1096</v>
+        <v>1070</v>
       </c>
       <c r="J13" s="5" t="s">
         <v>197</v>
@@ -4997,10 +4997,10 @@
         <v>171</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>1075</v>
+        <v>1049</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>1097</v>
+        <v>1071</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>118</v>
@@ -5015,7 +5015,7 @@
         <v>193</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>1097</v>
+        <v>1071</v>
       </c>
       <c r="J14" s="5" t="s">
         <v>198</v>
@@ -5038,10 +5038,10 @@
         <v>172</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>1075</v>
+        <v>1049</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>1098</v>
+        <v>1072</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>120</v>
@@ -5056,7 +5056,7 @@
         <v>194</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>1098</v>
+        <v>1072</v>
       </c>
       <c r="J15" s="5" t="s">
         <v>199</v>
@@ -5079,10 +5079,10 @@
         <v>173</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>1075</v>
+        <v>1049</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>1099</v>
+        <v>1073</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>152</v>
@@ -5097,7 +5097,7 @@
         <v>148</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>1099</v>
+        <v>1073</v>
       </c>
       <c r="J16" s="5" t="s">
         <v>149</v>
@@ -5117,40 +5117,40 @@
         <v>332</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>892</v>
+        <v>875</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>1075</v>
+        <v>1049</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>1100</v>
+        <v>1074</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>893</v>
+        <v>876</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>894</v>
+        <v>877</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>895</v>
+        <v>878</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>896</v>
+        <v>879</v>
       </c>
       <c r="I17" s="9" t="s">
-        <v>1100</v>
+        <v>1074</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>897</v>
+        <v>880</v>
       </c>
       <c r="K17" s="5" t="s">
-        <v>898</v>
+        <v>881</v>
       </c>
       <c r="L17" s="5" t="s">
-        <v>899</v>
+        <v>882</v>
       </c>
       <c r="M17" s="5" t="s">
-        <v>900</v>
+        <v>883</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
@@ -5158,40 +5158,40 @@
         <v>342</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>1039</v>
+        <v>1014</v>
       </c>
       <c r="C18" s="9" t="s">
+        <v>1049</v>
+      </c>
+      <c r="D18" s="9" t="s">
         <v>1075</v>
       </c>
-      <c r="D18" s="9" t="s">
-        <v>1101</v>
-      </c>
       <c r="E18" s="5" t="s">
-        <v>1040</v>
+        <v>1015</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>1041</v>
+        <v>1016</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>1042</v>
+        <v>1017</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>1043</v>
+        <v>1018</v>
       </c>
       <c r="I18" s="9" t="s">
-        <v>1101</v>
+        <v>1075</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>1044</v>
+        <v>1019</v>
       </c>
       <c r="K18" s="5" t="s">
-        <v>1045</v>
+        <v>1020</v>
       </c>
       <c r="L18" s="5" t="s">
-        <v>1046</v>
+        <v>1021</v>
       </c>
       <c r="M18" s="5" t="s">
-        <v>1047</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
@@ -5199,40 +5199,40 @@
         <v>352</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>981</v>
+        <v>961</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>1075</v>
+        <v>1049</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>1102</v>
+        <v>1076</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>982</v>
+        <v>962</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>983</v>
+        <v>963</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>984</v>
+        <v>964</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>985</v>
+        <v>965</v>
       </c>
       <c r="I19" s="9" t="s">
-        <v>1102</v>
+        <v>1076</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>986</v>
+        <v>966</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>987</v>
+        <v>967</v>
       </c>
       <c r="L19" s="5" t="s">
-        <v>988</v>
+        <v>968</v>
       </c>
       <c r="M19" s="5" t="s">
-        <v>989</v>
+        <v>969</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
@@ -5243,10 +5243,10 @@
         <v>174</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>1075</v>
+        <v>1049</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>1103</v>
+        <v>1077</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>206</v>
@@ -5261,7 +5261,7 @@
         <v>195</v>
       </c>
       <c r="I20" s="9" t="s">
-        <v>1103</v>
+        <v>1077</v>
       </c>
       <c r="J20" s="5" t="s">
         <v>200</v>
@@ -5284,10 +5284,10 @@
         <v>219</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>1075</v>
+        <v>1049</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>1104</v>
+        <v>1078</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>210</v>
@@ -5302,7 +5302,7 @@
         <v>214</v>
       </c>
       <c r="I21" s="9" t="s">
-        <v>1104</v>
+        <v>1078</v>
       </c>
       <c r="J21" s="5" t="s">
         <v>215</v>
@@ -5325,10 +5325,10 @@
         <v>220</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>1075</v>
+        <v>1049</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>1094</v>
+        <v>1068</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>221</v>
@@ -5343,7 +5343,7 @@
         <v>224</v>
       </c>
       <c r="I22" s="9" t="s">
-        <v>1094</v>
+        <v>1068</v>
       </c>
       <c r="J22" s="5" t="s">
         <v>225</v>
@@ -5366,10 +5366,10 @@
         <v>230</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>1075</v>
+        <v>1049</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>1105</v>
+        <v>1079</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>239</v>
@@ -5384,7 +5384,7 @@
         <v>234</v>
       </c>
       <c r="I23" s="9" t="s">
-        <v>1105</v>
+        <v>1079</v>
       </c>
       <c r="J23" s="5" t="s">
         <v>235</v>
@@ -5404,40 +5404,40 @@
         <v>427</v>
       </c>
       <c r="B24" s="5" t="s">
+        <v>554</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>1049</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>1080</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>556</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>557</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>558</v>
+      </c>
+      <c r="I24" s="9" t="s">
+        <v>1080</v>
+      </c>
+      <c r="J24" s="5" t="s">
         <v>559</v>
       </c>
-      <c r="C24" s="9" t="s">
-        <v>1075</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>1106</v>
-      </c>
-      <c r="E24" s="6" t="s">
+      <c r="K24" s="5" t="s">
         <v>560</v>
       </c>
-      <c r="F24" s="5" t="s">
+      <c r="L24" s="5" t="s">
         <v>561</v>
       </c>
-      <c r="G24" s="5" t="s">
+      <c r="M24" s="5" t="s">
         <v>562</v>
-      </c>
-      <c r="H24" s="5" t="s">
-        <v>563</v>
-      </c>
-      <c r="I24" s="9" t="s">
-        <v>1106</v>
-      </c>
-      <c r="J24" s="5" t="s">
-        <v>564</v>
-      </c>
-      <c r="K24" s="5" t="s">
-        <v>565</v>
-      </c>
-      <c r="L24" s="5" t="s">
-        <v>566</v>
-      </c>
-      <c r="M24" s="5" t="s">
-        <v>567</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
@@ -5445,40 +5445,40 @@
         <v>437</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>576</v>
+        <v>571</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>1075</v>
+        <v>1049</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>1107</v>
+        <v>1081</v>
       </c>
       <c r="E25" s="6" t="s">
+        <v>563</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>564</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>565</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>566</v>
+      </c>
+      <c r="I25" s="9" t="s">
+        <v>1081</v>
+      </c>
+      <c r="J25" s="5" t="s">
+        <v>567</v>
+      </c>
+      <c r="K25" s="5" t="s">
         <v>568</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="L25" s="5" t="s">
         <v>569</v>
       </c>
-      <c r="G25" s="5" t="s">
+      <c r="M25" s="5" t="s">
         <v>570</v>
-      </c>
-      <c r="H25" s="5" t="s">
-        <v>571</v>
-      </c>
-      <c r="I25" s="9" t="s">
-        <v>1107</v>
-      </c>
-      <c r="J25" s="5" t="s">
-        <v>572</v>
-      </c>
-      <c r="K25" s="5" t="s">
-        <v>573</v>
-      </c>
-      <c r="L25" s="5" t="s">
-        <v>574</v>
-      </c>
-      <c r="M25" s="5" t="s">
-        <v>575</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -5486,40 +5486,40 @@
         <v>447</v>
       </c>
       <c r="B26" s="5" t="s">
+        <v>683</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>1049</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>1082</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>684</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>685</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>686</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>687</v>
+      </c>
+      <c r="I26" s="9" t="s">
+        <v>1082</v>
+      </c>
+      <c r="J26" s="5" t="s">
+        <v>688</v>
+      </c>
+      <c r="K26" s="5" t="s">
+        <v>689</v>
+      </c>
+      <c r="L26" s="5" t="s">
         <v>690</v>
       </c>
-      <c r="C26" s="9" t="s">
-        <v>1075</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>1108</v>
-      </c>
-      <c r="E26" s="6" t="s">
+      <c r="M26" s="5" t="s">
         <v>691</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>692</v>
-      </c>
-      <c r="G26" s="5" t="s">
-        <v>693</v>
-      </c>
-      <c r="H26" s="5" t="s">
-        <v>694</v>
-      </c>
-      <c r="I26" s="9" t="s">
-        <v>1108</v>
-      </c>
-      <c r="J26" s="5" t="s">
-        <v>695</v>
-      </c>
-      <c r="K26" s="5" t="s">
-        <v>696</v>
-      </c>
-      <c r="L26" s="5" t="s">
-        <v>697</v>
-      </c>
-      <c r="M26" s="5" t="s">
-        <v>698</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
@@ -5527,40 +5527,40 @@
         <v>457</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>1048</v>
+        <v>1023</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>1075</v>
+        <v>1049</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>1084</v>
+        <v>1058</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>1049</v>
+        <v>1024</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>1050</v>
+        <v>1025</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>1051</v>
+        <v>1026</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>1052</v>
+        <v>1027</v>
       </c>
       <c r="I27" s="9" t="s">
-        <v>1084</v>
+        <v>1058</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>1053</v>
+        <v>1028</v>
       </c>
       <c r="K27" s="5" t="s">
-        <v>1054</v>
+        <v>1029</v>
       </c>
       <c r="L27" s="5" t="s">
-        <v>1055</v>
+        <v>1030</v>
       </c>
       <c r="M27" s="5" t="s">
-        <v>1056</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
@@ -5568,618 +5568,618 @@
         <v>467</v>
       </c>
       <c r="B28" s="5" t="s">
+        <v>658</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>1049</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>1083</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>659</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>660</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>661</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>662</v>
+      </c>
+      <c r="I28" s="9" t="s">
+        <v>1083</v>
+      </c>
+      <c r="J28" s="5" t="s">
+        <v>663</v>
+      </c>
+      <c r="K28" s="5" t="s">
         <v>664</v>
       </c>
-      <c r="C28" s="9" t="s">
-        <v>1075</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>1109</v>
-      </c>
-      <c r="E28" s="6" t="s">
+      <c r="L28" s="5" t="s">
         <v>665</v>
       </c>
-      <c r="F28" s="5" t="s">
+      <c r="M28" s="5" t="s">
         <v>666</v>
-      </c>
-      <c r="G28" s="5" t="s">
-        <v>667</v>
-      </c>
-      <c r="H28" s="5" t="s">
-        <v>668</v>
-      </c>
-      <c r="I28" s="9" t="s">
-        <v>1109</v>
-      </c>
-      <c r="J28" s="5" t="s">
-        <v>669</v>
-      </c>
-      <c r="K28" s="5" t="s">
-        <v>670</v>
-      </c>
-      <c r="L28" s="5" t="s">
-        <v>671</v>
-      </c>
-      <c r="M28" s="5" t="s">
-        <v>672</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="11" t="s">
-        <v>585</v>
+        <v>579</v>
       </c>
       <c r="B29" s="5" t="s">
+        <v>667</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>1049</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>1084</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>668</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>669</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>670</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>671</v>
+      </c>
+      <c r="I29" s="9" t="s">
+        <v>1084</v>
+      </c>
+      <c r="J29" s="5" t="s">
+        <v>672</v>
+      </c>
+      <c r="K29" s="5" t="s">
         <v>673</v>
       </c>
-      <c r="C29" s="9" t="s">
-        <v>1075</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>1110</v>
-      </c>
-      <c r="E29" s="6" t="s">
+      <c r="L29" s="5" t="s">
         <v>674</v>
       </c>
-      <c r="F29" s="5" t="s">
+      <c r="M29" s="5" t="s">
         <v>675</v>
-      </c>
-      <c r="G29" s="5" t="s">
-        <v>676</v>
-      </c>
-      <c r="H29" s="5" t="s">
-        <v>677</v>
-      </c>
-      <c r="I29" s="9" t="s">
-        <v>1110</v>
-      </c>
-      <c r="J29" s="5" t="s">
-        <v>678</v>
-      </c>
-      <c r="K29" s="5" t="s">
-        <v>679</v>
-      </c>
-      <c r="L29" s="5" t="s">
-        <v>680</v>
-      </c>
-      <c r="M29" s="5" t="s">
-        <v>681</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
-        <v>603</v>
+        <v>597</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>707</v>
+        <v>700</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>1075</v>
+        <v>1049</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>1111</v>
+        <v>1085</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>721</v>
+        <v>714</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>708</v>
+        <v>701</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>709</v>
+        <v>702</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>710</v>
+        <v>703</v>
       </c>
       <c r="I30" s="9" t="s">
-        <v>1111</v>
+        <v>1085</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>711</v>
+        <v>704</v>
       </c>
       <c r="K30" s="5" t="s">
-        <v>712</v>
+        <v>705</v>
       </c>
       <c r="L30" s="5" t="s">
-        <v>722</v>
+        <v>715</v>
       </c>
       <c r="M30" s="5" t="s">
-        <v>713</v>
+        <v>706</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="11" t="s">
-        <v>720</v>
+        <v>713</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>707</v>
+        <v>700</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>1075</v>
+        <v>1049</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>1111</v>
+        <v>1085</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>719</v>
+        <v>712</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>708</v>
+        <v>701</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>709</v>
+        <v>702</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>710</v>
+        <v>703</v>
       </c>
       <c r="I31" s="9" t="s">
-        <v>1111</v>
+        <v>1085</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>711</v>
+        <v>704</v>
       </c>
       <c r="K31" s="5" t="s">
-        <v>712</v>
+        <v>705</v>
       </c>
       <c r="L31" s="5" t="s">
-        <v>723</v>
+        <v>716</v>
       </c>
       <c r="M31" s="5" t="s">
-        <v>713</v>
+        <v>706</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
-        <v>612</v>
+        <v>606</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>901</v>
+        <v>884</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>1075</v>
+        <v>1049</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>1112</v>
+        <v>1086</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>902</v>
+        <v>885</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>903</v>
+        <v>886</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>904</v>
+        <v>887</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>905</v>
+        <v>888</v>
       </c>
       <c r="I32" s="9" t="s">
-        <v>1112</v>
+        <v>1086</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>906</v>
+        <v>889</v>
       </c>
       <c r="K32" s="5" t="s">
-        <v>907</v>
+        <v>890</v>
       </c>
       <c r="L32" s="5" t="s">
-        <v>908</v>
+        <v>891</v>
       </c>
       <c r="M32" s="5" t="s">
-        <v>909</v>
+        <v>892</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" s="11" t="s">
-        <v>621</v>
+        <v>615</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>910</v>
+        <v>893</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>1075</v>
+        <v>1049</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>1113</v>
+        <v>1087</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>911</v>
+        <v>894</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>912</v>
+        <v>895</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>913</v>
+        <v>896</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>914</v>
+        <v>897</v>
       </c>
       <c r="I33" s="9" t="s">
-        <v>1113</v>
+        <v>1087</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>915</v>
+        <v>898</v>
       </c>
       <c r="K33" s="5" t="s">
-        <v>916</v>
+        <v>899</v>
       </c>
       <c r="L33" s="5" t="s">
-        <v>917</v>
+        <v>900</v>
       </c>
       <c r="M33" s="5" t="s">
-        <v>918</v>
+        <v>901</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" s="11" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>919</v>
+        <v>902</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>1075</v>
+        <v>1049</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>1114</v>
+        <v>1088</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>920</v>
+        <v>903</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>921</v>
+        <v>904</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>922</v>
+        <v>905</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>923</v>
+        <v>906</v>
       </c>
       <c r="I34" s="9" t="s">
-        <v>1114</v>
+        <v>1088</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>924</v>
+        <v>907</v>
       </c>
       <c r="K34" s="5" t="s">
-        <v>925</v>
+        <v>908</v>
       </c>
       <c r="L34" s="5" t="s">
-        <v>926</v>
+        <v>909</v>
       </c>
       <c r="M34" s="5" t="s">
-        <v>927</v>
+        <v>910</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" s="11" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>928</v>
+        <v>911</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>1075</v>
+        <v>1049</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>1115</v>
+        <v>1089</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>929</v>
+        <v>912</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>930</v>
+        <v>913</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>931</v>
+        <v>914</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>932</v>
+        <v>915</v>
       </c>
       <c r="I35" s="9" t="s">
-        <v>1115</v>
+        <v>1089</v>
       </c>
       <c r="J35" s="5" t="s">
-        <v>933</v>
+        <v>916</v>
       </c>
       <c r="K35" s="5" t="s">
-        <v>934</v>
+        <v>917</v>
       </c>
       <c r="L35" s="5" t="s">
-        <v>935</v>
+        <v>918</v>
       </c>
       <c r="M35" s="5" t="s">
-        <v>936</v>
+        <v>919</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36" s="11" t="s">
-        <v>937</v>
+        <v>920</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>938</v>
+        <v>921</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>1075</v>
+        <v>1049</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>1083</v>
+        <v>1057</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>939</v>
+        <v>922</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>940</v>
+        <v>923</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>941</v>
+        <v>924</v>
       </c>
       <c r="H36" s="5" t="s">
-        <v>942</v>
+        <v>925</v>
       </c>
       <c r="I36" s="9" t="s">
-        <v>1083</v>
+        <v>1057</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>943</v>
+        <v>926</v>
       </c>
       <c r="K36" s="5" t="s">
-        <v>944</v>
+        <v>927</v>
       </c>
       <c r="L36" s="5" t="s">
-        <v>945</v>
+        <v>928</v>
       </c>
       <c r="M36" s="5" t="s">
-        <v>946</v>
+        <v>929</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
-        <v>1057</v>
+        <v>1032</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>1058</v>
+        <v>1033</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>1075</v>
+        <v>1049</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>1116</v>
+        <v>1090</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>1059</v>
+        <v>1034</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>1060</v>
+        <v>1035</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>1061</v>
+        <v>1036</v>
       </c>
       <c r="H37" s="5" t="s">
-        <v>1062</v>
+        <v>1037</v>
       </c>
       <c r="I37" s="9" t="s">
-        <v>1116</v>
+        <v>1090</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>1063</v>
+        <v>1038</v>
       </c>
       <c r="K37" s="5" t="s">
-        <v>1064</v>
+        <v>1039</v>
       </c>
       <c r="L37" s="5" t="s">
-        <v>1065</v>
+        <v>1040</v>
       </c>
       <c r="M37" s="5" t="s">
-        <v>1066</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A38" s="11" t="s">
+        <v>717</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>718</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>1049</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>1091</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>719</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>720</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>721</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>722</v>
+      </c>
+      <c r="I38" s="9" t="s">
+        <v>1091</v>
+      </c>
+      <c r="J38" s="5" t="s">
+        <v>723</v>
+      </c>
+      <c r="K38" s="5" t="s">
         <v>724</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="L38" s="5" t="s">
         <v>725</v>
       </c>
-      <c r="C38" s="9" t="s">
-        <v>1075</v>
-      </c>
-      <c r="D38" s="9" t="s">
-        <v>1117</v>
-      </c>
-      <c r="E38" s="6" t="s">
+      <c r="M38" s="5" t="s">
         <v>726</v>
-      </c>
-      <c r="F38" s="5" t="s">
-        <v>727</v>
-      </c>
-      <c r="G38" s="5" t="s">
-        <v>728</v>
-      </c>
-      <c r="H38" s="5" t="s">
-        <v>729</v>
-      </c>
-      <c r="I38" s="9" t="s">
-        <v>1117</v>
-      </c>
-      <c r="J38" s="5" t="s">
-        <v>730</v>
-      </c>
-      <c r="K38" s="5" t="s">
-        <v>731</v>
-      </c>
-      <c r="L38" s="5" t="s">
-        <v>732</v>
-      </c>
-      <c r="M38" s="5" t="s">
-        <v>733</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A39" s="11" t="s">
+        <v>747</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>748</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>1049</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>1092</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>749</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>750</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>751</v>
+      </c>
+      <c r="H39" s="5" t="s">
+        <v>752</v>
+      </c>
+      <c r="I39" s="9" t="s">
+        <v>1092</v>
+      </c>
+      <c r="J39" s="5" t="s">
+        <v>753</v>
+      </c>
+      <c r="K39" s="5" t="s">
         <v>754</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="L39" s="5" t="s">
         <v>755</v>
       </c>
-      <c r="C39" s="9" t="s">
-        <v>1075</v>
-      </c>
-      <c r="D39" s="9" t="s">
-        <v>1118</v>
-      </c>
-      <c r="E39" s="6" t="s">
+      <c r="M39" s="5" t="s">
         <v>756</v>
       </c>
-      <c r="F39" s="5" t="s">
-        <v>757</v>
-      </c>
-      <c r="G39" s="5" t="s">
+      <c r="N39" s="5" t="s">
         <v>758</v>
-      </c>
-      <c r="H39" s="5" t="s">
-        <v>759</v>
-      </c>
-      <c r="I39" s="9" t="s">
-        <v>1118</v>
-      </c>
-      <c r="J39" s="5" t="s">
-        <v>760</v>
-      </c>
-      <c r="K39" s="5" t="s">
-        <v>761</v>
-      </c>
-      <c r="L39" s="5" t="s">
-        <v>762</v>
-      </c>
-      <c r="M39" s="5" t="s">
-        <v>763</v>
-      </c>
-      <c r="N39" s="5" t="s">
-        <v>765</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A40" s="11" t="s">
+        <v>759</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>760</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>1049</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>761</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>762</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>763</v>
+      </c>
+      <c r="H40" s="5" t="s">
+        <v>764</v>
+      </c>
+      <c r="I40" s="9" t="s">
+        <v>1093</v>
+      </c>
+      <c r="J40" s="5" t="s">
+        <v>765</v>
+      </c>
+      <c r="K40" s="5" t="s">
         <v>766</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="L40" s="5" t="s">
         <v>767</v>
       </c>
-      <c r="C40" s="9" t="s">
-        <v>1075</v>
-      </c>
-      <c r="D40" s="9" t="s">
-        <v>1119</v>
-      </c>
-      <c r="E40" s="6" t="s">
+      <c r="M40" s="5" t="s">
         <v>768</v>
-      </c>
-      <c r="F40" s="5" t="s">
-        <v>769</v>
-      </c>
-      <c r="G40" s="5" t="s">
-        <v>770</v>
-      </c>
-      <c r="H40" s="5" t="s">
-        <v>771</v>
-      </c>
-      <c r="I40" s="9" t="s">
-        <v>1119</v>
-      </c>
-      <c r="J40" s="5" t="s">
-        <v>772</v>
-      </c>
-      <c r="K40" s="5" t="s">
-        <v>773</v>
-      </c>
-      <c r="L40" s="5" t="s">
-        <v>774</v>
-      </c>
-      <c r="M40" s="5" t="s">
-        <v>775</v>
       </c>
       <c r="N40" s="5"/>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A41" s="11" t="s">
+        <v>727</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>728</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>1049</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>1094</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>729</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>730</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>731</v>
+      </c>
+      <c r="H41" s="5" t="s">
+        <v>732</v>
+      </c>
+      <c r="I41" s="9" t="s">
+        <v>1094</v>
+      </c>
+      <c r="J41" s="5" t="s">
+        <v>733</v>
+      </c>
+      <c r="K41" s="5" t="s">
         <v>734</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="L41" s="5" t="s">
         <v>735</v>
       </c>
-      <c r="C41" s="9" t="s">
-        <v>1075</v>
-      </c>
-      <c r="D41" s="9" t="s">
-        <v>1120</v>
-      </c>
-      <c r="E41" s="6" t="s">
+      <c r="M41" s="5" t="s">
         <v>736</v>
-      </c>
-      <c r="F41" s="5" t="s">
-        <v>737</v>
-      </c>
-      <c r="G41" s="5" t="s">
-        <v>738</v>
-      </c>
-      <c r="H41" s="5" t="s">
-        <v>739</v>
-      </c>
-      <c r="I41" s="9" t="s">
-        <v>1120</v>
-      </c>
-      <c r="J41" s="5" t="s">
-        <v>740</v>
-      </c>
-      <c r="K41" s="5" t="s">
-        <v>741</v>
-      </c>
-      <c r="L41" s="5" t="s">
-        <v>742</v>
-      </c>
-      <c r="M41" s="5" t="s">
-        <v>743</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A42" s="11" t="s">
+        <v>737</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>738</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>1049</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>1095</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>739</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>740</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>741</v>
+      </c>
+      <c r="H42" s="5" t="s">
+        <v>742</v>
+      </c>
+      <c r="I42" s="9" t="s">
+        <v>1095</v>
+      </c>
+      <c r="J42" s="5" t="s">
+        <v>743</v>
+      </c>
+      <c r="K42" s="5" t="s">
         <v>744</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="L42" s="5" t="s">
         <v>745</v>
       </c>
-      <c r="C42" s="9" t="s">
-        <v>1075</v>
-      </c>
-      <c r="D42" s="9" t="s">
-        <v>1121</v>
-      </c>
-      <c r="E42" s="6" t="s">
+      <c r="M42" s="5" t="s">
         <v>746</v>
-      </c>
-      <c r="F42" s="5" t="s">
-        <v>747</v>
-      </c>
-      <c r="G42" s="5" t="s">
-        <v>748</v>
-      </c>
-      <c r="H42" s="5" t="s">
-        <v>749</v>
-      </c>
-      <c r="I42" s="9" t="s">
-        <v>1121</v>
-      </c>
-      <c r="J42" s="5" t="s">
-        <v>750</v>
-      </c>
-      <c r="K42" s="5" t="s">
-        <v>751</v>
-      </c>
-      <c r="L42" s="5" t="s">
-        <v>752</v>
-      </c>
-      <c r="M42" s="5" t="s">
-        <v>753</v>
       </c>
     </row>
   </sheetData>
@@ -6249,7 +6249,7 @@
         <v>17</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>1074</v>
+        <v>1048</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>1</v>
@@ -6288,7 +6288,7 @@
         <v>121</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>1067</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
@@ -6299,10 +6299,10 @@
         <v>44</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>1077</v>
+        <v>1051</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>1078</v>
+        <v>1052</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>131</v>
@@ -6317,7 +6317,7 @@
         <v>48</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>1078</v>
+        <v>1052</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>129</v>
@@ -6362,7 +6362,7 @@
         <v>74</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>658</v>
+        <v>652</v>
       </c>
       <c r="J3" s="5" t="s">
         <v>75</v>
@@ -6407,7 +6407,7 @@
         <v>85</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>659</v>
+        <v>653</v>
       </c>
       <c r="J4" s="5" t="s">
         <v>81</v>
@@ -6452,7 +6452,7 @@
         <v>86</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>660</v>
+        <v>654</v>
       </c>
       <c r="J5" s="5" t="s">
         <v>82</v>
@@ -6497,7 +6497,7 @@
         <v>91</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>661</v>
+        <v>655</v>
       </c>
       <c r="J6" s="5" t="s">
         <v>92</v>
@@ -6542,7 +6542,7 @@
         <v>126</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>662</v>
+        <v>656</v>
       </c>
       <c r="J7" s="5" t="s">
         <v>127</v>
@@ -6575,7 +6575,7 @@
         <v>130</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>977</v>
+        <v>957</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>259</v>
@@ -6587,7 +6587,7 @@
         <v>261</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>663</v>
+        <v>657</v>
       </c>
       <c r="J8" s="5" t="s">
         <v>262</v>
@@ -6620,7 +6620,7 @@
         <v>130</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>978</v>
+        <v>958</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>267</v>
@@ -6632,7 +6632,7 @@
         <v>269</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>657</v>
+        <v>651</v>
       </c>
       <c r="J9" s="5" t="s">
         <v>270</v>
@@ -6665,7 +6665,7 @@
         <v>130</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>979</v>
+        <v>959</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>275</v>
@@ -6677,7 +6677,7 @@
         <v>277</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>656</v>
+        <v>650</v>
       </c>
       <c r="J10" s="5" t="s">
         <v>278</v>
@@ -6710,7 +6710,7 @@
         <v>130</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>980</v>
+        <v>960</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>283</v>
@@ -6722,7 +6722,7 @@
         <v>285</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>647</v>
+        <v>641</v>
       </c>
       <c r="J11" s="5" t="s">
         <v>286</v>
@@ -6755,7 +6755,7 @@
         <v>130</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>1071</v>
+        <v>1045</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>291</v>
@@ -6767,7 +6767,7 @@
         <v>293</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>648</v>
+        <v>642</v>
       </c>
       <c r="J12" s="5" t="s">
         <v>294</v>
@@ -6800,7 +6800,7 @@
         <v>130</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>1072</v>
+        <v>1046</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>299</v>
@@ -6812,7 +6812,7 @@
         <v>301</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>649</v>
+        <v>643</v>
       </c>
       <c r="J13" s="5" t="s">
         <v>302</v>
@@ -6845,7 +6845,7 @@
         <v>130</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>1073</v>
+        <v>1047</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>307</v>
@@ -6857,7 +6857,7 @@
         <v>309</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>650</v>
+        <v>644</v>
       </c>
       <c r="J14" s="5" t="s">
         <v>310</v>
@@ -6902,7 +6902,7 @@
         <v>318</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>651</v>
+        <v>645</v>
       </c>
       <c r="J15" s="5" t="s">
         <v>319</v>
@@ -6947,7 +6947,7 @@
         <v>327</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>652</v>
+        <v>646</v>
       </c>
       <c r="J16" s="5" t="s">
         <v>328</v>
@@ -6992,7 +6992,7 @@
         <v>337</v>
       </c>
       <c r="I17" s="9" t="s">
-        <v>653</v>
+        <v>647</v>
       </c>
       <c r="J17" s="5" t="s">
         <v>338</v>
@@ -7037,7 +7037,7 @@
         <v>347</v>
       </c>
       <c r="I18" s="9" t="s">
-        <v>654</v>
+        <v>648</v>
       </c>
       <c r="J18" s="5" t="s">
         <v>348</v>
@@ -7082,7 +7082,7 @@
         <v>357</v>
       </c>
       <c r="I19" s="9" t="s">
-        <v>655</v>
+        <v>649</v>
       </c>
       <c r="J19" s="5" t="s">
         <v>358</v>
@@ -7127,7 +7127,7 @@
         <v>366</v>
       </c>
       <c r="I20" s="9" t="s">
-        <v>646</v>
+        <v>640</v>
       </c>
       <c r="J20" s="5" t="s">
         <v>367</v>
@@ -7148,7 +7148,7 @@
         <v>242</v>
       </c>
       <c r="P20" s="5" t="s">
-        <v>1068</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
@@ -7175,7 +7175,7 @@
         <v>375</v>
       </c>
       <c r="I21" s="9" t="s">
-        <v>637</v>
+        <v>631</v>
       </c>
       <c r="J21" s="5" t="s">
         <v>376</v>
@@ -7220,7 +7220,7 @@
         <v>384</v>
       </c>
       <c r="I22" s="9" t="s">
-        <v>638</v>
+        <v>632</v>
       </c>
       <c r="J22" s="5" t="s">
         <v>385</v>
@@ -7265,7 +7265,7 @@
         <v>393</v>
       </c>
       <c r="I23" s="9" t="s">
-        <v>639</v>
+        <v>633</v>
       </c>
       <c r="J23" s="5" t="s">
         <v>394</v>
@@ -7310,7 +7310,7 @@
         <v>403</v>
       </c>
       <c r="I24" s="9" t="s">
-        <v>640</v>
+        <v>634</v>
       </c>
       <c r="J24" s="5" t="s">
         <v>404</v>
@@ -7355,7 +7355,7 @@
         <v>413</v>
       </c>
       <c r="I25" s="9" t="s">
-        <v>641</v>
+        <v>635</v>
       </c>
       <c r="J25" s="5" t="s">
         <v>414</v>
@@ -7400,7 +7400,7 @@
         <v>422</v>
       </c>
       <c r="I26" s="9" t="s">
-        <v>642</v>
+        <v>636</v>
       </c>
       <c r="J26" s="5" t="s">
         <v>423</v>
@@ -7445,7 +7445,7 @@
         <v>432</v>
       </c>
       <c r="I27" s="9" t="s">
-        <v>643</v>
+        <v>637</v>
       </c>
       <c r="J27" s="5" t="s">
         <v>433</v>
@@ -7490,7 +7490,7 @@
         <v>442</v>
       </c>
       <c r="I28" s="9" t="s">
-        <v>644</v>
+        <v>638</v>
       </c>
       <c r="J28" s="5" t="s">
         <v>443</v>
@@ -7535,7 +7535,7 @@
         <v>452</v>
       </c>
       <c r="I29" s="9" t="s">
-        <v>645</v>
+        <v>639</v>
       </c>
       <c r="J29" s="5" t="s">
         <v>453</v>
@@ -7580,7 +7580,7 @@
         <v>462</v>
       </c>
       <c r="I30" s="9" t="s">
-        <v>636</v>
+        <v>630</v>
       </c>
       <c r="J30" s="5" t="s">
         <v>463</v>
@@ -7625,7 +7625,7 @@
         <v>472</v>
       </c>
       <c r="I31" s="9" t="s">
-        <v>635</v>
+        <v>629</v>
       </c>
       <c r="J31" s="5" t="s">
         <v>473</v>
@@ -7648,41 +7648,41 @@
     </row>
     <row r="32" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
-        <v>585</v>
+        <v>579</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>586</v>
+        <v>580</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="9" t="s">
         <v>130</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>714</v>
+        <v>707</v>
       </c>
       <c r="F32" s="5" t="s">
+        <v>581</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>582</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>583</v>
+      </c>
+      <c r="I32" s="9" t="s">
+        <v>628</v>
+      </c>
+      <c r="J32" s="5" t="s">
+        <v>584</v>
+      </c>
+      <c r="K32" s="5" t="s">
+        <v>585</v>
+      </c>
+      <c r="L32" s="5" t="s">
+        <v>586</v>
+      </c>
+      <c r="M32" s="5" t="s">
         <v>587</v>
-      </c>
-      <c r="G32" s="5" t="s">
-        <v>588</v>
-      </c>
-      <c r="H32" s="5" t="s">
-        <v>589</v>
-      </c>
-      <c r="I32" s="9" t="s">
-        <v>634</v>
-      </c>
-      <c r="J32" s="5" t="s">
-        <v>590</v>
-      </c>
-      <c r="K32" s="5" t="s">
-        <v>591</v>
-      </c>
-      <c r="L32" s="5" t="s">
-        <v>592</v>
-      </c>
-      <c r="M32" s="5" t="s">
-        <v>593</v>
       </c>
       <c r="N32" s="5" t="s">
         <v>12</v>
@@ -7693,41 +7693,41 @@
     </row>
     <row r="33" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
-        <v>594</v>
+        <v>588</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>595</v>
+        <v>589</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="9" t="s">
         <v>130</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>715</v>
+        <v>708</v>
       </c>
       <c r="F33" s="5" t="s">
+        <v>590</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>591</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>592</v>
+      </c>
+      <c r="I33" s="9" t="s">
+        <v>627</v>
+      </c>
+      <c r="J33" s="5" t="s">
+        <v>593</v>
+      </c>
+      <c r="K33" s="5" t="s">
+        <v>594</v>
+      </c>
+      <c r="L33" s="5" t="s">
+        <v>595</v>
+      </c>
+      <c r="M33" s="5" t="s">
         <v>596</v>
-      </c>
-      <c r="G33" s="5" t="s">
-        <v>597</v>
-      </c>
-      <c r="H33" s="5" t="s">
-        <v>598</v>
-      </c>
-      <c r="I33" s="9" t="s">
-        <v>633</v>
-      </c>
-      <c r="J33" s="5" t="s">
-        <v>599</v>
-      </c>
-      <c r="K33" s="5" t="s">
-        <v>600</v>
-      </c>
-      <c r="L33" s="5" t="s">
-        <v>601</v>
-      </c>
-      <c r="M33" s="5" t="s">
-        <v>602</v>
       </c>
       <c r="N33" s="5" t="s">
         <v>12</v>
@@ -7738,41 +7738,41 @@
     </row>
     <row r="34" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
-        <v>603</v>
+        <v>597</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>604</v>
+        <v>598</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="9" t="s">
         <v>130</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>716</v>
+        <v>709</v>
       </c>
       <c r="F34" s="5" t="s">
+        <v>599</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>600</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>601</v>
+      </c>
+      <c r="I34" s="9" t="s">
+        <v>626</v>
+      </c>
+      <c r="J34" s="5" t="s">
+        <v>602</v>
+      </c>
+      <c r="K34" s="5" t="s">
+        <v>603</v>
+      </c>
+      <c r="L34" s="5" t="s">
+        <v>604</v>
+      </c>
+      <c r="M34" s="5" t="s">
         <v>605</v>
-      </c>
-      <c r="G34" s="5" t="s">
-        <v>606</v>
-      </c>
-      <c r="H34" s="5" t="s">
-        <v>607</v>
-      </c>
-      <c r="I34" s="9" t="s">
-        <v>632</v>
-      </c>
-      <c r="J34" s="5" t="s">
-        <v>608</v>
-      </c>
-      <c r="K34" s="5" t="s">
-        <v>609</v>
-      </c>
-      <c r="L34" s="5" t="s">
-        <v>610</v>
-      </c>
-      <c r="M34" s="5" t="s">
-        <v>611</v>
       </c>
       <c r="N34" s="5" t="s">
         <v>12</v>
@@ -7783,41 +7783,41 @@
     </row>
     <row r="35" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
-        <v>612</v>
+        <v>606</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="C35" s="5"/>
       <c r="D35" s="9" t="s">
         <v>130</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>717</v>
+        <v>710</v>
       </c>
       <c r="F35" s="5" t="s">
+        <v>608</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>609</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>610</v>
+      </c>
+      <c r="I35" s="9" t="s">
+        <v>625</v>
+      </c>
+      <c r="J35" s="5" t="s">
+        <v>611</v>
+      </c>
+      <c r="K35" s="5" t="s">
+        <v>612</v>
+      </c>
+      <c r="L35" s="5" t="s">
+        <v>613</v>
+      </c>
+      <c r="M35" s="5" t="s">
         <v>614</v>
-      </c>
-      <c r="G35" s="5" t="s">
-        <v>615</v>
-      </c>
-      <c r="H35" s="5" t="s">
-        <v>616</v>
-      </c>
-      <c r="I35" s="9" t="s">
-        <v>631</v>
-      </c>
-      <c r="J35" s="5" t="s">
-        <v>617</v>
-      </c>
-      <c r="K35" s="5" t="s">
-        <v>618</v>
-      </c>
-      <c r="L35" s="5" t="s">
-        <v>619</v>
-      </c>
-      <c r="M35" s="5" t="s">
-        <v>620</v>
       </c>
       <c r="N35" s="5" t="s">
         <v>12</v>
@@ -7828,41 +7828,41 @@
     </row>
     <row r="36" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
-        <v>621</v>
+        <v>615</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>622</v>
+        <v>616</v>
       </c>
       <c r="C36" s="5"/>
       <c r="D36" s="9" t="s">
         <v>130</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>718</v>
+        <v>711</v>
       </c>
       <c r="F36" s="5" t="s">
+        <v>617</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>618</v>
+      </c>
+      <c r="H36" s="5" t="s">
+        <v>619</v>
+      </c>
+      <c r="I36" s="9" t="s">
+        <v>624</v>
+      </c>
+      <c r="J36" s="5" t="s">
+        <v>620</v>
+      </c>
+      <c r="K36" s="5" t="s">
+        <v>621</v>
+      </c>
+      <c r="L36" s="5" t="s">
+        <v>622</v>
+      </c>
+      <c r="M36" s="5" t="s">
         <v>623</v>
-      </c>
-      <c r="G36" s="5" t="s">
-        <v>624</v>
-      </c>
-      <c r="H36" s="5" t="s">
-        <v>625</v>
-      </c>
-      <c r="I36" s="9" t="s">
-        <v>630</v>
-      </c>
-      <c r="J36" s="5" t="s">
-        <v>626</v>
-      </c>
-      <c r="K36" s="5" t="s">
-        <v>627</v>
-      </c>
-      <c r="L36" s="5" t="s">
-        <v>628</v>
-      </c>
-      <c r="M36" s="5" t="s">
-        <v>629</v>
       </c>
       <c r="N36" s="5" t="s">
         <v>12</v>
@@ -7899,14 +7899,14 @@
   <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="12.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="67.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="63.5546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="94" style="1" customWidth="1"/>
     <col min="5" max="5" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="33.33203125" style="1" bestFit="1" customWidth="1"/>
@@ -7968,10 +7968,10 @@
         <v>139</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>1079</v>
+        <v>1053</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>1080</v>
+        <v>1054</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>142</v>
@@ -7983,7 +7983,7 @@
         <v>144</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>1079</v>
+        <v>1053</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>165</v>
@@ -8006,37 +8006,37 @@
         <v>479</v>
       </c>
       <c r="C3" s="9" t="s">
+        <v>1110</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>799</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>808</v>
-      </c>
-      <c r="E3" s="5" t="s">
+      <c r="F3" s="5" t="s">
         <v>481</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="G3" s="5" t="s">
         <v>482</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="H3" s="5" t="s">
+        <v>787</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>1110</v>
+      </c>
+      <c r="J3" s="5" t="s">
         <v>483</v>
       </c>
-      <c r="H3" s="5" t="s">
-        <v>795</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>480</v>
-      </c>
-      <c r="J3" s="5" t="s">
+      <c r="K3" s="5" t="s">
         <v>484</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="L3" s="5" t="s">
         <v>485</v>
       </c>
-      <c r="L3" s="5" t="s">
-        <v>486</v>
-      </c>
       <c r="M3" s="5" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8044,40 +8044,40 @@
         <v>36</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>849</v>
+        <v>836</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>850</v>
+        <v>1111</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>858</v>
+        <v>844</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>851</v>
+        <v>837</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>852</v>
+        <v>838</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>853</v>
+        <v>839</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>854</v>
+        <v>840</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>850</v>
+        <v>1111</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>855</v>
+        <v>841</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>856</v>
+        <v>842</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>857</v>
+        <v>843</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>857</v>
+        <v>843</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8085,40 +8085,40 @@
         <v>43</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>859</v>
+        <v>845</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>860</v>
+        <v>1112</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>868</v>
+        <v>853</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>861</v>
+        <v>846</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>862</v>
+        <v>847</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>863</v>
+        <v>848</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>864</v>
+        <v>849</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>860</v>
+        <v>1112</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>865</v>
+        <v>850</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>866</v>
+        <v>851</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>867</v>
+        <v>852</v>
       </c>
       <c r="M5" s="5" t="s">
-        <v>867</v>
+        <v>852</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8126,40 +8126,40 @@
         <v>64</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>1113</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>789</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>790</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>791</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>792</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>793</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>1113</v>
+      </c>
+      <c r="J6" s="5" t="s">
         <v>796</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="K6" s="5" t="s">
         <v>797</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="L6" s="5" t="s">
         <v>798</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>799</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>800</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>801</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>802</v>
-      </c>
-      <c r="I6" s="9" t="s">
-        <v>797</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>805</v>
-      </c>
-      <c r="K6" s="5" t="s">
-        <v>806</v>
-      </c>
-      <c r="L6" s="5" t="s">
-        <v>807</v>
-      </c>
       <c r="M6" s="5" t="s">
-        <v>807</v>
+        <v>798</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8167,40 +8167,40 @@
         <v>96</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>781</v>
+        <v>773</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>1081</v>
+        <v>1055</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>1082</v>
+        <v>1056</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>782</v>
+        <v>774</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>783</v>
+        <v>775</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>803</v>
+        <v>794</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>1081</v>
+        <v>1055</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>785</v>
+        <v>777</v>
       </c>
       <c r="K7" s="5" t="s">
+        <v>778</v>
+      </c>
+      <c r="L7" s="5" t="s">
         <v>786</v>
       </c>
-      <c r="L7" s="5" t="s">
-        <v>794</v>
-      </c>
       <c r="M7" s="5" t="s">
-        <v>794</v>
+        <v>786</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8208,40 +8208,40 @@
         <v>103</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>787</v>
+        <v>779</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>1126</v>
+        <v>1100</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>1127</v>
+        <v>1101</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>788</v>
+        <v>780</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>789</v>
+        <v>781</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>790</v>
+        <v>782</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>804</v>
+        <v>795</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>1126</v>
+        <v>1100</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>791</v>
+        <v>783</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>792</v>
+        <v>784</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>793</v>
+        <v>785</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8249,40 +8249,40 @@
         <v>111</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>809</v>
+        <v>800</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>810</v>
+        <v>1114</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>811</v>
+        <v>801</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>812</v>
+        <v>802</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>813</v>
+        <v>803</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>814</v>
+        <v>804</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>815</v>
+        <v>805</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>810</v>
+        <v>1114</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>816</v>
+        <v>806</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>817</v>
+        <v>807</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>818</v>
+        <v>808</v>
       </c>
       <c r="M9" s="5" t="s">
-        <v>818</v>
+        <v>808</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8290,40 +8290,40 @@
         <v>113</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>486</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>1096</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>1097</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>487</v>
       </c>
-      <c r="C10" s="9" t="s">
-        <v>1122</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>1123</v>
-      </c>
-      <c r="E10" s="5" t="s">
+      <c r="F10" s="5" t="s">
         <v>488</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="G10" s="5" t="s">
         <v>489</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="H10" s="5" t="s">
+        <v>809</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>1096</v>
+      </c>
+      <c r="J10" s="5" t="s">
         <v>490</v>
       </c>
-      <c r="H10" s="5" t="s">
-        <v>819</v>
-      </c>
-      <c r="I10" s="9" t="s">
-        <v>1122</v>
-      </c>
-      <c r="J10" s="5" t="s">
+      <c r="K10" s="5" t="s">
         <v>491</v>
       </c>
-      <c r="K10" s="5" t="s">
+      <c r="L10" s="5" t="s">
         <v>492</v>
       </c>
-      <c r="L10" s="5" t="s">
-        <v>493</v>
-      </c>
       <c r="M10" s="5" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8331,40 +8331,40 @@
         <v>115</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>990</v>
+        <v>970</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>991</v>
+        <v>1115</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>992</v>
+        <v>971</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>993</v>
+        <v>972</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>994</v>
+        <v>973</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>995</v>
+        <v>974</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>996</v>
+        <v>975</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>991</v>
+        <v>1115</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>997</v>
+        <v>976</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>998</v>
+        <v>977</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>999</v>
+        <v>978</v>
       </c>
       <c r="M11" s="5" t="s">
-        <v>999</v>
+        <v>978</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8372,40 +8372,40 @@
         <v>117</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>1000</v>
+        <v>979</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>1001</v>
+        <v>1116</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>1002</v>
+        <v>980</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>1003</v>
+        <v>981</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>1004</v>
+        <v>982</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>1005</v>
+        <v>983</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>1006</v>
+        <v>984</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>1001</v>
+        <v>1116</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>1007</v>
+        <v>985</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>1008</v>
+        <v>986</v>
       </c>
       <c r="L12" s="5" t="s">
-        <v>1009</v>
+        <v>987</v>
       </c>
       <c r="M12" s="5" t="s">
-        <v>1009</v>
+        <v>987</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8413,40 +8413,40 @@
         <v>119</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>879</v>
+        <v>863</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>880</v>
+        <v>1117</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>881</v>
+        <v>864</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>882</v>
+        <v>865</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>883</v>
+        <v>866</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>884</v>
+        <v>867</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>885</v>
+        <v>868</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>880</v>
+        <v>1117</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>886</v>
+        <v>869</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>887</v>
+        <v>870</v>
       </c>
       <c r="L13" s="5" t="s">
-        <v>888</v>
+        <v>871</v>
       </c>
       <c r="M13" s="5" t="s">
-        <v>888</v>
+        <v>871</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8454,116 +8454,116 @@
         <v>145</v>
       </c>
       <c r="B14" s="5" t="s">
+        <v>493</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>1098</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>1099</v>
+      </c>
+      <c r="E14" s="5" t="s">
         <v>494</v>
       </c>
-      <c r="C14" s="9" t="s">
-        <v>1124</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>1125</v>
-      </c>
-      <c r="E14" s="5" t="s">
+      <c r="F14" s="5" t="s">
         <v>495</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="G14" s="5" t="s">
         <v>496</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>497</v>
       </c>
       <c r="H14" s="5"/>
       <c r="I14" s="9" t="s">
-        <v>1124</v>
+        <v>1098</v>
       </c>
       <c r="J14" s="5" t="s">
+        <v>497</v>
+      </c>
+      <c r="K14" s="5" t="s">
         <v>498</v>
       </c>
-      <c r="K14" s="5" t="s">
+      <c r="L14" s="5" t="s">
         <v>499</v>
       </c>
-      <c r="L14" s="5" t="s">
-        <v>500</v>
-      </c>
       <c r="M14" s="5" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
+        <v>500</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>501</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="C15" s="9" t="s">
+        <v>1102</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>1103</v>
+      </c>
+      <c r="E15" s="5" t="s">
         <v>502</v>
       </c>
-      <c r="C15" s="9" t="s">
-        <v>1128</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>1129</v>
-      </c>
-      <c r="E15" s="5" t="s">
+      <c r="F15" s="5" t="s">
         <v>503</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="G15" s="5" t="s">
         <v>504</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>505</v>
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="9" t="s">
-        <v>1128</v>
+        <v>1102</v>
       </c>
       <c r="J15" s="5" t="s">
+        <v>505</v>
+      </c>
+      <c r="K15" s="5" t="s">
         <v>506</v>
       </c>
-      <c r="K15" s="5" t="s">
+      <c r="L15" s="5" t="s">
         <v>507</v>
       </c>
-      <c r="L15" s="5" t="s">
-        <v>508</v>
-      </c>
       <c r="M15" s="5" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
+        <v>508</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>509</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="C16" s="9" t="s">
+        <v>1102</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>1104</v>
+      </c>
+      <c r="E16" s="5" t="s">
         <v>510</v>
       </c>
-      <c r="C16" s="9" t="s">
-        <v>1128</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>1130</v>
-      </c>
-      <c r="E16" s="5" t="s">
+      <c r="F16" s="5" t="s">
         <v>511</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="G16" s="5" t="s">
         <v>512</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>513</v>
       </c>
       <c r="H16" s="5"/>
       <c r="I16" s="9" t="s">
-        <v>1128</v>
+        <v>1102</v>
       </c>
       <c r="J16" s="5" t="s">
+        <v>513</v>
+      </c>
+      <c r="K16" s="5" t="s">
         <v>514</v>
       </c>
-      <c r="K16" s="5" t="s">
+      <c r="L16" s="5" t="s">
         <v>515</v>
       </c>
-      <c r="L16" s="5" t="s">
-        <v>516</v>
-      </c>
       <c r="M16" s="5" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8571,40 +8571,40 @@
         <v>17</v>
       </c>
       <c r="B17" s="5" t="s">
+        <v>516</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>1105</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>1106</v>
+      </c>
+      <c r="E17" s="5" t="s">
         <v>517</v>
       </c>
-      <c r="C17" s="9" t="s">
-        <v>1131</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>1132</v>
-      </c>
-      <c r="E17" s="5" t="s">
+      <c r="F17" s="5" t="s">
         <v>518</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="G17" s="5" t="s">
         <v>519</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="H17" s="5" t="s">
         <v>520</v>
       </c>
-      <c r="H17" s="5" t="s">
+      <c r="I17" s="9" t="s">
+        <v>1105</v>
+      </c>
+      <c r="J17" s="5" t="s">
         <v>521</v>
       </c>
-      <c r="I17" s="9" t="s">
-        <v>1131</v>
-      </c>
-      <c r="J17" s="5" t="s">
+      <c r="K17" s="5" t="s">
         <v>522</v>
       </c>
-      <c r="K17" s="5" t="s">
+      <c r="L17" s="5" t="s">
         <v>523</v>
       </c>
-      <c r="L17" s="5" t="s">
-        <v>524</v>
-      </c>
       <c r="M17" s="5" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8612,38 +8612,38 @@
         <v>18</v>
       </c>
       <c r="B18" s="5" t="s">
+        <v>524</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>1107</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>1131</v>
+      </c>
+      <c r="E18" s="5" t="s">
         <v>525</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="F18" s="5" t="s">
         <v>526</v>
       </c>
-      <c r="D18" s="6" t="s">
-        <v>776</v>
-      </c>
-      <c r="E18" s="5" t="s">
+      <c r="G18" s="5" t="s">
         <v>527</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>528</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>529</v>
       </c>
       <c r="H18" s="5"/>
       <c r="I18" s="9" t="s">
-        <v>526</v>
+        <v>1107</v>
       </c>
       <c r="J18" s="5" t="s">
+        <v>528</v>
+      </c>
+      <c r="K18" s="5" t="s">
+        <v>529</v>
+      </c>
+      <c r="L18" s="5" t="s">
         <v>530</v>
       </c>
-      <c r="K18" s="5" t="s">
-        <v>531</v>
-      </c>
-      <c r="L18" s="5" t="s">
-        <v>532</v>
-      </c>
       <c r="M18" s="5" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8651,38 +8651,38 @@
         <v>19</v>
       </c>
       <c r="B19" s="5" t="s">
+        <v>531</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>1108</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>769</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>532</v>
+      </c>
+      <c r="F19" s="5" t="s">
         <v>533</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="G19" s="5" t="s">
         <v>534</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>777</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>535</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>536</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>537</v>
       </c>
       <c r="H19" s="5"/>
       <c r="I19" s="9" t="s">
-        <v>534</v>
+        <v>1108</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="L19" s="5" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="M19" s="5" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8690,38 +8690,38 @@
         <v>209</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>682</v>
+        <v>676</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>683</v>
+        <v>1109</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>778</v>
+        <v>770</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>684</v>
+        <v>677</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>685</v>
+        <v>678</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>686</v>
+        <v>679</v>
       </c>
       <c r="H20" s="5"/>
       <c r="I20" s="9" t="s">
-        <v>683</v>
+        <v>1109</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>687</v>
+        <v>680</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>688</v>
+        <v>681</v>
       </c>
       <c r="L20" s="5" t="s">
-        <v>689</v>
+        <v>682</v>
       </c>
       <c r="M20" s="5" t="s">
-        <v>689</v>
+        <v>682</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8729,38 +8729,38 @@
         <v>229</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>577</v>
+        <v>572</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>578</v>
+        <v>1118</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>778</v>
+        <v>770</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>579</v>
+        <v>573</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>580</v>
+        <v>574</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>581</v>
+        <v>575</v>
       </c>
       <c r="H21" s="5"/>
       <c r="I21" s="9" t="s">
+        <v>1118</v>
+      </c>
+      <c r="J21" s="5" t="s">
+        <v>576</v>
+      </c>
+      <c r="K21" s="5" t="s">
+        <v>577</v>
+      </c>
+      <c r="L21" s="5" t="s">
         <v>578</v>
       </c>
-      <c r="J21" s="5" t="s">
-        <v>582</v>
-      </c>
-      <c r="K21" s="5" t="s">
-        <v>583</v>
-      </c>
-      <c r="L21" s="5" t="s">
-        <v>584</v>
-      </c>
       <c r="M21" s="5" t="s">
-        <v>584</v>
+        <v>578</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8768,40 +8768,40 @@
         <v>418</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>1030</v>
+        <v>1006</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>1031</v>
+        <v>1119</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>1069</v>
+        <v>1132</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>1032</v>
+        <v>1007</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>1033</v>
+        <v>1008</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>1034</v>
+        <v>1009</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>1035</v>
+        <v>1010</v>
       </c>
       <c r="I22" s="9" t="s">
-        <v>1031</v>
+        <v>1119</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>1036</v>
+        <v>1011</v>
       </c>
       <c r="K22" s="5" t="s">
-        <v>1037</v>
+        <v>1012</v>
       </c>
       <c r="L22" s="5" t="s">
-        <v>1038</v>
+        <v>1013</v>
       </c>
       <c r="M22" s="5" t="s">
-        <v>1038</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8809,40 +8809,40 @@
         <v>427</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>820</v>
+        <v>810</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>821</v>
+        <v>1120</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>1070</v>
+        <v>1044</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>822</v>
+        <v>811</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>823</v>
+        <v>812</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>824</v>
+        <v>813</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>825</v>
+        <v>814</v>
       </c>
       <c r="I23" s="9" t="s">
-        <v>821</v>
+        <v>1120</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>826</v>
+        <v>815</v>
       </c>
       <c r="K23" s="5" t="s">
-        <v>827</v>
+        <v>816</v>
       </c>
       <c r="L23" s="5" t="s">
-        <v>828</v>
+        <v>817</v>
       </c>
       <c r="M23" s="5" t="s">
-        <v>828</v>
+        <v>817</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8850,40 +8850,40 @@
         <v>437</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>829</v>
+        <v>818</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>831</v>
+        <v>1121</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>832</v>
+        <v>820</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>833</v>
+        <v>821</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>834</v>
+        <v>822</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>835</v>
+        <v>823</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>836</v>
+        <v>824</v>
       </c>
       <c r="I24" s="9" t="s">
-        <v>831</v>
+        <v>1121</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>837</v>
+        <v>825</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>838</v>
+        <v>826</v>
       </c>
       <c r="L24" s="5" t="s">
-        <v>839</v>
+        <v>827</v>
       </c>
       <c r="M24" s="5" t="s">
-        <v>839</v>
+        <v>827</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8891,40 +8891,40 @@
         <v>447</v>
       </c>
       <c r="B25" s="5" t="s">
+        <v>819</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>1122</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>828</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>829</v>
+      </c>
+      <c r="F25" s="5" t="s">
         <v>830</v>
       </c>
-      <c r="C25" s="9" t="s">
-        <v>840</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>841</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>842</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>843</v>
-      </c>
       <c r="G25" s="5" t="s">
-        <v>844</v>
+        <v>831</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>845</v>
+        <v>832</v>
       </c>
       <c r="I25" s="9" t="s">
-        <v>840</v>
+        <v>1122</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>846</v>
+        <v>833</v>
       </c>
       <c r="K25" s="5" t="s">
-        <v>847</v>
+        <v>834</v>
       </c>
       <c r="L25" s="5" t="s">
-        <v>848</v>
+        <v>835</v>
       </c>
       <c r="M25" s="5" t="s">
-        <v>848</v>
+        <v>835</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8932,40 +8932,40 @@
         <v>457</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>947</v>
+        <v>930</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>948</v>
+        <v>1123</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>949</v>
+        <v>931</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>950</v>
+        <v>932</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>951</v>
+        <v>933</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>952</v>
+        <v>934</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>953</v>
+        <v>935</v>
       </c>
       <c r="I26" s="9" t="s">
-        <v>948</v>
+        <v>1123</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>954</v>
+        <v>936</v>
       </c>
       <c r="K26" s="5" t="s">
-        <v>955</v>
+        <v>937</v>
       </c>
       <c r="L26" s="5" t="s">
-        <v>956</v>
+        <v>938</v>
       </c>
       <c r="M26" s="5" t="s">
-        <v>956</v>
+        <v>938</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8973,304 +8973,290 @@
         <v>467</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>957</v>
+        <v>939</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>958</v>
+        <v>1124</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>959</v>
+        <v>940</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>960</v>
+        <v>941</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>961</v>
+        <v>942</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>962</v>
+        <v>943</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>963</v>
+        <v>944</v>
       </c>
       <c r="I27" s="9" t="s">
-        <v>958</v>
+        <v>1124</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>964</v>
+        <v>945</v>
       </c>
       <c r="K27" s="5" t="s">
-        <v>965</v>
+        <v>946</v>
       </c>
       <c r="L27" s="5" t="s">
-        <v>966</v>
+        <v>947</v>
       </c>
       <c r="M27" s="5" t="s">
-        <v>966</v>
+        <v>947</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
-        <v>585</v>
+        <v>579</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>967</v>
+        <v>948</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>968</v>
+        <v>1125</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>969</v>
+        <v>949</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>970</v>
+        <v>950</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>971</v>
+        <v>951</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>972</v>
+        <v>952</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>973</v>
+        <v>953</v>
       </c>
       <c r="I28" s="9" t="s">
-        <v>968</v>
+        <v>1125</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>974</v>
+        <v>954</v>
       </c>
       <c r="K28" s="5" t="s">
-        <v>975</v>
+        <v>955</v>
       </c>
       <c r="L28" s="5" t="s">
-        <v>976</v>
+        <v>956</v>
       </c>
       <c r="M28" s="5" t="s">
-        <v>976</v>
+        <v>956</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
-        <v>594</v>
+        <v>588</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>1010</v>
+        <v>988</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>1011</v>
+        <v>1126</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>1012</v>
+        <v>989</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>1013</v>
+        <v>990</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>1014</v>
+        <v>991</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>1015</v>
+        <v>992</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>1016</v>
+        <v>993</v>
       </c>
       <c r="I29" s="9" t="s">
-        <v>1011</v>
+        <v>1126</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>1017</v>
+        <v>994</v>
       </c>
       <c r="K29" s="5" t="s">
-        <v>1018</v>
+        <v>995</v>
       </c>
       <c r="L29" s="5" t="s">
-        <v>1019</v>
+        <v>996</v>
       </c>
       <c r="M29" s="5" t="s">
-        <v>1019</v>
+        <v>996</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
-        <v>603</v>
+        <v>597</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>1020</v>
+        <v>997</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>1021</v>
+        <v>1127</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>1022</v>
+        <v>998</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>1023</v>
+        <v>999</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>1024</v>
+        <v>1000</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>1025</v>
+        <v>1001</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>1026</v>
+        <v>1002</v>
       </c>
       <c r="I30" s="9" t="s">
-        <v>1021</v>
+        <v>1127</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>1027</v>
+        <v>1003</v>
       </c>
       <c r="K30" s="5" t="s">
-        <v>1028</v>
+        <v>1004</v>
       </c>
       <c r="L30" s="5" t="s">
-        <v>1029</v>
+        <v>1005</v>
       </c>
       <c r="M30" s="5" t="s">
-        <v>1029</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
-        <v>621</v>
+        <v>615</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>869</v>
+        <v>854</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>870</v>
+        <v>1128</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>878</v>
+        <v>862</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>871</v>
+        <v>855</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>872</v>
+        <v>856</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>873</v>
+        <v>857</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>874</v>
+        <v>858</v>
       </c>
       <c r="I31" s="9" t="s">
-        <v>870</v>
+        <v>1128</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>875</v>
+        <v>859</v>
       </c>
       <c r="K31" s="5" t="s">
-        <v>876</v>
+        <v>860</v>
       </c>
       <c r="L31" s="5" t="s">
-        <v>877</v>
+        <v>861</v>
       </c>
       <c r="M31" s="5" t="s">
-        <v>877</v>
+        <v>861</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
+        <v>538</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>539</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>1129</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>771</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>540</v>
+      </c>
+      <c r="F32" s="5" t="s">
         <v>541</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="G32" s="5" t="s">
         <v>542</v>
-      </c>
-      <c r="C32" s="9" t="s">
-        <v>543</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>779</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>544</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>545</v>
-      </c>
-      <c r="G32" s="5" t="s">
-        <v>546</v>
       </c>
       <c r="H32" s="5"/>
       <c r="I32" s="9" t="s">
+        <v>1129</v>
+      </c>
+      <c r="J32" s="5" t="s">
         <v>543</v>
       </c>
-      <c r="J32" s="5" t="s">
-        <v>547</v>
-      </c>
       <c r="K32" s="5" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="L32" s="5" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="M32" s="5" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
+        <v>546</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>547</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>1130</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>772</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>548</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>549</v>
+      </c>
+      <c r="G33" s="5" t="s">
         <v>550</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>551</v>
-      </c>
-      <c r="C33" s="9" t="s">
-        <v>552</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>780</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>553</v>
-      </c>
-      <c r="F33" s="5" t="s">
-        <v>554</v>
-      </c>
-      <c r="G33" s="5" t="s">
-        <v>555</v>
       </c>
       <c r="H33" s="5"/>
       <c r="I33" s="9" t="s">
+        <v>1130</v>
+      </c>
+      <c r="J33" s="5" t="s">
+        <v>551</v>
+      </c>
+      <c r="K33" s="5" t="s">
         <v>552</v>
       </c>
-      <c r="J33" s="5" t="s">
-        <v>556</v>
-      </c>
-      <c r="K33" s="5" t="s">
-        <v>557</v>
-      </c>
       <c r="L33" s="5" t="s">
-        <v>558</v>
+        <v>553</v>
       </c>
       <c r="M33" s="5" t="s">
-        <v>558</v>
+        <v>553</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C26" r:id="rId1" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{47554786-550A-41E9-AF83-B6969AD357DC}"/>
-    <hyperlink ref="I26" r:id="rId2" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{E1BBE2F9-8E32-4E4D-AEFE-43FA02765A58}"/>
-    <hyperlink ref="C27" r:id="rId3" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{993DD2A2-B832-44A7-AA80-CCC5C19C765A}"/>
-    <hyperlink ref="I27" r:id="rId4" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{AD4E0AC8-D9A9-4391-B80D-4FDD236094A9}"/>
-    <hyperlink ref="C30" r:id="rId5" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{889F9053-9FF6-4D5A-B636-90737961BD78}"/>
-    <hyperlink ref="I30" r:id="rId6" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{52F1A0B0-B3EF-4196-9723-AF1D81794325}"/>
-    <hyperlink ref="C28" r:id="rId7" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{9E97B247-4F12-47FB-B824-A9C8EE015367}"/>
-    <hyperlink ref="I28" r:id="rId8" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{1EDA50B5-1DDE-4ABB-9353-B3AF32C0D269}"/>
-    <hyperlink ref="C29" r:id="rId9" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{5BC5C9C8-3CD1-4A40-8170-1D0AC81580C7}"/>
-    <hyperlink ref="I29" r:id="rId10" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{42A3303C-BA7A-49DE-8323-C772CFCF1F43}"/>
-    <hyperlink ref="C11" r:id="rId11" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{96AC723F-D956-4FC1-9FA1-B481C6608FA1}"/>
-    <hyperlink ref="I11" r:id="rId12" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{7CECBDA1-EDB5-4EA3-8CAB-FF77BAF10FF0}"/>
-    <hyperlink ref="C12" r:id="rId13" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{2DF60C4B-F0D0-4E92-BC3C-029858EE6E91}"/>
-    <hyperlink ref="I12" r:id="rId14" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{F3BDE6DD-1CE6-44F7-85A8-71859FDB93DA}"/>
-    <hyperlink ref="C22" r:id="rId15" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{5CE45785-443D-4B93-94C8-46519383162E}"/>
-    <hyperlink ref="I22" r:id="rId16" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{C768F8CA-C09C-46D8-8EFF-8D6D4DFE5A02}"/>
-    <hyperlink ref="C2" r:id="rId17" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{06F53D74-C7A6-4A0D-8D9C-4D7B09C907DB}"/>
-    <hyperlink ref="I2" r:id="rId18" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{CB2C38DA-1BB9-46E6-B59C-F655A3FBE838}"/>
+    <hyperlink ref="C2" r:id="rId1" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{06F53D74-C7A6-4A0D-8D9C-4D7B09C907DB}"/>
+    <hyperlink ref="C3:C6" r:id="rId2" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{37CAF0AB-C08F-4CE8-87FD-1B69D2C45BE7}"/>
+    <hyperlink ref="I2" r:id="rId3" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{94B27E7B-FF67-4DD9-A3F0-603C0ED793EF}"/>
+    <hyperlink ref="I3:I6" r:id="rId4" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{3CEFB26C-2E1E-4FFB-8E5B-1F7DF3CE0F44}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.3" right="0.3" top="0.61" bottom="0.37" header="0.1" footer="0.1"/>

</xml_diff>

<commit_message>
GDE-7311 Data set and files for TL_CAL_19
</commit_message>
<xml_diff>
--- a/DataSet/Integration_DataSet/TL/TL_Data_Set_AU.xlsx
+++ b/DataSet/Integration_DataSet/TL/TL_Data_Set_AU.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\Integration_DataSet\TL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0F2A5CB-3FD4-4B4F-83E5-FAF943C54997}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15D185F2-EFB5-4B16-ADBD-A484A32E1E43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BaseRate_Fields" sheetId="1" r:id="rId1"/>
@@ -2330,9 +2330,6 @@
   </si>
   <si>
     <t>Actual_ResponseMechanism_TL_BASE_42</t>
-  </si>
-  <si>
-    <t>Holidays_Banks_20190119_1.csv,Holidays_Banks_20190119_1.xlsx,Holidays_Banks_20190119_2.csv,Holidays_Banks_20190119_2.xlsx,Holidays_Misc_20190119.xlsx</t>
   </si>
   <si>
     <t>Holidays_Banks_20190121_1.csv,Holidays_Banks_20190121_1.xlsx,Holidays_Banks_20190121_2.csv,Holidays_Banks_20190121_2.xlsx,Holidays_Misc_20190121.xlsx</t>
@@ -3479,6 +3476,9 @@
   </si>
   <si>
     <t>Holidays_Banks_20190125_2.xls,Holidays_Banks_20200125_1.csv,Holidays_Banks_20200125_2.csv,Holidays_Misc_20190125.xls</t>
+  </si>
+  <si>
+    <t>Holidays_Banks_20200119_1.csv,Holidays_Banks_20200119_1.xlsx,Holidays_Banks_20200119_2.csv,Holidays_Banks_20200119_2.xlsx,Holidays_Misc_20200119.xlsx</t>
   </si>
 </sst>
 </file>
@@ -4461,7 +4461,7 @@
         <v>17</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>1</v>
@@ -4505,10 +4505,10 @@
         <v>11</v>
       </c>
       <c r="C2" s="9" t="s">
+        <v>1048</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>1049</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>1050</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>94</v>
@@ -4523,7 +4523,7 @@
         <v>18</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>21</v>
@@ -4546,10 +4546,10 @@
         <v>23</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>95</v>
@@ -4564,7 +4564,7 @@
         <v>25</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="J3" s="5" t="s">
         <v>26</v>
@@ -4587,10 +4587,10 @@
         <v>30</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>140</v>
@@ -4605,7 +4605,7 @@
         <v>33</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="J4" s="5" t="s">
         <v>34</v>
@@ -4628,10 +4628,10 @@
         <v>37</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>153</v>
@@ -4646,7 +4646,7 @@
         <v>40</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="J5" s="5" t="s">
         <v>41</v>
@@ -4669,10 +4669,10 @@
         <v>50</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>51</v>
@@ -4687,7 +4687,7 @@
         <v>54</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="J6" s="5" t="s">
         <v>55</v>
@@ -4710,13 +4710,13 @@
         <v>58</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>59</v>
@@ -4728,7 +4728,7 @@
         <v>61</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="J7" s="5" t="s">
         <v>62</v>
@@ -4751,13 +4751,13 @@
         <v>65</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>66</v>
@@ -4769,7 +4769,7 @@
         <v>68</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="J8" s="5" t="s">
         <v>69</v>
@@ -4792,13 +4792,13 @@
         <v>97</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>98</v>
@@ -4810,7 +4810,7 @@
         <v>100</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="J9" s="5" t="s">
         <v>101</v>
@@ -4833,10 +4833,10 @@
         <v>104</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>105</v>
@@ -4851,7 +4851,7 @@
         <v>108</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="J10" s="5" t="s">
         <v>109</v>
@@ -4874,10 +4874,10 @@
         <v>156</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>112</v>
@@ -4892,7 +4892,7 @@
         <v>159</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="J11" s="5" t="s">
         <v>160</v>
@@ -4915,10 +4915,10 @@
         <v>169</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>114</v>
@@ -4933,7 +4933,7 @@
         <v>191</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="J12" s="5" t="s">
         <v>196</v>
@@ -4956,10 +4956,10 @@
         <v>170</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>116</v>
@@ -4974,7 +4974,7 @@
         <v>192</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="J13" s="5" t="s">
         <v>197</v>
@@ -4997,10 +4997,10 @@
         <v>171</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>118</v>
@@ -5015,7 +5015,7 @@
         <v>193</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="J14" s="5" t="s">
         <v>198</v>
@@ -5038,10 +5038,10 @@
         <v>172</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>120</v>
@@ -5056,7 +5056,7 @@
         <v>194</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="J15" s="5" t="s">
         <v>199</v>
@@ -5079,10 +5079,10 @@
         <v>173</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>152</v>
@@ -5097,7 +5097,7 @@
         <v>148</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="J16" s="5" t="s">
         <v>149</v>
@@ -5117,40 +5117,40 @@
         <v>332</v>
       </c>
       <c r="B17" s="5" t="s">
+        <v>874</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>1048</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>1073</v>
+      </c>
+      <c r="E17" s="5" t="s">
         <v>875</v>
       </c>
-      <c r="C17" s="9" t="s">
-        <v>1049</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>1074</v>
-      </c>
-      <c r="E17" s="5" t="s">
+      <c r="F17" s="5" t="s">
         <v>876</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="G17" s="5" t="s">
         <v>877</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="H17" s="5" t="s">
         <v>878</v>
       </c>
-      <c r="H17" s="5" t="s">
+      <c r="I17" s="9" t="s">
+        <v>1073</v>
+      </c>
+      <c r="J17" s="5" t="s">
         <v>879</v>
       </c>
-      <c r="I17" s="9" t="s">
-        <v>1074</v>
-      </c>
-      <c r="J17" s="5" t="s">
+      <c r="K17" s="5" t="s">
         <v>880</v>
       </c>
-      <c r="K17" s="5" t="s">
+      <c r="L17" s="5" t="s">
         <v>881</v>
       </c>
-      <c r="L17" s="5" t="s">
+      <c r="M17" s="5" t="s">
         <v>882</v>
-      </c>
-      <c r="M17" s="5" t="s">
-        <v>883</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
@@ -5158,40 +5158,40 @@
         <v>342</v>
       </c>
       <c r="B18" s="5" t="s">
+        <v>1013</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>1048</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>1074</v>
+      </c>
+      <c r="E18" s="5" t="s">
         <v>1014</v>
       </c>
-      <c r="C18" s="9" t="s">
-        <v>1049</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>1075</v>
-      </c>
-      <c r="E18" s="5" t="s">
+      <c r="F18" s="5" t="s">
         <v>1015</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="G18" s="5" t="s">
         <v>1016</v>
       </c>
-      <c r="G18" s="5" t="s">
+      <c r="H18" s="5" t="s">
         <v>1017</v>
       </c>
-      <c r="H18" s="5" t="s">
+      <c r="I18" s="9" t="s">
+        <v>1074</v>
+      </c>
+      <c r="J18" s="5" t="s">
         <v>1018</v>
       </c>
-      <c r="I18" s="9" t="s">
-        <v>1075</v>
-      </c>
-      <c r="J18" s="5" t="s">
+      <c r="K18" s="5" t="s">
         <v>1019</v>
       </c>
-      <c r="K18" s="5" t="s">
+      <c r="L18" s="5" t="s">
         <v>1020</v>
       </c>
-      <c r="L18" s="5" t="s">
+      <c r="M18" s="5" t="s">
         <v>1021</v>
-      </c>
-      <c r="M18" s="5" t="s">
-        <v>1022</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
@@ -5199,40 +5199,40 @@
         <v>352</v>
       </c>
       <c r="B19" s="5" t="s">
+        <v>960</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>1048</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>1075</v>
+      </c>
+      <c r="E19" s="5" t="s">
         <v>961</v>
       </c>
-      <c r="C19" s="9" t="s">
-        <v>1049</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>1076</v>
-      </c>
-      <c r="E19" s="5" t="s">
+      <c r="F19" s="5" t="s">
         <v>962</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="G19" s="5" t="s">
         <v>963</v>
       </c>
-      <c r="G19" s="5" t="s">
+      <c r="H19" s="5" t="s">
         <v>964</v>
       </c>
-      <c r="H19" s="5" t="s">
+      <c r="I19" s="9" t="s">
+        <v>1075</v>
+      </c>
+      <c r="J19" s="5" t="s">
         <v>965</v>
       </c>
-      <c r="I19" s="9" t="s">
-        <v>1076</v>
-      </c>
-      <c r="J19" s="5" t="s">
+      <c r="K19" s="5" t="s">
         <v>966</v>
       </c>
-      <c r="K19" s="5" t="s">
+      <c r="L19" s="5" t="s">
         <v>967</v>
       </c>
-      <c r="L19" s="5" t="s">
+      <c r="M19" s="5" t="s">
         <v>968</v>
-      </c>
-      <c r="M19" s="5" t="s">
-        <v>969</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
@@ -5243,10 +5243,10 @@
         <v>174</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>206</v>
@@ -5261,7 +5261,7 @@
         <v>195</v>
       </c>
       <c r="I20" s="9" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="J20" s="5" t="s">
         <v>200</v>
@@ -5284,10 +5284,10 @@
         <v>219</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>210</v>
@@ -5302,7 +5302,7 @@
         <v>214</v>
       </c>
       <c r="I21" s="9" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="J21" s="5" t="s">
         <v>215</v>
@@ -5325,10 +5325,10 @@
         <v>220</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>221</v>
@@ -5343,7 +5343,7 @@
         <v>224</v>
       </c>
       <c r="I22" s="9" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="J22" s="5" t="s">
         <v>225</v>
@@ -5366,10 +5366,10 @@
         <v>230</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>239</v>
@@ -5384,7 +5384,7 @@
         <v>234</v>
       </c>
       <c r="I23" s="9" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="J23" s="5" t="s">
         <v>235</v>
@@ -5407,10 +5407,10 @@
         <v>554</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>555</v>
@@ -5425,7 +5425,7 @@
         <v>558</v>
       </c>
       <c r="I24" s="9" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="J24" s="5" t="s">
         <v>559</v>
@@ -5448,10 +5448,10 @@
         <v>571</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>563</v>
@@ -5466,7 +5466,7 @@
         <v>566</v>
       </c>
       <c r="I25" s="9" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="J25" s="5" t="s">
         <v>567</v>
@@ -5489,10 +5489,10 @@
         <v>683</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>684</v>
@@ -5507,7 +5507,7 @@
         <v>687</v>
       </c>
       <c r="I26" s="9" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="J26" s="5" t="s">
         <v>688</v>
@@ -5527,40 +5527,40 @@
         <v>457</v>
       </c>
       <c r="B27" s="5" t="s">
+        <v>1022</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>1048</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>1057</v>
+      </c>
+      <c r="E27" s="5" t="s">
         <v>1023</v>
       </c>
-      <c r="C27" s="9" t="s">
-        <v>1049</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>1058</v>
-      </c>
-      <c r="E27" s="5" t="s">
+      <c r="F27" s="5" t="s">
         <v>1024</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="G27" s="5" t="s">
         <v>1025</v>
       </c>
-      <c r="G27" s="5" t="s">
+      <c r="H27" s="5" t="s">
         <v>1026</v>
       </c>
-      <c r="H27" s="5" t="s">
+      <c r="I27" s="9" t="s">
+        <v>1057</v>
+      </c>
+      <c r="J27" s="5" t="s">
         <v>1027</v>
       </c>
-      <c r="I27" s="9" t="s">
-        <v>1058</v>
-      </c>
-      <c r="J27" s="5" t="s">
+      <c r="K27" s="5" t="s">
         <v>1028</v>
       </c>
-      <c r="K27" s="5" t="s">
+      <c r="L27" s="5" t="s">
         <v>1029</v>
       </c>
-      <c r="L27" s="5" t="s">
+      <c r="M27" s="5" t="s">
         <v>1030</v>
-      </c>
-      <c r="M27" s="5" t="s">
-        <v>1031</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
@@ -5571,10 +5571,10 @@
         <v>658</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>659</v>
@@ -5589,7 +5589,7 @@
         <v>662</v>
       </c>
       <c r="I28" s="9" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="J28" s="5" t="s">
         <v>663</v>
@@ -5612,10 +5612,10 @@
         <v>667</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="E29" s="6" t="s">
         <v>668</v>
@@ -5630,7 +5630,7 @@
         <v>671</v>
       </c>
       <c r="I29" s="9" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="J29" s="5" t="s">
         <v>672</v>
@@ -5653,10 +5653,10 @@
         <v>700</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="E30" s="6" t="s">
         <v>714</v>
@@ -5671,7 +5671,7 @@
         <v>703</v>
       </c>
       <c r="I30" s="9" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="J30" s="5" t="s">
         <v>704</v>
@@ -5694,10 +5694,10 @@
         <v>700</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>712</v>
@@ -5712,7 +5712,7 @@
         <v>703</v>
       </c>
       <c r="I31" s="9" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="J31" s="5" t="s">
         <v>704</v>
@@ -5732,40 +5732,40 @@
         <v>606</v>
       </c>
       <c r="B32" s="5" t="s">
+        <v>883</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>1048</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>1085</v>
+      </c>
+      <c r="E32" s="6" t="s">
         <v>884</v>
       </c>
-      <c r="C32" s="9" t="s">
-        <v>1049</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>1086</v>
-      </c>
-      <c r="E32" s="6" t="s">
+      <c r="F32" s="5" t="s">
         <v>885</v>
       </c>
-      <c r="F32" s="5" t="s">
+      <c r="G32" s="5" t="s">
         <v>886</v>
       </c>
-      <c r="G32" s="5" t="s">
+      <c r="H32" s="5" t="s">
         <v>887</v>
       </c>
-      <c r="H32" s="5" t="s">
+      <c r="I32" s="9" t="s">
+        <v>1085</v>
+      </c>
+      <c r="J32" s="5" t="s">
         <v>888</v>
       </c>
-      <c r="I32" s="9" t="s">
-        <v>1086</v>
-      </c>
-      <c r="J32" s="5" t="s">
+      <c r="K32" s="5" t="s">
         <v>889</v>
       </c>
-      <c r="K32" s="5" t="s">
+      <c r="L32" s="5" t="s">
         <v>890</v>
       </c>
-      <c r="L32" s="5" t="s">
+      <c r="M32" s="5" t="s">
         <v>891</v>
-      </c>
-      <c r="M32" s="5" t="s">
-        <v>892</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.3">
@@ -5773,40 +5773,40 @@
         <v>615</v>
       </c>
       <c r="B33" s="5" t="s">
+        <v>892</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>1048</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>1086</v>
+      </c>
+      <c r="E33" s="6" t="s">
         <v>893</v>
       </c>
-      <c r="C33" s="9" t="s">
-        <v>1049</v>
-      </c>
-      <c r="D33" s="9" t="s">
-        <v>1087</v>
-      </c>
-      <c r="E33" s="6" t="s">
+      <c r="F33" s="5" t="s">
         <v>894</v>
       </c>
-      <c r="F33" s="5" t="s">
+      <c r="G33" s="5" t="s">
         <v>895</v>
       </c>
-      <c r="G33" s="5" t="s">
+      <c r="H33" s="5" t="s">
         <v>896</v>
       </c>
-      <c r="H33" s="5" t="s">
+      <c r="I33" s="9" t="s">
+        <v>1086</v>
+      </c>
+      <c r="J33" s="5" t="s">
         <v>897</v>
       </c>
-      <c r="I33" s="9" t="s">
-        <v>1087</v>
-      </c>
-      <c r="J33" s="5" t="s">
+      <c r="K33" s="5" t="s">
         <v>898</v>
       </c>
-      <c r="K33" s="5" t="s">
+      <c r="L33" s="5" t="s">
         <v>899</v>
       </c>
-      <c r="L33" s="5" t="s">
+      <c r="M33" s="5" t="s">
         <v>900</v>
-      </c>
-      <c r="M33" s="5" t="s">
-        <v>901</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.3">
@@ -5814,40 +5814,40 @@
         <v>538</v>
       </c>
       <c r="B34" s="5" t="s">
+        <v>901</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>1048</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>1087</v>
+      </c>
+      <c r="E34" s="6" t="s">
         <v>902</v>
       </c>
-      <c r="C34" s="9" t="s">
-        <v>1049</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>1088</v>
-      </c>
-      <c r="E34" s="6" t="s">
+      <c r="F34" s="5" t="s">
         <v>903</v>
       </c>
-      <c r="F34" s="5" t="s">
+      <c r="G34" s="5" t="s">
         <v>904</v>
       </c>
-      <c r="G34" s="5" t="s">
+      <c r="H34" s="5" t="s">
         <v>905</v>
       </c>
-      <c r="H34" s="5" t="s">
+      <c r="I34" s="9" t="s">
+        <v>1087</v>
+      </c>
+      <c r="J34" s="5" t="s">
         <v>906</v>
       </c>
-      <c r="I34" s="9" t="s">
-        <v>1088</v>
-      </c>
-      <c r="J34" s="5" t="s">
+      <c r="K34" s="5" t="s">
         <v>907</v>
       </c>
-      <c r="K34" s="5" t="s">
+      <c r="L34" s="5" t="s">
         <v>908</v>
       </c>
-      <c r="L34" s="5" t="s">
+      <c r="M34" s="5" t="s">
         <v>909</v>
-      </c>
-      <c r="M34" s="5" t="s">
-        <v>910</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.3">
@@ -5855,122 +5855,122 @@
         <v>546</v>
       </c>
       <c r="B35" s="5" t="s">
+        <v>910</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>1048</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>1088</v>
+      </c>
+      <c r="E35" s="6" t="s">
         <v>911</v>
       </c>
-      <c r="C35" s="9" t="s">
-        <v>1049</v>
-      </c>
-      <c r="D35" s="9" t="s">
-        <v>1089</v>
-      </c>
-      <c r="E35" s="6" t="s">
+      <c r="F35" s="5" t="s">
         <v>912</v>
       </c>
-      <c r="F35" s="5" t="s">
+      <c r="G35" s="5" t="s">
         <v>913</v>
       </c>
-      <c r="G35" s="5" t="s">
+      <c r="H35" s="5" t="s">
         <v>914</v>
       </c>
-      <c r="H35" s="5" t="s">
+      <c r="I35" s="9" t="s">
+        <v>1088</v>
+      </c>
+      <c r="J35" s="5" t="s">
         <v>915</v>
       </c>
-      <c r="I35" s="9" t="s">
-        <v>1089</v>
-      </c>
-      <c r="J35" s="5" t="s">
+      <c r="K35" s="5" t="s">
         <v>916</v>
       </c>
-      <c r="K35" s="5" t="s">
+      <c r="L35" s="5" t="s">
         <v>917</v>
       </c>
-      <c r="L35" s="5" t="s">
+      <c r="M35" s="5" t="s">
         <v>918</v>
-      </c>
-      <c r="M35" s="5" t="s">
-        <v>919</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36" s="11" t="s">
+        <v>919</v>
+      </c>
+      <c r="B36" s="5" t="s">
         <v>920</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="C36" s="9" t="s">
+        <v>1048</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>1056</v>
+      </c>
+      <c r="E36" s="6" t="s">
         <v>921</v>
       </c>
-      <c r="C36" s="9" t="s">
-        <v>1049</v>
-      </c>
-      <c r="D36" s="9" t="s">
-        <v>1057</v>
-      </c>
-      <c r="E36" s="6" t="s">
+      <c r="F36" s="5" t="s">
         <v>922</v>
       </c>
-      <c r="F36" s="5" t="s">
+      <c r="G36" s="5" t="s">
         <v>923</v>
       </c>
-      <c r="G36" s="5" t="s">
+      <c r="H36" s="5" t="s">
         <v>924</v>
       </c>
-      <c r="H36" s="5" t="s">
+      <c r="I36" s="9" t="s">
+        <v>1056</v>
+      </c>
+      <c r="J36" s="5" t="s">
         <v>925</v>
       </c>
-      <c r="I36" s="9" t="s">
-        <v>1057</v>
-      </c>
-      <c r="J36" s="5" t="s">
+      <c r="K36" s="5" t="s">
         <v>926</v>
       </c>
-      <c r="K36" s="5" t="s">
+      <c r="L36" s="5" t="s">
         <v>927</v>
       </c>
-      <c r="L36" s="5" t="s">
+      <c r="M36" s="5" t="s">
         <v>928</v>
-      </c>
-      <c r="M36" s="5" t="s">
-        <v>929</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
+        <v>1031</v>
+      </c>
+      <c r="B37" s="5" t="s">
         <v>1032</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="C37" s="9" t="s">
+        <v>1048</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>1089</v>
+      </c>
+      <c r="E37" s="5" t="s">
         <v>1033</v>
       </c>
-      <c r="C37" s="9" t="s">
-        <v>1049</v>
-      </c>
-      <c r="D37" s="9" t="s">
-        <v>1090</v>
-      </c>
-      <c r="E37" s="5" t="s">
+      <c r="F37" s="5" t="s">
         <v>1034</v>
       </c>
-      <c r="F37" s="5" t="s">
+      <c r="G37" s="5" t="s">
         <v>1035</v>
       </c>
-      <c r="G37" s="5" t="s">
+      <c r="H37" s="5" t="s">
         <v>1036</v>
       </c>
-      <c r="H37" s="5" t="s">
+      <c r="I37" s="9" t="s">
+        <v>1089</v>
+      </c>
+      <c r="J37" s="5" t="s">
         <v>1037</v>
       </c>
-      <c r="I37" s="9" t="s">
-        <v>1090</v>
-      </c>
-      <c r="J37" s="5" t="s">
+      <c r="K37" s="5" t="s">
         <v>1038</v>
       </c>
-      <c r="K37" s="5" t="s">
+      <c r="L37" s="5" t="s">
         <v>1039</v>
       </c>
-      <c r="L37" s="5" t="s">
+      <c r="M37" s="5" t="s">
         <v>1040</v>
-      </c>
-      <c r="M37" s="5" t="s">
-        <v>1041</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.3">
@@ -5981,10 +5981,10 @@
         <v>718</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="E38" s="6" t="s">
         <v>719</v>
@@ -5999,7 +5999,7 @@
         <v>722</v>
       </c>
       <c r="I38" s="9" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="J38" s="5" t="s">
         <v>723</v>
@@ -6022,10 +6022,10 @@
         <v>748</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="E39" s="6" t="s">
         <v>749</v>
@@ -6040,7 +6040,7 @@
         <v>752</v>
       </c>
       <c r="I39" s="9" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="J39" s="5" t="s">
         <v>753</v>
@@ -6066,10 +6066,10 @@
         <v>760</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="E40" s="6" t="s">
         <v>761</v>
@@ -6084,7 +6084,7 @@
         <v>764</v>
       </c>
       <c r="I40" s="9" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="J40" s="5" t="s">
         <v>765</v>
@@ -6108,10 +6108,10 @@
         <v>728</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="E41" s="6" t="s">
         <v>729</v>
@@ -6126,7 +6126,7 @@
         <v>732</v>
       </c>
       <c r="I41" s="9" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="J41" s="5" t="s">
         <v>733</v>
@@ -6149,10 +6149,10 @@
         <v>738</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="E42" s="6" t="s">
         <v>739</v>
@@ -6167,7 +6167,7 @@
         <v>742</v>
       </c>
       <c r="I42" s="9" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="J42" s="5" t="s">
         <v>743</v>
@@ -6249,7 +6249,7 @@
         <v>17</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>1</v>
@@ -6288,7 +6288,7 @@
         <v>121</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
@@ -6299,10 +6299,10 @@
         <v>44</v>
       </c>
       <c r="C2" s="9" t="s">
+        <v>1050</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>1051</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>1052</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>131</v>
@@ -6317,7 +6317,7 @@
         <v>48</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>129</v>
@@ -6575,7 +6575,7 @@
         <v>130</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>259</v>
@@ -6620,7 +6620,7 @@
         <v>130</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>267</v>
@@ -6665,7 +6665,7 @@
         <v>130</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>275</v>
@@ -6710,7 +6710,7 @@
         <v>130</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>283</v>
@@ -6755,7 +6755,7 @@
         <v>130</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>291</v>
@@ -6800,7 +6800,7 @@
         <v>130</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>299</v>
@@ -6845,7 +6845,7 @@
         <v>130</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>307</v>
@@ -7148,7 +7148,7 @@
         <v>242</v>
       </c>
       <c r="P20" s="5" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
@@ -7898,8 +7898,8 @@
   </sheetPr>
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7968,10 +7968,10 @@
         <v>139</v>
       </c>
       <c r="C2" s="9" t="s">
+        <v>1052</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>1053</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>1054</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>142</v>
@@ -7983,7 +7983,7 @@
         <v>144</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>165</v>
@@ -8006,10 +8006,10 @@
         <v>479</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>480</v>
@@ -8021,10 +8021,10 @@
         <v>482</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="J3" s="5" t="s">
         <v>483</v>
@@ -8044,40 +8044,40 @@
         <v>36</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>835</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>1110</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>843</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>836</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>1111</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>844</v>
-      </c>
-      <c r="E4" s="5" t="s">
+      <c r="F4" s="5" t="s">
         <v>837</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="G4" s="5" t="s">
         <v>838</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="H4" s="5" t="s">
         <v>839</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="I4" s="9" t="s">
+        <v>1110</v>
+      </c>
+      <c r="J4" s="5" t="s">
         <v>840</v>
       </c>
-      <c r="I4" s="9" t="s">
-        <v>1111</v>
-      </c>
-      <c r="J4" s="5" t="s">
+      <c r="K4" s="5" t="s">
         <v>841</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="L4" s="5" t="s">
         <v>842</v>
       </c>
-      <c r="L4" s="5" t="s">
-        <v>843</v>
-      </c>
       <c r="M4" s="5" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8085,40 +8085,40 @@
         <v>43</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>844</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>1111</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>852</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>845</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>1112</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>853</v>
-      </c>
-      <c r="E5" s="5" t="s">
+      <c r="F5" s="5" t="s">
         <v>846</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="G5" s="5" t="s">
         <v>847</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="H5" s="5" t="s">
         <v>848</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="I5" s="9" t="s">
+        <v>1111</v>
+      </c>
+      <c r="J5" s="5" t="s">
         <v>849</v>
       </c>
-      <c r="I5" s="9" t="s">
-        <v>1112</v>
-      </c>
-      <c r="J5" s="5" t="s">
+      <c r="K5" s="5" t="s">
         <v>850</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="L5" s="5" t="s">
         <v>851</v>
       </c>
-      <c r="L5" s="5" t="s">
-        <v>852</v>
-      </c>
       <c r="M5" s="5" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8126,40 +8126,40 @@
         <v>64</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>787</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>1112</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>788</v>
       </c>
-      <c r="C6" s="9" t="s">
-        <v>1113</v>
-      </c>
-      <c r="D6" s="6" t="s">
+      <c r="E6" s="5" t="s">
         <v>789</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="F6" s="5" t="s">
         <v>790</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="G6" s="5" t="s">
         <v>791</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="H6" s="5" t="s">
         <v>792</v>
       </c>
-      <c r="H6" s="5" t="s">
-        <v>793</v>
-      </c>
       <c r="I6" s="9" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="J6" s="5" t="s">
+        <v>795</v>
+      </c>
+      <c r="K6" s="5" t="s">
         <v>796</v>
       </c>
-      <c r="K6" s="5" t="s">
+      <c r="L6" s="5" t="s">
         <v>797</v>
       </c>
-      <c r="L6" s="5" t="s">
-        <v>798</v>
-      </c>
       <c r="M6" s="5" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8167,40 +8167,40 @@
         <v>96</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>772</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>1054</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>1055</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>773</v>
       </c>
-      <c r="C7" s="9" t="s">
-        <v>1055</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>1056</v>
-      </c>
-      <c r="E7" s="5" t="s">
+      <c r="F7" s="5" t="s">
         <v>774</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="G7" s="5" t="s">
         <v>775</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="H7" s="5" t="s">
+        <v>793</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>1054</v>
+      </c>
+      <c r="J7" s="5" t="s">
         <v>776</v>
       </c>
-      <c r="H7" s="5" t="s">
-        <v>794</v>
-      </c>
-      <c r="I7" s="9" t="s">
-        <v>1055</v>
-      </c>
-      <c r="J7" s="5" t="s">
+      <c r="K7" s="5" t="s">
         <v>777</v>
       </c>
-      <c r="K7" s="5" t="s">
-        <v>778</v>
-      </c>
       <c r="L7" s="5" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="M7" s="5" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8208,40 +8208,40 @@
         <v>103</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>778</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>1099</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>1100</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>779</v>
       </c>
-      <c r="C8" s="9" t="s">
-        <v>1100</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>1101</v>
-      </c>
-      <c r="E8" s="5" t="s">
+      <c r="F8" s="5" t="s">
         <v>780</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="G8" s="5" t="s">
         <v>781</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="H8" s="5" t="s">
+        <v>794</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>1099</v>
+      </c>
+      <c r="J8" s="5" t="s">
         <v>782</v>
       </c>
-      <c r="H8" s="5" t="s">
-        <v>795</v>
-      </c>
-      <c r="I8" s="9" t="s">
-        <v>1100</v>
-      </c>
-      <c r="J8" s="5" t="s">
+      <c r="K8" s="5" t="s">
         <v>783</v>
-      </c>
-      <c r="K8" s="5" t="s">
-        <v>784</v>
       </c>
       <c r="L8" s="5" t="s">
         <v>485</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8249,40 +8249,40 @@
         <v>111</v>
       </c>
       <c r="B9" s="5" t="s">
+        <v>799</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>1113</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>800</v>
       </c>
-      <c r="C9" s="9" t="s">
-        <v>1114</v>
-      </c>
-      <c r="D9" s="6" t="s">
+      <c r="E9" s="5" t="s">
         <v>801</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="F9" s="5" t="s">
         <v>802</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="G9" s="5" t="s">
         <v>803</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="H9" s="5" t="s">
         <v>804</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="I9" s="9" t="s">
+        <v>1113</v>
+      </c>
+      <c r="J9" s="5" t="s">
         <v>805</v>
       </c>
-      <c r="I9" s="9" t="s">
-        <v>1114</v>
-      </c>
-      <c r="J9" s="5" t="s">
+      <c r="K9" s="5" t="s">
         <v>806</v>
       </c>
-      <c r="K9" s="5" t="s">
+      <c r="L9" s="5" t="s">
         <v>807</v>
       </c>
-      <c r="L9" s="5" t="s">
-        <v>808</v>
-      </c>
       <c r="M9" s="5" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8293,10 +8293,10 @@
         <v>486</v>
       </c>
       <c r="C10" s="9" t="s">
+        <v>1095</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>1096</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>1097</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>487</v>
@@ -8308,10 +8308,10 @@
         <v>489</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="J10" s="5" t="s">
         <v>490</v>
@@ -8331,40 +8331,40 @@
         <v>115</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>969</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>1114</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>970</v>
       </c>
-      <c r="C11" s="9" t="s">
-        <v>1115</v>
-      </c>
-      <c r="D11" s="6" t="s">
+      <c r="E11" s="5" t="s">
         <v>971</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="F11" s="5" t="s">
         <v>972</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="G11" s="5" t="s">
         <v>973</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="H11" s="5" t="s">
         <v>974</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="I11" s="9" t="s">
+        <v>1114</v>
+      </c>
+      <c r="J11" s="5" t="s">
         <v>975</v>
       </c>
-      <c r="I11" s="9" t="s">
-        <v>1115</v>
-      </c>
-      <c r="J11" s="5" t="s">
+      <c r="K11" s="5" t="s">
         <v>976</v>
       </c>
-      <c r="K11" s="5" t="s">
+      <c r="L11" s="5" t="s">
         <v>977</v>
       </c>
-      <c r="L11" s="5" t="s">
-        <v>978</v>
-      </c>
       <c r="M11" s="5" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8372,40 +8372,40 @@
         <v>117</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>978</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>1115</v>
+      </c>
+      <c r="D12" s="6" t="s">
         <v>979</v>
       </c>
-      <c r="C12" s="9" t="s">
-        <v>1116</v>
-      </c>
-      <c r="D12" s="6" t="s">
+      <c r="E12" s="5" t="s">
         <v>980</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="F12" s="5" t="s">
         <v>981</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="G12" s="5" t="s">
         <v>982</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="H12" s="5" t="s">
         <v>983</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="I12" s="9" t="s">
+        <v>1115</v>
+      </c>
+      <c r="J12" s="5" t="s">
         <v>984</v>
       </c>
-      <c r="I12" s="9" t="s">
-        <v>1116</v>
-      </c>
-      <c r="J12" s="5" t="s">
+      <c r="K12" s="5" t="s">
         <v>985</v>
       </c>
-      <c r="K12" s="5" t="s">
+      <c r="L12" s="5" t="s">
         <v>986</v>
       </c>
-      <c r="L12" s="5" t="s">
-        <v>987</v>
-      </c>
       <c r="M12" s="5" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8413,40 +8413,40 @@
         <v>119</v>
       </c>
       <c r="B13" s="5" t="s">
+        <v>862</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>1116</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>863</v>
       </c>
-      <c r="C13" s="9" t="s">
-        <v>1117</v>
-      </c>
-      <c r="D13" s="6" t="s">
+      <c r="E13" s="5" t="s">
         <v>864</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="F13" s="5" t="s">
         <v>865</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="G13" s="5" t="s">
         <v>866</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="H13" s="5" t="s">
         <v>867</v>
       </c>
-      <c r="H13" s="5" t="s">
+      <c r="I13" s="9" t="s">
+        <v>1116</v>
+      </c>
+      <c r="J13" s="5" t="s">
         <v>868</v>
       </c>
-      <c r="I13" s="9" t="s">
-        <v>1117</v>
-      </c>
-      <c r="J13" s="5" t="s">
+      <c r="K13" s="5" t="s">
         <v>869</v>
       </c>
-      <c r="K13" s="5" t="s">
+      <c r="L13" s="5" t="s">
         <v>870</v>
       </c>
-      <c r="L13" s="5" t="s">
-        <v>871</v>
-      </c>
       <c r="M13" s="5" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8457,10 +8457,10 @@
         <v>493</v>
       </c>
       <c r="C14" s="9" t="s">
+        <v>1097</v>
+      </c>
+      <c r="D14" s="6" t="s">
         <v>1098</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>1099</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>494</v>
@@ -8473,7 +8473,7 @@
       </c>
       <c r="H14" s="5"/>
       <c r="I14" s="9" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="J14" s="5" t="s">
         <v>497</v>
@@ -8496,10 +8496,10 @@
         <v>501</v>
       </c>
       <c r="C15" s="9" t="s">
+        <v>1101</v>
+      </c>
+      <c r="D15" s="6" t="s">
         <v>1102</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>1103</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>502</v>
@@ -8512,7 +8512,7 @@
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="9" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="J15" s="5" t="s">
         <v>505</v>
@@ -8535,10 +8535,10 @@
         <v>509</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>510</v>
@@ -8551,7 +8551,7 @@
       </c>
       <c r="H16" s="5"/>
       <c r="I16" s="9" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="J16" s="5" t="s">
         <v>513</v>
@@ -8574,10 +8574,10 @@
         <v>516</v>
       </c>
       <c r="C17" s="9" t="s">
+        <v>1104</v>
+      </c>
+      <c r="D17" s="6" t="s">
         <v>1105</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>1106</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>517</v>
@@ -8592,7 +8592,7 @@
         <v>520</v>
       </c>
       <c r="I17" s="9" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="J17" s="5" t="s">
         <v>521</v>
@@ -8615,10 +8615,10 @@
         <v>524</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>525</v>
@@ -8631,7 +8631,7 @@
       </c>
       <c r="H18" s="5"/>
       <c r="I18" s="9" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="J18" s="5" t="s">
         <v>528</v>
@@ -8654,10 +8654,10 @@
         <v>531</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>769</v>
+        <v>1132</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>532</v>
@@ -8670,7 +8670,7 @@
       </c>
       <c r="H19" s="5"/>
       <c r="I19" s="9" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="J19" s="5" t="s">
         <v>535</v>
@@ -8693,10 +8693,10 @@
         <v>676</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>677</v>
@@ -8709,7 +8709,7 @@
       </c>
       <c r="H20" s="5"/>
       <c r="I20" s="9" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="J20" s="5" t="s">
         <v>680</v>
@@ -8732,10 +8732,10 @@
         <v>572</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>573</v>
@@ -8748,7 +8748,7 @@
       </c>
       <c r="H21" s="5"/>
       <c r="I21" s="9" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="J21" s="5" t="s">
         <v>576</v>
@@ -8768,40 +8768,40 @@
         <v>418</v>
       </c>
       <c r="B22" s="5" t="s">
+        <v>1005</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>1118</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>1131</v>
+      </c>
+      <c r="E22" s="5" t="s">
         <v>1006</v>
       </c>
-      <c r="C22" s="9" t="s">
-        <v>1119</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>1132</v>
-      </c>
-      <c r="E22" s="5" t="s">
+      <c r="F22" s="5" t="s">
         <v>1007</v>
       </c>
-      <c r="F22" s="5" t="s">
+      <c r="G22" s="5" t="s">
         <v>1008</v>
       </c>
-      <c r="G22" s="5" t="s">
+      <c r="H22" s="5" t="s">
         <v>1009</v>
       </c>
-      <c r="H22" s="5" t="s">
+      <c r="I22" s="9" t="s">
+        <v>1118</v>
+      </c>
+      <c r="J22" s="5" t="s">
         <v>1010</v>
       </c>
-      <c r="I22" s="9" t="s">
-        <v>1119</v>
-      </c>
-      <c r="J22" s="5" t="s">
+      <c r="K22" s="5" t="s">
         <v>1011</v>
       </c>
-      <c r="K22" s="5" t="s">
+      <c r="L22" s="5" t="s">
         <v>1012</v>
       </c>
-      <c r="L22" s="5" t="s">
-        <v>1013</v>
-      </c>
       <c r="M22" s="5" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8809,40 +8809,40 @@
         <v>427</v>
       </c>
       <c r="B23" s="5" t="s">
+        <v>809</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>1119</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>1043</v>
+      </c>
+      <c r="E23" s="5" t="s">
         <v>810</v>
       </c>
-      <c r="C23" s="9" t="s">
-        <v>1120</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>1044</v>
-      </c>
-      <c r="E23" s="5" t="s">
+      <c r="F23" s="5" t="s">
         <v>811</v>
       </c>
-      <c r="F23" s="5" t="s">
+      <c r="G23" s="5" t="s">
         <v>812</v>
       </c>
-      <c r="G23" s="5" t="s">
+      <c r="H23" s="5" t="s">
         <v>813</v>
       </c>
-      <c r="H23" s="5" t="s">
+      <c r="I23" s="9" t="s">
+        <v>1119</v>
+      </c>
+      <c r="J23" s="5" t="s">
         <v>814</v>
       </c>
-      <c r="I23" s="9" t="s">
-        <v>1120</v>
-      </c>
-      <c r="J23" s="5" t="s">
+      <c r="K23" s="5" t="s">
         <v>815</v>
       </c>
-      <c r="K23" s="5" t="s">
+      <c r="L23" s="5" t="s">
         <v>816</v>
       </c>
-      <c r="L23" s="5" t="s">
-        <v>817</v>
-      </c>
       <c r="M23" s="5" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8850,40 +8850,40 @@
         <v>437</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="D24" s="6" t="s">
+        <v>819</v>
+      </c>
+      <c r="E24" s="5" t="s">
         <v>820</v>
       </c>
-      <c r="E24" s="5" t="s">
+      <c r="F24" s="5" t="s">
         <v>821</v>
       </c>
-      <c r="F24" s="5" t="s">
+      <c r="G24" s="5" t="s">
         <v>822</v>
       </c>
-      <c r="G24" s="5" t="s">
+      <c r="H24" s="5" t="s">
         <v>823</v>
       </c>
-      <c r="H24" s="5" t="s">
+      <c r="I24" s="9" t="s">
+        <v>1120</v>
+      </c>
+      <c r="J24" s="5" t="s">
         <v>824</v>
       </c>
-      <c r="I24" s="9" t="s">
-        <v>1121</v>
-      </c>
-      <c r="J24" s="5" t="s">
+      <c r="K24" s="5" t="s">
         <v>825</v>
       </c>
-      <c r="K24" s="5" t="s">
+      <c r="L24" s="5" t="s">
         <v>826</v>
       </c>
-      <c r="L24" s="5" t="s">
-        <v>827</v>
-      </c>
       <c r="M24" s="5" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8891,40 +8891,40 @@
         <v>447</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="D25" s="6" t="s">
+        <v>827</v>
+      </c>
+      <c r="E25" s="5" t="s">
         <v>828</v>
       </c>
-      <c r="E25" s="5" t="s">
+      <c r="F25" s="5" t="s">
         <v>829</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="G25" s="5" t="s">
         <v>830</v>
       </c>
-      <c r="G25" s="5" t="s">
+      <c r="H25" s="5" t="s">
         <v>831</v>
       </c>
-      <c r="H25" s="5" t="s">
+      <c r="I25" s="9" t="s">
+        <v>1121</v>
+      </c>
+      <c r="J25" s="5" t="s">
         <v>832</v>
       </c>
-      <c r="I25" s="9" t="s">
-        <v>1122</v>
-      </c>
-      <c r="J25" s="5" t="s">
+      <c r="K25" s="5" t="s">
         <v>833</v>
       </c>
-      <c r="K25" s="5" t="s">
+      <c r="L25" s="5" t="s">
         <v>834</v>
       </c>
-      <c r="L25" s="5" t="s">
-        <v>835</v>
-      </c>
       <c r="M25" s="5" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8932,40 +8932,40 @@
         <v>457</v>
       </c>
       <c r="B26" s="5" t="s">
+        <v>929</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>1122</v>
+      </c>
+      <c r="D26" s="6" t="s">
         <v>930</v>
       </c>
-      <c r="C26" s="9" t="s">
-        <v>1123</v>
-      </c>
-      <c r="D26" s="6" t="s">
+      <c r="E26" s="5" t="s">
         <v>931</v>
       </c>
-      <c r="E26" s="5" t="s">
+      <c r="F26" s="5" t="s">
         <v>932</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="G26" s="5" t="s">
         <v>933</v>
       </c>
-      <c r="G26" s="5" t="s">
+      <c r="H26" s="5" t="s">
         <v>934</v>
       </c>
-      <c r="H26" s="5" t="s">
+      <c r="I26" s="9" t="s">
+        <v>1122</v>
+      </c>
+      <c r="J26" s="5" t="s">
         <v>935</v>
       </c>
-      <c r="I26" s="9" t="s">
-        <v>1123</v>
-      </c>
-      <c r="J26" s="5" t="s">
+      <c r="K26" s="5" t="s">
         <v>936</v>
       </c>
-      <c r="K26" s="5" t="s">
+      <c r="L26" s="5" t="s">
         <v>937</v>
       </c>
-      <c r="L26" s="5" t="s">
-        <v>938</v>
-      </c>
       <c r="M26" s="5" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -8973,40 +8973,40 @@
         <v>467</v>
       </c>
       <c r="B27" s="5" t="s">
+        <v>938</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>1123</v>
+      </c>
+      <c r="D27" s="6" t="s">
         <v>939</v>
       </c>
-      <c r="C27" s="9" t="s">
-        <v>1124</v>
-      </c>
-      <c r="D27" s="6" t="s">
+      <c r="E27" s="5" t="s">
         <v>940</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="F27" s="5" t="s">
         <v>941</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="G27" s="5" t="s">
         <v>942</v>
       </c>
-      <c r="G27" s="5" t="s">
+      <c r="H27" s="5" t="s">
         <v>943</v>
       </c>
-      <c r="H27" s="5" t="s">
+      <c r="I27" s="9" t="s">
+        <v>1123</v>
+      </c>
+      <c r="J27" s="5" t="s">
         <v>944</v>
       </c>
-      <c r="I27" s="9" t="s">
-        <v>1124</v>
-      </c>
-      <c r="J27" s="5" t="s">
+      <c r="K27" s="5" t="s">
         <v>945</v>
       </c>
-      <c r="K27" s="5" t="s">
+      <c r="L27" s="5" t="s">
         <v>946</v>
       </c>
-      <c r="L27" s="5" t="s">
-        <v>947</v>
-      </c>
       <c r="M27" s="5" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -9014,40 +9014,40 @@
         <v>579</v>
       </c>
       <c r="B28" s="5" t="s">
+        <v>947</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>1124</v>
+      </c>
+      <c r="D28" s="6" t="s">
         <v>948</v>
       </c>
-      <c r="C28" s="9" t="s">
-        <v>1125</v>
-      </c>
-      <c r="D28" s="6" t="s">
+      <c r="E28" s="5" t="s">
         <v>949</v>
       </c>
-      <c r="E28" s="5" t="s">
+      <c r="F28" s="5" t="s">
         <v>950</v>
       </c>
-      <c r="F28" s="5" t="s">
+      <c r="G28" s="5" t="s">
         <v>951</v>
       </c>
-      <c r="G28" s="5" t="s">
+      <c r="H28" s="5" t="s">
         <v>952</v>
       </c>
-      <c r="H28" s="5" t="s">
+      <c r="I28" s="9" t="s">
+        <v>1124</v>
+      </c>
+      <c r="J28" s="5" t="s">
         <v>953</v>
       </c>
-      <c r="I28" s="9" t="s">
-        <v>1125</v>
-      </c>
-      <c r="J28" s="5" t="s">
+      <c r="K28" s="5" t="s">
         <v>954</v>
       </c>
-      <c r="K28" s="5" t="s">
+      <c r="L28" s="5" t="s">
         <v>955</v>
       </c>
-      <c r="L28" s="5" t="s">
-        <v>956</v>
-      </c>
       <c r="M28" s="5" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -9055,40 +9055,40 @@
         <v>588</v>
       </c>
       <c r="B29" s="5" t="s">
+        <v>987</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>1125</v>
+      </c>
+      <c r="D29" s="6" t="s">
         <v>988</v>
       </c>
-      <c r="C29" s="9" t="s">
-        <v>1126</v>
-      </c>
-      <c r="D29" s="6" t="s">
+      <c r="E29" s="5" t="s">
         <v>989</v>
       </c>
-      <c r="E29" s="5" t="s">
+      <c r="F29" s="5" t="s">
         <v>990</v>
       </c>
-      <c r="F29" s="5" t="s">
+      <c r="G29" s="5" t="s">
         <v>991</v>
       </c>
-      <c r="G29" s="5" t="s">
+      <c r="H29" s="5" t="s">
         <v>992</v>
       </c>
-      <c r="H29" s="5" t="s">
+      <c r="I29" s="9" t="s">
+        <v>1125</v>
+      </c>
+      <c r="J29" s="5" t="s">
         <v>993</v>
       </c>
-      <c r="I29" s="9" t="s">
-        <v>1126</v>
-      </c>
-      <c r="J29" s="5" t="s">
+      <c r="K29" s="5" t="s">
         <v>994</v>
       </c>
-      <c r="K29" s="5" t="s">
+      <c r="L29" s="5" t="s">
         <v>995</v>
       </c>
-      <c r="L29" s="5" t="s">
-        <v>996</v>
-      </c>
       <c r="M29" s="5" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -9096,40 +9096,40 @@
         <v>597</v>
       </c>
       <c r="B30" s="5" t="s">
+        <v>996</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>1126</v>
+      </c>
+      <c r="D30" s="6" t="s">
         <v>997</v>
       </c>
-      <c r="C30" s="9" t="s">
-        <v>1127</v>
-      </c>
-      <c r="D30" s="6" t="s">
+      <c r="E30" s="5" t="s">
         <v>998</v>
       </c>
-      <c r="E30" s="5" t="s">
+      <c r="F30" s="5" t="s">
         <v>999</v>
       </c>
-      <c r="F30" s="5" t="s">
+      <c r="G30" s="5" t="s">
         <v>1000</v>
       </c>
-      <c r="G30" s="5" t="s">
+      <c r="H30" s="5" t="s">
         <v>1001</v>
       </c>
-      <c r="H30" s="5" t="s">
+      <c r="I30" s="9" t="s">
+        <v>1126</v>
+      </c>
+      <c r="J30" s="5" t="s">
         <v>1002</v>
       </c>
-      <c r="I30" s="9" t="s">
-        <v>1127</v>
-      </c>
-      <c r="J30" s="5" t="s">
+      <c r="K30" s="5" t="s">
         <v>1003</v>
       </c>
-      <c r="K30" s="5" t="s">
+      <c r="L30" s="5" t="s">
         <v>1004</v>
       </c>
-      <c r="L30" s="5" t="s">
-        <v>1005</v>
-      </c>
       <c r="M30" s="5" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -9137,40 +9137,40 @@
         <v>615</v>
       </c>
       <c r="B31" s="5" t="s">
+        <v>853</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>1127</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>861</v>
+      </c>
+      <c r="E31" s="5" t="s">
         <v>854</v>
       </c>
-      <c r="C31" s="9" t="s">
-        <v>1128</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>862</v>
-      </c>
-      <c r="E31" s="5" t="s">
+      <c r="F31" s="5" t="s">
         <v>855</v>
       </c>
-      <c r="F31" s="5" t="s">
+      <c r="G31" s="5" t="s">
         <v>856</v>
       </c>
-      <c r="G31" s="5" t="s">
+      <c r="H31" s="5" t="s">
         <v>857</v>
       </c>
-      <c r="H31" s="5" t="s">
+      <c r="I31" s="9" t="s">
+        <v>1127</v>
+      </c>
+      <c r="J31" s="5" t="s">
         <v>858</v>
       </c>
-      <c r="I31" s="9" t="s">
-        <v>1128</v>
-      </c>
-      <c r="J31" s="5" t="s">
+      <c r="K31" s="5" t="s">
         <v>859</v>
       </c>
-      <c r="K31" s="5" t="s">
+      <c r="L31" s="5" t="s">
         <v>860</v>
       </c>
-      <c r="L31" s="5" t="s">
-        <v>861</v>
-      </c>
       <c r="M31" s="5" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -9181,10 +9181,10 @@
         <v>539</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="E32" s="5" t="s">
         <v>540</v>
@@ -9197,7 +9197,7 @@
       </c>
       <c r="H32" s="5"/>
       <c r="I32" s="9" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="J32" s="5" t="s">
         <v>543</v>
@@ -9220,10 +9220,10 @@
         <v>547</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="E33" s="5" t="s">
         <v>548</v>
@@ -9236,7 +9236,7 @@
       </c>
       <c r="H33" s="5"/>
       <c r="I33" s="9" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="J33" s="5" t="s">
         <v>551</v>

</xml_diff>

<commit_message>
Added datasets for this test case
</commit_message>
<xml_diff>
--- a/DataSet/Integration_DataSet/TL/TL_Data_Set_AU.xlsx
+++ b/DataSet/Integration_DataSet/TL/TL_Data_Set_AU.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\Integration_DataSet\TL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{771FE3C2-D3D3-4C48-9950-967EE18C3DAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C11B6090-57B2-47E4-B9BC-244D90A8D92D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BaseRate_Fields" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1477" uniqueCount="1133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1478" uniqueCount="1133">
   <si>
     <t>rowid</t>
   </si>
@@ -1961,9 +1961,6 @@
   </si>
   <si>
     <t>\DataSet\TL_DataSet\FxRates_GSFile\TL_FX_15_Files\</t>
-  </si>
-  <si>
-    <t>\DataSet\TL_DataSet\FxRates_GSFile\TL_FX_16_Files\</t>
   </si>
   <si>
     <t>\DataSet\TL_DataSet\FxRates_GSFile\TL_FX_17_Files\</t>
@@ -3479,6 +3476,9 @@
   </si>
   <si>
     <t>\DataSet\Integration_DataSet\TL\FXRates_GSFile\AU\TL_FX_33_Files\</t>
+  </si>
+  <si>
+    <t>\DataSet\Integration_DataSet\TL\FXRates_GSFile\AU\TL_FX_16_Files\</t>
   </si>
 </sst>
 </file>
@@ -4435,25 +4435,25 @@
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="65.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="53.44140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="21.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="41.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="65.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="33.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="38.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="44.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="41.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="65.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="53.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="41.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="65.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="33.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="38.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="44.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="41.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="34.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4461,7 +4461,7 @@
         <v>17</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>1</v>
@@ -4494,10 +4494,10 @@
         <v>154</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>756</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -4505,10 +4505,10 @@
         <v>11</v>
       </c>
       <c r="C2" s="9" t="s">
+        <v>1046</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>1047</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>1048</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>94</v>
@@ -4523,7 +4523,7 @@
         <v>18</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>21</v>
@@ -4538,7 +4538,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>22</v>
       </c>
@@ -4546,10 +4546,10 @@
         <v>23</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>95</v>
@@ -4564,7 +4564,7 @@
         <v>25</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="J3" s="5" t="s">
         <v>26</v>
@@ -4579,7 +4579,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>36</v>
       </c>
@@ -4587,10 +4587,10 @@
         <v>30</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>140</v>
@@ -4605,7 +4605,7 @@
         <v>33</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="J4" s="5" t="s">
         <v>34</v>
@@ -4617,10 +4617,10 @@
         <v>135</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>698</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>43</v>
       </c>
@@ -4628,10 +4628,10 @@
         <v>37</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>153</v>
@@ -4646,7 +4646,7 @@
         <v>40</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="J5" s="5" t="s">
         <v>41</v>
@@ -4661,7 +4661,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>49</v>
       </c>
@@ -4669,10 +4669,10 @@
         <v>50</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>51</v>
@@ -4687,7 +4687,7 @@
         <v>54</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="J6" s="5" t="s">
         <v>55</v>
@@ -4702,7 +4702,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>57</v>
       </c>
@@ -4710,13 +4710,13 @@
         <v>58</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>59</v>
@@ -4728,7 +4728,7 @@
         <v>61</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="J7" s="5" t="s">
         <v>62</v>
@@ -4740,10 +4740,10 @@
         <v>138</v>
       </c>
       <c r="M7" s="5" t="s">
-        <v>694</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>64</v>
       </c>
@@ -4751,13 +4751,13 @@
         <v>65</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>66</v>
@@ -4769,7 +4769,7 @@
         <v>68</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="J8" s="5" t="s">
         <v>69</v>
@@ -4778,13 +4778,13 @@
         <v>70</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>695</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>96</v>
       </c>
@@ -4792,13 +4792,13 @@
         <v>97</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>98</v>
@@ -4810,7 +4810,7 @@
         <v>100</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="J9" s="5" t="s">
         <v>101</v>
@@ -4819,13 +4819,13 @@
         <v>102</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="M9" s="5" t="s">
-        <v>696</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>103</v>
       </c>
@@ -4833,10 +4833,10 @@
         <v>104</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>105</v>
@@ -4851,7 +4851,7 @@
         <v>108</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="J10" s="5" t="s">
         <v>109</v>
@@ -4860,13 +4860,13 @@
         <v>110</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="M10" s="5" t="s">
-        <v>697</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>111</v>
       </c>
@@ -4874,10 +4874,10 @@
         <v>156</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>112</v>
@@ -4892,7 +4892,7 @@
         <v>159</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="J11" s="5" t="s">
         <v>160</v>
@@ -4907,7 +4907,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>113</v>
       </c>
@@ -4915,10 +4915,10 @@
         <v>169</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>114</v>
@@ -4933,7 +4933,7 @@
         <v>191</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="J12" s="5" t="s">
         <v>196</v>
@@ -4948,7 +4948,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>115</v>
       </c>
@@ -4956,10 +4956,10 @@
         <v>170</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>116</v>
@@ -4974,7 +4974,7 @@
         <v>192</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="J13" s="5" t="s">
         <v>197</v>
@@ -4989,7 +4989,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>117</v>
       </c>
@@ -4997,10 +4997,10 @@
         <v>171</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>118</v>
@@ -5015,7 +5015,7 @@
         <v>193</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="J14" s="5" t="s">
         <v>198</v>
@@ -5030,7 +5030,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>119</v>
       </c>
@@ -5038,10 +5038,10 @@
         <v>172</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>120</v>
@@ -5056,7 +5056,7 @@
         <v>194</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="J15" s="5" t="s">
         <v>199</v>
@@ -5071,7 +5071,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>145</v>
       </c>
@@ -5079,10 +5079,10 @@
         <v>173</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>152</v>
@@ -5097,7 +5097,7 @@
         <v>148</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="J16" s="5" t="s">
         <v>149</v>
@@ -5112,130 +5112,130 @@
         <v>184</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>332</v>
       </c>
       <c r="B17" s="5" t="s">
+        <v>872</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>1046</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>1071</v>
+      </c>
+      <c r="E17" s="5" t="s">
         <v>873</v>
       </c>
-      <c r="C17" s="9" t="s">
-        <v>1047</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>1072</v>
-      </c>
-      <c r="E17" s="5" t="s">
+      <c r="F17" s="5" t="s">
         <v>874</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="G17" s="5" t="s">
         <v>875</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="H17" s="5" t="s">
         <v>876</v>
       </c>
-      <c r="H17" s="5" t="s">
+      <c r="I17" s="9" t="s">
+        <v>1071</v>
+      </c>
+      <c r="J17" s="5" t="s">
         <v>877</v>
       </c>
-      <c r="I17" s="9" t="s">
-        <v>1072</v>
-      </c>
-      <c r="J17" s="5" t="s">
+      <c r="K17" s="5" t="s">
         <v>878</v>
       </c>
-      <c r="K17" s="5" t="s">
+      <c r="L17" s="5" t="s">
         <v>879</v>
       </c>
-      <c r="L17" s="5" t="s">
+      <c r="M17" s="5" t="s">
         <v>880</v>
       </c>
-      <c r="M17" s="5" t="s">
-        <v>881</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>342</v>
       </c>
       <c r="B18" s="5" t="s">
+        <v>1011</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>1046</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>1072</v>
+      </c>
+      <c r="E18" s="5" t="s">
         <v>1012</v>
       </c>
-      <c r="C18" s="9" t="s">
-        <v>1047</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>1073</v>
-      </c>
-      <c r="E18" s="5" t="s">
+      <c r="F18" s="5" t="s">
         <v>1013</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="G18" s="5" t="s">
         <v>1014</v>
       </c>
-      <c r="G18" s="5" t="s">
+      <c r="H18" s="5" t="s">
         <v>1015</v>
       </c>
-      <c r="H18" s="5" t="s">
+      <c r="I18" s="9" t="s">
+        <v>1072</v>
+      </c>
+      <c r="J18" s="5" t="s">
         <v>1016</v>
       </c>
-      <c r="I18" s="9" t="s">
-        <v>1073</v>
-      </c>
-      <c r="J18" s="5" t="s">
+      <c r="K18" s="5" t="s">
         <v>1017</v>
       </c>
-      <c r="K18" s="5" t="s">
+      <c r="L18" s="5" t="s">
         <v>1018</v>
       </c>
-      <c r="L18" s="5" t="s">
+      <c r="M18" s="5" t="s">
         <v>1019</v>
       </c>
-      <c r="M18" s="5" t="s">
-        <v>1020</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>352</v>
       </c>
       <c r="B19" s="5" t="s">
+        <v>958</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>1046</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>1073</v>
+      </c>
+      <c r="E19" s="5" t="s">
         <v>959</v>
       </c>
-      <c r="C19" s="9" t="s">
-        <v>1047</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>1074</v>
-      </c>
-      <c r="E19" s="5" t="s">
+      <c r="F19" s="5" t="s">
         <v>960</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="G19" s="5" t="s">
         <v>961</v>
       </c>
-      <c r="G19" s="5" t="s">
+      <c r="H19" s="5" t="s">
         <v>962</v>
       </c>
-      <c r="H19" s="5" t="s">
+      <c r="I19" s="9" t="s">
+        <v>1073</v>
+      </c>
+      <c r="J19" s="5" t="s">
         <v>963</v>
       </c>
-      <c r="I19" s="9" t="s">
-        <v>1074</v>
-      </c>
-      <c r="J19" s="5" t="s">
+      <c r="K19" s="5" t="s">
         <v>964</v>
       </c>
-      <c r="K19" s="5" t="s">
+      <c r="L19" s="5" t="s">
         <v>965</v>
       </c>
-      <c r="L19" s="5" t="s">
+      <c r="M19" s="5" t="s">
         <v>966</v>
       </c>
-      <c r="M19" s="5" t="s">
-        <v>967</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>168</v>
       </c>
@@ -5243,10 +5243,10 @@
         <v>174</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>206</v>
@@ -5261,7 +5261,7 @@
         <v>195</v>
       </c>
       <c r="I20" s="9" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="J20" s="5" t="s">
         <v>200</v>
@@ -5276,7 +5276,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>209</v>
       </c>
@@ -5284,10 +5284,10 @@
         <v>219</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>210</v>
@@ -5302,7 +5302,7 @@
         <v>214</v>
       </c>
       <c r="I21" s="9" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="J21" s="5" t="s">
         <v>215</v>
@@ -5317,7 +5317,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>229</v>
       </c>
@@ -5325,10 +5325,10 @@
         <v>220</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>221</v>
@@ -5343,7 +5343,7 @@
         <v>224</v>
       </c>
       <c r="I22" s="9" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="J22" s="5" t="s">
         <v>225</v>
@@ -5358,7 +5358,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>231</v>
       </c>
@@ -5366,10 +5366,10 @@
         <v>230</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>239</v>
@@ -5384,7 +5384,7 @@
         <v>234</v>
       </c>
       <c r="I23" s="9" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="J23" s="5" t="s">
         <v>235</v>
@@ -5399,7 +5399,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
         <v>427</v>
       </c>
@@ -5407,10 +5407,10 @@
         <v>554</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>555</v>
@@ -5425,7 +5425,7 @@
         <v>558</v>
       </c>
       <c r="I24" s="9" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="J24" s="5" t="s">
         <v>559</v>
@@ -5440,7 +5440,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>437</v>
       </c>
@@ -5448,10 +5448,10 @@
         <v>571</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>563</v>
@@ -5466,7 +5466,7 @@
         <v>566</v>
       </c>
       <c r="I25" s="9" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="J25" s="5" t="s">
         <v>567</v>
@@ -5481,705 +5481,705 @@
         <v>570</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
         <v>447</v>
       </c>
       <c r="B26" s="5" t="s">
+        <v>681</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>1046</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>1079</v>
+      </c>
+      <c r="E26" s="6" t="s">
         <v>682</v>
       </c>
-      <c r="C26" s="9" t="s">
-        <v>1047</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>1080</v>
-      </c>
-      <c r="E26" s="6" t="s">
+      <c r="F26" s="5" t="s">
         <v>683</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="G26" s="5" t="s">
         <v>684</v>
       </c>
-      <c r="G26" s="5" t="s">
+      <c r="H26" s="5" t="s">
         <v>685</v>
       </c>
-      <c r="H26" s="5" t="s">
+      <c r="I26" s="9" t="s">
+        <v>1079</v>
+      </c>
+      <c r="J26" s="5" t="s">
         <v>686</v>
       </c>
-      <c r="I26" s="9" t="s">
-        <v>1080</v>
-      </c>
-      <c r="J26" s="5" t="s">
+      <c r="K26" s="5" t="s">
         <v>687</v>
       </c>
-      <c r="K26" s="5" t="s">
+      <c r="L26" s="5" t="s">
         <v>688</v>
       </c>
-      <c r="L26" s="5" t="s">
+      <c r="M26" s="5" t="s">
         <v>689</v>
       </c>
-      <c r="M26" s="5" t="s">
-        <v>690</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>457</v>
       </c>
       <c r="B27" s="5" t="s">
+        <v>1020</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>1046</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>1055</v>
+      </c>
+      <c r="E27" s="5" t="s">
         <v>1021</v>
       </c>
-      <c r="C27" s="9" t="s">
-        <v>1047</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>1056</v>
-      </c>
-      <c r="E27" s="5" t="s">
+      <c r="F27" s="5" t="s">
         <v>1022</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="G27" s="5" t="s">
         <v>1023</v>
       </c>
-      <c r="G27" s="5" t="s">
+      <c r="H27" s="5" t="s">
         <v>1024</v>
       </c>
-      <c r="H27" s="5" t="s">
+      <c r="I27" s="9" t="s">
+        <v>1055</v>
+      </c>
+      <c r="J27" s="5" t="s">
         <v>1025</v>
       </c>
-      <c r="I27" s="9" t="s">
-        <v>1056</v>
-      </c>
-      <c r="J27" s="5" t="s">
+      <c r="K27" s="5" t="s">
         <v>1026</v>
       </c>
-      <c r="K27" s="5" t="s">
+      <c r="L27" s="5" t="s">
         <v>1027</v>
       </c>
-      <c r="L27" s="5" t="s">
+      <c r="M27" s="5" t="s">
         <v>1028</v>
       </c>
-      <c r="M27" s="5" t="s">
-        <v>1029</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
         <v>467</v>
       </c>
       <c r="B28" s="5" t="s">
+        <v>656</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>1046</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>1080</v>
+      </c>
+      <c r="E28" s="6" t="s">
         <v>657</v>
       </c>
-      <c r="C28" s="9" t="s">
-        <v>1047</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>1081</v>
-      </c>
-      <c r="E28" s="6" t="s">
+      <c r="F28" s="5" t="s">
         <v>658</v>
       </c>
-      <c r="F28" s="5" t="s">
+      <c r="G28" s="5" t="s">
         <v>659</v>
       </c>
-      <c r="G28" s="5" t="s">
+      <c r="H28" s="5" t="s">
         <v>660</v>
       </c>
-      <c r="H28" s="5" t="s">
+      <c r="I28" s="9" t="s">
+        <v>1080</v>
+      </c>
+      <c r="J28" s="5" t="s">
         <v>661</v>
       </c>
-      <c r="I28" s="9" t="s">
-        <v>1081</v>
-      </c>
-      <c r="J28" s="5" t="s">
+      <c r="K28" s="5" t="s">
         <v>662</v>
       </c>
-      <c r="K28" s="5" t="s">
+      <c r="L28" s="5" t="s">
         <v>663</v>
       </c>
-      <c r="L28" s="5" t="s">
+      <c r="M28" s="5" t="s">
         <v>664</v>
       </c>
-      <c r="M28" s="5" t="s">
-        <v>665</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
         <v>579</v>
       </c>
       <c r="B29" s="5" t="s">
+        <v>665</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>1046</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>1081</v>
+      </c>
+      <c r="E29" s="6" t="s">
         <v>666</v>
       </c>
-      <c r="C29" s="9" t="s">
-        <v>1047</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>1082</v>
-      </c>
-      <c r="E29" s="6" t="s">
+      <c r="F29" s="5" t="s">
         <v>667</v>
       </c>
-      <c r="F29" s="5" t="s">
+      <c r="G29" s="5" t="s">
         <v>668</v>
       </c>
-      <c r="G29" s="5" t="s">
+      <c r="H29" s="5" t="s">
         <v>669</v>
       </c>
-      <c r="H29" s="5" t="s">
+      <c r="I29" s="9" t="s">
+        <v>1081</v>
+      </c>
+      <c r="J29" s="5" t="s">
         <v>670</v>
       </c>
-      <c r="I29" s="9" t="s">
-        <v>1082</v>
-      </c>
-      <c r="J29" s="5" t="s">
+      <c r="K29" s="5" t="s">
         <v>671</v>
       </c>
-      <c r="K29" s="5" t="s">
+      <c r="L29" s="5" t="s">
         <v>672</v>
       </c>
-      <c r="L29" s="5" t="s">
+      <c r="M29" s="5" t="s">
         <v>673</v>
       </c>
-      <c r="M29" s="5" t="s">
-        <v>674</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
         <v>597</v>
       </c>
       <c r="B30" s="5" t="s">
+        <v>698</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>1046</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>1082</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>712</v>
+      </c>
+      <c r="F30" s="5" t="s">
         <v>699</v>
       </c>
-      <c r="C30" s="9" t="s">
-        <v>1047</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>1083</v>
-      </c>
-      <c r="E30" s="6" t="s">
+      <c r="G30" s="5" t="s">
+        <v>700</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>701</v>
+      </c>
+      <c r="I30" s="9" t="s">
+        <v>1082</v>
+      </c>
+      <c r="J30" s="5" t="s">
+        <v>702</v>
+      </c>
+      <c r="K30" s="5" t="s">
+        <v>703</v>
+      </c>
+      <c r="L30" s="5" t="s">
         <v>713</v>
       </c>
-      <c r="F30" s="5" t="s">
+      <c r="M30" s="5" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="11" t="s">
+        <v>711</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>698</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>1046</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>1082</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>710</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>699</v>
+      </c>
+      <c r="G31" s="5" t="s">
         <v>700</v>
       </c>
-      <c r="G30" s="5" t="s">
+      <c r="H31" s="5" t="s">
         <v>701</v>
       </c>
-      <c r="H30" s="5" t="s">
+      <c r="I31" s="9" t="s">
+        <v>1082</v>
+      </c>
+      <c r="J31" s="5" t="s">
         <v>702</v>
       </c>
-      <c r="I30" s="9" t="s">
-        <v>1083</v>
-      </c>
-      <c r="J30" s="5" t="s">
+      <c r="K31" s="5" t="s">
         <v>703</v>
       </c>
-      <c r="K30" s="5" t="s">
+      <c r="L31" s="5" t="s">
+        <v>714</v>
+      </c>
+      <c r="M31" s="5" t="s">
         <v>704</v>
       </c>
-      <c r="L30" s="5" t="s">
-        <v>714</v>
-      </c>
-      <c r="M30" s="5" t="s">
-        <v>705</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A31" s="11" t="s">
-        <v>712</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>699</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>1047</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>1083</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>711</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>700</v>
-      </c>
-      <c r="G31" s="5" t="s">
-        <v>701</v>
-      </c>
-      <c r="H31" s="5" t="s">
-        <v>702</v>
-      </c>
-      <c r="I31" s="9" t="s">
-        <v>1083</v>
-      </c>
-      <c r="J31" s="5" t="s">
-        <v>703</v>
-      </c>
-      <c r="K31" s="5" t="s">
-        <v>704</v>
-      </c>
-      <c r="L31" s="5" t="s">
-        <v>715</v>
-      </c>
-      <c r="M31" s="5" t="s">
-        <v>705</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>606</v>
       </c>
       <c r="B32" s="5" t="s">
+        <v>881</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>1046</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>1083</v>
+      </c>
+      <c r="E32" s="6" t="s">
         <v>882</v>
       </c>
-      <c r="C32" s="9" t="s">
-        <v>1047</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>1084</v>
-      </c>
-      <c r="E32" s="6" t="s">
+      <c r="F32" s="5" t="s">
         <v>883</v>
       </c>
-      <c r="F32" s="5" t="s">
+      <c r="G32" s="5" t="s">
         <v>884</v>
       </c>
-      <c r="G32" s="5" t="s">
+      <c r="H32" s="5" t="s">
         <v>885</v>
       </c>
-      <c r="H32" s="5" t="s">
+      <c r="I32" s="9" t="s">
+        <v>1083</v>
+      </c>
+      <c r="J32" s="5" t="s">
         <v>886</v>
       </c>
-      <c r="I32" s="9" t="s">
-        <v>1084</v>
-      </c>
-      <c r="J32" s="5" t="s">
+      <c r="K32" s="5" t="s">
         <v>887</v>
       </c>
-      <c r="K32" s="5" t="s">
+      <c r="L32" s="5" t="s">
         <v>888</v>
       </c>
-      <c r="L32" s="5" t="s">
+      <c r="M32" s="5" t="s">
         <v>889</v>
       </c>
-      <c r="M32" s="5" t="s">
-        <v>890</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
         <v>615</v>
       </c>
       <c r="B33" s="5" t="s">
+        <v>890</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>1046</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>1084</v>
+      </c>
+      <c r="E33" s="6" t="s">
         <v>891</v>
       </c>
-      <c r="C33" s="9" t="s">
-        <v>1047</v>
-      </c>
-      <c r="D33" s="9" t="s">
-        <v>1085</v>
-      </c>
-      <c r="E33" s="6" t="s">
+      <c r="F33" s="5" t="s">
         <v>892</v>
       </c>
-      <c r="F33" s="5" t="s">
+      <c r="G33" s="5" t="s">
         <v>893</v>
       </c>
-      <c r="G33" s="5" t="s">
+      <c r="H33" s="5" t="s">
         <v>894</v>
       </c>
-      <c r="H33" s="5" t="s">
+      <c r="I33" s="9" t="s">
+        <v>1084</v>
+      </c>
+      <c r="J33" s="5" t="s">
         <v>895</v>
       </c>
-      <c r="I33" s="9" t="s">
-        <v>1085</v>
-      </c>
-      <c r="J33" s="5" t="s">
+      <c r="K33" s="5" t="s">
         <v>896</v>
       </c>
-      <c r="K33" s="5" t="s">
+      <c r="L33" s="5" t="s">
         <v>897</v>
       </c>
-      <c r="L33" s="5" t="s">
+      <c r="M33" s="5" t="s">
         <v>898</v>
       </c>
-      <c r="M33" s="5" t="s">
-        <v>899</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
         <v>538</v>
       </c>
       <c r="B34" s="5" t="s">
+        <v>899</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>1046</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>1085</v>
+      </c>
+      <c r="E34" s="6" t="s">
         <v>900</v>
       </c>
-      <c r="C34" s="9" t="s">
-        <v>1047</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>1086</v>
-      </c>
-      <c r="E34" s="6" t="s">
+      <c r="F34" s="5" t="s">
         <v>901</v>
       </c>
-      <c r="F34" s="5" t="s">
+      <c r="G34" s="5" t="s">
         <v>902</v>
       </c>
-      <c r="G34" s="5" t="s">
+      <c r="H34" s="5" t="s">
         <v>903</v>
       </c>
-      <c r="H34" s="5" t="s">
+      <c r="I34" s="9" t="s">
+        <v>1085</v>
+      </c>
+      <c r="J34" s="5" t="s">
         <v>904</v>
       </c>
-      <c r="I34" s="9" t="s">
-        <v>1086</v>
-      </c>
-      <c r="J34" s="5" t="s">
+      <c r="K34" s="5" t="s">
         <v>905</v>
       </c>
-      <c r="K34" s="5" t="s">
+      <c r="L34" s="5" t="s">
         <v>906</v>
       </c>
-      <c r="L34" s="5" t="s">
+      <c r="M34" s="5" t="s">
         <v>907</v>
       </c>
-      <c r="M34" s="5" t="s">
-        <v>908</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
         <v>546</v>
       </c>
       <c r="B35" s="5" t="s">
+        <v>908</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>1046</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>1086</v>
+      </c>
+      <c r="E35" s="6" t="s">
         <v>909</v>
       </c>
-      <c r="C35" s="9" t="s">
-        <v>1047</v>
-      </c>
-      <c r="D35" s="9" t="s">
+      <c r="F35" s="5" t="s">
+        <v>910</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>911</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>912</v>
+      </c>
+      <c r="I35" s="9" t="s">
+        <v>1086</v>
+      </c>
+      <c r="J35" s="5" t="s">
+        <v>913</v>
+      </c>
+      <c r="K35" s="5" t="s">
+        <v>914</v>
+      </c>
+      <c r="L35" s="5" t="s">
+        <v>915</v>
+      </c>
+      <c r="M35" s="5" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A36" s="11" t="s">
+        <v>917</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>918</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>1046</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>1054</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>919</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>920</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>921</v>
+      </c>
+      <c r="H36" s="5" t="s">
+        <v>922</v>
+      </c>
+      <c r="I36" s="9" t="s">
+        <v>1054</v>
+      </c>
+      <c r="J36" s="5" t="s">
+        <v>923</v>
+      </c>
+      <c r="K36" s="5" t="s">
+        <v>924</v>
+      </c>
+      <c r="L36" s="5" t="s">
+        <v>925</v>
+      </c>
+      <c r="M36" s="5" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
+        <v>1029</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>1030</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>1046</v>
+      </c>
+      <c r="D37" s="9" t="s">
         <v>1087</v>
       </c>
-      <c r="E35" s="6" t="s">
-        <v>910</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>911</v>
-      </c>
-      <c r="G35" s="5" t="s">
-        <v>912</v>
-      </c>
-      <c r="H35" s="5" t="s">
-        <v>913</v>
-      </c>
-      <c r="I35" s="9" t="s">
+      <c r="E37" s="5" t="s">
+        <v>1031</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>1032</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>1033</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>1034</v>
+      </c>
+      <c r="I37" s="9" t="s">
         <v>1087</v>
       </c>
-      <c r="J35" s="5" t="s">
-        <v>914</v>
-      </c>
-      <c r="K35" s="5" t="s">
-        <v>915</v>
-      </c>
-      <c r="L35" s="5" t="s">
-        <v>916</v>
-      </c>
-      <c r="M35" s="5" t="s">
-        <v>917</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A36" s="11" t="s">
-        <v>918</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>919</v>
-      </c>
-      <c r="C36" s="9" t="s">
-        <v>1047</v>
-      </c>
-      <c r="D36" s="9" t="s">
-        <v>1055</v>
-      </c>
-      <c r="E36" s="6" t="s">
-        <v>920</v>
-      </c>
-      <c r="F36" s="5" t="s">
-        <v>921</v>
-      </c>
-      <c r="G36" s="5" t="s">
-        <v>922</v>
-      </c>
-      <c r="H36" s="5" t="s">
-        <v>923</v>
-      </c>
-      <c r="I36" s="9" t="s">
-        <v>1055</v>
-      </c>
-      <c r="J36" s="5" t="s">
-        <v>924</v>
-      </c>
-      <c r="K36" s="5" t="s">
-        <v>925</v>
-      </c>
-      <c r="L36" s="5" t="s">
-        <v>926</v>
-      </c>
-      <c r="M36" s="5" t="s">
-        <v>927</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A37" s="5" t="s">
-        <v>1030</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>1031</v>
-      </c>
-      <c r="C37" s="9" t="s">
-        <v>1047</v>
-      </c>
-      <c r="D37" s="9" t="s">
+      <c r="J37" s="5" t="s">
+        <v>1035</v>
+      </c>
+      <c r="K37" s="5" t="s">
+        <v>1036</v>
+      </c>
+      <c r="L37" s="5" t="s">
+        <v>1037</v>
+      </c>
+      <c r="M37" s="5" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A38" s="11" t="s">
+        <v>715</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>716</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>1046</v>
+      </c>
+      <c r="D38" s="9" t="s">
         <v>1088</v>
       </c>
-      <c r="E37" s="5" t="s">
-        <v>1032</v>
-      </c>
-      <c r="F37" s="5" t="s">
-        <v>1033</v>
-      </c>
-      <c r="G37" s="5" t="s">
-        <v>1034</v>
-      </c>
-      <c r="H37" s="5" t="s">
-        <v>1035</v>
-      </c>
-      <c r="I37" s="9" t="s">
+      <c r="E38" s="6" t="s">
+        <v>717</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>718</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>719</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>720</v>
+      </c>
+      <c r="I38" s="9" t="s">
         <v>1088</v>
       </c>
-      <c r="J37" s="5" t="s">
-        <v>1036</v>
-      </c>
-      <c r="K37" s="5" t="s">
-        <v>1037</v>
-      </c>
-      <c r="L37" s="5" t="s">
-        <v>1038</v>
-      </c>
-      <c r="M37" s="5" t="s">
-        <v>1039</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A38" s="11" t="s">
-        <v>716</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>717</v>
-      </c>
-      <c r="C38" s="9" t="s">
-        <v>1047</v>
-      </c>
-      <c r="D38" s="9" t="s">
+      <c r="J38" s="5" t="s">
+        <v>721</v>
+      </c>
+      <c r="K38" s="5" t="s">
+        <v>722</v>
+      </c>
+      <c r="L38" s="5" t="s">
+        <v>723</v>
+      </c>
+      <c r="M38" s="5" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A39" s="11" t="s">
+        <v>745</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>746</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>1046</v>
+      </c>
+      <c r="D39" s="9" t="s">
         <v>1089</v>
       </c>
-      <c r="E38" s="6" t="s">
-        <v>718</v>
-      </c>
-      <c r="F38" s="5" t="s">
-        <v>719</v>
-      </c>
-      <c r="G38" s="5" t="s">
-        <v>720</v>
-      </c>
-      <c r="H38" s="5" t="s">
-        <v>721</v>
-      </c>
-      <c r="I38" s="9" t="s">
+      <c r="E39" s="6" t="s">
+        <v>747</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>748</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>749</v>
+      </c>
+      <c r="H39" s="5" t="s">
+        <v>750</v>
+      </c>
+      <c r="I39" s="9" t="s">
         <v>1089</v>
       </c>
-      <c r="J38" s="5" t="s">
-        <v>722</v>
-      </c>
-      <c r="K38" s="5" t="s">
-        <v>723</v>
-      </c>
-      <c r="L38" s="5" t="s">
-        <v>724</v>
-      </c>
-      <c r="M38" s="5" t="s">
+      <c r="J39" s="5" t="s">
+        <v>751</v>
+      </c>
+      <c r="K39" s="5" t="s">
+        <v>752</v>
+      </c>
+      <c r="L39" s="5" t="s">
+        <v>753</v>
+      </c>
+      <c r="M39" s="5" t="s">
+        <v>754</v>
+      </c>
+      <c r="N39" s="5" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A40" s="11" t="s">
+        <v>757</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>758</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>1046</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>1090</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>759</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>760</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>761</v>
+      </c>
+      <c r="H40" s="5" t="s">
+        <v>762</v>
+      </c>
+      <c r="I40" s="9" t="s">
+        <v>1090</v>
+      </c>
+      <c r="J40" s="5" t="s">
+        <v>763</v>
+      </c>
+      <c r="K40" s="5" t="s">
+        <v>764</v>
+      </c>
+      <c r="L40" s="5" t="s">
+        <v>765</v>
+      </c>
+      <c r="M40" s="5" t="s">
+        <v>766</v>
+      </c>
+      <c r="N40" s="5"/>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A41" s="11" t="s">
         <v>725</v>
       </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A39" s="11" t="s">
-        <v>746</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>747</v>
-      </c>
-      <c r="C39" s="9" t="s">
-        <v>1047</v>
-      </c>
-      <c r="D39" s="9" t="s">
-        <v>1090</v>
-      </c>
-      <c r="E39" s="6" t="s">
-        <v>748</v>
-      </c>
-      <c r="F39" s="5" t="s">
-        <v>749</v>
-      </c>
-      <c r="G39" s="5" t="s">
-        <v>750</v>
-      </c>
-      <c r="H39" s="5" t="s">
-        <v>751</v>
-      </c>
-      <c r="I39" s="9" t="s">
-        <v>1090</v>
-      </c>
-      <c r="J39" s="5" t="s">
-        <v>752</v>
-      </c>
-      <c r="K39" s="5" t="s">
-        <v>753</v>
-      </c>
-      <c r="L39" s="5" t="s">
-        <v>754</v>
-      </c>
-      <c r="M39" s="5" t="s">
-        <v>755</v>
-      </c>
-      <c r="N39" s="5" t="s">
-        <v>757</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A40" s="11" t="s">
-        <v>758</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>759</v>
-      </c>
-      <c r="C40" s="9" t="s">
-        <v>1047</v>
-      </c>
-      <c r="D40" s="9" t="s">
+      <c r="B41" s="5" t="s">
+        <v>726</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>1046</v>
+      </c>
+      <c r="D41" s="9" t="s">
         <v>1091</v>
       </c>
-      <c r="E40" s="6" t="s">
-        <v>760</v>
-      </c>
-      <c r="F40" s="5" t="s">
-        <v>761</v>
-      </c>
-      <c r="G40" s="5" t="s">
-        <v>762</v>
-      </c>
-      <c r="H40" s="5" t="s">
-        <v>763</v>
-      </c>
-      <c r="I40" s="9" t="s">
+      <c r="E41" s="6" t="s">
+        <v>727</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>728</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>729</v>
+      </c>
+      <c r="H41" s="5" t="s">
+        <v>730</v>
+      </c>
+      <c r="I41" s="9" t="s">
         <v>1091</v>
       </c>
-      <c r="J40" s="5" t="s">
-        <v>764</v>
-      </c>
-      <c r="K40" s="5" t="s">
-        <v>765</v>
-      </c>
-      <c r="L40" s="5" t="s">
-        <v>766</v>
-      </c>
-      <c r="M40" s="5" t="s">
-        <v>767</v>
-      </c>
-      <c r="N40" s="5"/>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A41" s="11" t="s">
-        <v>726</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>727</v>
-      </c>
-      <c r="C41" s="9" t="s">
-        <v>1047</v>
-      </c>
-      <c r="D41" s="9" t="s">
+      <c r="J41" s="5" t="s">
+        <v>731</v>
+      </c>
+      <c r="K41" s="5" t="s">
+        <v>732</v>
+      </c>
+      <c r="L41" s="5" t="s">
+        <v>733</v>
+      </c>
+      <c r="M41" s="5" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A42" s="11" t="s">
+        <v>735</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>736</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>1046</v>
+      </c>
+      <c r="D42" s="9" t="s">
         <v>1092</v>
       </c>
-      <c r="E41" s="6" t="s">
-        <v>728</v>
-      </c>
-      <c r="F41" s="5" t="s">
-        <v>729</v>
-      </c>
-      <c r="G41" s="5" t="s">
-        <v>730</v>
-      </c>
-      <c r="H41" s="5" t="s">
-        <v>731</v>
-      </c>
-      <c r="I41" s="9" t="s">
+      <c r="E42" s="6" t="s">
+        <v>737</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>738</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>739</v>
+      </c>
+      <c r="H42" s="5" t="s">
+        <v>740</v>
+      </c>
+      <c r="I42" s="9" t="s">
         <v>1092</v>
       </c>
-      <c r="J41" s="5" t="s">
-        <v>732</v>
-      </c>
-      <c r="K41" s="5" t="s">
-        <v>733</v>
-      </c>
-      <c r="L41" s="5" t="s">
-        <v>734</v>
-      </c>
-      <c r="M41" s="5" t="s">
-        <v>735</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A42" s="11" t="s">
-        <v>736</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>737</v>
-      </c>
-      <c r="C42" s="9" t="s">
-        <v>1047</v>
-      </c>
-      <c r="D42" s="9" t="s">
-        <v>1093</v>
-      </c>
-      <c r="E42" s="6" t="s">
-        <v>738</v>
-      </c>
-      <c r="F42" s="5" t="s">
-        <v>739</v>
-      </c>
-      <c r="G42" s="5" t="s">
-        <v>740</v>
-      </c>
-      <c r="H42" s="5" t="s">
+      <c r="J42" s="5" t="s">
         <v>741</v>
       </c>
-      <c r="I42" s="9" t="s">
-        <v>1093</v>
-      </c>
-      <c r="J42" s="5" t="s">
+      <c r="K42" s="5" t="s">
         <v>742</v>
       </c>
-      <c r="K42" s="5" t="s">
+      <c r="L42" s="5" t="s">
         <v>743</v>
       </c>
-      <c r="L42" s="5" t="s">
+      <c r="M42" s="5" t="s">
         <v>744</v>
-      </c>
-      <c r="M42" s="5" t="s">
-        <v>745</v>
       </c>
     </row>
   </sheetData>
@@ -6218,31 +6218,31 @@
   <sheetPr codeName="FXRates_Fields"/>
   <dimension ref="A1:P36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="66.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="44.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="43.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="61.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="45.88671875" customWidth="1"/>
-    <col min="11" max="11" width="40.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="40.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="66.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="61.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="45.85546875" customWidth="1"/>
+    <col min="11" max="11" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -6250,7 +6250,7 @@
         <v>17</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>1</v>
@@ -6289,10 +6289,10 @@
         <v>121</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>1040</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -6300,10 +6300,10 @@
         <v>44</v>
       </c>
       <c r="C2" s="9" t="s">
+        <v>1048</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>1049</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>1050</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>131</v>
@@ -6318,7 +6318,7 @@
         <v>48</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>129</v>
@@ -6339,7 +6339,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>22</v>
       </c>
@@ -6363,7 +6363,7 @@
         <v>74</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="J3" s="5" t="s">
         <v>75</v>
@@ -6384,7 +6384,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>36</v>
       </c>
@@ -6408,7 +6408,7 @@
         <v>85</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="J4" s="5" t="s">
         <v>81</v>
@@ -6429,7 +6429,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>43</v>
       </c>
@@ -6453,7 +6453,7 @@
         <v>86</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="J5" s="5" t="s">
         <v>82</v>
@@ -6474,7 +6474,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>49</v>
       </c>
@@ -6498,7 +6498,7 @@
         <v>91</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="J6" s="5" t="s">
         <v>92</v>
@@ -6519,7 +6519,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>57</v>
       </c>
@@ -6543,7 +6543,7 @@
         <v>126</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="J7" s="5" t="s">
         <v>127</v>
@@ -6564,7 +6564,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>64</v>
       </c>
@@ -6576,7 +6576,7 @@
         <v>130</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>259</v>
@@ -6588,7 +6588,7 @@
         <v>261</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="J8" s="5" t="s">
         <v>262</v>
@@ -6609,7 +6609,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>96</v>
       </c>
@@ -6621,7 +6621,7 @@
         <v>130</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>267</v>
@@ -6633,7 +6633,7 @@
         <v>269</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="J9" s="5" t="s">
         <v>270</v>
@@ -6654,7 +6654,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>103</v>
       </c>
@@ -6666,7 +6666,7 @@
         <v>130</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>275</v>
@@ -6678,7 +6678,7 @@
         <v>277</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="J10" s="5" t="s">
         <v>278</v>
@@ -6699,7 +6699,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>111</v>
       </c>
@@ -6711,7 +6711,7 @@
         <v>130</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>283</v>
@@ -6744,7 +6744,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>113</v>
       </c>
@@ -6756,7 +6756,7 @@
         <v>130</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>291</v>
@@ -6789,7 +6789,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>115</v>
       </c>
@@ -6801,7 +6801,7 @@
         <v>130</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>299</v>
@@ -6834,7 +6834,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>117</v>
       </c>
@@ -6846,7 +6846,7 @@
         <v>130</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>307</v>
@@ -6879,7 +6879,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>119</v>
       </c>
@@ -6924,7 +6924,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>145</v>
       </c>
@@ -6969,16 +6969,18 @@
         <v>242</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>332</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>333</v>
       </c>
-      <c r="C17" s="5"/>
+      <c r="C17" s="9" t="s">
+        <v>1048</v>
+      </c>
       <c r="D17" s="9" t="s">
-        <v>130</v>
+        <v>1132</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>334</v>
@@ -6993,7 +6995,7 @@
         <v>337</v>
       </c>
       <c r="I17" s="9" t="s">
-        <v>646</v>
+        <v>1132</v>
       </c>
       <c r="J17" s="5" t="s">
         <v>338</v>
@@ -7014,7 +7016,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>342</v>
       </c>
@@ -7038,7 +7040,7 @@
         <v>347</v>
       </c>
       <c r="I18" s="9" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="J18" s="5" t="s">
         <v>348</v>
@@ -7059,7 +7061,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>352</v>
       </c>
@@ -7083,7 +7085,7 @@
         <v>357</v>
       </c>
       <c r="I19" s="9" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="J19" s="5" t="s">
         <v>358</v>
@@ -7104,7 +7106,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>168</v>
       </c>
@@ -7149,10 +7151,10 @@
         <v>242</v>
       </c>
       <c r="P20" s="5" t="s">
-        <v>1041</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+        <v>1040</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>209</v>
       </c>
@@ -7197,7 +7199,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>229</v>
       </c>
@@ -7242,7 +7244,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>231</v>
       </c>
@@ -7287,7 +7289,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>398</v>
       </c>
@@ -7332,7 +7334,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>408</v>
       </c>
@@ -7377,7 +7379,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="26" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>418</v>
       </c>
@@ -7422,7 +7424,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="27" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>427</v>
       </c>
@@ -7467,7 +7469,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>437</v>
       </c>
@@ -7512,7 +7514,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>447</v>
       </c>
@@ -7557,7 +7559,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>457</v>
       </c>
@@ -7602,7 +7604,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="31" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>467</v>
       </c>
@@ -7647,7 +7649,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="32" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>579</v>
       </c>
@@ -7659,7 +7661,7 @@
         <v>130</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>581</v>
@@ -7692,7 +7694,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
         <v>588</v>
       </c>
@@ -7704,7 +7706,7 @@
         <v>130</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="F33" s="5" t="s">
         <v>590</v>
@@ -7737,7 +7739,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>597</v>
       </c>
@@ -7745,13 +7747,13 @@
         <v>598</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="F34" s="5" t="s">
         <v>599</v>
@@ -7763,7 +7765,7 @@
         <v>601</v>
       </c>
       <c r="I34" s="9" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="J34" s="5" t="s">
         <v>602</v>
@@ -7784,7 +7786,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>606</v>
       </c>
@@ -7796,7 +7798,7 @@
         <v>130</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="F35" s="5" t="s">
         <v>608</v>
@@ -7829,7 +7831,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
         <v>615</v>
       </c>
@@ -7841,7 +7843,7 @@
         <v>130</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="F36" s="5" t="s">
         <v>617</v>
@@ -7877,20 +7879,21 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D3:D7" r:id="rId1" display="\\DataSet\\TL_DataSet\\FxRates_GSFile\\" xr:uid="{1C2361F4-1B13-456E-9BA3-E3D8B7F812A7}"/>
-    <hyperlink ref="D8:D22" r:id="rId2" display="\\DataSet\\TL_DataSet\\FxRates_GSFile\\" xr:uid="{30D6AB87-ED81-4A29-A8BC-F1B921F77AB7}"/>
-    <hyperlink ref="I8:I22" r:id="rId3" display="\\DataSet\\TL_DataSet\\FxRates_GSFile\\" xr:uid="{6E3D10A6-4C88-4334-881C-8676178CABF0}"/>
-    <hyperlink ref="D23:D31" r:id="rId4" display="\\DataSet\\TL_DataSet\\FxRates_GSFile\\" xr:uid="{6B3504B3-9870-47D0-8E2F-5CAB415D1405}"/>
-    <hyperlink ref="I23:I31" r:id="rId5" display="\\DataSet\\TL_DataSet\\FxRates_GSFile\\" xr:uid="{57CD682C-3C14-436B-ADDE-9A80258650CD}"/>
-    <hyperlink ref="D32:D34" r:id="rId6" display="\\DataSet\\TL_DataSet\\FxRates_GSFile\\" xr:uid="{202A1715-BE83-4EB7-A90F-52978138A4F3}"/>
-    <hyperlink ref="D35:D36" r:id="rId7" display="\\DataSet\\TL_DataSet\\FxRates_GSFile\\" xr:uid="{9840F825-8637-4C41-AA65-6AF3ECBC53D3}"/>
-    <hyperlink ref="I35:I36" r:id="rId8" display="\\DataSet\\TL_DataSet\\FxRates_GSFile\\" xr:uid="{E6DF1C66-E06C-4508-BF64-80E6763D6FB9}"/>
-    <hyperlink ref="I21:I29" r:id="rId9" display="\\DataSet\\TL_DataSet\\FxRates_GSFile\\" xr:uid="{47A9315B-DFC8-4430-A45E-9D03C065A594}"/>
-    <hyperlink ref="C2" r:id="rId10" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{DC17FF84-1D37-4112-BF5D-BCB4C73CD0FB}"/>
-    <hyperlink ref="D2" r:id="rId11" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{7887B602-EE56-45AE-936D-8A968AF005AA}"/>
-    <hyperlink ref="I2" r:id="rId12" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{883636BB-DB43-4D2E-AC6F-B249FF19C9EB}"/>
-    <hyperlink ref="C34" r:id="rId13" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{7E8D6D8F-1005-42BD-A3F6-43B98FF5E132}"/>
-    <hyperlink ref="D34" r:id="rId14" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{36136DFC-9943-43B9-854E-C945D3088DDC}"/>
-    <hyperlink ref="I34" r:id="rId15" display="\\DataSet\\TL_DataSet\\FxRates_GSFile\\" xr:uid="{8E038F53-FC39-49CE-903E-024526995D11}"/>
+    <hyperlink ref="D23:D31" r:id="rId2" display="\\DataSet\\TL_DataSet\\FxRates_GSFile\\" xr:uid="{6B3504B3-9870-47D0-8E2F-5CAB415D1405}"/>
+    <hyperlink ref="I23:I31" r:id="rId3" display="\\DataSet\\TL_DataSet\\FxRates_GSFile\\" xr:uid="{57CD682C-3C14-436B-ADDE-9A80258650CD}"/>
+    <hyperlink ref="D32:D34" r:id="rId4" display="\\DataSet\\TL_DataSet\\FxRates_GSFile\\" xr:uid="{202A1715-BE83-4EB7-A90F-52978138A4F3}"/>
+    <hyperlink ref="D35:D36" r:id="rId5" display="\\DataSet\\TL_DataSet\\FxRates_GSFile\\" xr:uid="{9840F825-8637-4C41-AA65-6AF3ECBC53D3}"/>
+    <hyperlink ref="I35:I36" r:id="rId6" display="\\DataSet\\TL_DataSet\\FxRates_GSFile\\" xr:uid="{E6DF1C66-E06C-4508-BF64-80E6763D6FB9}"/>
+    <hyperlink ref="I21:I29" r:id="rId7" display="\\DataSet\\TL_DataSet\\FxRates_GSFile\\" xr:uid="{47A9315B-DFC8-4430-A45E-9D03C065A594}"/>
+    <hyperlink ref="C2" r:id="rId8" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{DC17FF84-1D37-4112-BF5D-BCB4C73CD0FB}"/>
+    <hyperlink ref="D2" r:id="rId9" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{7887B602-EE56-45AE-936D-8A968AF005AA}"/>
+    <hyperlink ref="I2" r:id="rId10" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{883636BB-DB43-4D2E-AC6F-B249FF19C9EB}"/>
+    <hyperlink ref="C34" r:id="rId11" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{7E8D6D8F-1005-42BD-A3F6-43B98FF5E132}"/>
+    <hyperlink ref="D34" r:id="rId12" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{36136DFC-9943-43B9-854E-C945D3088DDC}"/>
+    <hyperlink ref="I34" r:id="rId13" display="\\DataSet\\TL_DataSet\\FxRates_GSFile\\" xr:uid="{8E038F53-FC39-49CE-903E-024526995D11}"/>
+    <hyperlink ref="C17" r:id="rId14" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{F000EAE0-6BA8-48C7-9B53-7A06A8C6DCD7}"/>
+    <hyperlink ref="D17" r:id="rId15" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{7C1323CC-374D-40E7-971A-F564504DFCE4}"/>
+    <hyperlink ref="I17" r:id="rId16" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{B4382CB1-FCE5-4651-AB39-67F2F2B0722F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7907,24 +7910,24 @@
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="63.5546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.5703125" style="1" customWidth="1"/>
     <col min="4" max="4" width="94" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="42.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="36.33203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="75.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="37.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="42.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="36.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="75.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="37.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="40" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="60.33203125" customWidth="1"/>
+    <col min="12" max="12" width="60.28515625" customWidth="1"/>
     <col min="13" max="13" width="45" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -7965,7 +7968,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -7973,10 +7976,10 @@
         <v>139</v>
       </c>
       <c r="C2" s="9" t="s">
+        <v>1050</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>1051</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>1052</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>142</v>
@@ -7988,7 +7991,7 @@
         <v>144</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>165</v>
@@ -8003,7 +8006,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>22</v>
       </c>
@@ -8011,10 +8014,10 @@
         <v>479</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>480</v>
@@ -8026,10 +8029,10 @@
         <v>482</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="J3" s="5" t="s">
         <v>483</v>
@@ -8044,253 +8047,253 @@
         <v>485</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>36</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>833</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>1108</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>841</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>834</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>1109</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>842</v>
-      </c>
-      <c r="E4" s="5" t="s">
+      <c r="F4" s="5" t="s">
         <v>835</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="G4" s="5" t="s">
         <v>836</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="H4" s="5" t="s">
         <v>837</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="I4" s="9" t="s">
+        <v>1108</v>
+      </c>
+      <c r="J4" s="5" t="s">
         <v>838</v>
       </c>
-      <c r="I4" s="9" t="s">
-        <v>1109</v>
-      </c>
-      <c r="J4" s="5" t="s">
+      <c r="K4" s="5" t="s">
         <v>839</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="L4" s="5" t="s">
         <v>840</v>
       </c>
-      <c r="L4" s="5" t="s">
-        <v>841</v>
-      </c>
       <c r="M4" s="5" t="s">
-        <v>841</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>43</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>842</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>1109</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>850</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>843</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>1110</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>851</v>
-      </c>
-      <c r="E5" s="5" t="s">
+      <c r="F5" s="5" t="s">
         <v>844</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="G5" s="5" t="s">
         <v>845</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="H5" s="5" t="s">
         <v>846</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="I5" s="9" t="s">
+        <v>1109</v>
+      </c>
+      <c r="J5" s="5" t="s">
         <v>847</v>
       </c>
-      <c r="I5" s="9" t="s">
-        <v>1110</v>
-      </c>
-      <c r="J5" s="5" t="s">
+      <c r="K5" s="5" t="s">
         <v>848</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="L5" s="5" t="s">
         <v>849</v>
       </c>
-      <c r="L5" s="5" t="s">
-        <v>850</v>
-      </c>
       <c r="M5" s="5" t="s">
-        <v>850</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>64</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>785</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>1110</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>786</v>
       </c>
-      <c r="C6" s="9" t="s">
-        <v>1111</v>
-      </c>
-      <c r="D6" s="6" t="s">
+      <c r="E6" s="5" t="s">
         <v>787</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="F6" s="5" t="s">
         <v>788</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="G6" s="5" t="s">
         <v>789</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="H6" s="5" t="s">
         <v>790</v>
       </c>
-      <c r="H6" s="5" t="s">
-        <v>791</v>
-      </c>
       <c r="I6" s="9" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="J6" s="5" t="s">
+        <v>793</v>
+      </c>
+      <c r="K6" s="5" t="s">
         <v>794</v>
       </c>
-      <c r="K6" s="5" t="s">
+      <c r="L6" s="5" t="s">
         <v>795</v>
       </c>
-      <c r="L6" s="5" t="s">
-        <v>796</v>
-      </c>
       <c r="M6" s="5" t="s">
-        <v>796</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>96</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>770</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>1052</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>1053</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>771</v>
       </c>
-      <c r="C7" s="9" t="s">
-        <v>1053</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>1054</v>
-      </c>
-      <c r="E7" s="5" t="s">
+      <c r="F7" s="5" t="s">
         <v>772</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="G7" s="5" t="s">
         <v>773</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="H7" s="5" t="s">
+        <v>791</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>1052</v>
+      </c>
+      <c r="J7" s="5" t="s">
         <v>774</v>
       </c>
-      <c r="H7" s="5" t="s">
-        <v>792</v>
-      </c>
-      <c r="I7" s="9" t="s">
-        <v>1053</v>
-      </c>
-      <c r="J7" s="5" t="s">
+      <c r="K7" s="5" t="s">
         <v>775</v>
       </c>
-      <c r="K7" s="5" t="s">
-        <v>776</v>
-      </c>
       <c r="L7" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="M7" s="5" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>103</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>776</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>1097</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>1098</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>777</v>
       </c>
-      <c r="C8" s="9" t="s">
-        <v>1098</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>1099</v>
-      </c>
-      <c r="E8" s="5" t="s">
+      <c r="F8" s="5" t="s">
         <v>778</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="G8" s="5" t="s">
         <v>779</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="H8" s="5" t="s">
+        <v>792</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>1097</v>
+      </c>
+      <c r="J8" s="5" t="s">
         <v>780</v>
       </c>
-      <c r="H8" s="5" t="s">
-        <v>793</v>
-      </c>
-      <c r="I8" s="9" t="s">
-        <v>1098</v>
-      </c>
-      <c r="J8" s="5" t="s">
+      <c r="K8" s="5" t="s">
         <v>781</v>
-      </c>
-      <c r="K8" s="5" t="s">
-        <v>782</v>
       </c>
       <c r="L8" s="5" t="s">
         <v>485</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>783</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>111</v>
       </c>
       <c r="B9" s="5" t="s">
+        <v>797</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>1111</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>798</v>
       </c>
-      <c r="C9" s="9" t="s">
-        <v>1112</v>
-      </c>
-      <c r="D9" s="6" t="s">
+      <c r="E9" s="5" t="s">
         <v>799</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="F9" s="5" t="s">
         <v>800</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="G9" s="5" t="s">
         <v>801</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="H9" s="5" t="s">
         <v>802</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="I9" s="9" t="s">
+        <v>1111</v>
+      </c>
+      <c r="J9" s="5" t="s">
         <v>803</v>
       </c>
-      <c r="I9" s="9" t="s">
-        <v>1112</v>
-      </c>
-      <c r="J9" s="5" t="s">
+      <c r="K9" s="5" t="s">
         <v>804</v>
       </c>
-      <c r="K9" s="5" t="s">
+      <c r="L9" s="5" t="s">
         <v>805</v>
       </c>
-      <c r="L9" s="5" t="s">
-        <v>806</v>
-      </c>
       <c r="M9" s="5" t="s">
-        <v>806</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>113</v>
       </c>
@@ -8298,10 +8301,10 @@
         <v>486</v>
       </c>
       <c r="C10" s="9" t="s">
+        <v>1093</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>1094</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>1095</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>487</v>
@@ -8313,10 +8316,10 @@
         <v>489</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="J10" s="5" t="s">
         <v>490</v>
@@ -8331,130 +8334,130 @@
         <v>492</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>115</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>967</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>1112</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>968</v>
       </c>
-      <c r="C11" s="9" t="s">
-        <v>1113</v>
-      </c>
-      <c r="D11" s="6" t="s">
+      <c r="E11" s="5" t="s">
         <v>969</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="F11" s="5" t="s">
         <v>970</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="G11" s="5" t="s">
         <v>971</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="H11" s="5" t="s">
         <v>972</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="I11" s="9" t="s">
+        <v>1112</v>
+      </c>
+      <c r="J11" s="5" t="s">
         <v>973</v>
       </c>
-      <c r="I11" s="9" t="s">
-        <v>1113</v>
-      </c>
-      <c r="J11" s="5" t="s">
+      <c r="K11" s="5" t="s">
         <v>974</v>
       </c>
-      <c r="K11" s="5" t="s">
+      <c r="L11" s="5" t="s">
         <v>975</v>
       </c>
-      <c r="L11" s="5" t="s">
-        <v>976</v>
-      </c>
       <c r="M11" s="5" t="s">
-        <v>976</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>117</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>976</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>1113</v>
+      </c>
+      <c r="D12" s="6" t="s">
         <v>977</v>
       </c>
-      <c r="C12" s="9" t="s">
-        <v>1114</v>
-      </c>
-      <c r="D12" s="6" t="s">
+      <c r="E12" s="5" t="s">
         <v>978</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="F12" s="5" t="s">
         <v>979</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="G12" s="5" t="s">
         <v>980</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="H12" s="5" t="s">
         <v>981</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="I12" s="9" t="s">
+        <v>1113</v>
+      </c>
+      <c r="J12" s="5" t="s">
         <v>982</v>
       </c>
-      <c r="I12" s="9" t="s">
-        <v>1114</v>
-      </c>
-      <c r="J12" s="5" t="s">
+      <c r="K12" s="5" t="s">
         <v>983</v>
       </c>
-      <c r="K12" s="5" t="s">
+      <c r="L12" s="5" t="s">
         <v>984</v>
       </c>
-      <c r="L12" s="5" t="s">
-        <v>985</v>
-      </c>
       <c r="M12" s="5" t="s">
-        <v>985</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>119</v>
       </c>
       <c r="B13" s="5" t="s">
+        <v>860</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>1114</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>861</v>
       </c>
-      <c r="C13" s="9" t="s">
-        <v>1115</v>
-      </c>
-      <c r="D13" s="6" t="s">
+      <c r="E13" s="5" t="s">
         <v>862</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="F13" s="5" t="s">
         <v>863</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="G13" s="5" t="s">
         <v>864</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="H13" s="5" t="s">
         <v>865</v>
       </c>
-      <c r="H13" s="5" t="s">
+      <c r="I13" s="9" t="s">
+        <v>1114</v>
+      </c>
+      <c r="J13" s="5" t="s">
         <v>866</v>
       </c>
-      <c r="I13" s="9" t="s">
-        <v>1115</v>
-      </c>
-      <c r="J13" s="5" t="s">
+      <c r="K13" s="5" t="s">
         <v>867</v>
       </c>
-      <c r="K13" s="5" t="s">
+      <c r="L13" s="5" t="s">
         <v>868</v>
       </c>
-      <c r="L13" s="5" t="s">
-        <v>869</v>
-      </c>
       <c r="M13" s="5" t="s">
-        <v>869</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>145</v>
       </c>
@@ -8462,10 +8465,10 @@
         <v>493</v>
       </c>
       <c r="C14" s="9" t="s">
+        <v>1095</v>
+      </c>
+      <c r="D14" s="6" t="s">
         <v>1096</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>1097</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>494</v>
@@ -8478,7 +8481,7 @@
       </c>
       <c r="H14" s="5"/>
       <c r="I14" s="9" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="J14" s="5" t="s">
         <v>497</v>
@@ -8493,7 +8496,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>500</v>
       </c>
@@ -8501,10 +8504,10 @@
         <v>501</v>
       </c>
       <c r="C15" s="9" t="s">
+        <v>1099</v>
+      </c>
+      <c r="D15" s="6" t="s">
         <v>1100</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>1101</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>502</v>
@@ -8517,7 +8520,7 @@
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="9" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="J15" s="5" t="s">
         <v>505</v>
@@ -8532,7 +8535,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>508</v>
       </c>
@@ -8540,10 +8543,10 @@
         <v>509</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>510</v>
@@ -8556,7 +8559,7 @@
       </c>
       <c r="H16" s="5"/>
       <c r="I16" s="9" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="J16" s="5" t="s">
         <v>513</v>
@@ -8571,7 +8574,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>17</v>
       </c>
@@ -8579,10 +8582,10 @@
         <v>516</v>
       </c>
       <c r="C17" s="9" t="s">
+        <v>1102</v>
+      </c>
+      <c r="D17" s="6" t="s">
         <v>1103</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>1104</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>517</v>
@@ -8597,7 +8600,7 @@
         <v>520</v>
       </c>
       <c r="I17" s="9" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="J17" s="5" t="s">
         <v>521</v>
@@ -8612,7 +8615,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>18</v>
       </c>
@@ -8620,10 +8623,10 @@
         <v>524</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>525</v>
@@ -8636,7 +8639,7 @@
       </c>
       <c r="H18" s="5"/>
       <c r="I18" s="9" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="J18" s="5" t="s">
         <v>528</v>
@@ -8651,7 +8654,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>19</v>
       </c>
@@ -8659,10 +8662,10 @@
         <v>531</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>532</v>
@@ -8675,7 +8678,7 @@
       </c>
       <c r="H19" s="5"/>
       <c r="I19" s="9" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="J19" s="5" t="s">
         <v>535</v>
@@ -8690,46 +8693,46 @@
         <v>537</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>209</v>
       </c>
       <c r="B20" s="5" t="s">
+        <v>674</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>1106</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>767</v>
+      </c>
+      <c r="E20" s="5" t="s">
         <v>675</v>
       </c>
-      <c r="C20" s="9" t="s">
-        <v>1107</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>768</v>
-      </c>
-      <c r="E20" s="5" t="s">
+      <c r="F20" s="5" t="s">
         <v>676</v>
       </c>
-      <c r="F20" s="5" t="s">
+      <c r="G20" s="5" t="s">
         <v>677</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>678</v>
       </c>
       <c r="H20" s="5"/>
       <c r="I20" s="9" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="J20" s="5" t="s">
+        <v>678</v>
+      </c>
+      <c r="K20" s="5" t="s">
         <v>679</v>
       </c>
-      <c r="K20" s="5" t="s">
+      <c r="L20" s="5" t="s">
         <v>680</v>
       </c>
-      <c r="L20" s="5" t="s">
-        <v>681</v>
-      </c>
       <c r="M20" s="5" t="s">
-        <v>681</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>229</v>
       </c>
@@ -8737,10 +8740,10 @@
         <v>572</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>573</v>
@@ -8753,7 +8756,7 @@
       </c>
       <c r="H21" s="5"/>
       <c r="I21" s="9" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="J21" s="5" t="s">
         <v>576</v>
@@ -8768,417 +8771,417 @@
         <v>578</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>418</v>
       </c>
       <c r="B22" s="5" t="s">
+        <v>1003</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>1116</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>1129</v>
+      </c>
+      <c r="E22" s="5" t="s">
         <v>1004</v>
       </c>
-      <c r="C22" s="9" t="s">
-        <v>1117</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>1130</v>
-      </c>
-      <c r="E22" s="5" t="s">
+      <c r="F22" s="5" t="s">
         <v>1005</v>
       </c>
-      <c r="F22" s="5" t="s">
+      <c r="G22" s="5" t="s">
         <v>1006</v>
       </c>
-      <c r="G22" s="5" t="s">
+      <c r="H22" s="5" t="s">
         <v>1007</v>
       </c>
-      <c r="H22" s="5" t="s">
+      <c r="I22" s="9" t="s">
+        <v>1116</v>
+      </c>
+      <c r="J22" s="5" t="s">
         <v>1008</v>
       </c>
-      <c r="I22" s="9" t="s">
-        <v>1117</v>
-      </c>
-      <c r="J22" s="5" t="s">
+      <c r="K22" s="5" t="s">
         <v>1009</v>
       </c>
-      <c r="K22" s="5" t="s">
+      <c r="L22" s="5" t="s">
         <v>1010</v>
       </c>
-      <c r="L22" s="5" t="s">
-        <v>1011</v>
-      </c>
       <c r="M22" s="5" t="s">
-        <v>1011</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>427</v>
       </c>
       <c r="B23" s="5" t="s">
+        <v>807</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>1117</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>1041</v>
+      </c>
+      <c r="E23" s="5" t="s">
         <v>808</v>
       </c>
-      <c r="C23" s="9" t="s">
-        <v>1118</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>1042</v>
-      </c>
-      <c r="E23" s="5" t="s">
+      <c r="F23" s="5" t="s">
         <v>809</v>
       </c>
-      <c r="F23" s="5" t="s">
+      <c r="G23" s="5" t="s">
         <v>810</v>
       </c>
-      <c r="G23" s="5" t="s">
+      <c r="H23" s="5" t="s">
         <v>811</v>
       </c>
-      <c r="H23" s="5" t="s">
+      <c r="I23" s="9" t="s">
+        <v>1117</v>
+      </c>
+      <c r="J23" s="5" t="s">
         <v>812</v>
       </c>
-      <c r="I23" s="9" t="s">
-        <v>1118</v>
-      </c>
-      <c r="J23" s="5" t="s">
+      <c r="K23" s="5" t="s">
         <v>813</v>
       </c>
-      <c r="K23" s="5" t="s">
+      <c r="L23" s="5" t="s">
         <v>814</v>
       </c>
-      <c r="L23" s="5" t="s">
-        <v>815</v>
-      </c>
       <c r="M23" s="5" t="s">
-        <v>815</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>437</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="D24" s="6" t="s">
+        <v>817</v>
+      </c>
+      <c r="E24" s="5" t="s">
         <v>818</v>
       </c>
-      <c r="E24" s="5" t="s">
+      <c r="F24" s="5" t="s">
         <v>819</v>
       </c>
-      <c r="F24" s="5" t="s">
+      <c r="G24" s="5" t="s">
         <v>820</v>
       </c>
-      <c r="G24" s="5" t="s">
+      <c r="H24" s="5" t="s">
         <v>821</v>
       </c>
-      <c r="H24" s="5" t="s">
+      <c r="I24" s="9" t="s">
+        <v>1118</v>
+      </c>
+      <c r="J24" s="5" t="s">
         <v>822</v>
       </c>
-      <c r="I24" s="9" t="s">
-        <v>1119</v>
-      </c>
-      <c r="J24" s="5" t="s">
+      <c r="K24" s="5" t="s">
         <v>823</v>
       </c>
-      <c r="K24" s="5" t="s">
+      <c r="L24" s="5" t="s">
         <v>824</v>
       </c>
-      <c r="L24" s="5" t="s">
-        <v>825</v>
-      </c>
       <c r="M24" s="5" t="s">
-        <v>825</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>447</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="D25" s="6" t="s">
+        <v>825</v>
+      </c>
+      <c r="E25" s="5" t="s">
         <v>826</v>
       </c>
-      <c r="E25" s="5" t="s">
+      <c r="F25" s="5" t="s">
         <v>827</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="G25" s="5" t="s">
         <v>828</v>
       </c>
-      <c r="G25" s="5" t="s">
+      <c r="H25" s="5" t="s">
         <v>829</v>
       </c>
-      <c r="H25" s="5" t="s">
+      <c r="I25" s="9" t="s">
+        <v>1119</v>
+      </c>
+      <c r="J25" s="5" t="s">
         <v>830</v>
       </c>
-      <c r="I25" s="9" t="s">
-        <v>1120</v>
-      </c>
-      <c r="J25" s="5" t="s">
+      <c r="K25" s="5" t="s">
         <v>831</v>
       </c>
-      <c r="K25" s="5" t="s">
+      <c r="L25" s="5" t="s">
         <v>832</v>
       </c>
-      <c r="L25" s="5" t="s">
-        <v>833</v>
-      </c>
       <c r="M25" s="5" t="s">
-        <v>833</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>457</v>
       </c>
       <c r="B26" s="5" t="s">
+        <v>927</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>1120</v>
+      </c>
+      <c r="D26" s="6" t="s">
         <v>928</v>
       </c>
-      <c r="C26" s="9" t="s">
-        <v>1121</v>
-      </c>
-      <c r="D26" s="6" t="s">
+      <c r="E26" s="5" t="s">
         <v>929</v>
       </c>
-      <c r="E26" s="5" t="s">
+      <c r="F26" s="5" t="s">
         <v>930</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="G26" s="5" t="s">
         <v>931</v>
       </c>
-      <c r="G26" s="5" t="s">
+      <c r="H26" s="5" t="s">
         <v>932</v>
       </c>
-      <c r="H26" s="5" t="s">
+      <c r="I26" s="9" t="s">
+        <v>1120</v>
+      </c>
+      <c r="J26" s="5" t="s">
         <v>933</v>
       </c>
-      <c r="I26" s="9" t="s">
-        <v>1121</v>
-      </c>
-      <c r="J26" s="5" t="s">
+      <c r="K26" s="5" t="s">
         <v>934</v>
       </c>
-      <c r="K26" s="5" t="s">
+      <c r="L26" s="5" t="s">
         <v>935</v>
       </c>
-      <c r="L26" s="5" t="s">
-        <v>936</v>
-      </c>
       <c r="M26" s="5" t="s">
-        <v>936</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>467</v>
       </c>
       <c r="B27" s="5" t="s">
+        <v>936</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>1121</v>
+      </c>
+      <c r="D27" s="6" t="s">
         <v>937</v>
       </c>
-      <c r="C27" s="9" t="s">
-        <v>1122</v>
-      </c>
-      <c r="D27" s="6" t="s">
+      <c r="E27" s="5" t="s">
         <v>938</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="F27" s="5" t="s">
         <v>939</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="G27" s="5" t="s">
         <v>940</v>
       </c>
-      <c r="G27" s="5" t="s">
+      <c r="H27" s="5" t="s">
         <v>941</v>
       </c>
-      <c r="H27" s="5" t="s">
+      <c r="I27" s="9" t="s">
+        <v>1121</v>
+      </c>
+      <c r="J27" s="5" t="s">
         <v>942</v>
       </c>
-      <c r="I27" s="9" t="s">
-        <v>1122</v>
-      </c>
-      <c r="J27" s="5" t="s">
+      <c r="K27" s="5" t="s">
         <v>943</v>
       </c>
-      <c r="K27" s="5" t="s">
+      <c r="L27" s="5" t="s">
         <v>944</v>
       </c>
-      <c r="L27" s="5" t="s">
-        <v>945</v>
-      </c>
       <c r="M27" s="5" t="s">
-        <v>945</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>579</v>
       </c>
       <c r="B28" s="5" t="s">
+        <v>945</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>1122</v>
+      </c>
+      <c r="D28" s="6" t="s">
         <v>946</v>
       </c>
-      <c r="C28" s="9" t="s">
-        <v>1123</v>
-      </c>
-      <c r="D28" s="6" t="s">
+      <c r="E28" s="5" t="s">
         <v>947</v>
       </c>
-      <c r="E28" s="5" t="s">
+      <c r="F28" s="5" t="s">
         <v>948</v>
       </c>
-      <c r="F28" s="5" t="s">
+      <c r="G28" s="5" t="s">
         <v>949</v>
       </c>
-      <c r="G28" s="5" t="s">
+      <c r="H28" s="5" t="s">
         <v>950</v>
       </c>
-      <c r="H28" s="5" t="s">
+      <c r="I28" s="9" t="s">
+        <v>1122</v>
+      </c>
+      <c r="J28" s="5" t="s">
         <v>951</v>
       </c>
-      <c r="I28" s="9" t="s">
-        <v>1123</v>
-      </c>
-      <c r="J28" s="5" t="s">
+      <c r="K28" s="5" t="s">
         <v>952</v>
       </c>
-      <c r="K28" s="5" t="s">
+      <c r="L28" s="5" t="s">
         <v>953</v>
       </c>
-      <c r="L28" s="5" t="s">
-        <v>954</v>
-      </c>
       <c r="M28" s="5" t="s">
-        <v>954</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>588</v>
       </c>
       <c r="B29" s="5" t="s">
+        <v>985</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>1123</v>
+      </c>
+      <c r="D29" s="6" t="s">
         <v>986</v>
       </c>
-      <c r="C29" s="9" t="s">
-        <v>1124</v>
-      </c>
-      <c r="D29" s="6" t="s">
+      <c r="E29" s="5" t="s">
         <v>987</v>
       </c>
-      <c r="E29" s="5" t="s">
+      <c r="F29" s="5" t="s">
         <v>988</v>
       </c>
-      <c r="F29" s="5" t="s">
+      <c r="G29" s="5" t="s">
         <v>989</v>
       </c>
-      <c r="G29" s="5" t="s">
+      <c r="H29" s="5" t="s">
         <v>990</v>
       </c>
-      <c r="H29" s="5" t="s">
+      <c r="I29" s="9" t="s">
+        <v>1123</v>
+      </c>
+      <c r="J29" s="5" t="s">
         <v>991</v>
       </c>
-      <c r="I29" s="9" t="s">
-        <v>1124</v>
-      </c>
-      <c r="J29" s="5" t="s">
+      <c r="K29" s="5" t="s">
         <v>992</v>
       </c>
-      <c r="K29" s="5" t="s">
+      <c r="L29" s="5" t="s">
         <v>993</v>
       </c>
-      <c r="L29" s="5" t="s">
-        <v>994</v>
-      </c>
       <c r="M29" s="5" t="s">
-        <v>994</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>597</v>
       </c>
       <c r="B30" s="5" t="s">
+        <v>994</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>1124</v>
+      </c>
+      <c r="D30" s="6" t="s">
         <v>995</v>
       </c>
-      <c r="C30" s="9" t="s">
-        <v>1125</v>
-      </c>
-      <c r="D30" s="6" t="s">
+      <c r="E30" s="5" t="s">
         <v>996</v>
       </c>
-      <c r="E30" s="5" t="s">
+      <c r="F30" s="5" t="s">
         <v>997</v>
       </c>
-      <c r="F30" s="5" t="s">
+      <c r="G30" s="5" t="s">
         <v>998</v>
       </c>
-      <c r="G30" s="5" t="s">
+      <c r="H30" s="5" t="s">
         <v>999</v>
       </c>
-      <c r="H30" s="5" t="s">
+      <c r="I30" s="9" t="s">
+        <v>1124</v>
+      </c>
+      <c r="J30" s="5" t="s">
         <v>1000</v>
       </c>
-      <c r="I30" s="9" t="s">
-        <v>1125</v>
-      </c>
-      <c r="J30" s="5" t="s">
+      <c r="K30" s="5" t="s">
         <v>1001</v>
       </c>
-      <c r="K30" s="5" t="s">
+      <c r="L30" s="5" t="s">
         <v>1002</v>
       </c>
-      <c r="L30" s="5" t="s">
-        <v>1003</v>
-      </c>
       <c r="M30" s="5" t="s">
-        <v>1003</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>615</v>
       </c>
       <c r="B31" s="5" t="s">
+        <v>851</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>1125</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>859</v>
+      </c>
+      <c r="E31" s="5" t="s">
         <v>852</v>
       </c>
-      <c r="C31" s="9" t="s">
-        <v>1126</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>860</v>
-      </c>
-      <c r="E31" s="5" t="s">
+      <c r="F31" s="5" t="s">
         <v>853</v>
       </c>
-      <c r="F31" s="5" t="s">
+      <c r="G31" s="5" t="s">
         <v>854</v>
       </c>
-      <c r="G31" s="5" t="s">
+      <c r="H31" s="5" t="s">
         <v>855</v>
       </c>
-      <c r="H31" s="5" t="s">
+      <c r="I31" s="9" t="s">
+        <v>1125</v>
+      </c>
+      <c r="J31" s="5" t="s">
         <v>856</v>
       </c>
-      <c r="I31" s="9" t="s">
-        <v>1126</v>
-      </c>
-      <c r="J31" s="5" t="s">
+      <c r="K31" s="5" t="s">
         <v>857</v>
       </c>
-      <c r="K31" s="5" t="s">
+      <c r="L31" s="5" t="s">
         <v>858</v>
       </c>
-      <c r="L31" s="5" t="s">
-        <v>859</v>
-      </c>
       <c r="M31" s="5" t="s">
-        <v>859</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>538</v>
       </c>
@@ -9186,10 +9189,10 @@
         <v>539</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="E32" s="5" t="s">
         <v>540</v>
@@ -9202,7 +9205,7 @@
       </c>
       <c r="H32" s="5"/>
       <c r="I32" s="9" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="J32" s="5" t="s">
         <v>543</v>
@@ -9217,7 +9220,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>546</v>
       </c>
@@ -9225,10 +9228,10 @@
         <v>547</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="E33" s="5" t="s">
         <v>548</v>
@@ -9241,7 +9244,7 @@
       </c>
       <c r="H33" s="5"/>
       <c r="I33" s="9" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="J33" s="5" t="s">
         <v>551</v>
@@ -9282,9 +9285,9 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -9292,7 +9295,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
GDE-7287: Added dataset for TL_FXRates_17 Updated TL_Data_Set_AU.xlsx for TL_FX_17
</commit_message>
<xml_diff>
--- a/DataSet/Integration_DataSet/TL/TL_Data_Set_AU.xlsx
+++ b/DataSet/Integration_DataSet/TL/TL_Data_Set_AU.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\Integration_DataSet\TL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54170B65-BFDF-4326-936A-D4C15F71F5FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAC87AFF-EB1C-4F31-BB62-F8A8AABA8F7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BaseRate_Fields" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1480" uniqueCount="1133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1481" uniqueCount="1133">
   <si>
     <t>rowid</t>
   </si>
@@ -1955,9 +1955,6 @@
   </si>
   <si>
     <t>\DataSet\TL_DataSet\FxRates_GSFile\TL_FX_15_Files\</t>
-  </si>
-  <si>
-    <t>\DataSet\TL_DataSet\FxRates_GSFile\TL_FX_17_Files\</t>
   </si>
   <si>
     <t>\DataSet\TL_DataSet\FxRates_GSFile\TL_FX_18_Files\</t>
@@ -3479,6 +3476,9 @@
   </si>
   <si>
     <t>\DataSet\Integration_DataSet\TL\FXRates_GSFile\AU\TL_FX_31_Files\</t>
+  </si>
+  <si>
+    <t>\DataSet\Integration_DataSet\TL\FXRates_GSFile\AU\TL_FX_17_Files\</t>
   </si>
 </sst>
 </file>
@@ -4435,25 +4435,25 @@
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="65.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="53.44140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="21.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="41.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="65.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="33.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="38.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="44.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="41.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="65.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="53.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="41.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="65.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="33.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="38.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="44.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="41.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="34.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4461,7 +4461,7 @@
         <v>17</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>1</v>
@@ -4494,10 +4494,10 @@
         <v>154</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>753</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -4505,10 +4505,10 @@
         <v>11</v>
       </c>
       <c r="C2" s="9" t="s">
+        <v>1043</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>1044</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>1045</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>94</v>
@@ -4523,7 +4523,7 @@
         <v>18</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>21</v>
@@ -4538,7 +4538,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>22</v>
       </c>
@@ -4546,10 +4546,10 @@
         <v>23</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>95</v>
@@ -4564,7 +4564,7 @@
         <v>25</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="J3" s="5" t="s">
         <v>26</v>
@@ -4579,7 +4579,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>36</v>
       </c>
@@ -4587,10 +4587,10 @@
         <v>30</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>140</v>
@@ -4605,7 +4605,7 @@
         <v>33</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="J4" s="5" t="s">
         <v>34</v>
@@ -4617,10 +4617,10 @@
         <v>135</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>695</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>43</v>
       </c>
@@ -4628,10 +4628,10 @@
         <v>37</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>153</v>
@@ -4646,7 +4646,7 @@
         <v>40</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="J5" s="5" t="s">
         <v>41</v>
@@ -4661,7 +4661,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>49</v>
       </c>
@@ -4669,10 +4669,10 @@
         <v>50</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>51</v>
@@ -4687,7 +4687,7 @@
         <v>54</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="J6" s="5" t="s">
         <v>55</v>
@@ -4702,7 +4702,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>57</v>
       </c>
@@ -4710,13 +4710,13 @@
         <v>58</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>59</v>
@@ -4728,7 +4728,7 @@
         <v>61</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="J7" s="5" t="s">
         <v>62</v>
@@ -4740,10 +4740,10 @@
         <v>138</v>
       </c>
       <c r="M7" s="5" t="s">
-        <v>691</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>64</v>
       </c>
@@ -4751,13 +4751,13 @@
         <v>65</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>66</v>
@@ -4769,7 +4769,7 @@
         <v>68</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="J8" s="5" t="s">
         <v>69</v>
@@ -4778,13 +4778,13 @@
         <v>70</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>692</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>96</v>
       </c>
@@ -4792,13 +4792,13 @@
         <v>97</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>98</v>
@@ -4810,7 +4810,7 @@
         <v>100</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="J9" s="5" t="s">
         <v>101</v>
@@ -4819,13 +4819,13 @@
         <v>102</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="M9" s="5" t="s">
-        <v>693</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>103</v>
       </c>
@@ -4833,10 +4833,10 @@
         <v>104</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>105</v>
@@ -4851,7 +4851,7 @@
         <v>108</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="J10" s="5" t="s">
         <v>109</v>
@@ -4860,13 +4860,13 @@
         <v>110</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="M10" s="5" t="s">
-        <v>694</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>111</v>
       </c>
@@ -4874,10 +4874,10 @@
         <v>156</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>112</v>
@@ -4892,7 +4892,7 @@
         <v>159</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="J11" s="5" t="s">
         <v>160</v>
@@ -4907,7 +4907,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>113</v>
       </c>
@@ -4915,10 +4915,10 @@
         <v>169</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>114</v>
@@ -4933,7 +4933,7 @@
         <v>191</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="J12" s="5" t="s">
         <v>196</v>
@@ -4948,7 +4948,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>115</v>
       </c>
@@ -4956,10 +4956,10 @@
         <v>170</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>116</v>
@@ -4974,7 +4974,7 @@
         <v>192</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="J13" s="5" t="s">
         <v>197</v>
@@ -4989,7 +4989,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>117</v>
       </c>
@@ -4997,10 +4997,10 @@
         <v>171</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>118</v>
@@ -5015,7 +5015,7 @@
         <v>193</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="J14" s="5" t="s">
         <v>198</v>
@@ -5030,7 +5030,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>119</v>
       </c>
@@ -5038,10 +5038,10 @@
         <v>172</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>120</v>
@@ -5056,7 +5056,7 @@
         <v>194</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="J15" s="5" t="s">
         <v>199</v>
@@ -5071,7 +5071,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>145</v>
       </c>
@@ -5079,10 +5079,10 @@
         <v>173</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>152</v>
@@ -5097,7 +5097,7 @@
         <v>148</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="J16" s="5" t="s">
         <v>149</v>
@@ -5112,130 +5112,130 @@
         <v>184</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>332</v>
       </c>
       <c r="B17" s="5" t="s">
+        <v>869</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>1043</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>1068</v>
+      </c>
+      <c r="E17" s="5" t="s">
         <v>870</v>
       </c>
-      <c r="C17" s="9" t="s">
-        <v>1044</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>1069</v>
-      </c>
-      <c r="E17" s="5" t="s">
+      <c r="F17" s="5" t="s">
         <v>871</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="G17" s="5" t="s">
         <v>872</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="H17" s="5" t="s">
         <v>873</v>
       </c>
-      <c r="H17" s="5" t="s">
+      <c r="I17" s="9" t="s">
+        <v>1068</v>
+      </c>
+      <c r="J17" s="5" t="s">
         <v>874</v>
       </c>
-      <c r="I17" s="9" t="s">
-        <v>1069</v>
-      </c>
-      <c r="J17" s="5" t="s">
+      <c r="K17" s="5" t="s">
         <v>875</v>
       </c>
-      <c r="K17" s="5" t="s">
+      <c r="L17" s="5" t="s">
         <v>876</v>
       </c>
-      <c r="L17" s="5" t="s">
+      <c r="M17" s="5" t="s">
         <v>877</v>
       </c>
-      <c r="M17" s="5" t="s">
-        <v>878</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>342</v>
       </c>
       <c r="B18" s="5" t="s">
+        <v>1008</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>1043</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>1069</v>
+      </c>
+      <c r="E18" s="5" t="s">
         <v>1009</v>
       </c>
-      <c r="C18" s="9" t="s">
-        <v>1044</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>1070</v>
-      </c>
-      <c r="E18" s="5" t="s">
+      <c r="F18" s="5" t="s">
         <v>1010</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="G18" s="5" t="s">
         <v>1011</v>
       </c>
-      <c r="G18" s="5" t="s">
+      <c r="H18" s="5" t="s">
         <v>1012</v>
       </c>
-      <c r="H18" s="5" t="s">
+      <c r="I18" s="9" t="s">
+        <v>1069</v>
+      </c>
+      <c r="J18" s="5" t="s">
         <v>1013</v>
       </c>
-      <c r="I18" s="9" t="s">
-        <v>1070</v>
-      </c>
-      <c r="J18" s="5" t="s">
+      <c r="K18" s="5" t="s">
         <v>1014</v>
       </c>
-      <c r="K18" s="5" t="s">
+      <c r="L18" s="5" t="s">
         <v>1015</v>
       </c>
-      <c r="L18" s="5" t="s">
+      <c r="M18" s="5" t="s">
         <v>1016</v>
       </c>
-      <c r="M18" s="5" t="s">
-        <v>1017</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>352</v>
       </c>
       <c r="B19" s="5" t="s">
+        <v>955</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>1043</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>1070</v>
+      </c>
+      <c r="E19" s="5" t="s">
         <v>956</v>
       </c>
-      <c r="C19" s="9" t="s">
-        <v>1044</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>1071</v>
-      </c>
-      <c r="E19" s="5" t="s">
+      <c r="F19" s="5" t="s">
         <v>957</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="G19" s="5" t="s">
         <v>958</v>
       </c>
-      <c r="G19" s="5" t="s">
+      <c r="H19" s="5" t="s">
         <v>959</v>
       </c>
-      <c r="H19" s="5" t="s">
+      <c r="I19" s="9" t="s">
+        <v>1070</v>
+      </c>
+      <c r="J19" s="5" t="s">
         <v>960</v>
       </c>
-      <c r="I19" s="9" t="s">
-        <v>1071</v>
-      </c>
-      <c r="J19" s="5" t="s">
+      <c r="K19" s="5" t="s">
         <v>961</v>
       </c>
-      <c r="K19" s="5" t="s">
+      <c r="L19" s="5" t="s">
         <v>962</v>
       </c>
-      <c r="L19" s="5" t="s">
+      <c r="M19" s="5" t="s">
         <v>963</v>
       </c>
-      <c r="M19" s="5" t="s">
-        <v>964</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>168</v>
       </c>
@@ -5243,10 +5243,10 @@
         <v>174</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>206</v>
@@ -5261,7 +5261,7 @@
         <v>195</v>
       </c>
       <c r="I20" s="9" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="J20" s="5" t="s">
         <v>200</v>
@@ -5276,7 +5276,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>209</v>
       </c>
@@ -5284,10 +5284,10 @@
         <v>219</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>210</v>
@@ -5302,7 +5302,7 @@
         <v>214</v>
       </c>
       <c r="I21" s="9" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="J21" s="5" t="s">
         <v>215</v>
@@ -5317,7 +5317,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>229</v>
       </c>
@@ -5325,10 +5325,10 @@
         <v>220</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>221</v>
@@ -5343,7 +5343,7 @@
         <v>224</v>
       </c>
       <c r="I22" s="9" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="J22" s="5" t="s">
         <v>225</v>
@@ -5358,7 +5358,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>231</v>
       </c>
@@ -5366,10 +5366,10 @@
         <v>230</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>239</v>
@@ -5384,7 +5384,7 @@
         <v>234</v>
       </c>
       <c r="I23" s="9" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="J23" s="5" t="s">
         <v>235</v>
@@ -5399,7 +5399,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
         <v>427</v>
       </c>
@@ -5407,10 +5407,10 @@
         <v>554</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>555</v>
@@ -5425,7 +5425,7 @@
         <v>558</v>
       </c>
       <c r="I24" s="9" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="J24" s="5" t="s">
         <v>559</v>
@@ -5440,7 +5440,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>437</v>
       </c>
@@ -5448,10 +5448,10 @@
         <v>571</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>563</v>
@@ -5466,7 +5466,7 @@
         <v>566</v>
       </c>
       <c r="I25" s="9" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="J25" s="5" t="s">
         <v>567</v>
@@ -5481,705 +5481,705 @@
         <v>570</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
         <v>447</v>
       </c>
       <c r="B26" s="5" t="s">
+        <v>678</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>1043</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>1076</v>
+      </c>
+      <c r="E26" s="6" t="s">
         <v>679</v>
       </c>
-      <c r="C26" s="9" t="s">
-        <v>1044</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>1077</v>
-      </c>
-      <c r="E26" s="6" t="s">
+      <c r="F26" s="5" t="s">
         <v>680</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="G26" s="5" t="s">
         <v>681</v>
       </c>
-      <c r="G26" s="5" t="s">
+      <c r="H26" s="5" t="s">
         <v>682</v>
       </c>
-      <c r="H26" s="5" t="s">
+      <c r="I26" s="9" t="s">
+        <v>1076</v>
+      </c>
+      <c r="J26" s="5" t="s">
         <v>683</v>
       </c>
-      <c r="I26" s="9" t="s">
-        <v>1077</v>
-      </c>
-      <c r="J26" s="5" t="s">
+      <c r="K26" s="5" t="s">
         <v>684</v>
       </c>
-      <c r="K26" s="5" t="s">
+      <c r="L26" s="5" t="s">
         <v>685</v>
       </c>
-      <c r="L26" s="5" t="s">
+      <c r="M26" s="5" t="s">
         <v>686</v>
       </c>
-      <c r="M26" s="5" t="s">
-        <v>687</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>457</v>
       </c>
       <c r="B27" s="5" t="s">
+        <v>1017</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>1043</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>1052</v>
+      </c>
+      <c r="E27" s="5" t="s">
         <v>1018</v>
       </c>
-      <c r="C27" s="9" t="s">
-        <v>1044</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>1053</v>
-      </c>
-      <c r="E27" s="5" t="s">
+      <c r="F27" s="5" t="s">
         <v>1019</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="G27" s="5" t="s">
         <v>1020</v>
       </c>
-      <c r="G27" s="5" t="s">
+      <c r="H27" s="5" t="s">
         <v>1021</v>
       </c>
-      <c r="H27" s="5" t="s">
+      <c r="I27" s="9" t="s">
+        <v>1052</v>
+      </c>
+      <c r="J27" s="5" t="s">
         <v>1022</v>
       </c>
-      <c r="I27" s="9" t="s">
-        <v>1053</v>
-      </c>
-      <c r="J27" s="5" t="s">
+      <c r="K27" s="5" t="s">
         <v>1023</v>
       </c>
-      <c r="K27" s="5" t="s">
+      <c r="L27" s="5" t="s">
         <v>1024</v>
       </c>
-      <c r="L27" s="5" t="s">
+      <c r="M27" s="5" t="s">
         <v>1025</v>
       </c>
-      <c r="M27" s="5" t="s">
-        <v>1026</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
         <v>467</v>
       </c>
       <c r="B28" s="5" t="s">
+        <v>653</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>1043</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>1077</v>
+      </c>
+      <c r="E28" s="6" t="s">
         <v>654</v>
       </c>
-      <c r="C28" s="9" t="s">
-        <v>1044</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>1078</v>
-      </c>
-      <c r="E28" s="6" t="s">
+      <c r="F28" s="5" t="s">
         <v>655</v>
       </c>
-      <c r="F28" s="5" t="s">
+      <c r="G28" s="5" t="s">
         <v>656</v>
       </c>
-      <c r="G28" s="5" t="s">
+      <c r="H28" s="5" t="s">
         <v>657</v>
       </c>
-      <c r="H28" s="5" t="s">
+      <c r="I28" s="9" t="s">
+        <v>1077</v>
+      </c>
+      <c r="J28" s="5" t="s">
         <v>658</v>
       </c>
-      <c r="I28" s="9" t="s">
-        <v>1078</v>
-      </c>
-      <c r="J28" s="5" t="s">
+      <c r="K28" s="5" t="s">
         <v>659</v>
       </c>
-      <c r="K28" s="5" t="s">
+      <c r="L28" s="5" t="s">
         <v>660</v>
       </c>
-      <c r="L28" s="5" t="s">
+      <c r="M28" s="5" t="s">
         <v>661</v>
       </c>
-      <c r="M28" s="5" t="s">
-        <v>662</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
         <v>579</v>
       </c>
       <c r="B29" s="5" t="s">
+        <v>662</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>1043</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>1078</v>
+      </c>
+      <c r="E29" s="6" t="s">
         <v>663</v>
       </c>
-      <c r="C29" s="9" t="s">
-        <v>1044</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>1079</v>
-      </c>
-      <c r="E29" s="6" t="s">
+      <c r="F29" s="5" t="s">
         <v>664</v>
       </c>
-      <c r="F29" s="5" t="s">
+      <c r="G29" s="5" t="s">
         <v>665</v>
       </c>
-      <c r="G29" s="5" t="s">
+      <c r="H29" s="5" t="s">
         <v>666</v>
       </c>
-      <c r="H29" s="5" t="s">
+      <c r="I29" s="9" t="s">
+        <v>1078</v>
+      </c>
+      <c r="J29" s="5" t="s">
         <v>667</v>
       </c>
-      <c r="I29" s="9" t="s">
-        <v>1079</v>
-      </c>
-      <c r="J29" s="5" t="s">
+      <c r="K29" s="5" t="s">
         <v>668</v>
       </c>
-      <c r="K29" s="5" t="s">
+      <c r="L29" s="5" t="s">
         <v>669</v>
       </c>
-      <c r="L29" s="5" t="s">
+      <c r="M29" s="5" t="s">
         <v>670</v>
       </c>
-      <c r="M29" s="5" t="s">
-        <v>671</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
         <v>597</v>
       </c>
       <c r="B30" s="5" t="s">
+        <v>695</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>1043</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>1079</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>709</v>
+      </c>
+      <c r="F30" s="5" t="s">
         <v>696</v>
       </c>
-      <c r="C30" s="9" t="s">
-        <v>1044</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>1080</v>
-      </c>
-      <c r="E30" s="6" t="s">
+      <c r="G30" s="5" t="s">
+        <v>697</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>698</v>
+      </c>
+      <c r="I30" s="9" t="s">
+        <v>1079</v>
+      </c>
+      <c r="J30" s="5" t="s">
+        <v>699</v>
+      </c>
+      <c r="K30" s="5" t="s">
+        <v>700</v>
+      </c>
+      <c r="L30" s="5" t="s">
         <v>710</v>
       </c>
-      <c r="F30" s="5" t="s">
+      <c r="M30" s="5" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="11" t="s">
+        <v>708</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>695</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>1043</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>1079</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>707</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>696</v>
+      </c>
+      <c r="G31" s="5" t="s">
         <v>697</v>
       </c>
-      <c r="G30" s="5" t="s">
+      <c r="H31" s="5" t="s">
         <v>698</v>
       </c>
-      <c r="H30" s="5" t="s">
+      <c r="I31" s="9" t="s">
+        <v>1079</v>
+      </c>
+      <c r="J31" s="5" t="s">
         <v>699</v>
       </c>
-      <c r="I30" s="9" t="s">
-        <v>1080</v>
-      </c>
-      <c r="J30" s="5" t="s">
+      <c r="K31" s="5" t="s">
         <v>700</v>
       </c>
-      <c r="K30" s="5" t="s">
+      <c r="L31" s="5" t="s">
+        <v>711</v>
+      </c>
+      <c r="M31" s="5" t="s">
         <v>701</v>
       </c>
-      <c r="L30" s="5" t="s">
-        <v>711</v>
-      </c>
-      <c r="M30" s="5" t="s">
-        <v>702</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A31" s="11" t="s">
-        <v>709</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>696</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>1044</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>1080</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>708</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>697</v>
-      </c>
-      <c r="G31" s="5" t="s">
-        <v>698</v>
-      </c>
-      <c r="H31" s="5" t="s">
-        <v>699</v>
-      </c>
-      <c r="I31" s="9" t="s">
-        <v>1080</v>
-      </c>
-      <c r="J31" s="5" t="s">
-        <v>700</v>
-      </c>
-      <c r="K31" s="5" t="s">
-        <v>701</v>
-      </c>
-      <c r="L31" s="5" t="s">
-        <v>712</v>
-      </c>
-      <c r="M31" s="5" t="s">
-        <v>702</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>606</v>
       </c>
       <c r="B32" s="5" t="s">
+        <v>878</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>1043</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>1080</v>
+      </c>
+      <c r="E32" s="6" t="s">
         <v>879</v>
       </c>
-      <c r="C32" s="9" t="s">
-        <v>1044</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>1081</v>
-      </c>
-      <c r="E32" s="6" t="s">
+      <c r="F32" s="5" t="s">
         <v>880</v>
       </c>
-      <c r="F32" s="5" t="s">
+      <c r="G32" s="5" t="s">
         <v>881</v>
       </c>
-      <c r="G32" s="5" t="s">
+      <c r="H32" s="5" t="s">
         <v>882</v>
       </c>
-      <c r="H32" s="5" t="s">
+      <c r="I32" s="9" t="s">
+        <v>1080</v>
+      </c>
+      <c r="J32" s="5" t="s">
         <v>883</v>
       </c>
-      <c r="I32" s="9" t="s">
-        <v>1081</v>
-      </c>
-      <c r="J32" s="5" t="s">
+      <c r="K32" s="5" t="s">
         <v>884</v>
       </c>
-      <c r="K32" s="5" t="s">
+      <c r="L32" s="5" t="s">
         <v>885</v>
       </c>
-      <c r="L32" s="5" t="s">
+      <c r="M32" s="5" t="s">
         <v>886</v>
       </c>
-      <c r="M32" s="5" t="s">
-        <v>887</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
         <v>615</v>
       </c>
       <c r="B33" s="5" t="s">
+        <v>887</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>1043</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>1081</v>
+      </c>
+      <c r="E33" s="6" t="s">
         <v>888</v>
       </c>
-      <c r="C33" s="9" t="s">
-        <v>1044</v>
-      </c>
-      <c r="D33" s="9" t="s">
-        <v>1082</v>
-      </c>
-      <c r="E33" s="6" t="s">
+      <c r="F33" s="5" t="s">
         <v>889</v>
       </c>
-      <c r="F33" s="5" t="s">
+      <c r="G33" s="5" t="s">
         <v>890</v>
       </c>
-      <c r="G33" s="5" t="s">
+      <c r="H33" s="5" t="s">
         <v>891</v>
       </c>
-      <c r="H33" s="5" t="s">
+      <c r="I33" s="9" t="s">
+        <v>1081</v>
+      </c>
+      <c r="J33" s="5" t="s">
         <v>892</v>
       </c>
-      <c r="I33" s="9" t="s">
-        <v>1082</v>
-      </c>
-      <c r="J33" s="5" t="s">
+      <c r="K33" s="5" t="s">
         <v>893</v>
       </c>
-      <c r="K33" s="5" t="s">
+      <c r="L33" s="5" t="s">
         <v>894</v>
       </c>
-      <c r="L33" s="5" t="s">
+      <c r="M33" s="5" t="s">
         <v>895</v>
       </c>
-      <c r="M33" s="5" t="s">
-        <v>896</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
         <v>538</v>
       </c>
       <c r="B34" s="5" t="s">
+        <v>896</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>1043</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>1082</v>
+      </c>
+      <c r="E34" s="6" t="s">
         <v>897</v>
       </c>
-      <c r="C34" s="9" t="s">
-        <v>1044</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>1083</v>
-      </c>
-      <c r="E34" s="6" t="s">
+      <c r="F34" s="5" t="s">
         <v>898</v>
       </c>
-      <c r="F34" s="5" t="s">
+      <c r="G34" s="5" t="s">
         <v>899</v>
       </c>
-      <c r="G34" s="5" t="s">
+      <c r="H34" s="5" t="s">
         <v>900</v>
       </c>
-      <c r="H34" s="5" t="s">
+      <c r="I34" s="9" t="s">
+        <v>1082</v>
+      </c>
+      <c r="J34" s="5" t="s">
         <v>901</v>
       </c>
-      <c r="I34" s="9" t="s">
-        <v>1083</v>
-      </c>
-      <c r="J34" s="5" t="s">
+      <c r="K34" s="5" t="s">
         <v>902</v>
       </c>
-      <c r="K34" s="5" t="s">
+      <c r="L34" s="5" t="s">
         <v>903</v>
       </c>
-      <c r="L34" s="5" t="s">
+      <c r="M34" s="5" t="s">
         <v>904</v>
       </c>
-      <c r="M34" s="5" t="s">
-        <v>905</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
         <v>546</v>
       </c>
       <c r="B35" s="5" t="s">
+        <v>905</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>1043</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>1083</v>
+      </c>
+      <c r="E35" s="6" t="s">
         <v>906</v>
       </c>
-      <c r="C35" s="9" t="s">
-        <v>1044</v>
-      </c>
-      <c r="D35" s="9" t="s">
+      <c r="F35" s="5" t="s">
+        <v>907</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>908</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>909</v>
+      </c>
+      <c r="I35" s="9" t="s">
+        <v>1083</v>
+      </c>
+      <c r="J35" s="5" t="s">
+        <v>910</v>
+      </c>
+      <c r="K35" s="5" t="s">
+        <v>911</v>
+      </c>
+      <c r="L35" s="5" t="s">
+        <v>912</v>
+      </c>
+      <c r="M35" s="5" t="s">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A36" s="11" t="s">
+        <v>914</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>915</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>1043</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>1051</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>916</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>917</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>918</v>
+      </c>
+      <c r="H36" s="5" t="s">
+        <v>919</v>
+      </c>
+      <c r="I36" s="9" t="s">
+        <v>1051</v>
+      </c>
+      <c r="J36" s="5" t="s">
+        <v>920</v>
+      </c>
+      <c r="K36" s="5" t="s">
+        <v>921</v>
+      </c>
+      <c r="L36" s="5" t="s">
+        <v>922</v>
+      </c>
+      <c r="M36" s="5" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
+        <v>1026</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>1027</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>1043</v>
+      </c>
+      <c r="D37" s="9" t="s">
         <v>1084</v>
       </c>
-      <c r="E35" s="6" t="s">
-        <v>907</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>908</v>
-      </c>
-      <c r="G35" s="5" t="s">
-        <v>909</v>
-      </c>
-      <c r="H35" s="5" t="s">
-        <v>910</v>
-      </c>
-      <c r="I35" s="9" t="s">
+      <c r="E37" s="5" t="s">
+        <v>1028</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>1029</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>1030</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>1031</v>
+      </c>
+      <c r="I37" s="9" t="s">
         <v>1084</v>
       </c>
-      <c r="J35" s="5" t="s">
-        <v>911</v>
-      </c>
-      <c r="K35" s="5" t="s">
-        <v>912</v>
-      </c>
-      <c r="L35" s="5" t="s">
-        <v>913</v>
-      </c>
-      <c r="M35" s="5" t="s">
-        <v>914</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A36" s="11" t="s">
-        <v>915</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>916</v>
-      </c>
-      <c r="C36" s="9" t="s">
-        <v>1044</v>
-      </c>
-      <c r="D36" s="9" t="s">
-        <v>1052</v>
-      </c>
-      <c r="E36" s="6" t="s">
-        <v>917</v>
-      </c>
-      <c r="F36" s="5" t="s">
-        <v>918</v>
-      </c>
-      <c r="G36" s="5" t="s">
-        <v>919</v>
-      </c>
-      <c r="H36" s="5" t="s">
-        <v>920</v>
-      </c>
-      <c r="I36" s="9" t="s">
-        <v>1052</v>
-      </c>
-      <c r="J36" s="5" t="s">
-        <v>921</v>
-      </c>
-      <c r="K36" s="5" t="s">
-        <v>922</v>
-      </c>
-      <c r="L36" s="5" t="s">
-        <v>923</v>
-      </c>
-      <c r="M36" s="5" t="s">
-        <v>924</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A37" s="5" t="s">
-        <v>1027</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>1028</v>
-      </c>
-      <c r="C37" s="9" t="s">
-        <v>1044</v>
-      </c>
-      <c r="D37" s="9" t="s">
+      <c r="J37" s="5" t="s">
+        <v>1032</v>
+      </c>
+      <c r="K37" s="5" t="s">
+        <v>1033</v>
+      </c>
+      <c r="L37" s="5" t="s">
+        <v>1034</v>
+      </c>
+      <c r="M37" s="5" t="s">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A38" s="11" t="s">
+        <v>712</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>713</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>1043</v>
+      </c>
+      <c r="D38" s="9" t="s">
         <v>1085</v>
       </c>
-      <c r="E37" s="5" t="s">
-        <v>1029</v>
-      </c>
-      <c r="F37" s="5" t="s">
-        <v>1030</v>
-      </c>
-      <c r="G37" s="5" t="s">
-        <v>1031</v>
-      </c>
-      <c r="H37" s="5" t="s">
-        <v>1032</v>
-      </c>
-      <c r="I37" s="9" t="s">
+      <c r="E38" s="6" t="s">
+        <v>714</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>715</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>716</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>717</v>
+      </c>
+      <c r="I38" s="9" t="s">
         <v>1085</v>
       </c>
-      <c r="J37" s="5" t="s">
-        <v>1033</v>
-      </c>
-      <c r="K37" s="5" t="s">
-        <v>1034</v>
-      </c>
-      <c r="L37" s="5" t="s">
-        <v>1035</v>
-      </c>
-      <c r="M37" s="5" t="s">
-        <v>1036</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A38" s="11" t="s">
-        <v>713</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>714</v>
-      </c>
-      <c r="C38" s="9" t="s">
-        <v>1044</v>
-      </c>
-      <c r="D38" s="9" t="s">
+      <c r="J38" s="5" t="s">
+        <v>718</v>
+      </c>
+      <c r="K38" s="5" t="s">
+        <v>719</v>
+      </c>
+      <c r="L38" s="5" t="s">
+        <v>720</v>
+      </c>
+      <c r="M38" s="5" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A39" s="11" t="s">
+        <v>742</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>743</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>1043</v>
+      </c>
+      <c r="D39" s="9" t="s">
         <v>1086</v>
       </c>
-      <c r="E38" s="6" t="s">
-        <v>715</v>
-      </c>
-      <c r="F38" s="5" t="s">
-        <v>716</v>
-      </c>
-      <c r="G38" s="5" t="s">
-        <v>717</v>
-      </c>
-      <c r="H38" s="5" t="s">
-        <v>718</v>
-      </c>
-      <c r="I38" s="9" t="s">
+      <c r="E39" s="6" t="s">
+        <v>744</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>745</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>746</v>
+      </c>
+      <c r="H39" s="5" t="s">
+        <v>747</v>
+      </c>
+      <c r="I39" s="9" t="s">
         <v>1086</v>
       </c>
-      <c r="J38" s="5" t="s">
-        <v>719</v>
-      </c>
-      <c r="K38" s="5" t="s">
-        <v>720</v>
-      </c>
-      <c r="L38" s="5" t="s">
-        <v>721</v>
-      </c>
-      <c r="M38" s="5" t="s">
+      <c r="J39" s="5" t="s">
+        <v>748</v>
+      </c>
+      <c r="K39" s="5" t="s">
+        <v>749</v>
+      </c>
+      <c r="L39" s="5" t="s">
+        <v>750</v>
+      </c>
+      <c r="M39" s="5" t="s">
+        <v>751</v>
+      </c>
+      <c r="N39" s="5" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A40" s="11" t="s">
+        <v>754</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>755</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>1043</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>1087</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>756</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>757</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>758</v>
+      </c>
+      <c r="H40" s="5" t="s">
+        <v>759</v>
+      </c>
+      <c r="I40" s="9" t="s">
+        <v>1087</v>
+      </c>
+      <c r="J40" s="5" t="s">
+        <v>760</v>
+      </c>
+      <c r="K40" s="5" t="s">
+        <v>761</v>
+      </c>
+      <c r="L40" s="5" t="s">
+        <v>762</v>
+      </c>
+      <c r="M40" s="5" t="s">
+        <v>763</v>
+      </c>
+      <c r="N40" s="5"/>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A41" s="11" t="s">
         <v>722</v>
       </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A39" s="11" t="s">
-        <v>743</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>744</v>
-      </c>
-      <c r="C39" s="9" t="s">
-        <v>1044</v>
-      </c>
-      <c r="D39" s="9" t="s">
-        <v>1087</v>
-      </c>
-      <c r="E39" s="6" t="s">
-        <v>745</v>
-      </c>
-      <c r="F39" s="5" t="s">
-        <v>746</v>
-      </c>
-      <c r="G39" s="5" t="s">
-        <v>747</v>
-      </c>
-      <c r="H39" s="5" t="s">
-        <v>748</v>
-      </c>
-      <c r="I39" s="9" t="s">
-        <v>1087</v>
-      </c>
-      <c r="J39" s="5" t="s">
-        <v>749</v>
-      </c>
-      <c r="K39" s="5" t="s">
-        <v>750</v>
-      </c>
-      <c r="L39" s="5" t="s">
-        <v>751</v>
-      </c>
-      <c r="M39" s="5" t="s">
-        <v>752</v>
-      </c>
-      <c r="N39" s="5" t="s">
-        <v>754</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A40" s="11" t="s">
-        <v>755</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>756</v>
-      </c>
-      <c r="C40" s="9" t="s">
-        <v>1044</v>
-      </c>
-      <c r="D40" s="9" t="s">
+      <c r="B41" s="5" t="s">
+        <v>723</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>1043</v>
+      </c>
+      <c r="D41" s="9" t="s">
         <v>1088</v>
       </c>
-      <c r="E40" s="6" t="s">
-        <v>757</v>
-      </c>
-      <c r="F40" s="5" t="s">
-        <v>758</v>
-      </c>
-      <c r="G40" s="5" t="s">
-        <v>759</v>
-      </c>
-      <c r="H40" s="5" t="s">
-        <v>760</v>
-      </c>
-      <c r="I40" s="9" t="s">
+      <c r="E41" s="6" t="s">
+        <v>724</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>725</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>726</v>
+      </c>
+      <c r="H41" s="5" t="s">
+        <v>727</v>
+      </c>
+      <c r="I41" s="9" t="s">
         <v>1088</v>
       </c>
-      <c r="J40" s="5" t="s">
-        <v>761</v>
-      </c>
-      <c r="K40" s="5" t="s">
-        <v>762</v>
-      </c>
-      <c r="L40" s="5" t="s">
-        <v>763</v>
-      </c>
-      <c r="M40" s="5" t="s">
-        <v>764</v>
-      </c>
-      <c r="N40" s="5"/>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A41" s="11" t="s">
-        <v>723</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>724</v>
-      </c>
-      <c r="C41" s="9" t="s">
-        <v>1044</v>
-      </c>
-      <c r="D41" s="9" t="s">
+      <c r="J41" s="5" t="s">
+        <v>728</v>
+      </c>
+      <c r="K41" s="5" t="s">
+        <v>729</v>
+      </c>
+      <c r="L41" s="5" t="s">
+        <v>730</v>
+      </c>
+      <c r="M41" s="5" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A42" s="11" t="s">
+        <v>732</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>733</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>1043</v>
+      </c>
+      <c r="D42" s="9" t="s">
         <v>1089</v>
       </c>
-      <c r="E41" s="6" t="s">
-        <v>725</v>
-      </c>
-      <c r="F41" s="5" t="s">
-        <v>726</v>
-      </c>
-      <c r="G41" s="5" t="s">
-        <v>727</v>
-      </c>
-      <c r="H41" s="5" t="s">
-        <v>728</v>
-      </c>
-      <c r="I41" s="9" t="s">
+      <c r="E42" s="6" t="s">
+        <v>734</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>735</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>736</v>
+      </c>
+      <c r="H42" s="5" t="s">
+        <v>737</v>
+      </c>
+      <c r="I42" s="9" t="s">
         <v>1089</v>
       </c>
-      <c r="J41" s="5" t="s">
-        <v>729</v>
-      </c>
-      <c r="K41" s="5" t="s">
-        <v>730</v>
-      </c>
-      <c r="L41" s="5" t="s">
-        <v>731</v>
-      </c>
-      <c r="M41" s="5" t="s">
-        <v>732</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A42" s="11" t="s">
-        <v>733</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>734</v>
-      </c>
-      <c r="C42" s="9" t="s">
-        <v>1044</v>
-      </c>
-      <c r="D42" s="9" t="s">
-        <v>1090</v>
-      </c>
-      <c r="E42" s="6" t="s">
-        <v>735</v>
-      </c>
-      <c r="F42" s="5" t="s">
-        <v>736</v>
-      </c>
-      <c r="G42" s="5" t="s">
-        <v>737</v>
-      </c>
-      <c r="H42" s="5" t="s">
+      <c r="J42" s="5" t="s">
         <v>738</v>
       </c>
-      <c r="I42" s="9" t="s">
-        <v>1090</v>
-      </c>
-      <c r="J42" s="5" t="s">
+      <c r="K42" s="5" t="s">
         <v>739</v>
       </c>
-      <c r="K42" s="5" t="s">
+      <c r="L42" s="5" t="s">
         <v>740</v>
       </c>
-      <c r="L42" s="5" t="s">
+      <c r="M42" s="5" t="s">
         <v>741</v>
-      </c>
-      <c r="M42" s="5" t="s">
-        <v>742</v>
       </c>
     </row>
   </sheetData>
@@ -6218,31 +6218,31 @@
   <sheetPr codeName="FXRates_Fields"/>
   <dimension ref="A1:P36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I32" sqref="I32"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="66.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="44.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="43.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="61.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="45.88671875" customWidth="1"/>
-    <col min="11" max="11" width="40.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="40.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="66.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="61.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="45.85546875" customWidth="1"/>
+    <col min="11" max="11" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -6250,7 +6250,7 @@
         <v>17</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>1</v>
@@ -6289,10 +6289,10 @@
         <v>121</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>1037</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+        <v>1036</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -6300,10 +6300,10 @@
         <v>44</v>
       </c>
       <c r="C2" s="9" t="s">
+        <v>1045</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>1046</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>1047</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>131</v>
@@ -6318,7 +6318,7 @@
         <v>48</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>129</v>
@@ -6339,7 +6339,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>22</v>
       </c>
@@ -6363,7 +6363,7 @@
         <v>74</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="J3" s="5" t="s">
         <v>75</v>
@@ -6384,7 +6384,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>36</v>
       </c>
@@ -6408,7 +6408,7 @@
         <v>85</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="J4" s="5" t="s">
         <v>81</v>
@@ -6429,7 +6429,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>43</v>
       </c>
@@ -6453,7 +6453,7 @@
         <v>86</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="J5" s="5" t="s">
         <v>82</v>
@@ -6474,7 +6474,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>49</v>
       </c>
@@ -6498,7 +6498,7 @@
         <v>91</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="J6" s="5" t="s">
         <v>92</v>
@@ -6519,7 +6519,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>57</v>
       </c>
@@ -6543,7 +6543,7 @@
         <v>126</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="J7" s="5" t="s">
         <v>127</v>
@@ -6564,7 +6564,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>64</v>
       </c>
@@ -6576,7 +6576,7 @@
         <v>130</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>259</v>
@@ -6588,7 +6588,7 @@
         <v>261</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="J8" s="5" t="s">
         <v>262</v>
@@ -6609,7 +6609,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>96</v>
       </c>
@@ -6621,7 +6621,7 @@
         <v>130</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>267</v>
@@ -6633,7 +6633,7 @@
         <v>269</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="J9" s="5" t="s">
         <v>270</v>
@@ -6654,7 +6654,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>103</v>
       </c>
@@ -6666,7 +6666,7 @@
         <v>130</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>275</v>
@@ -6678,7 +6678,7 @@
         <v>277</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="J10" s="5" t="s">
         <v>278</v>
@@ -6699,7 +6699,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>111</v>
       </c>
@@ -6711,7 +6711,7 @@
         <v>130</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>283</v>
@@ -6744,7 +6744,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>113</v>
       </c>
@@ -6756,7 +6756,7 @@
         <v>130</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>291</v>
@@ -6789,7 +6789,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>115</v>
       </c>
@@ -6801,7 +6801,7 @@
         <v>130</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>299</v>
@@ -6834,7 +6834,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>117</v>
       </c>
@@ -6846,7 +6846,7 @@
         <v>130</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>307</v>
@@ -6879,7 +6879,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>119</v>
       </c>
@@ -6924,7 +6924,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>145</v>
       </c>
@@ -6969,7 +6969,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>332</v>
       </c>
@@ -6977,10 +6977,10 @@
         <v>333</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>334</v>
@@ -6995,7 +6995,7 @@
         <v>337</v>
       </c>
       <c r="I17" s="9" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="J17" s="5" t="s">
         <v>338</v>
@@ -7016,16 +7016,18 @@
         <v>242</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>342</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>343</v>
       </c>
-      <c r="C18" s="5"/>
+      <c r="C18" s="9" t="s">
+        <v>1045</v>
+      </c>
       <c r="D18" s="9" t="s">
-        <v>130</v>
+        <v>1132</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>344</v>
@@ -7040,7 +7042,7 @@
         <v>347</v>
       </c>
       <c r="I18" s="9" t="s">
-        <v>644</v>
+        <v>1132</v>
       </c>
       <c r="J18" s="5" t="s">
         <v>348</v>
@@ -7061,7 +7063,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>352</v>
       </c>
@@ -7085,7 +7087,7 @@
         <v>357</v>
       </c>
       <c r="I19" s="9" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="J19" s="5" t="s">
         <v>358</v>
@@ -7106,7 +7108,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>168</v>
       </c>
@@ -7151,10 +7153,10 @@
         <v>242</v>
       </c>
       <c r="P20" s="5" t="s">
-        <v>1038</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+        <v>1037</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>209</v>
       </c>
@@ -7199,7 +7201,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>229</v>
       </c>
@@ -7244,7 +7246,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>231</v>
       </c>
@@ -7289,7 +7291,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>398</v>
       </c>
@@ -7334,7 +7336,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>408</v>
       </c>
@@ -7379,7 +7381,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="26" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>418</v>
       </c>
@@ -7424,7 +7426,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="27" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>427</v>
       </c>
@@ -7469,7 +7471,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>437</v>
       </c>
@@ -7514,7 +7516,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>447</v>
       </c>
@@ -7559,7 +7561,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>457</v>
       </c>
@@ -7604,7 +7606,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="31" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>467</v>
       </c>
@@ -7649,7 +7651,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="32" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>579</v>
       </c>
@@ -7657,13 +7659,13 @@
         <v>580</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>581</v>
@@ -7675,7 +7677,7 @@
         <v>583</v>
       </c>
       <c r="I32" s="9" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="J32" s="5" t="s">
         <v>584</v>
@@ -7696,7 +7698,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
         <v>588</v>
       </c>
@@ -7704,13 +7706,13 @@
         <v>589</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="F33" s="5" t="s">
         <v>590</v>
@@ -7722,7 +7724,7 @@
         <v>592</v>
       </c>
       <c r="I33" s="9" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="J33" s="5" t="s">
         <v>593</v>
@@ -7743,7 +7745,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>597</v>
       </c>
@@ -7751,13 +7753,13 @@
         <v>598</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="F34" s="5" t="s">
         <v>599</v>
@@ -7769,7 +7771,7 @@
         <v>601</v>
       </c>
       <c r="I34" s="9" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="J34" s="5" t="s">
         <v>602</v>
@@ -7790,7 +7792,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>606</v>
       </c>
@@ -7802,7 +7804,7 @@
         <v>130</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="F35" s="5" t="s">
         <v>608</v>
@@ -7835,7 +7837,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
         <v>615</v>
       </c>
@@ -7847,7 +7849,7 @@
         <v>130</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="F36" s="5" t="s">
         <v>617</v>
@@ -7904,6 +7906,9 @@
     <hyperlink ref="D32" r:id="rId20" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{7FAB28EE-139E-4DE6-8707-4F3F7499621E}"/>
     <hyperlink ref="C32" r:id="rId21" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{0E12DF56-B2CA-4E41-9C06-A1D39031AB16}"/>
     <hyperlink ref="I32" r:id="rId22" display="\\DataSet\\TL_DataSet\\FxRates_GSFile\\" xr:uid="{CF580B19-5CF8-4F35-98BE-09114339AF39}"/>
+    <hyperlink ref="C18" r:id="rId23" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{87A78F77-1B98-4252-BED6-FB3DE690FC0D}"/>
+    <hyperlink ref="D18" r:id="rId24" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{C8D735C2-31EA-44C8-BB32-E6A25A2B0C6E}"/>
+    <hyperlink ref="I18" r:id="rId25" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{115AD9D0-C985-4A6D-9C3D-7EC98FC8A6E4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7920,24 +7925,24 @@
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="63.5546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.5703125" style="1" customWidth="1"/>
     <col min="4" max="4" width="94" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="42.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="36.33203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="75.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="37.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="42.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="36.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="75.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="37.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="40" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="60.33203125" customWidth="1"/>
+    <col min="12" max="12" width="60.28515625" customWidth="1"/>
     <col min="13" max="13" width="45" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -7978,7 +7983,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -7986,10 +7991,10 @@
         <v>139</v>
       </c>
       <c r="C2" s="9" t="s">
+        <v>1047</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>1048</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>1049</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>142</v>
@@ -8001,7 +8006,7 @@
         <v>144</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>165</v>
@@ -8016,7 +8021,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>22</v>
       </c>
@@ -8024,10 +8029,10 @@
         <v>479</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>480</v>
@@ -8039,10 +8044,10 @@
         <v>482</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="J3" s="5" t="s">
         <v>483</v>
@@ -8057,253 +8062,253 @@
         <v>485</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>36</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>830</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>1105</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>838</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>831</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>1106</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>839</v>
-      </c>
-      <c r="E4" s="5" t="s">
+      <c r="F4" s="5" t="s">
         <v>832</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="G4" s="5" t="s">
         <v>833</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="H4" s="5" t="s">
         <v>834</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="I4" s="9" t="s">
+        <v>1105</v>
+      </c>
+      <c r="J4" s="5" t="s">
         <v>835</v>
       </c>
-      <c r="I4" s="9" t="s">
-        <v>1106</v>
-      </c>
-      <c r="J4" s="5" t="s">
+      <c r="K4" s="5" t="s">
         <v>836</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="L4" s="5" t="s">
         <v>837</v>
       </c>
-      <c r="L4" s="5" t="s">
-        <v>838</v>
-      </c>
       <c r="M4" s="5" t="s">
-        <v>838</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>43</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>839</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>1106</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>847</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>840</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>1107</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>848</v>
-      </c>
-      <c r="E5" s="5" t="s">
+      <c r="F5" s="5" t="s">
         <v>841</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="G5" s="5" t="s">
         <v>842</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="H5" s="5" t="s">
         <v>843</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="I5" s="9" t="s">
+        <v>1106</v>
+      </c>
+      <c r="J5" s="5" t="s">
         <v>844</v>
       </c>
-      <c r="I5" s="9" t="s">
-        <v>1107</v>
-      </c>
-      <c r="J5" s="5" t="s">
+      <c r="K5" s="5" t="s">
         <v>845</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="L5" s="5" t="s">
         <v>846</v>
       </c>
-      <c r="L5" s="5" t="s">
-        <v>847</v>
-      </c>
       <c r="M5" s="5" t="s">
-        <v>847</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>64</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>782</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>1107</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>783</v>
       </c>
-      <c r="C6" s="9" t="s">
-        <v>1108</v>
-      </c>
-      <c r="D6" s="6" t="s">
+      <c r="E6" s="5" t="s">
         <v>784</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="F6" s="5" t="s">
         <v>785</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="G6" s="5" t="s">
         <v>786</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="H6" s="5" t="s">
         <v>787</v>
       </c>
-      <c r="H6" s="5" t="s">
-        <v>788</v>
-      </c>
       <c r="I6" s="9" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="J6" s="5" t="s">
+        <v>790</v>
+      </c>
+      <c r="K6" s="5" t="s">
         <v>791</v>
       </c>
-      <c r="K6" s="5" t="s">
+      <c r="L6" s="5" t="s">
         <v>792</v>
       </c>
-      <c r="L6" s="5" t="s">
-        <v>793</v>
-      </c>
       <c r="M6" s="5" t="s">
-        <v>793</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>96</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>767</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>1049</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>1050</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>768</v>
       </c>
-      <c r="C7" s="9" t="s">
-        <v>1050</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>1051</v>
-      </c>
-      <c r="E7" s="5" t="s">
+      <c r="F7" s="5" t="s">
         <v>769</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="G7" s="5" t="s">
         <v>770</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="H7" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>1049</v>
+      </c>
+      <c r="J7" s="5" t="s">
         <v>771</v>
       </c>
-      <c r="H7" s="5" t="s">
-        <v>789</v>
-      </c>
-      <c r="I7" s="9" t="s">
-        <v>1050</v>
-      </c>
-      <c r="J7" s="5" t="s">
+      <c r="K7" s="5" t="s">
         <v>772</v>
       </c>
-      <c r="K7" s="5" t="s">
-        <v>773</v>
-      </c>
       <c r="L7" s="5" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="M7" s="5" t="s">
-        <v>781</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>103</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>773</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>1094</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>1095</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>774</v>
       </c>
-      <c r="C8" s="9" t="s">
-        <v>1095</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>1096</v>
-      </c>
-      <c r="E8" s="5" t="s">
+      <c r="F8" s="5" t="s">
         <v>775</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="G8" s="5" t="s">
         <v>776</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="H8" s="5" t="s">
+        <v>789</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>1094</v>
+      </c>
+      <c r="J8" s="5" t="s">
         <v>777</v>
       </c>
-      <c r="H8" s="5" t="s">
-        <v>790</v>
-      </c>
-      <c r="I8" s="9" t="s">
-        <v>1095</v>
-      </c>
-      <c r="J8" s="5" t="s">
+      <c r="K8" s="5" t="s">
         <v>778</v>
-      </c>
-      <c r="K8" s="5" t="s">
-        <v>779</v>
       </c>
       <c r="L8" s="5" t="s">
         <v>485</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>780</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>111</v>
       </c>
       <c r="B9" s="5" t="s">
+        <v>794</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>1108</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>795</v>
       </c>
-      <c r="C9" s="9" t="s">
-        <v>1109</v>
-      </c>
-      <c r="D9" s="6" t="s">
+      <c r="E9" s="5" t="s">
         <v>796</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="F9" s="5" t="s">
         <v>797</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="G9" s="5" t="s">
         <v>798</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="H9" s="5" t="s">
         <v>799</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="I9" s="9" t="s">
+        <v>1108</v>
+      </c>
+      <c r="J9" s="5" t="s">
         <v>800</v>
       </c>
-      <c r="I9" s="9" t="s">
-        <v>1109</v>
-      </c>
-      <c r="J9" s="5" t="s">
+      <c r="K9" s="5" t="s">
         <v>801</v>
       </c>
-      <c r="K9" s="5" t="s">
+      <c r="L9" s="5" t="s">
         <v>802</v>
       </c>
-      <c r="L9" s="5" t="s">
-        <v>803</v>
-      </c>
       <c r="M9" s="5" t="s">
-        <v>803</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>113</v>
       </c>
@@ -8311,10 +8316,10 @@
         <v>486</v>
       </c>
       <c r="C10" s="9" t="s">
+        <v>1090</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>1091</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>1092</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>487</v>
@@ -8326,10 +8331,10 @@
         <v>489</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="J10" s="5" t="s">
         <v>490</v>
@@ -8344,130 +8349,130 @@
         <v>492</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>115</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>964</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>1109</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>965</v>
       </c>
-      <c r="C11" s="9" t="s">
-        <v>1110</v>
-      </c>
-      <c r="D11" s="6" t="s">
+      <c r="E11" s="5" t="s">
         <v>966</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="F11" s="5" t="s">
         <v>967</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="G11" s="5" t="s">
         <v>968</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="H11" s="5" t="s">
         <v>969</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="I11" s="9" t="s">
+        <v>1109</v>
+      </c>
+      <c r="J11" s="5" t="s">
         <v>970</v>
       </c>
-      <c r="I11" s="9" t="s">
-        <v>1110</v>
-      </c>
-      <c r="J11" s="5" t="s">
+      <c r="K11" s="5" t="s">
         <v>971</v>
       </c>
-      <c r="K11" s="5" t="s">
+      <c r="L11" s="5" t="s">
         <v>972</v>
       </c>
-      <c r="L11" s="5" t="s">
-        <v>973</v>
-      </c>
       <c r="M11" s="5" t="s">
-        <v>973</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>117</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>973</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>1110</v>
+      </c>
+      <c r="D12" s="6" t="s">
         <v>974</v>
       </c>
-      <c r="C12" s="9" t="s">
-        <v>1111</v>
-      </c>
-      <c r="D12" s="6" t="s">
+      <c r="E12" s="5" t="s">
         <v>975</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="F12" s="5" t="s">
         <v>976</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="G12" s="5" t="s">
         <v>977</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="H12" s="5" t="s">
         <v>978</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="I12" s="9" t="s">
+        <v>1110</v>
+      </c>
+      <c r="J12" s="5" t="s">
         <v>979</v>
       </c>
-      <c r="I12" s="9" t="s">
-        <v>1111</v>
-      </c>
-      <c r="J12" s="5" t="s">
+      <c r="K12" s="5" t="s">
         <v>980</v>
       </c>
-      <c r="K12" s="5" t="s">
+      <c r="L12" s="5" t="s">
         <v>981</v>
       </c>
-      <c r="L12" s="5" t="s">
-        <v>982</v>
-      </c>
       <c r="M12" s="5" t="s">
-        <v>982</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>119</v>
       </c>
       <c r="B13" s="5" t="s">
+        <v>857</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>1111</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>858</v>
       </c>
-      <c r="C13" s="9" t="s">
-        <v>1112</v>
-      </c>
-      <c r="D13" s="6" t="s">
+      <c r="E13" s="5" t="s">
         <v>859</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="F13" s="5" t="s">
         <v>860</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="G13" s="5" t="s">
         <v>861</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="H13" s="5" t="s">
         <v>862</v>
       </c>
-      <c r="H13" s="5" t="s">
+      <c r="I13" s="9" t="s">
+        <v>1111</v>
+      </c>
+      <c r="J13" s="5" t="s">
         <v>863</v>
       </c>
-      <c r="I13" s="9" t="s">
-        <v>1112</v>
-      </c>
-      <c r="J13" s="5" t="s">
+      <c r="K13" s="5" t="s">
         <v>864</v>
       </c>
-      <c r="K13" s="5" t="s">
+      <c r="L13" s="5" t="s">
         <v>865</v>
       </c>
-      <c r="L13" s="5" t="s">
-        <v>866</v>
-      </c>
       <c r="M13" s="5" t="s">
-        <v>866</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>145</v>
       </c>
@@ -8475,10 +8480,10 @@
         <v>493</v>
       </c>
       <c r="C14" s="9" t="s">
+        <v>1092</v>
+      </c>
+      <c r="D14" s="6" t="s">
         <v>1093</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>1094</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>494</v>
@@ -8491,7 +8496,7 @@
       </c>
       <c r="H14" s="5"/>
       <c r="I14" s="9" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="J14" s="5" t="s">
         <v>497</v>
@@ -8506,7 +8511,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>500</v>
       </c>
@@ -8514,10 +8519,10 @@
         <v>501</v>
       </c>
       <c r="C15" s="9" t="s">
+        <v>1096</v>
+      </c>
+      <c r="D15" s="6" t="s">
         <v>1097</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>1098</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>502</v>
@@ -8530,7 +8535,7 @@
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="9" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="J15" s="5" t="s">
         <v>505</v>
@@ -8545,7 +8550,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>508</v>
       </c>
@@ -8553,10 +8558,10 @@
         <v>509</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>510</v>
@@ -8569,7 +8574,7 @@
       </c>
       <c r="H16" s="5"/>
       <c r="I16" s="9" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="J16" s="5" t="s">
         <v>513</v>
@@ -8584,7 +8589,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>17</v>
       </c>
@@ -8592,10 +8597,10 @@
         <v>516</v>
       </c>
       <c r="C17" s="9" t="s">
+        <v>1099</v>
+      </c>
+      <c r="D17" s="6" t="s">
         <v>1100</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>1101</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>517</v>
@@ -8610,7 +8615,7 @@
         <v>520</v>
       </c>
       <c r="I17" s="9" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="J17" s="5" t="s">
         <v>521</v>
@@ -8625,7 +8630,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>18</v>
       </c>
@@ -8633,10 +8638,10 @@
         <v>524</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>525</v>
@@ -8649,7 +8654,7 @@
       </c>
       <c r="H18" s="5"/>
       <c r="I18" s="9" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="J18" s="5" t="s">
         <v>528</v>
@@ -8664,7 +8669,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>19</v>
       </c>
@@ -8672,10 +8677,10 @@
         <v>531</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>532</v>
@@ -8688,7 +8693,7 @@
       </c>
       <c r="H19" s="5"/>
       <c r="I19" s="9" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="J19" s="5" t="s">
         <v>535</v>
@@ -8703,46 +8708,46 @@
         <v>537</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>209</v>
       </c>
       <c r="B20" s="5" t="s">
+        <v>671</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>1103</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>764</v>
+      </c>
+      <c r="E20" s="5" t="s">
         <v>672</v>
       </c>
-      <c r="C20" s="9" t="s">
-        <v>1104</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>765</v>
-      </c>
-      <c r="E20" s="5" t="s">
+      <c r="F20" s="5" t="s">
         <v>673</v>
       </c>
-      <c r="F20" s="5" t="s">
+      <c r="G20" s="5" t="s">
         <v>674</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>675</v>
       </c>
       <c r="H20" s="5"/>
       <c r="I20" s="9" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="J20" s="5" t="s">
+        <v>675</v>
+      </c>
+      <c r="K20" s="5" t="s">
         <v>676</v>
       </c>
-      <c r="K20" s="5" t="s">
+      <c r="L20" s="5" t="s">
         <v>677</v>
       </c>
-      <c r="L20" s="5" t="s">
-        <v>678</v>
-      </c>
       <c r="M20" s="5" t="s">
-        <v>678</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>229</v>
       </c>
@@ -8750,10 +8755,10 @@
         <v>572</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>573</v>
@@ -8766,7 +8771,7 @@
       </c>
       <c r="H21" s="5"/>
       <c r="I21" s="9" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="J21" s="5" t="s">
         <v>576</v>
@@ -8781,417 +8786,417 @@
         <v>578</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>418</v>
       </c>
       <c r="B22" s="5" t="s">
+        <v>1000</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>1113</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>1126</v>
+      </c>
+      <c r="E22" s="5" t="s">
         <v>1001</v>
       </c>
-      <c r="C22" s="9" t="s">
-        <v>1114</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>1127</v>
-      </c>
-      <c r="E22" s="5" t="s">
+      <c r="F22" s="5" t="s">
         <v>1002</v>
       </c>
-      <c r="F22" s="5" t="s">
+      <c r="G22" s="5" t="s">
         <v>1003</v>
       </c>
-      <c r="G22" s="5" t="s">
+      <c r="H22" s="5" t="s">
         <v>1004</v>
       </c>
-      <c r="H22" s="5" t="s">
+      <c r="I22" s="9" t="s">
+        <v>1113</v>
+      </c>
+      <c r="J22" s="5" t="s">
         <v>1005</v>
       </c>
-      <c r="I22" s="9" t="s">
-        <v>1114</v>
-      </c>
-      <c r="J22" s="5" t="s">
+      <c r="K22" s="5" t="s">
         <v>1006</v>
       </c>
-      <c r="K22" s="5" t="s">
+      <c r="L22" s="5" t="s">
         <v>1007</v>
       </c>
-      <c r="L22" s="5" t="s">
-        <v>1008</v>
-      </c>
       <c r="M22" s="5" t="s">
-        <v>1008</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>427</v>
       </c>
       <c r="B23" s="5" t="s">
+        <v>804</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>1114</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>1038</v>
+      </c>
+      <c r="E23" s="5" t="s">
         <v>805</v>
       </c>
-      <c r="C23" s="9" t="s">
-        <v>1115</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>1039</v>
-      </c>
-      <c r="E23" s="5" t="s">
+      <c r="F23" s="5" t="s">
         <v>806</v>
       </c>
-      <c r="F23" s="5" t="s">
+      <c r="G23" s="5" t="s">
         <v>807</v>
       </c>
-      <c r="G23" s="5" t="s">
+      <c r="H23" s="5" t="s">
         <v>808</v>
       </c>
-      <c r="H23" s="5" t="s">
+      <c r="I23" s="9" t="s">
+        <v>1114</v>
+      </c>
+      <c r="J23" s="5" t="s">
         <v>809</v>
       </c>
-      <c r="I23" s="9" t="s">
-        <v>1115</v>
-      </c>
-      <c r="J23" s="5" t="s">
+      <c r="K23" s="5" t="s">
         <v>810</v>
       </c>
-      <c r="K23" s="5" t="s">
+      <c r="L23" s="5" t="s">
         <v>811</v>
       </c>
-      <c r="L23" s="5" t="s">
-        <v>812</v>
-      </c>
       <c r="M23" s="5" t="s">
-        <v>812</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>437</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="D24" s="6" t="s">
+        <v>814</v>
+      </c>
+      <c r="E24" s="5" t="s">
         <v>815</v>
       </c>
-      <c r="E24" s="5" t="s">
+      <c r="F24" s="5" t="s">
         <v>816</v>
       </c>
-      <c r="F24" s="5" t="s">
+      <c r="G24" s="5" t="s">
         <v>817</v>
       </c>
-      <c r="G24" s="5" t="s">
+      <c r="H24" s="5" t="s">
         <v>818</v>
       </c>
-      <c r="H24" s="5" t="s">
+      <c r="I24" s="9" t="s">
+        <v>1115</v>
+      </c>
+      <c r="J24" s="5" t="s">
         <v>819</v>
       </c>
-      <c r="I24" s="9" t="s">
-        <v>1116</v>
-      </c>
-      <c r="J24" s="5" t="s">
+      <c r="K24" s="5" t="s">
         <v>820</v>
       </c>
-      <c r="K24" s="5" t="s">
+      <c r="L24" s="5" t="s">
         <v>821</v>
       </c>
-      <c r="L24" s="5" t="s">
-        <v>822</v>
-      </c>
       <c r="M24" s="5" t="s">
-        <v>822</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>447</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="D25" s="6" t="s">
+        <v>822</v>
+      </c>
+      <c r="E25" s="5" t="s">
         <v>823</v>
       </c>
-      <c r="E25" s="5" t="s">
+      <c r="F25" s="5" t="s">
         <v>824</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="G25" s="5" t="s">
         <v>825</v>
       </c>
-      <c r="G25" s="5" t="s">
+      <c r="H25" s="5" t="s">
         <v>826</v>
       </c>
-      <c r="H25" s="5" t="s">
+      <c r="I25" s="9" t="s">
+        <v>1116</v>
+      </c>
+      <c r="J25" s="5" t="s">
         <v>827</v>
       </c>
-      <c r="I25" s="9" t="s">
-        <v>1117</v>
-      </c>
-      <c r="J25" s="5" t="s">
+      <c r="K25" s="5" t="s">
         <v>828</v>
       </c>
-      <c r="K25" s="5" t="s">
+      <c r="L25" s="5" t="s">
         <v>829</v>
       </c>
-      <c r="L25" s="5" t="s">
-        <v>830</v>
-      </c>
       <c r="M25" s="5" t="s">
-        <v>830</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>457</v>
       </c>
       <c r="B26" s="5" t="s">
+        <v>924</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>1117</v>
+      </c>
+      <c r="D26" s="6" t="s">
         <v>925</v>
       </c>
-      <c r="C26" s="9" t="s">
-        <v>1118</v>
-      </c>
-      <c r="D26" s="6" t="s">
+      <c r="E26" s="5" t="s">
         <v>926</v>
       </c>
-      <c r="E26" s="5" t="s">
+      <c r="F26" s="5" t="s">
         <v>927</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="G26" s="5" t="s">
         <v>928</v>
       </c>
-      <c r="G26" s="5" t="s">
+      <c r="H26" s="5" t="s">
         <v>929</v>
       </c>
-      <c r="H26" s="5" t="s">
+      <c r="I26" s="9" t="s">
+        <v>1117</v>
+      </c>
+      <c r="J26" s="5" t="s">
         <v>930</v>
       </c>
-      <c r="I26" s="9" t="s">
-        <v>1118</v>
-      </c>
-      <c r="J26" s="5" t="s">
+      <c r="K26" s="5" t="s">
         <v>931</v>
       </c>
-      <c r="K26" s="5" t="s">
+      <c r="L26" s="5" t="s">
         <v>932</v>
       </c>
-      <c r="L26" s="5" t="s">
-        <v>933</v>
-      </c>
       <c r="M26" s="5" t="s">
-        <v>933</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>467</v>
       </c>
       <c r="B27" s="5" t="s">
+        <v>933</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>1118</v>
+      </c>
+      <c r="D27" s="6" t="s">
         <v>934</v>
       </c>
-      <c r="C27" s="9" t="s">
-        <v>1119</v>
-      </c>
-      <c r="D27" s="6" t="s">
+      <c r="E27" s="5" t="s">
         <v>935</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="F27" s="5" t="s">
         <v>936</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="G27" s="5" t="s">
         <v>937</v>
       </c>
-      <c r="G27" s="5" t="s">
+      <c r="H27" s="5" t="s">
         <v>938</v>
       </c>
-      <c r="H27" s="5" t="s">
+      <c r="I27" s="9" t="s">
+        <v>1118</v>
+      </c>
+      <c r="J27" s="5" t="s">
         <v>939</v>
       </c>
-      <c r="I27" s="9" t="s">
-        <v>1119</v>
-      </c>
-      <c r="J27" s="5" t="s">
+      <c r="K27" s="5" t="s">
         <v>940</v>
       </c>
-      <c r="K27" s="5" t="s">
+      <c r="L27" s="5" t="s">
         <v>941</v>
       </c>
-      <c r="L27" s="5" t="s">
-        <v>942</v>
-      </c>
       <c r="M27" s="5" t="s">
-        <v>942</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>579</v>
       </c>
       <c r="B28" s="5" t="s">
+        <v>942</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>1119</v>
+      </c>
+      <c r="D28" s="6" t="s">
         <v>943</v>
       </c>
-      <c r="C28" s="9" t="s">
-        <v>1120</v>
-      </c>
-      <c r="D28" s="6" t="s">
+      <c r="E28" s="5" t="s">
         <v>944</v>
       </c>
-      <c r="E28" s="5" t="s">
+      <c r="F28" s="5" t="s">
         <v>945</v>
       </c>
-      <c r="F28" s="5" t="s">
+      <c r="G28" s="5" t="s">
         <v>946</v>
       </c>
-      <c r="G28" s="5" t="s">
+      <c r="H28" s="5" t="s">
         <v>947</v>
       </c>
-      <c r="H28" s="5" t="s">
+      <c r="I28" s="9" t="s">
+        <v>1119</v>
+      </c>
+      <c r="J28" s="5" t="s">
         <v>948</v>
       </c>
-      <c r="I28" s="9" t="s">
-        <v>1120</v>
-      </c>
-      <c r="J28" s="5" t="s">
+      <c r="K28" s="5" t="s">
         <v>949</v>
       </c>
-      <c r="K28" s="5" t="s">
+      <c r="L28" s="5" t="s">
         <v>950</v>
       </c>
-      <c r="L28" s="5" t="s">
-        <v>951</v>
-      </c>
       <c r="M28" s="5" t="s">
-        <v>951</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>588</v>
       </c>
       <c r="B29" s="5" t="s">
+        <v>982</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>1120</v>
+      </c>
+      <c r="D29" s="6" t="s">
         <v>983</v>
       </c>
-      <c r="C29" s="9" t="s">
-        <v>1121</v>
-      </c>
-      <c r="D29" s="6" t="s">
+      <c r="E29" s="5" t="s">
         <v>984</v>
       </c>
-      <c r="E29" s="5" t="s">
+      <c r="F29" s="5" t="s">
         <v>985</v>
       </c>
-      <c r="F29" s="5" t="s">
+      <c r="G29" s="5" t="s">
         <v>986</v>
       </c>
-      <c r="G29" s="5" t="s">
+      <c r="H29" s="5" t="s">
         <v>987</v>
       </c>
-      <c r="H29" s="5" t="s">
+      <c r="I29" s="9" t="s">
+        <v>1120</v>
+      </c>
+      <c r="J29" s="5" t="s">
         <v>988</v>
       </c>
-      <c r="I29" s="9" t="s">
-        <v>1121</v>
-      </c>
-      <c r="J29" s="5" t="s">
+      <c r="K29" s="5" t="s">
         <v>989</v>
       </c>
-      <c r="K29" s="5" t="s">
+      <c r="L29" s="5" t="s">
         <v>990</v>
       </c>
-      <c r="L29" s="5" t="s">
-        <v>991</v>
-      </c>
       <c r="M29" s="5" t="s">
-        <v>991</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>597</v>
       </c>
       <c r="B30" s="5" t="s">
+        <v>991</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>1121</v>
+      </c>
+      <c r="D30" s="6" t="s">
         <v>992</v>
       </c>
-      <c r="C30" s="9" t="s">
-        <v>1122</v>
-      </c>
-      <c r="D30" s="6" t="s">
+      <c r="E30" s="5" t="s">
         <v>993</v>
       </c>
-      <c r="E30" s="5" t="s">
+      <c r="F30" s="5" t="s">
         <v>994</v>
       </c>
-      <c r="F30" s="5" t="s">
+      <c r="G30" s="5" t="s">
         <v>995</v>
       </c>
-      <c r="G30" s="5" t="s">
+      <c r="H30" s="5" t="s">
         <v>996</v>
       </c>
-      <c r="H30" s="5" t="s">
+      <c r="I30" s="9" t="s">
+        <v>1121</v>
+      </c>
+      <c r="J30" s="5" t="s">
         <v>997</v>
       </c>
-      <c r="I30" s="9" t="s">
-        <v>1122</v>
-      </c>
-      <c r="J30" s="5" t="s">
+      <c r="K30" s="5" t="s">
         <v>998</v>
       </c>
-      <c r="K30" s="5" t="s">
+      <c r="L30" s="5" t="s">
         <v>999</v>
       </c>
-      <c r="L30" s="5" t="s">
-        <v>1000</v>
-      </c>
       <c r="M30" s="5" t="s">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>615</v>
       </c>
       <c r="B31" s="5" t="s">
+        <v>848</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>1122</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>856</v>
+      </c>
+      <c r="E31" s="5" t="s">
         <v>849</v>
       </c>
-      <c r="C31" s="9" t="s">
-        <v>1123</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>857</v>
-      </c>
-      <c r="E31" s="5" t="s">
+      <c r="F31" s="5" t="s">
         <v>850</v>
       </c>
-      <c r="F31" s="5" t="s">
+      <c r="G31" s="5" t="s">
         <v>851</v>
       </c>
-      <c r="G31" s="5" t="s">
+      <c r="H31" s="5" t="s">
         <v>852</v>
       </c>
-      <c r="H31" s="5" t="s">
+      <c r="I31" s="9" t="s">
+        <v>1122</v>
+      </c>
+      <c r="J31" s="5" t="s">
         <v>853</v>
       </c>
-      <c r="I31" s="9" t="s">
-        <v>1123</v>
-      </c>
-      <c r="J31" s="5" t="s">
+      <c r="K31" s="5" t="s">
         <v>854</v>
       </c>
-      <c r="K31" s="5" t="s">
+      <c r="L31" s="5" t="s">
         <v>855</v>
       </c>
-      <c r="L31" s="5" t="s">
-        <v>856</v>
-      </c>
       <c r="M31" s="5" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>538</v>
       </c>
@@ -9199,10 +9204,10 @@
         <v>539</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="E32" s="5" t="s">
         <v>540</v>
@@ -9215,7 +9220,7 @@
       </c>
       <c r="H32" s="5"/>
       <c r="I32" s="9" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="J32" s="5" t="s">
         <v>543</v>
@@ -9230,7 +9235,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>546</v>
       </c>
@@ -9238,10 +9243,10 @@
         <v>547</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="E33" s="5" t="s">
         <v>548</v>
@@ -9254,7 +9259,7 @@
       </c>
       <c r="H33" s="5"/>
       <c r="I33" s="9" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="J33" s="5" t="s">
         <v>551</v>
@@ -9295,9 +9300,9 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -9305,7 +9310,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
GDE-7260 initial fixes for tlbase41
</commit_message>
<xml_diff>
--- a/DataSet/Integration_DataSet/TL/TL_Data_Set_AU.xlsx
+++ b/DataSet/Integration_DataSet/TL/TL_Data_Set_AU.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\Integration_DataSet\TL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE4B0B44-3E58-4C02-8886-0BF612E8A493}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF84869C-E6A7-41C5-A619-97B6B6A39683}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BaseRate_Fields" sheetId="1" r:id="rId1"/>
@@ -2192,9 +2192,6 @@
   </si>
   <si>
     <t>DealName</t>
-  </si>
-  <si>
-    <t>TL_BASE_INACTIVE_PRICING_OPTION</t>
   </si>
   <si>
     <t>42</t>
@@ -3476,6 +3473,9 @@
   </si>
   <si>
     <t>\DataSet\Integration_DataSet\TL\FXRates_GSFile\AU\TL_FX_35_Files\</t>
+  </si>
+  <si>
+    <t>ATM BILAT AUD108.6M 29JUN15</t>
   </si>
 </sst>
 </file>
@@ -4428,29 +4428,29 @@
   </sheetPr>
   <dimension ref="A1:N42"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="I19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N40" sqref="N40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="65.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="53.44140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="21.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="41.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="65.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="33.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="38.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="44.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="41.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="65.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="53.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="41.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="65.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="33.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="38.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="44.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="41.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="34.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4458,7 +4458,7 @@
         <v>17</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>1</v>
@@ -4494,7 +4494,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -4502,10 +4502,10 @@
         <v>11</v>
       </c>
       <c r="C2" s="9" t="s">
+        <v>1012</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>1013</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>1014</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>94</v>
@@ -4520,7 +4520,7 @@
         <v>18</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>21</v>
@@ -4535,7 +4535,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>22</v>
       </c>
@@ -4543,10 +4543,10 @@
         <v>23</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>95</v>
@@ -4561,7 +4561,7 @@
         <v>25</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="J3" s="5" t="s">
         <v>26</v>
@@ -4576,7 +4576,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>36</v>
       </c>
@@ -4584,10 +4584,10 @@
         <v>30</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>139</v>
@@ -4602,7 +4602,7 @@
         <v>33</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="J4" s="5" t="s">
         <v>34</v>
@@ -4617,7 +4617,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>43</v>
       </c>
@@ -4625,10 +4625,10 @@
         <v>37</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>152</v>
@@ -4643,7 +4643,7 @@
         <v>40</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="J5" s="5" t="s">
         <v>41</v>
@@ -4658,7 +4658,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>49</v>
       </c>
@@ -4666,10 +4666,10 @@
         <v>50</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>51</v>
@@ -4684,7 +4684,7 @@
         <v>54</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="J6" s="5" t="s">
         <v>55</v>
@@ -4699,7 +4699,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>57</v>
       </c>
@@ -4707,13 +4707,13 @@
         <v>58</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>59</v>
@@ -4725,7 +4725,7 @@
         <v>61</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="J7" s="5" t="s">
         <v>62</v>
@@ -4740,7 +4740,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>64</v>
       </c>
@@ -4748,13 +4748,13 @@
         <v>65</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>66</v>
@@ -4766,7 +4766,7 @@
         <v>68</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="J8" s="5" t="s">
         <v>69</v>
@@ -4781,7 +4781,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>96</v>
       </c>
@@ -4789,13 +4789,13 @@
         <v>97</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>98</v>
@@ -4807,7 +4807,7 @@
         <v>100</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="J9" s="5" t="s">
         <v>101</v>
@@ -4822,7 +4822,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>103</v>
       </c>
@@ -4830,10 +4830,10 @@
         <v>104</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>105</v>
@@ -4848,7 +4848,7 @@
         <v>108</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="J10" s="5" t="s">
         <v>109</v>
@@ -4863,7 +4863,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>111</v>
       </c>
@@ -4871,10 +4871,10 @@
         <v>155</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>112</v>
@@ -4889,7 +4889,7 @@
         <v>158</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="J11" s="5" t="s">
         <v>159</v>
@@ -4904,7 +4904,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>113</v>
       </c>
@@ -4912,10 +4912,10 @@
         <v>168</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>114</v>
@@ -4930,7 +4930,7 @@
         <v>190</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="J12" s="5" t="s">
         <v>195</v>
@@ -4945,7 +4945,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>115</v>
       </c>
@@ -4953,10 +4953,10 @@
         <v>169</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>116</v>
@@ -4971,7 +4971,7 @@
         <v>191</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="J13" s="5" t="s">
         <v>196</v>
@@ -4986,7 +4986,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>117</v>
       </c>
@@ -4994,10 +4994,10 @@
         <v>170</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>118</v>
@@ -5012,7 +5012,7 @@
         <v>192</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="J14" s="5" t="s">
         <v>197</v>
@@ -5027,7 +5027,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>119</v>
       </c>
@@ -5035,10 +5035,10 @@
         <v>171</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>120</v>
@@ -5053,7 +5053,7 @@
         <v>193</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="J15" s="5" t="s">
         <v>198</v>
@@ -5068,7 +5068,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>144</v>
       </c>
@@ -5076,10 +5076,10 @@
         <v>172</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>151</v>
@@ -5094,7 +5094,7 @@
         <v>147</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="J16" s="5" t="s">
         <v>148</v>
@@ -5109,130 +5109,130 @@
         <v>183</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>331</v>
       </c>
       <c r="B17" s="5" t="s">
+        <v>838</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>1012</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>1037</v>
+      </c>
+      <c r="E17" s="5" t="s">
         <v>839</v>
       </c>
-      <c r="C17" s="9" t="s">
-        <v>1013</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>1038</v>
-      </c>
-      <c r="E17" s="5" t="s">
+      <c r="F17" s="5" t="s">
         <v>840</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="G17" s="5" t="s">
         <v>841</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="H17" s="5" t="s">
         <v>842</v>
       </c>
-      <c r="H17" s="5" t="s">
+      <c r="I17" s="9" t="s">
+        <v>1037</v>
+      </c>
+      <c r="J17" s="5" t="s">
         <v>843</v>
       </c>
-      <c r="I17" s="9" t="s">
-        <v>1038</v>
-      </c>
-      <c r="J17" s="5" t="s">
+      <c r="K17" s="5" t="s">
         <v>844</v>
       </c>
-      <c r="K17" s="5" t="s">
+      <c r="L17" s="5" t="s">
         <v>845</v>
       </c>
-      <c r="L17" s="5" t="s">
+      <c r="M17" s="5" t="s">
         <v>846</v>
       </c>
-      <c r="M17" s="5" t="s">
-        <v>847</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>341</v>
       </c>
       <c r="B18" s="5" t="s">
+        <v>977</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>1012</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>1038</v>
+      </c>
+      <c r="E18" s="5" t="s">
         <v>978</v>
       </c>
-      <c r="C18" s="9" t="s">
-        <v>1013</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>1039</v>
-      </c>
-      <c r="E18" s="5" t="s">
+      <c r="F18" s="5" t="s">
         <v>979</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="G18" s="5" t="s">
         <v>980</v>
       </c>
-      <c r="G18" s="5" t="s">
+      <c r="H18" s="5" t="s">
         <v>981</v>
       </c>
-      <c r="H18" s="5" t="s">
+      <c r="I18" s="9" t="s">
+        <v>1038</v>
+      </c>
+      <c r="J18" s="5" t="s">
         <v>982</v>
       </c>
-      <c r="I18" s="9" t="s">
-        <v>1039</v>
-      </c>
-      <c r="J18" s="5" t="s">
+      <c r="K18" s="5" t="s">
         <v>983</v>
       </c>
-      <c r="K18" s="5" t="s">
+      <c r="L18" s="5" t="s">
         <v>984</v>
       </c>
-      <c r="L18" s="5" t="s">
+      <c r="M18" s="5" t="s">
         <v>985</v>
       </c>
-      <c r="M18" s="5" t="s">
-        <v>986</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>351</v>
       </c>
       <c r="B19" s="5" t="s">
+        <v>924</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>1012</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>1039</v>
+      </c>
+      <c r="E19" s="5" t="s">
         <v>925</v>
       </c>
-      <c r="C19" s="9" t="s">
-        <v>1013</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>1040</v>
-      </c>
-      <c r="E19" s="5" t="s">
+      <c r="F19" s="5" t="s">
         <v>926</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="G19" s="5" t="s">
         <v>927</v>
       </c>
-      <c r="G19" s="5" t="s">
+      <c r="H19" s="5" t="s">
         <v>928</v>
       </c>
-      <c r="H19" s="5" t="s">
+      <c r="I19" s="9" t="s">
+        <v>1039</v>
+      </c>
+      <c r="J19" s="5" t="s">
         <v>929</v>
       </c>
-      <c r="I19" s="9" t="s">
-        <v>1040</v>
-      </c>
-      <c r="J19" s="5" t="s">
+      <c r="K19" s="5" t="s">
         <v>930</v>
       </c>
-      <c r="K19" s="5" t="s">
+      <c r="L19" s="5" t="s">
         <v>931</v>
       </c>
-      <c r="L19" s="5" t="s">
+      <c r="M19" s="5" t="s">
         <v>932</v>
       </c>
-      <c r="M19" s="5" t="s">
-        <v>933</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>167</v>
       </c>
@@ -5240,10 +5240,10 @@
         <v>173</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>205</v>
@@ -5258,7 +5258,7 @@
         <v>194</v>
       </c>
       <c r="I20" s="9" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="J20" s="5" t="s">
         <v>199</v>
@@ -5273,7 +5273,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>208</v>
       </c>
@@ -5281,10 +5281,10 @@
         <v>218</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>209</v>
@@ -5299,7 +5299,7 @@
         <v>213</v>
       </c>
       <c r="I21" s="9" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="J21" s="5" t="s">
         <v>214</v>
@@ -5314,7 +5314,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>228</v>
       </c>
@@ -5322,10 +5322,10 @@
         <v>219</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>220</v>
@@ -5340,7 +5340,7 @@
         <v>223</v>
       </c>
       <c r="I22" s="9" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="J22" s="5" t="s">
         <v>224</v>
@@ -5355,7 +5355,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>230</v>
       </c>
@@ -5363,10 +5363,10 @@
         <v>229</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>238</v>
@@ -5381,7 +5381,7 @@
         <v>233</v>
       </c>
       <c r="I23" s="9" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="J23" s="5" t="s">
         <v>234</v>
@@ -5396,7 +5396,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
         <v>426</v>
       </c>
@@ -5404,10 +5404,10 @@
         <v>553</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>554</v>
@@ -5422,7 +5422,7 @@
         <v>557</v>
       </c>
       <c r="I24" s="9" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="J24" s="5" t="s">
         <v>558</v>
@@ -5437,7 +5437,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>436</v>
       </c>
@@ -5445,10 +5445,10 @@
         <v>570</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>562</v>
@@ -5463,7 +5463,7 @@
         <v>565</v>
       </c>
       <c r="I25" s="9" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="J25" s="5" t="s">
         <v>566</v>
@@ -5478,7 +5478,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
         <v>446</v>
       </c>
@@ -5486,10 +5486,10 @@
         <v>648</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>649</v>
@@ -5504,7 +5504,7 @@
         <v>652</v>
       </c>
       <c r="I26" s="9" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="J26" s="5" t="s">
         <v>653</v>
@@ -5519,48 +5519,48 @@
         <v>656</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>456</v>
       </c>
       <c r="B27" s="5" t="s">
+        <v>986</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>1012</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>1021</v>
+      </c>
+      <c r="E27" s="5" t="s">
         <v>987</v>
       </c>
-      <c r="C27" s="9" t="s">
-        <v>1013</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>1022</v>
-      </c>
-      <c r="E27" s="5" t="s">
+      <c r="F27" s="5" t="s">
         <v>988</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="G27" s="5" t="s">
         <v>989</v>
       </c>
-      <c r="G27" s="5" t="s">
+      <c r="H27" s="5" t="s">
         <v>990</v>
       </c>
-      <c r="H27" s="5" t="s">
+      <c r="I27" s="9" t="s">
+        <v>1021</v>
+      </c>
+      <c r="J27" s="5" t="s">
         <v>991</v>
       </c>
-      <c r="I27" s="9" t="s">
-        <v>1022</v>
-      </c>
-      <c r="J27" s="5" t="s">
+      <c r="K27" s="5" t="s">
         <v>992</v>
       </c>
-      <c r="K27" s="5" t="s">
+      <c r="L27" s="5" t="s">
         <v>993</v>
       </c>
-      <c r="L27" s="5" t="s">
+      <c r="M27" s="5" t="s">
         <v>994</v>
       </c>
-      <c r="M27" s="5" t="s">
-        <v>995</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
         <v>466</v>
       </c>
@@ -5568,10 +5568,10 @@
         <v>623</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>624</v>
@@ -5586,7 +5586,7 @@
         <v>627</v>
       </c>
       <c r="I28" s="9" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="J28" s="5" t="s">
         <v>628</v>
@@ -5601,7 +5601,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
         <v>578</v>
       </c>
@@ -5609,10 +5609,10 @@
         <v>632</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="E29" s="6" t="s">
         <v>633</v>
@@ -5627,7 +5627,7 @@
         <v>636</v>
       </c>
       <c r="I29" s="9" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="J29" s="5" t="s">
         <v>637</v>
@@ -5642,7 +5642,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
         <v>596</v>
       </c>
@@ -5650,10 +5650,10 @@
         <v>665</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="E30" s="6" t="s">
         <v>679</v>
@@ -5668,7 +5668,7 @@
         <v>668</v>
       </c>
       <c r="I30" s="9" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="J30" s="5" t="s">
         <v>669</v>
@@ -5683,7 +5683,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
         <v>678</v>
       </c>
@@ -5691,10 +5691,10 @@
         <v>665</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>677</v>
@@ -5709,7 +5709,7 @@
         <v>668</v>
       </c>
       <c r="I31" s="9" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="J31" s="5" t="s">
         <v>669</v>
@@ -5724,253 +5724,253 @@
         <v>671</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>605</v>
       </c>
       <c r="B32" s="5" t="s">
+        <v>847</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>1012</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>1049</v>
+      </c>
+      <c r="E32" s="6" t="s">
         <v>848</v>
       </c>
-      <c r="C32" s="9" t="s">
-        <v>1013</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>1050</v>
-      </c>
-      <c r="E32" s="6" t="s">
+      <c r="F32" s="5" t="s">
         <v>849</v>
       </c>
-      <c r="F32" s="5" t="s">
+      <c r="G32" s="5" t="s">
         <v>850</v>
       </c>
-      <c r="G32" s="5" t="s">
+      <c r="H32" s="5" t="s">
         <v>851</v>
       </c>
-      <c r="H32" s="5" t="s">
+      <c r="I32" s="9" t="s">
+        <v>1049</v>
+      </c>
+      <c r="J32" s="5" t="s">
         <v>852</v>
       </c>
-      <c r="I32" s="9" t="s">
-        <v>1050</v>
-      </c>
-      <c r="J32" s="5" t="s">
+      <c r="K32" s="5" t="s">
         <v>853</v>
       </c>
-      <c r="K32" s="5" t="s">
+      <c r="L32" s="5" t="s">
         <v>854</v>
       </c>
-      <c r="L32" s="5" t="s">
+      <c r="M32" s="5" t="s">
         <v>855</v>
       </c>
-      <c r="M32" s="5" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
         <v>614</v>
       </c>
       <c r="B33" s="5" t="s">
+        <v>856</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>1012</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>1050</v>
+      </c>
+      <c r="E33" s="6" t="s">
         <v>857</v>
       </c>
-      <c r="C33" s="9" t="s">
-        <v>1013</v>
-      </c>
-      <c r="D33" s="9" t="s">
-        <v>1051</v>
-      </c>
-      <c r="E33" s="6" t="s">
+      <c r="F33" s="5" t="s">
         <v>858</v>
       </c>
-      <c r="F33" s="5" t="s">
+      <c r="G33" s="5" t="s">
         <v>859</v>
       </c>
-      <c r="G33" s="5" t="s">
+      <c r="H33" s="5" t="s">
         <v>860</v>
       </c>
-      <c r="H33" s="5" t="s">
+      <c r="I33" s="9" t="s">
+        <v>1050</v>
+      </c>
+      <c r="J33" s="5" t="s">
         <v>861</v>
       </c>
-      <c r="I33" s="9" t="s">
-        <v>1051</v>
-      </c>
-      <c r="J33" s="5" t="s">
+      <c r="K33" s="5" t="s">
         <v>862</v>
       </c>
-      <c r="K33" s="5" t="s">
+      <c r="L33" s="5" t="s">
         <v>863</v>
       </c>
-      <c r="L33" s="5" t="s">
+      <c r="M33" s="5" t="s">
         <v>864</v>
       </c>
-      <c r="M33" s="5" t="s">
-        <v>865</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
         <v>537</v>
       </c>
       <c r="B34" s="5" t="s">
+        <v>865</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>1012</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>1051</v>
+      </c>
+      <c r="E34" s="6" t="s">
         <v>866</v>
       </c>
-      <c r="C34" s="9" t="s">
-        <v>1013</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>1052</v>
-      </c>
-      <c r="E34" s="6" t="s">
+      <c r="F34" s="5" t="s">
         <v>867</v>
       </c>
-      <c r="F34" s="5" t="s">
+      <c r="G34" s="5" t="s">
         <v>868</v>
       </c>
-      <c r="G34" s="5" t="s">
+      <c r="H34" s="5" t="s">
         <v>869</v>
       </c>
-      <c r="H34" s="5" t="s">
+      <c r="I34" s="9" t="s">
+        <v>1051</v>
+      </c>
+      <c r="J34" s="5" t="s">
         <v>870</v>
       </c>
-      <c r="I34" s="9" t="s">
-        <v>1052</v>
-      </c>
-      <c r="J34" s="5" t="s">
+      <c r="K34" s="5" t="s">
         <v>871</v>
       </c>
-      <c r="K34" s="5" t="s">
+      <c r="L34" s="5" t="s">
         <v>872</v>
       </c>
-      <c r="L34" s="5" t="s">
+      <c r="M34" s="5" t="s">
         <v>873</v>
       </c>
-      <c r="M34" s="5" t="s">
-        <v>874</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
         <v>545</v>
       </c>
       <c r="B35" s="5" t="s">
+        <v>874</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>1012</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>1052</v>
+      </c>
+      <c r="E35" s="6" t="s">
         <v>875</v>
       </c>
-      <c r="C35" s="9" t="s">
-        <v>1013</v>
-      </c>
-      <c r="D35" s="9" t="s">
+      <c r="F35" s="5" t="s">
+        <v>876</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>877</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>878</v>
+      </c>
+      <c r="I35" s="9" t="s">
+        <v>1052</v>
+      </c>
+      <c r="J35" s="5" t="s">
+        <v>879</v>
+      </c>
+      <c r="K35" s="5" t="s">
+        <v>880</v>
+      </c>
+      <c r="L35" s="5" t="s">
+        <v>881</v>
+      </c>
+      <c r="M35" s="5" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A36" s="11" t="s">
+        <v>883</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>884</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>1012</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>1020</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>885</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>886</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>887</v>
+      </c>
+      <c r="H36" s="5" t="s">
+        <v>888</v>
+      </c>
+      <c r="I36" s="9" t="s">
+        <v>1020</v>
+      </c>
+      <c r="J36" s="5" t="s">
+        <v>889</v>
+      </c>
+      <c r="K36" s="5" t="s">
+        <v>890</v>
+      </c>
+      <c r="L36" s="5" t="s">
+        <v>891</v>
+      </c>
+      <c r="M36" s="5" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
+        <v>995</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>996</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>1012</v>
+      </c>
+      <c r="D37" s="9" t="s">
         <v>1053</v>
       </c>
-      <c r="E35" s="6" t="s">
-        <v>876</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>877</v>
-      </c>
-      <c r="G35" s="5" t="s">
-        <v>878</v>
-      </c>
-      <c r="H35" s="5" t="s">
-        <v>879</v>
-      </c>
-      <c r="I35" s="9" t="s">
+      <c r="E37" s="5" t="s">
+        <v>997</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>998</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>999</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>1000</v>
+      </c>
+      <c r="I37" s="9" t="s">
         <v>1053</v>
       </c>
-      <c r="J35" s="5" t="s">
-        <v>880</v>
-      </c>
-      <c r="K35" s="5" t="s">
-        <v>881</v>
-      </c>
-      <c r="L35" s="5" t="s">
-        <v>882</v>
-      </c>
-      <c r="M35" s="5" t="s">
-        <v>883</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A36" s="11" t="s">
-        <v>884</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>885</v>
-      </c>
-      <c r="C36" s="9" t="s">
-        <v>1013</v>
-      </c>
-      <c r="D36" s="9" t="s">
-        <v>1021</v>
-      </c>
-      <c r="E36" s="6" t="s">
-        <v>886</v>
-      </c>
-      <c r="F36" s="5" t="s">
-        <v>887</v>
-      </c>
-      <c r="G36" s="5" t="s">
-        <v>888</v>
-      </c>
-      <c r="H36" s="5" t="s">
-        <v>889</v>
-      </c>
-      <c r="I36" s="9" t="s">
-        <v>1021</v>
-      </c>
-      <c r="J36" s="5" t="s">
-        <v>890</v>
-      </c>
-      <c r="K36" s="5" t="s">
-        <v>891</v>
-      </c>
-      <c r="L36" s="5" t="s">
-        <v>892</v>
-      </c>
-      <c r="M36" s="5" t="s">
-        <v>893</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A37" s="5" t="s">
-        <v>996</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>997</v>
-      </c>
-      <c r="C37" s="9" t="s">
-        <v>1013</v>
-      </c>
-      <c r="D37" s="9" t="s">
-        <v>1054</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>998</v>
-      </c>
-      <c r="F37" s="5" t="s">
-        <v>999</v>
-      </c>
-      <c r="G37" s="5" t="s">
-        <v>1000</v>
-      </c>
-      <c r="H37" s="5" t="s">
+      <c r="J37" s="5" t="s">
         <v>1001</v>
       </c>
-      <c r="I37" s="9" t="s">
-        <v>1054</v>
-      </c>
-      <c r="J37" s="5" t="s">
+      <c r="K37" s="5" t="s">
         <v>1002</v>
       </c>
-      <c r="K37" s="5" t="s">
+      <c r="L37" s="5" t="s">
         <v>1003</v>
       </c>
-      <c r="L37" s="5" t="s">
+      <c r="M37" s="5" t="s">
         <v>1004</v>
       </c>
-      <c r="M37" s="5" t="s">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
         <v>682</v>
       </c>
@@ -5978,10 +5978,10 @@
         <v>683</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="E38" s="6" t="s">
         <v>684</v>
@@ -5996,7 +5996,7 @@
         <v>687</v>
       </c>
       <c r="I38" s="9" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="J38" s="5" t="s">
         <v>688</v>
@@ -6011,7 +6011,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
         <v>712</v>
       </c>
@@ -6019,10 +6019,10 @@
         <v>713</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="E39" s="6" t="s">
         <v>714</v>
@@ -6037,7 +6037,7 @@
         <v>717</v>
       </c>
       <c r="I39" s="9" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="J39" s="5" t="s">
         <v>718</v>
@@ -6052,52 +6052,52 @@
         <v>721</v>
       </c>
       <c r="N39" s="5" t="s">
+        <v>1131</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A40" s="11" t="s">
         <v>723</v>
       </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A40" s="11" t="s">
+      <c r="B40" s="5" t="s">
         <v>724</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="C40" s="9" t="s">
+        <v>1012</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>1056</v>
+      </c>
+      <c r="E40" s="6" t="s">
         <v>725</v>
       </c>
-      <c r="C40" s="9" t="s">
-        <v>1013</v>
-      </c>
-      <c r="D40" s="9" t="s">
-        <v>1057</v>
-      </c>
-      <c r="E40" s="6" t="s">
+      <c r="F40" s="5" t="s">
         <v>726</v>
       </c>
-      <c r="F40" s="5" t="s">
+      <c r="G40" s="5" t="s">
         <v>727</v>
       </c>
-      <c r="G40" s="5" t="s">
+      <c r="H40" s="5" t="s">
         <v>728</v>
       </c>
-      <c r="H40" s="5" t="s">
+      <c r="I40" s="9" t="s">
+        <v>1056</v>
+      </c>
+      <c r="J40" s="5" t="s">
         <v>729</v>
       </c>
-      <c r="I40" s="9" t="s">
-        <v>1057</v>
-      </c>
-      <c r="J40" s="5" t="s">
+      <c r="K40" s="5" t="s">
         <v>730</v>
       </c>
-      <c r="K40" s="5" t="s">
+      <c r="L40" s="5" t="s">
         <v>731</v>
       </c>
-      <c r="L40" s="5" t="s">
+      <c r="M40" s="5" t="s">
         <v>732</v>
       </c>
-      <c r="M40" s="5" t="s">
-        <v>733</v>
-      </c>
       <c r="N40" s="5"/>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="11" t="s">
         <v>692</v>
       </c>
@@ -6105,10 +6105,10 @@
         <v>693</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="E41" s="6" t="s">
         <v>694</v>
@@ -6123,7 +6123,7 @@
         <v>697</v>
       </c>
       <c r="I41" s="9" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="J41" s="5" t="s">
         <v>698</v>
@@ -6138,7 +6138,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
         <v>702</v>
       </c>
@@ -6146,10 +6146,10 @@
         <v>703</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="E42" s="6" t="s">
         <v>704</v>
@@ -6164,7 +6164,7 @@
         <v>707</v>
       </c>
       <c r="I42" s="9" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="J42" s="5" t="s">
         <v>708</v>
@@ -6215,31 +6215,31 @@
   <sheetPr codeName="FXRates_Fields"/>
   <dimension ref="A1:P36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="66.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="44.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="43.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="61.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="45.88671875" customWidth="1"/>
-    <col min="11" max="11" width="40.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="40.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="66.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="61.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="45.85546875" customWidth="1"/>
+    <col min="11" max="11" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -6247,7 +6247,7 @@
         <v>17</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>1</v>
@@ -6286,10 +6286,10 @@
         <v>121</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>1006</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -6297,10 +6297,10 @@
         <v>44</v>
       </c>
       <c r="C2" s="9" t="s">
+        <v>1014</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>1015</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>1016</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>130</v>
@@ -6315,7 +6315,7 @@
         <v>48</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>129</v>
@@ -6336,7 +6336,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>22</v>
       </c>
@@ -6344,10 +6344,10 @@
         <v>71</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>242</v>
@@ -6362,7 +6362,7 @@
         <v>74</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="J3" s="5" t="s">
         <v>75</v>
@@ -6383,7 +6383,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>36</v>
       </c>
@@ -6391,10 +6391,10 @@
         <v>77</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>245</v>
@@ -6409,7 +6409,7 @@
         <v>85</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="J4" s="5" t="s">
         <v>81</v>
@@ -6430,7 +6430,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>43</v>
       </c>
@@ -6438,10 +6438,10 @@
         <v>78</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>248</v>
@@ -6456,7 +6456,7 @@
         <v>86</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="J5" s="5" t="s">
         <v>82</v>
@@ -6477,7 +6477,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>49</v>
       </c>
@@ -6485,10 +6485,10 @@
         <v>87</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>251</v>
@@ -6503,7 +6503,7 @@
         <v>91</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="J6" s="5" t="s">
         <v>92</v>
@@ -6524,7 +6524,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>57</v>
       </c>
@@ -6532,10 +6532,10 @@
         <v>123</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>254</v>
@@ -6550,7 +6550,7 @@
         <v>126</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="J7" s="5" t="s">
         <v>127</v>
@@ -6571,7 +6571,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>64</v>
       </c>
@@ -6579,13 +6579,13 @@
         <v>257</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>258</v>
@@ -6597,7 +6597,7 @@
         <v>260</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="J8" s="5" t="s">
         <v>261</v>
@@ -6618,7 +6618,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>96</v>
       </c>
@@ -6626,13 +6626,13 @@
         <v>265</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>266</v>
@@ -6644,7 +6644,7 @@
         <v>268</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="J9" s="5" t="s">
         <v>269</v>
@@ -6665,7 +6665,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>103</v>
       </c>
@@ -6673,13 +6673,13 @@
         <v>273</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>274</v>
@@ -6691,7 +6691,7 @@
         <v>276</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="J10" s="5" t="s">
         <v>277</v>
@@ -6712,7 +6712,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>111</v>
       </c>
@@ -6720,13 +6720,13 @@
         <v>281</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>282</v>
@@ -6738,7 +6738,7 @@
         <v>284</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="J11" s="5" t="s">
         <v>285</v>
@@ -6759,7 +6759,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>113</v>
       </c>
@@ -6767,13 +6767,13 @@
         <v>289</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>290</v>
@@ -6785,7 +6785,7 @@
         <v>292</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="J12" s="5" t="s">
         <v>293</v>
@@ -6806,7 +6806,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>115</v>
       </c>
@@ -6814,13 +6814,13 @@
         <v>297</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>298</v>
@@ -6832,7 +6832,7 @@
         <v>300</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="J13" s="5" t="s">
         <v>301</v>
@@ -6853,7 +6853,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>117</v>
       </c>
@@ -6861,13 +6861,13 @@
         <v>305</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>306</v>
@@ -6879,7 +6879,7 @@
         <v>308</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="J14" s="5" t="s">
         <v>309</v>
@@ -6900,7 +6900,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>119</v>
       </c>
@@ -6908,10 +6908,10 @@
         <v>313</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>314</v>
@@ -6926,7 +6926,7 @@
         <v>317</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="J15" s="5" t="s">
         <v>318</v>
@@ -6947,7 +6947,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>144</v>
       </c>
@@ -6955,10 +6955,10 @@
         <v>322</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>323</v>
@@ -6973,7 +6973,7 @@
         <v>326</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="J16" s="5" t="s">
         <v>327</v>
@@ -6994,7 +6994,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>331</v>
       </c>
@@ -7002,10 +7002,10 @@
         <v>332</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>333</v>
@@ -7020,7 +7020,7 @@
         <v>336</v>
       </c>
       <c r="I17" s="9" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="J17" s="5" t="s">
         <v>337</v>
@@ -7041,7 +7041,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>341</v>
       </c>
@@ -7049,10 +7049,10 @@
         <v>342</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>343</v>
@@ -7067,7 +7067,7 @@
         <v>346</v>
       </c>
       <c r="I18" s="9" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="J18" s="5" t="s">
         <v>347</v>
@@ -7088,7 +7088,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>351</v>
       </c>
@@ -7096,10 +7096,10 @@
         <v>352</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>353</v>
@@ -7114,7 +7114,7 @@
         <v>356</v>
       </c>
       <c r="I19" s="9" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="J19" s="5" t="s">
         <v>357</v>
@@ -7135,7 +7135,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>167</v>
       </c>
@@ -7143,10 +7143,10 @@
         <v>361</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>362</v>
@@ -7161,7 +7161,7 @@
         <v>365</v>
       </c>
       <c r="I20" s="9" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="J20" s="5" t="s">
         <v>366</v>
@@ -7182,10 +7182,10 @@
         <v>241</v>
       </c>
       <c r="P20" s="5" t="s">
-        <v>1007</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>208</v>
       </c>
@@ -7193,10 +7193,10 @@
         <v>370</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>371</v>
@@ -7211,7 +7211,7 @@
         <v>374</v>
       </c>
       <c r="I21" s="9" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="J21" s="5" t="s">
         <v>375</v>
@@ -7232,7 +7232,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>228</v>
       </c>
@@ -7240,10 +7240,10 @@
         <v>379</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>380</v>
@@ -7258,7 +7258,7 @@
         <v>383</v>
       </c>
       <c r="I22" s="9" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="J22" s="5" t="s">
         <v>384</v>
@@ -7279,7 +7279,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>230</v>
       </c>
@@ -7287,10 +7287,10 @@
         <v>388</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>389</v>
@@ -7305,7 +7305,7 @@
         <v>392</v>
       </c>
       <c r="I23" s="9" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="J23" s="5" t="s">
         <v>393</v>
@@ -7326,7 +7326,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>397</v>
       </c>
@@ -7334,10 +7334,10 @@
         <v>398</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>399</v>
@@ -7352,7 +7352,7 @@
         <v>402</v>
       </c>
       <c r="I24" s="9" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="J24" s="5" t="s">
         <v>403</v>
@@ -7373,7 +7373,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>407</v>
       </c>
@@ -7381,10 +7381,10 @@
         <v>408</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>409</v>
@@ -7399,7 +7399,7 @@
         <v>412</v>
       </c>
       <c r="I25" s="9" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="J25" s="5" t="s">
         <v>413</v>
@@ -7420,7 +7420,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="26" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>417</v>
       </c>
@@ -7428,10 +7428,10 @@
         <v>418</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>476</v>
@@ -7446,7 +7446,7 @@
         <v>421</v>
       </c>
       <c r="I26" s="9" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="J26" s="5" t="s">
         <v>422</v>
@@ -7467,7 +7467,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="27" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>426</v>
       </c>
@@ -7475,10 +7475,10 @@
         <v>427</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>428</v>
@@ -7493,7 +7493,7 @@
         <v>431</v>
       </c>
       <c r="I27" s="9" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="J27" s="5" t="s">
         <v>432</v>
@@ -7514,7 +7514,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>436</v>
       </c>
@@ -7522,10 +7522,10 @@
         <v>437</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>438</v>
@@ -7540,7 +7540,7 @@
         <v>441</v>
       </c>
       <c r="I28" s="9" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="J28" s="5" t="s">
         <v>442</v>
@@ -7561,7 +7561,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>446</v>
       </c>
@@ -7569,10 +7569,10 @@
         <v>447</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>448</v>
@@ -7587,7 +7587,7 @@
         <v>451</v>
       </c>
       <c r="I29" s="9" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="J29" s="5" t="s">
         <v>452</v>
@@ -7608,7 +7608,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>456</v>
       </c>
@@ -7616,10 +7616,10 @@
         <v>457</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>458</v>
@@ -7634,7 +7634,7 @@
         <v>461</v>
       </c>
       <c r="I30" s="9" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="J30" s="5" t="s">
         <v>462</v>
@@ -7655,7 +7655,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="31" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>466</v>
       </c>
@@ -7663,10 +7663,10 @@
         <v>467</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="E31" s="5" t="s">
         <v>468</v>
@@ -7681,7 +7681,7 @@
         <v>471</v>
       </c>
       <c r="I31" s="9" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="J31" s="5" t="s">
         <v>472</v>
@@ -7702,7 +7702,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="32" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>578</v>
       </c>
@@ -7710,10 +7710,10 @@
         <v>579</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="E32" s="5" t="s">
         <v>672</v>
@@ -7728,7 +7728,7 @@
         <v>582</v>
       </c>
       <c r="I32" s="9" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="J32" s="5" t="s">
         <v>583</v>
@@ -7749,7 +7749,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
         <v>587</v>
       </c>
@@ -7757,10 +7757,10 @@
         <v>588</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="E33" s="5" t="s">
         <v>673</v>
@@ -7775,7 +7775,7 @@
         <v>591</v>
       </c>
       <c r="I33" s="9" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="J33" s="5" t="s">
         <v>592</v>
@@ -7796,7 +7796,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>596</v>
       </c>
@@ -7804,10 +7804,10 @@
         <v>597</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="E34" s="5" t="s">
         <v>674</v>
@@ -7822,7 +7822,7 @@
         <v>600</v>
       </c>
       <c r="I34" s="9" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="J34" s="5" t="s">
         <v>601</v>
@@ -7843,7 +7843,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>605</v>
       </c>
@@ -7851,10 +7851,10 @@
         <v>606</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="E35" s="5" t="s">
         <v>675</v>
@@ -7869,7 +7869,7 @@
         <v>609</v>
       </c>
       <c r="I35" s="9" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="J35" s="5" t="s">
         <v>610</v>
@@ -7890,7 +7890,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
         <v>614</v>
       </c>
@@ -7898,10 +7898,10 @@
         <v>615</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="E36" s="5" t="s">
         <v>676</v>
@@ -7916,7 +7916,7 @@
         <v>618</v>
       </c>
       <c r="I36" s="9" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="J36" s="5" t="s">
         <v>619</v>
@@ -7993,24 +7993,24 @@
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="63.5546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.5703125" style="1" customWidth="1"/>
     <col min="4" max="4" width="94" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="42.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="36.33203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="75.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="37.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="42.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="36.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="75.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="37.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="40" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="60.33203125" customWidth="1"/>
+    <col min="12" max="12" width="60.28515625" customWidth="1"/>
     <col min="13" max="13" width="45" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -8051,7 +8051,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -8059,10 +8059,10 @@
         <v>138</v>
       </c>
       <c r="C2" s="9" t="s">
+        <v>1016</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>1017</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>1018</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>141</v>
@@ -8074,7 +8074,7 @@
         <v>143</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>164</v>
@@ -8089,7 +8089,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>22</v>
       </c>
@@ -8097,10 +8097,10 @@
         <v>478</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>479</v>
@@ -8112,10 +8112,10 @@
         <v>481</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="J3" s="5" t="s">
         <v>482</v>
@@ -8130,253 +8130,253 @@
         <v>484</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>36</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>799</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>1074</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>807</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>800</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>1075</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>808</v>
-      </c>
-      <c r="E4" s="5" t="s">
+      <c r="F4" s="5" t="s">
         <v>801</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="G4" s="5" t="s">
         <v>802</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="H4" s="5" t="s">
         <v>803</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="I4" s="9" t="s">
+        <v>1074</v>
+      </c>
+      <c r="J4" s="5" t="s">
         <v>804</v>
       </c>
-      <c r="I4" s="9" t="s">
-        <v>1075</v>
-      </c>
-      <c r="J4" s="5" t="s">
+      <c r="K4" s="5" t="s">
         <v>805</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="L4" s="5" t="s">
         <v>806</v>
       </c>
-      <c r="L4" s="5" t="s">
-        <v>807</v>
-      </c>
       <c r="M4" s="5" t="s">
-        <v>807</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>43</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>808</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>1075</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>816</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>809</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>1076</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>817</v>
-      </c>
-      <c r="E5" s="5" t="s">
+      <c r="F5" s="5" t="s">
         <v>810</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="G5" s="5" t="s">
         <v>811</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="H5" s="5" t="s">
         <v>812</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="I5" s="9" t="s">
+        <v>1075</v>
+      </c>
+      <c r="J5" s="5" t="s">
         <v>813</v>
       </c>
-      <c r="I5" s="9" t="s">
-        <v>1076</v>
-      </c>
-      <c r="J5" s="5" t="s">
+      <c r="K5" s="5" t="s">
         <v>814</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="L5" s="5" t="s">
         <v>815</v>
       </c>
-      <c r="L5" s="5" t="s">
-        <v>816</v>
-      </c>
       <c r="M5" s="5" t="s">
-        <v>816</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>64</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>751</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>1076</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>752</v>
       </c>
-      <c r="C6" s="9" t="s">
-        <v>1077</v>
-      </c>
-      <c r="D6" s="6" t="s">
+      <c r="E6" s="5" t="s">
         <v>753</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="F6" s="5" t="s">
         <v>754</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="G6" s="5" t="s">
         <v>755</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="H6" s="5" t="s">
         <v>756</v>
       </c>
-      <c r="H6" s="5" t="s">
-        <v>757</v>
-      </c>
       <c r="I6" s="9" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="J6" s="5" t="s">
+        <v>759</v>
+      </c>
+      <c r="K6" s="5" t="s">
         <v>760</v>
       </c>
-      <c r="K6" s="5" t="s">
+      <c r="L6" s="5" t="s">
         <v>761</v>
       </c>
-      <c r="L6" s="5" t="s">
-        <v>762</v>
-      </c>
       <c r="M6" s="5" t="s">
-        <v>762</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>96</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>736</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>1018</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>1019</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>737</v>
       </c>
-      <c r="C7" s="9" t="s">
-        <v>1019</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>1020</v>
-      </c>
-      <c r="E7" s="5" t="s">
+      <c r="F7" s="5" t="s">
         <v>738</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="G7" s="5" t="s">
         <v>739</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="H7" s="5" t="s">
+        <v>757</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>1018</v>
+      </c>
+      <c r="J7" s="5" t="s">
         <v>740</v>
       </c>
-      <c r="H7" s="5" t="s">
-        <v>758</v>
-      </c>
-      <c r="I7" s="9" t="s">
-        <v>1019</v>
-      </c>
-      <c r="J7" s="5" t="s">
+      <c r="K7" s="5" t="s">
         <v>741</v>
       </c>
-      <c r="K7" s="5" t="s">
-        <v>742</v>
-      </c>
       <c r="L7" s="5" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="M7" s="5" t="s">
-        <v>750</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>103</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>742</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>1063</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>1064</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>743</v>
       </c>
-      <c r="C8" s="9" t="s">
-        <v>1064</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>1065</v>
-      </c>
-      <c r="E8" s="5" t="s">
+      <c r="F8" s="5" t="s">
         <v>744</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="G8" s="5" t="s">
         <v>745</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="H8" s="5" t="s">
+        <v>758</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>1063</v>
+      </c>
+      <c r="J8" s="5" t="s">
         <v>746</v>
       </c>
-      <c r="H8" s="5" t="s">
-        <v>759</v>
-      </c>
-      <c r="I8" s="9" t="s">
-        <v>1064</v>
-      </c>
-      <c r="J8" s="5" t="s">
+      <c r="K8" s="5" t="s">
         <v>747</v>
-      </c>
-      <c r="K8" s="5" t="s">
-        <v>748</v>
       </c>
       <c r="L8" s="5" t="s">
         <v>484</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>749</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>111</v>
       </c>
       <c r="B9" s="5" t="s">
+        <v>763</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>764</v>
       </c>
-      <c r="C9" s="9" t="s">
-        <v>1078</v>
-      </c>
-      <c r="D9" s="6" t="s">
+      <c r="E9" s="5" t="s">
         <v>765</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="F9" s="5" t="s">
         <v>766</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="G9" s="5" t="s">
         <v>767</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="H9" s="5" t="s">
         <v>768</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="I9" s="9" t="s">
+        <v>1077</v>
+      </c>
+      <c r="J9" s="5" t="s">
         <v>769</v>
       </c>
-      <c r="I9" s="9" t="s">
-        <v>1078</v>
-      </c>
-      <c r="J9" s="5" t="s">
+      <c r="K9" s="5" t="s">
         <v>770</v>
       </c>
-      <c r="K9" s="5" t="s">
+      <c r="L9" s="5" t="s">
         <v>771</v>
       </c>
-      <c r="L9" s="5" t="s">
-        <v>772</v>
-      </c>
       <c r="M9" s="5" t="s">
-        <v>772</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>113</v>
       </c>
@@ -8384,10 +8384,10 @@
         <v>485</v>
       </c>
       <c r="C10" s="9" t="s">
+        <v>1059</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>1060</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>1061</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>486</v>
@@ -8399,10 +8399,10 @@
         <v>488</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="J10" s="5" t="s">
         <v>489</v>
@@ -8417,130 +8417,130 @@
         <v>491</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>115</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>933</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>1078</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>934</v>
       </c>
-      <c r="C11" s="9" t="s">
-        <v>1079</v>
-      </c>
-      <c r="D11" s="6" t="s">
+      <c r="E11" s="5" t="s">
         <v>935</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="F11" s="5" t="s">
         <v>936</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="G11" s="5" t="s">
         <v>937</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="H11" s="5" t="s">
         <v>938</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="I11" s="9" t="s">
+        <v>1078</v>
+      </c>
+      <c r="J11" s="5" t="s">
         <v>939</v>
       </c>
-      <c r="I11" s="9" t="s">
-        <v>1079</v>
-      </c>
-      <c r="J11" s="5" t="s">
+      <c r="K11" s="5" t="s">
         <v>940</v>
       </c>
-      <c r="K11" s="5" t="s">
+      <c r="L11" s="5" t="s">
         <v>941</v>
       </c>
-      <c r="L11" s="5" t="s">
-        <v>942</v>
-      </c>
       <c r="M11" s="5" t="s">
-        <v>942</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>117</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>942</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>1079</v>
+      </c>
+      <c r="D12" s="6" t="s">
         <v>943</v>
       </c>
-      <c r="C12" s="9" t="s">
-        <v>1080</v>
-      </c>
-      <c r="D12" s="6" t="s">
+      <c r="E12" s="5" t="s">
         <v>944</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="F12" s="5" t="s">
         <v>945</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="G12" s="5" t="s">
         <v>946</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="H12" s="5" t="s">
         <v>947</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="I12" s="9" t="s">
+        <v>1079</v>
+      </c>
+      <c r="J12" s="5" t="s">
         <v>948</v>
       </c>
-      <c r="I12" s="9" t="s">
-        <v>1080</v>
-      </c>
-      <c r="J12" s="5" t="s">
+      <c r="K12" s="5" t="s">
         <v>949</v>
       </c>
-      <c r="K12" s="5" t="s">
+      <c r="L12" s="5" t="s">
         <v>950</v>
       </c>
-      <c r="L12" s="5" t="s">
-        <v>951</v>
-      </c>
       <c r="M12" s="5" t="s">
-        <v>951</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>119</v>
       </c>
       <c r="B13" s="5" t="s">
+        <v>826</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>1080</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>827</v>
       </c>
-      <c r="C13" s="9" t="s">
-        <v>1081</v>
-      </c>
-      <c r="D13" s="6" t="s">
+      <c r="E13" s="5" t="s">
         <v>828</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="F13" s="5" t="s">
         <v>829</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="G13" s="5" t="s">
         <v>830</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="H13" s="5" t="s">
         <v>831</v>
       </c>
-      <c r="H13" s="5" t="s">
+      <c r="I13" s="9" t="s">
+        <v>1080</v>
+      </c>
+      <c r="J13" s="5" t="s">
         <v>832</v>
       </c>
-      <c r="I13" s="9" t="s">
-        <v>1081</v>
-      </c>
-      <c r="J13" s="5" t="s">
+      <c r="K13" s="5" t="s">
         <v>833</v>
       </c>
-      <c r="K13" s="5" t="s">
+      <c r="L13" s="5" t="s">
         <v>834</v>
       </c>
-      <c r="L13" s="5" t="s">
-        <v>835</v>
-      </c>
       <c r="M13" s="5" t="s">
-        <v>835</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>144</v>
       </c>
@@ -8548,10 +8548,10 @@
         <v>492</v>
       </c>
       <c r="C14" s="9" t="s">
+        <v>1061</v>
+      </c>
+      <c r="D14" s="6" t="s">
         <v>1062</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>1063</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>493</v>
@@ -8564,7 +8564,7 @@
       </c>
       <c r="H14" s="5"/>
       <c r="I14" s="9" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="J14" s="5" t="s">
         <v>496</v>
@@ -8579,7 +8579,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>499</v>
       </c>
@@ -8587,10 +8587,10 @@
         <v>500</v>
       </c>
       <c r="C15" s="9" t="s">
+        <v>1065</v>
+      </c>
+      <c r="D15" s="6" t="s">
         <v>1066</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>1067</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>501</v>
@@ -8603,7 +8603,7 @@
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="9" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="J15" s="5" t="s">
         <v>504</v>
@@ -8618,7 +8618,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>507</v>
       </c>
@@ -8626,10 +8626,10 @@
         <v>508</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>509</v>
@@ -8642,7 +8642,7 @@
       </c>
       <c r="H16" s="5"/>
       <c r="I16" s="9" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="J16" s="5" t="s">
         <v>512</v>
@@ -8657,7 +8657,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>17</v>
       </c>
@@ -8665,10 +8665,10 @@
         <v>515</v>
       </c>
       <c r="C17" s="9" t="s">
+        <v>1068</v>
+      </c>
+      <c r="D17" s="6" t="s">
         <v>1069</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>1070</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>516</v>
@@ -8683,7 +8683,7 @@
         <v>519</v>
       </c>
       <c r="I17" s="9" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="J17" s="5" t="s">
         <v>520</v>
@@ -8698,7 +8698,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>18</v>
       </c>
@@ -8706,10 +8706,10 @@
         <v>523</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>524</v>
@@ -8722,7 +8722,7 @@
       </c>
       <c r="H18" s="5"/>
       <c r="I18" s="9" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="J18" s="5" t="s">
         <v>527</v>
@@ -8737,7 +8737,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>19</v>
       </c>
@@ -8745,10 +8745,10 @@
         <v>530</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>531</v>
@@ -8761,7 +8761,7 @@
       </c>
       <c r="H19" s="5"/>
       <c r="I19" s="9" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="J19" s="5" t="s">
         <v>534</v>
@@ -8776,7 +8776,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>208</v>
       </c>
@@ -8784,10 +8784,10 @@
         <v>641</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>642</v>
@@ -8800,7 +8800,7 @@
       </c>
       <c r="H20" s="5"/>
       <c r="I20" s="9" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="J20" s="5" t="s">
         <v>645</v>
@@ -8815,7 +8815,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>228</v>
       </c>
@@ -8823,10 +8823,10 @@
         <v>571</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>572</v>
@@ -8839,7 +8839,7 @@
       </c>
       <c r="H21" s="5"/>
       <c r="I21" s="9" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="J21" s="5" t="s">
         <v>575</v>
@@ -8854,417 +8854,417 @@
         <v>577</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>417</v>
       </c>
       <c r="B22" s="5" t="s">
+        <v>969</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>1082</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>1095</v>
+      </c>
+      <c r="E22" s="5" t="s">
         <v>970</v>
       </c>
-      <c r="C22" s="9" t="s">
-        <v>1083</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>1096</v>
-      </c>
-      <c r="E22" s="5" t="s">
+      <c r="F22" s="5" t="s">
         <v>971</v>
       </c>
-      <c r="F22" s="5" t="s">
+      <c r="G22" s="5" t="s">
         <v>972</v>
       </c>
-      <c r="G22" s="5" t="s">
+      <c r="H22" s="5" t="s">
         <v>973</v>
       </c>
-      <c r="H22" s="5" t="s">
+      <c r="I22" s="9" t="s">
+        <v>1082</v>
+      </c>
+      <c r="J22" s="5" t="s">
         <v>974</v>
       </c>
-      <c r="I22" s="9" t="s">
-        <v>1083</v>
-      </c>
-      <c r="J22" s="5" t="s">
+      <c r="K22" s="5" t="s">
         <v>975</v>
       </c>
-      <c r="K22" s="5" t="s">
+      <c r="L22" s="5" t="s">
         <v>976</v>
       </c>
-      <c r="L22" s="5" t="s">
-        <v>977</v>
-      </c>
       <c r="M22" s="5" t="s">
-        <v>977</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>426</v>
       </c>
       <c r="B23" s="5" t="s">
+        <v>773</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>1083</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>1007</v>
+      </c>
+      <c r="E23" s="5" t="s">
         <v>774</v>
       </c>
-      <c r="C23" s="9" t="s">
-        <v>1084</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>1008</v>
-      </c>
-      <c r="E23" s="5" t="s">
+      <c r="F23" s="5" t="s">
         <v>775</v>
       </c>
-      <c r="F23" s="5" t="s">
+      <c r="G23" s="5" t="s">
         <v>776</v>
       </c>
-      <c r="G23" s="5" t="s">
+      <c r="H23" s="5" t="s">
         <v>777</v>
       </c>
-      <c r="H23" s="5" t="s">
+      <c r="I23" s="9" t="s">
+        <v>1083</v>
+      </c>
+      <c r="J23" s="5" t="s">
         <v>778</v>
       </c>
-      <c r="I23" s="9" t="s">
-        <v>1084</v>
-      </c>
-      <c r="J23" s="5" t="s">
+      <c r="K23" s="5" t="s">
         <v>779</v>
       </c>
-      <c r="K23" s="5" t="s">
+      <c r="L23" s="5" t="s">
         <v>780</v>
       </c>
-      <c r="L23" s="5" t="s">
-        <v>781</v>
-      </c>
       <c r="M23" s="5" t="s">
-        <v>781</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>436</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="D24" s="6" t="s">
+        <v>783</v>
+      </c>
+      <c r="E24" s="5" t="s">
         <v>784</v>
       </c>
-      <c r="E24" s="5" t="s">
+      <c r="F24" s="5" t="s">
         <v>785</v>
       </c>
-      <c r="F24" s="5" t="s">
+      <c r="G24" s="5" t="s">
         <v>786</v>
       </c>
-      <c r="G24" s="5" t="s">
+      <c r="H24" s="5" t="s">
         <v>787</v>
       </c>
-      <c r="H24" s="5" t="s">
+      <c r="I24" s="9" t="s">
+        <v>1084</v>
+      </c>
+      <c r="J24" s="5" t="s">
         <v>788</v>
       </c>
-      <c r="I24" s="9" t="s">
-        <v>1085</v>
-      </c>
-      <c r="J24" s="5" t="s">
+      <c r="K24" s="5" t="s">
         <v>789</v>
       </c>
-      <c r="K24" s="5" t="s">
+      <c r="L24" s="5" t="s">
         <v>790</v>
       </c>
-      <c r="L24" s="5" t="s">
-        <v>791</v>
-      </c>
       <c r="M24" s="5" t="s">
-        <v>791</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>446</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="D25" s="6" t="s">
+        <v>791</v>
+      </c>
+      <c r="E25" s="5" t="s">
         <v>792</v>
       </c>
-      <c r="E25" s="5" t="s">
+      <c r="F25" s="5" t="s">
         <v>793</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="G25" s="5" t="s">
         <v>794</v>
       </c>
-      <c r="G25" s="5" t="s">
+      <c r="H25" s="5" t="s">
         <v>795</v>
       </c>
-      <c r="H25" s="5" t="s">
+      <c r="I25" s="9" t="s">
+        <v>1085</v>
+      </c>
+      <c r="J25" s="5" t="s">
         <v>796</v>
       </c>
-      <c r="I25" s="9" t="s">
-        <v>1086</v>
-      </c>
-      <c r="J25" s="5" t="s">
+      <c r="K25" s="5" t="s">
         <v>797</v>
       </c>
-      <c r="K25" s="5" t="s">
+      <c r="L25" s="5" t="s">
         <v>798</v>
       </c>
-      <c r="L25" s="5" t="s">
-        <v>799</v>
-      </c>
       <c r="M25" s="5" t="s">
-        <v>799</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>456</v>
       </c>
       <c r="B26" s="5" t="s">
+        <v>893</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>1086</v>
+      </c>
+      <c r="D26" s="6" t="s">
         <v>894</v>
       </c>
-      <c r="C26" s="9" t="s">
-        <v>1087</v>
-      </c>
-      <c r="D26" s="6" t="s">
+      <c r="E26" s="5" t="s">
         <v>895</v>
       </c>
-      <c r="E26" s="5" t="s">
+      <c r="F26" s="5" t="s">
         <v>896</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="G26" s="5" t="s">
         <v>897</v>
       </c>
-      <c r="G26" s="5" t="s">
+      <c r="H26" s="5" t="s">
         <v>898</v>
       </c>
-      <c r="H26" s="5" t="s">
+      <c r="I26" s="9" t="s">
+        <v>1086</v>
+      </c>
+      <c r="J26" s="5" t="s">
         <v>899</v>
       </c>
-      <c r="I26" s="9" t="s">
-        <v>1087</v>
-      </c>
-      <c r="J26" s="5" t="s">
+      <c r="K26" s="5" t="s">
         <v>900</v>
       </c>
-      <c r="K26" s="5" t="s">
+      <c r="L26" s="5" t="s">
         <v>901</v>
       </c>
-      <c r="L26" s="5" t="s">
-        <v>902</v>
-      </c>
       <c r="M26" s="5" t="s">
-        <v>902</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>466</v>
       </c>
       <c r="B27" s="5" t="s">
+        <v>902</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>1087</v>
+      </c>
+      <c r="D27" s="6" t="s">
         <v>903</v>
       </c>
-      <c r="C27" s="9" t="s">
-        <v>1088</v>
-      </c>
-      <c r="D27" s="6" t="s">
+      <c r="E27" s="5" t="s">
         <v>904</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="F27" s="5" t="s">
         <v>905</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="G27" s="5" t="s">
         <v>906</v>
       </c>
-      <c r="G27" s="5" t="s">
+      <c r="H27" s="5" t="s">
         <v>907</v>
       </c>
-      <c r="H27" s="5" t="s">
+      <c r="I27" s="9" t="s">
+        <v>1087</v>
+      </c>
+      <c r="J27" s="5" t="s">
         <v>908</v>
       </c>
-      <c r="I27" s="9" t="s">
-        <v>1088</v>
-      </c>
-      <c r="J27" s="5" t="s">
+      <c r="K27" s="5" t="s">
         <v>909</v>
       </c>
-      <c r="K27" s="5" t="s">
+      <c r="L27" s="5" t="s">
         <v>910</v>
       </c>
-      <c r="L27" s="5" t="s">
-        <v>911</v>
-      </c>
       <c r="M27" s="5" t="s">
-        <v>911</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>578</v>
       </c>
       <c r="B28" s="5" t="s">
+        <v>911</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>1088</v>
+      </c>
+      <c r="D28" s="6" t="s">
         <v>912</v>
       </c>
-      <c r="C28" s="9" t="s">
-        <v>1089</v>
-      </c>
-      <c r="D28" s="6" t="s">
+      <c r="E28" s="5" t="s">
         <v>913</v>
       </c>
-      <c r="E28" s="5" t="s">
+      <c r="F28" s="5" t="s">
         <v>914</v>
       </c>
-      <c r="F28" s="5" t="s">
+      <c r="G28" s="5" t="s">
         <v>915</v>
       </c>
-      <c r="G28" s="5" t="s">
+      <c r="H28" s="5" t="s">
         <v>916</v>
       </c>
-      <c r="H28" s="5" t="s">
+      <c r="I28" s="9" t="s">
+        <v>1088</v>
+      </c>
+      <c r="J28" s="5" t="s">
         <v>917</v>
       </c>
-      <c r="I28" s="9" t="s">
-        <v>1089</v>
-      </c>
-      <c r="J28" s="5" t="s">
+      <c r="K28" s="5" t="s">
         <v>918</v>
       </c>
-      <c r="K28" s="5" t="s">
+      <c r="L28" s="5" t="s">
         <v>919</v>
       </c>
-      <c r="L28" s="5" t="s">
-        <v>920</v>
-      </c>
       <c r="M28" s="5" t="s">
-        <v>920</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>587</v>
       </c>
       <c r="B29" s="5" t="s">
+        <v>951</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>1089</v>
+      </c>
+      <c r="D29" s="6" t="s">
         <v>952</v>
       </c>
-      <c r="C29" s="9" t="s">
-        <v>1090</v>
-      </c>
-      <c r="D29" s="6" t="s">
+      <c r="E29" s="5" t="s">
         <v>953</v>
       </c>
-      <c r="E29" s="5" t="s">
+      <c r="F29" s="5" t="s">
         <v>954</v>
       </c>
-      <c r="F29" s="5" t="s">
+      <c r="G29" s="5" t="s">
         <v>955</v>
       </c>
-      <c r="G29" s="5" t="s">
+      <c r="H29" s="5" t="s">
         <v>956</v>
       </c>
-      <c r="H29" s="5" t="s">
+      <c r="I29" s="9" t="s">
+        <v>1089</v>
+      </c>
+      <c r="J29" s="5" t="s">
         <v>957</v>
       </c>
-      <c r="I29" s="9" t="s">
-        <v>1090</v>
-      </c>
-      <c r="J29" s="5" t="s">
+      <c r="K29" s="5" t="s">
         <v>958</v>
       </c>
-      <c r="K29" s="5" t="s">
+      <c r="L29" s="5" t="s">
         <v>959</v>
       </c>
-      <c r="L29" s="5" t="s">
-        <v>960</v>
-      </c>
       <c r="M29" s="5" t="s">
-        <v>960</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>596</v>
       </c>
       <c r="B30" s="5" t="s">
+        <v>960</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>1090</v>
+      </c>
+      <c r="D30" s="6" t="s">
         <v>961</v>
       </c>
-      <c r="C30" s="9" t="s">
-        <v>1091</v>
-      </c>
-      <c r="D30" s="6" t="s">
+      <c r="E30" s="5" t="s">
         <v>962</v>
       </c>
-      <c r="E30" s="5" t="s">
+      <c r="F30" s="5" t="s">
         <v>963</v>
       </c>
-      <c r="F30" s="5" t="s">
+      <c r="G30" s="5" t="s">
         <v>964</v>
       </c>
-      <c r="G30" s="5" t="s">
+      <c r="H30" s="5" t="s">
         <v>965</v>
       </c>
-      <c r="H30" s="5" t="s">
+      <c r="I30" s="9" t="s">
+        <v>1090</v>
+      </c>
+      <c r="J30" s="5" t="s">
         <v>966</v>
       </c>
-      <c r="I30" s="9" t="s">
-        <v>1091</v>
-      </c>
-      <c r="J30" s="5" t="s">
+      <c r="K30" s="5" t="s">
         <v>967</v>
       </c>
-      <c r="K30" s="5" t="s">
+      <c r="L30" s="5" t="s">
         <v>968</v>
       </c>
-      <c r="L30" s="5" t="s">
-        <v>969</v>
-      </c>
       <c r="M30" s="5" t="s">
-        <v>969</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>614</v>
       </c>
       <c r="B31" s="5" t="s">
+        <v>817</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>1091</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>825</v>
+      </c>
+      <c r="E31" s="5" t="s">
         <v>818</v>
       </c>
-      <c r="C31" s="9" t="s">
-        <v>1092</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>826</v>
-      </c>
-      <c r="E31" s="5" t="s">
+      <c r="F31" s="5" t="s">
         <v>819</v>
       </c>
-      <c r="F31" s="5" t="s">
+      <c r="G31" s="5" t="s">
         <v>820</v>
       </c>
-      <c r="G31" s="5" t="s">
+      <c r="H31" s="5" t="s">
         <v>821</v>
       </c>
-      <c r="H31" s="5" t="s">
+      <c r="I31" s="9" t="s">
+        <v>1091</v>
+      </c>
+      <c r="J31" s="5" t="s">
         <v>822</v>
       </c>
-      <c r="I31" s="9" t="s">
-        <v>1092</v>
-      </c>
-      <c r="J31" s="5" t="s">
+      <c r="K31" s="5" t="s">
         <v>823</v>
       </c>
-      <c r="K31" s="5" t="s">
+      <c r="L31" s="5" t="s">
         <v>824</v>
       </c>
-      <c r="L31" s="5" t="s">
-        <v>825</v>
-      </c>
       <c r="M31" s="5" t="s">
-        <v>825</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>537</v>
       </c>
@@ -9272,10 +9272,10 @@
         <v>538</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="E32" s="5" t="s">
         <v>539</v>
@@ -9288,7 +9288,7 @@
       </c>
       <c r="H32" s="5"/>
       <c r="I32" s="9" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="J32" s="5" t="s">
         <v>542</v>
@@ -9303,7 +9303,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>545</v>
       </c>
@@ -9311,10 +9311,10 @@
         <v>546</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="E33" s="5" t="s">
         <v>547</v>
@@ -9327,7 +9327,7 @@
       </c>
       <c r="H33" s="5"/>
       <c r="I33" s="9" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="J33" s="5" t="s">
         <v>550</v>
@@ -9368,9 +9368,9 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -9378,7 +9378,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>

</xml_diff>